<commit_message>
"Actualizando PIB,VAB y resultado fiscal"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
   <si>
     <t>Período</t>
   </si>
@@ -508,7 +508,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -585,6 +585,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2046,7 +2049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
@@ -2424,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C66"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2457,7 +2460,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="13">
-        <v>475571.25053602818</v>
+        <v>475540.07912460313</v>
       </c>
       <c r="D2" s="13">
         <v>460369.44223294873</v>
@@ -2471,7 +2474,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="13">
-        <v>470108.44496971456</v>
+        <v>470121.1274420924</v>
       </c>
       <c r="D3" s="13">
         <v>514395.68177236168</v>
@@ -2485,7 +2488,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="13">
-        <v>493804.50440805691</v>
+        <v>493832.66195269296</v>
       </c>
       <c r="D4" s="13">
         <v>481151.97994350811</v>
@@ -2499,7 +2502,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="13">
-        <v>500976.58062363119</v>
+        <v>500966.91203686345</v>
       </c>
       <c r="D5" s="13">
         <v>484543.6768765623</v>
@@ -2513,7 +2516,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="13">
-        <v>515427.02206872503</v>
+        <v>515472.67133145465</v>
       </c>
       <c r="D6" s="13">
         <v>493602.53057785495</v>
@@ -2527,7 +2530,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="13">
-        <v>526326.24994458677</v>
+        <v>526263.57981290342</v>
       </c>
       <c r="D7" s="13">
         <v>581668.24987960246</v>
@@ -2541,7 +2544,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="13">
-        <v>530023.10626443173</v>
+        <v>530051.55276184448</v>
       </c>
       <c r="D8" s="13">
         <v>514697.78950542817</v>
@@ -2555,7 +2558,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="13">
-        <v>540447.391735913</v>
+        <v>540435.96610745403</v>
       </c>
       <c r="D9" s="13">
         <v>522255.20005077147</v>
@@ -2569,7 +2572,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="13">
-        <v>554538.32519139664</v>
+        <v>554527.00541241898</v>
       </c>
       <c r="D10" s="13">
         <v>532348.2120169173</v>
@@ -2583,7 +2586,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="13">
-        <v>561239.01822536462</v>
+        <v>561248.73864931497</v>
       </c>
       <c r="D11" s="13">
         <v>614076.39260854386</v>
@@ -2597,7 +2600,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="13">
-        <v>576947.66556417441</v>
+        <v>576963.188307025</v>
       </c>
       <c r="D12" s="13">
         <v>562978.96562687657</v>
@@ -2611,7 +2614,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="13">
-        <v>589472.60790199053</v>
+        <v>589458.68451416725</v>
       </c>
       <c r="D13" s="13">
         <v>572794.04663058836</v>
@@ -2625,7 +2628,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="13">
-        <v>603212.57489060587</v>
+        <v>603178.72917975707</v>
       </c>
       <c r="D14" s="13">
         <v>576846.88569942722</v>
@@ -2639,7 +2642,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="13">
-        <v>616343.09880483733</v>
+        <v>616364.16815246514</v>
       </c>
       <c r="D15" s="13">
         <v>674620.56300648488</v>
@@ -2653,7 +2656,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="13">
-        <v>624525.68012624152</v>
+        <v>624543.47956237034</v>
       </c>
       <c r="D16" s="13">
         <v>610425.69401485357</v>
@@ -2667,7 +2670,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="13">
-        <v>643688.65676267829</v>
+        <v>643683.63368976943</v>
       </c>
       <c r="D17" s="13">
         <v>625876.86786359688</v>
@@ -2681,7 +2684,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="13">
-        <v>649501.46048697969</v>
+        <v>649543.926967607</v>
       </c>
       <c r="D18" s="13">
         <v>616720.35706447833</v>
@@ -2695,7 +2698,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="13">
-        <v>653583.96665373468</v>
+        <v>653526.34668452281</v>
       </c>
       <c r="D19" s="13">
         <v>711405.50045523292</v>
@@ -2709,7 +2712,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="13">
-        <v>658379.55318123323</v>
+        <v>658399.44773779658</v>
       </c>
       <c r="D20" s="13">
         <v>647087.95974249416</v>
@@ -2723,7 +2726,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="13">
-        <v>627239.65864290029</v>
+        <v>627234.91757492337</v>
       </c>
       <c r="D21" s="13">
         <v>613490.82170264097</v>
@@ -2737,7 +2740,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="13">
-        <v>604363.4433370214</v>
+        <v>604302.82642057771</v>
       </c>
       <c r="D22" s="13">
         <v>578553.04424240452</v>
@@ -2751,7 +2754,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="13">
-        <v>591251.99427603523</v>
+        <v>591301.39090571832</v>
       </c>
       <c r="D23" s="13">
         <v>631197.75186006888</v>
@@ -2765,7 +2768,7 @@
         <v>29</v>
       </c>
       <c r="C24" s="13">
-        <v>614122.08939859062</v>
+        <v>614138.8940492504</v>
       </c>
       <c r="D24" s="13">
         <v>610519.85461172729</v>
@@ -2779,7 +2782,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="13">
-        <v>625753.97863985004</v>
+        <v>625748.39427595027</v>
       </c>
       <c r="D25" s="13">
         <v>615220.85493729718</v>
@@ -2793,7 +2796,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="13">
-        <v>644803.69602679112</v>
+        <v>644736.40918322548</v>
       </c>
       <c r="D26" s="13">
         <v>611607.33658973</v>
@@ -2807,7 +2810,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="13">
-        <v>673842.7320587663</v>
+        <v>673861.03054801899</v>
       </c>
       <c r="D27" s="13">
         <v>733730.77396890335</v>
@@ -2821,7 +2824,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="13">
-        <v>677041.99107720074</v>
+        <v>677043.3951807589</v>
       </c>
       <c r="D28" s="13">
         <v>668566.50948898587</v>
@@ -2835,7 +2838,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="13">
-        <v>686406.29860443575</v>
+        <v>686453.88285519055</v>
       </c>
       <c r="D29" s="13">
         <v>668190.09771957388</v>
@@ -2849,7 +2852,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="13">
-        <v>702868.46139711433</v>
+        <v>702907.26087639318</v>
       </c>
       <c r="D30" s="13">
         <v>662325.58597269515</v>
@@ -2863,7 +2866,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="13">
-        <v>709429.12082686974</v>
+        <v>709431.71628614096</v>
       </c>
       <c r="D31" s="13">
         <v>766332.95457161264</v>
@@ -2877,7 +2880,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="13">
-        <v>715057.02219640778</v>
+        <v>715005.9318030047</v>
       </c>
       <c r="D32" s="13">
         <v>711417.39193010493</v>
@@ -2891,7 +2894,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="13">
-        <v>715771.78446201445</v>
+        <v>715781.4799168685</v>
       </c>
       <c r="D33" s="13">
         <v>703050.45640799252</v>
@@ -2905,7 +2908,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="13">
-        <v>708015.47620610939</v>
+        <v>708078.06134200457</v>
       </c>
       <c r="D34" s="13">
         <v>672685.99363050424</v>
@@ -2919,7 +2922,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="13">
-        <v>683363.36592014041</v>
+        <v>683459.32064082299</v>
       </c>
       <c r="D35" s="13">
         <v>730838.27259277587</v>
@@ -2933,7 +2936,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="13">
-        <v>705154.06936352607</v>
+        <v>705124.75367552775</v>
       </c>
       <c r="D36" s="13">
         <v>703461.65253019624</v>
@@ -2947,7 +2950,7 @@
         <v>30</v>
       </c>
       <c r="C37" s="13">
-        <v>717411.04634602205</v>
+        <v>717281.82217744179</v>
       </c>
       <c r="D37" s="13">
         <v>706958.03908231878</v>
@@ -2961,7 +2964,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="13">
-        <v>716256.44662174792</v>
+        <v>717239.15360811248</v>
       </c>
       <c r="D38" s="13">
         <v>677085.52917315089</v>
@@ -2975,7 +2978,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="13">
-        <v>721021.13494934991</v>
+        <v>720685.01098355697</v>
       </c>
       <c r="D39" s="13">
         <v>776486.60279942001</v>
@@ -2989,7 +2992,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="13">
-        <v>725695.4215217717</v>
+        <v>725384.14728916402</v>
       </c>
       <c r="D40" s="13">
         <v>721458.94421618234</v>
@@ -3003,7 +3006,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="13">
-        <v>718655.41811838944</v>
+        <v>718320.1093304262</v>
       </c>
       <c r="D41" s="13">
         <v>706597.3450225069</v>
@@ -3017,7 +3020,7 @@
         <v>27</v>
       </c>
       <c r="C42" s="13">
-        <v>707735.35421217524</v>
+        <v>707643.75498086831</v>
       </c>
       <c r="D42" s="13">
         <v>671066.04663506267</v>
@@ -3031,7 +3034,7 @@
         <v>28</v>
       </c>
       <c r="C43" s="13">
-        <v>703067.06032733177</v>
+        <v>703081.73838811077</v>
       </c>
       <c r="D43" s="13">
         <v>760576.86834800406</v>
@@ -3045,7 +3048,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="13">
-        <v>697385.00183770189</v>
+        <v>697440.75014498399</v>
       </c>
       <c r="D44" s="13">
         <v>690879.79825168336</v>
@@ -3059,7 +3062,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="13">
-        <v>701036.76747625391</v>
+        <v>701057.94033949706</v>
       </c>
       <c r="D45" s="13">
         <v>686701.4706187105</v>
@@ -3073,7 +3076,7 @@
         <v>27</v>
       </c>
       <c r="C46" s="13">
-        <v>711582.18940482533</v>
+        <v>711623.61102894158</v>
       </c>
       <c r="D46" s="13">
         <v>672749.81139169924</v>
@@ -3087,7 +3090,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="13">
-        <v>727761.09033965564</v>
+        <v>727716.46790551464</v>
       </c>
       <c r="D47" s="13">
         <v>791235.96554167022</v>
@@ -3101,7 +3104,7 @@
         <v>29</v>
       </c>
       <c r="C48" s="13">
-        <v>727254.70071660064</v>
+        <v>727288.65197496035</v>
       </c>
       <c r="D48" s="13">
         <v>718281.26544978167</v>
@@ -3115,7 +3118,7 @@
         <v>30</v>
       </c>
       <c r="C49" s="13">
-        <v>719350.60609107849</v>
+        <v>719319.85564274376</v>
       </c>
       <c r="D49" s="13">
         <v>703681.54416900803</v>
@@ -3129,7 +3132,7 @@
         <v>27</v>
       </c>
       <c r="C50" s="13">
-        <v>713366.05270365754</v>
+        <v>713343.55352433119</v>
       </c>
       <c r="D50" s="13">
         <v>677652.08911570266</v>
@@ -3143,7 +3146,7 @@
         <v>28</v>
       </c>
       <c r="C51" s="13">
-        <v>700905.07564341312</v>
+        <v>700876.98894771049</v>
       </c>
       <c r="D51" s="13">
         <v>760703.28015165636</v>
@@ -3157,7 +3160,7 @@
         <v>29</v>
       </c>
       <c r="C52" s="13">
-        <v>703426.86159018159</v>
+        <v>703503.3059038705</v>
       </c>
       <c r="D52" s="13">
         <v>694382.47577623045</v>
@@ -3171,7 +3174,7 @@
         <v>30</v>
       </c>
       <c r="C53" s="13">
-        <v>708213.40445339365</v>
+        <v>708187.54601473617</v>
       </c>
       <c r="D53" s="13">
         <v>693173.54934705782</v>
@@ -3185,7 +3188,7 @@
         <v>27</v>
       </c>
       <c r="C54" s="13">
-        <v>715597.31010988436</v>
+        <v>715541.12430242822</v>
       </c>
       <c r="D54" s="13">
         <v>681444.76611022244</v>
@@ -3199,7 +3202,7 @@
         <v>28</v>
       </c>
       <c r="C55" s="13">
-        <v>720796.54414836504</v>
+        <v>720864.54544404813</v>
       </c>
       <c r="D55" s="13">
         <v>778401.67644931667</v>
@@ -3213,7 +3216,7 @@
         <v>29</v>
       </c>
       <c r="C56" s="13">
-        <v>730363.31705270614</v>
+        <v>730409.70809090615</v>
       </c>
       <c r="D56" s="13">
         <v>721120.42685279413</v>
@@ -3227,7 +3230,7 @@
         <v>30</v>
       </c>
       <c r="C57" s="13">
-        <v>738802.61974034144</v>
+        <v>738744.41321391251</v>
       </c>
       <c r="D57" s="13">
         <v>724592.92163896293</v>
@@ -3241,7 +3244,7 @@
         <v>27</v>
       </c>
       <c r="C58" s="13">
-        <v>737939.9250553248</v>
+        <v>738063.50607312412</v>
       </c>
       <c r="D58" s="13">
         <v>707231.01699200924</v>
@@ -3255,7 +3258,7 @@
         <v>28</v>
       </c>
       <c r="C59" s="13">
-        <v>700406.75563108665</v>
+        <v>700381.81266289623</v>
       </c>
       <c r="D59" s="13">
         <v>747420.07441892265</v>
@@ -3269,7 +3272,7 @@
         <v>29</v>
       </c>
       <c r="C60" s="13">
-        <v>699939.38850586105</v>
+        <v>699912.37833407056</v>
       </c>
       <c r="D60" s="13">
         <v>696471.25579377101</v>
@@ -3283,7 +3286,7 @@
         <v>30</v>
       </c>
       <c r="C61" s="13">
-        <v>692735.88922230015</v>
+        <v>692664.26134448207</v>
       </c>
       <c r="D61" s="13">
         <v>679899.61120987148</v>
@@ -3297,7 +3300,7 @@
         <v>27</v>
       </c>
       <c r="C62" s="13">
-        <v>693692.82113442535</v>
+        <v>693888.02579630702</v>
       </c>
       <c r="D62" s="13">
         <v>665471.48418794025</v>
@@ -3311,7 +3314,7 @@
         <v>28</v>
       </c>
       <c r="C63" s="13">
-        <v>691076.98633239197</v>
+        <v>690911.4545944538</v>
       </c>
       <c r="D63" s="13">
         <v>750203.91624211951</v>
@@ -3325,7 +3328,7 @@
         <v>29</v>
       </c>
       <c r="C64" s="13">
-        <v>696715.27710983693</v>
+        <v>696760.17457923503</v>
       </c>
       <c r="D64" s="13">
         <v>683792.55791734927</v>
@@ -3339,7 +3342,7 @@
         <v>30</v>
       </c>
       <c r="C65" s="13">
-        <v>690424.7181702106</v>
+        <v>690350.14788672794</v>
       </c>
       <c r="D65" s="12">
         <v>672441.84078677045</v>
@@ -3353,10 +3356,24 @@
         <v>27</v>
       </c>
       <c r="C66" s="12">
-        <v>656978.78374522761</v>
+        <v>661654.94892247976</v>
       </c>
       <c r="D66" s="12">
-        <v>629398.33221060247</v>
+        <v>630971.49375148444</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="26">
+        <v>2020</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="12">
+        <v>554316.13938229729</v>
+      </c>
+      <c r="D67">
+        <v>606992.80173888081</v>
       </c>
     </row>
   </sheetData>
@@ -3382,14 +3399,14 @@
       <c r="A1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -3985,14 +4002,14 @@
       <c r="A1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4457,8 +4474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4483,10 +4500,10 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>522595</v>
+        <v>512359.57668351842</v>
       </c>
       <c r="C2">
-        <v>-5.0999999999999996</v>
+        <v>-19.367085851183731</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4494,10 +4511,10 @@
         <v>101</v>
       </c>
       <c r="B3">
-        <v>37895</v>
+        <v>92004.645068881611</v>
       </c>
       <c r="C3">
-        <v>-6.2</v>
+        <v>-10.662776074013092</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4505,10 +4522,10 @@
         <v>102</v>
       </c>
       <c r="B4">
-        <v>1578</v>
+        <v>1762.0229144674997</v>
       </c>
       <c r="C4">
-        <v>-30.4</v>
+        <v>-14.012780295759219</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4516,10 +4533,10 @@
         <v>103</v>
       </c>
       <c r="B5">
-        <v>20975</v>
+        <v>17786.684208885996</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>-18.257336008282532</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4527,10 +4544,10 @@
         <v>104</v>
       </c>
       <c r="B6">
-        <v>92632</v>
+        <v>87855.640061666243</v>
       </c>
       <c r="C6">
-        <v>-6.5</v>
+        <v>-20.78211950432992</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4538,10 +4555,10 @@
         <v>105</v>
       </c>
       <c r="B7">
-        <v>1267</v>
+        <v>11444.28144229284</v>
       </c>
       <c r="C7">
-        <v>3.8</v>
+        <v>-3.322617578802578</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4549,10 +4566,10 @@
         <v>106</v>
       </c>
       <c r="B8">
-        <v>17239</v>
+        <v>10168.960336140055</v>
       </c>
       <c r="C8">
-        <v>-20.8</v>
+        <v>-52.061712371385013</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4560,10 +4577,10 @@
         <v>107</v>
       </c>
       <c r="B9">
-        <v>7634</v>
+        <v>71161.53514765836</v>
       </c>
       <c r="C9">
-        <v>-6.5</v>
+        <v>-16.915809495210297</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4571,10 +4588,10 @@
         <v>108</v>
       </c>
       <c r="B10">
-        <v>10353</v>
+        <v>2846.6104571211044</v>
       </c>
       <c r="C10">
-        <v>-10.199999999999999</v>
+        <v>-73.358743089924516</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4582,10 +4599,10 @@
         <v>109</v>
       </c>
       <c r="B11">
-        <v>52738</v>
+        <v>45942.355822993144</v>
       </c>
       <c r="C11">
-        <v>-5.4</v>
+        <v>-22.455757918651422</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4593,10 +4610,10 @@
         <v>110</v>
       </c>
       <c r="B12">
-        <v>24704</v>
+        <v>24870.172648461972</v>
       </c>
       <c r="C12">
-        <v>-5.9</v>
+        <v>-1.2002304258781127</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4604,10 +4621,10 @@
         <v>111</v>
       </c>
       <c r="B13">
-        <v>71147</v>
+        <v>64522.940872450235</v>
       </c>
       <c r="C13">
-        <v>-2</v>
+        <v>-14.315387598774443</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4615,10 +4632,10 @@
         <v>117</v>
       </c>
       <c r="B14">
-        <v>33142</v>
+        <v>28996.867587962621</v>
       </c>
       <c r="C14">
-        <v>0.2</v>
+        <v>-12.799845828932533</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4626,10 +4643,10 @@
         <v>112</v>
       </c>
       <c r="B15">
-        <v>27302</v>
+        <v>25007.616698329046</v>
       </c>
       <c r="C15">
-        <v>1.2</v>
+        <v>-9.2094014857966862</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4637,10 +4654,10 @@
         <v>113</v>
       </c>
       <c r="B16">
-        <v>22567</v>
+        <v>19525.683527571011</v>
       </c>
       <c r="C16">
-        <v>-3.7</v>
+        <v>-23.468530609699613</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4648,10 +4665,10 @@
         <v>114</v>
       </c>
       <c r="B17">
-        <v>16874</v>
+        <v>5830.5199163868256</v>
       </c>
       <c r="C17">
-        <v>-7.2</v>
+        <v>-67.712814571577965</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4659,10 +4676,10 @@
         <v>115</v>
       </c>
       <c r="B18">
-        <v>4438</v>
+        <v>2633.0399722498255</v>
       </c>
       <c r="C18">
-        <v>-2.6</v>
+        <v>-38.021339999999981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos de comercio exterior, resultado fiscal y Emae"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -568,11 +568,13 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2051,7 +2053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
@@ -2432,7 +2434,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3401,14 +3403,14 @@
       <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="38"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -3568,7 +3570,7 @@
       <c r="B11" s="25">
         <v>39.299999999999997</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="36">
         <v>48.7</v>
       </c>
       <c r="D11" s="25">
@@ -4012,14 +4014,14 @@
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="38"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4167,8 +4169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4195,14 +4197,14 @@
         <v>77</v>
       </c>
       <c r="B2" s="16">
-        <v>5950</v>
+        <v>6909</v>
       </c>
       <c r="C2">
-        <v>6997</v>
+        <v>8187</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>-1047</v>
+        <v>-1278</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4210,14 +4212,14 @@
         <v>78</v>
       </c>
       <c r="B3" s="16">
-        <v>1914</v>
+        <v>2170</v>
       </c>
       <c r="C3">
-        <v>313</v>
+        <v>368</v>
       </c>
       <c r="D3" s="16">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
-        <v>1601</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4225,14 +4227,14 @@
         <v>79</v>
       </c>
       <c r="B4" s="16">
-        <v>1997</v>
+        <v>2293</v>
       </c>
       <c r="C4">
-        <v>1102</v>
+        <v>1249</v>
       </c>
       <c r="D4" s="16">
         <f t="shared" si="0"/>
-        <v>895</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4240,14 +4242,14 @@
         <v>80</v>
       </c>
       <c r="B5" s="16">
-        <v>371</v>
+        <v>450</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>356</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4255,14 +4257,14 @@
         <v>81</v>
       </c>
       <c r="B6" s="16">
-        <v>2803</v>
+        <v>3163</v>
       </c>
       <c r="C6">
-        <v>3679</v>
+        <v>4125</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>-876</v>
+        <v>-962</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4270,14 +4272,14 @@
         <v>82</v>
       </c>
       <c r="B7" s="16">
-        <v>4358</v>
+        <v>5116</v>
       </c>
       <c r="C7">
-        <v>4168</v>
+        <v>4773</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="16" customFormat="1">
@@ -4285,14 +4287,14 @@
         <v>95</v>
       </c>
       <c r="B8" s="16">
-        <v>381</v>
+        <v>430</v>
       </c>
       <c r="C8" s="16">
-        <v>212</v>
+        <v>263</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4300,14 +4302,14 @@
         <v>83</v>
       </c>
       <c r="B9" s="16">
-        <v>741</v>
+        <v>818</v>
       </c>
       <c r="C9">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>464</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4315,14 +4317,14 @@
         <v>84</v>
       </c>
       <c r="B10" s="16">
-        <v>502</v>
+        <v>548</v>
       </c>
       <c r="C10">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
-        <v>383</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4330,14 +4332,14 @@
         <v>85</v>
       </c>
       <c r="B11" s="16">
-        <v>4365</v>
+        <v>4794</v>
       </c>
       <c r="C11">
-        <v>1531</v>
+        <v>1741</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>2834</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4345,14 +4347,14 @@
         <v>86</v>
       </c>
       <c r="B12" s="16">
-        <v>4016</v>
+        <v>4318</v>
       </c>
       <c r="C12">
-        <v>5049</v>
+        <v>5939</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>-1033</v>
+        <v>-1621</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4360,14 +4362,14 @@
         <v>87</v>
       </c>
       <c r="B13" s="16">
-        <v>472</v>
+        <v>568</v>
       </c>
       <c r="C13">
-        <v>236</v>
+        <v>265</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4375,14 +4377,14 @@
         <v>88</v>
       </c>
       <c r="B14" s="16">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="C14">
-        <v>449</v>
+        <v>521</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>-259</v>
+        <v>-300</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4390,14 +4392,14 @@
         <v>89</v>
       </c>
       <c r="B15" s="16">
-        <v>1664</v>
+        <v>1861</v>
       </c>
       <c r="C15">
-        <v>512</v>
+        <v>613</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="0"/>
-        <v>1152</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4405,14 +4407,14 @@
         <v>90</v>
       </c>
       <c r="B16" s="16">
-        <v>2229</v>
+        <v>2488</v>
       </c>
       <c r="C16">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4420,14 +4422,14 @@
         <v>91</v>
       </c>
       <c r="B17" s="16">
-        <v>2282</v>
+        <v>2494</v>
       </c>
       <c r="C17">
-        <v>288</v>
+        <v>371</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
-        <v>1994</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4435,14 +4437,14 @@
         <v>92</v>
       </c>
       <c r="B18" s="16">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="C18">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
-        <v>161</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4450,14 +4452,14 @@
         <v>93</v>
       </c>
       <c r="B19" s="16">
-        <v>435</v>
+        <v>493</v>
       </c>
       <c r="C19">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4465,14 +4467,14 @@
         <v>94</v>
       </c>
       <c r="B20" s="16">
-        <v>2334</v>
+        <v>2542</v>
       </c>
       <c r="C20">
-        <v>800</v>
+        <v>943</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
-        <v>1534</v>
+        <v>1599</v>
       </c>
     </row>
   </sheetData>
@@ -4699,10 +4701,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5461,39 +5463,53 @@
       <c r="B54" s="35">
         <v>130.13225514839269</v>
       </c>
-      <c r="C54" s="35">
-        <v>114.72899046127216</v>
-      </c>
-      <c r="D54" s="35">
-        <v>140.3510371312704</v>
+      <c r="C54" s="39">
+        <v>114.73360798359479</v>
+      </c>
+      <c r="D54" s="39">
+        <v>140.34891097987008</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="34">
         <v>43983</v>
       </c>
-      <c r="B55" s="35">
-        <v>133.58364281124869</v>
-      </c>
-      <c r="C55" s="35">
-        <v>123.30795437489482</v>
-      </c>
-      <c r="D55" s="35">
-        <v>140.22560266513267</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="25" customFormat="1">
-      <c r="A56" s="21">
+      <c r="B55" s="39">
+        <v>133.52620730377282</v>
+      </c>
+      <c r="C55" s="39">
+        <v>123.25271683159407</v>
+      </c>
+      <c r="D55" s="39">
+        <v>140.22372337296835</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="38" customFormat="1">
+      <c r="A56" s="34">
         <v>44013</v>
       </c>
-      <c r="B56" s="36">
-        <v>126.86534109692857</v>
-      </c>
-      <c r="C56" s="36">
-        <v>124.6261665150967</v>
-      </c>
-      <c r="D56" s="36">
-        <v>140.23476944254631</v>
+      <c r="B56" s="39">
+        <v>126.9829202465486</v>
+      </c>
+      <c r="C56" s="39">
+        <v>124.78864869025028</v>
+      </c>
+      <c r="D56" s="39">
+        <v>140.12676343211612</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="21">
+        <v>44044</v>
+      </c>
+      <c r="B57" s="40">
+        <v>125.11192759501449</v>
+      </c>
+      <c r="C57" s="40">
+        <v>127.15005964981405</v>
+      </c>
+      <c r="D57" s="40">
+        <v>140.05265261624049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando EMAE e ICA"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -2070,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
@@ -4186,8 +4186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4214,14 +4214,14 @@
         <v>77</v>
       </c>
       <c r="B2" s="16">
-        <v>6909</v>
+        <v>7830</v>
       </c>
       <c r="C2">
-        <v>8187</v>
+        <v>9317</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>-1278</v>
+        <v>-1487</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4229,14 +4229,14 @@
         <v>78</v>
       </c>
       <c r="B3" s="16">
-        <v>2170</v>
+        <v>2422</v>
       </c>
       <c r="C3">
-        <v>368</v>
+        <v>426</v>
       </c>
       <c r="D3" s="16">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
-        <v>1802</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4244,14 +4244,14 @@
         <v>79</v>
       </c>
       <c r="B4" s="16">
-        <v>2293</v>
+        <v>2560</v>
       </c>
       <c r="C4">
-        <v>1249</v>
+        <v>1384</v>
       </c>
       <c r="D4" s="16">
         <f t="shared" si="0"/>
-        <v>1044</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4259,14 +4259,14 @@
         <v>80</v>
       </c>
       <c r="B5" s="16">
-        <v>450</v>
+        <v>488</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>432</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4274,14 +4274,14 @@
         <v>81</v>
       </c>
       <c r="B6" s="16">
-        <v>3163</v>
+        <v>3507</v>
       </c>
       <c r="C6">
-        <v>4125</v>
+        <v>4611</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>-962</v>
+        <v>-1104</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4289,14 +4289,14 @@
         <v>82</v>
       </c>
       <c r="B7" s="16">
-        <v>5116</v>
+        <v>5782</v>
       </c>
       <c r="C7">
-        <v>4773</v>
+        <v>5360</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>343</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="16" customFormat="1">
@@ -4304,14 +4304,14 @@
         <v>95</v>
       </c>
       <c r="B8" s="16">
-        <v>430</v>
+        <v>503</v>
       </c>
       <c r="C8" s="16">
-        <v>263</v>
+        <v>295</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>167</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4319,14 +4319,14 @@
         <v>83</v>
       </c>
       <c r="B9" s="16">
-        <v>818</v>
+        <v>895</v>
       </c>
       <c r="C9">
-        <v>316</v>
+        <v>358</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>502</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4334,14 +4334,14 @@
         <v>84</v>
       </c>
       <c r="B10" s="16">
-        <v>548</v>
+        <v>605</v>
       </c>
       <c r="C10">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4349,14 +4349,14 @@
         <v>85</v>
       </c>
       <c r="B11" s="16">
-        <v>4794</v>
+        <v>5180</v>
       </c>
       <c r="C11">
-        <v>1741</v>
+        <v>2003</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>3053</v>
+        <v>3177</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4364,14 +4364,14 @@
         <v>86</v>
       </c>
       <c r="B12" s="16">
-        <v>4318</v>
+        <v>4750</v>
       </c>
       <c r="C12">
-        <v>5939</v>
+        <v>6798</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>-1621</v>
+        <v>-2048</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4379,14 +4379,14 @@
         <v>87</v>
       </c>
       <c r="B13" s="16">
-        <v>568</v>
+        <v>646</v>
       </c>
       <c r="C13">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="0"/>
-        <v>303</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4394,14 +4394,14 @@
         <v>88</v>
       </c>
       <c r="B14" s="16">
-        <v>221</v>
+        <v>265</v>
       </c>
       <c r="C14">
-        <v>521</v>
+        <v>580</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>-300</v>
+        <v>-315</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4409,14 +4409,14 @@
         <v>89</v>
       </c>
       <c r="B15" s="16">
-        <v>1861</v>
+        <v>2118</v>
       </c>
       <c r="C15">
-        <v>613</v>
+        <v>676</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="0"/>
-        <v>1248</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4424,14 +4424,14 @@
         <v>90</v>
       </c>
       <c r="B16" s="16">
-        <v>2488</v>
+        <v>2694</v>
       </c>
       <c r="C16">
-        <v>368</v>
+        <v>399</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="0"/>
-        <v>2120</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4439,14 +4439,14 @@
         <v>91</v>
       </c>
       <c r="B17" s="16">
-        <v>2494</v>
+        <v>2665</v>
       </c>
       <c r="C17">
-        <v>371</v>
+        <v>434</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
-        <v>2123</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4454,14 +4454,14 @@
         <v>92</v>
       </c>
       <c r="B18" s="16">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="C18">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4469,14 +4469,14 @@
         <v>93</v>
       </c>
       <c r="B19" s="16">
-        <v>493</v>
+        <v>581</v>
       </c>
       <c r="C19">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
-        <v>386</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4484,14 +4484,14 @@
         <v>94</v>
       </c>
       <c r="B20" s="16">
-        <v>2542</v>
+        <v>2785</v>
       </c>
       <c r="C20">
-        <v>943</v>
+        <v>1057</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
-        <v>1599</v>
+        <v>1728</v>
       </c>
     </row>
   </sheetData>
@@ -4718,10 +4718,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4921,10 +4921,10 @@
         <v>136.7258774086435</v>
       </c>
       <c r="C14" s="20">
-        <v>147.61405239987857</v>
+        <v>147.6</v>
       </c>
       <c r="D14" s="20">
-        <v>146.61657419760434</v>
+        <v>146.80000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4935,10 +4935,10 @@
         <v>132.54052520440143</v>
       </c>
       <c r="C15" s="20">
-        <v>146.80840714667116</v>
+        <v>146.5</v>
       </c>
       <c r="D15" s="20">
-        <v>147.18068897228747</v>
+        <v>147.30000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4949,10 +4949,10 @@
         <v>152.145731768997</v>
       </c>
       <c r="C16" s="20">
-        <v>148.07519627379236</v>
+        <v>148.4</v>
       </c>
       <c r="D16" s="20">
-        <v>147.78581762528452</v>
+        <v>147.80000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4963,10 +4963,10 @@
         <v>152.20883250679566</v>
       </c>
       <c r="C17" s="20">
-        <v>147.65382778205736</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="D17" s="20">
-        <v>148.41248070650221</v>
+        <v>148.4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4977,10 +4977,10 @@
         <v>167.46154818637638</v>
       </c>
       <c r="C18" s="20">
-        <v>148.27602945341309</v>
+        <v>148.6</v>
       </c>
       <c r="D18" s="20">
-        <v>149.03726903893946</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4991,10 +4991,10 @@
         <v>161.70085905013559</v>
       </c>
       <c r="C19" s="20">
-        <v>149.85985638237861</v>
+        <v>150.19999999999999</v>
       </c>
       <c r="D19" s="20">
-        <v>149.6299106659998</v>
+        <v>149.6</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5005,10 +5005,10 @@
         <v>149.78297310853262</v>
       </c>
       <c r="C20" s="20">
-        <v>149.99771584335744</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="D20" s="20">
-        <v>150.15534093554578</v>
+        <v>150.1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5019,10 +5019,10 @@
         <v>149.4590923353316</v>
       </c>
       <c r="C21" s="20">
-        <v>149.93734112861281</v>
+        <v>150.5</v>
       </c>
       <c r="D21" s="20">
-        <v>150.57598699101979</v>
+        <v>150.5</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5033,10 +5033,10 @@
         <v>146.70588711165021</v>
       </c>
       <c r="C22" s="20">
-        <v>151.75747869191821</v>
+        <v>151.4</v>
       </c>
       <c r="D22" s="20">
-        <v>150.8555392336381</v>
+        <v>150.80000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5047,10 +5047,10 @@
         <v>149.62906247744323</v>
       </c>
       <c r="C23" s="20">
-        <v>151.42353157286692</v>
+        <v>151.1</v>
       </c>
       <c r="D23" s="20">
-        <v>150.96333628180651</v>
+        <v>150.9</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5061,10 +5061,10 @@
         <v>152.38283025725997</v>
       </c>
       <c r="C24" s="20">
-        <v>153.05967068973709</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="D24" s="20">
-        <v>150.87607723057013</v>
+        <v>150.9</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5075,10 +5075,10 @@
         <v>146.08348469256237</v>
       </c>
       <c r="C25" s="20">
-        <v>152.36359699262178</v>
+        <v>152.4</v>
       </c>
       <c r="D25" s="20">
-        <v>150.58322064649997</v>
+        <v>150.6</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5089,10 +5089,10 @@
         <v>142.64696239584413</v>
       </c>
       <c r="C26" s="20">
-        <v>152.18718012229664</v>
+        <v>152.5</v>
       </c>
       <c r="D26" s="20">
-        <v>150.09380330106256</v>
+        <v>150.19999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5103,10 +5103,10 @@
         <v>139.07181989111268</v>
       </c>
       <c r="C27" s="20">
-        <v>152.14740308563989</v>
+        <v>151.9</v>
       </c>
       <c r="D27" s="20">
-        <v>149.43107896008593</v>
+        <v>149.5</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5117,10 +5117,10 @@
         <v>155.63982283229944</v>
       </c>
       <c r="C28" s="20">
-        <v>152.0911330688333</v>
+        <v>152</v>
       </c>
       <c r="D28" s="20">
-        <v>148.63061866008715</v>
+        <v>148.69999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5131,10 +5131,10 @@
         <v>151.60135644382305</v>
       </c>
       <c r="C29" s="20">
-        <v>146.97102238315017</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="D29" s="20">
-        <v>147.73838474507906</v>
+        <v>147.9</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5145,10 +5145,10 @@
         <v>159.16207548226589</v>
       </c>
       <c r="C30" s="20">
-        <v>143.86439552450364</v>
+        <v>144.30000000000001</v>
       </c>
       <c r="D30" s="20">
-        <v>146.80738436414754</v>
+        <v>146.9</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5159,10 +5159,10 @@
         <v>151.44848091721315</v>
       </c>
       <c r="C31" s="20">
-        <v>142.28757369118409</v>
+        <v>142.4</v>
       </c>
       <c r="D31" s="20">
-        <v>145.89161546626929</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5173,10 +5173,10 @@
         <v>145.76463042864052</v>
       </c>
       <c r="C32" s="20">
-        <v>143.1735202789892</v>
+        <v>143.5</v>
       </c>
       <c r="D32" s="20">
-        <v>145.03881329250115</v>
+        <v>145.1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5187,10 +5187,10 @@
         <v>147.04553382400547</v>
       </c>
       <c r="C33" s="20">
-        <v>145.89114386993973</v>
+        <v>146.9</v>
       </c>
       <c r="D33" s="20">
-        <v>144.2864377931854</v>
+        <v>144.30000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5201,10 +5201,10 @@
         <v>137.8944988928931</v>
       </c>
       <c r="C34" s="20">
-        <v>143.76802317308389</v>
+        <v>142.5</v>
       </c>
       <c r="D34" s="20">
-        <v>143.65811682428125</v>
+        <v>143.69999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5215,10 +5215,10 @@
         <v>143.57320349337792</v>
       </c>
       <c r="C35" s="20">
-        <v>143.61958694114858</v>
+        <v>143.69999999999999</v>
       </c>
       <c r="D35" s="20">
-        <v>143.16783236739641</v>
+        <v>143.19999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5229,10 +5229,10 @@
         <v>141.21184890028576</v>
       </c>
       <c r="C36" s="20">
-        <v>142.21755105909986</v>
+        <v>142.30000000000001</v>
       </c>
       <c r="D36" s="20">
-        <v>142.81685029466342</v>
+        <v>142.9</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5243,10 +5243,10 @@
         <v>135.67154302632184</v>
       </c>
       <c r="C37" s="20">
-        <v>142.5132435730055</v>
+        <v>142</v>
       </c>
       <c r="D37" s="20">
-        <v>142.59342708728775</v>
+        <v>142.69999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5254,13 +5254,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="20">
-        <v>134.54499531326459</v>
+        <v>134.564995313265</v>
       </c>
       <c r="C38" s="20">
-        <v>143.29029549921839</v>
+        <v>143.69999999999999</v>
       </c>
       <c r="D38" s="20">
-        <v>142.47581458693261</v>
+        <v>142.6</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5271,10 +5271,10 @@
         <v>132.57194718265788</v>
       </c>
       <c r="C39" s="20">
-        <v>143.63578779494426</v>
+        <v>143.6</v>
       </c>
       <c r="D39" s="20">
-        <v>142.43623735552936</v>
+        <v>142.6</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5285,10 +5285,10 @@
         <v>144.41715750575651</v>
       </c>
       <c r="C40" s="20">
-        <v>142.18108049588707</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="D40" s="20">
-        <v>142.44518190407581</v>
+        <v>142.69999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5299,10 +5299,10 @@
         <v>149.83961931661509</v>
       </c>
       <c r="C41" s="20">
-        <v>142.26821474744145</v>
+        <v>142.30000000000001</v>
       </c>
       <c r="D41" s="20">
-        <v>142.47270600477859</v>
+        <v>142.80000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5313,10 +5313,10 @@
         <v>162.83974753189364</v>
       </c>
       <c r="C42" s="20">
-        <v>142.6905744166057</v>
+        <v>143.4</v>
       </c>
       <c r="D42" s="20">
-        <v>142.49064342229983</v>
+        <v>142.80000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5327,10 +5327,10 @@
         <v>151.25410111244764</v>
       </c>
       <c r="C43" s="20">
-        <v>142.30764129197613</v>
+        <v>141.9</v>
       </c>
       <c r="D43" s="20">
-        <v>142.47509654077692</v>
+        <v>142.80000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5341,10 +5341,10 @@
         <v>146.20323233619627</v>
       </c>
       <c r="C44" s="20">
-        <v>144.73761547036995</v>
+        <v>145.6</v>
       </c>
       <c r="D44" s="20">
-        <v>142.40857787309338</v>
+        <v>142.80000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5355,10 +5355,10 @@
         <v>141.60332874981128</v>
       </c>
       <c r="C45" s="20">
-        <v>143.86829469760013</v>
+        <v>144.69999999999999</v>
       </c>
       <c r="D45" s="20">
-        <v>142.28142802411494</v>
+        <v>142.6</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -5369,10 +5369,10 @@
         <v>135.0574708022306</v>
       </c>
       <c r="C46" s="20">
-        <v>142.27742307242687</v>
+        <v>140.80000000000001</v>
       </c>
       <c r="D46" s="20">
-        <v>142.09237518880394</v>
+        <v>142.4</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -5383,10 +5383,10 @@
         <v>142.24064825618933</v>
       </c>
       <c r="C47" s="20">
-        <v>143.52555021851464</v>
+        <v>143.6</v>
       </c>
       <c r="D47" s="35">
-        <v>141.93310318264281</v>
+        <v>142.1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -5397,10 +5397,10 @@
         <v>138.15855707957144</v>
       </c>
       <c r="C48" s="35">
-        <v>141.73280912224618</v>
+        <v>141.5</v>
       </c>
       <c r="D48" s="35">
-        <v>141.69183244738826</v>
+        <v>141.80000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -5411,10 +5411,10 @@
         <v>135.45406298998449</v>
       </c>
       <c r="C49" s="35">
-        <v>141.63667200198975</v>
+        <v>141.5</v>
       </c>
       <c r="D49" s="35">
-        <v>141.43356712044937</v>
+        <v>141.4</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -5425,10 +5425,10 @@
         <v>132.18766212782253</v>
       </c>
       <c r="C50" s="35">
-        <v>141.45897720759729</v>
+        <v>141.6</v>
       </c>
       <c r="D50" s="35">
-        <v>141.17414817301963</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -5439,10 +5439,10 @@
         <v>129.65346351336271</v>
       </c>
       <c r="C51" s="35">
-        <v>140.98042234137097</v>
+        <v>140.69999999999999</v>
       </c>
       <c r="D51" s="35">
-        <v>140.92679768414803</v>
+        <v>140.6</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -5453,10 +5453,10 @@
         <v>128.35784152357166</v>
       </c>
       <c r="C52" s="35">
-        <v>126.73451762724137</v>
+        <v>125.6</v>
       </c>
       <c r="D52" s="35">
-        <v>140.70283513015883</v>
+        <v>140.19999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5467,10 +5467,10 @@
         <v>111.65441062079474</v>
       </c>
       <c r="C53" s="35">
-        <v>104.7575985650648</v>
+        <v>104.1</v>
       </c>
       <c r="D53" s="35">
-        <v>140.50980458460467</v>
+        <v>139.80000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -5481,10 +5481,10 @@
         <v>130.13225514839269</v>
       </c>
       <c r="C54" s="38">
-        <v>114.73360798359479</v>
+        <v>113.8</v>
       </c>
       <c r="D54" s="38">
-        <v>140.34891097987008</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -5495,10 +5495,10 @@
         <v>133.52620730377282</v>
       </c>
       <c r="C55" s="38">
-        <v>123.25271683159407</v>
+        <v>122.9</v>
       </c>
       <c r="D55" s="38">
-        <v>140.22372337296835</v>
+        <v>139.1</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="37" customFormat="1">
@@ -5506,27 +5506,41 @@
         <v>44013</v>
       </c>
       <c r="B56" s="38">
-        <v>126.9829202465486</v>
+        <v>127.1</v>
       </c>
       <c r="C56" s="38">
-        <v>124.78864869025028</v>
+        <v>126.4</v>
       </c>
       <c r="D56" s="38">
-        <v>140.12676343211612</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="21">
+        <v>138.80000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="37" customFormat="1">
+      <c r="A57" s="34">
         <v>44044</v>
       </c>
-      <c r="B57" s="39">
-        <v>125.11192759501449</v>
-      </c>
-      <c r="C57" s="39">
-        <v>127.15005964981405</v>
-      </c>
-      <c r="D57" s="39">
-        <v>140.05265261624049</v>
+      <c r="B57" s="38">
+        <v>124.8</v>
+      </c>
+      <c r="C57" s="38">
+        <v>128.4</v>
+      </c>
+      <c r="D57" s="38">
+        <v>138.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="21">
+        <v>44075</v>
+      </c>
+      <c r="B58" s="39">
+        <v>125.7</v>
+      </c>
+      <c r="C58" s="39">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="D58" s="39">
+        <v>138.19999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
" PIB y VAB, tercer trimestre 2020"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="122">
   <si>
     <t>Período</t>
   </si>
@@ -513,7 +513,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -572,6 +572,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2087,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
@@ -2465,10 +2468,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2498,7 +2501,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="13">
-        <v>475540.07912460313</v>
+        <v>475650.85780757037</v>
       </c>
       <c r="D2" s="13">
         <v>460369.44223294873</v>
@@ -2512,7 +2515,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="13">
-        <v>470121.1274420924</v>
+        <v>470200.6020889256</v>
       </c>
       <c r="D3" s="13">
         <v>514395.68177236168</v>
@@ -2526,7 +2529,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="13">
-        <v>493832.66195269296</v>
+        <v>493615.70822853385</v>
       </c>
       <c r="D4" s="13">
         <v>481151.97994350811</v>
@@ -2540,7 +2543,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="13">
-        <v>500966.91203686345</v>
+        <v>500993.61242462596</v>
       </c>
       <c r="D5" s="13">
         <v>484543.6768765623</v>
@@ -2554,7 +2557,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="13">
-        <v>515472.67133145465</v>
+        <v>515571.86750064709</v>
       </c>
       <c r="D6" s="13">
         <v>493602.53057785495</v>
@@ -2568,7 +2571,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="13">
-        <v>526263.57981290342</v>
+        <v>526332.56309259648</v>
       </c>
       <c r="D7" s="13">
         <v>581668.24987960246</v>
@@ -2582,7 +2585,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="13">
-        <v>530051.55276184448</v>
+        <v>529869.68276198057</v>
       </c>
       <c r="D8" s="13">
         <v>514697.78950542817</v>
@@ -2596,7 +2599,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="13">
-        <v>540435.96610745403</v>
+        <v>540449.6566584328</v>
       </c>
       <c r="D9" s="13">
         <v>522255.20005077147</v>
@@ -2610,7 +2613,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="13">
-        <v>554527.00541241898</v>
+        <v>554621.45968089125</v>
       </c>
       <c r="D10" s="13">
         <v>532348.2120169173</v>
@@ -2624,7 +2627,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="13">
-        <v>561248.73864931497</v>
+        <v>561313.52972680668</v>
       </c>
       <c r="D11" s="13">
         <v>614076.39260854386</v>
@@ -2638,7 +2641,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="13">
-        <v>576963.188307025</v>
+        <v>576793.43266781571</v>
       </c>
       <c r="D12" s="13">
         <v>562978.96562687657</v>
@@ -2652,7 +2655,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="13">
-        <v>589458.68451416725</v>
+        <v>589469.19480741315</v>
       </c>
       <c r="D13" s="13">
         <v>572794.04663058836</v>
@@ -2666,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="13">
-        <v>603178.72917975707</v>
+        <v>603251.2892408435</v>
       </c>
       <c r="D14" s="13">
         <v>576846.88569942722</v>
@@ -2680,7 +2683,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="13">
-        <v>616364.16815246514</v>
+        <v>616403.66103707801</v>
       </c>
       <c r="D15" s="13">
         <v>674620.56300648488</v>
@@ -2694,7 +2697,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="13">
-        <v>624543.47956237034</v>
+        <v>624390.51247672434</v>
       </c>
       <c r="D16" s="13">
         <v>610425.69401485357</v>
@@ -2708,7 +2711,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="13">
-        <v>643683.63368976943</v>
+        <v>643724.54782971786</v>
       </c>
       <c r="D17" s="13">
         <v>625876.86786359688</v>
@@ -2722,7 +2725,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="13">
-        <v>649543.926967607</v>
+        <v>649595.94319119561</v>
       </c>
       <c r="D18" s="13">
         <v>616720.35706447833</v>
@@ -2736,7 +2739,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="13">
-        <v>653526.34668452281</v>
+        <v>653529.69259089709</v>
       </c>
       <c r="D19" s="13">
         <v>711405.50045523292</v>
@@ -2750,7 +2753,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="13">
-        <v>658399.44773779658</v>
+        <v>658314.88608520047</v>
       </c>
       <c r="D20" s="13">
         <v>647087.95974249416</v>
@@ -2764,7 +2767,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="13">
-        <v>627234.91757492337</v>
+        <v>627264.11709755403</v>
       </c>
       <c r="D21" s="13">
         <v>613490.82170264097</v>
@@ -2778,7 +2781,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="13">
-        <v>604302.82642057771</v>
+        <v>604308.14433576947</v>
       </c>
       <c r="D22" s="13">
         <v>578553.04424240452</v>
@@ -2792,7 +2795,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="13">
-        <v>591301.39090571832</v>
+        <v>591333.1456064278</v>
       </c>
       <c r="D23" s="13">
         <v>631197.75186006888</v>
@@ -2806,7 +2809,7 @@
         <v>29</v>
       </c>
       <c r="C24" s="13">
-        <v>614138.8940492504</v>
+        <v>614087.47629341518</v>
       </c>
       <c r="D24" s="13">
         <v>610519.85461172729</v>
@@ -2820,7 +2823,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="13">
-        <v>625748.39427595027</v>
+        <v>625762.7394158867</v>
       </c>
       <c r="D25" s="13">
         <v>615220.85493729718</v>
@@ -2834,7 +2837,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="13">
-        <v>644736.40918322548</v>
+        <v>644741.31149571575</v>
       </c>
       <c r="D26" s="13">
         <v>611607.33658973</v>
@@ -2848,7 +2851,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="13">
-        <v>673861.03054801899</v>
+        <v>673861.97073870804</v>
       </c>
       <c r="D27" s="13">
         <v>733730.77396890335</v>
@@ -2862,7 +2865,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="13">
-        <v>677043.3951807589</v>
+        <v>677026.42470050021</v>
       </c>
       <c r="D28" s="13">
         <v>668566.50948898587</v>
@@ -2876,7 +2879,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="13">
-        <v>686453.88285519055</v>
+        <v>686465.01083226933</v>
       </c>
       <c r="D29" s="13">
         <v>668190.09771957388</v>
@@ -2890,7 +2893,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="13">
-        <v>702907.26087639318</v>
+        <v>702904.08998715342</v>
       </c>
       <c r="D30" s="13">
         <v>662325.58597269515</v>
@@ -2904,7 +2907,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="13">
-        <v>709431.71628614096</v>
+        <v>709435.08224086522</v>
       </c>
       <c r="D31" s="13">
         <v>766332.95457161264</v>
@@ -2918,7 +2921,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="13">
-        <v>715005.9318030047</v>
+        <v>715017.17091026809</v>
       </c>
       <c r="D32" s="13">
         <v>711417.39193010493</v>
@@ -2932,7 +2935,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="13">
-        <v>715781.4799168685</v>
+        <v>715770.04574411944</v>
       </c>
       <c r="D33" s="13">
         <v>703050.45640799252</v>
@@ -2946,7 +2949,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="13">
-        <v>708078.06134200457</v>
+        <v>708074.96464657248</v>
       </c>
       <c r="D34" s="13">
         <v>672685.99363050424</v>
@@ -2960,7 +2963,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="13">
-        <v>683459.32064082299</v>
+        <v>683478.92421364074</v>
       </c>
       <c r="D35" s="13">
         <v>730838.27259277587</v>
@@ -2974,7 +2977,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="13">
-        <v>705124.75367552775</v>
+        <v>705130.92145055346</v>
       </c>
       <c r="D36" s="13">
         <v>703461.65253019624</v>
@@ -2988,7 +2991,7 @@
         <v>30</v>
       </c>
       <c r="C37" s="13">
-        <v>717281.82217744179</v>
+        <v>717259.14752503159</v>
       </c>
       <c r="D37" s="13">
         <v>706958.03908231878</v>
@@ -3002,7 +3005,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="13">
-        <v>717239.15360811248</v>
+        <v>717227.20759437967</v>
       </c>
       <c r="D38" s="13">
         <v>677085.52917315089</v>
@@ -3016,7 +3019,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="13">
-        <v>720685.01098355697</v>
+        <v>720706.50909504655</v>
       </c>
       <c r="D39" s="13">
         <v>776486.60279942001</v>
@@ -3030,7 +3033,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="13">
-        <v>725384.14728916402</v>
+        <v>725405.32342113496</v>
       </c>
       <c r="D40" s="13">
         <v>721458.94421618234</v>
@@ -3044,7 +3047,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="13">
-        <v>718320.1093304262</v>
+        <v>718289.38110069954</v>
       </c>
       <c r="D41" s="13">
         <v>706597.3450225069</v>
@@ -3058,7 +3061,7 @@
         <v>27</v>
       </c>
       <c r="C42" s="13">
-        <v>707643.75498086831</v>
+        <v>707573.6344303838</v>
       </c>
       <c r="D42" s="13">
         <v>671066.04663506267</v>
@@ -3072,7 +3075,7 @@
         <v>28</v>
       </c>
       <c r="C43" s="13">
-        <v>703081.73838811077</v>
+        <v>703157.70649718028</v>
       </c>
       <c r="D43" s="13">
         <v>760576.86834800406</v>
@@ -3086,7 +3089,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="13">
-        <v>697440.75014498399</v>
+        <v>697500.61696579761</v>
       </c>
       <c r="D44" s="13">
         <v>690879.79825168336</v>
@@ -3100,7 +3103,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="13">
-        <v>701057.94033949706</v>
+        <v>700992.22596009762</v>
       </c>
       <c r="D45" s="13">
         <v>686701.4706187105</v>
@@ -3114,7 +3117,7 @@
         <v>27</v>
       </c>
       <c r="C46" s="13">
-        <v>711623.61102894158</v>
+        <v>711536.92698772647</v>
       </c>
       <c r="D46" s="13">
         <v>672749.81139169924</v>
@@ -3128,7 +3131,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="13">
-        <v>727716.46790551464</v>
+        <v>727857.94621608069</v>
       </c>
       <c r="D47" s="13">
         <v>791235.96554167022</v>
@@ -3142,7 +3145,7 @@
         <v>29</v>
       </c>
       <c r="C48" s="13">
-        <v>727288.65197496035</v>
+        <v>727359.14360456448</v>
       </c>
       <c r="D48" s="13">
         <v>718281.26544978167</v>
@@ -3156,7 +3159,7 @@
         <v>30</v>
       </c>
       <c r="C49" s="13">
-        <v>719319.85564274376</v>
+        <v>719194.56974378857</v>
       </c>
       <c r="D49" s="13">
         <v>703681.54416900803</v>
@@ -3170,7 +3173,7 @@
         <v>27</v>
       </c>
       <c r="C50" s="13">
-        <v>713343.55352433119</v>
+        <v>713294.02690009261</v>
       </c>
       <c r="D50" s="13">
         <v>677652.08911570266</v>
@@ -3184,7 +3187,7 @@
         <v>28</v>
       </c>
       <c r="C51" s="13">
-        <v>700876.98894771049</v>
+        <v>701081.71610465948</v>
       </c>
       <c r="D51" s="13">
         <v>760703.28015165636</v>
@@ -3198,7 +3201,7 @@
         <v>29</v>
       </c>
       <c r="C52" s="13">
-        <v>703503.3059038705</v>
+        <v>703546.24600118131</v>
       </c>
       <c r="D52" s="13">
         <v>694382.47577623045</v>
@@ -3212,7 +3215,7 @@
         <v>30</v>
       </c>
       <c r="C53" s="13">
-        <v>708187.54601473617</v>
+        <v>707989.40538471367</v>
       </c>
       <c r="D53" s="13">
         <v>693173.54934705782</v>
@@ -3226,7 +3229,7 @@
         <v>27</v>
       </c>
       <c r="C54" s="13">
-        <v>715541.12430242822</v>
+        <v>715505.46537437034</v>
       </c>
       <c r="D54" s="13">
         <v>681444.76611022244</v>
@@ -3240,7 +3243,7 @@
         <v>28</v>
       </c>
       <c r="C55" s="13">
-        <v>720864.54544404813</v>
+        <v>721157.32004200399</v>
       </c>
       <c r="D55" s="13">
         <v>778401.67644931667</v>
@@ -3254,7 +3257,7 @@
         <v>29</v>
       </c>
       <c r="C56" s="13">
-        <v>730409.70809090615</v>
+        <v>730438.49818150653</v>
       </c>
       <c r="D56" s="13">
         <v>721120.42685279413</v>
@@ -3268,7 +3271,7 @@
         <v>30</v>
       </c>
       <c r="C57" s="13">
-        <v>738744.41321391251</v>
+        <v>738458.50745341461</v>
       </c>
       <c r="D57" s="13">
         <v>724592.92163896293</v>
@@ -3282,7 +3285,7 @@
         <v>27</v>
       </c>
       <c r="C58" s="13">
-        <v>738063.50607312412</v>
+        <v>738010.34181803011</v>
       </c>
       <c r="D58" s="13">
         <v>707231.01699200924</v>
@@ -3296,7 +3299,7 @@
         <v>28</v>
       </c>
       <c r="C59" s="13">
-        <v>700381.81266289623</v>
+        <v>700751.14273484622</v>
       </c>
       <c r="D59" s="13">
         <v>747420.07441892265</v>
@@ -3310,7 +3313,7 @@
         <v>29</v>
       </c>
       <c r="C60" s="13">
-        <v>699912.37833407056</v>
+        <v>699961.28848597896</v>
       </c>
       <c r="D60" s="13">
         <v>696471.25579377101</v>
@@ -3324,7 +3327,7 @@
         <v>30</v>
       </c>
       <c r="C61" s="13">
-        <v>692664.26134448207</v>
+        <v>692299.18537571817</v>
       </c>
       <c r="D61" s="13">
         <v>679899.61120987148</v>
@@ -3338,7 +3341,7 @@
         <v>27</v>
       </c>
       <c r="C62" s="13">
-        <v>693888.02579630702</v>
+        <v>693790.28996283363</v>
       </c>
       <c r="D62" s="13">
         <v>665471.48418794025</v>
@@ -3352,7 +3355,7 @@
         <v>28</v>
       </c>
       <c r="C63" s="13">
-        <v>690911.4545944538</v>
+        <v>691386.57998083381</v>
       </c>
       <c r="D63" s="13">
         <v>750203.91624211951</v>
@@ -3366,7 +3369,7 @@
         <v>29</v>
       </c>
       <c r="C64" s="13">
-        <v>696760.17457923503</v>
+        <v>696841.19016822055</v>
       </c>
       <c r="D64" s="13">
         <v>683792.55791734927</v>
@@ -3380,7 +3383,7 @@
         <v>30</v>
       </c>
       <c r="C65" s="13">
-        <v>690350.14788672794</v>
+        <v>689891.74272320268</v>
       </c>
       <c r="D65" s="12">
         <v>672441.84078677045</v>
@@ -3394,7 +3397,7 @@
         <v>27</v>
       </c>
       <c r="C66" s="12">
-        <v>661654.94892247976</v>
+        <v>661533.3179601978</v>
       </c>
       <c r="D66" s="12">
         <v>630971.49375148444</v>
@@ -3408,10 +3411,24 @@
         <v>28</v>
       </c>
       <c r="C67" s="12">
-        <v>554316.13938229729</v>
+        <v>555637.19845436804</v>
       </c>
       <c r="D67">
-        <v>606992.80173888081</v>
+        <v>607869.14959540777</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="12">
+        <v>2020</v>
+      </c>
+      <c r="B68" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" s="12">
+        <v>626543.19542912173</v>
+      </c>
+      <c r="D68" s="12">
+        <v>613801.41291105596</v>
       </c>
     </row>
   </sheetData>
@@ -3437,14 +3454,14 @@
       <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="40"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -4048,14 +4065,14 @@
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="40"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4520,8 +4537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4546,10 +4563,10 @@
         <v>99</v>
       </c>
       <c r="B2">
-        <v>512359.57668351842</v>
+        <v>511235.56787450501</v>
       </c>
       <c r="C2">
-        <v>-19.367085851183731</v>
+        <v>-10.255417328634142</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4557,10 +4574,10 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>92004.645068881611</v>
+        <v>34766.191625489824</v>
       </c>
       <c r="C3">
-        <v>-10.662776074013092</v>
+        <v>-2.4593647908442651</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4568,10 +4585,10 @@
         <v>101</v>
       </c>
       <c r="B4">
-        <v>1762.0229144674997</v>
+        <v>2775.155118162565</v>
       </c>
       <c r="C4">
-        <v>-14.012780295759219</v>
+        <v>-18.283529445145085</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4579,10 +4596,10 @@
         <v>102</v>
       </c>
       <c r="B5">
-        <v>17786.684208885996</v>
+        <v>19204.888120793898</v>
       </c>
       <c r="C5">
-        <v>-18.257336008282532</v>
+        <v>-12.761790706318122</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4590,10 +4607,10 @@
         <v>103</v>
       </c>
       <c r="B6">
-        <v>87855.640061666243</v>
+        <v>106091.26662120047</v>
       </c>
       <c r="C6">
-        <v>-20.78211950432992</v>
+        <v>-5.264001833835275</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4601,10 +4618,10 @@
         <v>104</v>
       </c>
       <c r="B7">
-        <v>11444.28144229284</v>
+        <v>12685.332330355359</v>
       </c>
       <c r="C7">
-        <v>-3.322617578802578</v>
+        <v>2.2873930582023139</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4612,10 +4629,10 @@
         <v>105</v>
       </c>
       <c r="B8">
-        <v>10168.960336140055</v>
+        <v>16084.076127725084</v>
       </c>
       <c r="C8">
-        <v>-52.061712371385013</v>
+        <v>-27.004453828361719</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4623,10 +4640,10 @@
         <v>106</v>
       </c>
       <c r="B9">
-        <v>71161.53514765836</v>
+        <v>82148.029517348172</v>
       </c>
       <c r="C9">
-        <v>-16.915809495210297</v>
+        <v>-2.1088117735366452</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4634,10 +4651,10 @@
         <v>107</v>
       </c>
       <c r="B10">
-        <v>2846.6104571211044</v>
+        <v>4484.705522659061</v>
       </c>
       <c r="C10">
-        <v>-73.358743089924516</v>
+        <v>-61.52166709552229</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4645,10 +4662,10 @@
         <v>108</v>
       </c>
       <c r="B11">
-        <v>45942.355822993144</v>
+        <v>44758.460785199029</v>
       </c>
       <c r="C11">
-        <v>-22.455757918651422</v>
+        <v>-21.709540042602871</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4656,10 +4673,10 @@
         <v>109</v>
       </c>
       <c r="B12">
-        <v>24870.172648461972</v>
+        <v>26256.880008073353</v>
       </c>
       <c r="C12">
-        <v>-1.2002304258781127</v>
+        <v>4.606972804154541</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4667,10 +4684,10 @@
         <v>110</v>
       </c>
       <c r="B13">
-        <v>64522.940872450235</v>
+        <v>71776.689320121382</v>
       </c>
       <c r="C13">
-        <v>-14.315387598774443</v>
+        <v>-5.8071163910641381</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4678,10 +4695,10 @@
         <v>116</v>
       </c>
       <c r="B14">
-        <v>28996.867587962621</v>
+        <v>29976.766555809754</v>
       </c>
       <c r="C14">
-        <v>-12.799845828932533</v>
+        <v>-9.7272670032516722</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4689,10 +4706,10 @@
         <v>111</v>
       </c>
       <c r="B15">
-        <v>25007.616698329046</v>
+        <v>26109.035629520033</v>
       </c>
       <c r="C15">
-        <v>-9.2094014857966862</v>
+        <v>-6.7025788852315475</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4700,10 +4717,10 @@
         <v>112</v>
       </c>
       <c r="B16">
-        <v>19525.683527571011</v>
+        <v>21929.617977242029</v>
       </c>
       <c r="C16">
-        <v>-23.468530609699613</v>
+        <v>-8.6671028803558485</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4711,10 +4728,10 @@
         <v>113</v>
       </c>
       <c r="B17">
-        <v>5830.5199163868256</v>
+        <v>8611.1941960524819</v>
       </c>
       <c r="C17">
-        <v>-67.712814571577965</v>
+        <v>-53.787777681410311</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4722,10 +4739,10 @@
         <v>114</v>
       </c>
       <c r="B18">
-        <v>2633.0399722498255</v>
+        <v>3577.2784187524389</v>
       </c>
       <c r="C18">
-        <v>-38.021339999999981</v>
+        <v>-16.800000000000015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos fiscales y EMAE"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -567,7 +566,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -578,6 +576,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1641,13 +1641,13 @@
       <c r="B45" s="1">
         <v>2.7</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C45" s="24">
         <v>4</v>
       </c>
-      <c r="D45" s="25">
+      <c r="D45" s="24">
         <v>3</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1747,25 +1747,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <v>3.2</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="26">
         <v>3</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="28">
         <v>3.4</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="28">
         <v>3.4</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <v>3.1</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="28">
         <v>3.1</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="28">
         <v>2.9</v>
       </c>
     </row>
@@ -1773,25 +1773,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>2.7</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>2.1</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>3.5</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>3.5</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="27">
         <v>2.1</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="27">
         <v>2.8</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="27">
         <v>3.1</v>
       </c>
     </row>
@@ -1799,25 +1799,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>3</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>2.4</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>3.4</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>3.4</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>4</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="27">
         <v>3.1</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <v>3.7</v>
       </c>
     </row>
@@ -1825,25 +1825,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>3.7</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>3</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>3.8</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <v>3.8</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>5.5</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="27">
         <v>4.5</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="27">
         <v>4.8</v>
       </c>
     </row>
@@ -1851,25 +1851,25 @@
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="27">
         <v>2.5</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <v>2.5</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>3</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>3</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <v>0.8</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="27">
         <v>2.4</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <v>2.4</v>
       </c>
     </row>
@@ -1877,25 +1877,25 @@
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="27">
         <v>3.9</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>3.9</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>3.7</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>3.7</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <v>5.3</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="27">
         <v>3.6</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <v>4</v>
       </c>
     </row>
@@ -1903,25 +1903,25 @@
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="27">
         <v>3.7</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <v>3.4</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>3.7</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="27">
         <v>3.7</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="27">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>2.8</v>
       </c>
     </row>
@@ -1929,25 +1929,25 @@
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="27">
         <v>3.6</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>3.1</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>3.1</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="27">
         <v>3.7</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <v>3.3</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>3.1</v>
       </c>
     </row>
@@ -1955,25 +1955,25 @@
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>-0.6</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="25">
         <v>-1.8</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>0.2</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>0.2</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>2</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="27">
         <v>0.7</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <v>-0.2</v>
       </c>
     </row>
@@ -1981,25 +1981,25 @@
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="27">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>5.5</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>5.3</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>5.3</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="27">
         <v>3.5</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="27">
         <v>4.7</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <v>1.3</v>
       </c>
     </row>
@@ -2007,25 +2007,25 @@
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="27">
         <v>0.4</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="25">
         <v>0.5</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>0.3</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="27">
         <v>0.3</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="27">
         <v>0</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>1.8</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>0.2</v>
       </c>
     </row>
@@ -2033,25 +2033,25 @@
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>3.2</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <v>3.5</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>3.1</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <v>3.1</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <v>3.6</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="27">
         <v>2.4</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -2059,25 +2059,25 @@
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="27">
         <v>2.6</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="25">
         <v>3.3</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="27">
         <v>2.6</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="27">
         <v>1.3</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>1.8</v>
       </c>
     </row>
@@ -2127,25 +2127,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>35.799999999999997</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="29">
         <v>34.200000000000003</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>37.1</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <v>40.1</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="31">
         <v>37.299999999999997</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="31">
         <v>36.4</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="31">
         <v>33.700000000000003</v>
       </c>
     </row>
@@ -2153,25 +2153,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <v>40.4</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>38.4</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <v>42.1</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>44.8</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <v>43.8</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="32">
         <v>40.700000000000003</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="32">
         <v>37.5</v>
       </c>
     </row>
@@ -2179,25 +2179,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="32">
         <v>32.700000000000003</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>32.5</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="32">
         <v>32.6</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>32.9</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>34.1</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="32">
         <v>32.9</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="32">
         <v>32.5</v>
       </c>
     </row>
@@ -2205,25 +2205,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <v>58.1</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>56.9</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <v>60.5</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>51.4</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>61.8</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="32">
         <v>61.8</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="32">
         <v>49.3</v>
       </c>
     </row>
@@ -2231,25 +2231,25 @@
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <v>16.600000000000001</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>16.2</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="32">
         <v>18.5</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="30">
         <v>19.5</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <v>8.1</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="32">
         <v>18.399999999999999</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="32">
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -2257,25 +2257,25 @@
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>41.7</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>42.6</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>40</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <v>52.2</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>41.7</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="32">
         <v>37.5</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="32">
         <v>41</v>
       </c>
     </row>
@@ -2283,25 +2283,25 @@
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>29.1</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>25.2</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <v>31.1</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="30">
         <v>35.6</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>34.5</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="32">
         <v>32.1</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="32">
         <v>32.5</v>
       </c>
     </row>
@@ -2309,25 +2309,25 @@
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>34.299999999999997</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>33.1</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>36</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="30">
         <v>37.6</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>29.5</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="32">
         <v>35.700000000000003</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="32">
         <v>36.1</v>
       </c>
     </row>
@@ -2335,25 +2335,25 @@
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="32">
         <v>17.899999999999999</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>18.600000000000001</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="32">
         <v>16.899999999999999</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="30">
         <v>18.5</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <v>18.7</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="32">
         <v>19.5</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="32">
         <v>15.8</v>
       </c>
     </row>
@@ -2361,25 +2361,25 @@
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <v>44.1</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>46.7</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="32">
         <v>42.1</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="30">
         <v>49.6</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="32">
         <v>40.6</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="32">
         <v>40.9</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="32">
         <v>37.799999999999997</v>
       </c>
     </row>
@@ -2387,25 +2387,25 @@
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>22.4</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>22.6</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="32">
         <v>20.100000000000001</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="30">
         <v>25.9</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <v>28.7</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="32">
         <v>26.7</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="32">
         <v>17.399999999999999</v>
       </c>
     </row>
@@ -2413,25 +2413,25 @@
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>34.6</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="30">
         <v>33.5</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>37.299999999999997</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="30">
         <v>35.700000000000003</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <v>33.700000000000003</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="32">
         <v>33</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="32">
         <v>26.6</v>
       </c>
     </row>
@@ -2439,25 +2439,25 @@
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>29</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="30">
         <v>33.4</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="32">
         <v>25.9</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="30">
         <v>28</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <v>26.6</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="32">
         <v>24.5</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H14" s="32">
         <v>21</v>
       </c>
     </row>
@@ -3404,10 +3404,10 @@
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="24">
+      <c r="A67" s="23">
         <v>2020</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="B67" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C67" s="12">
@@ -3421,7 +3421,7 @@
       <c r="A68" s="12">
         <v>2020</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="38" t="s">
         <v>29</v>
       </c>
       <c r="C68" s="12">
@@ -3454,14 +3454,14 @@
       <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -3499,16 +3499,16 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>11.3</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>17.3</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>3.1</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <v>3.7</v>
       </c>
     </row>
@@ -3516,16 +3516,16 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>37.5</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>47.5</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>11</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>13.6</v>
       </c>
     </row>
@@ -3533,16 +3533,16 @@
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>31</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>41.5</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>6.9</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>8.8000000000000007</v>
       </c>
     </row>
@@ -3550,16 +3550,16 @@
       <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>25.5</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>35.799999999999997</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>3.7</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>4.7</v>
       </c>
     </row>
@@ -3567,16 +3567,16 @@
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>29.5</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>39.200000000000003</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>6.3</v>
       </c>
     </row>
@@ -3584,16 +3584,16 @@
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>32.799999999999997</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>41.2</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>11.8</v>
       </c>
     </row>
@@ -3601,16 +3601,16 @@
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>35.200000000000003</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>42.4</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>7.1</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>8.8000000000000007</v>
       </c>
     </row>
@@ -3618,16 +3618,16 @@
       <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>39.299999999999997</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="34">
         <v>48.7</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>13.8</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <v>18.2</v>
       </c>
     </row>
@@ -3635,16 +3635,16 @@
       <c r="A12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="24">
         <v>27.1</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="24">
         <v>38.1</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>3.9</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="24">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -3652,16 +3652,16 @@
       <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="24">
         <v>27.6</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="24">
         <v>35.200000000000003</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <v>6.1</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="24">
         <v>8</v>
       </c>
     </row>
@@ -3669,16 +3669,16 @@
       <c r="A14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="24">
         <v>31.2</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="24">
         <v>41.5</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <v>7.3</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="24">
         <v>8.1</v>
       </c>
     </row>
@@ -3686,16 +3686,16 @@
       <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="24">
         <v>28.6</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="24">
         <v>38</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="24">
         <v>3.5</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="24">
         <v>4.8</v>
       </c>
     </row>
@@ -3703,16 +3703,16 @@
       <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="24">
         <v>20.9</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="24">
         <v>29.8</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="24">
         <v>1.9</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="24">
         <v>2.7</v>
       </c>
     </row>
@@ -3720,16 +3720,16 @@
       <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="24">
         <v>35.799999999999997</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="24">
         <v>45.5</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="24">
         <v>9.6</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <v>11.4</v>
       </c>
     </row>
@@ -3737,16 +3737,16 @@
       <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="24">
         <v>34.1</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="24">
         <v>42.9</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="24">
         <v>5.5</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="24">
         <v>7.5</v>
       </c>
     </row>
@@ -3754,16 +3754,16 @@
       <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="24">
         <v>23.2</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="24">
         <v>33.700000000000003</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="24">
         <v>3.2</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="24">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3771,16 +3771,16 @@
       <c r="A20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="24">
         <v>40.6</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="24">
         <v>52.2</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="24">
         <v>8.4</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="24">
         <v>12</v>
       </c>
     </row>
@@ -3788,16 +3788,16 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="24">
         <v>28.2</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="24">
         <v>40.700000000000003</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="24">
         <v>5.6</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="24">
         <v>8.1</v>
       </c>
     </row>
@@ -3805,16 +3805,16 @@
       <c r="A22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="24">
         <v>27.7</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="24">
         <v>37.4</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="24">
         <v>6.5</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="24">
         <v>9.9</v>
       </c>
     </row>
@@ -3822,16 +3822,16 @@
       <c r="A23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="24">
         <v>30.6</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="24">
         <v>41.8</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="24">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="24">
         <v>13.3</v>
       </c>
     </row>
@@ -3839,16 +3839,16 @@
       <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="24">
         <v>26.6</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="24">
         <v>36.299999999999997</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="24">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="24">
         <v>6.3</v>
       </c>
     </row>
@@ -3856,16 +3856,16 @@
       <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="24">
         <v>30.4</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="24">
         <v>42.6</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="24">
         <v>7.1</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="24">
         <v>10.9</v>
       </c>
     </row>
@@ -3873,16 +3873,16 @@
       <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="24">
         <v>30.8</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="24">
         <v>38.9</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="24">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="24">
         <v>12</v>
       </c>
     </row>
@@ -3890,16 +3890,16 @@
       <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="24">
         <v>25.2</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="24">
         <v>34.799999999999997</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="24">
         <v>6.2</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="24">
         <v>8.6</v>
       </c>
     </row>
@@ -3907,16 +3907,16 @@
       <c r="A28" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="24">
         <v>22.2</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="24">
         <v>32.799999999999997</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="24">
         <v>6.4</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="24">
         <v>8.9</v>
       </c>
     </row>
@@ -3924,16 +3924,16 @@
       <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="24">
         <v>29.8</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="24">
         <v>39.799999999999997</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="24">
         <v>7.4</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <v>10.199999999999999</v>
       </c>
     </row>
@@ -3941,16 +3941,16 @@
       <c r="A30" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="24">
         <v>26.9</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="24">
         <v>34.9</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="24">
         <v>5.6</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="24">
         <v>5.7</v>
       </c>
     </row>
@@ -3958,16 +3958,16 @@
       <c r="A31" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="24">
         <v>28.4</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="24">
         <v>37.5</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="24">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="24">
         <v>5.2</v>
       </c>
     </row>
@@ -3975,16 +3975,16 @@
       <c r="A32" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="24">
         <v>21.9</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="24">
         <v>28.7</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="24">
         <v>3.6</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="24">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -3992,16 +3992,16 @@
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="24">
         <v>28.4</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="24">
         <v>39.299999999999997</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="24">
         <v>7.5</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="24">
         <v>9.8000000000000007</v>
       </c>
     </row>
@@ -4009,16 +4009,16 @@
       <c r="A34" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="24">
         <v>28.5</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="24">
         <v>39.700000000000003</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="24">
         <v>7.5</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="24">
         <v>8.3000000000000007</v>
       </c>
     </row>
@@ -4026,16 +4026,16 @@
       <c r="A35" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="24">
         <v>30.1</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="24">
         <v>43.5</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="24">
         <v>4.7</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="24">
         <v>6.2</v>
       </c>
     </row>
@@ -4065,14 +4065,14 @@
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4092,16 +4092,16 @@
       <c r="A3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>30.4</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>40.9</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>8.1</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <v>10.5</v>
       </c>
     </row>
@@ -4537,7 +4537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
@@ -4752,10 +4752,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50:D58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4766,16 +4766,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4786,11 +4786,11 @@
       <c r="B2" s="20">
         <v>134.74645041349706</v>
       </c>
-      <c r="C2" s="20">
-        <v>147.86337571377604</v>
-      </c>
-      <c r="D2" s="20">
-        <v>147.17697825117915</v>
+      <c r="C2" s="36">
+        <v>147.40548950066798</v>
+      </c>
+      <c r="D2" s="36">
+        <v>147.13250454280865</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4800,11 +4800,11 @@
       <c r="B3" s="20">
         <v>134.23236103862521</v>
       </c>
-      <c r="C3" s="20">
-        <v>146.84393197927398</v>
-      </c>
-      <c r="D3" s="20">
-        <v>146.62106427636331</v>
+      <c r="C3" s="36">
+        <v>147.20703967782137</v>
+      </c>
+      <c r="D3" s="36">
+        <v>146.59655953359194</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4814,11 +4814,11 @@
       <c r="B4" s="20">
         <v>150.0878942366954</v>
       </c>
-      <c r="C4" s="20">
-        <v>146.43134947782625</v>
-      </c>
-      <c r="D4" s="20">
-        <v>146.10045078853742</v>
+      <c r="C4" s="36">
+        <v>146.49550086251253</v>
+      </c>
+      <c r="D4" s="36">
+        <v>146.10675364813869</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4828,11 +4828,11 @@
       <c r="B5" s="20">
         <v>153.25067436662908</v>
       </c>
-      <c r="C5" s="20">
-        <v>144.70726596935651</v>
-      </c>
-      <c r="D5" s="20">
-        <v>145.64999424484782</v>
+      <c r="C5" s="36">
+        <v>144.86737682873593</v>
+      </c>
+      <c r="D5" s="36">
+        <v>145.69282259206</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4842,11 +4842,11 @@
       <c r="B6" s="20">
         <v>163.51360808690507</v>
       </c>
-      <c r="C6" s="20">
-        <v>144.24555721449209</v>
-      </c>
-      <c r="D6" s="20">
-        <v>145.29558330185444</v>
+      <c r="C6" s="36">
+        <v>144.16229134006119</v>
+      </c>
+      <c r="D6" s="36">
+        <v>145.3781743875339</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4856,11 +4856,11 @@
       <c r="B7" s="20">
         <v>153.66209524099784</v>
       </c>
-      <c r="C7" s="20">
-        <v>144.47638888863597</v>
-      </c>
-      <c r="D7" s="20">
-        <v>145.05583857646258</v>
+      <c r="C7" s="36">
+        <v>144.52614896411009</v>
+      </c>
+      <c r="D7" s="36">
+        <v>145.17975049300318</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4870,11 +4870,11 @@
       <c r="B8" s="20">
         <v>143.73110098180126</v>
       </c>
-      <c r="C8" s="20">
-        <v>144.44793055599717</v>
-      </c>
-      <c r="D8" s="20">
-        <v>144.94036515112285</v>
+      <c r="C8" s="36">
+        <v>143.9570142488798</v>
+      </c>
+      <c r="D8" s="36">
+        <v>145.10264782100302</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4884,11 +4884,11 @@
       <c r="B9" s="20">
         <v>143.6741026486049</v>
       </c>
-      <c r="C9" s="20">
-        <v>145.35747190730874</v>
-      </c>
-      <c r="D9" s="20">
-        <v>144.95225973609783</v>
+      <c r="C9" s="36">
+        <v>145.56928975620252</v>
+      </c>
+      <c r="D9" s="36">
+        <v>145.1441038166339</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4898,11 +4898,11 @@
       <c r="B10" s="20">
         <v>142.00773744282046</v>
       </c>
-      <c r="C10" s="20">
-        <v>145.24795004611377</v>
-      </c>
-      <c r="D10" s="20">
-        <v>145.08656493324827</v>
+      <c r="C10" s="36">
+        <v>145.55360261495525</v>
+      </c>
+      <c r="D10" s="36">
+        <v>145.29804474277401</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4912,11 +4912,11 @@
       <c r="B11" s="20">
         <v>141.13686329808141</v>
       </c>
-      <c r="C11" s="20">
-        <v>145.06183294019505</v>
-      </c>
-      <c r="D11" s="20">
-        <v>145.33280595074299</v>
+      <c r="C11" s="36">
+        <v>144.37944165217016</v>
+      </c>
+      <c r="D11" s="36">
+        <v>145.55243811593579</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4926,11 +4926,11 @@
       <c r="B12" s="20">
         <v>144.93832064073018</v>
       </c>
-      <c r="C12" s="20">
-        <v>146.11022407387216</v>
-      </c>
-      <c r="D12" s="20">
-        <v>145.67842802271554</v>
+      <c r="C12" s="36">
+        <v>146.33104797653249</v>
+      </c>
+      <c r="D12" s="36">
+        <v>145.89829320034238</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4940,11 +4940,11 @@
       <c r="B13" s="20">
         <v>142.59014516031914</v>
       </c>
-      <c r="C13" s="20">
-        <v>146.7780750312121</v>
-      </c>
-      <c r="D13" s="20">
-        <v>146.11073335050062</v>
+      <c r="C13" s="36">
+        <v>147.11711038131926</v>
+      </c>
+      <c r="D13" s="36">
+        <v>146.32335632441931</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4954,11 +4954,11 @@
       <c r="B14" s="20">
         <v>136.7258774086435</v>
       </c>
-      <c r="C14" s="20">
-        <v>147.6</v>
-      </c>
-      <c r="D14" s="20">
-        <v>146.80000000000001</v>
+      <c r="C14" s="36">
+        <v>147.51218811787277</v>
+      </c>
+      <c r="D14" s="36">
+        <v>146.81320009733042</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4968,11 +4968,11 @@
       <c r="B15" s="20">
         <v>132.54052520440143</v>
       </c>
-      <c r="C15" s="20">
-        <v>146.5</v>
-      </c>
-      <c r="D15" s="20">
-        <v>147.30000000000001</v>
+      <c r="C15" s="36">
+        <v>146.55590467771026</v>
+      </c>
+      <c r="D15" s="36">
+        <v>147.35155431110869</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4982,11 +4982,11 @@
       <c r="B16" s="20">
         <v>152.145731768997</v>
       </c>
-      <c r="C16" s="20">
-        <v>148.4</v>
-      </c>
-      <c r="D16" s="20">
-        <v>147.80000000000001</v>
+      <c r="C16" s="36">
+        <v>148.40751251194064</v>
+      </c>
+      <c r="D16" s="36">
+        <v>147.92438453421599</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4996,11 +4996,11 @@
       <c r="B17" s="20">
         <v>152.20883250679566</v>
       </c>
-      <c r="C17" s="20">
-        <v>147.19999999999999</v>
-      </c>
-      <c r="D17" s="20">
-        <v>148.4</v>
+      <c r="C17" s="36">
+        <v>147.23855198711274</v>
+      </c>
+      <c r="D17" s="36">
+        <v>148.51514759345517</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5010,11 +5010,11 @@
       <c r="B18" s="20">
         <v>167.46154818637638</v>
       </c>
-      <c r="C18" s="20">
-        <v>148.6</v>
-      </c>
-      <c r="D18" s="20">
-        <v>149</v>
+      <c r="C18" s="36">
+        <v>148.65798864877942</v>
+      </c>
+      <c r="D18" s="36">
+        <v>149.10525330454533</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5024,11 +5024,11 @@
       <c r="B19" s="20">
         <v>161.70085905013559</v>
       </c>
-      <c r="C19" s="20">
-        <v>150.19999999999999</v>
-      </c>
-      <c r="D19" s="20">
-        <v>149.6</v>
+      <c r="C19" s="36">
+        <v>150.07422709343567</v>
+      </c>
+      <c r="D19" s="36">
+        <v>149.66871892773509</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5038,11 +5038,11 @@
       <c r="B20" s="20">
         <v>149.78297310853262</v>
       </c>
-      <c r="C20" s="20">
-        <v>149.80000000000001</v>
-      </c>
-      <c r="D20" s="20">
-        <v>150.1</v>
+      <c r="C20" s="36">
+        <v>149.7069308868486</v>
+      </c>
+      <c r="D20" s="36">
+        <v>150.17360583142343</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5052,11 +5052,11 @@
       <c r="B21" s="20">
         <v>149.4590923353316</v>
       </c>
-      <c r="C21" s="20">
-        <v>150.5</v>
-      </c>
-      <c r="D21" s="20">
-        <v>150.5</v>
+      <c r="C21" s="36">
+        <v>150.48723167737793</v>
+      </c>
+      <c r="D21" s="36">
+        <v>150.58343827682742</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5066,11 +5066,11 @@
       <c r="B22" s="20">
         <v>146.70588711165021</v>
       </c>
-      <c r="C22" s="20">
-        <v>151.4</v>
-      </c>
-      <c r="D22" s="20">
-        <v>150.80000000000001</v>
+      <c r="C22" s="36">
+        <v>151.51617685809143</v>
+      </c>
+      <c r="D22" s="36">
+        <v>150.86176489297546</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5080,11 +5080,11 @@
       <c r="B23" s="20">
         <v>149.62906247744323</v>
       </c>
-      <c r="C23" s="20">
-        <v>151.1</v>
-      </c>
-      <c r="D23" s="20">
-        <v>150.9</v>
+      <c r="C23" s="36">
+        <v>151.06711826752945</v>
+      </c>
+      <c r="D23" s="36">
+        <v>150.9773097525821</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5094,11 +5094,11 @@
       <c r="B24" s="20">
         <v>152.38283025725997</v>
       </c>
-      <c r="C24" s="20">
-        <v>153.19999999999999</v>
-      </c>
-      <c r="D24" s="20">
-        <v>150.9</v>
+      <c r="C24" s="36">
+        <v>153.23666431612583</v>
+      </c>
+      <c r="D24" s="36">
+        <v>150.9056274896343</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5108,11 +5108,11 @@
       <c r="B25" s="20">
         <v>146.08348469256237</v>
       </c>
-      <c r="C25" s="20">
-        <v>152.4</v>
-      </c>
-      <c r="D25" s="20">
-        <v>150.6</v>
+      <c r="C25" s="36">
+        <v>152.36620932056729</v>
+      </c>
+      <c r="D25" s="36">
+        <v>150.63658635205991</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5122,11 +5122,11 @@
       <c r="B26" s="20">
         <v>142.64696239584413</v>
       </c>
-      <c r="C26" s="20">
-        <v>152.5</v>
-      </c>
-      <c r="D26" s="20">
-        <v>150.19999999999999</v>
+      <c r="C26" s="36">
+        <v>152.48102197832938</v>
+      </c>
+      <c r="D26" s="36">
+        <v>150.17417863869139</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5136,11 +5136,11 @@
       <c r="B27" s="20">
         <v>139.07181989111268</v>
       </c>
-      <c r="C27" s="20">
-        <v>151.9</v>
-      </c>
-      <c r="D27" s="20">
-        <v>149.5</v>
+      <c r="C27" s="36">
+        <v>151.96713501492289</v>
+      </c>
+      <c r="D27" s="36">
+        <v>149.53476628845246</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5150,11 +5150,11 @@
       <c r="B28" s="20">
         <v>155.63982283229944</v>
       </c>
-      <c r="C28" s="20">
-        <v>152</v>
-      </c>
-      <c r="D28" s="20">
-        <v>148.69999999999999</v>
+      <c r="C28" s="36">
+        <v>151.9446848815268</v>
+      </c>
+      <c r="D28" s="36">
+        <v>148.74914090221233</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5164,11 +5164,11 @@
       <c r="B29" s="20">
         <v>151.60135644382305</v>
       </c>
-      <c r="C29" s="20">
-        <v>146.69999999999999</v>
-      </c>
-      <c r="D29" s="20">
-        <v>147.9</v>
+      <c r="C29" s="36">
+        <v>146.63322601094779</v>
+      </c>
+      <c r="D29" s="36">
+        <v>147.86111794804336</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5178,11 +5178,11 @@
       <c r="B30" s="20">
         <v>159.16207548226589</v>
       </c>
-      <c r="C30" s="20">
-        <v>144.30000000000001</v>
-      </c>
-      <c r="D30" s="20">
-        <v>146.9</v>
+      <c r="C30" s="36">
+        <v>144.34065398200235</v>
+      </c>
+      <c r="D30" s="36">
+        <v>146.92485841421757</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5192,11 +5192,11 @@
       <c r="B31" s="20">
         <v>151.44848091721315</v>
       </c>
-      <c r="C31" s="20">
-        <v>142.4</v>
-      </c>
-      <c r="D31" s="20">
-        <v>146</v>
+      <c r="C31" s="36">
+        <v>142.37750732217762</v>
+      </c>
+      <c r="D31" s="36">
+        <v>145.99344925825582</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5206,11 +5206,11 @@
       <c r="B32" s="20">
         <v>145.76463042864052</v>
       </c>
-      <c r="C32" s="20">
-        <v>143.5</v>
-      </c>
-      <c r="D32" s="20">
-        <v>145.1</v>
+      <c r="C32" s="36">
+        <v>143.36897326244727</v>
+      </c>
+      <c r="D32" s="36">
+        <v>145.11713487580218</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5220,11 +5220,11 @@
       <c r="B33" s="20">
         <v>147.04553382400547</v>
       </c>
-      <c r="C33" s="20">
-        <v>146.9</v>
-      </c>
-      <c r="D33" s="20">
-        <v>144.30000000000001</v>
+      <c r="C33" s="36">
+        <v>146.90927549984139</v>
+      </c>
+      <c r="D33" s="36">
+        <v>144.34259028880226</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5234,11 +5234,11 @@
       <c r="B34" s="20">
         <v>137.8944988928931</v>
       </c>
-      <c r="C34" s="20">
-        <v>142.5</v>
-      </c>
-      <c r="D34" s="20">
-        <v>143.69999999999999</v>
+      <c r="C34" s="36">
+        <v>142.5846849297898</v>
+      </c>
+      <c r="D34" s="36">
+        <v>143.70319907946219</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5248,11 +5248,11 @@
       <c r="B35" s="20">
         <v>143.57320349337792</v>
       </c>
-      <c r="C35" s="20">
-        <v>143.69999999999999</v>
-      </c>
-      <c r="D35" s="20">
-        <v>143.19999999999999</v>
+      <c r="C35" s="36">
+        <v>143.7134503260327</v>
+      </c>
+      <c r="D35" s="36">
+        <v>143.21634302411266</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5262,11 +5262,11 @@
       <c r="B36" s="20">
         <v>141.21184890028576</v>
       </c>
-      <c r="C36" s="20">
-        <v>142.30000000000001</v>
-      </c>
-      <c r="D36" s="20">
-        <v>142.9</v>
+      <c r="C36" s="36">
+        <v>142.37778125739862</v>
+      </c>
+      <c r="D36" s="36">
+        <v>142.88711354506074</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5276,11 +5276,11 @@
       <c r="B37" s="20">
         <v>135.67154302632184</v>
       </c>
-      <c r="C37" s="20">
-        <v>142</v>
-      </c>
-      <c r="D37" s="20">
-        <v>142.69999999999999</v>
+      <c r="C37" s="36">
+        <v>142.03338231137309</v>
+      </c>
+      <c r="D37" s="36">
+        <v>142.70534829565807</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5290,11 +5290,11 @@
       <c r="B38" s="20">
         <v>134.564995313265</v>
       </c>
-      <c r="C38" s="20">
-        <v>143.69999999999999</v>
-      </c>
-      <c r="D38" s="20">
-        <v>142.6</v>
+      <c r="C38" s="36">
+        <v>143.68095342507036</v>
+      </c>
+      <c r="D38" s="36">
+        <v>142.64695346044655</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5304,11 +5304,11 @@
       <c r="B39" s="20">
         <v>132.57194718265788</v>
       </c>
-      <c r="C39" s="20">
-        <v>143.6</v>
-      </c>
-      <c r="D39" s="20">
-        <v>142.6</v>
+      <c r="C39" s="36">
+        <v>143.65413385641389</v>
+      </c>
+      <c r="D39" s="36">
+        <v>142.68020665901747</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5318,11 +5318,11 @@
       <c r="B40" s="20">
         <v>144.41715750575651</v>
       </c>
-      <c r="C40" s="20">
-        <v>141.80000000000001</v>
-      </c>
-      <c r="D40" s="20">
-        <v>142.69999999999999</v>
+      <c r="C40" s="36">
+        <v>141.7116403310888</v>
+      </c>
+      <c r="D40" s="36">
+        <v>142.76867441729735</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5332,11 +5332,11 @@
       <c r="B41" s="20">
         <v>149.83961931661509</v>
       </c>
-      <c r="C41" s="20">
-        <v>142.30000000000001</v>
-      </c>
-      <c r="D41" s="20">
-        <v>142.80000000000001</v>
+      <c r="C41" s="36">
+        <v>142.30963439168579</v>
+      </c>
+      <c r="D41" s="36">
+        <v>142.87406175831902</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5346,11 +5346,11 @@
       <c r="B42" s="20">
         <v>162.83974753189364</v>
       </c>
-      <c r="C42" s="20">
-        <v>143.4</v>
-      </c>
-      <c r="D42" s="20">
-        <v>142.80000000000001</v>
+      <c r="C42" s="36">
+        <v>143.4153404616502</v>
+      </c>
+      <c r="D42" s="36">
+        <v>142.95895938660107</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5360,11 +5360,11 @@
       <c r="B43" s="20">
         <v>151.25410111244764</v>
       </c>
-      <c r="C43" s="20">
-        <v>141.9</v>
-      </c>
-      <c r="D43" s="20">
-        <v>142.80000000000001</v>
+      <c r="C43" s="36">
+        <v>141.83527490443359</v>
+      </c>
+      <c r="D43" s="36">
+        <v>142.9890906382563</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5374,11 +5374,11 @@
       <c r="B44" s="20">
         <v>146.20323233619627</v>
       </c>
-      <c r="C44" s="20">
-        <v>145.6</v>
-      </c>
-      <c r="D44" s="20">
-        <v>142.80000000000001</v>
+      <c r="C44" s="36">
+        <v>145.37887579033358</v>
+      </c>
+      <c r="D44" s="36">
+        <v>142.93518580755071</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5388,193 +5388,207 @@
       <c r="B45" s="20">
         <v>141.60332874981128</v>
       </c>
-      <c r="C45" s="20">
-        <v>144.69999999999999</v>
-      </c>
-      <c r="D45" s="20">
-        <v>142.6</v>
+      <c r="C45" s="36">
+        <v>144.68319699058412</v>
+      </c>
+      <c r="D45" s="36">
+        <v>142.77510427768922</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="11">
         <v>43709</v>
       </c>
-      <c r="B46" s="20">
-        <v>135.0574708022306</v>
-      </c>
-      <c r="C46" s="20">
-        <v>140.80000000000001</v>
-      </c>
-      <c r="D46" s="20">
-        <v>142.4</v>
+      <c r="B46" s="36">
+        <v>135.07531285730843</v>
+      </c>
+      <c r="C46" s="36">
+        <v>140.87136147533508</v>
+      </c>
+      <c r="D46" s="36">
+        <v>142.49559665045726</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="11">
         <v>43739</v>
       </c>
-      <c r="B47" s="20">
-        <v>142.24064825618933</v>
-      </c>
-      <c r="C47" s="20">
-        <v>143.6</v>
-      </c>
-      <c r="D47" s="35">
-        <v>142.1</v>
+      <c r="B47" s="36">
+        <v>142.25579775531418</v>
+      </c>
+      <c r="C47" s="36">
+        <v>143.54587561429835</v>
+      </c>
+      <c r="D47" s="36">
+        <v>142.0935891603549</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="11">
         <v>43770</v>
       </c>
-      <c r="B48" s="20">
-        <v>138.15855707957144</v>
-      </c>
-      <c r="C48" s="35">
-        <v>141.5</v>
-      </c>
-      <c r="D48" s="35">
-        <v>141.80000000000001</v>
+      <c r="B48" s="36">
+        <v>138.14131943492291</v>
+      </c>
+      <c r="C48" s="36">
+        <v>141.48456225642059</v>
+      </c>
+      <c r="D48" s="36">
+        <v>141.57666211619394</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="11">
         <v>43800</v>
       </c>
-      <c r="B49" s="35">
-        <v>135.45406298998449</v>
-      </c>
-      <c r="C49" s="35">
-        <v>141.5</v>
-      </c>
-      <c r="D49" s="35">
-        <v>141.4</v>
+      <c r="B49" s="36">
+        <v>135.44751977320297</v>
+      </c>
+      <c r="C49" s="36">
+        <v>141.60538984918296</v>
+      </c>
+      <c r="D49" s="36">
+        <v>140.96179182233465</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="11">
         <v>43831</v>
       </c>
-      <c r="B50" s="35">
-        <v>132.18766212782253</v>
-      </c>
-      <c r="C50" s="35">
-        <v>141.6</v>
-      </c>
-      <c r="D50" s="35">
-        <v>141</v>
+      <c r="B50" s="36">
+        <v>132.19356455544042</v>
+      </c>
+      <c r="C50" s="36">
+        <v>141.78898143893696</v>
+      </c>
+      <c r="D50" s="36">
+        <v>140.26998289408365</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="11">
         <v>43862</v>
       </c>
-      <c r="B51" s="35">
-        <v>129.65346351336271</v>
-      </c>
-      <c r="C51" s="35">
-        <v>140.69999999999999</v>
-      </c>
-      <c r="D51" s="35">
-        <v>140.6</v>
+      <c r="B51" s="36">
+        <v>129.61940932164029</v>
+      </c>
+      <c r="C51" s="36">
+        <v>141.09355092898466</v>
+      </c>
+      <c r="D51" s="36">
+        <v>139.53221814376042</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="11">
         <v>43891</v>
       </c>
-      <c r="B52" s="35">
-        <v>128.35784152357166</v>
-      </c>
-      <c r="C52" s="35">
-        <v>125.6</v>
-      </c>
-      <c r="D52" s="35">
-        <v>140.19999999999999</v>
+      <c r="B52" s="36">
+        <v>128.38599328767583</v>
+      </c>
+      <c r="C52" s="36">
+        <v>126.21616702827959</v>
+      </c>
+      <c r="D52" s="36">
+        <v>138.78278265769444</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="11">
         <v>43922</v>
       </c>
-      <c r="B53" s="35">
-        <v>111.65441062079474</v>
-      </c>
-      <c r="C53" s="35">
-        <v>104.1</v>
-      </c>
-      <c r="D53" s="35">
-        <v>139.80000000000001</v>
+      <c r="B53" s="36">
+        <v>111.81827837013516</v>
+      </c>
+      <c r="C53" s="36">
+        <v>105.02543573540743</v>
+      </c>
+      <c r="D53" s="36">
+        <v>138.05497481856813</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="11">
         <v>43952</v>
       </c>
-      <c r="B54" s="35">
-        <v>130.13225514839269</v>
-      </c>
-      <c r="C54" s="38">
-        <v>113.8</v>
-      </c>
-      <c r="D54" s="38">
-        <v>139.5</v>
+      <c r="B54" s="36">
+        <v>130.30963100770941</v>
+      </c>
+      <c r="C54" s="36">
+        <v>114.8263308793573</v>
+      </c>
+      <c r="D54" s="36">
+        <v>137.37686936607628</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="34">
+      <c r="A55" s="33">
         <v>43983</v>
       </c>
-      <c r="B55" s="38">
-        <v>133.52620730377282</v>
-      </c>
-      <c r="C55" s="38">
-        <v>122.9</v>
-      </c>
-      <c r="D55" s="38">
-        <v>139.1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="37" customFormat="1">
-      <c r="A56" s="34">
+      <c r="B55" s="36">
+        <v>133.78434132181565</v>
+      </c>
+      <c r="C55" s="36">
+        <v>123.75973268919545</v>
+      </c>
+      <c r="D55" s="36">
+        <v>136.76990492350836</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="35" customFormat="1">
+      <c r="A56" s="33">
         <v>44013</v>
       </c>
-      <c r="B56" s="38">
-        <v>127.1</v>
-      </c>
-      <c r="C56" s="38">
-        <v>126.4</v>
-      </c>
-      <c r="D56" s="38">
-        <v>138.80000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="37" customFormat="1">
-      <c r="A57" s="34">
+      <c r="B56" s="36">
+        <v>127.59092134022666</v>
+      </c>
+      <c r="C56" s="36">
+        <v>126.98460824930032</v>
+      </c>
+      <c r="D56" s="36">
+        <v>136.2456061431246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="35" customFormat="1">
+      <c r="A57" s="33">
         <v>44044</v>
       </c>
-      <c r="B57" s="38">
-        <v>124.8</v>
-      </c>
-      <c r="C57" s="38">
-        <v>128.4</v>
-      </c>
-      <c r="D57" s="38">
-        <v>138.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="21">
+      <c r="B57" s="36">
+        <v>125.38311528970522</v>
+      </c>
+      <c r="C57" s="36">
+        <v>128.90638362042134</v>
+      </c>
+      <c r="D57" s="36">
+        <v>135.80283112767688</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="40" customFormat="1">
+      <c r="A58" s="41">
         <v>44075</v>
       </c>
-      <c r="B58" s="39">
-        <v>125.7</v>
-      </c>
-      <c r="C58" s="39">
-        <v>130.80000000000001</v>
-      </c>
-      <c r="D58" s="39">
-        <v>138.19999999999999</v>
+      <c r="B58" s="36">
+        <v>126.60678395226415</v>
+      </c>
+      <c r="C58" s="36">
+        <v>131.56947218662361</v>
+      </c>
+      <c r="D58" s="36">
+        <v>135.43240498354692</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="11">
+        <v>44105</v>
+      </c>
+      <c r="B59" s="37">
+        <v>131.77379860345184</v>
+      </c>
+      <c r="C59" s="37">
+        <v>134.07861618184469</v>
+      </c>
+      <c r="D59" s="37">
+        <v>135.11905948666077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos comex y EMAE"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -268,9 +268,6 @@
     <t>SICA</t>
   </si>
   <si>
-    <t>NAFTA</t>
-  </si>
-  <si>
     <t>Unión Europea</t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>NACIONAL</t>
+  </si>
+  <si>
+    <t>USMCA (ex NAFTA)</t>
   </si>
 </sst>
 </file>
@@ -944,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C50" sqref="C50:E50"/>
     </sheetView>
   </sheetViews>
@@ -1823,33 +1823,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="41" t="s">
-        <v>127</v>
-      </c>
       <c r="H1" s="41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="43">
         <v>1.9</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="43">
         <v>6.4</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="43">
         <v>2.1</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="43">
         <v>2.2999999999999998</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="43">
         <v>10.4</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="43">
         <v>0.5</v>
@@ -2005,7 +2005,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="43">
         <v>-0.1</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="43">
         <v>1.5</v>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="43">
         <v>2.9</v>
@@ -3859,7 +3859,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>30.4</v>
@@ -3995,7 +3995,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="24">
         <v>39.299999999999997</v>
@@ -4599,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4627,14 +4627,14 @@
         <v>77</v>
       </c>
       <c r="B2" s="16">
-        <v>8758</v>
+        <v>966</v>
       </c>
       <c r="C2">
-        <v>10343</v>
+        <v>862</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>-1585</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4642,14 +4642,14 @@
         <v>78</v>
       </c>
       <c r="B3" s="16">
-        <v>2655</v>
+        <v>231</v>
       </c>
       <c r="C3">
-        <v>486</v>
+        <v>45</v>
       </c>
       <c r="D3" s="16">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
-        <v>2169</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4657,14 +4657,14 @@
         <v>79</v>
       </c>
       <c r="B4" s="16">
-        <v>2817</v>
+        <v>249</v>
       </c>
       <c r="C4">
-        <v>1508</v>
+        <v>158</v>
       </c>
       <c r="D4" s="16">
         <f t="shared" si="0"/>
-        <v>1309</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4672,239 +4672,239 @@
         <v>80</v>
       </c>
       <c r="B5" s="16">
-        <v>533</v>
+        <v>45</v>
       </c>
       <c r="C5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>510</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="B6" s="16">
-        <v>3866</v>
+        <v>367</v>
       </c>
       <c r="C6">
-        <v>5173</v>
+        <v>480</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>-1307</v>
+        <v>-113</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="16">
-        <v>6333</v>
+        <v>673</v>
       </c>
       <c r="C7">
-        <v>6019</v>
+        <v>679</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>314</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="16" customFormat="1">
       <c r="A8" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="16">
-        <v>542</v>
+        <v>69</v>
       </c>
       <c r="C8" s="16">
-        <v>348</v>
+        <v>42</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>194</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="16">
-        <v>958</v>
+        <v>47</v>
       </c>
       <c r="C9">
-        <v>394</v>
+        <v>37</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>564</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="16">
-        <v>661</v>
+        <v>51</v>
       </c>
       <c r="C10">
-        <v>172</v>
+        <v>11</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
-        <v>489</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="16">
-        <v>5644</v>
+        <v>509</v>
       </c>
       <c r="C11">
-        <v>2269</v>
+        <v>228</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>3375</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="16">
-        <v>5123</v>
+        <v>287</v>
       </c>
       <c r="C12">
-        <v>7677</v>
+        <v>871</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>-2554</v>
+        <v>-584</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="16">
-        <v>659</v>
+        <v>39</v>
       </c>
       <c r="C13">
-        <v>327</v>
+        <v>52</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="16">
-        <v>300</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>652</v>
+        <v>69</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>-352</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="16">
-        <v>2360</v>
+        <v>411</v>
       </c>
       <c r="C15">
-        <v>746</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="0"/>
-        <v>1614</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="16">
-        <v>2961</v>
+        <v>364</v>
       </c>
       <c r="C16">
-        <v>437</v>
+        <v>53</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="0"/>
-        <v>2524</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="16">
-        <v>2829</v>
+        <v>143</v>
       </c>
       <c r="C17">
-        <v>507</v>
+        <v>37</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
-        <v>2322</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="16">
-        <v>308</v>
+        <v>58</v>
       </c>
       <c r="C18">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
-        <v>205</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="16">
-        <v>642</v>
+        <v>78</v>
       </c>
       <c r="C19">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
-        <v>506</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="16">
-        <v>3048</v>
+        <v>313</v>
       </c>
       <c r="C20">
-        <v>1180</v>
+        <v>122</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
-        <v>1868</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4928,18 +4928,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>98</v>
-      </c>
       <c r="C1" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2">
         <v>511235.56787450501</v>
@@ -4950,7 +4950,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3">
         <v>34766.191625489824</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4">
         <v>2775.155118162565</v>
@@ -4972,7 +4972,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>19204.888120793898</v>
@@ -4983,7 +4983,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6">
         <v>106091.26662120047</v>
@@ -4994,7 +4994,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7">
         <v>12685.332330355359</v>
@@ -5005,7 +5005,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8">
         <v>16084.076127725084</v>
@@ -5016,7 +5016,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9">
         <v>82148.029517348172</v>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>4484.705522659061</v>
@@ -5038,7 +5038,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11">
         <v>44758.460785199029</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12">
         <v>26256.880008073353</v>
@@ -5060,7 +5060,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>71776.689320121382</v>
@@ -5071,7 +5071,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14">
         <v>29976.766555809754</v>
@@ -5082,7 +5082,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15">
         <v>26109.035629520033</v>
@@ -5093,7 +5093,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16">
         <v>21929.617977242029</v>
@@ -5104,7 +5104,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17">
         <v>8611.1941960524819</v>
@@ -5115,7 +5115,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18">
         <v>3577.2784187524389</v>
@@ -5131,10 +5131,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5146,16 +5146,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5166,10 +5166,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="36">
-        <v>147.40548950066798</v>
+        <v>147.50366136735829</v>
       </c>
       <c r="D2" s="36">
-        <v>147.13250454280865</v>
+        <v>147.26695403232921</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5180,10 +5180,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="36">
-        <v>147.20703967782137</v>
+        <v>147.02370380518278</v>
       </c>
       <c r="D3" s="36">
-        <v>146.59655953359194</v>
+        <v>146.72353169031206</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5194,10 +5194,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="36">
-        <v>146.49550086251253</v>
+        <v>146.40436911306105</v>
       </c>
       <c r="D4" s="36">
-        <v>146.10675364813869</v>
+        <v>146.21745577705076</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5208,10 +5208,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="36">
-        <v>144.86737682873593</v>
+        <v>144.83807002443319</v>
       </c>
       <c r="D5" s="36">
-        <v>145.69282259206</v>
+        <v>145.7810228850272</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5222,10 +5222,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="36">
-        <v>144.16229134006119</v>
+        <v>144.12929306853565</v>
       </c>
       <c r="D6" s="36">
-        <v>145.3781743875339</v>
+        <v>145.44103213177573</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5236,10 +5236,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="36">
-        <v>144.52614896411009</v>
+        <v>144.68529886288096</v>
       </c>
       <c r="D7" s="36">
-        <v>145.17975049300318</v>
+        <v>145.21797525509581</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5250,10 +5250,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="36">
-        <v>143.9570142488798</v>
+        <v>144.02283282661563</v>
       </c>
       <c r="D8" s="36">
-        <v>145.10264782100302</v>
+        <v>145.12099730130609</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5264,10 +5264,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="36">
-        <v>145.56928975620252</v>
+        <v>145.60417757461698</v>
       </c>
       <c r="D9" s="36">
-        <v>145.1441038166339</v>
+        <v>145.15040282795701</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5278,10 +5278,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="36">
-        <v>145.55360261495525</v>
+        <v>145.54393217587008</v>
       </c>
       <c r="D10" s="36">
-        <v>145.29804474277401</v>
+        <v>145.29778566623969</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5292,10 +5292,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="36">
-        <v>144.37944165217016</v>
+        <v>144.56510502187717</v>
       </c>
       <c r="D11" s="36">
-        <v>145.55243811593579</v>
+        <v>145.54707812248449</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5306,10 +5306,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="36">
-        <v>146.33104797653249</v>
+        <v>146.26101238624824</v>
       </c>
       <c r="D12" s="36">
-        <v>145.89829320034238</v>
+        <v>145.88383728436017</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5320,10 +5320,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="36">
-        <v>147.11711038131926</v>
+        <v>146.98989759133454</v>
       </c>
       <c r="D13" s="36">
-        <v>146.32335632441931</v>
+        <v>146.29347077049098</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5334,10 +5334,10 @@
         <v>136.7258774086435</v>
       </c>
       <c r="C14" s="36">
-        <v>147.51218811787277</v>
+        <v>147.51535062330427</v>
       </c>
       <c r="D14" s="36">
-        <v>146.81320009733042</v>
+        <v>146.76074754092934</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5348,10 +5348,10 @@
         <v>132.54052520440143</v>
       </c>
       <c r="C15" s="36">
-        <v>146.55590467771026</v>
+        <v>146.37304725211661</v>
       </c>
       <c r="D15" s="36">
-        <v>147.35155431110869</v>
+        <v>147.27262522190304</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5362,10 +5362,10 @@
         <v>152.145731768997</v>
       </c>
       <c r="C16" s="36">
-        <v>148.40751251194064</v>
+        <v>148.35561691806086</v>
       </c>
       <c r="D16" s="36">
-        <v>147.92438453421599</v>
+        <v>147.81845720436331</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5376,10 +5376,10 @@
         <v>152.20883250679566</v>
       </c>
       <c r="C17" s="36">
-        <v>147.23855198711274</v>
+        <v>147.15670753095645</v>
       </c>
       <c r="D17" s="36">
-        <v>148.51514759345517</v>
+        <v>148.38708067860398</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5390,10 +5390,10 @@
         <v>167.46154818637638</v>
       </c>
       <c r="C18" s="36">
-        <v>148.65798864877942</v>
+        <v>148.59204857162541</v>
       </c>
       <c r="D18" s="36">
-        <v>149.10525330454533</v>
+        <v>148.9628232751173</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5404,10 +5404,10 @@
         <v>161.70085905013559</v>
       </c>
       <c r="C19" s="36">
-        <v>150.07422709343567</v>
+        <v>150.46755677901072</v>
       </c>
       <c r="D19" s="36">
-        <v>149.66871892773509</v>
+        <v>149.5223851184582</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5418,10 +5418,10 @@
         <v>149.78297310853262</v>
       </c>
       <c r="C20" s="36">
-        <v>149.7069308868486</v>
+        <v>149.791259710465</v>
       </c>
       <c r="D20" s="36">
-        <v>150.17360583142343</v>
+        <v>150.03477671839531</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5432,10 +5432,10 @@
         <v>149.4590923353316</v>
       </c>
       <c r="C21" s="36">
-        <v>150.48723167737793</v>
+        <v>150.55431191737475</v>
       </c>
       <c r="D21" s="36">
-        <v>150.58343827682742</v>
+        <v>150.46175673264949</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5446,10 +5446,10 @@
         <v>146.70588711165021</v>
       </c>
       <c r="C22" s="36">
-        <v>151.51617685809143</v>
+        <v>151.50859687720134</v>
       </c>
       <c r="D22" s="36">
-        <v>150.86176489297546</v>
+        <v>150.76480595560452</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5460,10 +5460,10 @@
         <v>149.62906247744323</v>
       </c>
       <c r="C23" s="36">
-        <v>151.06711826752945</v>
+        <v>151.27000420642045</v>
       </c>
       <c r="D23" s="36">
-        <v>150.9773097525821</v>
+        <v>150.90964926794558</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5474,10 +5474,10 @@
         <v>152.38283025725997</v>
       </c>
       <c r="C24" s="36">
-        <v>153.23666431612583</v>
+        <v>153.12874692680333</v>
       </c>
       <c r="D24" s="36">
-        <v>150.9056274896343</v>
+        <v>150.86891363468686</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5488,10 +5488,10 @@
         <v>146.08348469256237</v>
       </c>
       <c r="C25" s="36">
-        <v>152.36620932056729</v>
+        <v>152.11345706448907</v>
       </c>
       <c r="D25" s="36">
-        <v>150.63658635205991</v>
+        <v>150.62706819395316</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5502,10 +5502,10 @@
         <v>142.64696239584413</v>
       </c>
       <c r="C26" s="36">
-        <v>152.48102197832938</v>
+        <v>152.3761260357814</v>
       </c>
       <c r="D26" s="36">
-        <v>150.17417863869139</v>
+        <v>150.18379417951783</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5516,10 +5516,10 @@
         <v>139.07181989111268</v>
       </c>
       <c r="C27" s="36">
-        <v>151.96713501492289</v>
+        <v>151.76466629226593</v>
       </c>
       <c r="D27" s="36">
-        <v>149.53476628845246</v>
+        <v>149.5534144027672</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5530,10 +5530,10 @@
         <v>155.63982283229944</v>
       </c>
       <c r="C28" s="36">
-        <v>151.9446848815268</v>
+        <v>151.88842379784495</v>
       </c>
       <c r="D28" s="36">
-        <v>148.74914090221233</v>
+        <v>148.76630112172487</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5544,10 +5544,10 @@
         <v>151.60135644382305</v>
       </c>
       <c r="C29" s="36">
-        <v>146.63322601094779</v>
+        <v>146.51299704538707</v>
       </c>
       <c r="D29" s="36">
-        <v>147.86111794804336</v>
+        <v>147.86885420425369</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5558,10 +5558,10 @@
         <v>159.16207548226589</v>
       </c>
       <c r="C30" s="36">
-        <v>144.34065398200235</v>
+        <v>144.31159019760548</v>
       </c>
       <c r="D30" s="36">
-        <v>146.92485841421757</v>
+        <v>146.91981307129296</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5572,10 +5572,10 @@
         <v>151.44848091721315</v>
       </c>
       <c r="C31" s="36">
-        <v>142.37750732217762</v>
+        <v>142.86390930633337</v>
       </c>
       <c r="D31" s="36">
-        <v>145.99344925825582</v>
+        <v>145.9776117258746</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5586,10 +5586,10 @@
         <v>145.76463042864052</v>
       </c>
       <c r="C32" s="36">
-        <v>143.36897326244727</v>
+        <v>143.51103174224647</v>
       </c>
       <c r="D32" s="36">
-        <v>145.11713487580218</v>
+        <v>145.09736764432378</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5600,10 +5600,10 @@
         <v>147.04553382400547</v>
       </c>
       <c r="C33" s="36">
-        <v>146.90927549984139</v>
+        <v>147.07492972620685</v>
       </c>
       <c r="D33" s="36">
-        <v>144.34259028880226</v>
+        <v>144.32505800877667</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5614,10 +5614,10 @@
         <v>137.8944988928931</v>
       </c>
       <c r="C34" s="36">
-        <v>142.5846849297898</v>
+        <v>142.70950611308439</v>
       </c>
       <c r="D34" s="36">
-        <v>143.70319907946219</v>
+        <v>143.69062347352028</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5628,10 +5628,10 @@
         <v>143.57320349337792</v>
       </c>
       <c r="C35" s="36">
-        <v>143.7134503260327</v>
+        <v>143.9576170743249</v>
       </c>
       <c r="D35" s="36">
-        <v>143.21634302411266</v>
+        <v>143.21026302969139</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5642,10 +5642,10 @@
         <v>141.21184890028576</v>
       </c>
       <c r="C36" s="36">
-        <v>142.37778125739862</v>
+        <v>142.1920417058401</v>
       </c>
       <c r="D36" s="36">
-        <v>142.88711354506074</v>
+        <v>142.88783700447289</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5656,10 +5656,10 @@
         <v>135.67154302632184</v>
       </c>
       <c r="C37" s="36">
-        <v>142.03338231137309</v>
+        <v>141.56893775394471</v>
       </c>
       <c r="D37" s="36">
-        <v>142.70534829565807</v>
+        <v>142.71104009201966</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5670,10 +5670,10 @@
         <v>134.564995313265</v>
       </c>
       <c r="C38" s="36">
-        <v>143.68095342507036</v>
+        <v>143.59497920094438</v>
       </c>
       <c r="D38" s="36">
-        <v>142.64695346044655</v>
+        <v>142.65777508550403</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5684,10 +5684,10 @@
         <v>132.57194718265788</v>
       </c>
       <c r="C39" s="36">
-        <v>143.65413385641389</v>
+        <v>143.51872512882031</v>
       </c>
       <c r="D39" s="36">
-        <v>142.68020665901747</v>
+        <v>142.69507237886896</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5698,10 +5698,10 @@
         <v>144.41715750575651</v>
       </c>
       <c r="C40" s="36">
-        <v>141.7116403310888</v>
+        <v>141.72151927438549</v>
       </c>
       <c r="D40" s="36">
-        <v>142.76867441729735</v>
+        <v>142.78366755840281</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5712,10 +5712,10 @@
         <v>149.83961931661509</v>
       </c>
       <c r="C41" s="36">
-        <v>142.30963439168579</v>
+        <v>142.16827581960777</v>
       </c>
       <c r="D41" s="36">
-        <v>142.87406175831902</v>
+        <v>142.88210837577913</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5726,10 +5726,10 @@
         <v>162.83974753189364</v>
       </c>
       <c r="C42" s="36">
-        <v>143.4153404616502</v>
+        <v>143.40456178237028</v>
       </c>
       <c r="D42" s="36">
-        <v>142.95895938660107</v>
+        <v>142.95218448938178</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5740,10 +5740,10 @@
         <v>151.25410111244764</v>
       </c>
       <c r="C43" s="36">
-        <v>141.83527490443359</v>
+        <v>142.64281375661039</v>
       </c>
       <c r="D43" s="36">
-        <v>142.9890906382563</v>
+        <v>142.95897712659476</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5754,10 +5754,10 @@
         <v>146.20323233619627</v>
       </c>
       <c r="C44" s="36">
-        <v>145.37887579033358</v>
+        <v>145.65505957835799</v>
       </c>
       <c r="D44" s="36">
-        <v>142.93518580755071</v>
+        <v>142.87079460778091</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5768,10 +5768,10 @@
         <v>141.60332874981128</v>
       </c>
       <c r="C45" s="36">
-        <v>144.68319699058412</v>
+        <v>145.05869311071385</v>
       </c>
       <c r="D45" s="36">
-        <v>142.77510427768922</v>
+        <v>142.66388623182772</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -5782,10 +5782,10 @@
         <v>135.07531285730843</v>
       </c>
       <c r="C46" s="36">
-        <v>140.87136147533508</v>
+        <v>141.07722855232893</v>
       </c>
       <c r="D46" s="36">
-        <v>142.49559665045726</v>
+        <v>142.32562087371397</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -5796,10 +5796,10 @@
         <v>142.25579775531418</v>
       </c>
       <c r="C47" s="36">
-        <v>143.54587561429835</v>
+        <v>143.7591652324204</v>
       </c>
       <c r="D47" s="36">
-        <v>142.0935891603549</v>
+        <v>141.85770467168294</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -5810,10 +5810,10 @@
         <v>138.14131943492291</v>
       </c>
       <c r="C48" s="36">
-        <v>141.48456225642059</v>
+        <v>140.8981273775014</v>
       </c>
       <c r="D48" s="36">
-        <v>141.57666211619394</v>
+        <v>141.27379611655988</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -5824,10 +5824,10 @@
         <v>135.44751977320297</v>
       </c>
       <c r="C49" s="36">
-        <v>141.60538984918296</v>
+        <v>140.67708825755284</v>
       </c>
       <c r="D49" s="36">
-        <v>140.96179182233465</v>
+        <v>140.59524617392546</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -5838,10 +5838,10 @@
         <v>132.19356455544042</v>
       </c>
       <c r="C50" s="36">
-        <v>141.78898143893696</v>
+        <v>141.36247287892007</v>
       </c>
       <c r="D50" s="36">
-        <v>140.26998289408365</v>
+        <v>139.85375458352752</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -5852,10 +5852,10 @@
         <v>129.61940932164029</v>
       </c>
       <c r="C51" s="36">
-        <v>141.09355092898466</v>
+        <v>140.61363722120234</v>
       </c>
       <c r="D51" s="36">
-        <v>139.53221814376042</v>
+        <v>139.09025370190088</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -5866,10 +5866,10 @@
         <v>128.38599328767583</v>
       </c>
       <c r="C52" s="36">
-        <v>126.21616702827959</v>
+        <v>125.89743278341957</v>
       </c>
       <c r="D52" s="36">
-        <v>138.78278265769444</v>
+        <v>138.3495869410784</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5880,10 +5880,10 @@
         <v>111.81827837013516</v>
       </c>
       <c r="C53" s="36">
-        <v>105.02543573540743</v>
+        <v>104.49629251825432</v>
       </c>
       <c r="D53" s="36">
-        <v>138.05497481856813</v>
+        <v>137.67467355466158</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -5894,10 +5894,10 @@
         <v>130.30963100770941</v>
       </c>
       <c r="C54" s="36">
-        <v>114.8263308793573</v>
+        <v>114.4239832590922</v>
       </c>
       <c r="D54" s="36">
-        <v>137.37686936607628</v>
+        <v>137.10398856958534</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -5908,10 +5908,10 @@
         <v>133.78434132181565</v>
       </c>
       <c r="C55" s="36">
-        <v>123.75973268919545</v>
+        <v>124.10816144121733</v>
       </c>
       <c r="D55" s="36">
-        <v>136.76990492350836</v>
+        <v>136.6653725095332</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="35" customFormat="1">
@@ -5922,10 +5922,10 @@
         <v>127.59092134022666</v>
       </c>
       <c r="C56" s="36">
-        <v>126.98460824930032</v>
+        <v>126.88426923698418</v>
       </c>
       <c r="D56" s="36">
-        <v>136.2456061431246</v>
+        <v>136.37104387236846</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="35" customFormat="1">
@@ -5936,10 +5936,10 @@
         <v>125.23224811923698</v>
       </c>
       <c r="C57" s="36">
-        <v>128.76234313823264</v>
+        <v>128.80156224686681</v>
       </c>
       <c r="D57" s="36">
-        <v>136.77872142062364</v>
+        <v>136.21398528279471</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="39" customFormat="1">
@@ -5950,10 +5950,10 @@
         <v>126.7092687596504</v>
       </c>
       <c r="C58" s="36">
-        <v>131.68105422539981</v>
+        <v>131.66307506776914</v>
       </c>
       <c r="D58" s="36">
-        <v>136.74238299189349</v>
+        <v>136.17613336672702</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -5964,24 +5964,38 @@
         <v>131.93155629327126</v>
       </c>
       <c r="C59" s="36">
-        <v>134.42700197395715</v>
+        <v>133.29338742400111</v>
       </c>
       <c r="D59" s="36">
-        <v>136.78025829111635</v>
+        <v>136.22833446787479</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="40">
         <v>44136</v>
       </c>
-      <c r="B60" s="37">
+      <c r="B60" s="36">
         <v>133.07361620887411</v>
       </c>
-      <c r="C60" s="37">
-        <v>136.31136575460536</v>
-      </c>
-      <c r="D60" s="37">
-        <v>136.85395184572889</v>
+      <c r="C60" s="36">
+        <v>135.13500852588487</v>
+      </c>
+      <c r="D60" s="36">
+        <v>136.3336184218339</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="24" customFormat="1">
+      <c r="A61" s="40">
+        <v>44166</v>
+      </c>
+      <c r="B61" s="37">
+        <v>132.44891764985255</v>
+      </c>
+      <c r="C61" s="37">
+        <v>136.41144179336155</v>
+      </c>
+      <c r="D61" s="37">
+        <v>136.45668119301254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Datos de Pobreza e Indigencia"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -610,7 +610,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,6 +642,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1837,262 +1838,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="45">
         <v>3.9</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="45">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="45">
         <v>4.5</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="45">
         <v>5</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="45">
         <v>5.4</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="45">
         <v>3.6</v>
       </c>
-      <c r="H2" s="35">
+      <c r="H2" s="34">
         <v>4.2171947754954697</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>2.7</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <v>2.6</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="45">
         <v>2.1</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="45">
         <v>3.8</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="45">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="45">
         <v>5.4</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="34">
         <v>2.8105374101642822</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>2.1</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>3.4</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>3.1</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>3.1</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="34">
         <v>2.8708072425776665</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>2.5</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>7.3</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="45">
         <v>15.9</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>8.9</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>6.2</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <v>8.6</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="34">
         <v>5.8933864340036335</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>7.9</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <v>4.8</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <v>10.9</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <v>7.4</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="45">
         <v>6.1</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>5.5</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="34">
         <v>6.7522580441937485</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>9.6</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>1.3</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="45">
         <v>2</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>3.7</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>1.3</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="34">
         <v>6.0632428064291144</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>3.4</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="45">
         <v>2.5</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="45">
         <v>3.1</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <v>3.3</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="45">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="35">
         <v>3.1517267253622583</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>5.4</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <v>5.2</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>4.8</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <v>6.5</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="34">
         <v>5.0040360696807396</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>3</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="45">
         <v>3.5</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="45">
         <v>3</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="45">
         <v>2.6</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>3.1</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="45">
         <v>4.3</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="34">
         <v>3.251614386284718</v>
       </c>
     </row>
@@ -2141,25 +2142,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="37">
         <v>3.6</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="40">
         <v>3.6</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>3.4</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="42">
         <v>3.8</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="42">
         <v>3.3</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H2" s="43">
+      <c r="H2" s="42">
         <v>3.9</v>
       </c>
     </row>
@@ -2167,25 +2168,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="38">
         <v>3.8</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>4</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="38">
         <v>3.6</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="39">
         <v>3.7</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="39">
         <v>3.9</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="39">
         <v>3.6</v>
       </c>
-      <c r="H3" s="40">
+      <c r="H3" s="39">
         <v>4.5</v>
       </c>
     </row>
@@ -2193,25 +2194,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="38">
         <v>3.6</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="41">
         <v>3.6</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="38">
         <v>3.4</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="39">
         <v>3</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="39">
         <v>4</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="39">
         <v>3.9</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="39">
         <v>3.9</v>
       </c>
     </row>
@@ -2219,25 +2220,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="38">
         <v>2.8</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="41">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="38">
         <v>3.1</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="39">
         <v>3.7</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="39">
         <v>2.4</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="39">
         <v>4.8</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="39">
         <v>3.5</v>
       </c>
     </row>
@@ -2245,25 +2246,25 @@
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="39">
         <v>2</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="41">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="38">
         <v>1.6</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="39">
         <v>1.3</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="39">
         <v>0.8</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="39">
         <v>5.8</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="39">
         <v>1.5</v>
       </c>
     </row>
@@ -2271,25 +2272,25 @@
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="38">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="41">
         <v>5</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="38">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="39">
         <v>4.2</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="39">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="39">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="39">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -2297,25 +2298,25 @@
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="38">
         <v>3.5</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="41">
         <v>2.9</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="38">
         <v>3.6</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="39">
         <v>6.3</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="39">
         <v>3.2</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="39">
         <v>3.8</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8" s="39">
         <v>4.7</v>
       </c>
     </row>
@@ -2323,25 +2324,25 @@
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="38">
         <v>4.8</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="41">
         <v>4.8</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="38">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="39">
         <v>4.8</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="39">
         <v>5.7</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="39">
         <v>4.3</v>
       </c>
     </row>
@@ -2349,25 +2350,25 @@
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="38">
         <v>1.8</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="41">
         <v>1</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="38">
         <v>2.9</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <v>3.3</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="39">
         <v>1.5</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="39">
         <v>1.2</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="39">
         <v>2.8</v>
       </c>
     </row>
@@ -2375,25 +2376,25 @@
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="38">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="41">
         <v>2.7</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>1.6</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="39">
         <v>2.8</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="39">
         <v>2.6</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="39">
         <v>0.9</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="39">
         <v>4.2</v>
       </c>
     </row>
@@ -2401,25 +2402,25 @@
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="38">
         <v>0.1</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="41">
         <v>0</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="38">
         <v>0.1</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="39">
         <v>1.7</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="39">
         <v>0.1</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="39">
         <v>0</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="39">
         <v>0</v>
       </c>
     </row>
@@ -2427,25 +2428,25 @@
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="38">
         <v>5.4</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="41">
         <v>5.8</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>5.2</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="39">
         <v>5.8</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="39">
         <v>3.9</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="39">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="39">
         <v>5.2</v>
       </c>
     </row>
@@ -2453,25 +2454,25 @@
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="38">
         <v>3.2</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="41">
         <v>3.3</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="38">
         <v>3.3</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="39">
         <v>2.8</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="39">
         <v>2.5</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="39">
         <v>4</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="39">
         <v>2.6</v>
       </c>
     </row>
@@ -2521,25 +2522,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="44">
         <v>40.700000000000003</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="44">
         <v>38.299999999999997</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="44">
         <v>42.4</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="44">
         <v>46.1</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="44">
         <v>44.3</v>
       </c>
-      <c r="G2" s="45">
+      <c r="G2" s="44">
         <v>42.8</v>
       </c>
-      <c r="H2" s="45">
+      <c r="H2" s="44">
         <v>37.1</v>
       </c>
     </row>
@@ -2547,25 +2548,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="43">
         <v>43.9</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="43">
         <v>39.6</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="43">
         <v>47.5</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="43">
         <v>52.5</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="43">
         <v>49.5</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="43">
         <v>45.9</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="43">
         <v>38.4</v>
       </c>
     </row>
@@ -2573,25 +2574,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="43">
         <v>36.299999999999997</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="43">
         <v>34.799999999999997</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="43">
         <v>37</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="43">
         <v>39</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="43">
         <v>39.200000000000003</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="43">
         <v>37.6</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="43">
         <v>36.5</v>
       </c>
     </row>
@@ -2599,25 +2600,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="43">
         <v>61.2</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="43">
         <v>59.3</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="43">
         <v>63.2</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="43">
         <v>56.8</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="43">
         <v>68.400000000000006</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <v>71</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="43">
         <v>47.5</v>
       </c>
     </row>
@@ -2625,25 +2626,25 @@
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="43">
         <v>19.8</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="43">
         <v>18.600000000000001</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="43">
         <v>21</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="43">
         <v>19.7</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="43">
         <v>18.899999999999999</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="43">
         <v>25</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="43">
         <v>18.8</v>
       </c>
     </row>
@@ -2651,25 +2652,25 @@
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="43">
         <v>47.1</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="43">
         <v>48.5</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="43">
         <v>44.5</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="43">
         <v>54.5</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="43">
         <v>47</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="43">
         <v>44.7</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="43">
         <v>48.6</v>
       </c>
     </row>
@@ -2677,25 +2678,25 @@
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="43">
         <v>39.799999999999997</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="43">
         <v>35</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="43">
         <v>42.1</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="43">
         <v>51.3</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="43">
         <v>47.6</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="43">
         <v>44</v>
       </c>
-      <c r="H8" s="44">
+      <c r="H8" s="43">
         <v>40.6</v>
       </c>
     </row>
@@ -2703,25 +2704,25 @@
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="43">
         <v>42.7</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="43">
         <v>41.3</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="43">
         <v>44.3</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="43">
         <v>44.5</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="43">
         <v>39.700000000000003</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="43">
         <v>45.6</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="43">
         <v>43.8</v>
       </c>
     </row>
@@ -2729,25 +2730,25 @@
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="43">
         <v>23.1</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="43">
         <v>23.7</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="43">
         <v>21.2</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="43">
         <v>26.1</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="43">
         <v>24.5</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="43">
         <v>24.6</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="43">
         <v>26</v>
       </c>
     </row>
@@ -2755,25 +2756,25 @@
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="43">
         <v>47.9</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <v>50.5</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="43">
         <v>48.2</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="43">
         <v>49.7</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="43">
         <v>43.5</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="43">
         <v>35.9</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="43">
         <v>41.3</v>
       </c>
     </row>
@@ -2781,25 +2782,25 @@
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="43">
         <v>18.600000000000001</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="43">
         <v>16.8</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="43">
         <v>18.100000000000001</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="43">
         <v>21.1</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="43">
         <v>29.3</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="43">
         <v>23.8</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="43">
         <v>14.7</v>
       </c>
     </row>
@@ -2807,25 +2808,25 @@
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="43">
         <v>41</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="43">
         <v>41.4</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="43">
         <v>40.6</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="43">
         <v>45.2</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="43">
         <v>42</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="43">
         <v>44.2</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="43">
         <v>30.3</v>
       </c>
     </row>
@@ -2833,25 +2834,25 @@
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="43">
         <v>26.3</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="43">
         <v>29.8</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="43">
         <v>24</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="43">
         <v>25.2</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="43">
         <v>25</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="43">
         <v>23.4</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="43">
         <v>18.600000000000001</v>
       </c>
     </row>
@@ -3816,7 +3817,7 @@
       <c r="A68" s="12">
         <v>2020</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C68" s="12">
@@ -3827,10 +3828,10 @@
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="37">
+      <c r="A69" s="36">
         <v>2020</v>
       </c>
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C69" s="12">
@@ -3850,8 +3851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3863,14 +3864,14 @@
       <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="47"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -3892,13 +3893,13 @@
         <v>120</v>
       </c>
       <c r="B3">
-        <v>30.4</v>
+        <v>31.6</v>
       </c>
       <c r="C3">
-        <v>40.9</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="E3">
         <v>10.5</v>
@@ -3909,16 +3910,16 @@
         <v>34</v>
       </c>
       <c r="B4" s="24">
-        <v>11.3</v>
+        <v>12.2</v>
       </c>
       <c r="C4" s="24">
-        <v>17.3</v>
+        <v>16.5</v>
       </c>
       <c r="D4" s="24">
-        <v>3.1</v>
+        <v>3.9</v>
       </c>
       <c r="E4" s="24">
-        <v>3.7</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3926,16 +3927,16 @@
         <v>35</v>
       </c>
       <c r="B5" s="24">
-        <v>37.5</v>
+        <v>40.9</v>
       </c>
       <c r="C5" s="24">
-        <v>47.5</v>
+        <v>51</v>
       </c>
       <c r="D5" s="24">
-        <v>11</v>
+        <v>11.8</v>
       </c>
       <c r="E5" s="24">
-        <v>13.6</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3943,16 +3944,16 @@
         <v>62</v>
       </c>
       <c r="B6" s="24">
-        <v>31</v>
+        <v>32.6</v>
       </c>
       <c r="C6" s="24">
-        <v>41.5</v>
+        <v>44</v>
       </c>
       <c r="D6" s="24">
-        <v>6.9</v>
+        <v>5.4</v>
       </c>
       <c r="E6" s="24">
-        <v>8.8000000000000007</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3960,16 +3961,16 @@
         <v>63</v>
       </c>
       <c r="B7" s="24">
-        <v>25.5</v>
+        <v>24.9</v>
       </c>
       <c r="C7" s="24">
-        <v>35.799999999999997</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="D7" s="24">
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="E7" s="24">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3977,16 +3978,16 @@
         <v>36</v>
       </c>
       <c r="B8" s="24">
-        <v>29.5</v>
+        <v>32.4</v>
       </c>
       <c r="C8" s="24">
-        <v>39.200000000000003</v>
+        <v>40.6</v>
       </c>
       <c r="D8" s="24">
-        <v>4.4000000000000004</v>
+        <v>3.5</v>
       </c>
       <c r="E8" s="24">
-        <v>6.3</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3994,16 +3995,16 @@
         <v>37</v>
       </c>
       <c r="B9" s="24">
-        <v>32.799999999999997</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="C9" s="24">
-        <v>41.2</v>
+        <v>42.9</v>
       </c>
       <c r="D9" s="24">
-        <v>8.8000000000000007</v>
+        <v>6.7</v>
       </c>
       <c r="E9" s="24">
-        <v>11.8</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4011,16 +4012,16 @@
         <v>38</v>
       </c>
       <c r="B10" s="24">
-        <v>35.200000000000003</v>
+        <v>25.7</v>
       </c>
       <c r="C10" s="24">
-        <v>42.4</v>
+        <v>36.4</v>
       </c>
       <c r="D10" s="24">
-        <v>7.1</v>
+        <v>2.5</v>
       </c>
       <c r="E10" s="24">
-        <v>8.8000000000000007</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4028,16 +4029,16 @@
         <v>95</v>
       </c>
       <c r="B11" s="24">
-        <v>39.299999999999997</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="C11" s="26">
-        <v>48.7</v>
+        <v>53.6</v>
       </c>
       <c r="D11" s="24">
-        <v>13.8</v>
+        <v>8</v>
       </c>
       <c r="E11" s="24">
-        <v>18.2</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4045,16 +4046,16 @@
         <v>39</v>
       </c>
       <c r="B12" s="24">
-        <v>27.1</v>
+        <v>27.6</v>
       </c>
       <c r="C12" s="24">
-        <v>38.1</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="D12" s="24">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
       <c r="E12" s="24">
-        <v>5.0999999999999996</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4062,16 +4063,16 @@
         <v>40</v>
       </c>
       <c r="B13" s="24">
-        <v>27.6</v>
+        <v>28.7</v>
       </c>
       <c r="C13" s="24">
-        <v>35.200000000000003</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="D13" s="24">
-        <v>6.1</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E13" s="24">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4079,16 +4080,16 @@
         <v>41</v>
       </c>
       <c r="B14" s="24">
-        <v>31.2</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="C14" s="24">
-        <v>41.5</v>
+        <v>43.5</v>
       </c>
       <c r="D14" s="24">
-        <v>7.3</v>
+        <v>5.7</v>
       </c>
       <c r="E14" s="24">
-        <v>8.1</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4096,16 +4097,16 @@
         <v>42</v>
       </c>
       <c r="B15" s="24">
-        <v>28.6</v>
+        <v>27.4</v>
       </c>
       <c r="C15" s="24">
-        <v>38</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="D15" s="24">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="E15" s="24">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4113,16 +4114,16 @@
         <v>64</v>
       </c>
       <c r="B16" s="24">
-        <v>20.9</v>
+        <v>25.3</v>
       </c>
       <c r="C16" s="24">
-        <v>29.8</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D16" s="24">
-        <v>1.9</v>
+        <v>3.2</v>
       </c>
       <c r="E16" s="24">
-        <v>2.7</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4130,16 +4131,16 @@
         <v>43</v>
       </c>
       <c r="B17" s="24">
-        <v>35.799999999999997</v>
+        <v>31.2</v>
       </c>
       <c r="C17" s="24">
-        <v>45.5</v>
+        <v>41.7</v>
       </c>
       <c r="D17" s="24">
-        <v>9.6</v>
+        <v>7.8</v>
       </c>
       <c r="E17" s="24">
-        <v>11.4</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4147,16 +4148,16 @@
         <v>65</v>
       </c>
       <c r="B18" s="24">
-        <v>34.1</v>
+        <v>31.4</v>
       </c>
       <c r="C18" s="24">
-        <v>42.9</v>
+        <v>39.4</v>
       </c>
       <c r="D18" s="24">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="E18" s="24">
-        <v>7.5</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4164,16 +4165,16 @@
         <v>45</v>
       </c>
       <c r="B19" s="24">
-        <v>23.2</v>
+        <v>18.7</v>
       </c>
       <c r="C19" s="24">
-        <v>33.700000000000003</v>
+        <v>24</v>
       </c>
       <c r="D19" s="24">
-        <v>3.2</v>
+        <v>5.2</v>
       </c>
       <c r="E19" s="24">
-        <v>4.4000000000000004</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -4181,16 +4182,16 @@
         <v>66</v>
       </c>
       <c r="B20" s="24">
-        <v>40.6</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="C20" s="24">
-        <v>52.2</v>
+        <v>49.5</v>
       </c>
       <c r="D20" s="24">
-        <v>8.4</v>
+        <v>6.6</v>
       </c>
       <c r="E20" s="24">
-        <v>12</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4198,16 +4199,16 @@
         <v>46</v>
       </c>
       <c r="B21" s="24">
-        <v>28.2</v>
+        <v>29.5</v>
       </c>
       <c r="C21" s="24">
-        <v>40.700000000000003</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="D21" s="24">
-        <v>5.6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E21" s="24">
-        <v>8.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4215,16 +4216,16 @@
         <v>47</v>
       </c>
       <c r="B22" s="24">
-        <v>27.7</v>
+        <v>24</v>
       </c>
       <c r="C22" s="24">
-        <v>37.4</v>
+        <v>31.7</v>
       </c>
       <c r="D22" s="24">
-        <v>6.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E22" s="24">
-        <v>9.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -4232,16 +4233,16 @@
         <v>48</v>
       </c>
       <c r="B23" s="24">
-        <v>30.6</v>
+        <v>29.1</v>
       </c>
       <c r="C23" s="24">
-        <v>41.8</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="D23" s="24">
-        <v>9.6999999999999993</v>
+        <v>5.8</v>
       </c>
       <c r="E23" s="24">
-        <v>13.3</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -4249,16 +4250,16 @@
         <v>61</v>
       </c>
       <c r="B24" s="24">
-        <v>26.6</v>
+        <v>30.4</v>
       </c>
       <c r="C24" s="24">
-        <v>36.299999999999997</v>
+        <v>40.9</v>
       </c>
       <c r="D24" s="24">
-        <v>5.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="E24" s="24">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -4266,16 +4267,16 @@
         <v>49</v>
       </c>
       <c r="B25" s="24">
-        <v>30.4</v>
+        <v>28</v>
       </c>
       <c r="C25" s="24">
-        <v>42.6</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D25" s="24">
-        <v>7.1</v>
+        <v>6</v>
       </c>
       <c r="E25" s="24">
-        <v>10.9</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -4283,16 +4284,16 @@
         <v>50</v>
       </c>
       <c r="B26" s="24">
-        <v>30.8</v>
+        <v>30.5</v>
       </c>
       <c r="C26" s="24">
-        <v>38.9</v>
+        <v>41.1</v>
       </c>
       <c r="D26" s="24">
-        <v>9.6999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="E26" s="24">
-        <v>12</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4300,16 +4301,16 @@
         <v>51</v>
       </c>
       <c r="B27" s="24">
-        <v>25.2</v>
+        <v>27.2</v>
       </c>
       <c r="C27" s="24">
-        <v>34.799999999999997</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="D27" s="24">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
       <c r="E27" s="24">
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4317,16 +4318,16 @@
         <v>52</v>
       </c>
       <c r="B28" s="24">
-        <v>22.2</v>
+        <v>24.9</v>
       </c>
       <c r="C28" s="24">
-        <v>32.799999999999997</v>
+        <v>33.5</v>
       </c>
       <c r="D28" s="24">
-        <v>6.4</v>
+        <v>5</v>
       </c>
       <c r="E28" s="24">
-        <v>8.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -4334,16 +4335,16 @@
         <v>59</v>
       </c>
       <c r="B29" s="24">
-        <v>29.8</v>
+        <v>32.4</v>
       </c>
       <c r="C29" s="24">
-        <v>39.799999999999997</v>
+        <v>43.6</v>
       </c>
       <c r="D29" s="24">
-        <v>7.4</v>
+        <v>6.6</v>
       </c>
       <c r="E29" s="24">
-        <v>10.199999999999999</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -4351,16 +4352,16 @@
         <v>54</v>
       </c>
       <c r="B30" s="24">
-        <v>26.9</v>
+        <v>24</v>
       </c>
       <c r="C30" s="24">
-        <v>34.9</v>
+        <v>31.7</v>
       </c>
       <c r="D30" s="24">
-        <v>5.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E30" s="24">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4368,16 +4369,16 @@
         <v>55</v>
       </c>
       <c r="B31" s="24">
-        <v>28.4</v>
+        <v>32.1</v>
       </c>
       <c r="C31" s="24">
-        <v>37.5</v>
+        <v>40.4</v>
       </c>
       <c r="D31" s="24">
-        <v>4.0999999999999996</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E31" s="24">
-        <v>5.2</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -4385,50 +4386,42 @@
         <v>56</v>
       </c>
       <c r="B32" s="24">
-        <v>21.9</v>
+        <v>26</v>
       </c>
       <c r="C32" s="24">
-        <v>28.7</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="D32" s="24">
-        <v>3.6</v>
+        <v>6.5</v>
       </c>
       <c r="E32" s="24">
-        <v>4.0999999999999996</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="24">
-        <v>28.4</v>
-      </c>
-      <c r="C33" s="24">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="D33" s="24">
-        <v>7.5</v>
-      </c>
-      <c r="E33" s="24">
-        <v>9.8000000000000007</v>
-      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>60</v>
       </c>
       <c r="B34" s="24">
-        <v>28.5</v>
+        <v>25.2</v>
       </c>
       <c r="C34" s="24">
-        <v>39.700000000000003</v>
+        <v>32</v>
       </c>
       <c r="D34" s="24">
-        <v>7.5</v>
+        <v>5.9</v>
       </c>
       <c r="E34" s="24">
-        <v>8.3000000000000007</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -4436,16 +4429,16 @@
         <v>58</v>
       </c>
       <c r="B35" s="24">
-        <v>30.1</v>
+        <v>25.2</v>
       </c>
       <c r="C35" s="24">
-        <v>43.5</v>
+        <v>35.1</v>
       </c>
       <c r="D35" s="24">
-        <v>4.7</v>
+        <v>3.8</v>
       </c>
       <c r="E35" s="24">
-        <v>6.2</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -4474,14 +4467,14 @@
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="47"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4502,13 +4495,13 @@
         <v>69</v>
       </c>
       <c r="B3" s="24">
-        <v>30.4</v>
+        <v>31.6</v>
       </c>
       <c r="C3" s="24">
-        <v>40.9</v>
+        <v>42</v>
       </c>
       <c r="D3" s="24">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="E3" s="24">
         <v>10.5</v>
@@ -4519,16 +4512,16 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>29.2</v>
+        <v>30.4</v>
       </c>
       <c r="C4">
-        <v>39.5</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="D4">
-        <v>5.7</v>
+        <v>4.5</v>
       </c>
       <c r="E4">
-        <v>7.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4536,16 +4529,16 @@
         <v>33</v>
       </c>
       <c r="B5">
-        <v>31.1</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="C5">
-        <v>41.6</v>
+        <v>44.3</v>
       </c>
       <c r="D5">
-        <v>9.1</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E5">
-        <v>11.7</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4553,16 +4546,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>33.5</v>
+        <v>32.1</v>
       </c>
       <c r="C6">
-        <v>42.8</v>
+        <v>43.5</v>
       </c>
       <c r="D6">
-        <v>8.5</v>
+        <v>5.4</v>
       </c>
       <c r="E6">
-        <v>11.4</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4570,16 +4563,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>31.2</v>
+        <v>30.9</v>
       </c>
       <c r="C7">
-        <v>40.700000000000003</v>
+        <v>40.4</v>
       </c>
       <c r="D7">
-        <v>6.5</v>
+        <v>5.2</v>
       </c>
       <c r="E7">
-        <v>7.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4587,16 +4580,16 @@
         <v>44</v>
       </c>
       <c r="B8">
-        <v>28.8</v>
+        <v>28.2</v>
       </c>
       <c r="C8">
-        <v>39.799999999999997</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="D8">
-        <v>7.1</v>
+        <v>5.6</v>
       </c>
       <c r="E8">
-        <v>10.1</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4604,16 +4597,16 @@
         <v>53</v>
       </c>
       <c r="B9">
-        <v>27.5</v>
+        <v>27.3</v>
       </c>
       <c r="C9">
-        <v>37</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="D9">
-        <v>5.4</v>
+        <v>6.1</v>
       </c>
       <c r="E9">
-        <v>6.4</v>
+        <v>7.8</v>
       </c>
     </row>
   </sheetData>
@@ -4629,7 +4622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -5161,10 +5154,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5195,11 +5188,11 @@
       <c r="B2" s="20">
         <v>134.74645041349706</v>
       </c>
-      <c r="C2" s="28">
-        <v>147.50366136735829</v>
-      </c>
-      <c r="D2" s="28">
-        <v>147.26695403232921</v>
+      <c r="C2" s="47">
+        <v>147.81375284986396</v>
+      </c>
+      <c r="D2" s="47">
+        <v>147.25937293698323</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5209,11 +5202,11 @@
       <c r="B3" s="20">
         <v>134.23236103862521</v>
       </c>
-      <c r="C3" s="28">
-        <v>147.02370380518278</v>
-      </c>
-      <c r="D3" s="28">
-        <v>146.72353169031206</v>
+      <c r="C3" s="47">
+        <v>146.90296489863664</v>
+      </c>
+      <c r="D3" s="47">
+        <v>146.68786327387261</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5223,11 +5216,11 @@
       <c r="B4" s="20">
         <v>150.0878942366954</v>
       </c>
-      <c r="C4" s="28">
-        <v>146.40436911306105</v>
-      </c>
-      <c r="D4" s="28">
-        <v>146.21745577705076</v>
+      <c r="C4" s="47">
+        <v>146.22284049683432</v>
+      </c>
+      <c r="D4" s="47">
+        <v>146.14844379616034</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5237,11 +5230,11 @@
       <c r="B5" s="20">
         <v>153.25067436662908</v>
       </c>
-      <c r="C5" s="28">
-        <v>144.83807002443319</v>
-      </c>
-      <c r="D5" s="28">
-        <v>145.7810228850272</v>
+      <c r="C5" s="47">
+        <v>145.05725221970036</v>
+      </c>
+      <c r="D5" s="47">
+        <v>145.67657387512367</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5251,11 +5244,11 @@
       <c r="B6" s="20">
         <v>163.51360808690507</v>
       </c>
-      <c r="C6" s="28">
-        <v>144.12929306853565</v>
-      </c>
-      <c r="D6" s="28">
-        <v>145.44103213177573</v>
+      <c r="C6" s="47">
+        <v>144.23564935853784</v>
+      </c>
+      <c r="D6" s="47">
+        <v>145.30144562272969</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5265,11 +5258,11 @@
       <c r="B7" s="20">
         <v>153.66209524099784</v>
       </c>
-      <c r="C7" s="28">
-        <v>144.68529886288096</v>
-      </c>
-      <c r="D7" s="28">
-        <v>145.21797525509581</v>
+      <c r="C7" s="47">
+        <v>144.49252359309975</v>
+      </c>
+      <c r="D7" s="47">
+        <v>145.04396501537391</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5279,11 +5272,11 @@
       <c r="B8" s="20">
         <v>143.73110098180126</v>
       </c>
-      <c r="C8" s="28">
-        <v>144.02283282661563</v>
-      </c>
-      <c r="D8" s="28">
-        <v>145.12099730130609</v>
+      <c r="C8" s="47">
+        <v>144.47360710434131</v>
+      </c>
+      <c r="D8" s="47">
+        <v>144.91436490184262</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5293,11 +5286,11 @@
       <c r="B9" s="20">
         <v>143.6741026486049</v>
       </c>
-      <c r="C9" s="28">
-        <v>145.60417757461698</v>
-      </c>
-      <c r="D9" s="28">
-        <v>145.15040282795701</v>
+      <c r="C9" s="47">
+        <v>145.44704464550816</v>
+      </c>
+      <c r="D9" s="47">
+        <v>144.91775720162804</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5307,11 +5300,11 @@
       <c r="B10" s="20">
         <v>142.00773744282046</v>
       </c>
-      <c r="C10" s="28">
-        <v>145.54393217587008</v>
-      </c>
-      <c r="D10" s="28">
-        <v>145.29778566623969</v>
+      <c r="C10" s="47">
+        <v>145.26005735768328</v>
+      </c>
+      <c r="D10" s="47">
+        <v>145.05167265405299</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5321,11 +5314,11 @@
       <c r="B11" s="20">
         <v>141.13686329808141</v>
       </c>
-      <c r="C11" s="28">
-        <v>144.56510502187717</v>
-      </c>
-      <c r="D11" s="28">
-        <v>145.54707812248449</v>
+      <c r="C11" s="47">
+        <v>144.94163009688663</v>
+      </c>
+      <c r="D11" s="47">
+        <v>145.30761397784812</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5335,11 +5328,11 @@
       <c r="B12" s="20">
         <v>144.93832064073018</v>
       </c>
-      <c r="C12" s="28">
-        <v>146.26101238624824</v>
-      </c>
-      <c r="D12" s="28">
-        <v>145.88383728436017</v>
+      <c r="C12" s="47">
+        <v>145.90775910782037</v>
+      </c>
+      <c r="D12" s="47">
+        <v>145.67312647589679</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5349,11 +5342,11 @@
       <c r="B13" s="20">
         <v>142.59014516031914</v>
       </c>
-      <c r="C13" s="28">
-        <v>146.98989759133454</v>
-      </c>
-      <c r="D13" s="28">
-        <v>146.29347077049098</v>
+      <c r="C13" s="47">
+        <v>146.81627206899782</v>
+      </c>
+      <c r="D13" s="47">
+        <v>146.13349684799101</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5363,11 +5356,11 @@
       <c r="B14" s="20">
         <v>136.7258774086435</v>
       </c>
-      <c r="C14" s="28">
-        <v>147.51535062330427</v>
-      </c>
-      <c r="D14" s="28">
-        <v>146.76074754092934</v>
+      <c r="C14" s="47">
+        <v>147.43623749809646</v>
+      </c>
+      <c r="D14" s="47">
+        <v>146.66995600407628</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5377,11 +5370,11 @@
       <c r="B15" s="20">
         <v>132.54052520440143</v>
       </c>
-      <c r="C15" s="28">
-        <v>146.37304725211661</v>
-      </c>
-      <c r="D15" s="28">
-        <v>147.27262522190304</v>
+      <c r="C15" s="47">
+        <v>146.75562367595387</v>
+      </c>
+      <c r="D15" s="47">
+        <v>147.26264169739869</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5391,11 +5384,11 @@
       <c r="B16" s="20">
         <v>152.145731768997</v>
       </c>
-      <c r="C16" s="28">
-        <v>148.35561691806086</v>
-      </c>
-      <c r="D16" s="28">
-        <v>147.81845720436331</v>
+      <c r="C16" s="47">
+        <v>148.11273124150642</v>
+      </c>
+      <c r="D16" s="47">
+        <v>147.89141030885224</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5405,11 +5398,11 @@
       <c r="B17" s="20">
         <v>152.20883250679566</v>
       </c>
-      <c r="C17" s="28">
-        <v>147.15670753095645</v>
-      </c>
-      <c r="D17" s="28">
-        <v>148.38708067860398</v>
+      <c r="C17" s="47">
+        <v>147.66287140410756</v>
+      </c>
+      <c r="D17" s="47">
+        <v>148.53428339881705</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5419,11 +5412,11 @@
       <c r="B18" s="20">
         <v>167.46154818637638</v>
       </c>
-      <c r="C18" s="28">
-        <v>148.59204857162541</v>
-      </c>
-      <c r="D18" s="28">
-        <v>148.9628232751173</v>
+      <c r="C18" s="47">
+        <v>148.32345630239612</v>
+      </c>
+      <c r="D18" s="47">
+        <v>149.16569646752109</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5433,11 +5426,11 @@
       <c r="B19" s="20">
         <v>161.70085905013559</v>
       </c>
-      <c r="C19" s="28">
-        <v>150.46755677901072</v>
-      </c>
-      <c r="D19" s="28">
-        <v>149.5223851184582</v>
+      <c r="C19" s="47">
+        <v>150.28797403928169</v>
+      </c>
+      <c r="D19" s="47">
+        <v>149.75596650201754</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5447,11 +5440,11 @@
       <c r="B20" s="20">
         <v>149.78297310853262</v>
       </c>
-      <c r="C20" s="28">
-        <v>149.791259710465</v>
-      </c>
-      <c r="D20" s="28">
-        <v>150.03477671839531</v>
+      <c r="C20" s="47">
+        <v>150.16419674873939</v>
+      </c>
+      <c r="D20" s="47">
+        <v>150.27202460612997</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5461,11 +5454,11 @@
       <c r="B21" s="20">
         <v>149.4590923353316</v>
       </c>
-      <c r="C21" s="28">
-        <v>150.55431191737475</v>
-      </c>
-      <c r="D21" s="28">
-        <v>150.46175673264949</v>
+      <c r="C21" s="47">
+        <v>150.21763547654584</v>
+      </c>
+      <c r="D21" s="47">
+        <v>150.67846148171677</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5475,11 +5468,11 @@
       <c r="B22" s="20">
         <v>146.70588711165021</v>
       </c>
-      <c r="C22" s="28">
-        <v>151.50859687720134</v>
-      </c>
-      <c r="D22" s="28">
-        <v>150.76480595560452</v>
+      <c r="C22" s="47">
+        <v>151.48900886896564</v>
+      </c>
+      <c r="D22" s="47">
+        <v>150.94091334886087</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5489,11 +5482,11 @@
       <c r="B23" s="20">
         <v>149.62906247744323</v>
       </c>
-      <c r="C23" s="28">
-        <v>151.27000420642045</v>
-      </c>
-      <c r="D23" s="28">
-        <v>150.90964926794558</v>
+      <c r="C23" s="47">
+        <v>151.28308212785262</v>
+      </c>
+      <c r="D23" s="47">
+        <v>151.03466911665774</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5503,11 +5496,11 @@
       <c r="B24" s="20">
         <v>152.38283025725997</v>
       </c>
-      <c r="C24" s="28">
-        <v>153.12874692680333</v>
-      </c>
-      <c r="D24" s="28">
-        <v>150.86891363468686</v>
+      <c r="C24" s="47">
+        <v>152.77664163187251</v>
+      </c>
+      <c r="D24" s="47">
+        <v>150.93915596143037</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5517,11 +5510,11 @@
       <c r="B25" s="20">
         <v>146.08348469256237</v>
       </c>
-      <c r="C25" s="28">
-        <v>152.11345706448907</v>
-      </c>
-      <c r="D25" s="28">
-        <v>150.62706819395316</v>
+      <c r="C25" s="47">
+        <v>152.31724534183923</v>
+      </c>
+      <c r="D25" s="47">
+        <v>150.644794138658</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5531,11 +5524,11 @@
       <c r="B26" s="20">
         <v>142.64696239584413</v>
       </c>
-      <c r="C26" s="28">
-        <v>152.3761260357814</v>
-      </c>
-      <c r="D26" s="28">
-        <v>150.18379417951783</v>
+      <c r="C26" s="47">
+        <v>151.97566535176</v>
+      </c>
+      <c r="D26" s="47">
+        <v>150.15834394558541</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5545,11 +5538,11 @@
       <c r="B27" s="20">
         <v>139.07181989111268</v>
       </c>
-      <c r="C27" s="28">
-        <v>151.76466629226593</v>
-      </c>
-      <c r="D27" s="28">
-        <v>149.5534144027672</v>
+      <c r="C27" s="47">
+        <v>152.15032530960136</v>
+      </c>
+      <c r="D27" s="47">
+        <v>149.4997378005412</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5559,11 +5552,11 @@
       <c r="B28" s="20">
         <v>155.63982283229944</v>
       </c>
-      <c r="C28" s="28">
-        <v>151.88842379784495</v>
-      </c>
-      <c r="D28" s="28">
-        <v>148.76630112172487</v>
+      <c r="C28" s="47">
+        <v>151.9198299086807</v>
+      </c>
+      <c r="D28" s="47">
+        <v>148.70383805097299</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5573,11 +5566,11 @@
       <c r="B29" s="20">
         <v>151.60135644382305</v>
       </c>
-      <c r="C29" s="28">
-        <v>146.51299704538707</v>
-      </c>
-      <c r="D29" s="28">
-        <v>147.86885420425369</v>
+      <c r="C29" s="47">
+        <v>146.69740654633495</v>
+      </c>
+      <c r="D29" s="47">
+        <v>147.81639418670636</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5587,11 +5580,11 @@
       <c r="B30" s="20">
         <v>159.16207548226589</v>
       </c>
-      <c r="C30" s="28">
-        <v>144.31159019760548</v>
-      </c>
-      <c r="D30" s="28">
-        <v>146.91981307129296</v>
+      <c r="C30" s="47">
+        <v>143.97218882278253</v>
+      </c>
+      <c r="D30" s="47">
+        <v>146.89068383354186</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5601,11 +5594,11 @@
       <c r="B31" s="20">
         <v>151.44848091721315</v>
       </c>
-      <c r="C31" s="28">
-        <v>142.86390930633337</v>
-      </c>
-      <c r="D31" s="28">
-        <v>145.9776117258746</v>
+      <c r="C31" s="47">
+        <v>143.06643427649834</v>
+      </c>
+      <c r="D31" s="47">
+        <v>145.98065030664691</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5615,11 +5608,11 @@
       <c r="B32" s="20">
         <v>145.76463042864052</v>
       </c>
-      <c r="C32" s="28">
-        <v>143.51103174224647</v>
-      </c>
-      <c r="D32" s="28">
-        <v>145.09736764432378</v>
+      <c r="C32" s="47">
+        <v>143.50090946819657</v>
+      </c>
+      <c r="D32" s="47">
+        <v>145.13521718903237</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5629,11 +5622,11 @@
       <c r="B33" s="20">
         <v>147.04553382400547</v>
       </c>
-      <c r="C33" s="28">
-        <v>147.07492972620685</v>
-      </c>
-      <c r="D33" s="28">
-        <v>144.32505800877667</v>
+      <c r="C33" s="47">
+        <v>146.65970576690739</v>
+      </c>
+      <c r="D33" s="47">
+        <v>144.39569006688157</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5643,11 +5636,11 @@
       <c r="B34" s="20">
         <v>137.8944988928931</v>
       </c>
-      <c r="C34" s="28">
-        <v>142.70950611308439</v>
-      </c>
-      <c r="D34" s="28">
-        <v>143.69062347352028</v>
+      <c r="C34" s="47">
+        <v>143.14528350657912</v>
+      </c>
+      <c r="D34" s="47">
+        <v>143.7881587002102</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5657,11 +5650,11 @@
       <c r="B35" s="20">
         <v>143.57320349337792</v>
       </c>
-      <c r="C35" s="28">
-        <v>143.9576170743249</v>
-      </c>
-      <c r="D35" s="28">
-        <v>143.21026302969139</v>
+      <c r="C35" s="47">
+        <v>143.73115244475574</v>
+      </c>
+      <c r="D35" s="47">
+        <v>143.32661363503777</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5671,11 +5664,11 @@
       <c r="B36" s="20">
         <v>141.21184890028576</v>
       </c>
-      <c r="C36" s="28">
-        <v>142.1920417058401</v>
-      </c>
-      <c r="D36" s="28">
-        <v>142.88783700447289</v>
+      <c r="C36" s="47">
+        <v>141.95324802504638</v>
+      </c>
+      <c r="D36" s="47">
+        <v>143.01237769116997</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5685,11 +5678,11 @@
       <c r="B37" s="20">
         <v>135.67154302632184</v>
       </c>
-      <c r="C37" s="28">
-        <v>141.56893775394471</v>
-      </c>
-      <c r="D37" s="28">
-        <v>142.71104009201966</v>
+      <c r="C37" s="47">
+        <v>141.95962734357732</v>
+      </c>
+      <c r="D37" s="47">
+        <v>142.83235270071802</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5699,11 +5692,11 @@
       <c r="B38" s="20">
         <v>134.564995313265</v>
       </c>
-      <c r="C38" s="28">
-        <v>143.59497920094438</v>
-      </c>
-      <c r="D38" s="28">
-        <v>142.65777508550403</v>
+      <c r="C38" s="47">
+        <v>143.11027500368212</v>
+      </c>
+      <c r="D38" s="47">
+        <v>142.76451430015953</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5713,11 +5706,11 @@
       <c r="B39" s="20">
         <v>132.57194718265788</v>
       </c>
-      <c r="C39" s="28">
-        <v>143.51872512882031</v>
-      </c>
-      <c r="D39" s="28">
-        <v>142.69507237886896</v>
+      <c r="C39" s="47">
+        <v>143.73622036138096</v>
+      </c>
+      <c r="D39" s="47">
+        <v>142.7783197295833</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5727,11 +5720,11 @@
       <c r="B40" s="20">
         <v>144.41715750575651</v>
       </c>
-      <c r="C40" s="28">
-        <v>141.72151927438549</v>
-      </c>
-      <c r="D40" s="28">
-        <v>142.78366755840281</v>
+      <c r="C40" s="47">
+        <v>142.04281024136395</v>
+      </c>
+      <c r="D40" s="47">
+        <v>142.83835520298595</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5741,11 +5734,11 @@
       <c r="B41" s="20">
         <v>149.83961931661509</v>
       </c>
-      <c r="C41" s="28">
-        <v>142.16827581960777</v>
-      </c>
-      <c r="D41" s="28">
-        <v>142.88210837577913</v>
+      <c r="C41" s="47">
+        <v>141.94304201775407</v>
+      </c>
+      <c r="D41" s="47">
+        <v>142.90761107787816</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5755,11 +5748,11 @@
       <c r="B42" s="20">
         <v>162.83974753189364</v>
       </c>
-      <c r="C42" s="28">
-        <v>143.40456178237028</v>
-      </c>
-      <c r="D42" s="28">
-        <v>142.95218448938178</v>
+      <c r="C42" s="47">
+        <v>143.03198403568797</v>
+      </c>
+      <c r="D42" s="47">
+        <v>142.95029852095175</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5769,11 +5762,11 @@
       <c r="B43" s="20">
         <v>151.25410111244764</v>
       </c>
-      <c r="C43" s="28">
-        <v>142.64281375661039</v>
-      </c>
-      <c r="D43" s="28">
-        <v>142.95897712659476</v>
+      <c r="C43" s="47">
+        <v>143.25581294849596</v>
+      </c>
+      <c r="D43" s="47">
+        <v>142.93421026895356</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5783,11 +5776,11 @@
       <c r="B44" s="20">
         <v>146.20323233619627</v>
       </c>
-      <c r="C44" s="28">
-        <v>145.65505957835799</v>
-      </c>
-      <c r="D44" s="28">
-        <v>142.87079460778091</v>
+      <c r="C44" s="47">
+        <v>145.41030021291587</v>
+      </c>
+      <c r="D44" s="47">
+        <v>142.83270084476686</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5797,11 +5790,11 @@
       <c r="B45" s="20">
         <v>141.60332874981128</v>
       </c>
-      <c r="C45" s="28">
-        <v>145.05869311071385</v>
-      </c>
-      <c r="D45" s="28">
-        <v>142.66388623182772</v>
+      <c r="C45" s="47">
+        <v>145.05726633592113</v>
+      </c>
+      <c r="D45" s="47">
+        <v>142.62633577508859</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -5811,11 +5804,11 @@
       <c r="B46" s="28">
         <v>135.07531285730843</v>
       </c>
-      <c r="C46" s="28">
-        <v>141.07722855232893</v>
-      </c>
-      <c r="D46" s="28">
-        <v>142.32562087371397</v>
+      <c r="C46" s="47">
+        <v>141.26972443721149</v>
+      </c>
+      <c r="D46" s="47">
+        <v>142.30418455373658</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -5825,11 +5818,11 @@
       <c r="B47" s="28">
         <v>142.25579775531418</v>
       </c>
-      <c r="C47" s="28">
-        <v>143.7591652324204</v>
-      </c>
-      <c r="D47" s="28">
-        <v>141.85770467168294</v>
+      <c r="C47" s="47">
+        <v>143.49992366439722</v>
+      </c>
+      <c r="D47" s="47">
+        <v>141.86538711007651</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -5839,11 +5832,11 @@
       <c r="B48" s="28">
         <v>138.14131943492291</v>
       </c>
-      <c r="C48" s="28">
-        <v>140.8981273775014</v>
-      </c>
-      <c r="D48" s="28">
-        <v>141.27379611655988</v>
+      <c r="C48" s="47">
+        <v>140.97101489691408</v>
+      </c>
+      <c r="D48" s="47">
+        <v>141.31896014217412</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -5853,11 +5846,11 @@
       <c r="B49" s="28">
         <v>135.44751977320297</v>
       </c>
-      <c r="C49" s="28">
-        <v>140.67708825755284</v>
-      </c>
-      <c r="D49" s="28">
-        <v>140.59524617392546</v>
+      <c r="C49" s="47">
+        <v>140.84786289616346</v>
+      </c>
+      <c r="D49" s="47">
+        <v>140.68380829425507</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -5867,11 +5860,11 @@
       <c r="B50" s="28">
         <v>132.19356455544042</v>
       </c>
-      <c r="C50" s="28">
-        <v>141.36247287892007</v>
-      </c>
-      <c r="D50" s="28">
-        <v>139.85375458352752</v>
+      <c r="C50" s="47">
+        <v>140.98724634775482</v>
+      </c>
+      <c r="D50" s="47">
+        <v>139.98745705311603</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -5881,11 +5874,11 @@
       <c r="B51" s="28">
         <v>129.61940932164029</v>
       </c>
-      <c r="C51" s="28">
-        <v>140.61363722120234</v>
-      </c>
-      <c r="D51" s="28">
-        <v>139.09025370190088</v>
+      <c r="C51" s="47">
+        <v>140.77526412993373</v>
+      </c>
+      <c r="D51" s="47">
+        <v>139.26850462119566</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -5895,11 +5888,11 @@
       <c r="B52" s="28">
         <v>128.38599328767583</v>
       </c>
-      <c r="C52" s="28">
-        <v>125.89743278341957</v>
-      </c>
-      <c r="D52" s="28">
-        <v>138.3495869410784</v>
+      <c r="C52" s="47">
+        <v>126.09175011718911</v>
+      </c>
+      <c r="D52" s="47">
+        <v>138.5728204114138</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5909,11 +5902,11 @@
       <c r="B53" s="28">
         <v>111.81827837013516</v>
       </c>
-      <c r="C53" s="28">
-        <v>104.49629251825432</v>
-      </c>
-      <c r="D53" s="28">
-        <v>137.67467355466158</v>
+      <c r="C53" s="47">
+        <v>104.3346244451472</v>
+      </c>
+      <c r="D53" s="47">
+        <v>137.944658251665</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -5923,11 +5916,11 @@
       <c r="B54" s="28">
         <v>130.30963100770941</v>
       </c>
-      <c r="C54" s="28">
-        <v>114.4239832590922</v>
-      </c>
-      <c r="D54" s="28">
-        <v>137.10398856958534</v>
+      <c r="C54" s="47">
+        <v>114.68274919519001</v>
+      </c>
+      <c r="D54" s="47">
+        <v>137.42264102187383</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -5937,11 +5930,11 @@
       <c r="B55" s="28">
         <v>133.78434132181565</v>
       </c>
-      <c r="C55" s="28">
-        <v>124.10816144121733</v>
-      </c>
-      <c r="D55" s="28">
-        <v>136.6653725095332</v>
+      <c r="C55" s="47">
+        <v>124.054874935404</v>
+      </c>
+      <c r="D55" s="47">
+        <v>137.03536567768828</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="27" customFormat="1">
@@ -5951,81 +5944,95 @@
       <c r="B56" s="28">
         <v>127.59092134022666</v>
       </c>
-      <c r="C56" s="28">
-        <v>126.88426923698418</v>
-      </c>
-      <c r="D56" s="28">
-        <v>136.37104387236846</v>
+      <c r="C56" s="47">
+        <v>126.71081992668883</v>
+      </c>
+      <c r="D56" s="47">
+        <v>136.79646180369235</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="27" customFormat="1">
       <c r="A57" s="25">
         <v>44044</v>
       </c>
-      <c r="B57" s="28">
-        <v>125.23224811923698</v>
-      </c>
-      <c r="C57" s="28">
-        <v>128.80156224686681</v>
-      </c>
-      <c r="D57" s="28">
-        <v>136.21398528279471</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="31" customFormat="1">
-      <c r="A58" s="32">
+      <c r="B57" s="47">
+        <v>125.44572625215507</v>
+      </c>
+      <c r="C57" s="47">
+        <v>129.29754939069412</v>
+      </c>
+      <c r="D57" s="47">
+        <v>136.70553779089326</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="30" customFormat="1">
+      <c r="A58" s="31">
         <v>44075</v>
       </c>
-      <c r="B58" s="28">
-        <v>126.7092687596504</v>
-      </c>
-      <c r="C58" s="28">
-        <v>131.66307506776914</v>
-      </c>
-      <c r="D58" s="28">
-        <v>136.17613336672702</v>
+      <c r="B58" s="47">
+        <v>127.10134993432418</v>
+      </c>
+      <c r="C58" s="47">
+        <v>131.92583380572995</v>
+      </c>
+      <c r="D58" s="47">
+        <v>136.74737548594547</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="11">
         <v>44105</v>
       </c>
-      <c r="B59" s="28">
-        <v>131.93155629327126</v>
-      </c>
-      <c r="C59" s="28">
-        <v>133.29338742400111</v>
-      </c>
-      <c r="D59" s="28">
-        <v>136.22833446787479</v>
+      <c r="B59" s="47">
+        <v>132.07223639537102</v>
+      </c>
+      <c r="C59" s="47">
+        <v>133.60819700079244</v>
+      </c>
+      <c r="D59" s="47">
+        <v>136.8945763455344</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="32">
+      <c r="A60" s="31">
         <v>44136</v>
       </c>
-      <c r="B60" s="28">
-        <v>133.07361620887411</v>
-      </c>
-      <c r="C60" s="28">
-        <v>135.13500852588487</v>
-      </c>
-      <c r="D60" s="28">
-        <v>136.3336184218339</v>
+      <c r="B60" s="47">
+        <v>133.31446072716284</v>
+      </c>
+      <c r="C60" s="47">
+        <v>135.49650145569024</v>
+      </c>
+      <c r="D60" s="47">
+        <v>137.11079116873049</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="24" customFormat="1">
-      <c r="A61" s="32">
+      <c r="A61" s="31">
         <v>44166</v>
       </c>
-      <c r="B61" s="29">
-        <v>132.44891764985255</v>
-      </c>
-      <c r="C61" s="29">
-        <v>136.41144179336155</v>
-      </c>
-      <c r="D61" s="29">
-        <v>136.45668119301254</v>
+      <c r="B61" s="47">
+        <v>132.68971782328498</v>
+      </c>
+      <c r="C61" s="47">
+        <v>136.41764561025201</v>
+      </c>
+      <c r="D61" s="47">
+        <v>137.35926590388848</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="11">
+        <v>44197</v>
+      </c>
+      <c r="B62" s="48">
+        <v>129.496695763514</v>
+      </c>
+      <c r="C62" s="48">
+        <v>139.00655195403516</v>
+      </c>
+      <c r="D62" s="48">
+        <v>137.60434144200701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos de EMAE e ICA"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -645,11 +645,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1852,7 +1852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -1891,7 +1891,7 @@
       <c r="A2" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="46">
         <v>3.7</v>
       </c>
       <c r="C2" s="34">
@@ -1917,7 +1917,7 @@
       <c r="A3" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="46">
         <v>6.8</v>
       </c>
       <c r="C3" s="34">
@@ -1943,7 +1943,7 @@
       <c r="A4" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="46">
         <v>8.6</v>
       </c>
       <c r="C4" s="34">
@@ -1969,7 +1969,7 @@
       <c r="A5" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="46">
         <v>6.4</v>
       </c>
       <c r="C5" s="34">
@@ -1995,7 +1995,7 @@
       <c r="A6" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="46">
         <v>-1.8</v>
       </c>
       <c r="C6" s="34">
@@ -2021,7 +2021,7 @@
       <c r="A7" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="46">
         <v>6.3</v>
       </c>
       <c r="C7" s="34">
@@ -2047,7 +2047,7 @@
       <c r="A8" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="46">
         <v>1.7</v>
       </c>
       <c r="C8" s="34">
@@ -2073,7 +2073,7 @@
       <c r="A9" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="46">
         <v>2.2999999999999998</v>
       </c>
       <c r="C9" s="34">
@@ -2099,7 +2099,7 @@
       <c r="A10" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="46">
         <v>0.2</v>
       </c>
       <c r="C10" s="34">
@@ -3888,14 +3888,14 @@
       <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -4491,14 +4491,14 @@
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4646,8 +4646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4674,14 +4674,14 @@
         <v>77</v>
       </c>
       <c r="B2" s="16">
-        <v>1897</v>
+        <v>2945</v>
       </c>
       <c r="C2">
-        <v>1809</v>
+        <v>3457</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>88</v>
+        <v>-512</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4689,14 +4689,14 @@
         <v>78</v>
       </c>
       <c r="B3" s="16">
-        <v>459</v>
+        <v>736</v>
       </c>
       <c r="C3">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="D3" s="16">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
-        <v>371</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4704,14 +4704,14 @@
         <v>79</v>
       </c>
       <c r="B4" s="16">
-        <v>508</v>
+        <v>892</v>
       </c>
       <c r="C4">
-        <v>289</v>
+        <v>455</v>
       </c>
       <c r="D4" s="16">
         <f t="shared" si="0"/>
-        <v>219</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4719,14 +4719,14 @@
         <v>80</v>
       </c>
       <c r="B5" s="16">
-        <v>91</v>
+        <v>164</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4734,14 +4734,14 @@
         <v>137</v>
       </c>
       <c r="B6" s="16">
-        <v>740</v>
+        <v>1109</v>
       </c>
       <c r="C6">
-        <v>851</v>
+        <v>1409</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>-111</v>
+        <v>-300</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4749,14 +4749,14 @@
         <v>81</v>
       </c>
       <c r="B7" s="16">
-        <v>1249</v>
+        <v>2042</v>
       </c>
       <c r="C7">
-        <v>1241</v>
+        <v>2037</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="16" customFormat="1">
@@ -4764,14 +4764,14 @@
         <v>94</v>
       </c>
       <c r="B8" s="16">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="C8" s="16">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4779,14 +4779,14 @@
         <v>82</v>
       </c>
       <c r="B9" s="16">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="C9">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4794,14 +4794,14 @@
         <v>83</v>
       </c>
       <c r="B10" s="16">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="C10">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4809,14 +4809,14 @@
         <v>84</v>
       </c>
       <c r="B11" s="16">
-        <v>1115</v>
+        <v>1788</v>
       </c>
       <c r="C11">
-        <v>487</v>
+        <v>826</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>628</v>
+        <v>962</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4824,14 +4824,14 @@
         <v>85</v>
       </c>
       <c r="B12" s="16">
-        <v>539</v>
+        <v>965</v>
       </c>
       <c r="C12">
-        <v>1736</v>
+        <v>2846</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>-1197</v>
+        <v>-1881</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4839,14 +4839,14 @@
         <v>86</v>
       </c>
       <c r="B13" s="16">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="C13">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4854,14 +4854,14 @@
         <v>87</v>
       </c>
       <c r="B14" s="16">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C14">
-        <v>141</v>
+        <v>236</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>-116</v>
+        <v>-192</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4869,14 +4869,14 @@
         <v>88</v>
       </c>
       <c r="B15" s="16">
-        <v>654</v>
+        <v>896</v>
       </c>
       <c r="C15">
-        <v>142</v>
+        <v>233</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="0"/>
-        <v>512</v>
+        <v>663</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4884,14 +4884,14 @@
         <v>89</v>
       </c>
       <c r="B16" s="16">
-        <v>717</v>
+        <v>1013</v>
       </c>
       <c r="C16">
-        <v>87</v>
+        <v>177</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="0"/>
-        <v>630</v>
+        <v>836</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4899,14 +4899,14 @@
         <v>90</v>
       </c>
       <c r="B17" s="16">
-        <v>399</v>
+        <v>860</v>
       </c>
       <c r="C17">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>762</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4914,14 +4914,14 @@
         <v>91</v>
       </c>
       <c r="B18" s="16">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="C18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4929,14 +4929,14 @@
         <v>92</v>
       </c>
       <c r="B19" s="16">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4944,14 +4944,14 @@
         <v>93</v>
       </c>
       <c r="B20" s="16">
-        <v>681</v>
+        <v>984</v>
       </c>
       <c r="C20">
-        <v>235</v>
+        <v>367</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
-        <v>446</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>
@@ -5178,10 +5178,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D62"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5213,10 +5213,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="37">
-        <v>147.81375284986396</v>
+        <v>147.77485442831252</v>
       </c>
       <c r="D2" s="37">
-        <v>147.25937293698323</v>
+        <v>147.27777610526303</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5227,10 +5227,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="37">
-        <v>146.90296489863664</v>
+        <v>146.95144750047629</v>
       </c>
       <c r="D3" s="37">
-        <v>146.68786327387261</v>
+        <v>146.71552151348317</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5241,10 +5241,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="37">
-        <v>146.22284049683432</v>
+        <v>146.21325631650075</v>
       </c>
       <c r="D4" s="37">
-        <v>146.14844379616034</v>
+        <v>146.1885531474108</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5255,10 +5255,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="37">
-        <v>145.05725221970036</v>
+        <v>145.05568084868733</v>
       </c>
       <c r="D5" s="37">
-        <v>145.67657387512367</v>
+        <v>145.73018658738758</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5269,10 +5269,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="37">
-        <v>144.23564935853784</v>
+        <v>144.2705436446106</v>
       </c>
       <c r="D6" s="37">
-        <v>145.30144562272969</v>
+        <v>145.36615926998158</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5283,10 +5283,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="37">
-        <v>144.49252359309975</v>
+        <v>144.45920067799636</v>
       </c>
       <c r="D7" s="37">
-        <v>145.04396501537391</v>
+        <v>145.11390082818312</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5297,10 +5297,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="37">
-        <v>144.47360710434131</v>
+        <v>144.48335339187298</v>
       </c>
       <c r="D8" s="37">
-        <v>144.91436490184262</v>
+        <v>144.98146130473719</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5311,10 +5311,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="37">
-        <v>145.44704464550816</v>
+        <v>145.39326839478437</v>
       </c>
       <c r="D9" s="37">
-        <v>144.91775720162804</v>
+        <v>144.97258013524555</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5325,10 +5325,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="37">
-        <v>145.26005735768328</v>
+        <v>145.30408732083038</v>
       </c>
       <c r="D10" s="37">
-        <v>145.05167265405299</v>
+        <v>145.08517583806733</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5339,10 +5339,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="37">
-        <v>144.94163009688663</v>
+        <v>144.93343810558488</v>
       </c>
       <c r="D11" s="37">
-        <v>145.30761397784812</v>
+        <v>145.31312719643807</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5353,10 +5353,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="37">
-        <v>145.90775910782037</v>
+        <v>145.90004059786054</v>
       </c>
       <c r="D12" s="37">
-        <v>145.67312647589679</v>
+        <v>145.64700386960172</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5367,10 +5367,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="37">
-        <v>146.81627206899782</v>
+        <v>146.83218257021494</v>
       </c>
       <c r="D13" s="37">
-        <v>146.13349684799101</v>
+        <v>146.07635871269616</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5381,10 +5381,10 @@
         <v>136.7258774086435</v>
       </c>
       <c r="C14" s="37">
-        <v>147.43623749809646</v>
+        <v>147.44087034178659</v>
       </c>
       <c r="D14" s="37">
-        <v>146.66995600407628</v>
+        <v>146.58657330417449</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5395,10 +5395,10 @@
         <v>132.54052520440143</v>
       </c>
       <c r="C15" s="37">
-        <v>146.75562367595387</v>
+        <v>146.84309726704396</v>
       </c>
       <c r="D15" s="37">
-        <v>147.26264169739869</v>
+        <v>147.16123018455093</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5409,10 +5409,10 @@
         <v>152.145731768997</v>
       </c>
       <c r="C16" s="37">
-        <v>148.11273124150642</v>
+        <v>148.02062480668152</v>
       </c>
       <c r="D16" s="37">
-        <v>147.89141030885224</v>
+        <v>147.78251935320955</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5423,10 +5423,10 @@
         <v>152.20883250679566</v>
       </c>
       <c r="C17" s="37">
-        <v>147.66287140410756</v>
+        <v>147.63191009550448</v>
       </c>
       <c r="D17" s="37">
-        <v>148.53428339881705</v>
+        <v>148.42890427495217</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5437,10 +5437,10 @@
         <v>167.46154818637638</v>
       </c>
       <c r="C18" s="37">
-        <v>148.32345630239612</v>
+        <v>148.34293834251449</v>
       </c>
       <c r="D18" s="37">
-        <v>149.16569646752109</v>
+        <v>149.07302787808862</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5451,10 +5451,10 @@
         <v>161.70085905013559</v>
       </c>
       <c r="C19" s="37">
-        <v>150.28797403928169</v>
+        <v>150.29945330772154</v>
       </c>
       <c r="D19" s="37">
-        <v>149.75596650201754</v>
+        <v>149.68201342435992</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5465,10 +5465,10 @@
         <v>149.78297310853262</v>
       </c>
       <c r="C20" s="37">
-        <v>150.16419674873939</v>
+        <v>150.14516460566466</v>
       </c>
       <c r="D20" s="37">
-        <v>150.27202460612997</v>
+        <v>150.21898099532191</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5479,10 +5479,10 @@
         <v>149.4590923353316</v>
       </c>
       <c r="C21" s="37">
-        <v>150.21763547654584</v>
+        <v>150.20814979587956</v>
       </c>
       <c r="D21" s="37">
-        <v>150.67846148171677</v>
+        <v>150.64532422903432</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5493,10 +5493,10 @@
         <v>146.70588711165021</v>
       </c>
       <c r="C22" s="37">
-        <v>151.48900886896564</v>
+        <v>151.51752669266034</v>
       </c>
       <c r="D22" s="37">
-        <v>150.94091334886087</v>
+        <v>150.9240736952674</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5507,10 +5507,10 @@
         <v>149.62906247744323</v>
       </c>
       <c r="C23" s="37">
-        <v>151.28308212785262</v>
+        <v>151.3571657671711</v>
       </c>
       <c r="D23" s="37">
-        <v>151.03466911665774</v>
+        <v>151.02910717628509</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5521,10 +5521,10 @@
         <v>152.38283025725997</v>
       </c>
       <c r="C24" s="37">
-        <v>152.77664163187251</v>
+        <v>152.73739505305679</v>
       </c>
       <c r="D24" s="37">
-        <v>150.93915596143037</v>
+        <v>150.93938129818486</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5535,10 +5535,10 @@
         <v>146.08348469256237</v>
       </c>
       <c r="C25" s="37">
-        <v>152.31724534183923</v>
+        <v>152.28240828128912</v>
       </c>
       <c r="D25" s="37">
-        <v>150.644794138658</v>
+        <v>150.64630876106287</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5549,10 +5549,10 @@
         <v>142.64696239584413</v>
       </c>
       <c r="C26" s="37">
-        <v>151.97566535176</v>
+        <v>151.9616039087191</v>
       </c>
       <c r="D26" s="37">
-        <v>150.15834394558541</v>
+        <v>150.15834259688179</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5563,10 +5563,10 @@
         <v>139.07181989111268</v>
       </c>
       <c r="C27" s="37">
-        <v>152.15032530960136</v>
+        <v>152.24013713827779</v>
       </c>
       <c r="D27" s="37">
-        <v>149.4997378005412</v>
+        <v>149.49721847601057</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5577,10 +5577,10 @@
         <v>155.63982283229944</v>
       </c>
       <c r="C28" s="37">
-        <v>151.9198299086807</v>
+        <v>151.84407952299696</v>
       </c>
       <c r="D28" s="37">
-        <v>148.70383805097299</v>
+        <v>148.699351570678</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5591,10 +5591,10 @@
         <v>151.60135644382305</v>
       </c>
       <c r="C29" s="37">
-        <v>146.69740654633495</v>
+        <v>146.71059521749663</v>
       </c>
       <c r="D29" s="37">
-        <v>147.81639418670636</v>
+        <v>147.81009673407749</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5605,10 +5605,10 @@
         <v>159.16207548226589</v>
       </c>
       <c r="C30" s="37">
-        <v>143.97218882278253</v>
+        <v>144.00386863146576</v>
       </c>
       <c r="D30" s="37">
-        <v>146.89068383354186</v>
+        <v>146.88333147737256</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5619,10 +5619,10 @@
         <v>151.44848091721315</v>
       </c>
       <c r="C31" s="37">
-        <v>143.06643427649834</v>
+        <v>143.02156579660877</v>
       </c>
       <c r="D31" s="37">
-        <v>145.98065030664691</v>
+        <v>145.97303418092244</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5633,10 +5633,10 @@
         <v>145.76463042864052</v>
       </c>
       <c r="C32" s="37">
-        <v>143.50090946819657</v>
+        <v>143.54221985511595</v>
       </c>
       <c r="D32" s="37">
-        <v>145.13521718903237</v>
+        <v>145.1289132526631</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5647,10 +5647,10 @@
         <v>147.04553382400547</v>
       </c>
       <c r="C33" s="37">
-        <v>146.65970576690739</v>
+        <v>146.67561906885047</v>
       </c>
       <c r="D33" s="37">
-        <v>144.39569006688157</v>
+        <v>144.39154289111033</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5661,10 +5661,10 @@
         <v>137.8944988928931</v>
       </c>
       <c r="C34" s="37">
-        <v>143.14528350657912</v>
+        <v>143.08805981767102</v>
       </c>
       <c r="D34" s="37">
-        <v>143.7881587002102</v>
+        <v>143.78630358826379</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5675,10 +5675,10 @@
         <v>143.57320349337792</v>
       </c>
       <c r="C35" s="37">
-        <v>143.73115244475574</v>
+        <v>143.76772571383782</v>
       </c>
       <c r="D35" s="37">
-        <v>143.32661363503777</v>
+        <v>143.32638712612882</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5689,10 +5689,10 @@
         <v>141.21184890028576</v>
       </c>
       <c r="C36" s="37">
-        <v>141.95324802504638</v>
+        <v>141.96874823084607</v>
       </c>
       <c r="D36" s="37">
-        <v>143.01237769116997</v>
+        <v>143.0128791281243</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5703,10 +5703,10 @@
         <v>135.67154302632184</v>
       </c>
       <c r="C37" s="37">
-        <v>141.95962734357732</v>
+        <v>141.90755386865095</v>
       </c>
       <c r="D37" s="37">
-        <v>142.83235270071802</v>
+        <v>142.83286108399358</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5717,10 +5717,10 @@
         <v>134.564995313265</v>
       </c>
       <c r="C38" s="37">
-        <v>143.11027500368212</v>
+        <v>143.10673026632992</v>
       </c>
       <c r="D38" s="37">
-        <v>142.76451430015953</v>
+        <v>142.76400870568844</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5731,10 +5731,10 @@
         <v>132.57194718265788</v>
       </c>
       <c r="C39" s="37">
-        <v>143.73622036138096</v>
+        <v>143.84766624936194</v>
       </c>
       <c r="D39" s="37">
-        <v>142.7783197295833</v>
+        <v>142.77570087867986</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5745,10 +5745,10 @@
         <v>144.41715750575651</v>
       </c>
       <c r="C40" s="37">
-        <v>142.04281024136395</v>
+        <v>141.9349090906895</v>
       </c>
       <c r="D40" s="37">
-        <v>142.83835520298595</v>
+        <v>142.83256119292363</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5759,10 +5759,10 @@
         <v>149.83961931661509</v>
       </c>
       <c r="C41" s="37">
-        <v>141.94304201775407</v>
+        <v>141.9983301682098</v>
       </c>
       <c r="D41" s="37">
-        <v>142.90761107787816</v>
+        <v>142.8976981521333</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5773,10 +5773,10 @@
         <v>162.83974753189364</v>
       </c>
       <c r="C42" s="37">
-        <v>143.03198403568797</v>
+        <v>143.13305027558306</v>
       </c>
       <c r="D42" s="37">
-        <v>142.95029852095175</v>
+        <v>142.93553075631897</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5787,10 +5787,10 @@
         <v>151.25410111244764</v>
       </c>
       <c r="C43" s="37">
-        <v>143.25581294849596</v>
+        <v>143.09945855809866</v>
       </c>
       <c r="D43" s="37">
-        <v>142.93421026895356</v>
+        <v>142.91419487292063</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5801,10 +5801,10 @@
         <v>146.20323233619627</v>
       </c>
       <c r="C44" s="37">
-        <v>145.41030021291587</v>
+        <v>145.43395888830977</v>
       </c>
       <c r="D44" s="37">
-        <v>142.83270084476686</v>
+        <v>142.80758712085614</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5815,10 +5815,10 @@
         <v>141.60332874981128</v>
       </c>
       <c r="C45" s="37">
-        <v>145.05726633592113</v>
+        <v>145.03508972134111</v>
       </c>
       <c r="D45" s="37">
-        <v>142.62633577508859</v>
+        <v>142.59705600143741</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -5829,10 +5829,10 @@
         <v>135.07531285730843</v>
       </c>
       <c r="C46" s="37">
-        <v>141.26972443721149</v>
+        <v>141.2682423763512</v>
       </c>
       <c r="D46" s="37">
-        <v>142.30418455373658</v>
+        <v>142.27267442050695</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -5843,10 +5843,10 @@
         <v>142.25579775531418</v>
       </c>
       <c r="C47" s="37">
-        <v>143.49992366439722</v>
+        <v>143.5531431673603</v>
       </c>
       <c r="D47" s="37">
-        <v>141.86538711007651</v>
+        <v>141.83577117009767</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -5857,10 +5857,10 @@
         <v>138.14131943492291</v>
       </c>
       <c r="C48" s="37">
-        <v>140.97101489691408</v>
+        <v>140.93089034348145</v>
       </c>
       <c r="D48" s="37">
-        <v>141.31896014217412</v>
+        <v>141.29440090065671</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -5871,10 +5871,10 @@
         <v>135.44751977320297</v>
       </c>
       <c r="C49" s="37">
-        <v>140.84786289616346</v>
+        <v>140.83476794658512</v>
       </c>
       <c r="D49" s="37">
-        <v>140.68380829425507</v>
+        <v>140.66886856928977</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -5885,10 +5885,10 @@
         <v>132.19356455544042</v>
       </c>
       <c r="C50" s="37">
-        <v>140.98724634775482</v>
+        <v>141.0172957796799</v>
       </c>
       <c r="D50" s="37">
-        <v>139.98745705311603</v>
+        <v>139.98691916698974</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -5899,10 +5899,10 @@
         <v>129.61940932164029</v>
       </c>
       <c r="C51" s="37">
-        <v>140.77526412993373</v>
+        <v>140.82397846349957</v>
       </c>
       <c r="D51" s="37">
-        <v>139.26850462119566</v>
+        <v>139.28358985447613</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -5913,10 +5913,10 @@
         <v>128.38599328767583</v>
       </c>
       <c r="C52" s="37">
-        <v>126.09175011718911</v>
+        <v>126.01298635165223</v>
       </c>
       <c r="D52" s="37">
-        <v>138.5728204114138</v>
+        <v>138.59891085324503</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5927,10 +5927,10 @@
         <v>111.81827837013516</v>
       </c>
       <c r="C53" s="37">
-        <v>104.3346244451472</v>
+        <v>104.29540079786129</v>
       </c>
       <c r="D53" s="37">
-        <v>137.944658251665</v>
+        <v>137.97049291200989</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -5941,10 +5941,10 @@
         <v>130.30963100770941</v>
       </c>
       <c r="C54" s="37">
-        <v>114.68274919519001</v>
+        <v>114.76826799366857</v>
       </c>
       <c r="D54" s="37">
-        <v>137.42264102187383</v>
+        <v>137.42962204822177</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -5955,10 +5955,10 @@
         <v>133.78434132181565</v>
       </c>
       <c r="C55" s="37">
-        <v>124.054874935404</v>
+        <v>124.00857978417032</v>
       </c>
       <c r="D55" s="37">
-        <v>137.03536567768828</v>
+        <v>136.99759826625882</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="27" customFormat="1">
@@ -5969,10 +5969,10 @@
         <v>127.59092134022666</v>
       </c>
       <c r="C56" s="37">
-        <v>126.71081992668883</v>
+        <v>126.7877742600087</v>
       </c>
       <c r="D56" s="37">
-        <v>136.79646180369235</v>
+        <v>136.68305408500382</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="27" customFormat="1">
@@ -5983,10 +5983,10 @@
         <v>125.44572625215507</v>
       </c>
       <c r="C57" s="37">
-        <v>129.29754939069412</v>
+        <v>129.24369156433485</v>
       </c>
       <c r="D57" s="37">
-        <v>136.70553779089326</v>
+        <v>136.4820277231529</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="30" customFormat="1">
@@ -5997,10 +5997,10 @@
         <v>127.10134993432418</v>
       </c>
       <c r="C58" s="37">
-        <v>131.92583380572995</v>
+        <v>131.90273729872393</v>
       </c>
       <c r="D58" s="37">
-        <v>136.74737548594547</v>
+        <v>136.37949333709039</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -6011,10 +6011,10 @@
         <v>132.07223639537102</v>
       </c>
       <c r="C59" s="37">
-        <v>133.60819700079244</v>
+        <v>133.59233473889026</v>
       </c>
       <c r="D59" s="37">
-        <v>136.8945763455344</v>
+        <v>136.35098476917821</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -6022,13 +6022,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="37">
-        <v>133.31446072716284</v>
+        <v>133.43700494930926</v>
       </c>
       <c r="C60" s="37">
-        <v>135.49650145569024</v>
+        <v>135.56679862668341</v>
       </c>
       <c r="D60" s="37">
-        <v>137.11079116873049</v>
+        <v>136.36596188260637</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="24" customFormat="1">
@@ -6036,27 +6036,41 @@
         <v>44166</v>
       </c>
       <c r="B61" s="37">
-        <v>132.68971782328498</v>
+        <v>132.57150330151808</v>
       </c>
       <c r="C61" s="37">
-        <v>136.41764561025201</v>
+        <v>136.36321070111322</v>
       </c>
       <c r="D61" s="37">
-        <v>137.35926590388848</v>
+        <v>136.39612699796803</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="11">
         <v>44197</v>
       </c>
-      <c r="B62" s="38">
-        <v>129.496695763514</v>
-      </c>
-      <c r="C62" s="38">
-        <v>139.00655195403516</v>
-      </c>
-      <c r="D62" s="38">
-        <v>137.60434144200701</v>
+      <c r="B62" s="37">
+        <v>129.22521775352402</v>
+      </c>
+      <c r="C62" s="37">
+        <v>138.97652161294636</v>
+      </c>
+      <c r="D62" s="37">
+        <v>136.41650437485583</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="24" customFormat="1">
+      <c r="A63" s="11">
+        <v>44228</v>
+      </c>
+      <c r="B63" s="38">
+        <v>126.2948878638516</v>
+      </c>
+      <c r="C63" s="38">
+        <v>137.53246960664117</v>
+      </c>
+      <c r="D63" s="38">
+        <v>136.40752715245807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos de Mayo"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15315" windowHeight="5445" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
-    <sheet name="IPC-Mar-Div" sheetId="2" r:id="rId2"/>
+    <sheet name="IPC-Abr-Div" sheetId="2" r:id="rId2"/>
     <sheet name="IPC-Interanual" sheetId="3" r:id="rId3"/>
     <sheet name="Producto" sheetId="4" r:id="rId4"/>
     <sheet name="Pobreza-Aglo" sheetId="8" r:id="rId5"/>
@@ -568,7 +568,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -603,7 +603,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -615,7 +614,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -639,18 +637,15 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52:E52"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1714,13 +1709,13 @@
       <c r="B45" s="1">
         <v>2.7</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="23">
         <v>4</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="23">
         <v>3</v>
       </c>
-      <c r="E45" s="24">
+      <c r="E45" s="23">
         <v>1</v>
       </c>
     </row>
@@ -1782,13 +1777,13 @@
       <c r="B49" s="1">
         <v>4</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="23">
         <v>2</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="23">
         <v>3.2</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="23">
         <v>4.3</v>
       </c>
     </row>
@@ -1799,13 +1794,13 @@
       <c r="B50" s="1">
         <v>4</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="23">
         <v>3</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="23">
         <v>3.9</v>
       </c>
-      <c r="E50" s="24">
+      <c r="E50" s="23">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -1833,14 +1828,31 @@
       <c r="B52" s="1">
         <v>4.8</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="23">
         <v>7.2</v>
       </c>
-      <c r="D52" s="24">
+      <c r="D52" s="23">
         <v>4.5</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E52" s="23">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="11">
+        <v>44287</v>
+      </c>
+      <c r="B53" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C53">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D53" s="23">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E53" s="23">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
@@ -1852,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1862,263 +1874,263 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="30" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="46">
-        <v>3.7</v>
-      </c>
-      <c r="C2" s="34">
+      <c r="B2" s="32">
+        <v>5.7</v>
+      </c>
+      <c r="C2" s="32">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32">
+        <v>3.4</v>
+      </c>
+      <c r="E2" s="32">
+        <v>5</v>
+      </c>
+      <c r="F2" s="32">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G2" s="32">
+        <v>4.2</v>
+      </c>
+      <c r="H2" s="32">
+        <v>4.4780459545347817</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="32">
+        <v>4.7</v>
+      </c>
+      <c r="C3" s="32">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D3" s="32">
+        <v>3.5</v>
+      </c>
+      <c r="E3" s="32">
+        <v>5.3</v>
+      </c>
+      <c r="F3" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="G3" s="32">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D2" s="34">
-        <v>2.5</v>
-      </c>
-      <c r="E2" s="34">
+      <c r="H3" s="32">
+        <v>4.1625654697070136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="32">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C4" s="32">
+        <v>7.7</v>
+      </c>
+      <c r="D4" s="32">
+        <v>7.7</v>
+      </c>
+      <c r="E4" s="32">
+        <v>6.4</v>
+      </c>
+      <c r="F4" s="32">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G4" s="32">
+        <v>8</v>
+      </c>
+      <c r="H4" s="32">
+        <v>7.9068708967513945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="32">
+        <v>7.9</v>
+      </c>
+      <c r="C5" s="32">
+        <v>8.1</v>
+      </c>
+      <c r="D5" s="32">
+        <v>8.4</v>
+      </c>
+      <c r="E5" s="32">
+        <v>5.5</v>
+      </c>
+      <c r="F5" s="32">
+        <v>7.3</v>
+      </c>
+      <c r="G5" s="32">
+        <v>7.5</v>
+      </c>
+      <c r="H5" s="32">
+        <v>7.2810491351317896</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="32">
+        <v>-0.6</v>
+      </c>
+      <c r="C6" s="32">
+        <v>-1.3</v>
+      </c>
+      <c r="D6" s="32">
+        <v>-3.1</v>
+      </c>
+      <c r="E6" s="32">
+        <v>-6</v>
+      </c>
+      <c r="F6" s="32">
+        <v>-1.4</v>
+      </c>
+      <c r="G6" s="32">
+        <v>1.3</v>
+      </c>
+      <c r="H6" s="32">
+        <v>-0.86916501336806729</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="32">
+        <v>-0.9</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="32">
+        <v>-0.5</v>
+      </c>
+      <c r="E7" s="32">
+        <v>-0.6</v>
+      </c>
+      <c r="F7" s="32">
+        <v>2.4</v>
+      </c>
+      <c r="G7" s="32">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H7" s="32">
+        <v>-7.5853437271966584E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="32">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C8" s="32">
         <v>2.9</v>
       </c>
-      <c r="F2" s="34">
-        <v>5</v>
-      </c>
-      <c r="G2" s="34">
+      <c r="D8" s="32">
+        <v>2.8</v>
+      </c>
+      <c r="E8" s="32">
         <v>3.5</v>
       </c>
-      <c r="H2" s="34">
-        <v>3.778617173607457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="46">
-        <v>6.8</v>
-      </c>
-      <c r="C3" s="34">
-        <v>5.4</v>
-      </c>
-      <c r="D3" s="34">
-        <v>3.7</v>
-      </c>
-      <c r="E3" s="34">
+      <c r="F8" s="32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G8" s="32">
+        <v>3.6</v>
+      </c>
+      <c r="H8" s="33">
+        <v>3.5916470748142304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="32">
+        <v>7.8</v>
+      </c>
+      <c r="C9" s="32">
+        <v>3.6</v>
+      </c>
+      <c r="D9" s="32">
+        <v>5.8</v>
+      </c>
+      <c r="E9" s="32">
         <v>5.3</v>
       </c>
-      <c r="F3" s="34">
-        <v>5.8</v>
-      </c>
-      <c r="G3" s="34">
-        <v>5.2</v>
-      </c>
-      <c r="H3" s="34">
-        <v>5.9242779351575958</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="46">
-        <v>8.6</v>
-      </c>
-      <c r="C4" s="34">
-        <v>6.3</v>
-      </c>
-      <c r="D4" s="34">
-        <v>6.3</v>
-      </c>
-      <c r="E4" s="34">
-        <v>5.4</v>
-      </c>
-      <c r="F4" s="34">
-        <v>6.7</v>
-      </c>
-      <c r="G4" s="34">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H4" s="34">
-        <v>7.1889301024673946</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="46">
-        <v>6.4</v>
-      </c>
-      <c r="C5" s="34">
-        <v>5.9</v>
-      </c>
-      <c r="D5" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="E5" s="34">
-        <v>8</v>
-      </c>
-      <c r="F5" s="34">
-        <v>5.3</v>
-      </c>
-      <c r="G5" s="34">
-        <v>6.9</v>
-      </c>
-      <c r="H5" s="34">
-        <v>6.032110063040208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="46">
-        <v>-1.8</v>
-      </c>
-      <c r="C6" s="34">
-        <v>1</v>
-      </c>
-      <c r="D6" s="34">
-        <v>0.3</v>
-      </c>
-      <c r="E6" s="34">
-        <v>-1.9</v>
-      </c>
-      <c r="F6" s="34">
-        <v>-5.3</v>
-      </c>
-      <c r="G6" s="34">
+      <c r="F9" s="32">
+        <v>4</v>
+      </c>
+      <c r="G9" s="32">
+        <v>6.1</v>
+      </c>
+      <c r="H9" s="32">
+        <v>5.3732817731649396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="32">
+        <v>3.5</v>
+      </c>
+      <c r="C10" s="32">
+        <v>3.9</v>
+      </c>
+      <c r="D10" s="32">
+        <v>4.2</v>
+      </c>
+      <c r="E10" s="32">
         <v>2.6</v>
       </c>
-      <c r="H6" s="34">
-        <v>-0.77272010587949858</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="46">
-        <v>6.3</v>
-      </c>
-      <c r="C7" s="34">
-        <v>5.6</v>
-      </c>
-      <c r="D7" s="34">
-        <v>1.5</v>
-      </c>
-      <c r="E7" s="34">
-        <v>-0.3</v>
-      </c>
-      <c r="F7" s="34">
-        <v>0.7</v>
-      </c>
-      <c r="G7" s="34">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H7" s="34">
-        <v>4.9036875481853537</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="46">
-        <v>1.7</v>
-      </c>
-      <c r="C8" s="34">
-        <v>3.1</v>
-      </c>
-      <c r="D8" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="34">
-        <v>2.4</v>
-      </c>
-      <c r="F8" s="34">
-        <v>2.7</v>
-      </c>
-      <c r="G8" s="34">
-        <v>2.7</v>
-      </c>
-      <c r="H8" s="35">
-        <v>2.2799609159769973</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="46">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C9" s="34">
-        <v>3.8</v>
-      </c>
-      <c r="D9" s="34">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E9" s="34">
-        <v>3.4</v>
-      </c>
-      <c r="F9" s="34">
-        <v>3.8</v>
-      </c>
-      <c r="G9" s="34">
-        <v>4.7</v>
-      </c>
-      <c r="H9" s="34">
-        <v>3.1002404834374442</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="46">
-        <v>0.2</v>
-      </c>
-      <c r="C10" s="34">
+      <c r="F10" s="32">
+        <v>3.9</v>
+      </c>
+      <c r="G10" s="32">
         <v>2.6</v>
       </c>
-      <c r="D10" s="34">
-        <v>3.1</v>
-      </c>
-      <c r="E10" s="34">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F10" s="34">
-        <v>2.6</v>
-      </c>
-      <c r="G10" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="H10" s="34">
-        <v>1.6105408706750701</v>
+      <c r="H10" s="32">
+        <v>3.4057612790158842</v>
       </c>
     </row>
   </sheetData>
@@ -2166,26 +2178,26 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="37">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C2" s="44">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D2" s="37">
+        <v>4</v>
+      </c>
+      <c r="E2" s="37">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F2" s="37">
+        <v>4</v>
+      </c>
+      <c r="G2" s="44">
+        <v>4.2</v>
+      </c>
+      <c r="H2" s="37">
         <v>4.8</v>
-      </c>
-      <c r="C2" s="40">
-        <v>5.2</v>
-      </c>
-      <c r="D2" s="39">
-        <v>4.8</v>
-      </c>
-      <c r="E2" s="39">
-        <v>3.3</v>
-      </c>
-      <c r="F2" s="39">
-        <v>4.2</v>
-      </c>
-      <c r="G2" s="39">
-        <v>4.3</v>
-      </c>
-      <c r="H2" s="39">
-        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2193,25 +2205,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="C3" s="43">
+        <v>4.7</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3.9</v>
+      </c>
+      <c r="G3" s="43">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C3" s="41">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D3" s="7">
-        <v>4.8</v>
-      </c>
-      <c r="E3" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="F3" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>4.3</v>
-      </c>
-      <c r="H3" s="7">
-        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2219,25 +2231,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="7">
-        <v>6.4</v>
-      </c>
-      <c r="C4" s="41">
-        <v>6.3</v>
+        <v>3.6</v>
+      </c>
+      <c r="C4" s="43">
+        <v>3.8</v>
       </c>
       <c r="D4" s="7">
-        <v>6.8</v>
+        <v>3.3</v>
       </c>
       <c r="E4" s="7">
-        <v>5.6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F4" s="7">
-        <v>6.5</v>
-      </c>
-      <c r="G4" s="7">
-        <v>6.4</v>
+        <v>3.2</v>
+      </c>
+      <c r="G4" s="43">
+        <v>3.5</v>
       </c>
       <c r="H4" s="7">
-        <v>6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2245,25 +2257,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="7">
-        <v>10.8</v>
-      </c>
-      <c r="C5" s="41">
-        <v>16.2</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="43">
+        <v>4.9000000000000004</v>
       </c>
       <c r="D5" s="7">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="E5" s="7">
-        <v>3.4</v>
+        <v>6.1</v>
       </c>
       <c r="F5" s="7">
         <v>6</v>
       </c>
-      <c r="G5" s="7">
-        <v>4.8</v>
+      <c r="G5" s="43">
+        <v>5.9</v>
       </c>
       <c r="H5" s="7">
-        <v>6.2</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2271,25 +2283,25 @@
         <v>24</v>
       </c>
       <c r="B6" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="C6" s="41">
-        <v>1</v>
+        <v>3.5</v>
+      </c>
+      <c r="C6" s="43">
+        <v>4.0999999999999996</v>
       </c>
       <c r="D6" s="7">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E6" s="7">
-        <v>2.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F6" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="G6" s="7">
-        <v>2.5</v>
+        <v>4.2</v>
+      </c>
+      <c r="G6" s="43">
+        <v>1.7</v>
       </c>
       <c r="H6" s="7">
-        <v>1.9</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2297,25 +2309,25 @@
         <v>16</v>
       </c>
       <c r="B7" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="C7" s="41">
-        <v>3.1</v>
+        <v>4.3</v>
+      </c>
+      <c r="C7" s="43">
+        <v>4.7</v>
       </c>
       <c r="D7" s="7">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="E7" s="7">
-        <v>2.9</v>
+        <v>4.2</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
       </c>
-      <c r="G7" s="7">
-        <v>3.6</v>
+      <c r="G7" s="43">
+        <v>2.8</v>
       </c>
       <c r="H7" s="7">
-        <v>2</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2323,25 +2335,25 @@
         <v>17</v>
       </c>
       <c r="B8" s="7">
-        <v>4</v>
-      </c>
-      <c r="C8" s="41">
-        <v>4</v>
+        <v>3.7</v>
+      </c>
+      <c r="C8" s="43">
+        <v>3.8</v>
       </c>
       <c r="D8" s="7">
-        <v>4.3</v>
+        <v>3.7</v>
       </c>
       <c r="E8" s="7">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="F8" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="G8" s="7">
-        <v>3.6</v>
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="43">
+        <v>3.7</v>
       </c>
       <c r="H8" s="7">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2349,25 +2361,25 @@
         <v>18</v>
       </c>
       <c r="B9" s="7">
-        <v>4.2</v>
-      </c>
-      <c r="C9" s="41">
-        <v>3.7</v>
+        <v>5.7</v>
+      </c>
+      <c r="C9" s="43">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D9" s="7">
-        <v>4.5</v>
+        <v>6.3</v>
       </c>
       <c r="E9" s="7">
-        <v>4.0999999999999996</v>
+        <v>6</v>
       </c>
       <c r="F9" s="7">
-        <v>5.6</v>
-      </c>
-      <c r="G9" s="7">
-        <v>4.5</v>
+        <v>5.4</v>
+      </c>
+      <c r="G9" s="43">
+        <v>6.5</v>
       </c>
       <c r="H9" s="7">
-        <v>3.8</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2375,25 +2387,25 @@
         <v>19</v>
       </c>
       <c r="B10" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="41">
-        <v>0.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="43">
+        <v>0.5</v>
       </c>
       <c r="D10" s="7">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="7">
-        <v>1.6</v>
+        <v>0.9</v>
       </c>
       <c r="F10" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="G10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="43">
         <v>1.3</v>
       </c>
       <c r="H10" s="7">
-        <v>0.7</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2401,25 +2413,25 @@
         <v>20</v>
       </c>
       <c r="B11" s="7">
-        <v>5.3</v>
-      </c>
-      <c r="C11" s="41">
-        <v>3.5</v>
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="43">
+        <v>2.7</v>
       </c>
       <c r="D11" s="7">
-        <v>8.8000000000000007</v>
+        <v>-0.7</v>
       </c>
       <c r="E11" s="7">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="F11" s="7">
-        <v>2.7</v>
-      </c>
-      <c r="G11" s="7">
-        <v>6.5</v>
+        <v>3</v>
+      </c>
+      <c r="G11" s="43">
+        <v>1.2</v>
       </c>
       <c r="H11" s="7">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2427,25 +2439,25 @@
         <v>21</v>
       </c>
       <c r="B12" s="7">
-        <v>28.5</v>
-      </c>
-      <c r="C12" s="41">
-        <v>30.1</v>
+        <v>2.5</v>
+      </c>
+      <c r="C12" s="43">
+        <v>3.1</v>
       </c>
       <c r="D12" s="7">
-        <v>29.7</v>
+        <v>1.9</v>
       </c>
       <c r="E12" s="7">
-        <v>23.4</v>
+        <v>6.1</v>
       </c>
       <c r="F12" s="7">
-        <v>26.9</v>
-      </c>
-      <c r="G12" s="7">
-        <v>16.5</v>
+        <v>1.6</v>
+      </c>
+      <c r="G12" s="43">
+        <v>0.5</v>
       </c>
       <c r="H12" s="7">
-        <v>24.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2453,25 +2465,25 @@
         <v>22</v>
       </c>
       <c r="B13" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="C13" s="41">
-        <v>2.7</v>
+        <v>3.9</v>
+      </c>
+      <c r="C13" s="43">
+        <v>3.2</v>
       </c>
       <c r="D13" s="7">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="E13" s="7">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="F13" s="7">
-        <v>4.3</v>
-      </c>
-      <c r="G13" s="7">
-        <v>4</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G13" s="43">
+        <v>5.6</v>
       </c>
       <c r="H13" s="7">
-        <v>4.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2479,25 +2491,25 @@
         <v>23</v>
       </c>
       <c r="B14" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C14" s="41">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D14" s="7">
-        <v>2.1</v>
+        <v>3.6</v>
+      </c>
+      <c r="C14" s="43">
+        <v>3.9</v>
+      </c>
+      <c r="D14" s="43">
+        <v>3.3</v>
       </c>
       <c r="E14" s="7">
-        <v>2.4</v>
+        <v>4.5</v>
       </c>
       <c r="F14" s="7">
-        <v>3</v>
-      </c>
-      <c r="G14" s="7">
-        <v>2.1</v>
+        <v>3.1</v>
+      </c>
+      <c r="G14" s="43">
+        <v>3.5</v>
       </c>
       <c r="H14" s="7">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
@@ -2546,285 +2558,285 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="42">
-        <v>42.6</v>
-      </c>
-      <c r="C2" s="44">
-        <v>40.4</v>
-      </c>
-      <c r="D2" s="42">
-        <v>44.9</v>
-      </c>
-      <c r="E2" s="44">
-        <v>45.9</v>
-      </c>
-      <c r="F2" s="42">
-        <v>44.9</v>
-      </c>
-      <c r="G2" s="42">
-        <v>44.5</v>
-      </c>
-      <c r="H2" s="42">
-        <v>39</v>
+      <c r="B2" s="38">
+        <v>46.3</v>
+      </c>
+      <c r="C2" s="40">
+        <v>44.2</v>
+      </c>
+      <c r="D2" s="38">
+        <v>48.4</v>
+      </c>
+      <c r="E2" s="40">
+        <v>48.8</v>
+      </c>
+      <c r="F2" s="38">
+        <v>46.9</v>
+      </c>
+      <c r="G2" s="38">
+        <v>48.6</v>
+      </c>
+      <c r="H2" s="38">
+        <v>44.7</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="43">
-        <v>44.8</v>
-      </c>
-      <c r="C3" s="45">
-        <v>41.1</v>
-      </c>
-      <c r="D3" s="43">
-        <v>48.3</v>
-      </c>
-      <c r="E3" s="45">
-        <v>52.4</v>
-      </c>
-      <c r="F3" s="43">
-        <v>47.4</v>
-      </c>
-      <c r="G3" s="43">
-        <v>46.8</v>
-      </c>
-      <c r="H3" s="43">
-        <v>39.6</v>
+      <c r="B3" s="39">
+        <v>46.4</v>
+      </c>
+      <c r="C3" s="41">
+        <v>43.2</v>
+      </c>
+      <c r="D3" s="39">
+        <v>49.6</v>
+      </c>
+      <c r="E3" s="41">
+        <v>52.3</v>
+      </c>
+      <c r="F3" s="39">
+        <v>46.3</v>
+      </c>
+      <c r="G3" s="39">
+        <v>48.5</v>
+      </c>
+      <c r="H3" s="39">
+        <v>45.1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="43">
-        <v>41</v>
-      </c>
-      <c r="C4" s="45">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="D4" s="43">
-        <v>42.8</v>
-      </c>
-      <c r="E4" s="45">
-        <v>43.6</v>
-      </c>
-      <c r="F4" s="43">
-        <v>44.1</v>
-      </c>
-      <c r="G4" s="43">
+      <c r="B4" s="39">
+        <v>44</v>
+      </c>
+      <c r="C4" s="41">
+        <v>42.7</v>
+      </c>
+      <c r="D4" s="39">
+        <v>44.9</v>
+      </c>
+      <c r="E4" s="41">
+        <v>46.7</v>
+      </c>
+      <c r="F4" s="39">
+        <v>46.5</v>
+      </c>
+      <c r="G4" s="39">
+        <v>45</v>
+      </c>
+      <c r="H4" s="39">
         <v>42.2</v>
-      </c>
-      <c r="H4" s="43">
-        <v>40.299999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="43">
-        <v>71.5</v>
-      </c>
-      <c r="C5" s="45">
-        <v>77.8</v>
-      </c>
-      <c r="D5" s="43">
-        <v>67.3</v>
-      </c>
-      <c r="E5" s="45">
-        <v>55.8</v>
-      </c>
-      <c r="F5" s="43">
-        <v>72.2</v>
-      </c>
-      <c r="G5" s="43">
-        <v>70.2</v>
-      </c>
-      <c r="H5" s="43">
-        <v>54.3</v>
+      <c r="B5" s="39">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="C5" s="41">
+        <v>84</v>
+      </c>
+      <c r="D5" s="39">
+        <v>76.7</v>
+      </c>
+      <c r="E5" s="41">
+        <v>61.9</v>
+      </c>
+      <c r="F5" s="39">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="G5" s="39">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="H5" s="39">
+        <v>67.400000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="43">
-        <v>19.8</v>
-      </c>
-      <c r="C6" s="45">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="D6" s="43">
-        <v>21.7</v>
-      </c>
-      <c r="E6" s="45">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="F6" s="43">
-        <v>20</v>
-      </c>
-      <c r="G6" s="43">
-        <v>27.8</v>
-      </c>
-      <c r="H6" s="43">
-        <v>19.600000000000001</v>
+      <c r="B6" s="39">
+        <v>23.9</v>
+      </c>
+      <c r="C6" s="41">
+        <v>22</v>
+      </c>
+      <c r="D6" s="39">
+        <v>24.9</v>
+      </c>
+      <c r="E6" s="41">
+        <v>24</v>
+      </c>
+      <c r="F6" s="39">
+        <v>24.9</v>
+      </c>
+      <c r="G6" s="39">
+        <v>31.5</v>
+      </c>
+      <c r="H6" s="39">
+        <v>25.6</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="43">
-        <v>47.5</v>
-      </c>
-      <c r="C7" s="45">
-        <v>48.7</v>
-      </c>
-      <c r="D7" s="43">
-        <v>45.3</v>
-      </c>
-      <c r="E7" s="45">
-        <v>54.9</v>
-      </c>
-      <c r="F7" s="43">
-        <v>47.4</v>
-      </c>
-      <c r="G7" s="43">
-        <v>47.1</v>
-      </c>
-      <c r="H7" s="43">
-        <v>45.5</v>
+      <c r="B7" s="39">
+        <v>52</v>
+      </c>
+      <c r="C7" s="41">
+        <v>54.2</v>
+      </c>
+      <c r="D7" s="39">
+        <v>49.2</v>
+      </c>
+      <c r="E7" s="41">
+        <v>58.1</v>
+      </c>
+      <c r="F7" s="39">
+        <v>49.3</v>
+      </c>
+      <c r="G7" s="39">
+        <v>49.3</v>
+      </c>
+      <c r="H7" s="39">
+        <v>52.1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="43">
-        <v>41.7</v>
-      </c>
-      <c r="C8" s="45">
-        <v>36.9</v>
-      </c>
-      <c r="D8" s="43">
-        <v>44.4</v>
-      </c>
-      <c r="E8" s="45">
-        <v>51</v>
-      </c>
-      <c r="F8" s="43">
-        <v>49.1</v>
-      </c>
-      <c r="G8" s="43">
-        <v>45.1</v>
-      </c>
-      <c r="H8" s="43">
-        <v>41.9</v>
+      <c r="B8" s="39">
+        <v>45.2</v>
+      </c>
+      <c r="C8" s="41">
+        <v>40.9</v>
+      </c>
+      <c r="D8" s="39">
+        <v>48.3</v>
+      </c>
+      <c r="E8" s="41">
+        <v>52</v>
+      </c>
+      <c r="F8" s="39">
+        <v>50.9</v>
+      </c>
+      <c r="G8" s="39">
+        <v>47.7</v>
+      </c>
+      <c r="H8" s="39">
+        <v>45.2</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="43">
-        <v>46.3</v>
-      </c>
-      <c r="C9" s="45">
-        <v>43.3</v>
-      </c>
-      <c r="D9" s="43">
-        <v>49.4</v>
-      </c>
-      <c r="E9" s="45">
-        <v>45.2</v>
-      </c>
-      <c r="F9" s="43">
-        <v>46.7</v>
-      </c>
-      <c r="G9" s="43">
-        <v>50.1</v>
-      </c>
-      <c r="H9" s="43">
+      <c r="B9" s="39">
+        <v>52.6</v>
+      </c>
+      <c r="C9" s="41">
         <v>47.8</v>
+      </c>
+      <c r="D9" s="39">
+        <v>57.1</v>
+      </c>
+      <c r="E9" s="41">
+        <v>53.3</v>
+      </c>
+      <c r="F9" s="39">
+        <v>51.9</v>
+      </c>
+      <c r="G9" s="39">
+        <v>61.2</v>
+      </c>
+      <c r="H9" s="39">
+        <v>53.5</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="43">
-        <v>13.8</v>
-      </c>
-      <c r="C10" s="45">
-        <v>14.3</v>
-      </c>
-      <c r="D10" s="43">
-        <v>11.8</v>
-      </c>
-      <c r="E10" s="45">
-        <v>18.8</v>
-      </c>
-      <c r="F10" s="43">
-        <v>14.6</v>
-      </c>
-      <c r="G10" s="43">
-        <v>15.6</v>
-      </c>
-      <c r="H10" s="43">
-        <v>17</v>
+      <c r="B10" s="39">
+        <v>19.3</v>
+      </c>
+      <c r="C10" s="41">
+        <v>18.2</v>
+      </c>
+      <c r="D10" s="39">
+        <v>19</v>
+      </c>
+      <c r="E10" s="41">
+        <v>25.8</v>
+      </c>
+      <c r="F10" s="39">
+        <v>20.3</v>
+      </c>
+      <c r="G10" s="39">
+        <v>22.6</v>
+      </c>
+      <c r="H10" s="39">
+        <v>21.9</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="43">
-        <v>52</v>
-      </c>
-      <c r="C11" s="45">
-        <v>50.7</v>
-      </c>
-      <c r="D11" s="43">
-        <v>59.2</v>
-      </c>
-      <c r="E11" s="45">
-        <v>46.6</v>
-      </c>
-      <c r="F11" s="43">
-        <v>42.6</v>
-      </c>
-      <c r="G11" s="43">
-        <v>41.9</v>
-      </c>
-      <c r="H11" s="43">
-        <v>44.5</v>
+      <c r="B11" s="39">
+        <v>50.8</v>
+      </c>
+      <c r="C11" s="41">
+        <v>51.7</v>
+      </c>
+      <c r="D11" s="39">
+        <v>54</v>
+      </c>
+      <c r="E11" s="41">
+        <v>47.5</v>
+      </c>
+      <c r="F11" s="39">
+        <v>43.1</v>
+      </c>
+      <c r="G11" s="39">
+        <v>41.4</v>
+      </c>
+      <c r="H11" s="39">
+        <v>45.4</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="43">
-        <v>29.7</v>
-      </c>
-      <c r="C12" s="45">
-        <v>26.6</v>
-      </c>
-      <c r="D12" s="43">
-        <v>34</v>
-      </c>
-      <c r="E12" s="45">
-        <v>28</v>
-      </c>
-      <c r="F12" s="43">
-        <v>39.9</v>
-      </c>
-      <c r="G12" s="43">
-        <v>26.5</v>
-      </c>
-      <c r="H12" s="43">
+      <c r="B12" s="39">
+        <v>34.9</v>
+      </c>
+      <c r="C12" s="41">
+        <v>33.4</v>
+      </c>
+      <c r="D12" s="39">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E12" s="41">
+        <v>36.5</v>
+      </c>
+      <c r="F12" s="39">
+        <v>41.2</v>
+      </c>
+      <c r="G12" s="39">
+        <v>23.3</v>
+      </c>
+      <c r="H12" s="39">
         <v>22.5</v>
       </c>
     </row>
@@ -2832,52 +2844,52 @@
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="43">
-        <v>42.4</v>
-      </c>
-      <c r="C13" s="45">
-        <v>42.4</v>
-      </c>
-      <c r="D13" s="43">
-        <v>42.3</v>
-      </c>
-      <c r="E13" s="45">
-        <v>46.1</v>
-      </c>
-      <c r="F13" s="43">
-        <v>43.5</v>
-      </c>
-      <c r="G13" s="43">
-        <v>44.7</v>
-      </c>
-      <c r="H13" s="43">
-        <v>34.4</v>
+      <c r="B13" s="39">
+        <v>45.7</v>
+      </c>
+      <c r="C13" s="41">
+        <v>44.9</v>
+      </c>
+      <c r="D13" s="39">
+        <v>46.5</v>
+      </c>
+      <c r="E13" s="41">
+        <v>47.7</v>
+      </c>
+      <c r="F13" s="39">
+        <v>45.6</v>
+      </c>
+      <c r="G13" s="39">
+        <v>50.8</v>
+      </c>
+      <c r="H13" s="39">
+        <v>38.700000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="43">
-        <v>26.6</v>
-      </c>
-      <c r="C14" s="45">
-        <v>29.7</v>
-      </c>
-      <c r="D14" s="43">
-        <v>24.5</v>
-      </c>
-      <c r="E14" s="45">
-        <v>25.3</v>
-      </c>
-      <c r="F14" s="43">
-        <v>25.7</v>
-      </c>
-      <c r="G14" s="43">
-        <v>23.2</v>
-      </c>
-      <c r="H14" s="43">
-        <v>19.100000000000001</v>
+      <c r="B14" s="39">
+        <v>30.9</v>
+      </c>
+      <c r="C14" s="41">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="D14" s="39">
+        <v>27.6</v>
+      </c>
+      <c r="E14" s="41">
+        <v>29.5</v>
+      </c>
+      <c r="F14" s="39">
+        <v>29.5</v>
+      </c>
+      <c r="G14" s="39">
+        <v>26.9</v>
+      </c>
+      <c r="H14" s="39">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3824,10 +3836,10 @@
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="23">
+      <c r="A67" s="22">
         <v>2020</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C67" s="12">
@@ -3841,7 +3853,7 @@
       <c r="A68" s="12">
         <v>2020</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="B68" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C68" s="12">
@@ -3852,10 +3864,10 @@
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="36">
+      <c r="A69" s="34">
         <v>2020</v>
       </c>
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="34" t="s">
         <v>30</v>
       </c>
       <c r="C69" s="12">
@@ -3888,14 +3900,14 @@
       <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="47"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16"/>
@@ -3933,16 +3945,16 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>12.2</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>16.5</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>3.9</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>5.3</v>
       </c>
     </row>
@@ -3950,16 +3962,16 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>40.9</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>51</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>11.8</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>15.2</v>
       </c>
     </row>
@@ -3967,16 +3979,16 @@
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>32.6</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>44</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>5.4</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="23">
         <v>5.9</v>
       </c>
     </row>
@@ -3984,16 +3996,16 @@
       <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>24.9</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>34.799999999999997</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>3.1</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="23">
         <v>4.5</v>
       </c>
     </row>
@@ -4001,16 +4013,16 @@
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>32.4</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>40.6</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>3.5</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="23">
         <v>4.7</v>
       </c>
     </row>
@@ -4018,16 +4030,16 @@
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>32.200000000000003</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>42.9</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>6.7</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="23">
         <v>8.6999999999999993</v>
       </c>
     </row>
@@ -4035,16 +4047,16 @@
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>25.7</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>36.4</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <v>2.5</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="23">
         <v>3.8</v>
       </c>
     </row>
@@ -4052,16 +4064,16 @@
       <c r="A11" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>40.299999999999997</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>53.6</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <v>8</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="23">
         <v>10.6</v>
       </c>
     </row>
@@ -4069,16 +4081,16 @@
       <c r="A12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>27.6</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>37.700000000000003</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <v>3.4</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="23">
         <v>5.9</v>
       </c>
     </row>
@@ -4086,16 +4098,16 @@
       <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>28.7</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="23">
         <v>35.700000000000003</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="23">
         <v>5</v>
       </c>
     </row>
@@ -4103,16 +4115,16 @@
       <c r="A14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>33.799999999999997</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>43.5</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <v>5.7</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="23">
         <v>7.7</v>
       </c>
     </row>
@@ -4120,16 +4132,16 @@
       <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>27.4</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <v>37.700000000000003</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <v>3.3</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="23">
         <v>4.7</v>
       </c>
     </row>
@@ -4137,16 +4149,16 @@
       <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>25.3</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="23">
         <v>35.299999999999997</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>3.2</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="23">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4154,16 +4166,16 @@
       <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>31.2</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="23">
         <v>41.7</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <v>7.8</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="23">
         <v>10.3</v>
       </c>
     </row>
@@ -4171,16 +4183,16 @@
       <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>31.4</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="23">
         <v>39.4</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="23">
         <v>3.5</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="23">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -4188,16 +4200,16 @@
       <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="23">
         <v>18.7</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="23">
         <v>24</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="23">
         <v>5.2</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="23">
         <v>7</v>
       </c>
     </row>
@@ -4205,16 +4217,16 @@
       <c r="A20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="23">
         <v>39.299999999999997</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="23">
         <v>49.5</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="23">
         <v>6.6</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -4222,16 +4234,16 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="23">
         <v>29.5</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="23">
         <v>40.799999999999997</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="23">
         <v>7</v>
       </c>
     </row>
@@ -4239,16 +4251,16 @@
       <c r="A22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="23">
         <v>24</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="23">
         <v>31.7</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="23">
         <v>7</v>
       </c>
     </row>
@@ -4256,16 +4268,16 @@
       <c r="A23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="23">
         <v>29.1</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="23">
         <v>38.299999999999997</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="23">
         <v>5.8</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="23">
         <v>7.4</v>
       </c>
     </row>
@@ -4273,16 +4285,16 @@
       <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="23">
         <v>30.4</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="23">
         <v>40.9</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <v>4</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="23">
         <v>5.7</v>
       </c>
     </row>
@@ -4290,16 +4302,16 @@
       <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="23">
         <v>28</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="23">
         <v>39.799999999999997</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <v>6</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="23">
         <v>9.1</v>
       </c>
     </row>
@@ -4307,16 +4319,16 @@
       <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="23">
         <v>30.5</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="23">
         <v>41.1</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="23">
         <v>7.5</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="23">
         <v>10.8</v>
       </c>
     </row>
@@ -4324,16 +4336,16 @@
       <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="23">
         <v>27.2</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="23">
         <v>39.200000000000003</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <v>6.4</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="23">
         <v>8.8000000000000007</v>
       </c>
     </row>
@@ -4341,16 +4353,16 @@
       <c r="A28" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="23">
         <v>24.9</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="23">
         <v>33.5</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <v>5</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="23">
         <v>7</v>
       </c>
     </row>
@@ -4358,16 +4370,16 @@
       <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="24">
+      <c r="B29" s="23">
         <v>32.4</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="23">
         <v>43.6</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <v>6.6</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="23">
         <v>8.1</v>
       </c>
     </row>
@@ -4375,16 +4387,16 @@
       <c r="A30" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="24">
+      <c r="B30" s="23">
         <v>24</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>31.7</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="23">
         <v>5</v>
       </c>
     </row>
@@ -4392,16 +4404,16 @@
       <c r="A31" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="24">
+      <c r="B31" s="23">
         <v>32.1</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="23">
         <v>40.4</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="23">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="23">
         <v>12.3</v>
       </c>
     </row>
@@ -4409,16 +4421,16 @@
       <c r="A32" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="24">
+      <c r="B32" s="23">
         <v>26</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="23">
         <v>33.200000000000003</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="23">
         <v>6.5</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E32" s="23">
         <v>7</v>
       </c>
     </row>
@@ -4426,25 +4438,25 @@
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="24">
+      <c r="B34" s="23">
         <v>25.2</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="23">
         <v>32</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="23">
         <v>5.9</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="23">
         <v>5.7</v>
       </c>
     </row>
@@ -4452,16 +4464,16 @@
       <c r="A35" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="24">
+      <c r="B35" s="23">
         <v>25.2</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="23">
         <v>35.1</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <v>3.8</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="23">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -4491,14 +4503,14 @@
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="47"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="8" t="s">
@@ -4518,16 +4530,16 @@
       <c r="A3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>31.6</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>42</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>7.8</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <v>10.5</v>
       </c>
     </row>
@@ -4674,14 +4686,14 @@
         <v>77</v>
       </c>
       <c r="B2" s="16">
-        <v>2945</v>
+        <v>3871</v>
       </c>
       <c r="C2">
-        <v>3457</v>
+        <v>4794</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>-512</v>
+        <v>-923</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4689,14 +4701,14 @@
         <v>78</v>
       </c>
       <c r="B3" s="16">
-        <v>736</v>
+        <v>1067</v>
       </c>
       <c r="C3">
-        <v>145</v>
+        <v>195</v>
       </c>
       <c r="D3" s="16">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
-        <v>591</v>
+        <v>872</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4704,14 +4716,14 @@
         <v>79</v>
       </c>
       <c r="B4" s="16">
-        <v>892</v>
+        <v>1249</v>
       </c>
       <c r="C4">
-        <v>455</v>
+        <v>609</v>
       </c>
       <c r="D4" s="16">
         <f t="shared" si="0"/>
-        <v>437</v>
+        <v>640</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4719,14 +4731,14 @@
         <v>80</v>
       </c>
       <c r="B5" s="16">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4734,14 +4746,14 @@
         <v>137</v>
       </c>
       <c r="B6" s="16">
-        <v>1109</v>
+        <v>1533</v>
       </c>
       <c r="C6">
-        <v>1409</v>
+        <v>1956</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>-300</v>
+        <v>-423</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4749,14 +4761,14 @@
         <v>81</v>
       </c>
       <c r="B7" s="16">
-        <v>2042</v>
+        <v>2671</v>
       </c>
       <c r="C7">
-        <v>2037</v>
+        <v>2746</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="16" customFormat="1">
@@ -4764,14 +4776,14 @@
         <v>94</v>
       </c>
       <c r="B8" s="16">
-        <v>195</v>
+        <v>296</v>
       </c>
       <c r="C8" s="16">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4779,14 +4791,14 @@
         <v>82</v>
       </c>
       <c r="B9" s="16">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="C9">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4794,14 +4806,14 @@
         <v>83</v>
       </c>
       <c r="B10" s="16">
-        <v>161</v>
+        <v>230</v>
       </c>
       <c r="C10">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4809,14 +4821,14 @@
         <v>84</v>
       </c>
       <c r="B11" s="16">
-        <v>1788</v>
+        <v>2541</v>
       </c>
       <c r="C11">
-        <v>826</v>
+        <v>1139</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>962</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4824,14 +4836,14 @@
         <v>85</v>
       </c>
       <c r="B12" s="16">
-        <v>965</v>
+        <v>1442</v>
       </c>
       <c r="C12">
-        <v>2846</v>
+        <v>3767</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>-1881</v>
+        <v>-2325</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4839,14 +4851,14 @@
         <v>86</v>
       </c>
       <c r="B13" s="16">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="C13">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4854,14 +4866,14 @@
         <v>87</v>
       </c>
       <c r="B14" s="16">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C14">
-        <v>236</v>
+        <v>331</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>-192</v>
+        <v>-255</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4869,14 +4881,14 @@
         <v>88</v>
       </c>
       <c r="B15" s="16">
-        <v>896</v>
+        <v>1226</v>
       </c>
       <c r="C15">
-        <v>233</v>
+        <v>330</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="0"/>
-        <v>663</v>
+        <v>896</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4884,14 +4896,14 @@
         <v>89</v>
       </c>
       <c r="B16" s="16">
-        <v>1013</v>
+        <v>1447</v>
       </c>
       <c r="C16">
-        <v>177</v>
+        <v>235</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="0"/>
-        <v>836</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4899,14 +4911,14 @@
         <v>90</v>
       </c>
       <c r="B17" s="16">
-        <v>860</v>
+        <v>1430</v>
       </c>
       <c r="C17">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
-        <v>762</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4914,14 +4926,14 @@
         <v>91</v>
       </c>
       <c r="B18" s="16">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="C18">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4929,14 +4941,14 @@
         <v>92</v>
       </c>
       <c r="B19" s="16">
-        <v>185</v>
+        <v>293</v>
       </c>
       <c r="C19">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4944,14 +4956,14 @@
         <v>93</v>
       </c>
       <c r="B20" s="16">
-        <v>984</v>
+        <v>1348</v>
       </c>
       <c r="C20">
-        <v>367</v>
+        <v>493</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
-        <v>617</v>
+        <v>855</v>
       </c>
     </row>
   </sheetData>
@@ -5178,10 +5190,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5192,16 +5204,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>119</v>
       </c>
     </row>
@@ -5209,868 +5221,882 @@
       <c r="A2" s="11">
         <v>42370</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="35">
         <v>134.74645041349706</v>
       </c>
-      <c r="C2" s="37">
-        <v>147.77485442831252</v>
-      </c>
-      <c r="D2" s="37">
-        <v>147.27777610526303</v>
+      <c r="C2" s="35">
+        <v>147.75498715030596</v>
+      </c>
+      <c r="D2" s="35">
+        <v>147.23579038288463</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="11">
         <v>42401</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="35">
         <v>134.23236103862521</v>
       </c>
-      <c r="C3" s="37">
-        <v>146.95144750047629</v>
-      </c>
-      <c r="D3" s="37">
-        <v>146.71552151348317</v>
+      <c r="C3" s="35">
+        <v>146.96934260981135</v>
+      </c>
+      <c r="D3" s="35">
+        <v>146.67361562308275</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11">
         <v>42430</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="35">
         <v>150.0878942366954</v>
       </c>
-      <c r="C4" s="37">
-        <v>146.21325631650075</v>
-      </c>
-      <c r="D4" s="37">
-        <v>146.1885531474108</v>
+      <c r="C4" s="35">
+        <v>146.15418576660139</v>
+      </c>
+      <c r="D4" s="35">
+        <v>146.14700241290353</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11">
         <v>42461</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="35">
         <v>153.25067436662908</v>
       </c>
-      <c r="C5" s="37">
-        <v>145.05568084868733</v>
-      </c>
-      <c r="D5" s="37">
-        <v>145.73018658738758</v>
+      <c r="C5" s="35">
+        <v>145.05972484724194</v>
+      </c>
+      <c r="D5" s="35">
+        <v>145.690009275112</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11">
         <v>42491</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="35">
         <v>163.51360808690507</v>
       </c>
-      <c r="C6" s="37">
-        <v>144.2705436446106</v>
-      </c>
-      <c r="D6" s="37">
-        <v>145.36615926998158</v>
+      <c r="C6" s="35">
+        <v>144.20745083223596</v>
+      </c>
+      <c r="D6" s="35">
+        <v>145.3288448995568</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11">
         <v>42522</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="35">
         <v>153.66209524099784</v>
       </c>
-      <c r="C7" s="37">
-        <v>144.45920067799636</v>
-      </c>
-      <c r="D7" s="37">
-        <v>145.11390082818312</v>
+      <c r="C7" s="35">
+        <v>144.43220745985715</v>
+      </c>
+      <c r="D7" s="35">
+        <v>145.08102494789711</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11">
         <v>42552</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="35">
         <v>143.73110098180126</v>
       </c>
-      <c r="C8" s="37">
-        <v>144.48335339187298</v>
-      </c>
-      <c r="D8" s="37">
-        <v>144.98146130473719</v>
+      <c r="C8" s="35">
+        <v>144.47210065927695</v>
+      </c>
+      <c r="D8" s="35">
+        <v>144.95513148513774</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11">
         <v>42583</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="35">
         <v>143.6741026486049</v>
       </c>
-      <c r="C9" s="37">
-        <v>145.39326839478437</v>
-      </c>
-      <c r="D9" s="37">
-        <v>144.97258013524555</v>
+      <c r="C9" s="35">
+        <v>145.42236934886503</v>
+      </c>
+      <c r="D9" s="35">
+        <v>144.95392303102321</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11">
         <v>42614</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="35">
         <v>142.00773744282046</v>
       </c>
-      <c r="C10" s="37">
-        <v>145.30408732083038</v>
-      </c>
-      <c r="D10" s="37">
-        <v>145.08517583806733</v>
+      <c r="C10" s="35">
+        <v>145.35207246219466</v>
+      </c>
+      <c r="D10" s="35">
+        <v>145.07378842370582</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11">
         <v>42644</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="35">
         <v>141.13686329808141</v>
       </c>
-      <c r="C11" s="37">
-        <v>144.93343810558488</v>
-      </c>
-      <c r="D11" s="37">
-        <v>145.31312719643807</v>
+      <c r="C11" s="35">
+        <v>144.9643512774424</v>
+      </c>
+      <c r="D11" s="35">
+        <v>145.30653838629783</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="11">
         <v>42675</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="35">
         <v>144.93832064073018</v>
       </c>
-      <c r="C12" s="37">
-        <v>145.90004059786054</v>
-      </c>
-      <c r="D12" s="37">
-        <v>145.64700386960172</v>
+      <c r="C12" s="35">
+        <v>145.9197540026999</v>
+      </c>
+      <c r="D12" s="35">
+        <v>145.64170122317205</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="11">
         <v>42705</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="35">
         <v>142.59014516031914</v>
       </c>
-      <c r="C13" s="37">
-        <v>146.83218257021494</v>
-      </c>
-      <c r="D13" s="37">
-        <v>146.07635871269616</v>
+      <c r="C13" s="35">
+        <v>146.86280738558727</v>
+      </c>
+      <c r="D13" s="35">
+        <v>146.06927378712319</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="11">
         <v>42736</v>
       </c>
-      <c r="B14" s="20">
-        <v>136.7258774086435</v>
-      </c>
-      <c r="C14" s="37">
-        <v>147.44087034178659</v>
-      </c>
-      <c r="D14" s="37">
-        <v>146.58657330417449</v>
+      <c r="B14" s="35">
+        <v>136.71584129022389</v>
+      </c>
+      <c r="C14" s="35">
+        <v>147.38505265463473</v>
+      </c>
+      <c r="D14" s="35">
+        <v>146.57594242400094</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11">
         <v>42767</v>
       </c>
-      <c r="B15" s="20">
-        <v>132.54052520440143</v>
-      </c>
-      <c r="C15" s="37">
-        <v>146.84309726704396</v>
-      </c>
-      <c r="D15" s="37">
-        <v>147.16123018455093</v>
+      <c r="B15" s="35">
+        <v>132.59571861886312</v>
+      </c>
+      <c r="C15" s="35">
+        <v>146.78041615963724</v>
+      </c>
+      <c r="D15" s="35">
+        <v>147.14660770655198</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="11">
         <v>42795</v>
       </c>
-      <c r="B16" s="20">
-        <v>152.145731768997</v>
-      </c>
-      <c r="C16" s="37">
-        <v>148.02062480668152</v>
-      </c>
-      <c r="D16" s="37">
-        <v>147.78251935320955</v>
+      <c r="B16" s="35">
+        <v>152.10057447295463</v>
+      </c>
+      <c r="C16" s="35">
+        <v>147.90694631470552</v>
+      </c>
+      <c r="D16" s="35">
+        <v>147.76427449754672</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="11">
         <v>42826</v>
       </c>
-      <c r="B17" s="20">
-        <v>152.20883250679566</v>
-      </c>
-      <c r="C17" s="37">
-        <v>147.63191009550448</v>
-      </c>
-      <c r="D17" s="37">
-        <v>148.42890427495217</v>
+      <c r="B17" s="35">
+        <v>152.24670859934483</v>
+      </c>
+      <c r="C17" s="35">
+        <v>147.58786006530389</v>
+      </c>
+      <c r="D17" s="35">
+        <v>148.40832435721458</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11">
         <v>42856</v>
       </c>
-      <c r="B18" s="20">
-        <v>167.46154818637638</v>
-      </c>
-      <c r="C18" s="37">
-        <v>148.34293834251449</v>
-      </c>
-      <c r="D18" s="37">
-        <v>149.07302787808862</v>
+      <c r="B18" s="35">
+        <v>167.43178967186597</v>
+      </c>
+      <c r="C18" s="35">
+        <v>148.27715869707779</v>
+      </c>
+      <c r="D18" s="35">
+        <v>149.05146752575178</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11">
         <v>42887</v>
       </c>
-      <c r="B19" s="20">
-        <v>161.70085905013559</v>
-      </c>
-      <c r="C19" s="37">
-        <v>150.29945330772154</v>
-      </c>
-      <c r="D19" s="37">
-        <v>149.68201342435992</v>
+      <c r="B19" s="35">
+        <v>161.6927414720964</v>
+      </c>
+      <c r="C19" s="35">
+        <v>150.3094618250027</v>
+      </c>
+      <c r="D19" s="35">
+        <v>149.66064711105008</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="11">
         <v>42917</v>
       </c>
-      <c r="B20" s="20">
-        <v>149.78297310853262</v>
-      </c>
-      <c r="C20" s="37">
-        <v>150.14516460566466</v>
-      </c>
-      <c r="D20" s="37">
-        <v>150.21898099532191</v>
+      <c r="B20" s="35">
+        <v>149.80340554028913</v>
+      </c>
+      <c r="C20" s="35">
+        <v>150.1712542016337</v>
+      </c>
+      <c r="D20" s="35">
+        <v>150.19855494430189</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="11">
         <v>42948</v>
       </c>
-      <c r="B21" s="20">
-        <v>149.4590923353316</v>
-      </c>
-      <c r="C21" s="37">
-        <v>150.20814979587956</v>
-      </c>
-      <c r="D21" s="37">
-        <v>150.64532422903432</v>
+      <c r="B21" s="35">
+        <v>149.43328785043016</v>
+      </c>
+      <c r="C21" s="35">
+        <v>150.2871237540742</v>
+      </c>
+      <c r="D21" s="35">
+        <v>150.62615778027421</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11">
         <v>42979</v>
       </c>
-      <c r="B22" s="20">
-        <v>146.70588711165021</v>
-      </c>
-      <c r="C22" s="37">
-        <v>151.51752669266034</v>
-      </c>
-      <c r="D22" s="37">
-        <v>150.9240736952674</v>
+      <c r="B22" s="35">
+        <v>146.71125916479468</v>
+      </c>
+      <c r="C22" s="35">
+        <v>151.60061466267052</v>
+      </c>
+      <c r="D22" s="35">
+        <v>150.90636994103053</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11">
         <v>43009</v>
       </c>
-      <c r="B23" s="20">
-        <v>149.62906247744323</v>
-      </c>
-      <c r="C23" s="37">
-        <v>151.3571657671711</v>
-      </c>
-      <c r="D23" s="37">
-        <v>151.02910717628509</v>
+      <c r="B23" s="35">
+        <v>149.63145472156614</v>
+      </c>
+      <c r="C23" s="35">
+        <v>151.44953742621686</v>
+      </c>
+      <c r="D23" s="35">
+        <v>151.01261150037126</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11">
         <v>43040</v>
       </c>
-      <c r="B24" s="20">
-        <v>152.38283025725997</v>
-      </c>
-      <c r="C24" s="37">
-        <v>152.73739505305679</v>
-      </c>
-      <c r="D24" s="37">
-        <v>150.93938129818486</v>
+      <c r="B24" s="35">
+        <v>152.35339540314538</v>
+      </c>
+      <c r="C24" s="35">
+        <v>152.76093865952978</v>
+      </c>
+      <c r="D24" s="35">
+        <v>150.9250510183947</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11">
         <v>43070</v>
       </c>
-      <c r="B25" s="20">
-        <v>146.08348469256237</v>
-      </c>
-      <c r="C25" s="37">
-        <v>152.28240828128912</v>
-      </c>
-      <c r="D25" s="37">
-        <v>150.64630876106287</v>
+      <c r="B25" s="35">
+        <v>146.11052730255409</v>
+      </c>
+      <c r="C25" s="35">
+        <v>152.31033994100818</v>
+      </c>
+      <c r="D25" s="35">
+        <v>150.63402000667153</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="11">
         <v>43101</v>
       </c>
-      <c r="B26" s="20">
-        <v>142.64696239584413</v>
-      </c>
-      <c r="C26" s="37">
-        <v>151.9616039087191</v>
-      </c>
-      <c r="D26" s="37">
-        <v>150.15834259688179</v>
+      <c r="B26" s="35">
+        <v>142.63067053864708</v>
+      </c>
+      <c r="C26" s="35">
+        <v>151.87366699883231</v>
+      </c>
+      <c r="D26" s="35">
+        <v>150.14651139143152</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="11">
         <v>43132</v>
       </c>
-      <c r="B27" s="20">
-        <v>139.07181989111268</v>
-      </c>
-      <c r="C27" s="37">
-        <v>152.24013713827779</v>
-      </c>
-      <c r="D27" s="37">
-        <v>149.49721847601057</v>
+      <c r="B27" s="35">
+        <v>139.11763783702028</v>
+      </c>
+      <c r="C27" s="35">
+        <v>152.06840738548016</v>
+      </c>
+      <c r="D27" s="35">
+        <v>149.48348776235963</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="11">
         <v>43160</v>
       </c>
-      <c r="B28" s="20">
-        <v>155.63982283229944</v>
-      </c>
-      <c r="C28" s="37">
-        <v>151.84407952299696</v>
-      </c>
-      <c r="D28" s="37">
-        <v>148.699351570678</v>
+      <c r="B28" s="35">
+        <v>155.61029674358846</v>
+      </c>
+      <c r="C28" s="35">
+        <v>151.61508472063704</v>
+      </c>
+      <c r="D28" s="35">
+        <v>148.68091277354083</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="11">
         <v>43191</v>
       </c>
-      <c r="B29" s="20">
-        <v>151.60135644382305</v>
-      </c>
-      <c r="C29" s="37">
-        <v>146.71059521749663</v>
-      </c>
-      <c r="D29" s="37">
-        <v>147.81009673407749</v>
+      <c r="B29" s="35">
+        <v>151.61325958969238</v>
+      </c>
+      <c r="C29" s="35">
+        <v>146.64916937013052</v>
+      </c>
+      <c r="D29" s="35">
+        <v>147.7852429003305</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="11">
         <v>43221</v>
       </c>
-      <c r="B30" s="20">
-        <v>159.16207548226589</v>
-      </c>
-      <c r="C30" s="37">
-        <v>144.00386863146576</v>
-      </c>
-      <c r="D30" s="37">
-        <v>146.88333147737256</v>
+      <c r="B30" s="35">
+        <v>159.13595869124873</v>
+      </c>
+      <c r="C30" s="35">
+        <v>143.95636495941713</v>
+      </c>
+      <c r="D30" s="35">
+        <v>146.85012447979031</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="11">
         <v>43252</v>
       </c>
-      <c r="B31" s="20">
-        <v>151.44848091721315</v>
-      </c>
-      <c r="C31" s="37">
-        <v>143.02156579660877</v>
-      </c>
-      <c r="D31" s="37">
-        <v>145.97303418092244</v>
+      <c r="B31" s="35">
+        <v>151.46269456236098</v>
+      </c>
+      <c r="C31" s="35">
+        <v>143.05146854500981</v>
+      </c>
+      <c r="D31" s="35">
+        <v>145.93009204640515</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="11">
         <v>43282</v>
       </c>
-      <c r="B32" s="20">
-        <v>145.76463042864052</v>
-      </c>
-      <c r="C32" s="37">
-        <v>143.54221985511595</v>
-      </c>
-      <c r="D32" s="37">
-        <v>145.1289132526631</v>
+      <c r="B32" s="35">
+        <v>145.79343908898738</v>
+      </c>
+      <c r="C32" s="35">
+        <v>143.63208537644388</v>
+      </c>
+      <c r="D32" s="35">
+        <v>145.07478446264395</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="11">
         <v>43313</v>
       </c>
-      <c r="B33" s="20">
-        <v>147.04553382400547</v>
-      </c>
-      <c r="C33" s="37">
-        <v>146.67561906885047</v>
-      </c>
-      <c r="D33" s="37">
-        <v>144.39154289111033</v>
+      <c r="B33" s="35">
+        <v>147.00711245330541</v>
+      </c>
+      <c r="C33" s="35">
+        <v>146.8093660770966</v>
+      </c>
+      <c r="D33" s="35">
+        <v>144.32445296296231</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="11">
         <v>43344</v>
       </c>
-      <c r="B34" s="20">
-        <v>137.8944988928931</v>
-      </c>
-      <c r="C34" s="37">
-        <v>143.08805981767102</v>
-      </c>
-      <c r="D34" s="37">
-        <v>143.78630358826379</v>
+      <c r="B34" s="35">
+        <v>137.90411160324618</v>
+      </c>
+      <c r="C34" s="35">
+        <v>143.24215290095827</v>
+      </c>
+      <c r="D34" s="35">
+        <v>143.70569687794375</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="11">
         <v>43374</v>
       </c>
-      <c r="B35" s="20">
-        <v>143.57320349337792</v>
-      </c>
-      <c r="C35" s="37">
-        <v>143.76772571383782</v>
-      </c>
-      <c r="D35" s="37">
-        <v>143.32638712612882</v>
+      <c r="B35" s="35">
+        <v>143.5505657355927</v>
+      </c>
+      <c r="C35" s="35">
+        <v>143.91080140921949</v>
+      </c>
+      <c r="D35" s="35">
+        <v>143.23342136025533</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="11">
         <v>43405</v>
       </c>
-      <c r="B36" s="20">
-        <v>141.21184890028576</v>
-      </c>
-      <c r="C36" s="37">
-        <v>141.96874823084607</v>
-      </c>
-      <c r="D36" s="37">
-        <v>143.0128791281243</v>
+      <c r="B36" s="35">
+        <v>141.19511754067145</v>
+      </c>
+      <c r="C36" s="35">
+        <v>142.02431264760253</v>
+      </c>
+      <c r="D36" s="35">
+        <v>142.91114915494589</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="11">
         <v>43435</v>
       </c>
-      <c r="B37" s="20">
-        <v>135.67154302632184</v>
-      </c>
-      <c r="C37" s="37">
-        <v>141.90755386865095</v>
-      </c>
-      <c r="D37" s="37">
-        <v>142.83286108399358</v>
+      <c r="B37" s="35">
+        <v>135.71091214372095</v>
+      </c>
+      <c r="C37" s="35">
+        <v>141.89889638412308</v>
+      </c>
+      <c r="D37" s="35">
+        <v>142.72824923367764</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="11">
         <v>43466</v>
       </c>
-      <c r="B38" s="20">
-        <v>134.564995313265</v>
-      </c>
-      <c r="C38" s="37">
-        <v>143.10673026632992</v>
-      </c>
-      <c r="D38" s="37">
-        <v>142.76400870568844</v>
+      <c r="B38" s="35">
+        <v>134.54153173178952</v>
+      </c>
+      <c r="C38" s="35">
+        <v>142.93731057979133</v>
+      </c>
+      <c r="D38" s="35">
+        <v>142.66368204545634</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="11">
         <v>43497</v>
       </c>
-      <c r="B39" s="20">
-        <v>132.57194718265788</v>
-      </c>
-      <c r="C39" s="37">
-        <v>143.84766624936194</v>
-      </c>
-      <c r="D39" s="37">
-        <v>142.77570087867986</v>
+      <c r="B39" s="35">
+        <v>132.58348332921133</v>
+      </c>
+      <c r="C39" s="35">
+        <v>143.52977756983168</v>
+      </c>
+      <c r="D39" s="35">
+        <v>142.68578642997429</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="11">
         <v>43525</v>
       </c>
-      <c r="B40" s="20">
-        <v>144.41715750575651</v>
-      </c>
-      <c r="C40" s="37">
-        <v>141.9349090906895</v>
-      </c>
-      <c r="D40" s="37">
-        <v>142.83256119292363</v>
+      <c r="B40" s="35">
+        <v>144.40908494067796</v>
+      </c>
+      <c r="C40" s="35">
+        <v>141.61215057293396</v>
+      </c>
+      <c r="D40" s="35">
+        <v>142.75846591546289</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="11">
         <v>43556</v>
       </c>
-      <c r="B41" s="20">
-        <v>149.83961931661509</v>
-      </c>
-      <c r="C41" s="37">
-        <v>141.9983301682098</v>
-      </c>
-      <c r="D41" s="37">
-        <v>142.8976981521333</v>
+      <c r="B41" s="35">
+        <v>149.85097232641965</v>
+      </c>
+      <c r="C41" s="35">
+        <v>141.93570954161453</v>
+      </c>
+      <c r="D41" s="35">
+        <v>142.84370787042153</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="11">
         <v>43586</v>
       </c>
-      <c r="B42" s="20">
-        <v>162.83974753189364</v>
-      </c>
-      <c r="C42" s="37">
-        <v>143.13305027558306</v>
-      </c>
-      <c r="D42" s="37">
-        <v>142.93553075631897</v>
+      <c r="B42" s="35">
+        <v>162.78706748951424</v>
+      </c>
+      <c r="C42" s="35">
+        <v>143.09213824698108</v>
+      </c>
+      <c r="D42" s="35">
+        <v>142.90441777999979</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="11">
         <v>43617</v>
       </c>
-      <c r="B43" s="20">
-        <v>151.25410111244764</v>
-      </c>
-      <c r="C43" s="37">
-        <v>143.09945855809866</v>
-      </c>
-      <c r="D43" s="37">
-        <v>142.91419487292063</v>
+      <c r="B43" s="35">
+        <v>151.29542814502213</v>
+      </c>
+      <c r="C43" s="35">
+        <v>143.19001616894928</v>
+      </c>
+      <c r="D43" s="35">
+        <v>142.90650502224193</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="11">
         <v>43647</v>
       </c>
-      <c r="B44" s="20">
-        <v>146.20323233619627</v>
-      </c>
-      <c r="C44" s="37">
-        <v>145.43395888830977</v>
-      </c>
-      <c r="D44" s="37">
-        <v>142.80758712085614</v>
+      <c r="B44" s="35">
+        <v>146.20252878862499</v>
+      </c>
+      <c r="C44" s="35">
+        <v>145.55331255996614</v>
+      </c>
+      <c r="D44" s="35">
+        <v>142.821534606461</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="11">
         <v>43678</v>
       </c>
-      <c r="B45" s="20">
-        <v>141.60332874981128</v>
-      </c>
-      <c r="C45" s="37">
-        <v>145.03508972134111</v>
-      </c>
-      <c r="D45" s="37">
-        <v>142.59705600143741</v>
+      <c r="B45" s="35">
+        <v>141.58115459244769</v>
+      </c>
+      <c r="C45" s="35">
+        <v>145.23888847488195</v>
+      </c>
+      <c r="D45" s="35">
+        <v>142.62899943698829</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="11">
         <v>43709</v>
       </c>
-      <c r="B46" s="28">
-        <v>135.07531285730843</v>
-      </c>
-      <c r="C46" s="37">
-        <v>141.2682423763512</v>
-      </c>
-      <c r="D46" s="37">
-        <v>142.27267442050695</v>
+      <c r="B46" s="35">
+        <v>135.08034850716521</v>
+      </c>
+      <c r="C46" s="35">
+        <v>141.51423006407049</v>
+      </c>
+      <c r="D46" s="35">
+        <v>142.31796201020825</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="11">
         <v>43739</v>
       </c>
-      <c r="B47" s="28">
-        <v>142.25579775531418</v>
-      </c>
-      <c r="C47" s="37">
-        <v>143.5531431673603</v>
-      </c>
-      <c r="D47" s="37">
-        <v>141.83577117009767</v>
+      <c r="B47" s="35">
+        <v>142.2437072946467</v>
+      </c>
+      <c r="C47" s="35">
+        <v>143.71902249234273</v>
+      </c>
+      <c r="D47" s="35">
+        <v>141.88932387326062</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="11">
         <v>43770</v>
       </c>
-      <c r="B48" s="28">
-        <v>138.14131943492291</v>
-      </c>
-      <c r="C48" s="37">
-        <v>140.93089034348145</v>
-      </c>
-      <c r="D48" s="37">
-        <v>141.29440090065671</v>
+      <c r="B48" s="35">
+        <v>138.14809580021154</v>
+      </c>
+      <c r="C48" s="35">
+        <v>140.99861247830086</v>
+      </c>
+      <c r="D48" s="35">
+        <v>141.35202699694972</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="11">
         <v>43800</v>
       </c>
-      <c r="B49" s="28">
-        <v>135.44751977320297</v>
-      </c>
-      <c r="C49" s="37">
-        <v>140.83476794658512</v>
-      </c>
-      <c r="D49" s="37">
-        <v>140.66886856928977</v>
+      <c r="B49" s="35">
+        <v>135.45283386858216</v>
+      </c>
+      <c r="C49" s="35">
+        <v>140.85506830637232</v>
+      </c>
+      <c r="D49" s="35">
+        <v>140.72524131544031</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="11">
         <v>43831</v>
       </c>
-      <c r="B50" s="28">
-        <v>132.19356455544042</v>
-      </c>
-      <c r="C50" s="37">
-        <v>141.0172957796799</v>
-      </c>
-      <c r="D50" s="37">
-        <v>139.98691916698974</v>
+      <c r="B50" s="35">
+        <v>132.1630994727924</v>
+      </c>
+      <c r="C50" s="35">
+        <v>140.7579392366286</v>
+      </c>
+      <c r="D50" s="35">
+        <v>140.03746181622614</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="11">
         <v>43862</v>
       </c>
-      <c r="B51" s="28">
-        <v>129.61940932164029</v>
-      </c>
-      <c r="C51" s="37">
-        <v>140.82397846349957</v>
-      </c>
-      <c r="D51" s="37">
-        <v>139.28358985447613</v>
+      <c r="B51" s="35">
+        <v>129.63900633914159</v>
+      </c>
+      <c r="C51" s="35">
+        <v>140.38441035757879</v>
+      </c>
+      <c r="D51" s="35">
+        <v>139.32756341576226</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="11">
         <v>43891</v>
       </c>
-      <c r="B52" s="28">
-        <v>128.38599328767583</v>
-      </c>
-      <c r="C52" s="37">
-        <v>126.01298635165223</v>
-      </c>
-      <c r="D52" s="37">
-        <v>138.59891085324503</v>
+      <c r="B52" s="35">
+        <v>128.39686135282281</v>
+      </c>
+      <c r="C52" s="35">
+        <v>125.67853123969753</v>
+      </c>
+      <c r="D52" s="35">
+        <v>138.64038957717426</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="11">
         <v>43922</v>
       </c>
-      <c r="B53" s="28">
-        <v>111.81827837013516</v>
-      </c>
-      <c r="C53" s="37">
-        <v>104.29540079786129</v>
-      </c>
-      <c r="D53" s="37">
-        <v>137.97049291200989</v>
+      <c r="B53" s="35">
+        <v>111.83582082559583</v>
+      </c>
+      <c r="C53" s="35">
+        <v>104.30203975954247</v>
+      </c>
+      <c r="D53" s="35">
+        <v>138.01785758912729</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="11">
         <v>43952</v>
       </c>
-      <c r="B54" s="28">
-        <v>130.30963100770941</v>
-      </c>
-      <c r="C54" s="37">
-        <v>114.76826799366857</v>
-      </c>
-      <c r="D54" s="37">
-        <v>137.42962204822177</v>
+      <c r="B54" s="35">
+        <v>130.29879688172196</v>
+      </c>
+      <c r="C54" s="35">
+        <v>114.71878588574795</v>
+      </c>
+      <c r="D54" s="35">
+        <v>137.49743527229873</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="25">
+      <c r="A55" s="24">
         <v>43983</v>
       </c>
-      <c r="B55" s="28">
-        <v>133.78434132181565</v>
-      </c>
-      <c r="C55" s="37">
-        <v>124.00857978417032</v>
-      </c>
-      <c r="D55" s="37">
-        <v>136.99759826625882</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="27" customFormat="1">
-      <c r="A56" s="25">
+      <c r="B55" s="35">
+        <v>133.77763299234232</v>
+      </c>
+      <c r="C55" s="35">
+        <v>124.09711863588124</v>
+      </c>
+      <c r="D55" s="35">
+        <v>137.10742954591234</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="26" customFormat="1">
+      <c r="A56" s="24">
         <v>44013</v>
       </c>
-      <c r="B56" s="28">
-        <v>127.59092134022666</v>
-      </c>
-      <c r="C56" s="37">
-        <v>126.7877742600087</v>
-      </c>
-      <c r="D56" s="37">
-        <v>136.68305408500382</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="27" customFormat="1">
-      <c r="A57" s="25">
+      <c r="B56" s="35">
+        <v>127.61990339421432</v>
+      </c>
+      <c r="C56" s="35">
+        <v>126.89789564817646</v>
+      </c>
+      <c r="D56" s="35">
+        <v>136.86088957424417</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="26" customFormat="1">
+      <c r="A57" s="24">
         <v>44044</v>
       </c>
-      <c r="B57" s="37">
-        <v>125.44572625215507</v>
-      </c>
-      <c r="C57" s="37">
-        <v>129.24369156433485</v>
-      </c>
-      <c r="D57" s="37">
-        <v>136.4820277231529</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="30" customFormat="1">
-      <c r="A58" s="31">
+      <c r="B57" s="35">
+        <v>125.43898663724799</v>
+      </c>
+      <c r="C57" s="35">
+        <v>129.48320700006892</v>
+      </c>
+      <c r="D57" s="35">
+        <v>136.75537329595369</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="28" customFormat="1">
+      <c r="A58" s="29">
         <v>44075</v>
       </c>
-      <c r="B58" s="37">
-        <v>127.10134993432418</v>
-      </c>
-      <c r="C58" s="37">
-        <v>131.90273729872393</v>
-      </c>
-      <c r="D58" s="37">
-        <v>136.37949333709039</v>
+      <c r="B58" s="35">
+        <v>127.13653193666156</v>
+      </c>
+      <c r="C58" s="35">
+        <v>132.20386247974432</v>
+      </c>
+      <c r="D58" s="35">
+        <v>136.77462008253579</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="11">
         <v>44105</v>
       </c>
-      <c r="B59" s="37">
-        <v>132.07223639537102</v>
-      </c>
-      <c r="C59" s="37">
-        <v>133.59233473889026</v>
-      </c>
-      <c r="D59" s="37">
-        <v>136.35098476917821</v>
+      <c r="B59" s="35">
+        <v>132.1713277082747</v>
+      </c>
+      <c r="C59" s="35">
+        <v>133.82124662037532</v>
+      </c>
+      <c r="D59" s="35">
+        <v>136.89212820711597</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="31">
+      <c r="A60" s="29">
         <v>44136</v>
       </c>
-      <c r="B60" s="37">
-        <v>133.43700494930926</v>
-      </c>
-      <c r="C60" s="37">
-        <v>135.56679862668341</v>
-      </c>
-      <c r="D60" s="37">
-        <v>136.36596188260637</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="24" customFormat="1">
-      <c r="A61" s="31">
+      <c r="B60" s="35">
+        <v>133.48252419058556</v>
+      </c>
+      <c r="C60" s="35">
+        <v>135.67203036551453</v>
+      </c>
+      <c r="D60" s="35">
+        <v>137.0731616754434</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="23" customFormat="1">
+      <c r="A61" s="29">
         <v>44166</v>
       </c>
-      <c r="B61" s="37">
-        <v>132.57150330151808</v>
-      </c>
-      <c r="C61" s="37">
-        <v>136.36321070111322</v>
-      </c>
-      <c r="D61" s="37">
-        <v>136.39612699796803</v>
+      <c r="B61" s="35">
+        <v>132.42256304695755</v>
+      </c>
+      <c r="C61" s="35">
+        <v>136.36598915545181</v>
+      </c>
+      <c r="D61" s="35">
+        <v>137.28396095093984</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="11">
         <v>44197</v>
       </c>
-      <c r="B62" s="37">
-        <v>129.22521775352402</v>
-      </c>
-      <c r="C62" s="37">
-        <v>138.97652161294636</v>
-      </c>
-      <c r="D62" s="37">
-        <v>136.41650437485583</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="24" customFormat="1">
+      <c r="B62" s="35">
+        <v>129.60926841868047</v>
+      </c>
+      <c r="C62" s="35">
+        <v>139.38818252853005</v>
+      </c>
+      <c r="D62" s="35">
+        <v>137.49288217141162</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="23" customFormat="1">
       <c r="A63" s="11">
         <v>44228</v>
       </c>
-      <c r="B63" s="38">
-        <v>126.2948878638516</v>
-      </c>
-      <c r="C63" s="38">
-        <v>137.53246960664117</v>
-      </c>
-      <c r="D63" s="38">
-        <v>136.40752715245807</v>
+      <c r="B63" s="35">
+        <v>126.91699408993593</v>
+      </c>
+      <c r="C63" s="35">
+        <v>138.12924188259592</v>
+      </c>
+      <c r="D63" s="35">
+        <v>137.67163056468692</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="11">
+        <v>44256</v>
+      </c>
+      <c r="B64" s="36">
+        <v>143.09296631437621</v>
+      </c>
+      <c r="C64" s="36">
+        <v>137.83962525261128</v>
+      </c>
+      <c r="D64" s="36">
+        <v>137.80110563557497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Se cargaron nuevos datos de EMAE, Comex y datos fiscales"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8BF305-521C-45BC-9369-3FF696023E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7F65A5-C563-4F3E-AAF8-374757F3BB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,7 +666,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1919,7 +1918,7 @@
       <c r="E52">
         <v>4.5</v>
       </c>
-      <c r="H52" s="30"/>
+      <c r="H52" s="29"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -1937,7 +1936,7 @@
       <c r="E53">
         <v>3.5</v>
       </c>
-      <c r="H53" s="30"/>
+      <c r="H53" s="29"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -1955,7 +1954,7 @@
       <c r="E54">
         <v>3.8</v>
       </c>
-      <c r="H54" s="30"/>
+      <c r="H54" s="29"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -2040,22 +2039,22 @@
       <c r="A2" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <v>3.1</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <v>3.7</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="28">
         <v>4.2</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="28">
         <v>1.9</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <v>2.9</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="28">
         <v>4.2</v>
       </c>
       <c r="H2" s="23">
@@ -2066,22 +2065,22 @@
       <c r="A3" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="28">
         <v>0.4</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="28">
         <v>1.2</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>1.5</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <v>1.7</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <v>0.8</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="28">
         <v>3.3</v>
       </c>
       <c r="H3" s="23">
@@ -2092,22 +2091,22 @@
       <c r="A4" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <v>4.5</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="28">
         <v>4.5</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <v>5</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <v>5.0999999999999996</v>
       </c>
       <c r="H4" s="23">
@@ -2118,22 +2117,22 @@
       <c r="A5" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="28">
         <v>5.9</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <v>3.6</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="28">
         <v>3.8</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <v>5.0999999999999996</v>
       </c>
       <c r="H5" s="23">
@@ -2144,22 +2143,22 @@
       <c r="A6" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>-0.6</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <v>1.3</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>3</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>-0.8</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <v>-1.4</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>1.7</v>
       </c>
       <c r="H6" s="23">
@@ -2170,22 +2169,22 @@
       <c r="A7" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>13.9</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>10.199999999999999</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <v>5.3</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <v>8</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="28">
         <v>13</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <v>6.8</v>
       </c>
       <c r="H7" s="23">
@@ -2196,22 +2195,22 @@
       <c r="A8" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="28">
         <v>4.8</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>3.1</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>5.4</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="28">
         <v>3</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="28">
         <v>4.8</v>
       </c>
       <c r="H8" s="24">
@@ -2222,22 +2221,22 @@
       <c r="A9" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="28">
         <v>6.1</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <v>5.8</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>2.6</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>5.8</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>9</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="28">
         <v>4.3</v>
       </c>
       <c r="H9" s="23">
@@ -2248,22 +2247,22 @@
       <c r="A10" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="28">
         <v>2.5</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>1.9</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="28">
         <v>2.8</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="28">
         <v>4.2</v>
       </c>
       <c r="H10" s="23">
@@ -2280,7 +2279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2316,25 +2315,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>3</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="33">
         <v>3.1</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="35">
         <v>2.9</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="39">
         <v>3</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="37">
         <v>2.8</v>
       </c>
-      <c r="G2" s="42">
+      <c r="G2" s="41">
         <v>3.2</v>
       </c>
-      <c r="H2" s="44">
+      <c r="H2" s="43">
         <v>3.3</v>
       </c>
     </row>
@@ -2342,25 +2341,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="30">
         <v>3.4</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="32">
         <v>3.6</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="34">
         <v>3.3</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="38">
         <v>3</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="36">
         <v>2.8</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="40">
         <v>3.3</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="42">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -2368,25 +2367,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="30">
         <v>3.1</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="32">
         <v>3.5</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="34">
         <v>2.8</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="38">
         <v>2.1</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="36">
         <v>3.3</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="40">
         <v>2.1</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="42">
         <v>2.6</v>
       </c>
     </row>
@@ -2394,25 +2393,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
         <v>1.2</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="32">
         <v>0.6</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <v>3.2</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <v>1.7</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="40">
         <v>3.3</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="42">
         <v>3.7</v>
       </c>
     </row>
@@ -2420,25 +2419,25 @@
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>2.9</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <v>3.6</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="34">
         <v>2.5</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <v>1.8</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <v>1.2</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G6" s="40">
         <v>2.4</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="42">
         <v>3</v>
       </c>
     </row>
@@ -2446,25 +2445,25 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="30">
         <v>2.7</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>2.7</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>2.7</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="38">
         <v>2.9</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="36">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="40">
         <v>3.2</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="42">
         <v>3</v>
       </c>
     </row>
@@ -2472,25 +2471,25 @@
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <v>3.8</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>2.9</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="38">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="36">
         <v>4.2</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="40">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="42">
         <v>3.9</v>
       </c>
     </row>
@@ -2498,25 +2497,25 @@
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="30">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>1.5</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <v>2.9</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="38">
         <v>2.9</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="36">
         <v>2.7</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="40">
         <v>2.8</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="42">
         <v>2.4</v>
       </c>
     </row>
@@ -2524,25 +2523,25 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="30">
         <v>0.4</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="32">
         <v>0.1</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="34">
         <v>0.3</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="38">
         <v>1.3</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="36">
         <v>2.1</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="40">
         <v>-0.5</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="42">
         <v>0.2</v>
       </c>
     </row>
@@ -2550,25 +2549,25 @@
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <v>3.1</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="32">
         <v>3.9</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <v>1.9</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="38">
         <v>3.1</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <v>3.6</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="40">
         <v>3.2</v>
       </c>
-      <c r="H11" s="43">
+      <c r="H11" s="42">
         <v>3.6</v>
       </c>
     </row>
@@ -2576,25 +2575,25 @@
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <v>2.5</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="32">
         <v>3.9</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="34">
         <v>1.3</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="38">
         <v>0.2</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="36">
         <v>0.9</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="40">
         <v>1.4</v>
       </c>
-      <c r="H12" s="43">
+      <c r="H12" s="42">
         <v>2.5</v>
       </c>
     </row>
@@ -2602,25 +2601,25 @@
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="30">
         <v>4.8</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>5.5</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="34">
         <v>3.9</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="38">
         <v>4.5</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="36">
         <v>4.5</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="40">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H13" s="43">
+      <c r="H13" s="42">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -2628,25 +2627,25 @@
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="30">
         <v>3.2</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="32">
         <v>3.7</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="34">
         <v>3</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="38">
         <v>2.7</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="36">
         <v>2.5</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="40">
         <v>1.9</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="42">
         <v>2.8</v>
       </c>
     </row>
@@ -2696,25 +2695,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="45">
         <v>51.8</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="47">
         <v>50.4</v>
       </c>
-      <c r="D2" s="50">
+      <c r="D2" s="49">
         <v>53</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="53">
         <v>52.9</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="51">
         <v>52</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="55">
         <v>55.1</v>
       </c>
-      <c r="H2" s="58">
+      <c r="H2" s="57">
         <v>50.6</v>
       </c>
     </row>
@@ -2722,25 +2721,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="44">
         <v>56.4</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="46">
         <v>53.8</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="48">
         <v>59</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="52">
         <v>59.6</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="50">
         <v>57</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="54">
         <v>59.8</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="56">
         <v>53.5</v>
       </c>
     </row>
@@ -2748,25 +2747,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="44">
         <v>51.2</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="46">
         <v>50.2</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="48">
         <v>52.1</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="52">
         <v>53.4</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="50">
         <v>53.4</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="54">
         <v>50.8</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="56">
         <v>48.4</v>
       </c>
     </row>
@@ -2774,25 +2773,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="44">
         <v>61.7</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="46">
         <v>64.2</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="48">
         <v>59.1</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="52">
         <v>57.5</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="50">
         <v>58.6</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="54">
         <v>64.599999999999994</v>
       </c>
-      <c r="H5" s="57">
+      <c r="H5" s="56">
         <v>62.2</v>
       </c>
     </row>
@@ -2800,25 +2799,25 @@
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <v>30.6</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="46">
         <v>30.8</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="48">
         <v>29.8</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="52">
         <v>28.9</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="50">
         <v>31.7</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="54">
         <v>35.1</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="56">
         <v>29</v>
       </c>
     </row>
@@ -2826,25 +2825,25 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <v>48.4</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="46">
         <v>48.9</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="48">
         <v>47.7</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="52">
         <v>48.6</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="50">
         <v>45.9</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="54">
         <v>50.7</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="56">
         <v>50.2</v>
       </c>
     </row>
@@ -2852,25 +2851,25 @@
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>54.4</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="46">
         <v>49.8</v>
       </c>
-      <c r="D8" s="49">
+      <c r="D8" s="48">
         <v>57.5</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="52">
         <v>60</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="50">
         <v>60.2</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="54">
         <v>60.3</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="56">
         <v>52.3</v>
       </c>
     </row>
@@ -2878,25 +2877,25 @@
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>62.9</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="46">
         <v>58.6</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="48">
         <v>66.3</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="52">
         <v>62.1</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="50">
         <v>63.6</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="54">
         <v>71.7</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="56">
         <v>67.900000000000006</v>
       </c>
     </row>
@@ -2904,25 +2903,25 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>27.6</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="46">
         <v>25.3</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="48">
         <v>28.1</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="52">
         <v>34.4</v>
       </c>
-      <c r="F10" s="51">
+      <c r="F10" s="50">
         <v>32.1</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="54">
         <v>27.5</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="56">
         <v>33.799999999999997</v>
       </c>
     </row>
@@ -2930,25 +2929,25 @@
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="44">
         <v>48.7</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="46">
         <v>50.3</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="48">
         <v>50.6</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="52">
         <v>44.9</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="50">
         <v>40.4</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="54">
         <v>43.2</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="56">
         <v>41.9</v>
       </c>
     </row>
@@ -2956,25 +2955,25 @@
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="44">
         <v>43</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="46">
         <v>48.3</v>
       </c>
-      <c r="D12" s="49">
+      <c r="D12" s="48">
         <v>40.9</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="52">
         <v>37.200000000000003</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="50">
         <v>36.200000000000003</v>
       </c>
-      <c r="G12" s="55">
+      <c r="G12" s="54">
         <v>32.200000000000003</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="56">
         <v>31.9</v>
       </c>
     </row>
@@ -2982,25 +2981,25 @@
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="44">
         <v>54.3</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="46">
         <v>56.1</v>
       </c>
-      <c r="D13" s="49">
+      <c r="D13" s="48">
         <v>52.2</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="52">
         <v>52</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="50">
         <v>54.4</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="54">
         <v>61.1</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H13" s="56">
         <v>46.4</v>
       </c>
     </row>
@@ -3008,25 +3007,25 @@
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="44">
         <v>35.5</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="46">
         <v>39.299999999999997</v>
       </c>
-      <c r="D14" s="49">
+      <c r="D14" s="48">
         <v>33.700000000000003</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="52">
         <v>34.5</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="50">
         <v>31.3</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="54">
         <v>28.8</v>
       </c>
-      <c r="H14" s="57">
+      <c r="H14" s="56">
         <v>29.4</v>
       </c>
     </row>
@@ -4052,14 +4051,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="59"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4651,14 +4650,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="59"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4807,8 +4806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,14 +4834,14 @@
         <v>79</v>
       </c>
       <c r="B2">
-        <v>4917</v>
+        <v>7314</v>
       </c>
       <c r="C2">
-        <v>6270</v>
+        <v>9141</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1353</v>
+        <v>-1827</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4850,14 +4849,14 @@
         <v>80</v>
       </c>
       <c r="B3">
-        <v>1421</v>
+        <v>2153</v>
       </c>
       <c r="C3">
-        <v>250</v>
+        <v>366</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1171</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4865,14 +4864,14 @@
         <v>81</v>
       </c>
       <c r="B4">
-        <v>1562</v>
+        <v>2397</v>
       </c>
       <c r="C4">
-        <v>766</v>
+        <v>1096</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>796</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4880,14 +4879,14 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>325</v>
+        <v>541</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>528</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4895,14 +4894,14 @@
         <v>83</v>
       </c>
       <c r="B6">
-        <v>2091</v>
+        <v>3283</v>
       </c>
       <c r="C6">
-        <v>2570</v>
+        <v>4176</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-479</v>
+        <v>-893</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4910,14 +4909,14 @@
         <v>84</v>
       </c>
       <c r="B7">
-        <v>3471</v>
+        <v>5580</v>
       </c>
       <c r="C7">
-        <v>3512</v>
+        <v>5116</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-41</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4925,14 +4924,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>355</v>
+        <v>504</v>
       </c>
       <c r="C8">
-        <v>208</v>
+        <v>310</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4940,14 +4939,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>330</v>
+        <v>549</v>
       </c>
       <c r="C9">
-        <v>192</v>
+        <v>318</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>138</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4955,14 +4954,14 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>299</v>
+        <v>449</v>
       </c>
       <c r="C10">
-        <v>237</v>
+        <v>456</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4970,14 +4969,14 @@
         <v>88</v>
       </c>
       <c r="B11">
-        <v>3203</v>
+        <v>4470</v>
       </c>
       <c r="C11">
-        <v>1474</v>
+        <v>2172</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1729</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4985,14 +4984,14 @@
         <v>89</v>
       </c>
       <c r="B12">
-        <v>2199</v>
+        <v>3353</v>
       </c>
       <c r="C12">
-        <v>4650</v>
+        <v>6916</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-2451</v>
+        <v>-3563</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5000,14 +4999,14 @@
         <v>90</v>
       </c>
       <c r="B13">
-        <v>350</v>
+        <v>731</v>
       </c>
       <c r="C13">
-        <v>258</v>
+        <v>342</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5015,14 +5014,14 @@
         <v>91</v>
       </c>
       <c r="B14">
-        <v>123</v>
+        <v>368</v>
       </c>
       <c r="C14">
-        <v>420</v>
+        <v>622</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-297</v>
+        <v>-254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,14 +5029,14 @@
         <v>92</v>
       </c>
       <c r="B15">
-        <v>1558</v>
+        <v>2122</v>
       </c>
       <c r="C15">
-        <v>504</v>
+        <v>789</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1054</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5045,14 +5044,14 @@
         <v>93</v>
       </c>
       <c r="B16">
-        <v>2016</v>
+        <v>3035</v>
       </c>
       <c r="C16">
-        <v>347</v>
+        <v>782</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1669</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5060,14 +5059,14 @@
         <v>94</v>
       </c>
       <c r="B17">
-        <v>1828</v>
+        <v>2721</v>
       </c>
       <c r="C17">
-        <v>195</v>
+        <v>409</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1633</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5075,14 +5074,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>204</v>
+        <v>269</v>
       </c>
       <c r="C18">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5090,14 +5089,14 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>353</v>
+        <v>466</v>
       </c>
       <c r="C19">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>255</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,14 +5104,14 @@
         <v>97</v>
       </c>
       <c r="B20">
-        <v>1711</v>
+        <v>2319</v>
       </c>
       <c r="C20">
-        <v>646</v>
+        <v>1019</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1065</v>
+        <v>1300</v>
       </c>
     </row>
   </sheetData>
@@ -5341,10 +5340,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D66"/>
+    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5375,11 +5374,11 @@
       <c r="B2" s="17">
         <v>134.746450413497</v>
       </c>
-      <c r="C2" s="27">
-        <v>147.88335432233677</v>
-      </c>
-      <c r="D2" s="27">
-        <v>147.11554539998707</v>
+      <c r="C2" s="26">
+        <v>147.9503650346366</v>
+      </c>
+      <c r="D2" s="26">
+        <v>147.11218303143568</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5389,11 +5388,11 @@
       <c r="B3" s="17">
         <v>134.23236103862499</v>
       </c>
-      <c r="C3" s="27">
-        <v>146.95941768324749</v>
-      </c>
-      <c r="D3" s="27">
-        <v>146.52998120307842</v>
+      <c r="C3" s="26">
+        <v>146.83927165376153</v>
+      </c>
+      <c r="D3" s="26">
+        <v>146.52013949247683</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5403,11 +5402,11 @@
       <c r="B4" s="17">
         <v>150.08789423669501</v>
       </c>
-      <c r="C4" s="27">
-        <v>145.97404778652685</v>
-      </c>
-      <c r="D4" s="27">
-        <v>145.97959679420725</v>
+      <c r="C4" s="26">
+        <v>145.92970847053681</v>
+      </c>
+      <c r="D4" s="26">
+        <v>145.96209323375285</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5417,11 +5416,11 @@
       <c r="B5" s="17">
         <v>153.250674366629</v>
       </c>
-      <c r="C5" s="27">
-        <v>144.92929964485376</v>
-      </c>
-      <c r="D5" s="27">
-        <v>145.50138741106167</v>
+      <c r="C5" s="26">
+        <v>144.99578843421494</v>
+      </c>
+      <c r="D5" s="26">
+        <v>145.47536386029111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5431,11 +5430,11 @@
       <c r="B6" s="17">
         <v>163.51360808690501</v>
       </c>
-      <c r="C6" s="27">
-        <v>144.23277687076845</v>
-      </c>
-      <c r="D6" s="27">
-        <v>145.12376717768629</v>
+      <c r="C6" s="26">
+        <v>144.33215794720019</v>
+      </c>
+      <c r="D6" s="26">
+        <v>145.08907396638045</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5445,11 +5444,11 @@
       <c r="B7" s="17">
         <v>153.66209524099801</v>
       </c>
-      <c r="C7" s="27">
-        <v>144.43990435090006</v>
-      </c>
-      <c r="D7" s="27">
-        <v>144.86655876821121</v>
+      <c r="C7" s="26">
+        <v>144.47004118760216</v>
+      </c>
+      <c r="D7" s="26">
+        <v>144.82436533343756</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5459,11 +5458,11 @@
       <c r="B8" s="17">
         <v>143.73110098180101</v>
       </c>
-      <c r="C8" s="27">
-        <v>144.47904017903048</v>
-      </c>
-      <c r="D8" s="27">
-        <v>144.7386858611662</v>
+      <c r="C8" s="26">
+        <v>144.4525553765445</v>
+      </c>
+      <c r="D8" s="26">
+        <v>144.69192838137894</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5473,11 +5472,11 @@
       <c r="B9" s="17">
         <v>143.67410264860499</v>
       </c>
-      <c r="C9" s="27">
-        <v>145.5637513243561</v>
-      </c>
-      <c r="D9" s="27">
-        <v>144.74348992567357</v>
+      <c r="C9" s="26">
+        <v>145.56531993248811</v>
+      </c>
+      <c r="D9" s="26">
+        <v>144.69533205846275</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5487,11 +5486,11 @@
       <c r="B10" s="17">
         <v>142.00773744282</v>
       </c>
-      <c r="C10" s="27">
-        <v>145.17412217342718</v>
-      </c>
-      <c r="D10" s="27">
-        <v>144.87858632853352</v>
+      <c r="C10" s="26">
+        <v>145.11133981162371</v>
+      </c>
+      <c r="D10" s="26">
+        <v>144.8314423805532</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5501,11 +5500,11 @@
       <c r="B11" s="17">
         <v>141.13686329808101</v>
       </c>
-      <c r="C11" s="27">
-        <v>144.95967387512559</v>
-      </c>
-      <c r="D11" s="27">
-        <v>145.13513191359877</v>
+      <c r="C11" s="26">
+        <v>145.04109776370345</v>
+      </c>
+      <c r="D11" s="26">
+        <v>145.09045492365055</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5515,11 +5514,11 @@
       <c r="B12" s="17">
         <v>144.93832064073001</v>
       </c>
-      <c r="C12" s="27">
-        <v>145.92678260665005</v>
-      </c>
-      <c r="D12" s="27">
-        <v>145.49870071033413</v>
+      <c r="C12" s="26">
+        <v>145.84305574159546</v>
+      </c>
+      <c r="D12" s="26">
+        <v>145.456028112436</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5529,11 +5528,11 @@
       <c r="B13" s="17">
         <v>142.590145160319</v>
       </c>
-      <c r="C13" s="27">
-        <v>147.04918298290536</v>
-      </c>
-      <c r="D13" s="27">
-        <v>145.95599626014913</v>
+      <c r="C13" s="26">
+        <v>147.04065242367525</v>
+      </c>
+      <c r="D13" s="26">
+        <v>145.91408159680924</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5543,11 +5542,11 @@
       <c r="B14" s="17">
         <v>136.63265948872001</v>
       </c>
-      <c r="C14" s="27">
-        <v>147.33001487986564</v>
-      </c>
-      <c r="D14" s="27">
-        <v>146.49060927580487</v>
+      <c r="C14" s="26">
+        <v>147.35877257761507</v>
+      </c>
+      <c r="D14" s="26">
+        <v>146.4480015691835</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5557,11 +5556,11 @@
       <c r="B15" s="17">
         <v>132.158516342166</v>
       </c>
-      <c r="C15" s="27">
-        <v>146.71869793117506</v>
-      </c>
-      <c r="D15" s="27">
-        <v>147.08442521245394</v>
+      <c r="C15" s="26">
+        <v>146.53352908833722</v>
+      </c>
+      <c r="D15" s="26">
+        <v>147.04021878673237</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5571,11 +5570,11 @@
       <c r="B16" s="17">
         <v>152.62095855115601</v>
       </c>
-      <c r="C16" s="27">
-        <v>147.93735460620078</v>
-      </c>
-      <c r="D16" s="27">
-        <v>147.71742611497612</v>
+      <c r="C16" s="26">
+        <v>147.92357089538024</v>
+      </c>
+      <c r="D16" s="26">
+        <v>147.67137805280174</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5585,11 +5584,11 @@
       <c r="B17" s="17">
         <v>151.94634477931299</v>
       </c>
-      <c r="C17" s="27">
-        <v>147.39684901903777</v>
-      </c>
-      <c r="D17" s="27">
-        <v>148.36783128320445</v>
+      <c r="C17" s="26">
+        <v>147.53801877515716</v>
+      </c>
+      <c r="D17" s="26">
+        <v>148.31974657066576</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5599,11 +5598,11 @@
       <c r="B18" s="17">
         <v>168.389209458756</v>
       </c>
-      <c r="C18" s="27">
-        <v>148.32921616094166</v>
-      </c>
-      <c r="D18" s="27">
-        <v>149.00793405185453</v>
+      <c r="C18" s="26">
+        <v>148.53019646261558</v>
+      </c>
+      <c r="D18" s="26">
+        <v>148.95823457754247</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5613,11 +5612,11 @@
       <c r="B19" s="17">
         <v>161.035685505239</v>
       </c>
-      <c r="C19" s="27">
-        <v>150.29265050625756</v>
-      </c>
-      <c r="D19" s="27">
-        <v>149.6065906595652</v>
+      <c r="C19" s="26">
+        <v>150.3196109616531</v>
+      </c>
+      <c r="D19" s="26">
+        <v>149.55663503812107</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5627,11 +5626,11 @@
       <c r="B20" s="17">
         <v>150.30605023794101</v>
       </c>
-      <c r="C20" s="27">
-        <v>150.23515842441637</v>
-      </c>
-      <c r="D20" s="27">
-        <v>150.12958763472528</v>
+      <c r="C20" s="26">
+        <v>150.20765294270382</v>
+      </c>
+      <c r="D20" s="26">
+        <v>150.08159435835401</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5641,11 +5640,11 @@
       <c r="B21" s="17">
         <v>149.255342821905</v>
       </c>
-      <c r="C21" s="27">
-        <v>150.34999364544547</v>
-      </c>
-      <c r="D21" s="27">
-        <v>150.54124357837162</v>
+      <c r="C21" s="26">
+        <v>150.28103752473896</v>
+      </c>
+      <c r="D21" s="26">
+        <v>150.49803396508725</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5655,11 +5654,11 @@
       <c r="B22" s="17">
         <v>146.38655949566899</v>
       </c>
-      <c r="C22" s="27">
-        <v>151.44914775980465</v>
-      </c>
-      <c r="D22" s="27">
-        <v>150.80656715855386</v>
+      <c r="C22" s="26">
+        <v>151.35568822608755</v>
+      </c>
+      <c r="D22" s="26">
+        <v>150.77128177847973</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5669,11 +5668,11 @@
       <c r="B23" s="17">
         <v>149.38594914959</v>
       </c>
-      <c r="C23" s="27">
-        <v>151.55543198952307</v>
-      </c>
-      <c r="D23" s="27">
-        <v>150.89816698537243</v>
+      <c r="C23" s="26">
+        <v>151.57943226974629</v>
+      </c>
+      <c r="D23" s="26">
+        <v>150.87359247107446</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5683,11 +5682,11 @@
       <c r="B24" s="17">
         <v>151.926042634336</v>
       </c>
-      <c r="C24" s="27">
-        <v>152.74147634278862</v>
-      </c>
-      <c r="D24" s="27">
-        <v>150.79484301484416</v>
+      <c r="C24" s="26">
+        <v>152.73084635410285</v>
+      </c>
+      <c r="D24" s="26">
+        <v>150.78307901321071</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5697,11 +5696,11 @@
       <c r="B25" s="17">
         <v>146.78338564334001</v>
       </c>
-      <c r="C25" s="27">
-        <v>152.49071309399477</v>
-      </c>
-      <c r="D25" s="27">
-        <v>150.48909594926957</v>
+      <c r="C25" s="26">
+        <v>152.46834825811229</v>
+      </c>
+      <c r="D25" s="26">
+        <v>150.49004210307629</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5711,11 +5710,11 @@
       <c r="B26" s="17">
         <v>142.754737365257</v>
       </c>
-      <c r="C26" s="27">
-        <v>152.06827499827583</v>
-      </c>
-      <c r="D26" s="27">
-        <v>149.99088015947336</v>
+      <c r="C26" s="26">
+        <v>152.00409144910782</v>
+      </c>
+      <c r="D26" s="26">
+        <v>150.00274424327796</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5725,11 +5724,11 @@
       <c r="B27" s="17">
         <v>138.81628446908201</v>
       </c>
-      <c r="C27" s="27">
-        <v>152.14854332169534</v>
-      </c>
-      <c r="D27" s="27">
-        <v>149.32301560733512</v>
+      <c r="C27" s="26">
+        <v>151.91202563792464</v>
+      </c>
+      <c r="D27" s="26">
+        <v>149.34241845963436</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5739,11 +5738,11 @@
       <c r="B28" s="17">
         <v>155.84525065925999</v>
       </c>
-      <c r="C28" s="27">
-        <v>151.1494701075371</v>
-      </c>
-      <c r="D28" s="27">
-        <v>148.52267385887751</v>
+      <c r="C28" s="26">
+        <v>151.21030949842233</v>
+      </c>
+      <c r="D28" s="26">
+        <v>148.54341560350122</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5753,11 +5752,11 @@
       <c r="B29" s="17">
         <v>151.55142032267901</v>
       </c>
-      <c r="C29" s="27">
-        <v>146.38126818716347</v>
-      </c>
-      <c r="D29" s="27">
-        <v>147.63657527497332</v>
+      <c r="C29" s="26">
+        <v>146.55811223731223</v>
+      </c>
+      <c r="D29" s="26">
+        <v>147.65249552769166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5767,11 +5766,11 @@
       <c r="B30" s="17">
         <v>159.57159359786201</v>
       </c>
-      <c r="C30" s="27">
-        <v>143.85058137262232</v>
-      </c>
-      <c r="D30" s="27">
-        <v>146.71729166578518</v>
+      <c r="C30" s="26">
+        <v>144.20010262138075</v>
+      </c>
+      <c r="D30" s="26">
+        <v>146.7235762160648</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5781,11 +5780,11 @@
       <c r="B31" s="17">
         <v>151.09398567477399</v>
       </c>
-      <c r="C31" s="27">
-        <v>143.10983252743671</v>
-      </c>
-      <c r="D31" s="27">
-        <v>145.81661639384396</v>
+      <c r="C31" s="26">
+        <v>143.04047123913992</v>
+      </c>
+      <c r="D31" s="26">
+        <v>145.81114359880948</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5795,11 +5794,11 @@
       <c r="B32" s="17">
         <v>145.98410181709701</v>
       </c>
-      <c r="C32" s="27">
-        <v>143.27961546980922</v>
-      </c>
-      <c r="D32" s="27">
-        <v>144.98229748832284</v>
+      <c r="C32" s="26">
+        <v>143.13673693758284</v>
+      </c>
+      <c r="D32" s="26">
+        <v>144.96543625441888</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5809,11 +5808,11 @@
       <c r="B33" s="17">
         <v>146.772858569193</v>
       </c>
-      <c r="C33" s="27">
-        <v>146.83913170420357</v>
-      </c>
-      <c r="D33" s="27">
-        <v>144.25535739802328</v>
+      <c r="C33" s="26">
+        <v>146.77792181071217</v>
+      </c>
+      <c r="D33" s="26">
+        <v>144.22778647059934</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5823,11 +5822,11 @@
       <c r="B34" s="17">
         <v>137.719093796501</v>
       </c>
-      <c r="C34" s="27">
-        <v>143.41859079471661</v>
-      </c>
-      <c r="D34" s="27">
-        <v>143.66189844596445</v>
+      <c r="C34" s="26">
+        <v>143.39883221579416</v>
+      </c>
+      <c r="D34" s="26">
+        <v>143.62496089305867</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5837,11 +5836,11 @@
       <c r="B35" s="17">
         <v>142.855053333749</v>
       </c>
-      <c r="C35" s="27">
-        <v>143.61959622678881</v>
-      </c>
-      <c r="D35" s="27">
-        <v>143.21426617109415</v>
+      <c r="C35" s="26">
+        <v>143.65423773753113</v>
+      </c>
+      <c r="D35" s="26">
+        <v>143.16979336655785</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5851,11 +5850,11 @@
       <c r="B36" s="17">
         <v>140.582050607355</v>
       </c>
-      <c r="C36" s="27">
-        <v>141.8133854317619</v>
-      </c>
-      <c r="D36" s="27">
-        <v>142.91370844605899</v>
+      <c r="C36" s="26">
+        <v>141.77062067057744</v>
+      </c>
+      <c r="D36" s="26">
+        <v>142.8633900889738</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5865,11 +5864,11 @@
       <c r="B37" s="17">
         <v>136.25019533785601</v>
       </c>
-      <c r="C37" s="27">
-        <v>142.11833565340044</v>
-      </c>
-      <c r="D37" s="27">
-        <v>142.7489042206137</v>
+      <c r="C37" s="26">
+        <v>142.13316371733174</v>
+      </c>
+      <c r="D37" s="26">
+        <v>142.69455357867798</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5879,11 +5878,11 @@
       <c r="B38" s="17">
         <v>134.51979187849801</v>
       </c>
-      <c r="C38" s="27">
-        <v>143.06898927995292</v>
-      </c>
-      <c r="D38" s="27">
-        <v>142.69925286058731</v>
+      <c r="C38" s="26">
+        <v>142.89617454343013</v>
+      </c>
+      <c r="D38" s="26">
+        <v>142.6417260756717</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -5893,11 +5892,11 @@
       <c r="B39" s="17">
         <v>132.28998286562299</v>
       </c>
-      <c r="C39" s="27">
-        <v>143.65147016037997</v>
-      </c>
-      <c r="D39" s="27">
-        <v>142.73239204526294</v>
+      <c r="C39" s="26">
+        <v>143.39932462059696</v>
+      </c>
+      <c r="D39" s="26">
+        <v>142.67191871352708</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5907,11 +5906,11 @@
       <c r="B40" s="17">
         <v>144.85982284623501</v>
       </c>
-      <c r="C40" s="27">
-        <v>141.33817932958303</v>
-      </c>
-      <c r="D40" s="27">
-        <v>142.81224269591752</v>
+      <c r="C40" s="26">
+        <v>141.34266148108074</v>
+      </c>
+      <c r="D40" s="26">
+        <v>142.74802368447902</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -5921,11 +5920,11 @@
       <c r="B41" s="17">
         <v>149.928058780725</v>
       </c>
-      <c r="C41" s="27">
-        <v>141.80397140849595</v>
-      </c>
-      <c r="D41" s="27">
-        <v>142.90173879164536</v>
+      <c r="C41" s="26">
+        <v>142.10138491426889</v>
+      </c>
+      <c r="D41" s="26">
+        <v>142.83168767210574</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -5935,11 +5934,11 @@
       <c r="B42" s="17">
         <v>164.155326806348</v>
       </c>
-      <c r="C42" s="27">
-        <v>143.41771433711941</v>
-      </c>
-      <c r="D42" s="27">
-        <v>142.96521212441903</v>
+      <c r="C42" s="26">
+        <v>144.13131290542941</v>
+      </c>
+      <c r="D42" s="26">
+        <v>142.88781410547449</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5949,11 +5948,11 @@
       <c r="B43" s="17">
         <v>150.81555730727399</v>
       </c>
-      <c r="C43" s="27">
-        <v>143.45039189644771</v>
-      </c>
-      <c r="D43" s="27">
-        <v>142.97068421008018</v>
+      <c r="C43" s="26">
+        <v>143.21663799390336</v>
+      </c>
+      <c r="D43" s="26">
+        <v>142.88280392193343</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -5963,11 +5962,11 @@
       <c r="B44" s="17">
         <v>146.802300676111</v>
       </c>
-      <c r="C44" s="27">
-        <v>145.68168859498596</v>
-      </c>
-      <c r="D44" s="27">
-        <v>142.89167026743129</v>
+      <c r="C44" s="26">
+        <v>145.39466234529115</v>
+      </c>
+      <c r="D44" s="26">
+        <v>142.78987947809517</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5977,11 +5976,11 @@
       <c r="B45" s="17">
         <v>141.28110289807901</v>
       </c>
-      <c r="C45" s="27">
-        <v>145.19818200395812</v>
-      </c>
-      <c r="D45" s="27">
-        <v>142.70875632060668</v>
+      <c r="C45" s="26">
+        <v>145.16465049100097</v>
+      </c>
+      <c r="D45" s="26">
+        <v>142.58835532493947</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -5991,11 +5990,11 @@
       <c r="B46" s="17">
         <v>134.85414768167001</v>
       </c>
-      <c r="C46" s="27">
-        <v>141.62239909983603</v>
-      </c>
-      <c r="D46" s="27">
-        <v>142.41095279357287</v>
+      <c r="C46" s="26">
+        <v>141.5894120969005</v>
+      </c>
+      <c r="D46" s="26">
+        <v>142.26698128209642</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6005,11 +6004,11 @@
       <c r="B47" s="17">
         <v>141.533472485842</v>
       </c>
-      <c r="C47" s="27">
-        <v>143.40158018396335</v>
-      </c>
-      <c r="D47" s="27">
-        <v>141.99679255219604</v>
+      <c r="C47" s="26">
+        <v>143.46674932041435</v>
+      </c>
+      <c r="D47" s="26">
+        <v>141.82712768235581</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6019,11 +6018,11 @@
       <c r="B48" s="17">
         <v>137.64907942573399</v>
       </c>
-      <c r="C48" s="27">
-        <v>140.93607368482947</v>
-      </c>
-      <c r="D48" s="27">
-        <v>141.47664407405117</v>
+      <c r="C48" s="26">
+        <v>140.91761910965727</v>
+      </c>
+      <c r="D48" s="26">
+        <v>141.28044030879806</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6033,11 +6032,11 @@
       <c r="B49" s="17">
         <v>135.65825305401</v>
       </c>
-      <c r="C49" s="27">
-        <v>140.77625696638907</v>
-      </c>
-      <c r="D49" s="27">
-        <v>140.87023436419642</v>
+      <c r="C49" s="26">
+        <v>140.72630710183159</v>
+      </c>
+      <c r="D49" s="26">
+        <v>140.65064693169228</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6047,11 +6046,11 @@
       <c r="B50" s="17">
         <v>132.421417398312</v>
       </c>
-      <c r="C50" s="27">
-        <v>140.88305556626042</v>
-      </c>
-      <c r="D50" s="27">
-        <v>140.20561055370058</v>
+      <c r="C50" s="26">
+        <v>140.59860571146595</v>
+      </c>
+      <c r="D50" s="26">
+        <v>139.96862495730957</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6061,11 +6060,11 @@
       <c r="B51" s="17">
         <v>129.859833639111</v>
       </c>
-      <c r="C51" s="27">
-        <v>141.03448647141076</v>
-      </c>
-      <c r="D51" s="27">
-        <v>139.5198710240673</v>
+      <c r="C51" s="26">
+        <v>140.76797300199243</v>
+      </c>
+      <c r="D51" s="26">
+        <v>139.27258735476616</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6075,11 +6074,11 @@
       <c r="B52" s="17">
         <v>128.843852053852</v>
       </c>
-      <c r="C52" s="27">
-        <v>125.64371703156486</v>
-      </c>
-      <c r="D52" s="27">
-        <v>138.85530353169298</v>
+      <c r="C52" s="26">
+        <v>125.60376450967458</v>
+      </c>
+      <c r="D52" s="26">
+        <v>138.60561301048406</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6089,11 +6088,11 @@
       <c r="B53" s="17">
         <v>111.733480782765</v>
       </c>
-      <c r="C53" s="27">
-        <v>104.19388044577852</v>
-      </c>
-      <c r="D53" s="27">
-        <v>138.25123505689692</v>
+      <c r="C53" s="26">
+        <v>104.58689612946046</v>
+      </c>
+      <c r="D53" s="26">
+        <v>138.00850199572105</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6103,11 +6102,11 @@
       <c r="B54" s="17">
         <v>131.32838384509699</v>
       </c>
-      <c r="C54" s="27">
-        <v>114.78631725401915</v>
-      </c>
-      <c r="D54" s="27">
-        <v>137.74058878476848</v>
+      <c r="C54" s="26">
+        <v>115.65998679629702</v>
+      </c>
+      <c r="D54" s="26">
+        <v>137.51467103017436</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6117,11 +6116,11 @@
       <c r="B55" s="17">
         <v>133.44056807983</v>
       </c>
-      <c r="C55" s="27">
-        <v>124.12572110482935</v>
-      </c>
-      <c r="D55" s="27">
-        <v>137.34621430227301</v>
+      <c r="C55" s="26">
+        <v>123.74494224963496</v>
+      </c>
+      <c r="D55" s="26">
+        <v>137.14579625550093</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6131,11 +6130,11 @@
       <c r="B56" s="17">
         <v>128.22854454607801</v>
       </c>
-      <c r="C56" s="27">
-        <v>126.97084945680278</v>
-      </c>
-      <c r="D56" s="27">
-        <v>137.07885676393786</v>
+      <c r="C56" s="26">
+        <v>126.71645733577206</v>
+      </c>
+      <c r="D56" s="26">
+        <v>136.91048070937404</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6145,11 +6144,11 @@
       <c r="B57" s="17">
         <v>125.17155715985901</v>
       </c>
-      <c r="C57" s="27">
-        <v>129.44177969780884</v>
-      </c>
-      <c r="D57" s="27">
-        <v>136.93672336724359</v>
+      <c r="C57" s="26">
+        <v>129.52046304421685</v>
+      </c>
+      <c r="D57" s="26">
+        <v>136.8011856134132</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -6159,11 +6158,11 @@
       <c r="B58" s="17">
         <v>126.560913056248</v>
       </c>
-      <c r="C58" s="27">
-        <v>132.01095247418175</v>
-      </c>
-      <c r="D58" s="27">
-        <v>136.90297637439519</v>
+      <c r="C58" s="26">
+        <v>131.8876635155116</v>
+      </c>
+      <c r="D58" s="26">
+        <v>136.79990008117321</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6173,11 +6172,11 @@
       <c r="B59" s="17">
         <v>131.73321685913601</v>
       </c>
-      <c r="C59" s="27">
-        <v>133.77899658983571</v>
-      </c>
-      <c r="D59" s="27">
-        <v>136.94659085129194</v>
+      <c r="C59" s="26">
+        <v>133.8420115380338</v>
+      </c>
+      <c r="D59" s="26">
+        <v>136.88349291065606</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6187,11 +6186,11 @@
       <c r="B60" s="17">
         <v>132.959514395936</v>
       </c>
-      <c r="C60" s="27">
-        <v>135.67401413095806</v>
-      </c>
-      <c r="D60" s="27">
-        <v>137.02824400611877</v>
+      <c r="C60" s="26">
+        <v>135.63515774913478</v>
+      </c>
+      <c r="D60" s="26">
+        <v>137.02404893408604</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6201,11 +6200,11 @@
       <c r="B61" s="17">
         <v>132.42953958490801</v>
       </c>
-      <c r="C61" s="27">
-        <v>136.16705275018504</v>
-      </c>
-      <c r="D61" s="27">
-        <v>137.10899424316074</v>
+      <c r="C61" s="26">
+        <v>136.14690115403474</v>
+      </c>
+      <c r="D61" s="26">
+        <v>137.19480839893086</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,11 +6214,11 @@
       <c r="B62" s="25">
         <v>129.57077798246249</v>
       </c>
-      <c r="C62" s="27">
-        <v>139.14106491064905</v>
-      </c>
-      <c r="D62" s="27">
-        <v>137.15395433101946</v>
+      <c r="C62" s="26">
+        <v>139.152192426281</v>
+      </c>
+      <c r="D62" s="26">
+        <v>137.37162767875344</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6229,11 +6228,11 @@
       <c r="B63" s="25">
         <v>126.78312261972776</v>
       </c>
-      <c r="C63" s="27">
-        <v>138.56126921154217</v>
-      </c>
-      <c r="D63" s="27">
-        <v>137.13497066862283</v>
+      <c r="C63" s="26">
+        <v>138.32545973734804</v>
+      </c>
+      <c r="D63" s="26">
+        <v>137.53380076319291</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6243,11 +6242,11 @@
       <c r="B64" s="25">
         <v>144.48387886298647</v>
       </c>
-      <c r="C64" s="27">
-        <v>138.64332985227912</v>
-      </c>
-      <c r="D64" s="27">
-        <v>137.03979770293472</v>
+      <c r="C64" s="26">
+        <v>138.01126936020287</v>
+      </c>
+      <c r="D64" s="26">
+        <v>137.66961172105025</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6257,25 +6256,39 @@
       <c r="B65" s="25">
         <v>144.79180664689375</v>
       </c>
-      <c r="C65" s="27">
-        <v>138.20927846510949</v>
-      </c>
-      <c r="D65" s="27">
-        <v>136.8677443031043</v>
+      <c r="C65" s="26">
+        <v>137.00807560440174</v>
+      </c>
+      <c r="D65" s="26">
+        <v>137.77104316966501</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>44317</v>
       </c>
-      <c r="B66" s="26">
+      <c r="B66" s="25">
         <v>149.09457542802394</v>
       </c>
-      <c r="C66" s="28">
-        <v>135.37844425905499</v>
-      </c>
-      <c r="D66" s="28">
-        <v>136.62999645251432</v>
+      <c r="C66" s="26">
+        <v>134.29929367844807</v>
+      </c>
+      <c r="D66" s="26">
+        <v>137.83502006088963</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B67" s="27">
+        <v>147.72957117667067</v>
+      </c>
+      <c r="C67" s="27">
+        <v>137.69519878151104</v>
+      </c>
+      <c r="D67" s="27">
+        <v>137.85990445061401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos producto,res. fiscal e ica, sep21"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141209BD-D458-44D5-B277-9590F49588EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F2B594-E5CB-4903-97CD-8A95D77D2A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="138">
   <si>
     <t>Período</t>
   </si>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,10 +698,11 @@
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -2009,14 +2010,14 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2028,7 +2029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
@@ -3065,10 +3066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,7 +3099,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="12">
-        <v>475667.39569409698</v>
+        <v>475642.42472660332</v>
       </c>
       <c r="D2" s="12">
         <v>460369.44223294902</v>
@@ -3112,7 +3113,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="12">
-        <v>470234.83454621502</v>
+        <v>470200.8392093571</v>
       </c>
       <c r="D3" s="12">
         <v>514395.68177236198</v>
@@ -3126,7 +3127,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="12">
-        <v>493591.08211802499</v>
+        <v>493619.48198730504</v>
       </c>
       <c r="D4" s="12">
         <v>481151.97994350799</v>
@@ -3140,7 +3141,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="12">
-        <v>500967.468195769</v>
+        <v>500998.0346564647</v>
       </c>
       <c r="D5" s="12">
         <v>484543.67687656201</v>
@@ -3154,7 +3155,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12">
-        <v>515582.09919616202</v>
+        <v>515549.17415220023</v>
       </c>
       <c r="D6" s="12">
         <v>493602.53057785501</v>
@@ -3168,7 +3169,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="12">
-        <v>526384.85112762696</v>
+        <v>526354.71445859282</v>
       </c>
       <c r="D7" s="12">
         <v>581668.24987960199</v>
@@ -3182,7 +3183,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12">
-        <v>529821.92893340799</v>
+        <v>529839.79042928014</v>
       </c>
       <c r="D8" s="12">
         <v>514697.78950542799</v>
@@ -3196,7 +3197,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="12">
-        <v>540434.89075646002</v>
+        <v>540480.09097358375</v>
       </c>
       <c r="D9" s="12">
         <v>522255.20005077199</v>
@@ -3210,7 +3211,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="12">
-        <v>554654.71176641702</v>
+        <v>554648.53967353096</v>
       </c>
       <c r="D10" s="12">
         <v>532348.21201691695</v>
@@ -3224,7 +3225,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="12">
-        <v>561319.85129211901</v>
+        <v>561234.94252824865</v>
       </c>
       <c r="D11" s="12">
         <v>614076.39260854397</v>
@@ -3238,7 +3239,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="12">
-        <v>576780.44907762494</v>
+        <v>576819.37412435515</v>
       </c>
       <c r="D12" s="12">
         <v>562978.96562687703</v>
@@ -3252,7 +3253,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="12">
-        <v>589442.60474676697</v>
+        <v>589494.76055679133</v>
       </c>
       <c r="D13" s="12">
         <v>572794.04663058801</v>
@@ -3266,7 +3267,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="12">
-        <v>603268.14293114597</v>
+        <v>603280.28298430704</v>
       </c>
       <c r="D14" s="12">
         <v>576846.88569942699</v>
@@ -3280,7 +3281,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="12">
-        <v>616472.20107953495</v>
+        <v>616335.90141357086</v>
       </c>
       <c r="D15" s="12">
         <v>674620.563006485</v>
@@ -3294,7 +3295,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="12">
-        <v>624384.85968006204</v>
+        <v>624449.95860950905</v>
       </c>
       <c r="D16" s="12">
         <v>610425.69401485403</v>
@@ -3308,7 +3309,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="12">
-        <v>643644.80689362099</v>
+        <v>643703.86757697607</v>
       </c>
       <c r="D17" s="12">
         <v>625876.867863597</v>
@@ -3322,7 +3323,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="12">
-        <v>649603.96296348295</v>
+        <v>649632.21729591175</v>
       </c>
       <c r="D18" s="12">
         <v>616720.35706447798</v>
@@ -3336,7 +3337,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="12">
-        <v>653657.97852411703</v>
+        <v>653489.30235832697</v>
       </c>
       <c r="D19" s="12">
         <v>711405.50045523304</v>
@@ -3350,7 +3351,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="12">
-        <v>658250.32227068197</v>
+        <v>658334.73239632417</v>
       </c>
       <c r="D20" s="12">
         <v>647087.95974249404</v>
@@ -3364,7 +3365,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="12">
-        <v>627192.37520656595</v>
+        <v>627248.38691428315</v>
       </c>
       <c r="D21" s="12">
         <v>613490.82170264097</v>
@@ -3378,7 +3379,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>604317.35709949199</v>
+        <v>604341.08831760916</v>
       </c>
       <c r="D22" s="12">
         <v>578553.04424240498</v>
@@ -3392,7 +3393,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="12">
-        <v>591422.74483261502</v>
+        <v>591270.90822089184</v>
       </c>
       <c r="D23" s="12">
         <v>631197.75186006899</v>
@@ -3406,7 +3407,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="12">
-        <v>614068.60526608396</v>
+        <v>614141.40675168403</v>
       </c>
       <c r="D24" s="12">
         <v>610519.85461172694</v>
@@ -3420,7 +3421,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="12">
-        <v>625682.79845330596</v>
+        <v>625738.10236131249</v>
       </c>
       <c r="D25" s="12">
         <v>615220.85493729694</v>
@@ -3434,7 +3435,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="12">
-        <v>644672.78031526005</v>
+        <v>644704.0935263203</v>
       </c>
       <c r="D26" s="12">
         <v>611607.33658973</v>
@@ -3448,7 +3449,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="12">
-        <v>674106.21659606101</v>
+        <v>673929.6973366529</v>
       </c>
       <c r="D27" s="12">
         <v>733730.773968903</v>
@@ -3462,7 +3463,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="12">
-        <v>676987.78036851296</v>
+        <v>677075.94519358559</v>
       </c>
       <c r="D28" s="12">
         <v>668566.50948898599</v>
@@ -3476,7 +3477,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="12">
-        <v>686327.94048736105</v>
+        <v>686384.98171063466</v>
       </c>
       <c r="D29" s="12">
         <v>668190.097719574</v>
@@ -3490,7 +3491,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="12">
-        <v>702767.07909804699</v>
+        <v>702780.77429836371</v>
       </c>
       <c r="D30" s="12">
         <v>662325.58597269503</v>
@@ -3504,7 +3505,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="12">
-        <v>709740.19643337897</v>
+        <v>709613.94817853905</v>
       </c>
       <c r="D31" s="12">
         <v>766332.95457161299</v>
@@ -3518,7 +3519,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="12">
-        <v>714948.85046085506</v>
+        <v>715012.15085344797</v>
       </c>
       <c r="D32" s="12">
         <v>711417.39193010505</v>
@@ -3532,7 +3533,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="12">
-        <v>715670.26289012702</v>
+        <v>715719.51555205544</v>
       </c>
       <c r="D33" s="12">
         <v>703050.45640799298</v>
@@ -3546,7 +3547,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="12">
-        <v>707932.02482495701</v>
+        <v>707932.16239044804</v>
       </c>
       <c r="D34" s="12">
         <v>672685.993630504</v>
@@ -3560,7 +3561,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="12">
-        <v>683745.83418921498</v>
+        <v>683661.59501312114</v>
       </c>
       <c r="D35" s="12">
         <v>730838.27259277599</v>
@@ -3574,7 +3575,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="12">
-        <v>705083.62105756195</v>
+        <v>705126.95508238499</v>
       </c>
       <c r="D36" s="12">
         <v>703461.65253019601</v>
@@ -3588,7 +3589,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="12">
-        <v>717182.47776406398</v>
+        <v>717223.24534984084</v>
       </c>
       <c r="D37" s="12">
         <v>706958.03908231901</v>
@@ -3602,7 +3603,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="12">
-        <v>717028.815273582</v>
+        <v>716977.20399880852</v>
       </c>
       <c r="D38" s="12">
         <v>677085.52917315101</v>
@@ -3616,7 +3617,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="12">
-        <v>720945.60931800597</v>
+        <v>720928.72319853469</v>
       </c>
       <c r="D39" s="12">
         <v>776486.60279942001</v>
@@ -3630,7 +3631,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="12">
-        <v>725432.18405580905</v>
+        <v>725463.71662261395</v>
       </c>
       <c r="D40" s="12">
         <v>721458.94421618199</v>
@@ -3644,7 +3645,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="12">
-        <v>718221.81256386195</v>
+        <v>718258.77739130252</v>
       </c>
       <c r="D41" s="12">
         <v>706597.34502250701</v>
@@ -3658,7 +3659,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="12">
-        <v>707464.19478501205</v>
+        <v>707438.27934149234</v>
       </c>
       <c r="D42" s="12">
         <v>671066.04663506302</v>
@@ -3672,7 +3673,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="12">
-        <v>703279.87768048199</v>
+        <v>703280.52095097885</v>
       </c>
       <c r="D43" s="12">
         <v>760576.86834800395</v>
@@ -3686,7 +3687,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="12">
-        <v>697514.59919327102</v>
+        <v>697512.66703546315</v>
       </c>
       <c r="D44" s="12">
         <v>690879.79825168301</v>
@@ -3700,7 +3701,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="12">
-        <v>700965.51219469495</v>
+        <v>700992.71652552695</v>
       </c>
       <c r="D45" s="12">
         <v>686701.47061871097</v>
@@ -3714,7 +3715,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="12">
-        <v>711327.76213022706</v>
+        <v>711244.85257803032</v>
       </c>
       <c r="D46" s="12">
         <v>672749.81139169901</v>
@@ -3728,7 +3729,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="12">
-        <v>727885.89800268004</v>
+        <v>727974.81740948593</v>
       </c>
       <c r="D47" s="12">
         <v>791235.96554166998</v>
@@ -3742,13 +3743,13 @@
         <v>31</v>
       </c>
       <c r="C48" s="12">
-        <v>727461.40825424099</v>
+        <v>727441.72813885717</v>
       </c>
       <c r="D48" s="12">
         <v>718281.26544978202</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>2015</v>
       </c>
@@ -3756,13 +3757,13 @@
         <v>32</v>
       </c>
       <c r="C49" s="12">
-        <v>719273.51816501305</v>
+        <v>719287.18842578714</v>
       </c>
       <c r="D49" s="12">
         <v>703681.54416900803</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>2016</v>
       </c>
@@ -3770,13 +3771,14 @@
         <v>29</v>
       </c>
       <c r="C50" s="12">
-        <v>712823.12517927005</v>
+        <v>712656.1058424965</v>
       </c>
       <c r="D50" s="12">
         <v>677652.08911570301</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H50" s="60"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>2016</v>
       </c>
@@ -3784,13 +3786,14 @@
         <v>30</v>
       </c>
       <c r="C51" s="12">
-        <v>701156.36520167196</v>
+        <v>701431.61607410666</v>
       </c>
       <c r="D51" s="12">
         <v>760703.28015165601</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H51" s="60"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>2016</v>
       </c>
@@ -3798,13 +3801,14 @@
         <v>31</v>
       </c>
       <c r="C52" s="12">
-        <v>703767.79335300601</v>
+        <v>703614.60301765869</v>
       </c>
       <c r="D52" s="12">
         <v>694382.47577623103</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H52" s="60"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>2016</v>
       </c>
@@ -3812,13 +3816,14 @@
         <v>32</v>
       </c>
       <c r="C53" s="12">
-        <v>708164.11065669905</v>
+        <v>708209.06945638417</v>
       </c>
       <c r="D53" s="12">
         <v>693173.54934705805</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H53" s="60"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>2017</v>
       </c>
@@ -3826,13 +3831,14 @@
         <v>29</v>
       </c>
       <c r="C54" s="12">
-        <v>714713.85781203397</v>
+        <v>714382.42875967419</v>
       </c>
       <c r="D54" s="12">
         <v>681444.76611022197</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H54" s="60"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>2017</v>
       </c>
@@ -3840,13 +3846,14 @@
         <v>30</v>
       </c>
       <c r="C55" s="12">
-        <v>721234.85431849596</v>
+        <v>721803.28483693185</v>
       </c>
       <c r="D55" s="12">
         <v>778401.67644931702</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H55" s="60"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>2017</v>
       </c>
@@ -3854,13 +3861,14 @@
         <v>31</v>
       </c>
       <c r="C56" s="12">
-        <v>730962.35857053404</v>
+        <v>730647.41174930311</v>
       </c>
       <c r="D56" s="12">
         <v>721120.42685279401</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H56" s="60"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>2017</v>
       </c>
@@ -3868,13 +3876,14 @@
         <v>32</v>
       </c>
       <c r="C57" s="12">
-        <v>738648.72035023302</v>
+        <v>738726.66570538515</v>
       </c>
       <c r="D57" s="12">
         <v>724592.92163896305</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H57" s="60"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>2018</v>
       </c>
@@ -3882,13 +3891,14 @@
         <v>29</v>
       </c>
       <c r="C58" s="12">
-        <v>736350.35290000297</v>
+        <v>735865.95958180574</v>
       </c>
       <c r="D58" s="12">
         <v>707324.26805721398</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H58" s="60"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>2018</v>
       </c>
@@ -3896,13 +3906,14 @@
         <v>30</v>
       </c>
       <c r="C59" s="12">
-        <v>700735.44889128604</v>
+        <v>701416.87787687394</v>
       </c>
       <c r="D59" s="12">
         <v>747428.29995457502</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H59" s="60"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>2018</v>
       </c>
@@ -3910,13 +3921,14 @@
         <v>31</v>
       </c>
       <c r="C60" s="12">
-        <v>701051.83436174004</v>
+        <v>700700.91527981544</v>
       </c>
       <c r="D60" s="12">
         <v>696101.58352180803</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H60" s="60"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>2018</v>
       </c>
@@ -3924,13 +3936,14 @@
         <v>32</v>
       </c>
       <c r="C61" s="12">
-        <v>691372.13576502097</v>
+        <v>691526.01917955582</v>
       </c>
       <c r="D61" s="12">
         <v>678655.62038445403</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H61" s="60"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>2019</v>
       </c>
@@ -3938,13 +3951,14 @@
         <v>29</v>
       </c>
       <c r="C62" s="12">
-        <v>692192.50025861606</v>
+        <v>691325.42465344083</v>
       </c>
       <c r="D62" s="12">
         <v>665690.59065187594</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H62" s="60"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>2019</v>
       </c>
@@ -3952,13 +3966,14 @@
         <v>30</v>
       </c>
       <c r="C63" s="12">
-        <v>693184.46198583802</v>
+        <v>694370.61904841068</v>
       </c>
       <c r="D63" s="12">
         <v>751765.13811138296</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H63" s="60"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>2019</v>
       </c>
@@ -3966,13 +3981,14 @@
         <v>31</v>
       </c>
       <c r="C64" s="12">
-        <v>699378.07654254395</v>
+        <v>698890.77807771834</v>
       </c>
       <c r="D64" s="12">
         <v>683911.44245860004</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H64" s="60"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>2019</v>
       </c>
@@ -3980,13 +3996,14 @@
         <v>32</v>
       </c>
       <c r="C65" s="12">
-        <v>687430.726036318</v>
+        <v>687598.9430437478</v>
       </c>
       <c r="D65" s="11">
         <v>670818.59360145801</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H65" s="60"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>2020</v>
       </c>
@@ -3994,13 +4011,14 @@
         <v>29</v>
       </c>
       <c r="C66" s="11">
-        <v>659047.19908087002</v>
+        <v>657901.84368946217</v>
       </c>
       <c r="D66" s="11">
         <v>632469.10245408595</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H66" s="60"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>2020</v>
       </c>
@@ -4008,13 +4026,14 @@
         <v>30</v>
       </c>
       <c r="C67" s="11">
-        <v>554819.64918026095</v>
+        <v>556121.19007352495</v>
       </c>
       <c r="D67" s="11">
         <v>608823.50379551796</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H67" s="60"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>2020</v>
       </c>
@@ -4022,13 +4041,14 @@
         <v>31</v>
       </c>
       <c r="C68" s="11">
-        <v>628100.60532747395</v>
+        <v>627739.31787237676</v>
       </c>
       <c r="D68" s="11">
         <v>614416.20615719398</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H68" s="60"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>2020</v>
       </c>
@@ -4036,13 +4056,14 @@
         <v>32</v>
       </c>
       <c r="C69" s="11">
-        <v>655908.18747603195</v>
+        <v>656108.17757241661</v>
       </c>
       <c r="D69" s="11">
         <v>642161.71494925604</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H69" s="60"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>2021</v>
       </c>
@@ -4050,11 +4071,27 @@
         <v>29</v>
       </c>
       <c r="C70" s="11">
-        <v>673252.02674679295</v>
-      </c>
-      <c r="D70" s="11">
-        <v>648176.44579293299</v>
-      </c>
+        <v>674394.71622935636</v>
+      </c>
+      <c r="D70">
+        <v>650821.34239924757</v>
+      </c>
+      <c r="H70" s="60"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="11">
+        <v>2021</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="11">
+        <v>665002.5579772027</v>
+      </c>
+      <c r="D71">
+        <v>717953.19096117874</v>
+      </c>
+      <c r="H71" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4079,14 +4116,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="58"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4678,14 +4715,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="58"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4834,8 +4871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4862,14 +4899,14 @@
         <v>79</v>
       </c>
       <c r="B2">
-        <v>7314</v>
+        <v>8839</v>
       </c>
       <c r="C2">
-        <v>9141</v>
+        <v>10563</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1827</v>
+        <v>-1724</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4877,14 +4914,14 @@
         <v>80</v>
       </c>
       <c r="B3">
-        <v>2153</v>
+        <v>2454</v>
       </c>
       <c r="C3">
-        <v>366</v>
+        <v>421</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1787</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4892,14 +4929,14 @@
         <v>81</v>
       </c>
       <c r="B4">
-        <v>2397</v>
+        <v>2921</v>
       </c>
       <c r="C4">
-        <v>1096</v>
+        <v>1265</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1301</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4907,14 +4944,14 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>541</v>
+        <v>659</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>528</v>
+        <v>644</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4922,14 +4959,14 @@
         <v>83</v>
       </c>
       <c r="B6">
-        <v>3283</v>
+        <v>3993</v>
       </c>
       <c r="C6">
-        <v>4176</v>
+        <v>5046</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-893</v>
+        <v>-1053</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,14 +4974,14 @@
         <v>84</v>
       </c>
       <c r="B7">
-        <v>5580</v>
+        <v>6610</v>
       </c>
       <c r="C7">
-        <v>5116</v>
+        <v>5788</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>464</v>
+        <v>822</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4952,14 +4989,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>504</v>
+        <v>576</v>
       </c>
       <c r="C8">
-        <v>310</v>
+        <v>354</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>194</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,14 +5004,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>549</v>
+        <v>648</v>
       </c>
       <c r="C9">
-        <v>318</v>
+        <v>363</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4982,14 +5019,14 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>449</v>
+        <v>524</v>
       </c>
       <c r="C10">
-        <v>456</v>
+        <v>514</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4997,14 +5034,14 @@
         <v>88</v>
       </c>
       <c r="B11">
-        <v>4470</v>
+        <v>5123</v>
       </c>
       <c r="C11">
-        <v>2172</v>
+        <v>2553</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2298</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5012,14 +5049,14 @@
         <v>89</v>
       </c>
       <c r="B12">
-        <v>3353</v>
+        <v>4395</v>
       </c>
       <c r="C12">
-        <v>6916</v>
+        <v>8138</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-3563</v>
+        <v>-3743</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5027,14 +5064,14 @@
         <v>90</v>
       </c>
       <c r="B13">
-        <v>731</v>
+        <v>898</v>
       </c>
       <c r="C13">
-        <v>342</v>
+        <v>416</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>389</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5042,14 +5079,14 @@
         <v>91</v>
       </c>
       <c r="B14">
-        <v>368</v>
+        <v>463</v>
       </c>
       <c r="C14">
-        <v>622</v>
+        <v>740</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-254</v>
+        <v>-277</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5057,14 +5094,14 @@
         <v>92</v>
       </c>
       <c r="B15">
-        <v>2122</v>
+        <v>2517</v>
       </c>
       <c r="C15">
-        <v>789</v>
+        <v>880</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1333</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5072,14 +5109,14 @@
         <v>93</v>
       </c>
       <c r="B16">
-        <v>3035</v>
+        <v>3457</v>
       </c>
       <c r="C16">
-        <v>782</v>
+        <v>989</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>2253</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5087,14 +5124,14 @@
         <v>94</v>
       </c>
       <c r="B17">
-        <v>2721</v>
+        <v>3102</v>
       </c>
       <c r="C17">
-        <v>409</v>
+        <v>509</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2312</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5102,14 +5139,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>269</v>
+        <v>306</v>
       </c>
       <c r="C18">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>143</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5117,14 +5154,14 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>466</v>
+        <v>536</v>
       </c>
       <c r="C19">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>318</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5132,14 +5169,14 @@
         <v>97</v>
       </c>
       <c r="B20">
-        <v>2319</v>
+        <v>2699</v>
       </c>
       <c r="C20">
-        <v>1019</v>
+        <v>1198</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>1501</v>
       </c>
     </row>
   </sheetData>
@@ -5153,7 +5190,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5178,10 +5215,10 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>535008.89523829205</v>
+        <v>604046.13319735427</v>
       </c>
       <c r="C2">
-        <v>2.00200823826462</v>
+        <v>17.580319315972215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5189,10 +5226,10 @@
         <v>102</v>
       </c>
       <c r="B3">
-        <v>39562.453670585201</v>
+        <v>89195.223928980049</v>
       </c>
       <c r="C3">
-        <v>2.9608041086455601</v>
+        <v>-3.9179249324300724</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5200,10 +5237,10 @@
         <v>103</v>
       </c>
       <c r="B4">
-        <v>1680.6613212101499</v>
+        <v>2258.9045828297758</v>
       </c>
       <c r="C4">
-        <v>6.5012219879517996</v>
+        <v>28.191552714517655</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5211,10 +5248,10 @@
         <v>104</v>
       </c>
       <c r="B5">
-        <v>19856.808137148601</v>
+        <v>20269.949560862842</v>
       </c>
       <c r="C5">
-        <v>-5.6552491310008399</v>
+        <v>13.946668684529229</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5222,10 +5259,10 @@
         <v>105</v>
       </c>
       <c r="B6">
-        <v>103274.399949311</v>
+        <v>115618.73755326691</v>
       </c>
       <c r="C6">
-        <v>11.365047613371001</v>
+        <v>32.403170628583446</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5233,10 +5270,10 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <v>12298.790901062899</v>
+        <v>12736.597747150905</v>
       </c>
       <c r="C7">
-        <v>-3.2346681986033898</v>
+        <v>10.913053342572132</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5244,10 +5281,10 @@
         <v>107</v>
       </c>
       <c r="B8">
-        <v>21196.476720577099</v>
+        <v>19532.524594231447</v>
       </c>
       <c r="C8">
-        <v>21.328720335983899</v>
+        <v>84.176585776301465</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5255,10 +5292,10 @@
         <v>108</v>
       </c>
       <c r="B9">
-        <v>84351.965876605303</v>
+        <v>89303.5485018787</v>
       </c>
       <c r="C9">
-        <v>9.8483253059785891</v>
+        <v>25.992692468317948</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5266,10 +5303,10 @@
         <v>109</v>
       </c>
       <c r="B10">
-        <v>6693.9213266070201</v>
+        <v>5517.1767351843646</v>
       </c>
       <c r="C10">
-        <v>-35.536848615812403</v>
+        <v>90.340020564698875</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5277,10 +5314,10 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>47043.3053997307</v>
+        <v>52694.386166101496</v>
       </c>
       <c r="C11">
-        <v>-10.5611575769762</v>
+        <v>14.485678244064705</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5288,10 +5325,10 @@
         <v>111</v>
       </c>
       <c r="B12">
-        <v>25204.754178798099</v>
+        <v>24702.765148763236</v>
       </c>
       <c r="C12">
-        <v>3.0733454764642101</v>
+        <v>0.79059187589880509</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5299,10 +5336,10 @@
         <v>112</v>
       </c>
       <c r="B13">
-        <v>73800.199429641201</v>
+        <v>75509.308936562651</v>
       </c>
       <c r="C13">
-        <v>3.4781191366634001</v>
+        <v>16.138468063927359</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5310,10 +5347,10 @@
         <v>113</v>
       </c>
       <c r="B14">
-        <v>32024.790497151698</v>
+        <v>31940.377494155731</v>
       </c>
       <c r="C14">
-        <v>-4.5980145052756303</v>
+        <v>8.5495978626258573</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5321,10 +5358,10 @@
         <v>114</v>
       </c>
       <c r="B15">
-        <v>26287.5440778335</v>
+        <v>26696.736156349034</v>
       </c>
       <c r="C15">
-        <v>-2.6450925455359098</v>
+        <v>6.3610364323609669</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5332,10 +5369,10 @@
         <v>115</v>
       </c>
       <c r="B16">
-        <v>22814.494951760302</v>
+        <v>22164.329459385022</v>
       </c>
       <c r="C16">
-        <v>-0.92836273753611498</v>
+        <v>13.625244325168806</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5343,10 +5380,10 @@
         <v>116</v>
       </c>
       <c r="B17">
-        <v>14889.3553812308</v>
+        <v>12520.75700054313</v>
       </c>
       <c r="C17">
-        <v>-12.110557766536999</v>
+        <v>113.75818667164168</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5354,10 +5391,10 @@
         <v>117</v>
       </c>
       <c r="B18">
-        <v>4028.9734190378799</v>
+        <v>3384.8096311087297</v>
       </c>
       <c r="C18">
-        <v>-9.6444177433244391</v>
+        <v>24.658035265591938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando datos EMAE- Pobreza"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F2B594-E5CB-4903-97CD-8A95D77D2A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C16C991-5E8C-4B2A-B72B-3C686F957456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -646,12 +646,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -665,7 +663,6 @@
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -699,10 +696,12 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -1920,7 +1919,7 @@
       <c r="E52">
         <v>4.5</v>
       </c>
-      <c r="H52" s="29"/>
+      <c r="H52" s="26"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -1938,7 +1937,7 @@
       <c r="E53">
         <v>3.5</v>
       </c>
-      <c r="H53" s="29"/>
+      <c r="H53" s="26"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -1956,7 +1955,7 @@
       <c r="E54">
         <v>3.8</v>
       </c>
-      <c r="H54" s="29"/>
+      <c r="H54" s="26"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -2010,14 +2009,14 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2065,236 +2064,236 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="25">
         <v>2.9</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <v>2.5</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="25">
         <v>3.5</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="21">
         <v>2.5617622027179987</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="25">
         <v>0.3</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="25">
         <v>0.7</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="25">
         <v>1.5</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="25">
         <v>0.6</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="25">
         <v>0.1</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="25">
         <v>3.4</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="21">
         <v>0.63169916317744601</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="25">
         <v>3.2</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="25">
         <v>2.6</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="25">
         <v>3.6</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="25">
         <v>3.1</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="25">
         <v>4</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="21">
         <v>3.1111663463149863</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="25">
         <v>3.1</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="25">
         <v>2</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="25">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="25">
         <v>2.4</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="25">
         <v>2.1</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="25">
         <v>2.6</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="21">
         <v>2.6790892714205983</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="25">
         <v>2.8</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="25">
         <v>0.1</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="25">
         <v>1.5</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="25">
         <v>0.8</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="21">
         <v>1.57865386681737</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="25">
         <v>-3.9</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="25">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="25">
         <v>-1.6</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="25">
         <v>-2.4</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <v>-5.2</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="25">
         <v>2.5</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="21">
         <v>-3.5714196769120132</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="25">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="25">
         <v>3.8</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="25">
         <v>4.7</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="25">
         <v>4.5</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="25">
         <v>3.5</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="25">
         <v>4</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="22">
         <v>4.1399856594682705</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="25">
         <v>5.9</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="25">
         <v>6.6</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="25">
         <v>5.6</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="25">
         <v>7</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="25">
         <v>7.9</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="25">
         <v>6.7</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <v>6.3152166274965227</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="25">
         <v>2</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="25">
         <v>1.4</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="25">
         <v>2.5</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="25">
         <v>2.8</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="25">
         <v>2.6</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="21">
         <v>2.2210285310618749</v>
       </c>
     </row>
@@ -2344,25 +2343,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="28">
         <v>2.5</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="30">
         <v>2.6</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="32">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="36">
         <v>2.7</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="34">
         <v>2.4</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="38">
         <v>1.8</v>
       </c>
-      <c r="H2" s="43">
+      <c r="H2" s="40">
         <v>3.4</v>
       </c>
     </row>
@@ -2370,25 +2369,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="27">
         <v>1.5</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="29">
         <v>1.4</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="31">
         <v>1.3</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="35">
         <v>2</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="33">
         <v>1.5</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="37">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H3" s="42">
+      <c r="H3" s="39">
         <v>3.4</v>
       </c>
     </row>
@@ -2396,25 +2395,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>2</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="29">
         <v>1.8</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="31">
         <v>2.1</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="35">
         <v>4</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="33">
         <v>2.1</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="37">
         <v>1.5</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="39">
         <v>1.6</v>
       </c>
     </row>
@@ -2422,25 +2421,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="27">
         <v>3.4</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="29">
         <v>3.9</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="31">
         <v>2.8</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="35">
         <v>5</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="33">
         <v>3.5</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="37">
         <v>2</v>
       </c>
-      <c r="H5" s="42">
+      <c r="H5" s="39">
         <v>3</v>
       </c>
     </row>
@@ -2448,25 +2447,25 @@
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="29">
         <v>2.9</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="31">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="35">
         <v>2.7</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="33">
         <v>0.7</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="37">
         <v>-2.6</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="39">
         <v>3.8</v>
       </c>
     </row>
@@ -2474,25 +2473,25 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="27">
         <v>3.3</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="31">
         <v>3.5</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="35">
         <v>3.7</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="33">
         <v>3.3</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="37">
         <v>3.7</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="39">
         <v>3.7</v>
       </c>
     </row>
@@ -2500,25 +2499,25 @@
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="27">
         <v>4.2</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="29">
         <v>4.7</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="31">
         <v>3.9</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="35">
         <v>3.4</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="33">
         <v>3.3</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="37">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="39">
         <v>4</v>
       </c>
     </row>
@@ -2526,25 +2525,25 @@
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="27">
         <v>2.4</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="29">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="31">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="35">
         <v>3</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="33">
         <v>1.9</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="37">
         <v>2.7</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="39">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -2552,25 +2551,25 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="27">
         <v>-0.6</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="29">
         <v>-1.2</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="31">
         <v>-0.3</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="35">
         <v>-0.9</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="33">
         <v>0.5</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="37">
         <v>1.4</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="39">
         <v>0.2</v>
       </c>
     </row>
@@ -2578,25 +2577,25 @@
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="27">
         <v>3.7</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="29">
         <v>3.8</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="31">
         <v>3.7</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="35">
         <v>3</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="33">
         <v>4.8</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="37">
         <v>2.7</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="39">
         <v>3.4</v>
       </c>
     </row>
@@ -2604,25 +2603,25 @@
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="27">
         <v>4.2</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="29">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="31">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="35">
         <v>1.2</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="33">
         <v>6.5</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="37">
         <v>1.7</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="39">
         <v>1.7</v>
       </c>
     </row>
@@ -2630,25 +2629,25 @@
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="27">
         <v>2.9</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <v>2</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="31">
         <v>4.2</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="35">
         <v>2</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="33">
         <v>3.4</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="37">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="39">
         <v>3.8</v>
       </c>
     </row>
@@ -2656,25 +2655,25 @@
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="27">
         <v>3.3</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="29">
         <v>3.1</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="31">
         <v>3.6</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="35">
         <v>3.4</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="33">
         <v>3</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="37">
         <v>2.9</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H14" s="39">
         <v>3.7</v>
       </c>
     </row>
@@ -2724,25 +2723,25 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="42">
         <v>51.4</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="44">
         <v>50.1</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="46">
         <v>52.4</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="50">
         <v>53.5</v>
       </c>
-      <c r="F2" s="51">
+      <c r="F2" s="48">
         <v>51.7</v>
       </c>
-      <c r="G2" s="55">
+      <c r="G2" s="52">
         <v>53.8</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="54">
         <v>51.3</v>
       </c>
     </row>
@@ -2750,25 +2749,25 @@
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="41">
         <v>53.4</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="43">
         <v>50.4</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="45">
         <v>55.8</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="49">
         <v>58.1</v>
       </c>
-      <c r="F3" s="50">
+      <c r="F3" s="47">
         <v>55</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="51">
         <v>56.5</v>
       </c>
-      <c r="H3" s="56">
+      <c r="H3" s="53">
         <v>53.4</v>
       </c>
     </row>
@@ -2776,25 +2775,25 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="41">
         <v>52.2</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="43">
         <v>50.7</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="45">
         <v>53.7</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="49">
         <v>56.9</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="47">
         <v>55</v>
       </c>
-      <c r="G4" s="54">
+      <c r="G4" s="51">
         <v>51.6</v>
       </c>
-      <c r="H4" s="56">
+      <c r="H4" s="53">
         <v>49.2</v>
       </c>
     </row>
@@ -2802,25 +2801,25 @@
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="41">
         <v>63.6</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="43">
         <v>66.3</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="45">
         <v>60.5</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="49">
         <v>66.099999999999994</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="47">
         <v>59.5</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="51">
         <v>64</v>
       </c>
-      <c r="H5" s="56">
+      <c r="H5" s="53">
         <v>63.1</v>
       </c>
     </row>
@@ -2828,25 +2827,25 @@
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="41">
         <v>29.1</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="43">
         <v>31.2</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="45">
         <v>25.8</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="49">
         <v>30.6</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F6" s="47">
         <v>29.1</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="51">
         <v>27.5</v>
       </c>
-      <c r="H6" s="56">
+      <c r="H6" s="53">
         <v>32.1</v>
       </c>
     </row>
@@ -2854,25 +2853,25 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="41">
         <v>48.2</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="43">
         <v>48.3</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="45">
         <v>47.8</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="49">
         <v>49.1</v>
       </c>
-      <c r="F7" s="50">
+      <c r="F7" s="47">
         <v>46.5</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="51">
         <v>50.2</v>
       </c>
-      <c r="H7" s="56">
+      <c r="H7" s="53">
         <v>49</v>
       </c>
     </row>
@@ -2880,25 +2879,25 @@
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="41">
         <v>57.1</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="43">
         <v>53.3</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="45">
         <v>60</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="49">
         <v>60.9</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="47">
         <v>61</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G8" s="51">
         <v>62.3</v>
       </c>
-      <c r="H8" s="56">
+      <c r="H8" s="53">
         <v>54.9</v>
       </c>
     </row>
@@ -2906,25 +2905,25 @@
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="41">
         <v>62.3</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="43">
         <v>57.9</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="45">
         <v>65.7</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="49">
         <v>60.7</v>
       </c>
-      <c r="F9" s="50">
+      <c r="F9" s="47">
         <v>62.5</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="51">
         <v>71.099999999999994</v>
       </c>
-      <c r="H9" s="56">
+      <c r="H9" s="53">
         <v>68.900000000000006</v>
       </c>
     </row>
@@ -2932,25 +2931,25 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="41">
         <v>26.4</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="43">
         <v>23.4</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="45">
         <v>27.7</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="49">
         <v>32.299999999999997</v>
       </c>
-      <c r="F10" s="50">
+      <c r="F10" s="47">
         <v>29.8</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="51">
         <v>29.7</v>
       </c>
-      <c r="H10" s="56">
+      <c r="H10" s="53">
         <v>34.1</v>
       </c>
     </row>
@@ -2958,25 +2957,25 @@
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="41">
         <v>49.2</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="43">
         <v>51</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="45">
         <v>50.9</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="49">
         <v>46.6</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="47">
         <v>43.8</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="51">
         <v>43.1</v>
       </c>
-      <c r="H11" s="56">
+      <c r="H11" s="53">
         <v>39.4</v>
       </c>
     </row>
@@ -2984,25 +2983,25 @@
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="41">
         <v>48</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="43">
         <v>53.2</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="45">
         <v>46.6</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="49">
         <v>37</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="47">
         <v>43.9</v>
       </c>
-      <c r="G12" s="54">
+      <c r="G12" s="51">
         <v>34.9</v>
       </c>
-      <c r="H12" s="56">
+      <c r="H12" s="53">
         <v>34.1</v>
       </c>
     </row>
@@ -3010,25 +3009,25 @@
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="41">
         <v>55.9</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="43">
         <v>56.9</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="45">
         <v>54.8</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="49">
         <v>52.7</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="47">
         <v>56.7</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="51">
         <v>62.3</v>
       </c>
-      <c r="H13" s="56">
+      <c r="H13" s="53">
         <v>49.3</v>
       </c>
     </row>
@@ -3036,25 +3035,25 @@
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="41">
         <v>35.5</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="43">
         <v>36.9</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="45">
         <v>35.6</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="49">
         <v>34.9</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="47">
         <v>32.799999999999997</v>
       </c>
-      <c r="G14" s="54">
+      <c r="G14" s="51">
         <v>31</v>
       </c>
-      <c r="H14" s="56">
+      <c r="H14" s="53">
         <v>31.4</v>
       </c>
     </row>
@@ -3776,7 +3775,7 @@
       <c r="D50" s="12">
         <v>677652.08911570301</v>
       </c>
-      <c r="H50" s="60"/>
+      <c r="H50" s="56"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
@@ -3791,7 +3790,7 @@
       <c r="D51" s="12">
         <v>760703.28015165601</v>
       </c>
-      <c r="H51" s="60"/>
+      <c r="H51" s="56"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
@@ -3806,7 +3805,7 @@
       <c r="D52" s="12">
         <v>694382.47577623103</v>
       </c>
-      <c r="H52" s="60"/>
+      <c r="H52" s="56"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
@@ -3821,7 +3820,7 @@
       <c r="D53" s="12">
         <v>693173.54934705805</v>
       </c>
-      <c r="H53" s="60"/>
+      <c r="H53" s="56"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
@@ -3836,7 +3835,7 @@
       <c r="D54" s="12">
         <v>681444.76611022197</v>
       </c>
-      <c r="H54" s="60"/>
+      <c r="H54" s="56"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
@@ -3851,7 +3850,7 @@
       <c r="D55" s="12">
         <v>778401.67644931702</v>
       </c>
-      <c r="H55" s="60"/>
+      <c r="H55" s="56"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
@@ -3866,7 +3865,7 @@
       <c r="D56" s="12">
         <v>721120.42685279401</v>
       </c>
-      <c r="H56" s="60"/>
+      <c r="H56" s="56"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
@@ -3881,7 +3880,7 @@
       <c r="D57" s="12">
         <v>724592.92163896305</v>
       </c>
-      <c r="H57" s="60"/>
+      <c r="H57" s="56"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
@@ -3896,7 +3895,7 @@
       <c r="D58" s="12">
         <v>707324.26805721398</v>
       </c>
-      <c r="H58" s="60"/>
+      <c r="H58" s="56"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
@@ -3911,7 +3910,7 @@
       <c r="D59" s="12">
         <v>747428.29995457502</v>
       </c>
-      <c r="H59" s="60"/>
+      <c r="H59" s="56"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
@@ -3926,7 +3925,7 @@
       <c r="D60" s="12">
         <v>696101.58352180803</v>
       </c>
-      <c r="H60" s="60"/>
+      <c r="H60" s="56"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -3941,7 +3940,7 @@
       <c r="D61" s="12">
         <v>678655.62038445403</v>
       </c>
-      <c r="H61" s="60"/>
+      <c r="H61" s="56"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
@@ -3956,7 +3955,7 @@
       <c r="D62" s="12">
         <v>665690.59065187594</v>
       </c>
-      <c r="H62" s="60"/>
+      <c r="H62" s="56"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
@@ -3971,7 +3970,7 @@
       <c r="D63" s="12">
         <v>751765.13811138296</v>
       </c>
-      <c r="H63" s="60"/>
+      <c r="H63" s="56"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
@@ -3986,7 +3985,7 @@
       <c r="D64" s="12">
         <v>683911.44245860004</v>
       </c>
-      <c r="H64" s="60"/>
+      <c r="H64" s="56"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
@@ -4001,7 +4000,7 @@
       <c r="D65" s="11">
         <v>670818.59360145801</v>
       </c>
-      <c r="H65" s="60"/>
+      <c r="H65" s="56"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
@@ -4016,7 +4015,7 @@
       <c r="D66" s="11">
         <v>632469.10245408595</v>
       </c>
-      <c r="H66" s="60"/>
+      <c r="H66" s="56"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
@@ -4031,7 +4030,7 @@
       <c r="D67" s="11">
         <v>608823.50379551796</v>
       </c>
-      <c r="H67" s="60"/>
+      <c r="H67" s="56"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
@@ -4046,7 +4045,7 @@
       <c r="D68" s="11">
         <v>614416.20615719398</v>
       </c>
-      <c r="H68" s="60"/>
+      <c r="H68" s="56"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
@@ -4061,7 +4060,7 @@
       <c r="D69" s="11">
         <v>642161.71494925604</v>
       </c>
-      <c r="H69" s="60"/>
+      <c r="H69" s="56"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
@@ -4076,7 +4075,7 @@
       <c r="D70">
         <v>650821.34239924757</v>
       </c>
-      <c r="H70" s="60"/>
+      <c r="H70" s="56"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
@@ -4091,7 +4090,7 @@
       <c r="D71">
         <v>717953.19096117874</v>
       </c>
-      <c r="H71" s="60"/>
+      <c r="H71" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4103,8 +4102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,14 +4115,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="59"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4143,101 +4142,101 @@
       <c r="A3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B3">
-        <v>31.6</v>
-      </c>
-      <c r="C3">
-        <v>42</v>
-      </c>
-      <c r="D3">
-        <v>7.8</v>
-      </c>
-      <c r="E3">
-        <v>10.5</v>
+      <c r="B3" s="58">
+        <v>31.2</v>
+      </c>
+      <c r="C3" s="58">
+        <v>40.6</v>
+      </c>
+      <c r="D3" s="58">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E3" s="58">
+        <v>10.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4">
-        <v>12.2</v>
-      </c>
-      <c r="C4">
-        <v>16.5</v>
-      </c>
-      <c r="D4">
-        <v>3.9</v>
-      </c>
-      <c r="E4">
-        <v>5.3</v>
+      <c r="B4" s="58">
+        <v>10.1</v>
+      </c>
+      <c r="C4" s="58">
+        <v>13.9</v>
+      </c>
+      <c r="D4" s="58">
+        <v>1.9</v>
+      </c>
+      <c r="E4" s="58">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5">
-        <v>40.9</v>
-      </c>
-      <c r="C5">
-        <v>51</v>
-      </c>
-      <c r="D5">
-        <v>11.8</v>
-      </c>
-      <c r="E5">
-        <v>15.2</v>
+      <c r="B5" s="58">
+        <v>37.1</v>
+      </c>
+      <c r="C5" s="58">
+        <v>45.3</v>
+      </c>
+      <c r="D5" s="58">
+        <v>11.2</v>
+      </c>
+      <c r="E5" s="58">
+        <v>13.8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6">
-        <v>32.6</v>
-      </c>
-      <c r="C6">
-        <v>44</v>
-      </c>
-      <c r="D6">
-        <v>5.4</v>
-      </c>
-      <c r="E6">
-        <v>5.9</v>
+      <c r="B6" s="58">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C6" s="58">
+        <v>43.7</v>
+      </c>
+      <c r="D6" s="58">
+        <v>5.3</v>
+      </c>
+      <c r="E6" s="58">
+        <v>6.9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7">
-        <v>24.9</v>
-      </c>
-      <c r="C7">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="D7">
-        <v>3.1</v>
-      </c>
-      <c r="E7">
+      <c r="B7" s="58">
+        <v>28.2</v>
+      </c>
+      <c r="C7" s="58">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D7" s="58">
         <v>4.5</v>
+      </c>
+      <c r="E7" s="58">
+        <v>6.3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8">
-        <v>32.4</v>
-      </c>
-      <c r="C8">
-        <v>40.6</v>
-      </c>
-      <c r="D8">
-        <v>3.5</v>
-      </c>
-      <c r="E8">
+      <c r="B8" s="58">
+        <v>36</v>
+      </c>
+      <c r="C8" s="58">
+        <v>44.3</v>
+      </c>
+      <c r="D8" s="58">
+        <v>4.2</v>
+      </c>
+      <c r="E8" s="58">
         <v>4.7</v>
       </c>
     </row>
@@ -4245,447 +4244,459 @@
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B9">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="C9">
-        <v>42.9</v>
-      </c>
-      <c r="D9">
-        <v>6.7</v>
-      </c>
-      <c r="E9">
-        <v>8.6999999999999993</v>
+      <c r="B9" s="58">
+        <v>32.9</v>
+      </c>
+      <c r="C9" s="58">
+        <v>43</v>
+      </c>
+      <c r="D9" s="58">
+        <v>6.9</v>
+      </c>
+      <c r="E9" s="58">
+        <v>9.1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10">
-        <v>25.7</v>
-      </c>
-      <c r="C10">
-        <v>36.4</v>
-      </c>
-      <c r="D10">
-        <v>2.5</v>
-      </c>
-      <c r="E10">
-        <v>3.8</v>
+      <c r="B10" s="58">
+        <v>37.9</v>
+      </c>
+      <c r="C10" s="58">
+        <v>47.4</v>
+      </c>
+      <c r="D10" s="58">
+        <v>11.6</v>
+      </c>
+      <c r="E10" s="58">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="C11" s="14">
-        <v>53.6</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>10.6</v>
+      <c r="B11" s="58">
+        <v>44.6</v>
+      </c>
+      <c r="C11" s="59">
+        <v>51.9</v>
+      </c>
+      <c r="D11" s="58">
+        <v>13.3</v>
+      </c>
+      <c r="E11" s="58">
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12">
-        <v>27.6</v>
-      </c>
-      <c r="C12">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="D12">
-        <v>3.4</v>
-      </c>
-      <c r="E12">
-        <v>5.9</v>
+      <c r="B12" s="58">
+        <v>30</v>
+      </c>
+      <c r="C12" s="58">
+        <v>39.4</v>
+      </c>
+      <c r="D12" s="58">
+        <v>4.7</v>
+      </c>
+      <c r="E12" s="58">
+        <v>6.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="B13">
-        <v>28.7</v>
-      </c>
-      <c r="C13">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="D13">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
+      <c r="B13" s="58">
+        <v>37.1</v>
+      </c>
+      <c r="C13" s="58">
+        <v>46</v>
+      </c>
+      <c r="D13" s="58">
+        <v>8</v>
+      </c>
+      <c r="E13" s="58">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B14">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="C14">
-        <v>43.5</v>
-      </c>
-      <c r="D14">
-        <v>5.7</v>
-      </c>
-      <c r="E14">
-        <v>7.7</v>
+      <c r="B14" s="58">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="C14" s="58">
+        <v>46.2</v>
+      </c>
+      <c r="D14" s="58">
+        <v>9.6</v>
+      </c>
+      <c r="E14" s="58">
+        <v>11.6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15">
-        <v>27.4</v>
-      </c>
-      <c r="C15">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="D15">
-        <v>3.3</v>
-      </c>
-      <c r="E15">
-        <v>4.7</v>
+      <c r="B15" s="58">
+        <v>33.4</v>
+      </c>
+      <c r="C15" s="58">
+        <v>42.5</v>
+      </c>
+      <c r="D15" s="58">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E15" s="58">
+        <v>5.7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="B16">
-        <v>25.3</v>
-      </c>
-      <c r="C16">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="D16">
-        <v>3.2</v>
-      </c>
-      <c r="E16">
-        <v>4.0999999999999996</v>
+      <c r="B16" s="58">
+        <v>26.7</v>
+      </c>
+      <c r="C16" s="58">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D16" s="58">
+        <v>3.1</v>
+      </c>
+      <c r="E16" s="58">
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17">
-        <v>31.2</v>
-      </c>
-      <c r="C17">
-        <v>41.7</v>
-      </c>
-      <c r="D17">
-        <v>7.8</v>
-      </c>
-      <c r="E17">
-        <v>10.3</v>
+      <c r="B17" s="58">
+        <v>33.9</v>
+      </c>
+      <c r="C17" s="58">
+        <v>42.3</v>
+      </c>
+      <c r="D17" s="58">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E17" s="58">
+        <v>11.2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18">
-        <v>31.4</v>
-      </c>
-      <c r="C18">
-        <v>39.4</v>
-      </c>
-      <c r="D18">
-        <v>3.5</v>
-      </c>
-      <c r="E18">
-        <v>4.9000000000000004</v>
+      <c r="B18" s="58">
+        <v>38.6</v>
+      </c>
+      <c r="C18" s="58">
+        <v>50.2</v>
+      </c>
+      <c r="D18" s="58">
+        <v>4.3</v>
+      </c>
+      <c r="E18" s="58">
+        <v>6.1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="B19">
-        <v>18.7</v>
-      </c>
-      <c r="C19">
-        <v>24</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="58">
+        <v>23.1</v>
+      </c>
+      <c r="C19" s="58">
+        <v>31.7</v>
+      </c>
+      <c r="D19" s="58">
         <v>5.2</v>
       </c>
-      <c r="E19">
-        <v>7</v>
+      <c r="E19" s="58">
+        <v>7.7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="B20">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="C20">
-        <v>49.5</v>
-      </c>
-      <c r="D20">
-        <v>6.6</v>
-      </c>
-      <c r="E20">
-        <v>8.1999999999999993</v>
+      <c r="B20" s="58">
+        <v>44.4</v>
+      </c>
+      <c r="C20" s="58">
+        <v>56.1</v>
+      </c>
+      <c r="D20" s="58">
+        <v>11</v>
+      </c>
+      <c r="E20" s="58">
+        <v>15.8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B21">
-        <v>29.5</v>
-      </c>
-      <c r="C21">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="D21">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
+      <c r="B21" s="58">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="C21" s="58">
+        <v>46.6</v>
+      </c>
+      <c r="D21" s="58">
+        <v>7.8</v>
+      </c>
+      <c r="E21" s="58">
+        <v>10.8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="B22">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>31.7</v>
-      </c>
-      <c r="D22">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E22">
-        <v>7</v>
+      <c r="B22" s="58">
+        <v>30.9</v>
+      </c>
+      <c r="C22" s="58">
+        <v>41.5</v>
+      </c>
+      <c r="D22" s="58">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E22" s="58">
+        <v>13.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
-      <c r="B23">
-        <v>29.1</v>
-      </c>
-      <c r="C23">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="D23">
-        <v>5.8</v>
-      </c>
-      <c r="E23">
-        <v>7.4</v>
+      <c r="B23" s="58">
+        <v>28.3</v>
+      </c>
+      <c r="C23" s="58">
+        <v>39.4</v>
+      </c>
+      <c r="D23" s="58">
+        <v>7.9</v>
+      </c>
+      <c r="E23" s="58">
+        <v>10.6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24">
-        <v>30.4</v>
-      </c>
-      <c r="C24">
-        <v>40.9</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>5.7</v>
+      <c r="B24" s="58">
+        <v>27.8</v>
+      </c>
+      <c r="C24" s="58">
+        <v>37</v>
+      </c>
+      <c r="D24" s="58">
+        <v>6.1</v>
+      </c>
+      <c r="E24" s="58">
+        <v>8.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25">
-        <v>28</v>
-      </c>
-      <c r="C25">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25">
-        <v>9.1</v>
+      <c r="B25" s="58">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="C25" s="58">
+        <v>50.5</v>
+      </c>
+      <c r="D25" s="58">
+        <v>7.2</v>
+      </c>
+      <c r="E25" s="58">
+        <v>10.4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B26">
-        <v>30.5</v>
-      </c>
-      <c r="C26">
-        <v>41.1</v>
-      </c>
-      <c r="D26">
-        <v>7.5</v>
-      </c>
-      <c r="E26">
-        <v>10.8</v>
+      <c r="B26" s="58">
+        <v>27.2</v>
+      </c>
+      <c r="C26" s="58">
+        <v>35</v>
+      </c>
+      <c r="D26" s="58">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E26" s="58">
+        <v>13.2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B27">
-        <v>27.2</v>
-      </c>
-      <c r="C27">
-        <v>39.200000000000003</v>
-      </c>
-      <c r="D27">
-        <v>6.4</v>
-      </c>
-      <c r="E27">
-        <v>8.8000000000000007</v>
+      <c r="B27" s="58">
+        <v>29.7</v>
+      </c>
+      <c r="C27" s="58">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="D27" s="58">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E27" s="58">
+        <v>6.2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B28">
-        <v>24.9</v>
-      </c>
-      <c r="C28">
-        <v>33.5</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
+      <c r="B28" s="58">
+        <v>25.8</v>
+      </c>
+      <c r="C28" s="58">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D28" s="58">
+        <v>7.2</v>
+      </c>
+      <c r="E28" s="58">
+        <v>9.6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29">
-        <v>32.4</v>
-      </c>
-      <c r="C29">
-        <v>43.6</v>
-      </c>
-      <c r="D29">
-        <v>6.6</v>
-      </c>
-      <c r="E29">
-        <v>8.1</v>
+      <c r="B29" s="58">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C29" s="58">
+        <v>47.1</v>
+      </c>
+      <c r="D29" s="58">
+        <v>8.5</v>
+      </c>
+      <c r="E29" s="58">
+        <v>11.2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30">
-        <v>24</v>
-      </c>
-      <c r="C30">
-        <v>31.7</v>
-      </c>
-      <c r="D30">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E30">
-        <v>5</v>
+      <c r="B30" s="58">
+        <v>18.7</v>
+      </c>
+      <c r="C30" s="58">
+        <v>23.9</v>
+      </c>
+      <c r="D30" s="58">
+        <v>2.8</v>
+      </c>
+      <c r="E30" s="58">
+        <v>2.9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B31">
-        <v>32.1</v>
-      </c>
-      <c r="C31">
-        <v>40.4</v>
-      </c>
-      <c r="D31">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E31">
-        <v>12.3</v>
+      <c r="B31" s="58">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="C31" s="58">
+        <v>41</v>
+      </c>
+      <c r="D31" s="58">
+        <v>7.5</v>
+      </c>
+      <c r="E31" s="58">
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B32">
-        <v>26</v>
-      </c>
-      <c r="C32">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="D32">
-        <v>6.5</v>
-      </c>
-      <c r="E32">
-        <v>7</v>
+      <c r="B32" s="58">
+        <v>25.9</v>
+      </c>
+      <c r="C32" s="58">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="D32" s="58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E32" s="58">
+        <v>5.4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
+      <c r="B33" s="58">
+        <v>27.4</v>
+      </c>
+      <c r="C33" s="58">
+        <v>36</v>
+      </c>
+      <c r="D33" s="58">
+        <v>3.3</v>
+      </c>
+      <c r="E33" s="58">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B34">
-        <v>25.2</v>
-      </c>
-      <c r="C34">
-        <v>32</v>
-      </c>
-      <c r="D34">
-        <v>5.9</v>
-      </c>
-      <c r="E34">
-        <v>5.7</v>
+      <c r="B34" s="58">
+        <v>26.2</v>
+      </c>
+      <c r="C34" s="58">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="D34" s="58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E34" s="58">
+        <v>5.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B35">
-        <v>25.2</v>
-      </c>
-      <c r="C35">
-        <v>35.1</v>
-      </c>
-      <c r="D35">
-        <v>3.8</v>
-      </c>
-      <c r="E35">
-        <v>4.4000000000000004</v>
+      <c r="B35" s="58">
+        <v>25</v>
+      </c>
+      <c r="C35" s="58">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="D35" s="58">
+        <v>3.6</v>
+      </c>
+      <c r="E35" s="58">
+        <v>4.8</v>
       </c>
     </row>
   </sheetData>
@@ -4703,7 +4714,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,14 +4726,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="59"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4742,119 +4753,119 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3">
-        <v>31.6</v>
-      </c>
-      <c r="C3">
-        <v>42</v>
-      </c>
-      <c r="D3">
-        <v>7.8</v>
-      </c>
-      <c r="E3">
-        <v>10.5</v>
+      <c r="B3" s="58">
+        <v>31.2</v>
+      </c>
+      <c r="C3" s="58">
+        <v>40.6</v>
+      </c>
+      <c r="D3" s="58">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E3" s="58">
+        <v>10.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>30.4</v>
-      </c>
-      <c r="C4">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="D4">
-        <v>4.5</v>
-      </c>
-      <c r="E4">
-        <v>5.3</v>
+      <c r="B4" s="58">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C4" s="58">
+        <v>41.5</v>
+      </c>
+      <c r="D4" s="58">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E4" s="58">
+        <v>6.4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B5">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="C5">
-        <v>44.3</v>
-      </c>
-      <c r="D5">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="E5">
-        <v>13.3</v>
+      <c r="B5" s="58">
+        <v>30.5</v>
+      </c>
+      <c r="C5" s="58">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="D5" s="58">
+        <v>8.9</v>
+      </c>
+      <c r="E5" s="58">
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>32.1</v>
-      </c>
-      <c r="C6">
-        <v>43.5</v>
-      </c>
-      <c r="D6">
-        <v>5.4</v>
-      </c>
-      <c r="E6">
-        <v>7.6</v>
+      <c r="B6" s="58">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C6" s="58">
+        <v>45.4</v>
+      </c>
+      <c r="D6" s="58">
+        <v>8.9</v>
+      </c>
+      <c r="E6" s="58">
+        <v>11.7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>30.9</v>
-      </c>
-      <c r="C7">
-        <v>40.4</v>
-      </c>
-      <c r="D7">
-        <v>5.2</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
+      <c r="B7" s="58">
+        <v>35</v>
+      </c>
+      <c r="C7" s="58">
+        <v>44.7</v>
+      </c>
+      <c r="D7" s="58">
+        <v>7.3</v>
+      </c>
+      <c r="E7" s="58">
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8">
-        <v>28.2</v>
-      </c>
-      <c r="C8">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="D8">
-        <v>5.6</v>
-      </c>
-      <c r="E8">
-        <v>7.7</v>
+      <c r="B8" s="58">
+        <v>31</v>
+      </c>
+      <c r="C8" s="58">
+        <v>42.1</v>
+      </c>
+      <c r="D8" s="58">
+        <v>8</v>
+      </c>
+      <c r="E8" s="58">
+        <v>11.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="B9">
-        <v>27.3</v>
-      </c>
-      <c r="C9">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="D9">
-        <v>6.1</v>
-      </c>
-      <c r="E9">
-        <v>7.8</v>
+      <c r="B9" s="58">
+        <v>26.3</v>
+      </c>
+      <c r="C9" s="58">
+        <v>34.4</v>
+      </c>
+      <c r="D9" s="58">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E9" s="58">
+        <v>5.9</v>
       </c>
     </row>
   </sheetData>
@@ -4871,7 +4882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C20"/>
     </sheetView>
   </sheetViews>
@@ -5405,10 +5416,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5419,16 +5430,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5436,924 +5447,938 @@
       <c r="A2" s="4">
         <v>42370</v>
       </c>
-      <c r="B2" s="17">
-        <v>134.746450413497</v>
-      </c>
-      <c r="C2" s="26">
-        <v>147.9503650346366</v>
-      </c>
-      <c r="D2" s="26">
-        <v>147.11218303143568</v>
+      <c r="B2" s="23">
+        <v>134.74645041349706</v>
+      </c>
+      <c r="C2" s="23">
+        <v>147.88700367414998</v>
+      </c>
+      <c r="D2" s="23">
+        <v>147.1434927696194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>42401</v>
       </c>
-      <c r="B3" s="17">
-        <v>134.23236103862499</v>
-      </c>
-      <c r="C3" s="26">
-        <v>146.83927165376153</v>
-      </c>
-      <c r="D3" s="26">
-        <v>146.52013949247683</v>
+      <c r="B3" s="23">
+        <v>134.23236103862521</v>
+      </c>
+      <c r="C3" s="23">
+        <v>146.82861339932541</v>
+      </c>
+      <c r="D3" s="23">
+        <v>146.56549851142034</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>42430</v>
       </c>
-      <c r="B4" s="17">
-        <v>150.08789423669501</v>
-      </c>
-      <c r="C4" s="26">
-        <v>145.92970847053681</v>
-      </c>
-      <c r="D4" s="26">
-        <v>145.96209323375285</v>
+      <c r="B4" s="23">
+        <v>150.0878942366954</v>
+      </c>
+      <c r="C4" s="23">
+        <v>145.99791631494946</v>
+      </c>
+      <c r="D4" s="23">
+        <v>146.02298231586113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>42461</v>
       </c>
-      <c r="B5" s="17">
-        <v>153.250674366629</v>
-      </c>
-      <c r="C5" s="26">
-        <v>144.99578843421494</v>
-      </c>
-      <c r="D5" s="26">
-        <v>145.47536386029111</v>
+      <c r="B5" s="23">
+        <v>153.25067436662908</v>
+      </c>
+      <c r="C5" s="23">
+        <v>145.01879220018384</v>
+      </c>
+      <c r="D5" s="23">
+        <v>145.55143347311628</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>42491</v>
       </c>
-      <c r="B6" s="17">
-        <v>163.51360808690501</v>
-      </c>
-      <c r="C6" s="26">
-        <v>144.33215794720019</v>
-      </c>
-      <c r="D6" s="26">
-        <v>145.08907396638045</v>
+      <c r="B6" s="23">
+        <v>163.51360808690507</v>
+      </c>
+      <c r="C6" s="23">
+        <v>144.34266968503366</v>
+      </c>
+      <c r="D6" s="23">
+        <v>145.17811227983293</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>42522</v>
       </c>
-      <c r="B7" s="17">
-        <v>153.66209524099801</v>
-      </c>
-      <c r="C7" s="26">
-        <v>144.47004118760216</v>
-      </c>
-      <c r="D7" s="26">
-        <v>144.82436533343756</v>
+      <c r="B7" s="23">
+        <v>153.66209524099784</v>
+      </c>
+      <c r="C7" s="23">
+        <v>144.4107368177192</v>
+      </c>
+      <c r="D7" s="23">
+        <v>144.92231009384119</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>42552</v>
       </c>
-      <c r="B8" s="17">
-        <v>143.73110098180101</v>
-      </c>
-      <c r="C8" s="26">
-        <v>144.4525553765445</v>
-      </c>
-      <c r="D8" s="26">
-        <v>144.69192838137894</v>
+      <c r="B8" s="23">
+        <v>143.73110098180126</v>
+      </c>
+      <c r="C8" s="23">
+        <v>144.42087919967207</v>
+      </c>
+      <c r="D8" s="23">
+        <v>144.79332031977881</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>42583</v>
       </c>
-      <c r="B9" s="17">
-        <v>143.67410264860499</v>
-      </c>
-      <c r="C9" s="26">
-        <v>145.56531993248811</v>
-      </c>
-      <c r="D9" s="26">
-        <v>144.69533205846275</v>
+      <c r="B9" s="23">
+        <v>143.6741026486049</v>
+      </c>
+      <c r="C9" s="23">
+        <v>145.52414969514919</v>
+      </c>
+      <c r="D9" s="23">
+        <v>144.79498361321015</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>42614</v>
       </c>
-      <c r="B10" s="17">
-        <v>142.00773744282</v>
-      </c>
-      <c r="C10" s="26">
-        <v>145.11133981162371</v>
-      </c>
-      <c r="D10" s="26">
-        <v>144.8314423805532</v>
+      <c r="B10" s="23">
+        <v>142.00773744282046</v>
+      </c>
+      <c r="C10" s="23">
+        <v>145.1771503686509</v>
+      </c>
+      <c r="D10" s="23">
+        <v>144.92427393244017</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>42644</v>
       </c>
-      <c r="B11" s="17">
-        <v>141.13686329808101</v>
-      </c>
-      <c r="C11" s="26">
-        <v>145.04109776370345</v>
-      </c>
-      <c r="D11" s="26">
-        <v>145.09045492365055</v>
+      <c r="B11" s="23">
+        <v>141.13686329808141</v>
+      </c>
+      <c r="C11" s="23">
+        <v>145.00616346059641</v>
+      </c>
+      <c r="D11" s="23">
+        <v>145.17270169777828</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>42675</v>
       </c>
-      <c r="B12" s="17">
-        <v>144.93832064073001</v>
-      </c>
-      <c r="C12" s="26">
-        <v>145.84305574159546</v>
-      </c>
-      <c r="D12" s="26">
-        <v>145.456028112436</v>
+      <c r="B12" s="23">
+        <v>144.93832064073018</v>
+      </c>
+      <c r="C12" s="23">
+        <v>145.82642064198311</v>
+      </c>
+      <c r="D12" s="23">
+        <v>145.52643152127982</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>42705</v>
       </c>
-      <c r="B13" s="17">
-        <v>142.590145160319</v>
-      </c>
-      <c r="C13" s="26">
-        <v>147.04065242367525</v>
-      </c>
-      <c r="D13" s="26">
-        <v>145.91408159680924</v>
+      <c r="B13" s="23">
+        <v>142.59014516031914</v>
+      </c>
+      <c r="C13" s="23">
+        <v>147.13085831944269</v>
+      </c>
+      <c r="D13" s="23">
+        <v>145.97395087495525</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42736</v>
       </c>
-      <c r="B14" s="17">
-        <v>136.63265948872001</v>
-      </c>
-      <c r="C14" s="26">
-        <v>147.35877257761507</v>
-      </c>
-      <c r="D14" s="26">
-        <v>146.4480015691835</v>
+      <c r="B14" s="23">
+        <v>136.63265948871924</v>
+      </c>
+      <c r="C14" s="23">
+        <v>147.30407378607961</v>
+      </c>
+      <c r="D14" s="23">
+        <v>146.50059460250873</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>42767</v>
       </c>
-      <c r="B15" s="17">
-        <v>132.158516342166</v>
-      </c>
-      <c r="C15" s="26">
-        <v>146.53352908833722</v>
-      </c>
-      <c r="D15" s="26">
-        <v>147.04021878673237</v>
+      <c r="B15" s="23">
+        <v>132.1585163421652</v>
+      </c>
+      <c r="C15" s="23">
+        <v>146.55527721081395</v>
+      </c>
+      <c r="D15" s="23">
+        <v>147.08984658880237</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>42795</v>
       </c>
-      <c r="B16" s="17">
-        <v>152.62095855115601</v>
-      </c>
-      <c r="C16" s="26">
-        <v>147.92357089538024</v>
-      </c>
-      <c r="D16" s="26">
-        <v>147.67137805280174</v>
+      <c r="B16" s="23">
+        <v>152.62095855115743</v>
+      </c>
+      <c r="C16" s="23">
+        <v>147.92175743419259</v>
+      </c>
+      <c r="D16" s="23">
+        <v>147.72229040292368</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>42826</v>
       </c>
-      <c r="B17" s="17">
-        <v>151.94634477931299</v>
-      </c>
-      <c r="C17" s="26">
-        <v>147.53801877515716</v>
-      </c>
-      <c r="D17" s="26">
-        <v>148.31974657066576</v>
+      <c r="B17" s="23">
+        <v>151.94634477931737</v>
+      </c>
+      <c r="C17" s="23">
+        <v>147.61733894735616</v>
+      </c>
+      <c r="D17" s="23">
+        <v>148.37505004762079</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>42856</v>
       </c>
-      <c r="B18" s="17">
-        <v>168.389209458756</v>
-      </c>
-      <c r="C18" s="26">
-        <v>148.53019646261558</v>
-      </c>
-      <c r="D18" s="26">
-        <v>148.95823457754247</v>
+      <c r="B18" s="23">
+        <v>168.3892094587577</v>
+      </c>
+      <c r="C18" s="23">
+        <v>148.48928637441227</v>
+      </c>
+      <c r="D18" s="23">
+        <v>149.01942006687807</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>42887</v>
       </c>
-      <c r="B19" s="17">
-        <v>161.035685505239</v>
-      </c>
-      <c r="C19" s="26">
-        <v>150.3196109616531</v>
-      </c>
-      <c r="D19" s="26">
-        <v>149.55663503812107</v>
+      <c r="B19" s="23">
+        <v>161.03568550523215</v>
+      </c>
+      <c r="C19" s="23">
+        <v>150.26361337251799</v>
+      </c>
+      <c r="D19" s="23">
+        <v>149.62290733255938</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>42917</v>
       </c>
-      <c r="B20" s="17">
-        <v>150.30605023794101</v>
-      </c>
-      <c r="C20" s="26">
-        <v>150.20765294270382</v>
-      </c>
-      <c r="D20" s="26">
-        <v>150.08159435835401</v>
+      <c r="B20" s="23">
+        <v>150.30605023791972</v>
+      </c>
+      <c r="C20" s="23">
+        <v>150.15658796093678</v>
+      </c>
+      <c r="D20" s="23">
+        <v>150.150023134131</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>42948</v>
       </c>
-      <c r="B21" s="17">
-        <v>149.255342821905</v>
-      </c>
-      <c r="C21" s="26">
-        <v>150.28103752473896</v>
-      </c>
-      <c r="D21" s="26">
-        <v>150.49803396508725</v>
+      <c r="B21" s="23">
+        <v>149.25534282189594</v>
+      </c>
+      <c r="C21" s="23">
+        <v>150.24111524080388</v>
+      </c>
+      <c r="D21" s="23">
+        <v>150.56455668685504</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>42979</v>
       </c>
-      <c r="B22" s="17">
-        <v>146.38655949566899</v>
-      </c>
-      <c r="C22" s="26">
-        <v>151.35568822608755</v>
-      </c>
-      <c r="D22" s="26">
-        <v>150.77128177847973</v>
+      <c r="B22" s="23">
+        <v>146.38655949569906</v>
+      </c>
+      <c r="C22" s="23">
+        <v>151.44183041520486</v>
+      </c>
+      <c r="D22" s="23">
+        <v>150.83267478003378</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43009</v>
       </c>
-      <c r="B23" s="17">
-        <v>149.38594914959</v>
-      </c>
-      <c r="C23" s="26">
-        <v>151.57943226974629</v>
-      </c>
-      <c r="D23" s="26">
-        <v>150.87359247107446</v>
+      <c r="B23" s="23">
+        <v>149.38594914968527</v>
+      </c>
+      <c r="C23" s="23">
+        <v>151.559414852066</v>
+      </c>
+      <c r="D23" s="23">
+        <v>150.92651512956135</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43040</v>
       </c>
-      <c r="B24" s="17">
-        <v>151.926042634336</v>
-      </c>
-      <c r="C24" s="26">
-        <v>152.73084635410285</v>
-      </c>
-      <c r="D24" s="26">
-        <v>150.78307901321071</v>
+      <c r="B24" s="23">
+        <v>151.92604263437596</v>
+      </c>
+      <c r="C24" s="23">
+        <v>152.74368535036876</v>
+      </c>
+      <c r="D24" s="23">
+        <v>150.82575811020519</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43070</v>
       </c>
-      <c r="B25" s="17">
-        <v>146.78338564334001</v>
-      </c>
-      <c r="C25" s="26">
-        <v>152.46834825811229</v>
-      </c>
-      <c r="D25" s="26">
-        <v>150.49004210307629</v>
+      <c r="B25" s="23">
+        <v>146.78338564320444</v>
+      </c>
+      <c r="C25" s="23">
+        <v>152.5327233907484</v>
+      </c>
+      <c r="D25" s="23">
+        <v>150.52299976265229</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43101</v>
       </c>
-      <c r="B26" s="17">
-        <v>142.754737365257</v>
-      </c>
-      <c r="C26" s="26">
-        <v>152.00409144910782</v>
-      </c>
-      <c r="D26" s="26">
-        <v>150.00274424327796</v>
+      <c r="B26" s="23">
+        <v>142.74091494473581</v>
+      </c>
+      <c r="C26" s="23">
+        <v>151.93668596038472</v>
+      </c>
+      <c r="D26" s="23">
+        <v>150.02868140471918</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43132</v>
       </c>
-      <c r="B27" s="17">
-        <v>138.81628446908201</v>
-      </c>
-      <c r="C27" s="26">
-        <v>151.91202563792464</v>
-      </c>
-      <c r="D27" s="26">
-        <v>149.34241845963436</v>
+      <c r="B27" s="23">
+        <v>138.81804133744413</v>
+      </c>
+      <c r="C27" s="23">
+        <v>151.9450243886817</v>
+      </c>
+      <c r="D27" s="23">
+        <v>149.36520082408629</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>43160</v>
       </c>
-      <c r="B28" s="17">
-        <v>155.84525065925999</v>
-      </c>
-      <c r="C28" s="26">
-        <v>151.21030949842233</v>
-      </c>
-      <c r="D28" s="26">
-        <v>148.54341560350122</v>
+      <c r="B28" s="23">
+        <v>155.85731621141912</v>
+      </c>
+      <c r="C28" s="23">
+        <v>151.18502448816403</v>
+      </c>
+      <c r="D28" s="23">
+        <v>148.56828523720617</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43191</v>
       </c>
-      <c r="B29" s="17">
-        <v>151.55142032267901</v>
-      </c>
-      <c r="C29" s="26">
-        <v>146.55811223731223</v>
-      </c>
-      <c r="D29" s="26">
-        <v>147.65249552769166</v>
+      <c r="B29" s="23">
+        <v>151.52453339209498</v>
+      </c>
+      <c r="C29" s="23">
+        <v>146.63295663919186</v>
+      </c>
+      <c r="D29" s="23">
+        <v>147.68358335101948</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43221</v>
       </c>
-      <c r="B30" s="17">
-        <v>159.57159359786201</v>
-      </c>
-      <c r="C30" s="26">
-        <v>144.20010262138075</v>
-      </c>
-      <c r="D30" s="26">
-        <v>146.7235762160648</v>
+      <c r="B30" s="23">
+        <v>159.56668791308005</v>
+      </c>
+      <c r="C30" s="23">
+        <v>144.12993828139321</v>
+      </c>
+      <c r="D30" s="23">
+        <v>146.76238799883495</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43252</v>
       </c>
-      <c r="B31" s="17">
-        <v>151.09398567477399</v>
-      </c>
-      <c r="C31" s="26">
-        <v>143.04047123913992</v>
-      </c>
-      <c r="D31" s="26">
-        <v>145.81114359880948</v>
+      <c r="B31" s="23">
+        <v>151.12577829014</v>
+      </c>
+      <c r="C31" s="23">
+        <v>143.00018953646909</v>
+      </c>
+      <c r="D31" s="23">
+        <v>145.85619939844577</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43282</v>
       </c>
-      <c r="B32" s="17">
-        <v>145.98410181709701</v>
-      </c>
-      <c r="C32" s="26">
-        <v>143.13673693758284</v>
-      </c>
-      <c r="D32" s="26">
-        <v>144.96543625441888</v>
+      <c r="B32" s="23">
+        <v>145.9635724027205</v>
+      </c>
+      <c r="C32" s="23">
+        <v>143.03027159777668</v>
+      </c>
+      <c r="D32" s="23">
+        <v>145.01272941649029</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43313</v>
       </c>
-      <c r="B33" s="17">
-        <v>146.772858569193</v>
-      </c>
-      <c r="C33" s="26">
-        <v>146.77792181071217</v>
-      </c>
-      <c r="D33" s="26">
-        <v>144.22778647059934</v>
+      <c r="B33" s="23">
+        <v>146.76598025632637</v>
+      </c>
+      <c r="C33" s="23">
+        <v>146.71646189186384</v>
+      </c>
+      <c r="D33" s="23">
+        <v>144.27177443687631</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43344</v>
       </c>
-      <c r="B34" s="17">
-        <v>137.719093796501</v>
-      </c>
-      <c r="C34" s="26">
-        <v>143.39883221579416</v>
-      </c>
-      <c r="D34" s="26">
-        <v>143.62496089305867</v>
+      <c r="B34" s="23">
+        <v>137.74650152374514</v>
+      </c>
+      <c r="C34" s="23">
+        <v>143.57359266739132</v>
+      </c>
+      <c r="D34" s="23">
+        <v>143.65924028082685</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43374</v>
       </c>
-      <c r="B35" s="17">
-        <v>142.855053333749</v>
-      </c>
-      <c r="C35" s="26">
-        <v>143.65423773753113</v>
-      </c>
-      <c r="D35" s="26">
-        <v>143.16979336655785</v>
+      <c r="B35" s="23">
+        <v>142.84305870601489</v>
+      </c>
+      <c r="C35" s="23">
+        <v>143.60866684846789</v>
+      </c>
+      <c r="D35" s="23">
+        <v>143.1896596943001</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43405</v>
       </c>
-      <c r="B36" s="17">
-        <v>140.582050607355</v>
-      </c>
-      <c r="C36" s="26">
-        <v>141.77062067057744</v>
-      </c>
-      <c r="D36" s="26">
-        <v>142.8633900889738</v>
+      <c r="B36" s="23">
+        <v>140.59231573478493</v>
+      </c>
+      <c r="C36" s="23">
+        <v>141.82152341740345</v>
+      </c>
+      <c r="D36" s="23">
+        <v>142.86638139604105</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>43435</v>
       </c>
-      <c r="B37" s="17">
-        <v>136.25019533785601</v>
-      </c>
-      <c r="C37" s="26">
-        <v>142.13316371733174</v>
-      </c>
-      <c r="D37" s="26">
-        <v>142.69455357867798</v>
+      <c r="B37" s="23">
+        <v>136.25192483815948</v>
+      </c>
+      <c r="C37" s="23">
+        <v>142.21629005490504</v>
+      </c>
+      <c r="D37" s="23">
+        <v>142.68056619325122</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43466</v>
       </c>
-      <c r="B38" s="17">
-        <v>134.51979187849801</v>
-      </c>
-      <c r="C38" s="26">
-        <v>142.89617454343013</v>
-      </c>
-      <c r="D38" s="26">
-        <v>142.6417260756717</v>
+      <c r="B38" s="23">
+        <v>134.52056073135645</v>
+      </c>
+      <c r="C38" s="23">
+        <v>142.9183739262744</v>
+      </c>
+      <c r="D38" s="23">
+        <v>142.61319923704102</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43497</v>
       </c>
-      <c r="B39" s="17">
-        <v>132.28998286562299</v>
-      </c>
-      <c r="C39" s="26">
-        <v>143.39932462059696</v>
-      </c>
-      <c r="D39" s="26">
-        <v>142.67191871352708</v>
+      <c r="B39" s="23">
+        <v>132.2752983795491</v>
+      </c>
+      <c r="C39" s="23">
+        <v>143.45407183820174</v>
+      </c>
+      <c r="D39" s="23">
+        <v>142.63362577605068</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>43525</v>
       </c>
-      <c r="B40" s="17">
-        <v>144.85982284623501</v>
-      </c>
-      <c r="C40" s="26">
-        <v>141.34266148108074</v>
-      </c>
-      <c r="D40" s="26">
-        <v>142.74802368447902</v>
+      <c r="B40" s="23">
+        <v>144.87373847945011</v>
+      </c>
+      <c r="C40" s="23">
+        <v>141.14998493172271</v>
+      </c>
+      <c r="D40" s="23">
+        <v>142.7067872375346</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43556</v>
       </c>
-      <c r="B41" s="17">
-        <v>149.928058780725</v>
-      </c>
-      <c r="C41" s="26">
-        <v>142.10138491426889</v>
-      </c>
-      <c r="D41" s="26">
-        <v>142.83168767210574</v>
+      <c r="B41" s="23">
+        <v>149.89913666554651</v>
+      </c>
+      <c r="C41" s="23">
+        <v>142.22577535334764</v>
+      </c>
+      <c r="D41" s="23">
+        <v>142.79548408691574</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43586</v>
       </c>
-      <c r="B42" s="17">
-        <v>164.155326806348</v>
-      </c>
-      <c r="C42" s="26">
-        <v>144.13131290542941</v>
-      </c>
-      <c r="D42" s="26">
-        <v>142.88781410547449</v>
+      <c r="B42" s="23">
+        <v>164.14987187524667</v>
+      </c>
+      <c r="C42" s="23">
+        <v>143.96727871307729</v>
+      </c>
+      <c r="D42" s="23">
+        <v>142.86435962927655</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43617</v>
       </c>
-      <c r="B43" s="17">
-        <v>150.81555730727399</v>
-      </c>
-      <c r="C43" s="26">
-        <v>143.21663799390336</v>
-      </c>
-      <c r="D43" s="26">
-        <v>142.88280392193343</v>
+      <c r="B43" s="23">
+        <v>150.84993435355395</v>
+      </c>
+      <c r="C43" s="23">
+        <v>143.21255474423813</v>
+      </c>
+      <c r="D43" s="23">
+        <v>142.87843518276907</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43647</v>
       </c>
-      <c r="B44" s="17">
-        <v>146.802300676111</v>
-      </c>
-      <c r="C44" s="26">
-        <v>145.39466234529115</v>
-      </c>
-      <c r="D44" s="26">
-        <v>142.78987947809517</v>
+      <c r="B44" s="23">
+        <v>146.76823737542938</v>
+      </c>
+      <c r="C44" s="23">
+        <v>145.18591426537057</v>
+      </c>
+      <c r="D44" s="23">
+        <v>142.80747129076016</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43678</v>
       </c>
-      <c r="B45" s="17">
-        <v>141.28110289807901</v>
-      </c>
-      <c r="C45" s="26">
-        <v>145.16465049100097</v>
-      </c>
-      <c r="D45" s="26">
-        <v>142.58835532493947</v>
+      <c r="B45" s="23">
+        <v>141.27943584642691</v>
+      </c>
+      <c r="C45" s="23">
+        <v>145.12946165220967</v>
+      </c>
+      <c r="D45" s="23">
+        <v>142.62804047168277</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43709</v>
       </c>
-      <c r="B46" s="17">
-        <v>134.85414768167001</v>
-      </c>
-      <c r="C46" s="26">
-        <v>141.5894120969005</v>
-      </c>
-      <c r="D46" s="26">
-        <v>142.26698128209642</v>
+      <c r="B46" s="23">
+        <v>134.8898780340036</v>
+      </c>
+      <c r="C46" s="23">
+        <v>141.88554362002733</v>
+      </c>
+      <c r="D46" s="23">
+        <v>142.32657272225879</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43739</v>
       </c>
-      <c r="B47" s="17">
-        <v>141.533472485842</v>
-      </c>
-      <c r="C47" s="26">
-        <v>143.46674932041435</v>
-      </c>
-      <c r="D47" s="26">
-        <v>141.82712768235581</v>
+      <c r="B47" s="23">
+        <v>141.51079081863656</v>
+      </c>
+      <c r="C47" s="23">
+        <v>143.43559427799272</v>
+      </c>
+      <c r="D47" s="23">
+        <v>141.90219009379146</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43770</v>
       </c>
-      <c r="B48" s="17">
-        <v>137.64907942573399</v>
-      </c>
-      <c r="C48" s="26">
-        <v>140.91761910965727</v>
-      </c>
-      <c r="D48" s="26">
-        <v>141.28044030879806</v>
+      <c r="B48" s="23">
+        <v>137.65812501310066</v>
+      </c>
+      <c r="C48" s="23">
+        <v>140.95073131422902</v>
+      </c>
+      <c r="D48" s="23">
+        <v>141.3669723322715</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43800</v>
       </c>
-      <c r="B49" s="17">
-        <v>135.65825305401</v>
-      </c>
-      <c r="C49" s="26">
-        <v>140.72630710183159</v>
-      </c>
-      <c r="D49" s="26">
-        <v>140.65064693169228</v>
+      <c r="B49" s="23">
+        <v>135.67188913384834</v>
+      </c>
+      <c r="C49" s="23">
+        <v>140.83161228640137</v>
+      </c>
+      <c r="D49" s="23">
+        <v>140.74408557644142</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43831</v>
       </c>
-      <c r="B50" s="17">
-        <v>132.421417398312</v>
-      </c>
-      <c r="C50" s="26">
-        <v>140.59860571146595</v>
-      </c>
-      <c r="D50" s="26">
-        <v>139.96862495730957</v>
+      <c r="B50" s="23">
+        <v>132.28222137059714</v>
+      </c>
+      <c r="C50" s="23">
+        <v>140.71315602198064</v>
+      </c>
+      <c r="D50" s="23">
+        <v>140.06505684091601</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>43862</v>
       </c>
-      <c r="B51" s="17">
-        <v>129.859833639111</v>
-      </c>
-      <c r="C51" s="26">
-        <v>140.76797300199243</v>
-      </c>
-      <c r="D51" s="26">
-        <v>139.27258735476616</v>
+      <c r="B51" s="23">
+        <v>129.74514246900199</v>
+      </c>
+      <c r="C51" s="23">
+        <v>140.8026758451025</v>
+      </c>
+      <c r="D51" s="23">
+        <v>139.36819826395134</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43891</v>
       </c>
-      <c r="B52" s="17">
-        <v>128.843852053852</v>
-      </c>
-      <c r="C52" s="26">
-        <v>125.60376450967458</v>
-      </c>
-      <c r="D52" s="26">
-        <v>138.60561301048406</v>
+      <c r="B52" s="23">
+        <v>129.09773925167573</v>
+      </c>
+      <c r="C52" s="23">
+        <v>125.33712817648855</v>
+      </c>
+      <c r="D52" s="23">
+        <v>138.69717756039833</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43922</v>
       </c>
-      <c r="B53" s="17">
-        <v>111.733480782765</v>
-      </c>
-      <c r="C53" s="26">
-        <v>104.58689612946046</v>
-      </c>
-      <c r="D53" s="26">
-        <v>138.00850199572105</v>
+      <c r="B53" s="23">
+        <v>111.90399788955911</v>
+      </c>
+      <c r="C53" s="23">
+        <v>104.57736601996343</v>
+      </c>
+      <c r="D53" s="23">
+        <v>138.09284317066485</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>43952</v>
       </c>
-      <c r="B54" s="17">
-        <v>131.32838384509699</v>
-      </c>
-      <c r="C54" s="26">
-        <v>115.65998679629702</v>
-      </c>
-      <c r="D54" s="26">
-        <v>137.51467103017436</v>
+      <c r="B54" s="23">
+        <v>131.2946318586888</v>
+      </c>
+      <c r="C54" s="23">
+        <v>115.54568944071245</v>
+      </c>
+      <c r="D54" s="23">
+        <v>137.58951969383398</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="18">
+      <c r="A55" s="16">
         <v>43983</v>
       </c>
-      <c r="B55" s="17">
-        <v>133.44056807983</v>
-      </c>
-      <c r="C55" s="26">
-        <v>123.74494224963496</v>
-      </c>
-      <c r="D55" s="26">
-        <v>137.14579625550093</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18">
+      <c r="B55" s="23">
+        <v>133.30380295944371</v>
+      </c>
+      <c r="C55" s="23">
+        <v>123.78774900754838</v>
+      </c>
+      <c r="D55" s="23">
+        <v>137.21139534855942</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
         <v>44013</v>
       </c>
-      <c r="B56" s="17">
-        <v>128.22854454607801</v>
-      </c>
-      <c r="C56" s="26">
-        <v>126.71645733577206</v>
-      </c>
-      <c r="D56" s="26">
-        <v>136.91048070937404</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18">
+      <c r="B56" s="23">
+        <v>128.19060020722847</v>
+      </c>
+      <c r="C56" s="23">
+        <v>126.39445194319801</v>
+      </c>
+      <c r="D56" s="23">
+        <v>136.97124538986577</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
         <v>44044</v>
       </c>
-      <c r="B57" s="17">
-        <v>125.17155715985901</v>
-      </c>
-      <c r="C57" s="26">
-        <v>129.52046304421685</v>
-      </c>
-      <c r="D57" s="26">
-        <v>136.8011856134132</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20">
+      <c r="B57" s="23">
+        <v>125.17398093090794</v>
+      </c>
+      <c r="C57" s="23">
+        <v>129.50665483971034</v>
+      </c>
+      <c r="D57" s="23">
+        <v>136.8674945472375</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
         <v>44075</v>
       </c>
-      <c r="B58" s="17">
-        <v>126.560913056248</v>
-      </c>
-      <c r="C58" s="26">
-        <v>131.8876635155116</v>
-      </c>
-      <c r="D58" s="26">
-        <v>136.79990008117321</v>
+      <c r="B58" s="23">
+        <v>126.59643362404854</v>
+      </c>
+      <c r="C58" s="23">
+        <v>132.29905113101225</v>
+      </c>
+      <c r="D58" s="23">
+        <v>136.88696962346384</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>44105</v>
       </c>
-      <c r="B59" s="17">
-        <v>131.73321685913601</v>
-      </c>
-      <c r="C59" s="26">
-        <v>133.8420115380338</v>
-      </c>
-      <c r="D59" s="26">
-        <v>136.88349291065606</v>
+      <c r="B59" s="23">
+        <v>131.72830919276413</v>
+      </c>
+      <c r="C59" s="23">
+        <v>133.80992361356132</v>
+      </c>
+      <c r="D59" s="23">
+        <v>137.00862743276676</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
+      <c r="A60" s="18">
         <v>44136</v>
       </c>
-      <c r="B60" s="17">
-        <v>132.959514395936</v>
-      </c>
-      <c r="C60" s="26">
-        <v>135.63515774913478</v>
-      </c>
-      <c r="D60" s="26">
-        <v>137.02404893408604</v>
+      <c r="B60" s="23">
+        <v>132.97012438356944</v>
+      </c>
+      <c r="C60" s="23">
+        <v>135.69015032185786</v>
+      </c>
+      <c r="D60" s="23">
+        <v>137.20482283224194</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="20">
+      <c r="A61" s="18">
         <v>44166</v>
       </c>
-      <c r="B61" s="17">
-        <v>132.42953958490801</v>
-      </c>
-      <c r="C61" s="26">
-        <v>136.14690115403474</v>
-      </c>
-      <c r="D61" s="26">
-        <v>137.19480839893086</v>
+      <c r="B61" s="23">
+        <v>132.42067625248373</v>
+      </c>
+      <c r="C61" s="23">
+        <v>136.24366536945175</v>
+      </c>
+      <c r="D61" s="23">
+        <v>137.44694174696019</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>44197</v>
       </c>
-      <c r="B62" s="25">
-        <v>129.57077798246249</v>
-      </c>
-      <c r="C62" s="26">
-        <v>139.152192426281</v>
-      </c>
-      <c r="D62" s="26">
-        <v>137.37162767875344</v>
+      <c r="B62" s="23">
+        <v>129.48861249275998</v>
+      </c>
+      <c r="C62" s="23">
+        <v>139.26820739172535</v>
+      </c>
+      <c r="D62" s="23">
+        <v>137.70869416463844</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>44228</v>
       </c>
-      <c r="B63" s="25">
-        <v>126.78312261972776</v>
-      </c>
-      <c r="C63" s="26">
-        <v>138.32545973734804</v>
-      </c>
-      <c r="D63" s="26">
-        <v>137.53380076319291</v>
+      <c r="B63" s="23">
+        <v>126.69207197318048</v>
+      </c>
+      <c r="C63" s="23">
+        <v>138.35838125671387</v>
+      </c>
+      <c r="D63" s="23">
+        <v>137.96766590471017</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>44256</v>
       </c>
-      <c r="B64" s="25">
-        <v>144.48387886298647</v>
-      </c>
-      <c r="C64" s="26">
-        <v>138.01126936020287</v>
-      </c>
-      <c r="D64" s="26">
-        <v>137.66961172105025</v>
+      <c r="B64" s="23">
+        <v>146.29362400573223</v>
+      </c>
+      <c r="C64" s="23">
+        <v>139.42572571650996</v>
+      </c>
+      <c r="D64" s="23">
+        <v>138.21076406361837</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>44287</v>
       </c>
-      <c r="B65" s="25">
-        <v>144.79180664689375</v>
-      </c>
-      <c r="C65" s="26">
-        <v>137.00807560440174</v>
-      </c>
-      <c r="D65" s="26">
-        <v>137.77104316966501</v>
+      <c r="B65" s="23">
+        <v>144.91616359474941</v>
+      </c>
+      <c r="C65" s="23">
+        <v>137.31459223680645</v>
+      </c>
+      <c r="D65" s="23">
+        <v>138.42905997527637</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>44317</v>
       </c>
-      <c r="B66" s="25">
-        <v>149.09457542802394</v>
-      </c>
-      <c r="C66" s="26">
-        <v>134.29929367844807</v>
-      </c>
-      <c r="D66" s="26">
-        <v>137.83502006088963</v>
+      <c r="B66" s="23">
+        <v>150.20777418280562</v>
+      </c>
+      <c r="C66" s="23">
+        <v>135.29958722574628</v>
+      </c>
+      <c r="D66" s="23">
+        <v>138.61742691269239</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>44348</v>
       </c>
-      <c r="B67" s="27">
-        <v>147.72957117667067</v>
-      </c>
-      <c r="C67" s="27">
-        <v>137.69519878151104</v>
-      </c>
-      <c r="D67" s="27">
-        <v>137.85990445061401</v>
+      <c r="B67" s="23">
+        <v>148.86536500389798</v>
+      </c>
+      <c r="C67" s="23">
+        <v>138.62993201812267</v>
+      </c>
+      <c r="D67" s="23">
+        <v>138.77171734659635</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B68" s="24">
+        <v>143.1915756885594</v>
+      </c>
+      <c r="C68" s="24">
+        <v>139.68439401987982</v>
+      </c>
+      <c r="D68" s="24">
+        <v>138.89266695465867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualización IPC Sept 21"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C16C991-5E8C-4B2A-B72B-3C686F957456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9F158F-9186-48F3-905A-D044956E8D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -697,11 +697,11 @@
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:E57"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,9 +2009,21 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
+      <c r="A58" s="4">
+        <v>44440</v>
+      </c>
+      <c r="B58" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C58">
+        <v>6.4</v>
+      </c>
+      <c r="D58">
+        <v>3.3</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C59" s="55"/>
@@ -2028,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,25 +2080,25 @@
         <v>129</v>
       </c>
       <c r="B2" s="25">
-        <v>2.2999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="C2" s="25">
+        <v>2.6</v>
+      </c>
+      <c r="D2" s="25">
         <v>2.9</v>
       </c>
-      <c r="D2" s="25">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="E2" s="25">
-        <v>2.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="F2" s="25">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="G2" s="25">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="H2" s="21">
-        <v>2.5617622027179987</v>
+        <v>2.9045723039986759</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2094,25 +2106,25 @@
         <v>130</v>
       </c>
       <c r="B3" s="25">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
       <c r="C3" s="25">
-        <v>0.7</v>
+        <v>1.7</v>
       </c>
       <c r="D3" s="25">
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="E3" s="25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F3" s="25">
         <v>0.6</v>
       </c>
-      <c r="F3" s="25">
-        <v>0.1</v>
-      </c>
       <c r="G3" s="25">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="H3" s="21">
-        <v>0.63169916317744601</v>
+        <v>1.5047122562551918</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2120,25 +2132,25 @@
         <v>131</v>
       </c>
       <c r="B4" s="25">
-        <v>3.2</v>
+        <v>4.7</v>
       </c>
       <c r="C4" s="25">
         <v>2.6</v>
       </c>
       <c r="D4" s="25">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="E4" s="25">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="25">
-        <v>4.0999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G4" s="25">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="H4" s="21">
-        <v>3.1111663463149863</v>
+        <v>3.4965580184090461</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2146,25 +2158,25 @@
         <v>132</v>
       </c>
       <c r="B5" s="25">
-        <v>3.1</v>
+        <v>2.6</v>
       </c>
       <c r="C5" s="25">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D5" s="25">
-        <v>4.9000000000000004</v>
+        <v>1</v>
       </c>
       <c r="E5" s="25">
         <v>2.4</v>
       </c>
       <c r="F5" s="25">
-        <v>2.1</v>
+        <v>0.8</v>
       </c>
       <c r="G5" s="25">
-        <v>2.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H5" s="21">
-        <v>2.6790892714205983</v>
+        <v>2.3369313585679397</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2172,25 +2184,25 @@
         <v>133</v>
       </c>
       <c r="B6" s="25">
-        <v>2.8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="25">
-        <v>0.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D6" s="25">
-        <v>2.2999999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="E6" s="25">
-        <v>1.5</v>
+        <v>5.6</v>
       </c>
       <c r="F6" s="25">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G6" s="25">
-        <v>0.8</v>
+        <v>5.8</v>
       </c>
       <c r="H6" s="21">
-        <v>1.57865386681737</v>
+        <v>5.129676551614315</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2198,25 +2210,25 @@
         <v>134</v>
       </c>
       <c r="B7" s="25">
-        <v>-3.9</v>
+        <v>5.8</v>
       </c>
       <c r="C7" s="25">
-        <v>-4.0999999999999996</v>
+        <v>3.7</v>
       </c>
       <c r="D7" s="25">
-        <v>-1.6</v>
+        <v>1.3</v>
       </c>
       <c r="E7" s="25">
-        <v>-2.4</v>
+        <v>4.3</v>
       </c>
       <c r="F7" s="25">
-        <v>-5.2</v>
+        <v>6.2</v>
       </c>
       <c r="G7" s="25">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H7" s="21">
-        <v>-3.5714196769120132</v>
+        <v>4.7631841929441476</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2224,25 +2236,25 @@
         <v>135</v>
       </c>
       <c r="B8" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="C8" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D8" s="25">
+        <v>5.7</v>
+      </c>
+      <c r="E8" s="25">
+        <v>4.2</v>
+      </c>
+      <c r="F8" s="25">
+        <v>3.4</v>
+      </c>
+      <c r="G8" s="25">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C8" s="25">
-        <v>3.8</v>
-      </c>
-      <c r="D8" s="25">
-        <v>4.7</v>
-      </c>
-      <c r="E8" s="25">
-        <v>4.5</v>
-      </c>
-      <c r="F8" s="25">
-        <v>3.5</v>
-      </c>
-      <c r="G8" s="25">
-        <v>4</v>
-      </c>
       <c r="H8" s="22">
-        <v>4.1399856594682705</v>
+        <v>4.637878225348091</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2250,25 +2262,25 @@
         <v>136</v>
       </c>
       <c r="B9" s="25">
-        <v>5.9</v>
+        <v>3.1</v>
       </c>
       <c r="C9" s="25">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="D9" s="25">
+        <v>3.4</v>
+      </c>
+      <c r="E9" s="25">
+        <v>5.2</v>
+      </c>
+      <c r="F9" s="25">
         <v>5.6</v>
       </c>
-      <c r="E9" s="25">
-        <v>7</v>
-      </c>
-      <c r="F9" s="25">
-        <v>7.9</v>
-      </c>
       <c r="G9" s="25">
-        <v>6.7</v>
+        <v>5.5</v>
       </c>
       <c r="H9" s="21">
-        <v>6.3152166274965227</v>
+        <v>4.228333300352638</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,25 +2288,25 @@
         <v>137</v>
       </c>
       <c r="B10" s="25">
-        <v>2.2999999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="C10" s="25">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="D10" s="25">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="E10" s="25">
-        <v>2.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F10" s="25">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="G10" s="25">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="H10" s="21">
-        <v>2.2210285310618749</v>
+        <v>2.875717204661532</v>
       </c>
     </row>
   </sheetData>
@@ -2308,7 +2320,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:H14"/>
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,25 +2356,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="28">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="C2" s="30">
-        <v>2.6</v>
+        <v>3.8</v>
       </c>
       <c r="D2" s="32">
-        <v>2.2999999999999998</v>
+        <v>3.4</v>
       </c>
       <c r="E2" s="36">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="F2" s="34">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="G2" s="38">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="H2" s="40">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2370,25 +2382,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="27">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="C3" s="29">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="D3" s="31">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
       <c r="E3" s="35">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="F3" s="33">
-        <v>1.5</v>
+        <v>2.6</v>
       </c>
       <c r="G3" s="37">
-        <v>1.1000000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="H3" s="39">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2396,25 +2408,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="27">
-        <v>2</v>
+        <v>5.9</v>
       </c>
       <c r="C4" s="29">
-        <v>1.8</v>
+        <v>6.2</v>
       </c>
       <c r="D4" s="31">
-        <v>2.1</v>
+        <v>5.6</v>
       </c>
       <c r="E4" s="35">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="F4" s="33">
-        <v>2.1</v>
+        <v>5.7</v>
       </c>
       <c r="G4" s="37">
-        <v>1.5</v>
+        <v>5.6</v>
       </c>
       <c r="H4" s="39">
-        <v>1.6</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2422,25 +2434,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="27">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="29">
-        <v>3.9</v>
+        <v>6.7</v>
       </c>
       <c r="D5" s="31">
-        <v>2.8</v>
+        <v>5.5</v>
       </c>
       <c r="E5" s="35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="33">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="37">
-        <v>2</v>
+        <v>5.9</v>
       </c>
       <c r="H5" s="39">
-        <v>3</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2448,25 +2460,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="27">
-        <v>1.1000000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="C6" s="29">
-        <v>2.9</v>
+        <v>1.4</v>
       </c>
       <c r="D6" s="31">
-        <v>-1.1000000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="E6" s="35">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="F6" s="33">
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="G6" s="37">
-        <v>-2.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H6" s="39">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2474,25 +2486,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="C7" s="29">
+        <v>3.9</v>
+      </c>
+      <c r="D7" s="31">
+        <v>3.2</v>
+      </c>
+      <c r="E7" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="F7" s="33">
+        <v>3.8</v>
+      </c>
+      <c r="G7" s="37">
+        <v>2.9</v>
+      </c>
+      <c r="H7" s="39">
         <v>3.3</v>
-      </c>
-      <c r="C7" s="29">
-        <v>3</v>
-      </c>
-      <c r="D7" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="E7" s="35">
-        <v>3.7</v>
-      </c>
-      <c r="F7" s="33">
-        <v>3.3</v>
-      </c>
-      <c r="G7" s="37">
-        <v>3.7</v>
-      </c>
-      <c r="H7" s="39">
-        <v>3.7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2500,25 +2512,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="27">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="C8" s="29">
         <v>4.7</v>
       </c>
       <c r="D8" s="31">
-        <v>3.9</v>
+        <v>4.2</v>
       </c>
       <c r="E8" s="35">
         <v>3.4</v>
       </c>
       <c r="F8" s="33">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="G8" s="37">
-        <v>4.0999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="H8" s="39">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2526,25 +2538,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="27">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="29">
-        <v>2.2999999999999998</v>
+        <v>3.7</v>
       </c>
       <c r="D9" s="31">
-        <v>2.2999999999999998</v>
+        <v>2.7</v>
       </c>
       <c r="E9" s="35">
-        <v>3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F9" s="33">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G9" s="37">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="H9" s="39">
-        <v>4.0999999999999996</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2552,25 +2564,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="27">
-        <v>-0.6</v>
+        <v>2.8</v>
       </c>
       <c r="C10" s="29">
-        <v>-1.2</v>
+        <v>3.9</v>
       </c>
       <c r="D10" s="31">
-        <v>-0.3</v>
+        <v>1.7</v>
       </c>
       <c r="E10" s="35">
-        <v>-0.9</v>
+        <v>3.1</v>
       </c>
       <c r="F10" s="33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G10" s="37">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="H10" s="39">
-        <v>0.2</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2578,25 +2590,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="27">
+        <v>3.8</v>
+      </c>
+      <c r="C11" s="29">
+        <v>3.4</v>
+      </c>
+      <c r="D11" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E11" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="F11" s="33">
         <v>3.7</v>
       </c>
-      <c r="C11" s="29">
-        <v>3.8</v>
-      </c>
-      <c r="D11" s="31">
-        <v>3.7</v>
-      </c>
-      <c r="E11" s="35">
-        <v>3</v>
-      </c>
-      <c r="F11" s="33">
-        <v>4.8</v>
-      </c>
       <c r="G11" s="37">
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H11" s="39">
-        <v>3.4</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2604,25 +2616,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="27">
-        <v>4.2</v>
+        <v>3.1</v>
       </c>
       <c r="C12" s="29">
-        <v>4.4000000000000004</v>
+        <v>3.7</v>
       </c>
       <c r="D12" s="31">
-        <v>4.5999999999999996</v>
+        <v>2.9</v>
       </c>
       <c r="E12" s="35">
-        <v>1.2</v>
+        <v>2.1</v>
       </c>
       <c r="F12" s="33">
-        <v>6.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G12" s="37">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="H12" s="39">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2630,25 +2642,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="27">
-        <v>2.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C13" s="29">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="D13" s="31">
-        <v>4.2</v>
+        <v>3.9</v>
       </c>
       <c r="E13" s="35">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F13" s="33">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="G13" s="37">
         <v>2.2000000000000002</v>
       </c>
       <c r="H13" s="39">
-        <v>3.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2656,22 +2668,22 @@
         <v>24</v>
       </c>
       <c r="B14" s="27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C14" s="29">
+        <v>1.8</v>
+      </c>
+      <c r="D14" s="31">
+        <v>2</v>
+      </c>
+      <c r="E14" s="35">
         <v>3.3</v>
       </c>
-      <c r="C14" s="29">
+      <c r="F14" s="33">
         <v>3.1</v>
       </c>
-      <c r="D14" s="31">
-        <v>3.6</v>
-      </c>
-      <c r="E14" s="35">
-        <v>3.4</v>
-      </c>
-      <c r="F14" s="33">
-        <v>3</v>
-      </c>
       <c r="G14" s="37">
-        <v>2.9</v>
+        <v>2.1</v>
       </c>
       <c r="H14" s="39">
         <v>3.7</v>
@@ -2688,7 +2700,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2724,25 +2736,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="42">
-        <v>51.4</v>
+        <v>52.5</v>
       </c>
       <c r="C2" s="44">
-        <v>50.1</v>
+        <v>51.7</v>
       </c>
       <c r="D2" s="46">
-        <v>52.4</v>
+        <v>53.2</v>
       </c>
       <c r="E2" s="50">
+        <v>52.7</v>
+      </c>
+      <c r="F2" s="48">
+        <v>53.1</v>
+      </c>
+      <c r="G2" s="52">
+        <v>52.7</v>
+      </c>
+      <c r="H2" s="54">
         <v>53.5</v>
-      </c>
-      <c r="F2" s="48">
-        <v>51.7</v>
-      </c>
-      <c r="G2" s="52">
-        <v>53.8</v>
-      </c>
-      <c r="H2" s="54">
-        <v>51.3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2753,22 +2765,22 @@
         <v>53.4</v>
       </c>
       <c r="C3" s="43">
-        <v>50.4</v>
+        <v>51.1</v>
       </c>
       <c r="D3" s="45">
-        <v>55.8</v>
+        <v>55.3</v>
       </c>
       <c r="E3" s="49">
-        <v>58.1</v>
+        <v>56.2</v>
       </c>
       <c r="F3" s="47">
-        <v>55</v>
+        <v>54.3</v>
       </c>
       <c r="G3" s="51">
-        <v>56.5</v>
+        <v>55.4</v>
       </c>
       <c r="H3" s="53">
-        <v>53.4</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2776,25 +2788,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="41">
-        <v>52.2</v>
+        <v>54.6</v>
       </c>
       <c r="C4" s="43">
-        <v>50.7</v>
+        <v>53.2</v>
       </c>
       <c r="D4" s="45">
-        <v>53.7</v>
+        <v>55.9</v>
       </c>
       <c r="E4" s="49">
-        <v>56.9</v>
+        <v>58.6</v>
       </c>
       <c r="F4" s="47">
-        <v>55</v>
+        <v>57.3</v>
       </c>
       <c r="G4" s="51">
+        <v>53.4</v>
+      </c>
+      <c r="H4" s="53">
         <v>51.6</v>
-      </c>
-      <c r="H4" s="53">
-        <v>49.2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2802,25 +2814,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="41">
+        <v>63.9</v>
+      </c>
+      <c r="C5" s="43">
+        <v>65.2</v>
+      </c>
+      <c r="D5" s="45">
+        <v>62.6</v>
+      </c>
+      <c r="E5" s="49">
         <v>63.6</v>
       </c>
-      <c r="C5" s="43">
-        <v>66.3</v>
-      </c>
-      <c r="D5" s="45">
-        <v>60.5</v>
-      </c>
-      <c r="E5" s="49">
-        <v>66.099999999999994</v>
-      </c>
       <c r="F5" s="47">
-        <v>59.5</v>
+        <v>64.5</v>
       </c>
       <c r="G5" s="51">
-        <v>64</v>
+        <v>58.8</v>
       </c>
       <c r="H5" s="53">
-        <v>63.1</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2828,25 +2840,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="41">
-        <v>29.1</v>
+        <v>29.6</v>
       </c>
       <c r="C6" s="43">
-        <v>31.2</v>
+        <v>31.6</v>
       </c>
       <c r="D6" s="45">
-        <v>25.8</v>
+        <v>26.2</v>
       </c>
       <c r="E6" s="49">
-        <v>30.6</v>
+        <v>32.5</v>
       </c>
       <c r="F6" s="47">
-        <v>29.1</v>
+        <v>30.4</v>
       </c>
       <c r="G6" s="51">
-        <v>27.5</v>
+        <v>26.3</v>
       </c>
       <c r="H6" s="53">
-        <v>32.1</v>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2854,25 +2866,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="41">
-        <v>48.2</v>
+        <v>49.5</v>
       </c>
       <c r="C7" s="43">
-        <v>48.3</v>
+        <v>49.6</v>
       </c>
       <c r="D7" s="45">
-        <v>47.8</v>
+        <v>49.1</v>
       </c>
       <c r="E7" s="49">
-        <v>49.1</v>
+        <v>46.3</v>
       </c>
       <c r="F7" s="47">
-        <v>46.5</v>
+        <v>49.7</v>
       </c>
       <c r="G7" s="51">
-        <v>50.2</v>
+        <v>51.2</v>
       </c>
       <c r="H7" s="53">
-        <v>49</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2880,25 +2892,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="41">
-        <v>57.1</v>
+        <v>58.4</v>
       </c>
       <c r="C8" s="43">
-        <v>53.3</v>
+        <v>56.1</v>
       </c>
       <c r="D8" s="45">
-        <v>60</v>
+        <v>60.4</v>
       </c>
       <c r="E8" s="49">
-        <v>60.9</v>
+        <v>59.1</v>
       </c>
       <c r="F8" s="47">
-        <v>61</v>
+        <v>60.8</v>
       </c>
       <c r="G8" s="51">
-        <v>62.3</v>
+        <v>62.5</v>
       </c>
       <c r="H8" s="53">
-        <v>54.9</v>
+        <v>54.1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2906,25 +2918,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="41">
-        <v>62.3</v>
+        <v>61.4</v>
       </c>
       <c r="C9" s="43">
-        <v>57.9</v>
+        <v>58.4</v>
       </c>
       <c r="D9" s="45">
-        <v>65.7</v>
+        <v>63.6</v>
       </c>
       <c r="E9" s="49">
-        <v>60.7</v>
+        <v>60.2</v>
       </c>
       <c r="F9" s="47">
-        <v>62.5</v>
+        <v>62.2</v>
       </c>
       <c r="G9" s="51">
-        <v>71.099999999999994</v>
+        <v>66.5</v>
       </c>
       <c r="H9" s="53">
-        <v>68.900000000000006</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2932,25 +2944,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="41">
-        <v>26.4</v>
+        <v>29.8</v>
       </c>
       <c r="C10" s="43">
-        <v>23.4</v>
+        <v>29.2</v>
       </c>
       <c r="D10" s="45">
-        <v>27.7</v>
+        <v>28</v>
       </c>
       <c r="E10" s="49">
-        <v>32.299999999999997</v>
+        <v>34.6</v>
       </c>
       <c r="F10" s="47">
-        <v>29.8</v>
+        <v>32.5</v>
       </c>
       <c r="G10" s="51">
-        <v>29.7</v>
+        <v>31.5</v>
       </c>
       <c r="H10" s="53">
-        <v>34.1</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2958,25 +2970,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="41">
-        <v>49.2</v>
+        <v>52</v>
       </c>
       <c r="C11" s="43">
-        <v>51</v>
+        <v>52.3</v>
       </c>
       <c r="D11" s="45">
-        <v>50.9</v>
+        <v>56.1</v>
       </c>
       <c r="E11" s="49">
-        <v>46.6</v>
+        <v>45.8</v>
       </c>
       <c r="F11" s="47">
-        <v>43.8</v>
+        <v>45.2</v>
       </c>
       <c r="G11" s="51">
-        <v>43.1</v>
+        <v>43.6</v>
       </c>
       <c r="H11" s="53">
-        <v>39.4</v>
+        <v>47.6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2984,25 +2996,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="41">
-        <v>48</v>
+        <v>52.1</v>
       </c>
       <c r="C12" s="43">
-        <v>53.2</v>
+        <v>58.4</v>
       </c>
       <c r="D12" s="45">
-        <v>46.6</v>
+        <v>50.2</v>
       </c>
       <c r="E12" s="49">
-        <v>37</v>
+        <v>39.9</v>
       </c>
       <c r="F12" s="47">
-        <v>43.9</v>
+        <v>46.9</v>
       </c>
       <c r="G12" s="51">
-        <v>34.9</v>
+        <v>36.9</v>
       </c>
       <c r="H12" s="53">
-        <v>34.1</v>
+        <v>36.9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3010,25 +3022,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="41">
-        <v>55.9</v>
+        <v>59.5</v>
       </c>
       <c r="C13" s="43">
-        <v>56.9</v>
+        <v>61.9</v>
       </c>
       <c r="D13" s="45">
-        <v>54.8</v>
+        <v>56.8</v>
       </c>
       <c r="E13" s="49">
-        <v>52.7</v>
+        <v>53.1</v>
       </c>
       <c r="F13" s="47">
-        <v>56.7</v>
+        <v>62.1</v>
       </c>
       <c r="G13" s="51">
-        <v>62.3</v>
+        <v>63.4</v>
       </c>
       <c r="H13" s="53">
-        <v>49.3</v>
+        <v>55.3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3036,25 +3048,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="41">
-        <v>35.5</v>
+        <v>35.9</v>
       </c>
       <c r="C14" s="43">
-        <v>36.9</v>
+        <v>35.6</v>
       </c>
       <c r="D14" s="45">
-        <v>35.6</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="E14" s="49">
-        <v>34.9</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="F14" s="47">
-        <v>32.799999999999997</v>
+        <v>35.1</v>
       </c>
       <c r="G14" s="51">
-        <v>31</v>
+        <v>33.6</v>
       </c>
       <c r="H14" s="53">
-        <v>31.4</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4115,14 +4127,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="57"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4142,16 +4154,16 @@
       <c r="A3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>31.2</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>40.6</v>
       </c>
-      <c r="D3" s="58">
+      <c r="D3" s="57">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="57">
         <v>10.7</v>
       </c>
     </row>
@@ -4159,16 +4171,16 @@
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="57">
         <v>10.1</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="57">
         <v>13.9</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="57">
         <v>1.9</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="57">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -4176,16 +4188,16 @@
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>37.1</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="57">
         <v>45.3</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="57">
         <v>11.2</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="57">
         <v>13.8</v>
       </c>
     </row>
@@ -4193,16 +4205,16 @@
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="57">
         <v>33.200000000000003</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="57">
         <v>43.7</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="57">
         <v>5.3</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="57">
         <v>6.9</v>
       </c>
     </row>
@@ -4210,16 +4222,16 @@
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>28.2</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="57">
         <v>36.200000000000003</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="57">
         <v>4.5</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="57">
         <v>6.3</v>
       </c>
     </row>
@@ -4227,16 +4239,16 @@
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="57">
         <v>36</v>
       </c>
-      <c r="C8" s="58">
+      <c r="C8" s="57">
         <v>44.3</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="57">
         <v>4.2</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="57">
         <v>4.7</v>
       </c>
     </row>
@@ -4244,16 +4256,16 @@
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="57">
         <v>32.9</v>
       </c>
-      <c r="C9" s="58">
+      <c r="C9" s="57">
         <v>43</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="57">
         <v>6.9</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="57">
         <v>9.1</v>
       </c>
     </row>
@@ -4261,16 +4273,16 @@
       <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="57">
         <v>37.9</v>
       </c>
-      <c r="C10" s="58">
+      <c r="C10" s="57">
         <v>47.4</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="57">
         <v>11.6</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="57">
         <v>15</v>
       </c>
     </row>
@@ -4278,16 +4290,16 @@
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="57">
         <v>44.6</v>
       </c>
-      <c r="C11" s="59">
+      <c r="C11" s="58">
         <v>51.9</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="57">
         <v>13.3</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="57">
         <v>16.899999999999999</v>
       </c>
     </row>
@@ -4295,16 +4307,16 @@
       <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="57">
         <v>30</v>
       </c>
-      <c r="C12" s="58">
+      <c r="C12" s="57">
         <v>39.4</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="57">
         <v>4.7</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="57">
         <v>6.5</v>
       </c>
     </row>
@@ -4312,16 +4324,16 @@
       <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="58">
+      <c r="B13" s="57">
         <v>37.1</v>
       </c>
-      <c r="C13" s="58">
+      <c r="C13" s="57">
         <v>46</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="57">
         <v>8</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="57">
         <v>10</v>
       </c>
     </row>
@@ -4329,16 +4341,16 @@
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="58">
+      <c r="B14" s="57">
         <v>36.200000000000003</v>
       </c>
-      <c r="C14" s="58">
+      <c r="C14" s="57">
         <v>46.2</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="57">
         <v>9.6</v>
       </c>
-      <c r="E14" s="58">
+      <c r="E14" s="57">
         <v>11.6</v>
       </c>
     </row>
@@ -4346,16 +4358,16 @@
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="58">
+      <c r="B15" s="57">
         <v>33.4</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="57">
         <v>42.5</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="57">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="57">
         <v>5.7</v>
       </c>
     </row>
@@ -4363,16 +4375,16 @@
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="58">
+      <c r="B16" s="57">
         <v>26.7</v>
       </c>
-      <c r="C16" s="58">
+      <c r="C16" s="57">
         <v>37.799999999999997</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="57">
         <v>3.1</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="57">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -4380,16 +4392,16 @@
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="58">
+      <c r="B17" s="57">
         <v>33.9</v>
       </c>
-      <c r="C17" s="58">
+      <c r="C17" s="57">
         <v>42.3</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="57">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="57">
         <v>11.2</v>
       </c>
     </row>
@@ -4397,16 +4409,16 @@
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="58">
+      <c r="B18" s="57">
         <v>38.6</v>
       </c>
-      <c r="C18" s="58">
+      <c r="C18" s="57">
         <v>50.2</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="57">
         <v>4.3</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E18" s="57">
         <v>6.1</v>
       </c>
     </row>
@@ -4414,16 +4426,16 @@
       <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="58">
+      <c r="B19" s="57">
         <v>23.1</v>
       </c>
-      <c r="C19" s="58">
+      <c r="C19" s="57">
         <v>31.7</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="57">
         <v>5.2</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="57">
         <v>7.7</v>
       </c>
     </row>
@@ -4431,16 +4443,16 @@
       <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="58">
+      <c r="B20" s="57">
         <v>44.4</v>
       </c>
-      <c r="C20" s="58">
+      <c r="C20" s="57">
         <v>56.1</v>
       </c>
-      <c r="D20" s="58">
+      <c r="D20" s="57">
         <v>11</v>
       </c>
-      <c r="E20" s="58">
+      <c r="E20" s="57">
         <v>15.8</v>
       </c>
     </row>
@@ -4448,16 +4460,16 @@
       <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="58">
+      <c r="B21" s="57">
         <v>34.299999999999997</v>
       </c>
-      <c r="C21" s="58">
+      <c r="C21" s="57">
         <v>46.6</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D21" s="57">
         <v>7.8</v>
       </c>
-      <c r="E21" s="58">
+      <c r="E21" s="57">
         <v>10.8</v>
       </c>
     </row>
@@ -4465,16 +4477,16 @@
       <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="58">
+      <c r="B22" s="57">
         <v>30.9</v>
       </c>
-      <c r="C22" s="58">
+      <c r="C22" s="57">
         <v>41.5</v>
       </c>
-      <c r="D22" s="58">
+      <c r="D22" s="57">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E22" s="58">
+      <c r="E22" s="57">
         <v>13.5</v>
       </c>
     </row>
@@ -4482,16 +4494,16 @@
       <c r="A23" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="58">
+      <c r="B23" s="57">
         <v>28.3</v>
       </c>
-      <c r="C23" s="58">
+      <c r="C23" s="57">
         <v>39.4</v>
       </c>
-      <c r="D23" s="58">
+      <c r="D23" s="57">
         <v>7.9</v>
       </c>
-      <c r="E23" s="58">
+      <c r="E23" s="57">
         <v>10.6</v>
       </c>
     </row>
@@ -4499,16 +4511,16 @@
       <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="58">
+      <c r="B24" s="57">
         <v>27.8</v>
       </c>
-      <c r="C24" s="58">
+      <c r="C24" s="57">
         <v>37</v>
       </c>
-      <c r="D24" s="58">
+      <c r="D24" s="57">
         <v>6.1</v>
       </c>
-      <c r="E24" s="58">
+      <c r="E24" s="57">
         <v>8.5</v>
       </c>
     </row>
@@ -4516,16 +4528,16 @@
       <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="58">
+      <c r="B25" s="57">
         <v>36.799999999999997</v>
       </c>
-      <c r="C25" s="58">
+      <c r="C25" s="57">
         <v>50.5</v>
       </c>
-      <c r="D25" s="58">
+      <c r="D25" s="57">
         <v>7.2</v>
       </c>
-      <c r="E25" s="58">
+      <c r="E25" s="57">
         <v>10.4</v>
       </c>
     </row>
@@ -4533,16 +4545,16 @@
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="58">
+      <c r="B26" s="57">
         <v>27.2</v>
       </c>
-      <c r="C26" s="58">
+      <c r="C26" s="57">
         <v>35</v>
       </c>
-      <c r="D26" s="58">
+      <c r="D26" s="57">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E26" s="58">
+      <c r="E26" s="57">
         <v>13.2</v>
       </c>
     </row>
@@ -4550,16 +4562,16 @@
       <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="58">
+      <c r="B27" s="57">
         <v>29.7</v>
       </c>
-      <c r="C27" s="58">
+      <c r="C27" s="57">
         <v>38.799999999999997</v>
       </c>
-      <c r="D27" s="58">
+      <c r="D27" s="57">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E27" s="58">
+      <c r="E27" s="57">
         <v>6.2</v>
       </c>
     </row>
@@ -4567,16 +4579,16 @@
       <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="58">
+      <c r="B28" s="57">
         <v>25.8</v>
       </c>
-      <c r="C28" s="58">
+      <c r="C28" s="57">
         <v>36.799999999999997</v>
       </c>
-      <c r="D28" s="58">
+      <c r="D28" s="57">
         <v>7.2</v>
       </c>
-      <c r="E28" s="58">
+      <c r="E28" s="57">
         <v>9.6</v>
       </c>
     </row>
@@ -4584,16 +4596,16 @@
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="58">
+      <c r="B29" s="57">
         <v>35.299999999999997</v>
       </c>
-      <c r="C29" s="58">
+      <c r="C29" s="57">
         <v>47.1</v>
       </c>
-      <c r="D29" s="58">
+      <c r="D29" s="57">
         <v>8.5</v>
       </c>
-      <c r="E29" s="58">
+      <c r="E29" s="57">
         <v>11.2</v>
       </c>
     </row>
@@ -4601,16 +4613,16 @@
       <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="58">
+      <c r="B30" s="57">
         <v>18.7</v>
       </c>
-      <c r="C30" s="58">
+      <c r="C30" s="57">
         <v>23.9</v>
       </c>
-      <c r="D30" s="58">
+      <c r="D30" s="57">
         <v>2.8</v>
       </c>
-      <c r="E30" s="58">
+      <c r="E30" s="57">
         <v>2.9</v>
       </c>
     </row>
@@ -4618,16 +4630,16 @@
       <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="58">
+      <c r="B31" s="57">
         <v>32.299999999999997</v>
       </c>
-      <c r="C31" s="58">
+      <c r="C31" s="57">
         <v>41</v>
       </c>
-      <c r="D31" s="58">
+      <c r="D31" s="57">
         <v>7.5</v>
       </c>
-      <c r="E31" s="58">
+      <c r="E31" s="57">
         <v>9.8000000000000007</v>
       </c>
     </row>
@@ -4635,16 +4647,16 @@
       <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="58">
+      <c r="B32" s="57">
         <v>25.9</v>
       </c>
-      <c r="C32" s="58">
+      <c r="C32" s="57">
         <v>34.700000000000003</v>
       </c>
-      <c r="D32" s="58">
+      <c r="D32" s="57">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E32" s="58">
+      <c r="E32" s="57">
         <v>5.4</v>
       </c>
     </row>
@@ -4652,16 +4664,16 @@
       <c r="A33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="58">
+      <c r="B33" s="57">
         <v>27.4</v>
       </c>
-      <c r="C33" s="58">
+      <c r="C33" s="57">
         <v>36</v>
       </c>
-      <c r="D33" s="58">
+      <c r="D33" s="57">
         <v>3.3</v>
       </c>
-      <c r="E33" s="58">
+      <c r="E33" s="57">
         <v>4.2</v>
       </c>
     </row>
@@ -4669,16 +4681,16 @@
       <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="58">
+      <c r="B34" s="57">
         <v>26.2</v>
       </c>
-      <c r="C34" s="58">
+      <c r="C34" s="57">
         <v>35.299999999999997</v>
       </c>
-      <c r="D34" s="58">
+      <c r="D34" s="57">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E34" s="58">
+      <c r="E34" s="57">
         <v>5.5</v>
       </c>
     </row>
@@ -4686,16 +4698,16 @@
       <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="58">
+      <c r="B35" s="57">
         <v>25</v>
       </c>
-      <c r="C35" s="58">
+      <c r="C35" s="57">
         <v>34.799999999999997</v>
       </c>
-      <c r="D35" s="58">
+      <c r="D35" s="57">
         <v>3.6</v>
       </c>
-      <c r="E35" s="58">
+      <c r="E35" s="57">
         <v>4.8</v>
       </c>
     </row>
@@ -4726,14 +4738,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="57"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4753,16 +4765,16 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>31.2</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>40.6</v>
       </c>
-      <c r="D3" s="58">
+      <c r="D3" s="57">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="57">
         <v>10.7</v>
       </c>
     </row>
@@ -4770,16 +4782,16 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="57">
         <v>32.200000000000003</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="57">
         <v>41.5</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="57">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="57">
         <v>6.4</v>
       </c>
     </row>
@@ -4787,16 +4799,16 @@
       <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>30.5</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="57">
         <v>39.200000000000003</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="57">
         <v>8.9</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="57">
         <v>11.5</v>
       </c>
     </row>
@@ -4804,16 +4816,16 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="57">
         <v>36.299999999999997</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="57">
         <v>45.4</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="57">
         <v>8.9</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="57">
         <v>11.7</v>
       </c>
     </row>
@@ -4821,16 +4833,16 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>35</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="57">
         <v>44.7</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="57">
         <v>7.3</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="57">
         <v>9.1999999999999993</v>
       </c>
     </row>
@@ -4838,16 +4850,16 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="57">
         <v>31</v>
       </c>
-      <c r="C8" s="58">
+      <c r="C8" s="57">
         <v>42.1</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="57">
         <v>8</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="57">
         <v>11.1</v>
       </c>
     </row>
@@ -4855,16 +4867,16 @@
       <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="57">
         <v>26.3</v>
       </c>
-      <c r="C9" s="58">
+      <c r="C9" s="57">
         <v>34.4</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="57">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="57">
         <v>5.9</v>
       </c>
     </row>
@@ -5418,7 +5430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
"Actualizo datos de emae, comex y resultado fiscal-sep21"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9F158F-9186-48F3-905A-D044956E8D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE58638-C76B-46D5-A457-A2B858F40A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="EMAE" sheetId="9" r:id="rId9"/>
     <sheet name="Aperturas" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -702,6 +702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -2040,7 +2041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4894,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4921,45 +4922,45 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="B2">
-        <v>8839</v>
-      </c>
-      <c r="C2">
-        <v>10563</v>
+      <c r="B2" s="60">
+        <v>10425</v>
+      </c>
+      <c r="C2" s="60">
+        <v>11927</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1724</v>
+        <v>-1502</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3">
-        <v>2454</v>
+      <c r="B3" s="60">
+        <v>2869</v>
       </c>
       <c r="C3">
-        <v>421</v>
+        <v>486</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>2033</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
-      <c r="B4">
-        <v>2921</v>
-      </c>
-      <c r="C4">
-        <v>1265</v>
+      <c r="B4" s="60">
+        <v>3322</v>
+      </c>
+      <c r="C4" s="60">
+        <v>1421</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1656</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,44 +4968,44 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>659</v>
+        <v>776</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>644</v>
+        <v>758</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6">
-        <v>3993</v>
-      </c>
-      <c r="C6">
-        <v>5046</v>
+      <c r="B6" s="60">
+        <v>4521</v>
+      </c>
+      <c r="C6" s="60">
+        <v>5752</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-1053</v>
+        <v>-1231</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7">
-        <v>6610</v>
-      </c>
-      <c r="C7">
-        <v>5788</v>
+      <c r="B7" s="60">
+        <v>7562</v>
+      </c>
+      <c r="C7" s="60">
+        <v>6699</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>822</v>
+        <v>863</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5012,14 +5013,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>576</v>
+        <v>629</v>
       </c>
       <c r="C8">
-        <v>354</v>
+        <v>395</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5027,14 +5028,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>648</v>
+        <v>741</v>
       </c>
       <c r="C9">
-        <v>363</v>
+        <v>402</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5042,59 +5043,59 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>524</v>
+        <v>616</v>
       </c>
       <c r="C10">
-        <v>514</v>
+        <v>589</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11">
-        <v>5123</v>
-      </c>
-      <c r="C11">
-        <v>2553</v>
+      <c r="B11" s="60">
+        <v>5776</v>
+      </c>
+      <c r="C11" s="60">
+        <v>2868</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2570</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B12">
-        <v>4395</v>
-      </c>
-      <c r="C12">
-        <v>8138</v>
+      <c r="B12" s="60">
+        <v>5107</v>
+      </c>
+      <c r="C12" s="60">
+        <v>9524</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-3743</v>
+        <v>-4417</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>90</v>
       </c>
-      <c r="B13">
-        <v>898</v>
+      <c r="B13" s="60">
+        <v>1218</v>
       </c>
       <c r="C13">
-        <v>416</v>
+        <v>464</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>482</v>
+        <v>754</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5102,59 +5103,59 @@
         <v>91</v>
       </c>
       <c r="B14">
-        <v>463</v>
+        <v>567</v>
       </c>
       <c r="C14">
-        <v>740</v>
+        <v>859</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-277</v>
+        <v>-292</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15">
-        <v>2517</v>
-      </c>
-      <c r="C15">
-        <v>880</v>
+      <c r="B15" s="60">
+        <v>2913</v>
+      </c>
+      <c r="C15" s="60">
+        <v>1035</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1637</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16">
-        <v>3457</v>
-      </c>
-      <c r="C16">
-        <v>989</v>
+      <c r="B16" s="60">
+        <v>3791</v>
+      </c>
+      <c r="C16" s="60">
+        <v>1114</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>2468</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B17">
-        <v>3102</v>
+      <c r="B17" s="60">
+        <v>3348</v>
       </c>
       <c r="C17">
-        <v>509</v>
+        <v>659</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2593</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5162,14 +5163,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c r="C18">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5177,29 +5178,29 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>536</v>
+        <v>582</v>
       </c>
       <c r="C19">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20">
-        <v>2699</v>
-      </c>
-      <c r="C20">
-        <v>1198</v>
+      <c r="B20" s="60">
+        <v>3174</v>
+      </c>
+      <c r="C20" s="60">
+        <v>1379</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1501</v>
+        <v>1795</v>
       </c>
     </row>
   </sheetData>
@@ -5428,10 +5429,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5463,10 +5464,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="23">
-        <v>147.88700367414998</v>
+        <v>148.08564975129613</v>
       </c>
       <c r="D2" s="23">
-        <v>147.1434927696194</v>
+        <v>147.03387226699309</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5477,10 +5478,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="23">
-        <v>146.82861339932541</v>
+        <v>146.69442984564876</v>
       </c>
       <c r="D3" s="23">
-        <v>146.56549851142034</v>
+        <v>146.44742243656174</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5491,10 +5492,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="23">
-        <v>145.99791631494946</v>
+        <v>145.93345379152709</v>
       </c>
       <c r="D4" s="23">
-        <v>146.02298231586113</v>
+        <v>145.90110763056185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5505,10 +5506,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="23">
-        <v>145.01879220018384</v>
+        <v>145.1412175425717</v>
       </c>
       <c r="D5" s="23">
-        <v>145.55143347311628</v>
+        <v>145.43068891856151</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5519,10 +5520,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="23">
-        <v>144.34266968503366</v>
+        <v>144.34300755730996</v>
       </c>
       <c r="D6" s="23">
-        <v>145.17811227983293</v>
+        <v>145.06188650681096</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5533,10 +5534,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="23">
-        <v>144.4107368177192</v>
+        <v>144.28797360310097</v>
       </c>
       <c r="D7" s="23">
-        <v>144.92231009384119</v>
+        <v>144.81328745028688</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5547,10 +5548,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="23">
-        <v>144.42087919967207</v>
+        <v>144.33935091916433</v>
       </c>
       <c r="D8" s="23">
-        <v>144.79332031977881</v>
+        <v>144.69210529007546</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5561,10 +5562,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="23">
-        <v>145.52414969514919</v>
+        <v>145.61154439316164</v>
       </c>
       <c r="D9" s="23">
-        <v>144.79498361321015</v>
+        <v>144.70068005337293</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5575,10 +5576,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="23">
-        <v>145.1771503686509</v>
+        <v>145.1712839511917</v>
       </c>
       <c r="D10" s="23">
-        <v>144.92427393244017</v>
+        <v>144.83573403445854</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5589,10 +5590,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="23">
-        <v>145.00616346059641</v>
+        <v>145.08094014452863</v>
       </c>
       <c r="D11" s="23">
-        <v>145.17270169777828</v>
+        <v>145.08853591163188</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5603,10 +5604,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="23">
-        <v>145.82642064198311</v>
+        <v>145.79753996707345</v>
       </c>
       <c r="D12" s="23">
-        <v>145.52643152127982</v>
+        <v>145.4447923388897</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5617,10 +5618,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="23">
-        <v>147.13085831944269</v>
+        <v>147.08496231046456</v>
       </c>
       <c r="D13" s="23">
-        <v>145.97395087495525</v>
+        <v>145.89313120267528</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5631,10 +5632,10 @@
         <v>136.63265948871924</v>
       </c>
       <c r="C14" s="23">
-        <v>147.30407378607961</v>
+        <v>147.39150858719742</v>
       </c>
       <c r="D14" s="23">
-        <v>146.50059460250873</v>
+        <v>146.41938683765051</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5645,10 +5646,10 @@
         <v>132.1585163421652</v>
       </c>
       <c r="C15" s="23">
-        <v>146.55527721081395</v>
+        <v>146.51248208221301</v>
       </c>
       <c r="D15" s="23">
-        <v>147.08984658880237</v>
+        <v>147.00801418718893</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5659,10 +5660,10 @@
         <v>152.62095855115743</v>
       </c>
       <c r="C16" s="23">
-        <v>147.92175743419259</v>
+        <v>147.87711776172259</v>
       </c>
       <c r="D16" s="23">
-        <v>147.72229040292368</v>
+        <v>147.64057421016545</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5673,10 +5674,10 @@
         <v>151.94634477931737</v>
       </c>
       <c r="C17" s="23">
-        <v>147.61733894735616</v>
+        <v>147.6200526471016</v>
       </c>
       <c r="D17" s="23">
-        <v>148.37505004762079</v>
+        <v>148.29435735221259</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5687,10 +5688,10 @@
         <v>168.3892094587577</v>
       </c>
       <c r="C18" s="23">
-        <v>148.48928637441227</v>
+        <v>148.56552023541587</v>
       </c>
       <c r="D18" s="23">
-        <v>149.01942006687807</v>
+        <v>148.94059438868203</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5701,10 +5702,10 @@
         <v>161.03568550523215</v>
       </c>
       <c r="C19" s="23">
-        <v>150.26361337251799</v>
+        <v>150.18466581181673</v>
       </c>
       <c r="D19" s="23">
-        <v>149.62290733255938</v>
+        <v>149.5458052491299</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5715,10 +5716,10 @@
         <v>150.30605023791972</v>
       </c>
       <c r="C20" s="23">
-        <v>150.15658796093678</v>
+        <v>150.18978161328192</v>
       </c>
       <c r="D20" s="23">
-        <v>150.150023134131</v>
+        <v>150.07439547417798</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5729,10 +5730,10 @@
         <v>149.25534282189594</v>
       </c>
       <c r="C21" s="23">
-        <v>150.24111524080388</v>
+        <v>150.2826717181747</v>
       </c>
       <c r="D21" s="23">
-        <v>150.56455668685504</v>
+        <v>150.49015578406019</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5743,10 +5744,10 @@
         <v>146.38655949569906</v>
       </c>
       <c r="C22" s="23">
-        <v>151.44183041520486</v>
+        <v>151.36708028553946</v>
       </c>
       <c r="D22" s="23">
-        <v>150.83267478003378</v>
+        <v>150.75935848143519</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5757,10 +5758,10 @@
         <v>149.38594914968527</v>
       </c>
       <c r="C23" s="23">
-        <v>151.559414852066</v>
+        <v>151.57469170698224</v>
       </c>
       <c r="D23" s="23">
-        <v>150.92651512956135</v>
+        <v>150.85468193676391</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5771,10 +5772,10 @@
         <v>151.92604263437596</v>
       </c>
       <c r="C24" s="23">
-        <v>152.74368535036876</v>
+        <v>152.71651174752355</v>
       </c>
       <c r="D24" s="23">
-        <v>150.82575811020519</v>
+        <v>150.75570011432879</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5785,10 +5786,10 @@
         <v>146.78338564320444</v>
       </c>
       <c r="C25" s="23">
-        <v>152.5327233907484</v>
+        <v>152.5446201387291</v>
       </c>
       <c r="D25" s="23">
-        <v>150.52299976265229</v>
+        <v>150.45464990026778</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5799,10 +5800,10 @@
         <v>142.74091494473581</v>
       </c>
       <c r="C26" s="23">
-        <v>151.93668596038472</v>
+        <v>152.04375046468527</v>
       </c>
       <c r="D26" s="23">
-        <v>150.02868140471918</v>
+        <v>149.96161463003151</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5813,10 +5814,10 @@
         <v>138.81804133744413</v>
       </c>
       <c r="C27" s="23">
-        <v>151.9450243886817</v>
+        <v>151.97256082257195</v>
       </c>
       <c r="D27" s="23">
-        <v>149.36520082408629</v>
+        <v>149.29867688702436</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5827,10 +5828,10 @@
         <v>155.85731621141912</v>
       </c>
       <c r="C28" s="23">
-        <v>151.18502448816403</v>
+        <v>151.05042355002405</v>
       </c>
       <c r="D28" s="23">
-        <v>148.56828523720617</v>
+        <v>148.5016840488164</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5841,10 +5842,10 @@
         <v>151.52453339209498</v>
       </c>
       <c r="C29" s="23">
-        <v>146.63295663919186</v>
+        <v>146.56859163367963</v>
       </c>
       <c r="D29" s="23">
-        <v>147.68358335101948</v>
+        <v>147.61657618242</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5855,10 +5856,10 @@
         <v>159.56668791308005</v>
       </c>
       <c r="C30" s="23">
-        <v>144.12993828139321</v>
+        <v>144.23166947605677</v>
       </c>
       <c r="D30" s="23">
-        <v>146.76238799883495</v>
+        <v>146.6948617947395</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5869,10 +5870,10 @@
         <v>151.12577829014</v>
       </c>
       <c r="C31" s="23">
-        <v>143.00018953646909</v>
+        <v>142.96282334736145</v>
       </c>
       <c r="D31" s="23">
-        <v>145.85619939844577</v>
+        <v>145.7883566744795</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5883,10 +5884,10 @@
         <v>145.9635724027205</v>
       </c>
       <c r="C32" s="23">
-        <v>143.03027159777668</v>
+        <v>143.13008060693846</v>
       </c>
       <c r="D32" s="23">
-        <v>145.01272941649029</v>
+        <v>144.94477555583887</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5897,10 +5898,10 @@
         <v>146.76598025632637</v>
       </c>
       <c r="C33" s="23">
-        <v>146.71646189186384</v>
+        <v>146.70640624813697</v>
       </c>
       <c r="D33" s="23">
-        <v>144.27177443687631</v>
+        <v>144.20530460973021</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5911,10 +5912,10 @@
         <v>137.74650152374514</v>
       </c>
       <c r="C34" s="23">
-        <v>143.57359266739132</v>
+        <v>143.48383930199907</v>
       </c>
       <c r="D34" s="23">
-        <v>143.65924028082685</v>
+        <v>143.59635909613405</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5925,10 +5926,10 @@
         <v>142.84305870601489</v>
       </c>
       <c r="C35" s="23">
-        <v>143.60866684846789</v>
+        <v>143.65586311368153</v>
       </c>
       <c r="D35" s="23">
-        <v>143.1896596943001</v>
+        <v>143.13174084303111</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5939,10 +5940,10 @@
         <v>140.59231573478493</v>
       </c>
       <c r="C36" s="23">
-        <v>141.82152341740345</v>
+        <v>141.84250630210019</v>
       </c>
       <c r="D36" s="23">
-        <v>142.86638139604105</v>
+        <v>142.81398711436555</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5953,10 +5954,10 @@
         <v>136.25192483815948</v>
       </c>
       <c r="C37" s="23">
-        <v>142.21629005490504</v>
+        <v>142.14811090503628</v>
       </c>
       <c r="D37" s="23">
-        <v>142.68056619325122</v>
+        <v>142.63379548165739</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5967,10 +5968,10 @@
         <v>134.52056073135645</v>
       </c>
       <c r="C38" s="23">
-        <v>142.9183739262744</v>
+        <v>142.97195995832118</v>
       </c>
       <c r="D38" s="23">
-        <v>142.61319923704102</v>
+        <v>142.57132998428619</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -5981,10 +5982,10 @@
         <v>132.2752983795491</v>
       </c>
       <c r="C39" s="23">
-        <v>143.45407183820174</v>
+        <v>143.64519108620124</v>
       </c>
       <c r="D39" s="23">
-        <v>142.63362577605068</v>
+        <v>142.59516808591269</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5995,10 +5996,10 @@
         <v>144.87373847945011</v>
       </c>
       <c r="C40" s="23">
-        <v>141.14998493172271</v>
+        <v>140.90527965171657</v>
       </c>
       <c r="D40" s="23">
-        <v>142.7067872375346</v>
+        <v>142.67036149247721</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6009,10 +6010,10 @@
         <v>149.89913666554651</v>
       </c>
       <c r="C41" s="23">
-        <v>142.22577535334764</v>
+        <v>142.02219124714563</v>
       </c>
       <c r="D41" s="23">
-        <v>142.79548408691574</v>
+        <v>142.76011834446297</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6023,10 +6024,10 @@
         <v>164.14987187524667</v>
       </c>
       <c r="C42" s="23">
-        <v>143.96727871307729</v>
+        <v>144.13658373694167</v>
       </c>
       <c r="D42" s="23">
-        <v>142.86435962927655</v>
+        <v>142.82904520635677</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6037,10 +6038,10 @@
         <v>150.84993435355395</v>
       </c>
       <c r="C43" s="23">
-        <v>143.21255474423813</v>
+        <v>143.24683382661794</v>
       </c>
       <c r="D43" s="23">
-        <v>142.87843518276907</v>
+        <v>142.84244568863187</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6051,10 +6052,10 @@
         <v>146.76823737542938</v>
       </c>
       <c r="C44" s="23">
-        <v>145.18591426537057</v>
+        <v>145.33902498209056</v>
       </c>
       <c r="D44" s="23">
-        <v>142.80747129076016</v>
+        <v>142.76979163074867</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6065,10 +6066,10 @@
         <v>141.27943584642691</v>
       </c>
       <c r="C45" s="23">
-        <v>145.12946165220967</v>
+        <v>145.04881896460523</v>
       </c>
       <c r="D45" s="23">
-        <v>142.62804047168277</v>
+        <v>142.58776942595657</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6079,10 +6080,10 @@
         <v>134.8898780340036</v>
       </c>
       <c r="C46" s="23">
-        <v>141.88554362002733</v>
+        <v>141.8130755909541</v>
       </c>
       <c r="D46" s="23">
-        <v>142.32657272225879</v>
+        <v>142.28279432966087</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6093,10 +6094,10 @@
         <v>141.51079081863656</v>
       </c>
       <c r="C47" s="23">
-        <v>143.43559427799272</v>
+        <v>143.37909086051801</v>
       </c>
       <c r="D47" s="23">
-        <v>141.90219009379146</v>
+        <v>141.8536202744846</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6107,10 +6108,10 @@
         <v>137.65812501310066</v>
       </c>
       <c r="C48" s="23">
-        <v>140.95073131422902</v>
+        <v>140.96866926544124</v>
       </c>
       <c r="D48" s="23">
-        <v>141.3669723322715</v>
+        <v>141.31017040744737</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6121,10 +6122,10 @@
         <v>135.67188913384834</v>
       </c>
       <c r="C49" s="23">
-        <v>140.83161228640137</v>
+        <v>140.87017775270306</v>
       </c>
       <c r="D49" s="23">
-        <v>140.74408557644142</v>
+        <v>140.67607996233244</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6135,10 +6136,10 @@
         <v>132.28222137059714</v>
       </c>
       <c r="C50" s="23">
-        <v>140.71315602198064</v>
+        <v>140.87243022762496</v>
       </c>
       <c r="D50" s="23">
-        <v>140.06505684091601</v>
+        <v>139.98285997787124</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6149,10 +6150,10 @@
         <v>129.74514246900199</v>
       </c>
       <c r="C51" s="23">
-        <v>140.8026758451025</v>
+        <v>140.77740788553311</v>
       </c>
       <c r="D51" s="23">
-        <v>139.36819826395134</v>
+        <v>139.26881128447522</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6163,10 +6164,10 @@
         <v>129.09773925167573</v>
       </c>
       <c r="C52" s="23">
-        <v>125.33712817648855</v>
+        <v>125.20312193044703</v>
       </c>
       <c r="D52" s="23">
-        <v>138.69717756039833</v>
+        <v>138.57780097019412</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6177,10 +6178,10 @@
         <v>111.90399788955911</v>
       </c>
       <c r="C53" s="23">
-        <v>104.57736601996343</v>
+        <v>104.44005959241511</v>
       </c>
       <c r="D53" s="23">
-        <v>138.09284317066485</v>
+        <v>137.95096969824294</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6191,10 +6192,10 @@
         <v>131.2946318586888</v>
       </c>
       <c r="C54" s="23">
-        <v>115.54568944071245</v>
+        <v>115.71920047673487</v>
       </c>
       <c r="D54" s="23">
-        <v>137.58951969383398</v>
+        <v>137.4234012268287</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6205,10 +6206,10 @@
         <v>133.30380295944371</v>
       </c>
       <c r="C55" s="23">
-        <v>123.78774900754838</v>
+        <v>123.75154439908655</v>
       </c>
       <c r="D55" s="23">
-        <v>137.21139534855942</v>
+        <v>137.02064480923019</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6219,10 +6220,10 @@
         <v>128.19060020722847</v>
       </c>
       <c r="C56" s="23">
-        <v>126.39445194319801</v>
+        <v>126.56252818867071</v>
       </c>
       <c r="D56" s="23">
-        <v>136.97124538986577</v>
+        <v>136.7566000833894</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6233,10 +6234,10 @@
         <v>125.17398093090794</v>
       </c>
       <c r="C57" s="23">
-        <v>129.50665483971034</v>
+        <v>129.45291983223831</v>
       </c>
       <c r="D57" s="23">
-        <v>136.8674945472375</v>
+        <v>136.63268166054903</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6247,10 +6248,10 @@
         <v>126.59643362404854</v>
       </c>
       <c r="C58" s="23">
-        <v>132.29905113101225</v>
+        <v>132.1847098930395</v>
       </c>
       <c r="D58" s="23">
-        <v>136.88696962346384</v>
+        <v>136.64003254109167</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6261,10 +6262,10 @@
         <v>131.72830919276413</v>
       </c>
       <c r="C59" s="23">
-        <v>133.80992361356132</v>
+        <v>133.91011357569636</v>
       </c>
       <c r="D59" s="23">
-        <v>137.00862743276676</v>
+        <v>136.7610441406427</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6275,10 +6276,10 @@
         <v>132.97012438356944</v>
       </c>
       <c r="C60" s="23">
-        <v>135.69015032185786</v>
+        <v>135.72163817827868</v>
       </c>
       <c r="D60" s="23">
-        <v>137.20482283224194</v>
+        <v>136.97347009900835</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6289,10 +6290,10 @@
         <v>132.42067625248373</v>
       </c>
       <c r="C61" s="23">
-        <v>136.24366536945175</v>
+        <v>136.11198755092875</v>
       </c>
       <c r="D61" s="23">
-        <v>137.44694174696019</v>
+        <v>137.2523896762242</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6303,10 +6304,10 @@
         <v>129.48861249275998</v>
       </c>
       <c r="C62" s="23">
-        <v>139.26820739172535</v>
+        <v>139.34038773157593</v>
       </c>
       <c r="D62" s="23">
-        <v>137.70869416463844</v>
+        <v>137.57482539473961</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6317,10 +6318,10 @@
         <v>126.69207197318048</v>
       </c>
       <c r="C63" s="23">
-        <v>138.35838125671387</v>
+        <v>138.34175606911657</v>
       </c>
       <c r="D63" s="23">
-        <v>137.96766590471017</v>
+        <v>137.92090390421299</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6331,10 +6332,10 @@
         <v>146.29362400573223</v>
       </c>
       <c r="C64" s="23">
-        <v>139.42572571650996</v>
+        <v>139.3701705642932</v>
       </c>
       <c r="D64" s="23">
-        <v>138.21076406361837</v>
+        <v>138.27787452165805</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6342,13 +6343,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="23">
-        <v>144.91616359474941</v>
+        <v>144.94098014353895</v>
       </c>
       <c r="C65" s="23">
-        <v>137.31459223680645</v>
+        <v>137.24704859854302</v>
       </c>
       <c r="D65" s="23">
-        <v>138.42905997527637</v>
+        <v>138.63375152919053</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -6356,13 +6357,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="23">
-        <v>150.20777418280562</v>
+        <v>150.19426546871918</v>
       </c>
       <c r="C66" s="23">
-        <v>135.29958722574628</v>
+        <v>135.53051816492388</v>
       </c>
       <c r="D66" s="23">
-        <v>138.61742691269239</v>
+        <v>138.97762924559697</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -6370,27 +6371,41 @@
         <v>44348</v>
       </c>
       <c r="B67" s="23">
-        <v>148.86536500389798</v>
+        <v>148.85405716919453</v>
       </c>
       <c r="C67" s="23">
-        <v>138.62993201812267</v>
+        <v>138.46654471724253</v>
       </c>
       <c r="D67" s="23">
-        <v>138.77171734659635</v>
+        <v>139.29779460751624</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>44378</v>
       </c>
-      <c r="B68" s="24">
-        <v>143.1915756885594</v>
-      </c>
-      <c r="C68" s="24">
-        <v>139.68439401987982</v>
-      </c>
-      <c r="D68" s="24">
-        <v>138.89266695465867</v>
+      <c r="B68" s="23">
+        <v>143.28775416943995</v>
+      </c>
+      <c r="C68" s="23">
+        <v>139.76360355605533</v>
+      </c>
+      <c r="D68" s="23">
+        <v>139.58597540884921</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>44409</v>
+      </c>
+      <c r="B69" s="24">
+        <v>141.21516835143112</v>
+      </c>
+      <c r="C69" s="24">
+        <v>141.26468534329823</v>
+      </c>
+      <c r="D69" s="24">
+        <v>139.83238178591031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizando dato fiscal a octubre y emae a septiembre"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FD0CE2-EA81-4AEF-A9AE-DDFD4D9B7ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C4945C-BA26-40CE-ABAD-A4E49F7C8515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -2056,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
@@ -5444,10 +5444,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D69"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5479,10 +5479,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="23">
-        <v>148.08564975129613</v>
+        <v>148.10165754695203</v>
       </c>
       <c r="D2" s="23">
-        <v>147.03387226699309</v>
+        <v>147.06011385125024</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5493,10 +5493,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="23">
-        <v>146.69442984564876</v>
+        <v>146.70606708828808</v>
       </c>
       <c r="D3" s="23">
-        <v>146.44742243656174</v>
+        <v>146.47796325278543</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,10 +5507,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="23">
-        <v>145.93345379152709</v>
+        <v>145.97990354527658</v>
       </c>
       <c r="D4" s="23">
-        <v>145.90110763056185</v>
+        <v>145.93317341480011</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5521,10 +5521,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="23">
-        <v>145.1412175425717</v>
+        <v>145.19152497659766</v>
       </c>
       <c r="D5" s="23">
-        <v>145.43068891856151</v>
+        <v>145.46083293448183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5535,10 +5535,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="23">
-        <v>144.34300755730996</v>
+        <v>144.39688540541056</v>
       </c>
       <c r="D6" s="23">
-        <v>145.06188650681096</v>
+        <v>145.08724802832404</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5549,10 +5549,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="23">
-        <v>144.28797360310097</v>
+        <v>144.31933374439532</v>
       </c>
       <c r="D7" s="23">
-        <v>144.81328745028688</v>
+        <v>144.83289463227342</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5563,10 +5563,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="23">
-        <v>144.33935091916433</v>
+        <v>144.38093157487899</v>
       </c>
       <c r="D8" s="23">
-        <v>144.69210529007546</v>
+        <v>144.70704419514331</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5577,10 +5577,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="23">
-        <v>145.61154439316164</v>
+        <v>145.62629617134974</v>
       </c>
       <c r="D9" s="23">
-        <v>144.70068005337293</v>
+        <v>144.7123284518546</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5591,10 +5591,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="23">
-        <v>145.1712839511917</v>
+        <v>145.11930463967713</v>
       </c>
       <c r="D10" s="23">
-        <v>144.83573403445854</v>
+        <v>144.84522772583608</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5605,10 +5605,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="23">
-        <v>145.08094014452863</v>
+        <v>145.01481318918368</v>
       </c>
       <c r="D11" s="23">
-        <v>145.08853591163188</v>
+        <v>145.09658500101486</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5619,10 +5619,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="23">
-        <v>145.79753996707345</v>
+        <v>145.72308843409533</v>
       </c>
       <c r="D12" s="23">
-        <v>145.4447923388897</v>
+        <v>145.45178504726957</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5633,10 +5633,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="23">
-        <v>147.08496231046456</v>
+        <v>147.01154744364237</v>
       </c>
       <c r="D13" s="23">
-        <v>145.89313120267528</v>
+        <v>145.89864030121484</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5644,13 +5644,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="23">
-        <v>136.63265948871924</v>
+        <v>136.63265948871918</v>
       </c>
       <c r="C14" s="23">
-        <v>147.39150858719742</v>
+        <v>147.42211146867183</v>
       </c>
       <c r="D14" s="23">
-        <v>146.41938683765051</v>
+        <v>146.42194598217245</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5658,13 +5658,13 @@
         <v>42767</v>
       </c>
       <c r="B15" s="23">
-        <v>132.1585163421652</v>
+        <v>132.15851634216514</v>
       </c>
       <c r="C15" s="23">
-        <v>146.51248208221301</v>
+        <v>146.52134192135418</v>
       </c>
       <c r="D15" s="23">
-        <v>147.00801418718893</v>
+        <v>147.00567489805485</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5672,13 +5672,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="23">
-        <v>152.62095855115743</v>
+        <v>152.62095855115714</v>
       </c>
       <c r="C16" s="23">
-        <v>147.87711776172259</v>
+        <v>147.92282798543368</v>
       </c>
       <c r="D16" s="23">
-        <v>147.64057421016545</v>
+        <v>147.63148434385997</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5686,13 +5686,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="23">
-        <v>151.94634477931737</v>
+        <v>151.94634477931677</v>
       </c>
       <c r="C17" s="23">
-        <v>147.6200526471016</v>
+        <v>147.71660613346299</v>
       </c>
       <c r="D17" s="23">
-        <v>148.29435735221259</v>
+        <v>148.27744686517678</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5700,13 +5700,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="23">
-        <v>168.3892094587577</v>
+        <v>168.38920945875736</v>
       </c>
       <c r="C18" s="23">
-        <v>148.56552023541587</v>
+        <v>148.66749690188567</v>
       </c>
       <c r="D18" s="23">
-        <v>148.94059438868203</v>
+        <v>148.91619756849141</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5714,13 +5714,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="23">
-        <v>161.03568550523215</v>
+        <v>161.03568550523272</v>
       </c>
       <c r="C19" s="23">
-        <v>150.18466581181673</v>
+        <v>150.27456340852842</v>
       </c>
       <c r="D19" s="23">
-        <v>149.5458052491299</v>
+        <v>149.51556034063185</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5728,13 +5728,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="23">
-        <v>150.30605023791972</v>
+        <v>150.30605023792174</v>
       </c>
       <c r="C20" s="23">
-        <v>150.18978161328192</v>
+        <v>150.2242120627169</v>
       </c>
       <c r="D20" s="23">
-        <v>150.07439547417798</v>
+        <v>150.04145507008428</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5742,13 +5742,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="23">
-        <v>149.25534282189594</v>
+        <v>149.25534282189673</v>
       </c>
       <c r="C21" s="23">
-        <v>150.2826717181747</v>
+        <v>150.28455103770648</v>
       </c>
       <c r="D21" s="23">
-        <v>150.49015578406019</v>
+        <v>150.45888970969398</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5756,13 +5756,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="23">
-        <v>146.38655949569906</v>
+        <v>146.38655949569588</v>
       </c>
       <c r="C22" s="23">
-        <v>151.36708028553946</v>
+        <v>151.26012541395224</v>
       </c>
       <c r="D22" s="23">
-        <v>150.75935848143519</v>
+        <v>150.73472510894828</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5770,13 +5770,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="23">
-        <v>149.38594914968527</v>
+        <v>149.38594914967547</v>
       </c>
       <c r="C23" s="23">
-        <v>151.57469170698224</v>
+        <v>151.49015645077984</v>
       </c>
       <c r="D23" s="23">
-        <v>150.85468193676391</v>
+        <v>150.84231133769393</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5784,13 +5784,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="23">
-        <v>151.92604263437596</v>
+        <v>151.92604263437173</v>
       </c>
       <c r="C24" s="23">
-        <v>152.71651174752355</v>
+        <v>152.5904784270094</v>
       </c>
       <c r="D24" s="23">
-        <v>150.75570011432879</v>
+        <v>150.75920810829331</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5798,13 +5798,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="23">
-        <v>146.78338564320444</v>
+        <v>146.78338564321811</v>
       </c>
       <c r="C25" s="23">
-        <v>152.5446201387291</v>
+        <v>152.45223310641683</v>
       </c>
       <c r="D25" s="23">
-        <v>150.45464990026778</v>
+        <v>150.47414360217039</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5812,13 +5812,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="23">
-        <v>142.74091494473581</v>
+        <v>142.74091494477966</v>
       </c>
       <c r="C26" s="23">
-        <v>152.04375046468527</v>
+        <v>152.05318910412834</v>
       </c>
       <c r="D26" s="23">
-        <v>149.96161463003151</v>
+        <v>149.99249933917798</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5826,13 +5826,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="23">
-        <v>138.81804133744413</v>
+        <v>138.81804133746257</v>
       </c>
       <c r="C27" s="23">
-        <v>151.97256082257195</v>
+        <v>151.95621824155725</v>
       </c>
       <c r="D27" s="23">
-        <v>149.29867688702436</v>
+        <v>149.33449846313019</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5840,13 +5840,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="23">
-        <v>155.85731621141912</v>
+        <v>155.85731621135642</v>
       </c>
       <c r="C28" s="23">
-        <v>151.05042355002405</v>
+        <v>151.13224640048483</v>
       </c>
       <c r="D28" s="23">
-        <v>148.5016840488164</v>
+        <v>148.5357327697711</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5854,13 +5854,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="23">
-        <v>151.52453339209498</v>
+        <v>151.5245333918956</v>
       </c>
       <c r="C29" s="23">
-        <v>146.56859163367963</v>
+        <v>146.76653086171689</v>
       </c>
       <c r="D29" s="23">
-        <v>147.61657618242</v>
+        <v>147.64353799666839</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5868,13 +5868,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="23">
-        <v>159.56668791308005</v>
+        <v>159.56668791299592</v>
       </c>
       <c r="C30" s="23">
-        <v>144.23166947605677</v>
+        <v>144.47116632154837</v>
       </c>
       <c r="D30" s="23">
-        <v>146.6948617947395</v>
+        <v>146.71224763922234</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5882,13 +5882,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="23">
-        <v>151.12577829014</v>
+        <v>151.12577829042309</v>
       </c>
       <c r="C31" s="23">
-        <v>142.96282334736145</v>
+        <v>143.16790060128201</v>
       </c>
       <c r="D31" s="23">
-        <v>145.7883566744795</v>
+        <v>145.79671418410095</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5896,13 +5896,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="23">
-        <v>145.9635724027205</v>
+        <v>145.96357240362272</v>
       </c>
       <c r="C32" s="23">
-        <v>143.13008060693846</v>
+        <v>143.18426460201746</v>
       </c>
       <c r="D32" s="23">
-        <v>144.94477555583887</v>
+        <v>144.94574021539933</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5910,13 +5910,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="23">
-        <v>146.76598025632637</v>
+        <v>146.7659802567066</v>
       </c>
       <c r="C33" s="23">
-        <v>146.70640624813697</v>
+        <v>146.6703002941353</v>
       </c>
       <c r="D33" s="23">
-        <v>144.20530460973021</v>
+        <v>144.20277495116173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5924,13 +5924,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="23">
-        <v>137.74650152374514</v>
+        <v>137.74650152246224</v>
       </c>
       <c r="C34" s="23">
-        <v>143.48383930199907</v>
+        <v>143.21441455276511</v>
       </c>
       <c r="D34" s="23">
-        <v>143.59635909613405</v>
+        <v>143.59765990622873</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5938,13 +5938,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="23">
-        <v>142.84305870601489</v>
+        <v>142.8430587019277</v>
       </c>
       <c r="C35" s="23">
-        <v>143.65586311368153</v>
+        <v>143.49041072556793</v>
       </c>
       <c r="D35" s="23">
-        <v>143.13174084303111</v>
+        <v>143.1462035088187</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5952,13 +5952,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="23">
-        <v>140.59231573478493</v>
+        <v>140.59231573306195</v>
       </c>
       <c r="C36" s="23">
-        <v>141.84250630210019</v>
+        <v>141.67662739598265</v>
       </c>
       <c r="D36" s="23">
-        <v>142.81398711436555</v>
+        <v>142.85070190595707</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5966,13 +5966,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="23">
-        <v>136.25192483815948</v>
+        <v>136.25192484396928</v>
       </c>
       <c r="C37" s="23">
-        <v>142.14811090503628</v>
+        <v>142.01335665376354</v>
       </c>
       <c r="D37" s="23">
-        <v>142.63379548165739</v>
+        <v>142.69985501276628</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5980,13 +5980,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="23">
-        <v>134.52056073135645</v>
+        <v>134.52056074986749</v>
       </c>
       <c r="C38" s="23">
-        <v>142.97195995832118</v>
+        <v>142.95142084393885</v>
       </c>
       <c r="D38" s="23">
-        <v>142.57132998428619</v>
+        <v>142.67065930569331</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -5994,13 +5994,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="23">
-        <v>132.2752983795491</v>
+        <v>132.27529838735211</v>
       </c>
       <c r="C39" s="23">
-        <v>143.64519108620124</v>
+        <v>143.6322881851294</v>
       </c>
       <c r="D39" s="23">
-        <v>142.59516808591269</v>
+        <v>142.72862801054333</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6008,13 +6008,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="23">
-        <v>144.87373847945011</v>
+        <v>144.87373845313573</v>
       </c>
       <c r="C40" s="23">
-        <v>140.90527965171657</v>
+        <v>141.06411060855854</v>
       </c>
       <c r="D40" s="23">
-        <v>142.67036149247721</v>
+        <v>142.83384953084763</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6022,13 +6022,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="23">
-        <v>149.89913666554651</v>
+        <v>149.89913658170545</v>
       </c>
       <c r="C41" s="23">
-        <v>142.02219124714563</v>
+        <v>142.43722546826555</v>
       </c>
       <c r="D41" s="23">
-        <v>142.76011834446297</v>
+        <v>142.9443961186353</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6036,13 +6036,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="23">
-        <v>164.14987187524667</v>
+        <v>164.14987183990465</v>
       </c>
       <c r="C42" s="23">
-        <v>144.13658373694167</v>
+        <v>144.59335254098048</v>
       </c>
       <c r="D42" s="23">
-        <v>142.82904520635677</v>
+        <v>143.0214232499377</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6050,13 +6050,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="23">
-        <v>150.84993435355395</v>
+        <v>150.84993447273672</v>
       </c>
       <c r="C43" s="23">
-        <v>143.24683382661794</v>
+        <v>143.60453096039134</v>
       </c>
       <c r="D43" s="23">
-        <v>142.84244568863187</v>
+        <v>143.02765620539995</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6064,13 +6064,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="23">
-        <v>146.76823737542938</v>
+        <v>146.76823775516263</v>
       </c>
       <c r="C44" s="23">
-        <v>145.33902498209056</v>
+        <v>145.34642155952127</v>
       </c>
       <c r="D44" s="23">
-        <v>142.76979163074867</v>
+        <v>142.93253718731484</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6078,13 +6078,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="23">
-        <v>141.27943584642691</v>
+        <v>141.27943600649775</v>
       </c>
       <c r="C45" s="23">
-        <v>145.04881896460523</v>
+        <v>144.85919857411906</v>
       </c>
       <c r="D45" s="23">
-        <v>142.58776942595657</v>
+        <v>142.71317686559692</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,13 +6092,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="23">
-        <v>134.8898780340036</v>
+        <v>134.88987749419911</v>
       </c>
       <c r="C46" s="23">
-        <v>141.8130755909541</v>
+        <v>141.26854176407389</v>
       </c>
       <c r="D46" s="23">
-        <v>142.28279432966087</v>
+        <v>142.35717694510186</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6106,13 +6106,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="23">
-        <v>141.51079081863656</v>
+        <v>141.51078909874374</v>
       </c>
       <c r="C47" s="23">
-        <v>143.37909086051801</v>
+        <v>143.10411391687347</v>
       </c>
       <c r="D47" s="23">
-        <v>141.8536202744846</v>
+        <v>141.86476337979974</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6120,13 +6120,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="23">
-        <v>137.65812501310066</v>
+        <v>137.65812428810526</v>
       </c>
       <c r="C48" s="23">
-        <v>140.96866926544124</v>
+        <v>140.74965352561472</v>
       </c>
       <c r="D48" s="23">
-        <v>141.31017040744737</v>
+        <v>141.24653817971588</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6134,13 +6134,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="23">
-        <v>135.67188913384834</v>
+        <v>135.67189157873614</v>
       </c>
       <c r="C49" s="23">
-        <v>140.87017775270306</v>
+        <v>140.73603895881791</v>
       </c>
       <c r="D49" s="23">
-        <v>140.67607996233244</v>
+        <v>140.52913239392791</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6148,13 +6148,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="23">
-        <v>132.28222137059714</v>
+        <v>132.28222916035381</v>
       </c>
       <c r="C50" s="23">
-        <v>140.87243022762496</v>
+        <v>140.81185507990034</v>
       </c>
       <c r="D50" s="23">
-        <v>139.98285997787124</v>
+        <v>139.7463204363649</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6162,13 +6162,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="23">
-        <v>129.74514246900199</v>
+        <v>129.74514575265826</v>
       </c>
       <c r="C51" s="23">
-        <v>140.77740788553311</v>
+        <v>140.76018526334047</v>
       </c>
       <c r="D51" s="23">
-        <v>139.26881128447522</v>
+        <v>138.94108713492236</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6176,13 +6176,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="23">
-        <v>129.09773925167573</v>
+        <v>129.09772817826237</v>
       </c>
       <c r="C52" s="23">
-        <v>125.20312193044703</v>
+        <v>125.44345572143716</v>
       </c>
       <c r="D52" s="23">
-        <v>138.57780097019412</v>
+        <v>138.16077967052419</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6190,13 +6190,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="23">
-        <v>111.90399788955911</v>
+        <v>111.90396260810687</v>
       </c>
       <c r="C53" s="23">
-        <v>104.44005959241511</v>
+        <v>105.060021984369</v>
       </c>
       <c r="D53" s="23">
-        <v>137.95096969824294</v>
+        <v>137.45001399955834</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6204,13 +6204,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="23">
-        <v>131.2946318586888</v>
+        <v>131.29461698631593</v>
       </c>
       <c r="C54" s="23">
-        <v>115.71920047673487</v>
+        <v>116.42987037482203</v>
       </c>
       <c r="D54" s="23">
-        <v>137.4234012268287</v>
+        <v>136.8470558971776</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6218,13 +6218,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="23">
-        <v>133.30380295944371</v>
+        <v>133.30385311326845</v>
       </c>
       <c r="C55" s="23">
-        <v>123.75154439908655</v>
+        <v>124.26297064486374</v>
       </c>
       <c r="D55" s="23">
-        <v>137.02064480923019</v>
+        <v>136.380845778571</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6232,13 +6232,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="23">
-        <v>128.19060020722847</v>
+        <v>128.19076000436911</v>
       </c>
       <c r="C56" s="23">
-        <v>126.56252818867071</v>
+        <v>126.53877089646882</v>
       </c>
       <c r="D56" s="23">
-        <v>136.7566000833894</v>
+        <v>136.06982493519877</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6246,13 +6246,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="23">
-        <v>125.17398093090794</v>
+        <v>125.17404829102199</v>
       </c>
       <c r="C57" s="23">
-        <v>129.45291983223831</v>
+        <v>129.09066106950357</v>
       </c>
       <c r="D57" s="23">
-        <v>136.63268166054903</v>
+        <v>135.92414136566811</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6260,13 +6260,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="23">
-        <v>126.59643362404854</v>
+        <v>126.59620646679346</v>
       </c>
       <c r="C58" s="23">
-        <v>132.1847098930395</v>
+        <v>131.38476382450102</v>
       </c>
       <c r="D58" s="23">
-        <v>136.64003254109167</v>
+        <v>135.93985666262162</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6274,13 +6274,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="23">
-        <v>131.72830919276413</v>
+        <v>131.72758543779744</v>
       </c>
       <c r="C59" s="23">
-        <v>133.91011357569636</v>
+        <v>133.50811059480836</v>
       </c>
       <c r="D59" s="23">
-        <v>136.7610441406427</v>
+        <v>136.10800278503356</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6288,13 +6288,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="23">
-        <v>132.97012438356944</v>
+        <v>132.96981929539976</v>
       </c>
       <c r="C60" s="23">
-        <v>135.72163817827868</v>
+        <v>135.43776511823836</v>
       </c>
       <c r="D60" s="23">
-        <v>136.97347009900835</v>
+        <v>136.41659440463644</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6302,13 +6302,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="23">
-        <v>132.42067625248373</v>
+        <v>132.42170509561973</v>
       </c>
       <c r="C61" s="23">
-        <v>136.11198755092875</v>
+        <v>135.97923105517145</v>
       </c>
       <c r="D61" s="23">
-        <v>137.2523896762242</v>
+        <v>136.85254997095157</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6316,13 +6316,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="23">
-        <v>129.48861249275998</v>
+        <v>129.49189053171025</v>
       </c>
       <c r="C62" s="23">
-        <v>139.34038773157593</v>
+        <v>139.35201155899171</v>
       </c>
       <c r="D62" s="23">
-        <v>137.57482539473961</v>
+        <v>137.40121353230373</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6330,13 +6330,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="23">
-        <v>126.69207197318048</v>
+        <v>126.69345378187154</v>
       </c>
       <c r="C63" s="23">
-        <v>138.34175606911657</v>
+        <v>138.39075101551828</v>
       </c>
       <c r="D63" s="23">
-        <v>137.92090390421299</v>
+        <v>138.05015746442569</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6344,13 +6344,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="23">
-        <v>146.29362400573223</v>
+        <v>146.28896415809047</v>
       </c>
       <c r="C64" s="23">
-        <v>139.3701705642932</v>
+        <v>139.54716265632311</v>
       </c>
       <c r="D64" s="23">
-        <v>138.27787452165805</v>
+        <v>138.78993448119593</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6358,13 +6358,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="23">
-        <v>144.94098014353895</v>
+        <v>144.97246200010414</v>
       </c>
       <c r="C65" s="23">
-        <v>137.24704859854302</v>
+        <v>137.67825682421994</v>
       </c>
       <c r="D65" s="23">
-        <v>138.63375152919053</v>
+        <v>139.60825864673919</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -6372,13 +6372,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="23">
-        <v>150.19426546871918</v>
+        <v>150.19619085954542</v>
       </c>
       <c r="C66" s="23">
-        <v>135.53051816492388</v>
+        <v>136.31489355433899</v>
       </c>
       <c r="D66" s="23">
-        <v>138.97762924559697</v>
+        <v>140.48752126720049</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -6386,13 +6386,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="23">
-        <v>148.85405716919453</v>
+        <v>148.82064992180284</v>
       </c>
       <c r="C67" s="23">
-        <v>138.46654471724253</v>
+        <v>139.82633552993781</v>
       </c>
       <c r="D67" s="23">
-        <v>139.29779460751624</v>
+        <v>141.40181328922912</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -6400,27 +6400,41 @@
         <v>44378</v>
       </c>
       <c r="B68" s="23">
-        <v>143.28775416943995</v>
+        <v>143.18898687078175</v>
       </c>
       <c r="C68" s="23">
-        <v>139.76360355605533</v>
+        <v>141.79948818923302</v>
       </c>
       <c r="D68" s="23">
-        <v>139.58597540884921</v>
+        <v>142.32133191397287</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>44409</v>
       </c>
-      <c r="B69" s="24">
-        <v>141.21516835143112</v>
-      </c>
-      <c r="C69" s="24">
-        <v>141.26468534329823</v>
-      </c>
-      <c r="D69" s="24">
-        <v>139.83238178591031</v>
+      <c r="B69" s="23">
+        <v>141.2025348207026</v>
+      </c>
+      <c r="C69" s="23">
+        <v>143.84582815883468</v>
+      </c>
+      <c r="D69" s="23">
+        <v>143.21355123184694</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>44440</v>
+      </c>
+      <c r="B70" s="24">
+        <v>141.25733334080709</v>
+      </c>
+      <c r="C70" s="24">
+        <v>145.60931096173624</v>
+      </c>
+      <c r="D70" s="24">
+        <v>144.04410694020132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Producto y VAB tercer trimestre 21, ipc noviembre21"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5113DE2B-1B44-4EA2-9454-486019B0D61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A4E659-9CA1-4383-A0B2-ED7D85B93545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
-    <sheet name="IPC-OCT-Div" sheetId="2" r:id="rId2"/>
+    <sheet name="IPC-NOV-Div" sheetId="2" r:id="rId2"/>
     <sheet name="IPC-Interanual" sheetId="3" r:id="rId3"/>
     <sheet name="Producto" sheetId="4" r:id="rId4"/>
     <sheet name="Pobreza-Aglo" sheetId="5" r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="138">
   <si>
     <t>Período</t>
   </si>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -665,34 +665,11 @@
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -703,6 +680,9 @@
     <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1029,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,7 +1903,7 @@
       <c r="E52">
         <v>4.5</v>
       </c>
-      <c r="H52" s="26"/>
+      <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -1941,7 +1921,7 @@
       <c r="E53">
         <v>3.5</v>
       </c>
-      <c r="H53" s="26"/>
+      <c r="H53" s="25"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -1959,7 +1939,7 @@
       <c r="E54">
         <v>3.8</v>
       </c>
-      <c r="H54" s="26"/>
+      <c r="H54" s="25"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -2030,7 +2010,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="59">
+      <c r="A59" s="36">
         <v>44470</v>
       </c>
       <c r="B59" s="1">
@@ -2044,6 +2024,23 @@
       </c>
       <c r="E59">
         <v>1.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>44501</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C60">
+        <v>0.5</v>
+      </c>
+      <c r="D60">
+        <v>3.3</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2056,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,234 +2092,234 @@
       <c r="A2" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="25">
-        <v>3.2</v>
-      </c>
-      <c r="C2" s="25">
-        <v>3.5</v>
-      </c>
-      <c r="D2" s="60">
-        <v>3</v>
-      </c>
-      <c r="E2" s="60">
-        <v>3.3</v>
-      </c>
-      <c r="F2" s="60">
-        <v>2.4</v>
-      </c>
-      <c r="G2" s="60">
-        <v>3.2</v>
+      <c r="B2" s="37">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C2" s="37">
+        <v>2</v>
+      </c>
+      <c r="D2" s="37">
+        <v>2</v>
+      </c>
+      <c r="E2" s="37">
+        <v>2.7</v>
+      </c>
+      <c r="F2" s="37">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G2" s="37">
+        <v>2.5</v>
       </c>
       <c r="H2" s="21">
-        <v>3.2691934955630719</v>
+        <v>2.2209945335743164</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="25">
-        <v>1.3</v>
-      </c>
-      <c r="C3" s="25">
-        <v>1</v>
-      </c>
-      <c r="D3" s="60">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="60">
-        <v>2.1</v>
-      </c>
-      <c r="F3" s="60">
-        <v>0.6</v>
-      </c>
-      <c r="G3" s="60">
-        <v>2.2999999999999998</v>
+      <c r="B3" s="37">
+        <v>7.3</v>
+      </c>
+      <c r="C3" s="37">
+        <v>5.9</v>
+      </c>
+      <c r="D3" s="37">
+        <v>4.8</v>
+      </c>
+      <c r="E3" s="37">
+        <v>4.8</v>
+      </c>
+      <c r="F3" s="37">
+        <v>5.4</v>
+      </c>
+      <c r="G3" s="37">
+        <v>3</v>
       </c>
       <c r="H3" s="21">
-        <v>1.3246759611466707</v>
+        <v>6.25328408827448</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="25">
-        <v>2.8</v>
-      </c>
-      <c r="C4" s="25">
-        <v>2</v>
-      </c>
-      <c r="D4" s="60">
-        <v>2.5</v>
-      </c>
-      <c r="E4" s="60">
-        <v>2.1</v>
-      </c>
-      <c r="F4" s="60">
-        <v>2.4</v>
-      </c>
-      <c r="G4" s="60">
-        <v>2.5</v>
+      <c r="B4" s="37">
+        <v>-0.6</v>
+      </c>
+      <c r="C4" s="37">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="37">
+        <v>0.7</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1.2</v>
+      </c>
+      <c r="G4" s="37">
+        <v>0.3</v>
       </c>
       <c r="H4" s="21">
-        <v>2.4094701722198408</v>
+        <v>3.1641887715627703E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="25">
-        <v>2.9</v>
-      </c>
-      <c r="C5" s="25">
-        <v>2.9</v>
-      </c>
-      <c r="D5" s="60">
-        <v>3.1</v>
-      </c>
-      <c r="E5" s="60">
+      <c r="B5" s="37">
+        <v>1.8</v>
+      </c>
+      <c r="C5" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="37">
+        <v>-0.3</v>
+      </c>
+      <c r="E5" s="37">
         <v>0.9</v>
       </c>
-      <c r="F5" s="60">
-        <v>-0.7</v>
-      </c>
-      <c r="G5" s="60">
-        <v>1.2</v>
+      <c r="F5" s="37">
+        <v>0.7</v>
+      </c>
+      <c r="G5" s="37">
+        <v>-0.8</v>
       </c>
       <c r="H5" s="21">
-        <v>2.4469570290369447</v>
+        <v>0.92556827125573893</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="25">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C6" s="25">
-        <v>7.1</v>
-      </c>
-      <c r="D6" s="60">
-        <v>5.3</v>
-      </c>
-      <c r="E6" s="60">
-        <v>6.5</v>
-      </c>
-      <c r="F6" s="60">
-        <v>6.7</v>
-      </c>
-      <c r="G6" s="60">
+      <c r="B6" s="37">
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="37">
+        <v>2.6</v>
+      </c>
+      <c r="D6" s="37">
+        <v>2.8</v>
+      </c>
+      <c r="E6" s="37">
         <v>6.6</v>
       </c>
+      <c r="F6" s="37">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G6" s="37">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="H6" s="21">
-        <v>7.6689066071334189</v>
+        <v>2.4536942395441352</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="25">
-        <v>10.9</v>
-      </c>
-      <c r="C7" s="25">
-        <v>12.2</v>
-      </c>
-      <c r="D7" s="60">
-        <v>5.2</v>
-      </c>
-      <c r="E7" s="60">
-        <v>9.4</v>
-      </c>
-      <c r="F7" s="60">
-        <v>8.5</v>
-      </c>
-      <c r="G7" s="60">
-        <v>5.3</v>
+      <c r="B7" s="37">
+        <v>-11.8</v>
+      </c>
+      <c r="C7" s="37">
+        <v>-5.8</v>
+      </c>
+      <c r="D7" s="37">
+        <v>-1.6</v>
+      </c>
+      <c r="E7" s="37">
+        <v>-4.8</v>
+      </c>
+      <c r="F7" s="37">
+        <v>-2.7</v>
+      </c>
+      <c r="G7" s="37">
+        <v>-1.1000000000000001</v>
       </c>
       <c r="H7" s="21">
-        <v>10.630898955419177</v>
+        <v>-7.9754643397108698</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="25">
-        <v>3.8</v>
-      </c>
-      <c r="C8" s="25">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D8" s="60">
-        <v>3.8</v>
-      </c>
-      <c r="E8" s="60">
-        <v>3.6</v>
-      </c>
-      <c r="F8" s="60">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G8" s="60">
-        <v>2.6</v>
+      <c r="B8" s="37">
+        <v>4.3</v>
+      </c>
+      <c r="C8" s="37">
+        <v>2.8</v>
+      </c>
+      <c r="D8" s="37">
+        <v>1.8</v>
+      </c>
+      <c r="E8" s="37">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8" s="37">
+        <v>2.7</v>
+      </c>
+      <c r="G8" s="37">
+        <v>0.8</v>
       </c>
       <c r="H8" s="22">
-        <v>3.9585100159720721</v>
+        <v>3.2248792332832288</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="25">
-        <v>3.9</v>
-      </c>
-      <c r="C9" s="25">
-        <v>4.2</v>
-      </c>
-      <c r="D9" s="60">
-        <v>5.5</v>
-      </c>
-      <c r="E9" s="60">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F9" s="60">
-        <v>3.9</v>
-      </c>
-      <c r="G9" s="60">
-        <v>3.2</v>
+      <c r="B9" s="37">
+        <v>2.1</v>
+      </c>
+      <c r="C9" s="37">
+        <v>1.8</v>
+      </c>
+      <c r="D9" s="37">
+        <v>2.1</v>
+      </c>
+      <c r="E9" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="F9" s="37">
+        <v>1.7</v>
+      </c>
+      <c r="G9" s="37">
+        <v>1.8</v>
       </c>
       <c r="H9" s="21">
-        <v>4.0434031518494562</v>
+        <v>1.9171178181551118</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="25">
-        <v>3.4</v>
-      </c>
-      <c r="C10" s="25">
-        <v>3.7</v>
-      </c>
-      <c r="D10" s="60">
-        <v>2.5</v>
-      </c>
-      <c r="E10" s="60">
-        <v>5.4</v>
-      </c>
-      <c r="F10" s="60">
-        <v>2.5</v>
-      </c>
-      <c r="G10" s="60">
-        <v>2.2000000000000002</v>
+      <c r="B10" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="37">
+        <v>1.7</v>
+      </c>
+      <c r="D10" s="37">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E10" s="37">
+        <v>1</v>
+      </c>
+      <c r="F10" s="37">
+        <v>1.4</v>
+      </c>
+      <c r="G10" s="37">
+        <v>1</v>
       </c>
       <c r="H10" s="21">
-        <v>3.496551282281013</v>
+        <v>1.5292688785707886</v>
       </c>
     </row>
   </sheetData>
@@ -2336,7 +2333,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+      <selection activeCell="G2" sqref="G2:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,207 +2368,207 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28">
-        <v>3.5</v>
-      </c>
-      <c r="C2" s="30">
-        <v>3.8</v>
-      </c>
-      <c r="D2" s="32">
-        <v>3.4</v>
-      </c>
-      <c r="E2" s="36">
-        <v>3.5</v>
-      </c>
-      <c r="F2" s="34">
-        <v>3.2</v>
-      </c>
-      <c r="G2" s="38">
-        <v>3.1</v>
-      </c>
-      <c r="H2" s="40">
-        <v>2.9</v>
+      <c r="B2" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="C2" s="39">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D2" s="39">
+        <v>2.8</v>
+      </c>
+      <c r="E2" s="39">
+        <v>3</v>
+      </c>
+      <c r="F2" s="39">
+        <v>2.7</v>
+      </c>
+      <c r="G2" s="39">
+        <v>2.7</v>
+      </c>
+      <c r="H2" s="29">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27">
-        <v>3.4</v>
-      </c>
-      <c r="C3" s="29">
-        <v>3.6</v>
-      </c>
-      <c r="D3" s="31">
-        <v>3.4</v>
-      </c>
-      <c r="E3" s="35">
-        <v>3.2</v>
-      </c>
-      <c r="F3" s="33">
-        <v>3.6</v>
-      </c>
-      <c r="G3" s="37">
-        <v>2.5</v>
-      </c>
-      <c r="H3" s="39">
-        <v>2.9</v>
+      <c r="B3" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="C3" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="D3" s="38">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E3" s="38">
+        <v>2.7</v>
+      </c>
+      <c r="F3" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="G3" s="38">
+        <v>2.7</v>
+      </c>
+      <c r="H3" s="28">
+        <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="27">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C4" s="29">
-        <v>1.4</v>
-      </c>
-      <c r="D4" s="31">
+      <c r="B4" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C4" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" s="38">
         <v>2.9</v>
       </c>
-      <c r="E4" s="35">
-        <v>2.9</v>
-      </c>
-      <c r="F4" s="33">
-        <v>2.7</v>
-      </c>
-      <c r="G4" s="37">
-        <v>2.8</v>
-      </c>
-      <c r="H4" s="39">
-        <v>2.1</v>
+      <c r="F4" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H4" s="28">
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="27">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C5" s="29">
-        <v>5.8</v>
-      </c>
-      <c r="D5" s="31">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E5" s="35">
-        <v>6.9</v>
-      </c>
-      <c r="F5" s="33">
+      <c r="B5" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G5" s="37">
-        <v>2.7</v>
-      </c>
-      <c r="H5" s="39">
-        <v>3.9</v>
+      <c r="C5" s="38">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="38">
+        <v>5.7</v>
+      </c>
+      <c r="E5" s="38">
+        <v>3.4</v>
+      </c>
+      <c r="F5" s="38">
+        <v>4.2</v>
+      </c>
+      <c r="G5" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="H5" s="28">
+        <v>2.9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="27">
-        <v>2.5</v>
-      </c>
-      <c r="C6" s="29">
-        <v>2.9</v>
-      </c>
-      <c r="D6" s="31">
-        <v>2</v>
-      </c>
-      <c r="E6" s="35">
+      <c r="B6" s="26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C6" s="38">
         <v>1.8</v>
       </c>
-      <c r="F6" s="33">
-        <v>1.4</v>
-      </c>
-      <c r="G6" s="37">
-        <v>4.8</v>
-      </c>
-      <c r="H6" s="39">
-        <v>2</v>
+      <c r="D6" s="38">
+        <v>2.7</v>
+      </c>
+      <c r="E6" s="38">
+        <v>3</v>
+      </c>
+      <c r="F6" s="38">
+        <v>2.6</v>
+      </c>
+      <c r="G6" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="H6" s="28">
+        <v>1.8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
+        <v>2.7</v>
+      </c>
+      <c r="C7" s="38">
         <v>2.8</v>
       </c>
-      <c r="C7" s="29">
-        <v>2.8</v>
-      </c>
-      <c r="D7" s="31">
+      <c r="D7" s="38">
+        <v>2.6</v>
+      </c>
+      <c r="E7" s="38">
         <v>2.7</v>
       </c>
-      <c r="E7" s="35">
+      <c r="F7" s="38">
         <v>2.5</v>
       </c>
-      <c r="F7" s="33">
-        <v>2.7</v>
-      </c>
-      <c r="G7" s="37">
-        <v>2.7</v>
-      </c>
-      <c r="H7" s="39">
-        <v>3.5</v>
+      <c r="G7" s="38">
+        <v>2.6</v>
+      </c>
+      <c r="H7" s="28">
+        <v>3.1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="27">
-        <v>4.7</v>
-      </c>
-      <c r="C8" s="29">
-        <v>5.7</v>
-      </c>
-      <c r="D8" s="31">
-        <v>4.3</v>
-      </c>
-      <c r="E8" s="35">
-        <v>3.5</v>
-      </c>
-      <c r="F8" s="33">
-        <v>3.2</v>
-      </c>
-      <c r="G8" s="37">
-        <v>3.8</v>
-      </c>
-      <c r="H8" s="39">
-        <v>3.8</v>
+      <c r="B8" s="26">
+        <v>2.4</v>
+      </c>
+      <c r="C8" s="38">
+        <v>2.1</v>
+      </c>
+      <c r="D8" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="38">
+        <v>3.4</v>
+      </c>
+      <c r="F8" s="38">
+        <v>2.8</v>
+      </c>
+      <c r="G8" s="38">
+        <v>2.9</v>
+      </c>
+      <c r="H8" s="28">
+        <v>3.4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="27">
-        <v>3.1</v>
-      </c>
-      <c r="C9" s="29">
+      <c r="B9" s="26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C9" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="D9" s="38">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E9" s="38">
+        <v>3.8</v>
+      </c>
+      <c r="F9" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="G9" s="38">
         <v>3.2</v>
       </c>
-      <c r="D9" s="31">
-        <v>2.9</v>
-      </c>
-      <c r="E9" s="35">
-        <v>4</v>
-      </c>
-      <c r="F9" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="G9" s="37">
-        <v>3.4</v>
-      </c>
-      <c r="H9" s="39">
+      <c r="H9" s="28">
         <v>3.1</v>
       </c>
     </row>
@@ -2579,25 +2576,25 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="27">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C10" s="29">
-        <v>1</v>
-      </c>
-      <c r="D10" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="E10" s="35">
-        <v>1.2</v>
-      </c>
-      <c r="F10" s="33">
-        <v>0.9</v>
-      </c>
-      <c r="G10" s="37">
-        <v>1.3</v>
-      </c>
-      <c r="H10" s="39">
+      <c r="B10" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="38">
+        <v>-0.1</v>
+      </c>
+      <c r="D10" s="38">
+        <v>2.1</v>
+      </c>
+      <c r="E10" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="F10" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="G10" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="28">
         <v>0.2</v>
       </c>
     </row>
@@ -2605,104 +2602,104 @@
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="27">
-        <v>4</v>
-      </c>
-      <c r="C11" s="29">
-        <v>4.8</v>
-      </c>
-      <c r="D11" s="31">
-        <v>3.2</v>
-      </c>
-      <c r="E11" s="35">
-        <v>3.8</v>
-      </c>
-      <c r="F11" s="33">
-        <v>4.8</v>
-      </c>
-      <c r="G11" s="37">
-        <v>3.7</v>
-      </c>
-      <c r="H11" s="39">
-        <v>1.6</v>
+      <c r="B11" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="D11" s="38">
+        <v>1.9</v>
+      </c>
+      <c r="E11" s="38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F11" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="G11" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="28">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="27">
-        <v>1.4</v>
-      </c>
-      <c r="C12" s="29">
-        <v>1</v>
-      </c>
-      <c r="D12" s="31">
-        <v>2</v>
-      </c>
-      <c r="E12" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="F12" s="33">
-        <v>0.9</v>
-      </c>
-      <c r="G12" s="37">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H12" s="39">
-        <v>1.1000000000000001</v>
+      <c r="B12" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="C12" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="E12" s="38">
+        <v>0</v>
+      </c>
+      <c r="F12" s="38">
+        <v>0.6</v>
+      </c>
+      <c r="G12" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="26">
+        <v>5</v>
+      </c>
+      <c r="C13" s="38">
+        <v>6</v>
+      </c>
+      <c r="D13" s="38">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E13" s="38">
+        <v>5.8</v>
+      </c>
+      <c r="F13" s="38">
+        <v>3.4</v>
+      </c>
+      <c r="G13" s="38">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="29">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D13" s="31">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E13" s="35">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F13" s="33">
-        <v>3.2</v>
-      </c>
-      <c r="G13" s="37">
-        <v>3.2</v>
-      </c>
-      <c r="H13" s="39">
-        <v>3.3</v>
+      <c r="H13" s="28">
+        <v>2.1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="27">
-        <v>3.3</v>
-      </c>
-      <c r="C14" s="29">
-        <v>3.9</v>
-      </c>
-      <c r="D14" s="31">
+      <c r="B14" s="26">
+        <v>2</v>
+      </c>
+      <c r="C14" s="38">
+        <v>2</v>
+      </c>
+      <c r="D14" s="38">
+        <v>1.9</v>
+      </c>
+      <c r="E14" s="38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F14" s="38">
         <v>2.9</v>
       </c>
-      <c r="E14" s="35">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F14" s="33">
-        <v>3.2</v>
-      </c>
-      <c r="G14" s="37">
-        <v>3</v>
-      </c>
-      <c r="H14" s="39">
-        <v>2.9</v>
+      <c r="G14" s="38">
+        <v>2.6</v>
+      </c>
+      <c r="H14" s="28">
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>
@@ -2751,207 +2748,207 @@
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="42">
-        <v>52.1</v>
-      </c>
-      <c r="C2" s="44">
-        <v>52</v>
-      </c>
-      <c r="D2" s="46">
-        <v>52.3</v>
-      </c>
-      <c r="E2" s="50">
-        <v>52.3</v>
-      </c>
-      <c r="F2" s="48">
-        <v>51.8</v>
-      </c>
-      <c r="G2" s="52">
-        <v>51.9</v>
-      </c>
-      <c r="H2" s="54">
-        <v>52.6</v>
+      <c r="B2" s="31">
+        <v>51.2</v>
+      </c>
+      <c r="C2" s="40">
+        <v>50.9</v>
+      </c>
+      <c r="D2" s="40">
+        <v>51.4</v>
+      </c>
+      <c r="E2" s="40">
+        <v>51.3</v>
+      </c>
+      <c r="F2" s="40">
+        <v>51.2</v>
+      </c>
+      <c r="G2" s="40">
+        <v>51.2</v>
+      </c>
+      <c r="H2" s="40">
+        <v>51.5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="41">
-        <v>51.4</v>
-      </c>
-      <c r="C3" s="43">
-        <v>49.3</v>
-      </c>
-      <c r="D3" s="45">
-        <v>53.5</v>
-      </c>
-      <c r="E3" s="49">
-        <v>54.2</v>
-      </c>
-      <c r="F3" s="47">
-        <v>51.5</v>
-      </c>
-      <c r="G3" s="51">
-        <v>52.3</v>
-      </c>
-      <c r="H3" s="53">
+      <c r="B3" s="30">
+        <v>50.5</v>
+      </c>
+      <c r="C3" s="23">
+        <v>48.8</v>
+      </c>
+      <c r="D3" s="23">
         <v>51.8</v>
+      </c>
+      <c r="E3" s="23">
+        <v>53.1</v>
+      </c>
+      <c r="F3" s="23">
+        <v>51.9</v>
+      </c>
+      <c r="G3" s="23">
+        <v>52.2</v>
+      </c>
+      <c r="H3" s="23">
+        <v>49.9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="41">
-        <v>55</v>
-      </c>
-      <c r="C4" s="43">
+      <c r="B4" s="30">
         <v>52.2</v>
       </c>
-      <c r="D4" s="45">
-        <v>57.3</v>
-      </c>
-      <c r="E4" s="49">
-        <v>61.1</v>
-      </c>
-      <c r="F4" s="47">
-        <v>59.1</v>
-      </c>
-      <c r="G4" s="51">
-        <v>55.3</v>
-      </c>
-      <c r="H4" s="53">
-        <v>53.8</v>
+      <c r="C4" s="23">
+        <v>50</v>
+      </c>
+      <c r="D4" s="23">
+        <v>53.7</v>
+      </c>
+      <c r="E4" s="23">
+        <v>60.9</v>
+      </c>
+      <c r="F4" s="23">
+        <v>55.2</v>
+      </c>
+      <c r="G4" s="23">
+        <v>52.3</v>
+      </c>
+      <c r="H4" s="23">
+        <v>49.6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="41">
-        <v>62.2</v>
-      </c>
-      <c r="C5" s="43">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="D5" s="45">
+      <c r="B5" s="30">
+        <v>62.8</v>
+      </c>
+      <c r="C5" s="23">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D5" s="23">
+        <v>61.6</v>
+      </c>
+      <c r="E5" s="23">
+        <v>63.9</v>
+      </c>
+      <c r="F5" s="23">
         <v>58.7</v>
       </c>
-      <c r="E5" s="49">
-        <v>66.3</v>
-      </c>
-      <c r="F5" s="47">
-        <v>60.7</v>
-      </c>
-      <c r="G5" s="51">
-        <v>59.3</v>
-      </c>
-      <c r="H5" s="53">
-        <v>65.599999999999994</v>
+      <c r="G5" s="23">
+        <v>56.2</v>
+      </c>
+      <c r="H5" s="23">
+        <v>62.6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="41">
-        <v>29.8</v>
-      </c>
-      <c r="C6" s="43">
-        <v>32.5</v>
-      </c>
-      <c r="D6" s="45">
-        <v>25.5</v>
-      </c>
-      <c r="E6" s="49">
-        <v>31.3</v>
-      </c>
-      <c r="F6" s="47">
-        <v>30.4</v>
-      </c>
-      <c r="G6" s="51">
-        <v>28.9</v>
-      </c>
-      <c r="H6" s="53">
-        <v>33.299999999999997</v>
+      <c r="B6" s="30">
+        <v>29.4</v>
+      </c>
+      <c r="C6" s="23">
+        <v>31.6</v>
+      </c>
+      <c r="D6" s="23">
+        <v>25.1</v>
+      </c>
+      <c r="E6" s="23">
+        <v>31.5</v>
+      </c>
+      <c r="F6" s="23">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="G6" s="23">
+        <v>28</v>
+      </c>
+      <c r="H6" s="23">
+        <v>32.6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="41">
-        <v>47</v>
-      </c>
-      <c r="C7" s="43">
-        <v>46.9</v>
-      </c>
-      <c r="D7" s="45">
-        <v>46.8</v>
-      </c>
-      <c r="E7" s="49">
-        <v>42.9</v>
-      </c>
-      <c r="F7" s="47">
-        <v>46.9</v>
-      </c>
-      <c r="G7" s="51">
-        <v>49.8</v>
-      </c>
-      <c r="H7" s="53">
-        <v>50.4</v>
+      <c r="B7" s="30">
+        <v>45.2</v>
+      </c>
+      <c r="C7" s="23">
+        <v>45.3</v>
+      </c>
+      <c r="D7" s="23">
+        <v>45.3</v>
+      </c>
+      <c r="E7" s="23">
+        <v>40.6</v>
+      </c>
+      <c r="F7" s="23">
+        <v>43.1</v>
+      </c>
+      <c r="G7" s="23">
+        <v>48.2</v>
+      </c>
+      <c r="H7" s="23">
+        <v>49.1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="41">
-        <v>60.9</v>
-      </c>
-      <c r="C8" s="43">
-        <v>61</v>
-      </c>
-      <c r="D8" s="45">
-        <v>61.6</v>
-      </c>
-      <c r="E8" s="49">
-        <v>60.1</v>
-      </c>
-      <c r="F8" s="47">
-        <v>60.1</v>
-      </c>
-      <c r="G8" s="51">
-        <v>62.1</v>
-      </c>
-      <c r="H8" s="53">
-        <v>54.5</v>
+      <c r="B8" s="30">
+        <v>59</v>
+      </c>
+      <c r="C8" s="23">
+        <v>58.9</v>
+      </c>
+      <c r="D8" s="23">
+        <v>59.7</v>
+      </c>
+      <c r="E8" s="23">
+        <v>58.7</v>
+      </c>
+      <c r="F8" s="23">
+        <v>57.3</v>
+      </c>
+      <c r="G8" s="23">
+        <v>60.2</v>
+      </c>
+      <c r="H8" s="23">
+        <v>55.3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="41">
-        <v>59.8</v>
-      </c>
-      <c r="C9" s="43">
-        <v>56.9</v>
-      </c>
-      <c r="D9" s="45">
-        <v>61.4</v>
-      </c>
-      <c r="E9" s="49">
-        <v>60.3</v>
-      </c>
-      <c r="F9" s="47">
-        <v>60.3</v>
-      </c>
-      <c r="G9" s="51">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="H9" s="53">
+      <c r="B9" s="30">
+        <v>57.6</v>
+      </c>
+      <c r="C9" s="23">
+        <v>53.2</v>
+      </c>
+      <c r="D9" s="23">
+        <v>60.2</v>
+      </c>
+      <c r="E9" s="23">
+        <v>60</v>
+      </c>
+      <c r="F9" s="23">
+        <v>58.3</v>
+      </c>
+      <c r="G9" s="23">
+        <v>64.3</v>
+      </c>
+      <c r="H9" s="23">
         <v>67.2</v>
       </c>
     </row>
@@ -2959,130 +2956,130 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="41">
-        <v>31.4</v>
-      </c>
-      <c r="C10" s="43">
-        <v>31.2</v>
-      </c>
-      <c r="D10" s="45">
-        <v>29.3</v>
-      </c>
-      <c r="E10" s="49">
-        <v>36</v>
-      </c>
-      <c r="F10" s="47">
-        <v>35.4</v>
-      </c>
-      <c r="G10" s="51">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="H10" s="53">
-        <v>38.299999999999997</v>
+      <c r="B10" s="30">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="C10" s="23">
+        <v>33.5</v>
+      </c>
+      <c r="D10" s="23">
+        <v>31.7</v>
+      </c>
+      <c r="E10" s="23">
+        <v>36.6</v>
+      </c>
+      <c r="F10" s="23">
+        <v>35</v>
+      </c>
+      <c r="G10" s="23">
+        <v>32</v>
+      </c>
+      <c r="H10" s="23">
+        <v>38.799999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="41">
-        <v>54.1</v>
-      </c>
-      <c r="C11" s="43">
-        <v>55.7</v>
-      </c>
-      <c r="D11" s="45">
-        <v>56.4</v>
-      </c>
-      <c r="E11" s="49">
-        <v>47.1</v>
-      </c>
-      <c r="F11" s="47">
+      <c r="B11" s="30">
+        <v>48.8</v>
+      </c>
+      <c r="C11" s="23">
+        <v>48.9</v>
+      </c>
+      <c r="D11" s="23">
         <v>51.4</v>
       </c>
-      <c r="G11" s="51">
-        <v>44.3</v>
-      </c>
-      <c r="H11" s="53">
-        <v>45.6</v>
+      <c r="E11" s="23">
+        <v>41.7</v>
+      </c>
+      <c r="F11" s="23">
+        <v>48.8</v>
+      </c>
+      <c r="G11" s="23">
+        <v>41.4</v>
+      </c>
+      <c r="H11" s="23">
+        <v>45.2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="41">
-        <v>54</v>
-      </c>
-      <c r="C12" s="43">
-        <v>59.9</v>
-      </c>
-      <c r="D12" s="45">
-        <v>52.9</v>
-      </c>
-      <c r="E12" s="49">
-        <v>39.9</v>
-      </c>
-      <c r="F12" s="47">
-        <v>48</v>
-      </c>
-      <c r="G12" s="51">
-        <v>41.9</v>
-      </c>
-      <c r="H12" s="53">
-        <v>38.5</v>
+      <c r="B12" s="30">
+        <v>54.6</v>
+      </c>
+      <c r="C12" s="23">
+        <v>59.7</v>
+      </c>
+      <c r="D12" s="23">
+        <v>54.9</v>
+      </c>
+      <c r="E12" s="23">
+        <v>39.5</v>
+      </c>
+      <c r="F12" s="23">
+        <v>48.9</v>
+      </c>
+      <c r="G12" s="23">
+        <v>41.8</v>
+      </c>
+      <c r="H12" s="23">
+        <v>38.799999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="41">
-        <v>60.6</v>
-      </c>
-      <c r="C13" s="43">
-        <v>63</v>
-      </c>
-      <c r="D13" s="45">
-        <v>58.3</v>
-      </c>
-      <c r="E13" s="49">
-        <v>57.9</v>
-      </c>
-      <c r="F13" s="47">
-        <v>60.5</v>
-      </c>
-      <c r="G13" s="51">
-        <v>62.2</v>
-      </c>
-      <c r="H13" s="53">
-        <v>57.1</v>
+      <c r="B13" s="30">
+        <v>63.4</v>
+      </c>
+      <c r="C13" s="23">
+        <v>67</v>
+      </c>
+      <c r="D13" s="23">
+        <v>60.4</v>
+      </c>
+      <c r="E13" s="23">
+        <v>61.6</v>
+      </c>
+      <c r="F13" s="23">
+        <v>60.3</v>
+      </c>
+      <c r="G13" s="23">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="H13" s="23">
+        <v>56.9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="41">
-        <v>37.6</v>
-      </c>
-      <c r="C14" s="43">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="D14" s="45">
-        <v>37.9</v>
-      </c>
-      <c r="E14" s="49">
-        <v>37</v>
-      </c>
-      <c r="F14" s="47">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="G14" s="51">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="H14" s="53">
+      <c r="B14" s="30">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="C14" s="23">
         <v>36.5</v>
+      </c>
+      <c r="D14" s="23">
+        <v>37.5</v>
+      </c>
+      <c r="E14" s="23">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="F14" s="23">
+        <v>36.6</v>
+      </c>
+      <c r="G14" s="23">
+        <v>34.9</v>
+      </c>
+      <c r="H14" s="23">
+        <v>36.700000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -3093,10 +3090,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,7 +3123,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="12">
-        <v>475642.42472660332</v>
+        <v>475580.6987789463</v>
       </c>
       <c r="D2" s="12">
         <v>460369.44223294902</v>
@@ -3140,7 +3137,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="12">
-        <v>470200.8392093571</v>
+        <v>470117.04863974027</v>
       </c>
       <c r="D3" s="12">
         <v>514395.68177236198</v>
@@ -3154,7 +3151,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="12">
-        <v>493619.48198730504</v>
+        <v>493688.23277629726</v>
       </c>
       <c r="D4" s="12">
         <v>481151.97994350799</v>
@@ -3168,7 +3165,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="12">
-        <v>500998.0346564647</v>
+        <v>501074.80040353234</v>
       </c>
       <c r="D5" s="12">
         <v>484543.67687656201</v>
@@ -3182,7 +3179,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12">
-        <v>515549.17415220023</v>
+        <v>515466.69291128084</v>
       </c>
       <c r="D6" s="12">
         <v>493602.53057785501</v>
@@ -3196,7 +3193,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="12">
-        <v>526354.71445859282</v>
+        <v>526287.52177886781</v>
       </c>
       <c r="D7" s="12">
         <v>581668.24987960199</v>
@@ -3210,7 +3207,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12">
-        <v>529839.79042928014</v>
+        <v>529905.85124294367</v>
       </c>
       <c r="D8" s="12">
         <v>514697.78950542799</v>
@@ -3224,7 +3221,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="12">
-        <v>540480.09097358375</v>
+        <v>540563.70408056455</v>
       </c>
       <c r="D9" s="12">
         <v>522255.20005077199</v>
@@ -3238,7 +3235,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="12">
-        <v>554648.53967353096</v>
+        <v>554560.99902440561</v>
       </c>
       <c r="D10" s="12">
         <v>532348.21201691695</v>
@@ -3252,7 +3249,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="12">
-        <v>561234.94252824865</v>
+        <v>561169.81491956639</v>
       </c>
       <c r="D11" s="12">
         <v>614076.39260854397</v>
@@ -3266,7 +3263,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="12">
-        <v>576819.37412435515</v>
+        <v>576896.43518582615</v>
       </c>
       <c r="D12" s="12">
         <v>562978.96562687703</v>
@@ -3280,7 +3277,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="12">
-        <v>589494.76055679133</v>
+        <v>589570.36775312782</v>
       </c>
       <c r="D13" s="12">
         <v>572794.04663058801</v>
@@ -3294,7 +3291,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="12">
-        <v>603280.28298430704</v>
+        <v>603213.94885090971</v>
       </c>
       <c r="D14" s="12">
         <v>576846.88569942699</v>
@@ -3308,7 +3305,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="12">
-        <v>616335.90141357086</v>
+        <v>616210.69847655308</v>
       </c>
       <c r="D15" s="12">
         <v>674620.563006485</v>
@@ -3322,7 +3319,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="12">
-        <v>624449.95860950905</v>
+        <v>624573.91952353565</v>
       </c>
       <c r="D16" s="12">
         <v>610425.69401485403</v>
@@ -3336,7 +3333,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="12">
-        <v>643703.86757697607</v>
+        <v>643771.44373336376</v>
       </c>
       <c r="D17" s="12">
         <v>625876.867863597</v>
@@ -3350,7 +3347,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="12">
-        <v>649632.21729591175</v>
+        <v>649568.57853084186</v>
       </c>
       <c r="D18" s="12">
         <v>616720.35706447798</v>
@@ -3364,7 +3361,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="12">
-        <v>653489.30235832697</v>
+        <v>653329.88824301912</v>
       </c>
       <c r="D19" s="12">
         <v>711405.50045523304</v>
@@ -3378,7 +3375,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="12">
-        <v>658334.73239632417</v>
+        <v>658526.0855344407</v>
       </c>
       <c r="D20" s="12">
         <v>647087.95974249404</v>
@@ -3392,7 +3389,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="12">
-        <v>627248.38691428315</v>
+        <v>627280.08665654622</v>
       </c>
       <c r="D21" s="12">
         <v>613490.82170264097</v>
@@ -3406,7 +3403,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>604341.08831760916</v>
+        <v>604353.82403393742</v>
       </c>
       <c r="D22" s="12">
         <v>578553.04424240498</v>
@@ -3420,7 +3417,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="12">
-        <v>591270.90822089184</v>
+        <v>591077.75225373311</v>
       </c>
       <c r="D23" s="12">
         <v>631197.75186006899</v>
@@ -3434,7 +3431,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="12">
-        <v>614141.40675168403</v>
+        <v>614278.67717957112</v>
       </c>
       <c r="D24" s="12">
         <v>610519.85461172694</v>
@@ -3448,7 +3445,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="12">
-        <v>625738.10236131249</v>
+        <v>625781.2521842561</v>
       </c>
       <c r="D25" s="12">
         <v>615220.85493729694</v>
@@ -3462,7 +3459,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="12">
-        <v>644704.0935263203</v>
+        <v>644789.01313001418</v>
       </c>
       <c r="D26" s="12">
         <v>611607.33658973</v>
@@ -3476,7 +3473,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="12">
-        <v>673929.6973366529</v>
+        <v>673595.52769258386</v>
       </c>
       <c r="D27" s="12">
         <v>733730.773968903</v>
@@ -3490,7 +3487,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="12">
-        <v>677075.94519358559</v>
+        <v>677244.35343238455</v>
       </c>
       <c r="D28" s="12">
         <v>668566.50948898599</v>
@@ -3504,7 +3501,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="12">
-        <v>686384.98171063466</v>
+        <v>686465.82351221156</v>
       </c>
       <c r="D29" s="12">
         <v>668190.097719574</v>
@@ -3518,7 +3515,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="12">
-        <v>702780.77429836371</v>
+        <v>702910.30347114604</v>
       </c>
       <c r="D30" s="12">
         <v>662325.58597269503</v>
@@ -3532,7 +3529,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="12">
-        <v>709613.94817853905</v>
+        <v>709227.10753214906</v>
       </c>
       <c r="D31" s="12">
         <v>766332.95457161299</v>
@@ -3546,7 +3543,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="12">
-        <v>715012.15085344797</v>
+        <v>715183.40697330865</v>
       </c>
       <c r="D32" s="12">
         <v>711417.39193010505</v>
@@ -3560,7 +3557,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="12">
-        <v>715719.51555205544</v>
+        <v>715805.57090580289</v>
       </c>
       <c r="D33" s="12">
         <v>703050.45640799298</v>
@@ -3574,7 +3571,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="12">
-        <v>707932.16239044804</v>
+        <v>708101.0604378581</v>
       </c>
       <c r="D34" s="12">
         <v>672685.993630504</v>
@@ -3588,7 +3585,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="12">
-        <v>683661.59501312114</v>
+        <v>683290.8369353821</v>
       </c>
       <c r="D35" s="12">
         <v>730838.27259277599</v>
@@ -3602,7 +3599,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="12">
-        <v>705126.95508238499</v>
+        <v>705279.72688988189</v>
       </c>
       <c r="D36" s="12">
         <v>703461.65253019601</v>
@@ -3616,7 +3613,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="12">
-        <v>717223.24534984084</v>
+        <v>717272.33357267547</v>
       </c>
       <c r="D37" s="12">
         <v>706958.03908231901</v>
@@ -3630,7 +3627,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="12">
-        <v>716977.20399880852</v>
+        <v>717112.53673472651</v>
       </c>
       <c r="D38" s="12">
         <v>677085.52917315101</v>
@@ -3644,7 +3641,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="12">
-        <v>720928.72319853469</v>
+        <v>720685.28631943744</v>
       </c>
       <c r="D39" s="12">
         <v>776486.60279942001</v>
@@ -3658,7 +3655,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="12">
-        <v>725463.71662261395</v>
+        <v>725535.58742117661</v>
       </c>
       <c r="D40" s="12">
         <v>721458.94421618199</v>
@@ -3672,7 +3669,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="12">
-        <v>718258.77739130252</v>
+        <v>718295.01073591749</v>
       </c>
       <c r="D41" s="12">
         <v>706597.34502250701</v>
@@ -3686,7 +3683,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="12">
-        <v>707438.27934149234</v>
+        <v>707558.45852418256</v>
       </c>
       <c r="D42" s="12">
         <v>671066.04663506302</v>
@@ -3700,7 +3697,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="12">
-        <v>703280.52095097885</v>
+        <v>703181.56088816281</v>
       </c>
       <c r="D43" s="12">
         <v>760576.86834800395</v>
@@ -3714,7 +3711,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="12">
-        <v>697512.66703546315</v>
+        <v>697574.98650736373</v>
       </c>
       <c r="D44" s="12">
         <v>690879.79825168301</v>
@@ -3728,7 +3725,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="12">
-        <v>700992.71652552695</v>
+        <v>700909.1779337523</v>
       </c>
       <c r="D45" s="12">
         <v>686701.47061871097</v>
@@ -3742,7 +3739,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="12">
-        <v>711244.85257803032</v>
+        <v>711343.55056484032</v>
       </c>
       <c r="D46" s="12">
         <v>672749.81139169901</v>
@@ -3756,7 +3753,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="12">
-        <v>727974.81740948593</v>
+        <v>728061.55982454459</v>
       </c>
       <c r="D47" s="12">
         <v>791235.96554166998</v>
@@ -3770,7 +3767,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="12">
-        <v>727441.72813885717</v>
+        <v>727465.84170856164</v>
       </c>
       <c r="D48" s="12">
         <v>718281.26544978202</v>
@@ -3784,7 +3781,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="12">
-        <v>719287.18842578714</v>
+        <v>719077.63445421401</v>
       </c>
       <c r="D49" s="12">
         <v>703681.54416900803</v>
@@ -3798,12 +3795,12 @@
         <v>29</v>
       </c>
       <c r="C50" s="12">
-        <v>712656.1058424965</v>
+        <v>712792.50733871781</v>
       </c>
       <c r="D50" s="12">
         <v>677652.08911570301</v>
       </c>
-      <c r="H50" s="55"/>
+      <c r="H50" s="32"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
@@ -3813,12 +3810,12 @@
         <v>30</v>
       </c>
       <c r="C51" s="12">
-        <v>701431.61607410666</v>
+        <v>701694.24333017843</v>
       </c>
       <c r="D51" s="12">
         <v>760703.28015165601</v>
       </c>
-      <c r="H51" s="55"/>
+      <c r="H51" s="32"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
@@ -3828,12 +3825,12 @@
         <v>31</v>
       </c>
       <c r="C52" s="12">
-        <v>703614.60301765869</v>
+        <v>703628.70200198307</v>
       </c>
       <c r="D52" s="12">
         <v>694382.47577623103</v>
       </c>
-      <c r="H52" s="55"/>
+      <c r="H52" s="32"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
@@ -3843,12 +3840,12 @@
         <v>32</v>
       </c>
       <c r="C53" s="12">
-        <v>708209.06945638417</v>
+        <v>707795.94171976787</v>
       </c>
       <c r="D53" s="12">
         <v>693173.54934705805</v>
       </c>
-      <c r="H53" s="55"/>
+      <c r="H53" s="32"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
@@ -3858,12 +3855,12 @@
         <v>29</v>
       </c>
       <c r="C54" s="12">
-        <v>714382.42875967419</v>
+        <v>714635.17781266733</v>
       </c>
       <c r="D54" s="12">
         <v>681444.76611022197</v>
       </c>
-      <c r="H54" s="55"/>
+      <c r="H54" s="32"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
@@ -3873,12 +3870,12 @@
         <v>30</v>
       </c>
       <c r="C55" s="12">
-        <v>721803.28483693185</v>
+        <v>722379.15414712264</v>
       </c>
       <c r="D55" s="12">
         <v>778401.67644931702</v>
       </c>
-      <c r="H55" s="55"/>
+      <c r="H55" s="32"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
@@ -3888,12 +3885,12 @@
         <v>31</v>
       </c>
       <c r="C56" s="12">
-        <v>730647.41174930311</v>
+        <v>730527.41861531767</v>
       </c>
       <c r="D56" s="12">
         <v>721120.42685279401</v>
       </c>
-      <c r="H56" s="55"/>
+      <c r="H56" s="32"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
@@ -3903,12 +3900,12 @@
         <v>32</v>
       </c>
       <c r="C57" s="12">
-        <v>738726.66570538515</v>
+        <v>738018.04047618899</v>
       </c>
       <c r="D57" s="12">
         <v>724592.92163896305</v>
       </c>
-      <c r="H57" s="55"/>
+      <c r="H57" s="32"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
@@ -3918,12 +3915,12 @@
         <v>29</v>
       </c>
       <c r="C58" s="12">
-        <v>735865.95958180574</v>
+        <v>736289.24838678283</v>
       </c>
       <c r="D58" s="12">
         <v>707324.26805721398</v>
       </c>
-      <c r="H58" s="55"/>
+      <c r="H58" s="32"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
@@ -3933,12 +3930,12 @@
         <v>30</v>
       </c>
       <c r="C59" s="12">
-        <v>701416.87787687394</v>
+        <v>702642.23655074975</v>
       </c>
       <c r="D59" s="12">
         <v>747428.29995457502</v>
       </c>
-      <c r="H59" s="55"/>
+      <c r="H59" s="32"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
@@ -3948,12 +3945,12 @@
         <v>31</v>
       </c>
       <c r="C60" s="12">
-        <v>700700.91527981544</v>
+        <v>700254.09096364852</v>
       </c>
       <c r="D60" s="12">
         <v>696101.58352180803</v>
       </c>
-      <c r="H60" s="55"/>
+      <c r="H60" s="32"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -3963,12 +3960,12 @@
         <v>32</v>
       </c>
       <c r="C61" s="12">
-        <v>691526.01917955582</v>
+        <v>690324.19601686858</v>
       </c>
       <c r="D61" s="12">
         <v>678655.62038445403</v>
       </c>
-      <c r="H61" s="55"/>
+      <c r="H61" s="32"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
@@ -3978,12 +3975,12 @@
         <v>29</v>
       </c>
       <c r="C62" s="12">
-        <v>691325.42465344083</v>
+        <v>692058.14479226689</v>
       </c>
       <c r="D62" s="12">
         <v>665690.59065187594</v>
       </c>
-      <c r="H62" s="55"/>
+      <c r="H62" s="32"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
@@ -3993,12 +3990,12 @@
         <v>30</v>
       </c>
       <c r="C63" s="12">
-        <v>694370.61904841068</v>
+        <v>696592.48711725208</v>
       </c>
       <c r="D63" s="12">
         <v>751765.13811138296</v>
       </c>
-      <c r="H63" s="55"/>
+      <c r="H63" s="32"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
@@ -4008,12 +4005,12 @@
         <v>31</v>
       </c>
       <c r="C64" s="12">
-        <v>698890.77807771834</v>
+        <v>697682.90181394049</v>
       </c>
       <c r="D64" s="12">
         <v>683911.44245860004</v>
       </c>
-      <c r="H64" s="55"/>
+      <c r="H64" s="32"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
@@ -4023,12 +4020,12 @@
         <v>32</v>
       </c>
       <c r="C65" s="12">
-        <v>687598.9430437478</v>
+        <v>685852.2310998576</v>
       </c>
       <c r="D65" s="11">
         <v>670818.59360145801</v>
       </c>
-      <c r="H65" s="55"/>
+      <c r="H65" s="32"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
@@ -4038,12 +4035,12 @@
         <v>29</v>
       </c>
       <c r="C66" s="11">
-        <v>657901.84368946217</v>
+        <v>658858.00489083584</v>
       </c>
       <c r="D66" s="11">
         <v>632469.10245408595</v>
       </c>
-      <c r="H66" s="55"/>
+      <c r="H66" s="32"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
@@ -4053,12 +4050,12 @@
         <v>30</v>
       </c>
       <c r="C67" s="11">
-        <v>556121.19007352495</v>
+        <v>559239.1902047121</v>
       </c>
       <c r="D67" s="11">
         <v>608823.50379551796</v>
       </c>
-      <c r="H67" s="55"/>
+      <c r="H67" s="32"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
@@ -4068,12 +4065,12 @@
         <v>31</v>
       </c>
       <c r="C68" s="11">
-        <v>627739.31787237676</v>
+        <v>625831.78875105421</v>
       </c>
       <c r="D68" s="11">
         <v>614416.20615719398</v>
       </c>
-      <c r="H68" s="55"/>
+      <c r="H68" s="32"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
@@ -4083,12 +4080,12 @@
         <v>32</v>
       </c>
       <c r="C69" s="11">
-        <v>656108.17757241661</v>
+        <v>653941.54519373132</v>
       </c>
       <c r="D69" s="11">
         <v>642161.71494925604</v>
       </c>
-      <c r="H69" s="55"/>
+      <c r="H69" s="32"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
@@ -4098,12 +4095,12 @@
         <v>29</v>
       </c>
       <c r="C70" s="11">
-        <v>674394.71622935636</v>
+        <v>675578.64671226148</v>
       </c>
       <c r="D70">
         <v>650821.34239924757</v>
       </c>
-      <c r="H70" s="55"/>
+      <c r="H70" s="32"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
@@ -4113,12 +4110,26 @@
         <v>30</v>
       </c>
       <c r="C71" s="11">
-        <v>665002.5579772027</v>
+        <v>669236.91863885184</v>
       </c>
       <c r="D71">
-        <v>717953.19096117874</v>
-      </c>
-      <c r="H71" s="55"/>
+        <v>717967.93370259111</v>
+      </c>
+      <c r="H71" s="32"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="11">
+        <v>2021</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="11">
+        <v>696523.61811405595</v>
+      </c>
+      <c r="D72" s="11">
+        <v>687344.44412307488</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4143,14 +4154,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="61"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4170,16 +4181,16 @@
       <c r="A3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="33">
         <v>31.2</v>
       </c>
-      <c r="C3" s="56">
+      <c r="C3" s="33">
         <v>40.6</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="33">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="33">
         <v>10.7</v>
       </c>
     </row>
@@ -4187,16 +4198,16 @@
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="33">
         <v>10.1</v>
       </c>
-      <c r="C4" s="56">
+      <c r="C4" s="33">
         <v>13.9</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="33">
         <v>1.9</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="33">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -4204,16 +4215,16 @@
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="33">
         <v>37.1</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="33">
         <v>45.3</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="33">
         <v>11.2</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="33">
         <v>13.8</v>
       </c>
     </row>
@@ -4221,16 +4232,16 @@
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="33">
         <v>33.200000000000003</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="33">
         <v>43.7</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="33">
         <v>5.3</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="33">
         <v>6.9</v>
       </c>
     </row>
@@ -4238,16 +4249,16 @@
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="33">
         <v>28.2</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="33">
         <v>36.200000000000003</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="33">
         <v>4.5</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="33">
         <v>6.3</v>
       </c>
     </row>
@@ -4255,16 +4266,16 @@
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="56">
+      <c r="B8" s="33">
         <v>36</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="33">
         <v>44.3</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="33">
         <v>4.2</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="33">
         <v>4.7</v>
       </c>
     </row>
@@ -4272,16 +4283,16 @@
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="33">
         <v>32.9</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="33">
         <v>43</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="33">
         <v>6.9</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="33">
         <v>9.1</v>
       </c>
     </row>
@@ -4289,16 +4300,16 @@
       <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="33">
         <v>37.9</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="33">
         <v>47.4</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="33">
         <v>11.6</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="33">
         <v>15</v>
       </c>
     </row>
@@ -4306,16 +4317,16 @@
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="56">
+      <c r="B11" s="33">
         <v>44.6</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="34">
         <v>51.9</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="33">
         <v>13.3</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="33">
         <v>16.899999999999999</v>
       </c>
     </row>
@@ -4323,16 +4334,16 @@
       <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="56">
+      <c r="B12" s="33">
         <v>30</v>
       </c>
-      <c r="C12" s="56">
+      <c r="C12" s="33">
         <v>39.4</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="33">
         <v>4.7</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="33">
         <v>6.5</v>
       </c>
     </row>
@@ -4340,16 +4351,16 @@
       <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="56">
+      <c r="B13" s="33">
         <v>37.1</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="33">
         <v>46</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="33">
         <v>8</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="33">
         <v>10</v>
       </c>
     </row>
@@ -4357,16 +4368,16 @@
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="56">
+      <c r="B14" s="33">
         <v>36.200000000000003</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="33">
         <v>46.2</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="33">
         <v>9.6</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E14" s="33">
         <v>11.6</v>
       </c>
     </row>
@@ -4374,16 +4385,16 @@
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="56">
+      <c r="B15" s="33">
         <v>33.4</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="33">
         <v>42.5</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="33">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E15" s="56">
+      <c r="E15" s="33">
         <v>5.7</v>
       </c>
     </row>
@@ -4391,16 +4402,16 @@
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="56">
+      <c r="B16" s="33">
         <v>26.7</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="33">
         <v>37.799999999999997</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="33">
         <v>3.1</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="33">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -4408,16 +4419,16 @@
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="33">
         <v>33.9</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="33">
         <v>42.3</v>
       </c>
-      <c r="D17" s="56">
+      <c r="D17" s="33">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E17" s="56">
+      <c r="E17" s="33">
         <v>11.2</v>
       </c>
     </row>
@@ -4425,16 +4436,16 @@
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="56">
+      <c r="B18" s="33">
         <v>38.6</v>
       </c>
-      <c r="C18" s="56">
+      <c r="C18" s="33">
         <v>50.2</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="33">
         <v>4.3</v>
       </c>
-      <c r="E18" s="56">
+      <c r="E18" s="33">
         <v>6.1</v>
       </c>
     </row>
@@ -4442,16 +4453,16 @@
       <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="56">
+      <c r="B19" s="33">
         <v>23.1</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="33">
         <v>31.7</v>
       </c>
-      <c r="D19" s="56">
+      <c r="D19" s="33">
         <v>5.2</v>
       </c>
-      <c r="E19" s="56">
+      <c r="E19" s="33">
         <v>7.7</v>
       </c>
     </row>
@@ -4459,16 +4470,16 @@
       <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="56">
+      <c r="B20" s="33">
         <v>44.4</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="33">
         <v>56.1</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="33">
         <v>11</v>
       </c>
-      <c r="E20" s="56">
+      <c r="E20" s="33">
         <v>15.8</v>
       </c>
     </row>
@@ -4476,16 +4487,16 @@
       <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="56">
+      <c r="B21" s="33">
         <v>34.299999999999997</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="33">
         <v>46.6</v>
       </c>
-      <c r="D21" s="56">
+      <c r="D21" s="33">
         <v>7.8</v>
       </c>
-      <c r="E21" s="56">
+      <c r="E21" s="33">
         <v>10.8</v>
       </c>
     </row>
@@ -4493,16 +4504,16 @@
       <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="56">
+      <c r="B22" s="33">
         <v>30.9</v>
       </c>
-      <c r="C22" s="56">
+      <c r="C22" s="33">
         <v>41.5</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="33">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E22" s="56">
+      <c r="E22" s="33">
         <v>13.5</v>
       </c>
     </row>
@@ -4510,16 +4521,16 @@
       <c r="A23" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="56">
+      <c r="B23" s="33">
         <v>28.3</v>
       </c>
-      <c r="C23" s="56">
+      <c r="C23" s="33">
         <v>39.4</v>
       </c>
-      <c r="D23" s="56">
+      <c r="D23" s="33">
         <v>7.9</v>
       </c>
-      <c r="E23" s="56">
+      <c r="E23" s="33">
         <v>10.6</v>
       </c>
     </row>
@@ -4527,16 +4538,16 @@
       <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="56">
+      <c r="B24" s="33">
         <v>27.8</v>
       </c>
-      <c r="C24" s="56">
+      <c r="C24" s="33">
         <v>37</v>
       </c>
-      <c r="D24" s="56">
+      <c r="D24" s="33">
         <v>6.1</v>
       </c>
-      <c r="E24" s="56">
+      <c r="E24" s="33">
         <v>8.5</v>
       </c>
     </row>
@@ -4544,16 +4555,16 @@
       <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="56">
+      <c r="B25" s="33">
         <v>36.799999999999997</v>
       </c>
-      <c r="C25" s="56">
+      <c r="C25" s="33">
         <v>50.5</v>
       </c>
-      <c r="D25" s="56">
+      <c r="D25" s="33">
         <v>7.2</v>
       </c>
-      <c r="E25" s="56">
+      <c r="E25" s="33">
         <v>10.4</v>
       </c>
     </row>
@@ -4561,16 +4572,16 @@
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="56">
+      <c r="B26" s="33">
         <v>27.2</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="33">
         <v>35</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="33">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E26" s="33">
         <v>13.2</v>
       </c>
     </row>
@@ -4578,16 +4589,16 @@
       <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="56">
+      <c r="B27" s="33">
         <v>29.7</v>
       </c>
-      <c r="C27" s="56">
+      <c r="C27" s="33">
         <v>38.799999999999997</v>
       </c>
-      <c r="D27" s="56">
+      <c r="D27" s="33">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E27" s="56">
+      <c r="E27" s="33">
         <v>6.2</v>
       </c>
     </row>
@@ -4595,16 +4606,16 @@
       <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="56">
+      <c r="B28" s="33">
         <v>25.8</v>
       </c>
-      <c r="C28" s="56">
+      <c r="C28" s="33">
         <v>36.799999999999997</v>
       </c>
-      <c r="D28" s="56">
+      <c r="D28" s="33">
         <v>7.2</v>
       </c>
-      <c r="E28" s="56">
+      <c r="E28" s="33">
         <v>9.6</v>
       </c>
     </row>
@@ -4612,16 +4623,16 @@
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="56">
+      <c r="B29" s="33">
         <v>35.299999999999997</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="33">
         <v>47.1</v>
       </c>
-      <c r="D29" s="56">
+      <c r="D29" s="33">
         <v>8.5</v>
       </c>
-      <c r="E29" s="56">
+      <c r="E29" s="33">
         <v>11.2</v>
       </c>
     </row>
@@ -4629,16 +4640,16 @@
       <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="56">
+      <c r="B30" s="33">
         <v>18.7</v>
       </c>
-      <c r="C30" s="56">
+      <c r="C30" s="33">
         <v>23.9</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="33">
         <v>2.8</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30" s="33">
         <v>2.9</v>
       </c>
     </row>
@@ -4646,16 +4657,16 @@
       <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="56">
+      <c r="B31" s="33">
         <v>32.299999999999997</v>
       </c>
-      <c r="C31" s="56">
+      <c r="C31" s="33">
         <v>41</v>
       </c>
-      <c r="D31" s="56">
+      <c r="D31" s="33">
         <v>7.5</v>
       </c>
-      <c r="E31" s="56">
+      <c r="E31" s="33">
         <v>9.8000000000000007</v>
       </c>
     </row>
@@ -4663,16 +4674,16 @@
       <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="56">
+      <c r="B32" s="33">
         <v>25.9</v>
       </c>
-      <c r="C32" s="56">
+      <c r="C32" s="33">
         <v>34.700000000000003</v>
       </c>
-      <c r="D32" s="56">
+      <c r="D32" s="33">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E32" s="56">
+      <c r="E32" s="33">
         <v>5.4</v>
       </c>
     </row>
@@ -4680,16 +4691,16 @@
       <c r="A33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="56">
+      <c r="B33" s="33">
         <v>27.4</v>
       </c>
-      <c r="C33" s="56">
+      <c r="C33" s="33">
         <v>36</v>
       </c>
-      <c r="D33" s="56">
+      <c r="D33" s="33">
         <v>3.3</v>
       </c>
-      <c r="E33" s="56">
+      <c r="E33" s="33">
         <v>4.2</v>
       </c>
     </row>
@@ -4697,16 +4708,16 @@
       <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="56">
+      <c r="B34" s="33">
         <v>26.2</v>
       </c>
-      <c r="C34" s="56">
+      <c r="C34" s="33">
         <v>35.299999999999997</v>
       </c>
-      <c r="D34" s="56">
+      <c r="D34" s="33">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E34" s="56">
+      <c r="E34" s="33">
         <v>5.5</v>
       </c>
     </row>
@@ -4714,16 +4725,16 @@
       <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="56">
+      <c r="B35" s="33">
         <v>25</v>
       </c>
-      <c r="C35" s="56">
+      <c r="C35" s="33">
         <v>34.799999999999997</v>
       </c>
-      <c r="D35" s="56">
+      <c r="D35" s="33">
         <v>3.6</v>
       </c>
-      <c r="E35" s="56">
+      <c r="E35" s="33">
         <v>4.8</v>
       </c>
     </row>
@@ -4754,14 +4765,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="61"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4781,16 +4792,16 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="33">
         <v>31.2</v>
       </c>
-      <c r="C3" s="56">
+      <c r="C3" s="33">
         <v>40.6</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="33">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="33">
         <v>10.7</v>
       </c>
     </row>
@@ -4798,16 +4809,16 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="33">
         <v>32.200000000000003</v>
       </c>
-      <c r="C4" s="56">
+      <c r="C4" s="33">
         <v>41.5</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="33">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="33">
         <v>6.4</v>
       </c>
     </row>
@@ -4815,16 +4826,16 @@
       <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="33">
         <v>30.5</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="33">
         <v>39.200000000000003</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="33">
         <v>8.9</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="33">
         <v>11.5</v>
       </c>
     </row>
@@ -4832,16 +4843,16 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="33">
         <v>36.299999999999997</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="33">
         <v>45.4</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="33">
         <v>8.9</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="33">
         <v>11.7</v>
       </c>
     </row>
@@ -4849,16 +4860,16 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="33">
         <v>35</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="33">
         <v>44.7</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="33">
         <v>7.3</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="33">
         <v>9.1999999999999993</v>
       </c>
     </row>
@@ -4866,16 +4877,16 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="56">
+      <c r="B8" s="33">
         <v>31</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="33">
         <v>42.1</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="33">
         <v>8</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="33">
         <v>11.1</v>
       </c>
     </row>
@@ -4883,16 +4894,16 @@
       <c r="A9" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="33">
         <v>26.3</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="33">
         <v>34.4</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="33">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="33">
         <v>5.9</v>
       </c>
     </row>
@@ -4910,7 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
@@ -4937,10 +4948,10 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="35">
         <v>11799</v>
       </c>
-      <c r="C2" s="58">
+      <c r="C2" s="35">
         <v>13165</v>
       </c>
       <c r="D2">
@@ -4952,7 +4963,7 @@
       <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="35">
         <v>3279</v>
       </c>
       <c r="C3">
@@ -4967,10 +4978,10 @@
       <c r="A4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="35">
         <v>3714</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="35">
         <v>1583</v>
       </c>
       <c r="D4">
@@ -4997,10 +5008,10 @@
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="35">
         <v>5176</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="35">
         <v>6269</v>
       </c>
       <c r="D6">
@@ -5012,10 +5023,10 @@
       <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="35">
         <v>8497</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="35">
         <v>7509</v>
       </c>
       <c r="D7">
@@ -5072,10 +5083,10 @@
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="35">
         <v>6313</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="35">
         <v>3164</v>
       </c>
       <c r="D11">
@@ -5087,10 +5098,10 @@
       <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="35">
         <v>5621</v>
       </c>
-      <c r="C12" s="58">
+      <c r="C12" s="35">
         <v>10847</v>
       </c>
       <c r="D12">
@@ -5102,7 +5113,7 @@
       <c r="A13" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="58">
+      <c r="B13" s="35">
         <v>1477</v>
       </c>
       <c r="C13">
@@ -5132,10 +5143,10 @@
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="58">
+      <c r="B15" s="35">
         <v>3350</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="35">
         <v>1165</v>
       </c>
       <c r="D15">
@@ -5147,10 +5158,10 @@
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="58">
+      <c r="B16" s="35">
         <v>4017</v>
       </c>
-      <c r="C16" s="58">
+      <c r="C16" s="35">
         <v>1181</v>
       </c>
       <c r="D16">
@@ -5162,7 +5173,7 @@
       <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="58">
+      <c r="B17" s="35">
         <v>3507</v>
       </c>
       <c r="C17">
@@ -5207,10 +5218,10 @@
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="58">
+      <c r="B20" s="35">
         <v>3669</v>
       </c>
-      <c r="C20" s="58">
+      <c r="C20" s="35">
         <v>1557</v>
       </c>
       <c r="D20">
@@ -5229,7 +5240,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5254,10 +5265,10 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>604046.13319735427</v>
+        <v>569629.40890678659</v>
       </c>
       <c r="C2">
-        <v>17.580319315972215</v>
+        <v>11.397276043853299</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5265,10 +5276,10 @@
         <v>102</v>
       </c>
       <c r="B3">
-        <v>89195.223928980049</v>
+        <v>34778.948230747541</v>
       </c>
       <c r="C3">
-        <v>-3.9179249324300724</v>
+        <v>-0.84794445835578713</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5276,10 +5287,10 @@
         <v>103</v>
       </c>
       <c r="B4">
-        <v>2258.9045828297758</v>
+        <v>3738.9140914018044</v>
       </c>
       <c r="C4">
-        <v>28.191552714517655</v>
+        <v>34.730552426653084</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5287,10 +5298,10 @@
         <v>104</v>
       </c>
       <c r="B5">
-        <v>20269.949560862842</v>
+        <v>21713.233857963307</v>
       </c>
       <c r="C5">
-        <v>13.946668684529229</v>
+        <v>13.145985625751354</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5298,10 +5309,10 @@
         <v>105</v>
       </c>
       <c r="B6">
-        <v>115618.73755326691</v>
+        <v>119933.99121636405</v>
       </c>
       <c r="C6">
-        <v>32.403170628583446</v>
+        <v>12.728493869734736</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5309,10 +5320,10 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <v>12736.597747150905</v>
+        <v>13395.50707056335</v>
       </c>
       <c r="C7">
-        <v>10.913053342572132</v>
+        <v>5.6213435666422562</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5320,10 +5331,10 @@
         <v>107</v>
       </c>
       <c r="B8">
-        <v>19532.524594231447</v>
+        <v>21715.967786364865</v>
       </c>
       <c r="C8">
-        <v>84.176585776301465</v>
+        <v>25.185695615024596</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5331,10 +5342,10 @@
         <v>108</v>
       </c>
       <c r="B9">
-        <v>89303.5485018787</v>
+        <v>91487.844850292531</v>
       </c>
       <c r="C9">
-        <v>25.992692468317948</v>
+        <v>11.072848471409035</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5342,10 +5353,10 @@
         <v>109</v>
       </c>
       <c r="B10">
-        <v>5517.1767351843646</v>
+        <v>7166.7167614790624</v>
       </c>
       <c r="C10">
-        <v>90.340020564698875</v>
+        <v>59.782555864799988</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5353,10 +5364,10 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>52694.386166101496</v>
+        <v>49992.374065828524</v>
       </c>
       <c r="C11">
-        <v>14.485678244064705</v>
+        <v>11.704739911297812</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5364,10 +5375,10 @@
         <v>111</v>
       </c>
       <c r="B12">
-        <v>24702.765148763236</v>
+        <v>25371.087569978205</v>
       </c>
       <c r="C12">
-        <v>0.79059187589880509</v>
+        <v>-7.6663383227870696E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5375,10 +5386,10 @@
         <v>112</v>
       </c>
       <c r="B13">
-        <v>75509.308936562651</v>
+        <v>77129.369084939375</v>
       </c>
       <c r="C13">
-        <v>16.138468063927359</v>
+        <v>8.7616924421587861</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5386,10 +5397,10 @@
         <v>113</v>
       </c>
       <c r="B14">
-        <v>31940.377494155731</v>
+        <v>32777.443981278891</v>
       </c>
       <c r="C14">
-        <v>8.5495978626258573</v>
+        <v>8.0276619288576647</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5397,10 +5408,10 @@
         <v>114</v>
       </c>
       <c r="B15">
-        <v>26696.736156349034</v>
+        <v>27683.57840795505</v>
       </c>
       <c r="C15">
-        <v>6.3610364323609669</v>
+        <v>5.1249743402094428</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5408,10 +5419,10 @@
         <v>115</v>
       </c>
       <c r="B16">
-        <v>22164.329459385022</v>
+        <v>24083.290055386617</v>
       </c>
       <c r="C16">
-        <v>13.625244325168806</v>
+        <v>10.707868644455832</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5419,10 +5430,10 @@
         <v>116</v>
       </c>
       <c r="B17">
-        <v>12520.75700054313</v>
+        <v>14855.887112915314</v>
       </c>
       <c r="C17">
-        <v>113.75818667164168</v>
+        <v>80.989403402298592</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5430,10 +5441,10 @@
         <v>117</v>
       </c>
       <c r="B18">
-        <v>3384.8096311087297</v>
+        <v>3805.2547633282738</v>
       </c>
       <c r="C18">
-        <v>24.658035265591938</v>
+        <v>13.50127591153154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo con dash con dato fiscal de nov, emae e ica"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A4E659-9CA1-4383-A0B2-ED7D85B93545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5480ACE0-D614-45E5-AF43-48C5D397A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -2053,7 +2053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -4921,7 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
@@ -4949,14 +4949,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="35">
-        <v>11799</v>
+        <v>13274</v>
       </c>
       <c r="C2" s="35">
-        <v>13165</v>
+        <v>14537</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1366</v>
+        <v>-1263</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4964,14 +4964,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="35">
-        <v>3279</v>
+        <v>3728</v>
       </c>
       <c r="C3">
-        <v>551</v>
+        <v>627</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>2728</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,14 +4979,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="35">
-        <v>3714</v>
+        <v>4069</v>
       </c>
       <c r="C4" s="35">
-        <v>1583</v>
+        <v>1745</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>2131</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4994,14 +4994,14 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>864</v>
+        <v>938</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>844</v>
+        <v>912</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5009,14 +5009,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="35">
-        <v>5176</v>
+        <v>5649</v>
       </c>
       <c r="C6" s="35">
-        <v>6269</v>
+        <v>6982</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-1093</v>
+        <v>-1333</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5024,14 +5024,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="35">
-        <v>8497</v>
+        <v>9170</v>
       </c>
       <c r="C7" s="35">
-        <v>7509</v>
+        <v>8470</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>988</v>
+        <v>700</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5039,14 +5039,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>678</v>
+        <v>715</v>
       </c>
       <c r="C8">
-        <v>435</v>
+        <v>481</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5054,14 +5054,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>800</v>
+        <v>881</v>
       </c>
       <c r="C9">
-        <v>436</v>
+        <v>488</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>364</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5069,14 +5069,14 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>699</v>
+        <v>769</v>
       </c>
       <c r="C10">
-        <v>609</v>
+        <v>661</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5084,14 +5084,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="35">
-        <v>6313</v>
+        <v>6786</v>
       </c>
       <c r="C11" s="35">
-        <v>3164</v>
+        <v>3490</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>3149</v>
+        <v>3296</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5099,14 +5099,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="35">
-        <v>5621</v>
+        <v>5923</v>
       </c>
       <c r="C12" s="35">
-        <v>10847</v>
+        <v>12001</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-5226</v>
+        <v>-6078</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5114,14 +5114,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="35">
-        <v>1477</v>
+        <v>1599</v>
       </c>
       <c r="C13">
-        <v>509</v>
+        <v>551</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>968</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5129,14 +5129,14 @@
         <v>91</v>
       </c>
       <c r="B14">
-        <v>638</v>
+        <v>686</v>
       </c>
       <c r="C14">
-        <v>952</v>
+        <v>1030</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-314</v>
+        <v>-344</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5144,14 +5144,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="35">
-        <v>3350</v>
+        <v>3808</v>
       </c>
       <c r="C15" s="35">
-        <v>1165</v>
+        <v>1281</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>2185</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5159,14 +5159,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="35">
-        <v>4017</v>
+        <v>4286</v>
       </c>
       <c r="C16" s="35">
-        <v>1181</v>
+        <v>1352</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>2836</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5174,14 +5174,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="35">
-        <v>3507</v>
+        <v>3795</v>
       </c>
       <c r="C17">
-        <v>797</v>
+        <v>931</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2710</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,14 +5189,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>380</v>
+        <v>429</v>
       </c>
       <c r="C18">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5204,14 +5204,14 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>663</v>
+        <v>741</v>
       </c>
       <c r="C19">
-        <v>273</v>
+        <v>355</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5219,14 +5219,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="35">
-        <v>3669</v>
+        <v>4074</v>
       </c>
       <c r="C20" s="35">
-        <v>1557</v>
+        <v>1768</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2112</v>
+        <v>2306</v>
       </c>
     </row>
   </sheetData>
@@ -5455,10 +5455,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5490,10 +5490,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="23">
-        <v>148.10165754695203</v>
+        <v>148.11468627419526</v>
       </c>
       <c r="D2" s="23">
-        <v>147.06011385125024</v>
+        <v>147.04614189145943</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5504,10 +5504,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="23">
-        <v>146.70606708828808</v>
+        <v>146.71239442947743</v>
       </c>
       <c r="D3" s="23">
-        <v>146.47796325278543</v>
+        <v>146.45682364061994</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5518,10 +5518,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="23">
-        <v>145.97990354527658</v>
+        <v>145.97080470504969</v>
       </c>
       <c r="D4" s="23">
-        <v>145.93317341480011</v>
+        <v>145.90492803881389</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5532,10 +5532,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="23">
-        <v>145.19152497659766</v>
+        <v>145.23663533073415</v>
       </c>
       <c r="D5" s="23">
-        <v>145.46083293448183</v>
+        <v>145.42639659456469</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5546,10 +5546,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="23">
-        <v>144.39688540541056</v>
+        <v>144.38767838671734</v>
       </c>
       <c r="D6" s="23">
-        <v>145.08724802832404</v>
+        <v>145.0485921415171</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5560,10 +5560,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="23">
-        <v>144.31933374439532</v>
+        <v>144.31029625514628</v>
       </c>
       <c r="D7" s="23">
-        <v>144.83289463227342</v>
+        <v>144.79332228946944</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5574,10 +5574,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="23">
-        <v>144.38093157487899</v>
+        <v>144.40504668581195</v>
       </c>
       <c r="D8" s="23">
-        <v>144.70704419514331</v>
+        <v>144.66963882606851</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5588,10 +5588,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="23">
-        <v>145.62629617134974</v>
+        <v>145.62451440768521</v>
       </c>
       <c r="D9" s="23">
-        <v>144.7123284518546</v>
+        <v>144.67961844005512</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5602,10 +5602,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="23">
-        <v>145.11930463967713</v>
+        <v>145.10133711608714</v>
       </c>
       <c r="D10" s="23">
-        <v>144.84522772583608</v>
+        <v>144.81979014966413</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5616,10 +5616,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="23">
-        <v>145.01481318918368</v>
+        <v>145.01637151220993</v>
       </c>
       <c r="D11" s="23">
-        <v>145.09658500101486</v>
+        <v>145.08032811462269</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5630,10 +5630,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="23">
-        <v>145.72308843409533</v>
+        <v>145.71569599298695</v>
       </c>
       <c r="D12" s="23">
-        <v>145.45178504726957</v>
+        <v>145.44518918718296</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5644,10 +5644,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="23">
-        <v>147.01154744364237</v>
+        <v>146.97589266376272</v>
       </c>
       <c r="D13" s="23">
-        <v>145.89864030121484</v>
+        <v>145.90045730320412</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5655,13 +5655,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="23">
-        <v>136.63265948871918</v>
+        <v>136.63265948871924</v>
       </c>
       <c r="C14" s="23">
-        <v>147.42211146867183</v>
+        <v>147.4177168199553</v>
       </c>
       <c r="D14" s="23">
-        <v>146.42194598217245</v>
+        <v>146.42945107242025</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5672,10 +5672,10 @@
         <v>132.15851634216514</v>
       </c>
       <c r="C15" s="23">
-        <v>146.52134192135418</v>
+        <v>146.53817112073898</v>
       </c>
       <c r="D15" s="23">
-        <v>147.00567489805485</v>
+        <v>147.01530661961766</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5683,13 +5683,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="23">
-        <v>152.62095855115714</v>
+        <v>152.62095855115712</v>
       </c>
       <c r="C16" s="23">
-        <v>147.92282798543368</v>
+        <v>147.98152298219952</v>
       </c>
       <c r="D16" s="23">
-        <v>147.63148434385997</v>
+        <v>147.63968585720585</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5697,13 +5697,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="23">
-        <v>151.94634477931677</v>
+        <v>151.94634477931669</v>
       </c>
       <c r="C17" s="23">
-        <v>147.71660613346299</v>
+        <v>147.74908531298937</v>
       </c>
       <c r="D17" s="23">
-        <v>148.27744686517678</v>
+        <v>148.28140654991836</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5711,13 +5711,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="23">
-        <v>168.38920945875736</v>
+        <v>168.38920945875734</v>
       </c>
       <c r="C18" s="23">
-        <v>148.66749690188567</v>
+        <v>148.69109529911194</v>
       </c>
       <c r="D18" s="23">
-        <v>148.91619756849141</v>
+        <v>148.91418653877889</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5725,13 +5725,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="23">
-        <v>161.03568550523272</v>
+        <v>161.03568550523281</v>
       </c>
       <c r="C19" s="23">
-        <v>150.27456340852842</v>
+        <v>150.28618131369643</v>
       </c>
       <c r="D19" s="23">
-        <v>149.51556034063185</v>
+        <v>149.50672294073226</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5739,13 +5739,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="23">
-        <v>150.30605023792174</v>
+        <v>150.30605023792208</v>
       </c>
       <c r="C20" s="23">
-        <v>150.2242120627169</v>
+        <v>150.27623096295713</v>
       </c>
       <c r="D20" s="23">
-        <v>150.04145507008428</v>
+        <v>150.0265267310433</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5753,13 +5753,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="23">
-        <v>149.25534282189673</v>
+        <v>149.25534282189685</v>
       </c>
       <c r="C21" s="23">
-        <v>150.28455103770648</v>
+        <v>150.28781585075035</v>
       </c>
       <c r="D21" s="23">
-        <v>150.45888970969398</v>
+        <v>150.43988099222108</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5767,13 +5767,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="23">
-        <v>146.38655949569588</v>
+        <v>146.38655949569539</v>
       </c>
       <c r="C22" s="23">
-        <v>151.26012541395224</v>
+        <v>151.20128186658101</v>
       </c>
       <c r="D22" s="23">
-        <v>150.73472510894828</v>
+        <v>150.71399370592346</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5781,13 +5781,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="23">
-        <v>149.38594914967547</v>
+        <v>149.38594914967399</v>
       </c>
       <c r="C23" s="23">
-        <v>151.49015645077984</v>
+        <v>151.46682461402608</v>
       </c>
       <c r="D23" s="23">
-        <v>150.84231133769393</v>
+        <v>150.82303686069662</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5795,13 +5795,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="23">
-        <v>151.92604263437173</v>
+        <v>151.9260426343711</v>
       </c>
       <c r="C24" s="23">
-        <v>152.5904784270094</v>
+        <v>152.52783357663273</v>
       </c>
       <c r="D24" s="23">
-        <v>150.75920810829331</v>
+        <v>150.74400684922901</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5809,13 +5809,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="23">
-        <v>146.78338564321811</v>
+        <v>146.78338564322021</v>
       </c>
       <c r="C25" s="23">
-        <v>152.45223310641683</v>
+        <v>152.40294459839527</v>
       </c>
       <c r="D25" s="23">
-        <v>150.47414360217039</v>
+        <v>150.46429730052779</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5823,13 +5823,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="23">
-        <v>142.74091494477966</v>
+        <v>142.7409149447864</v>
       </c>
       <c r="C26" s="23">
-        <v>152.05318910412834</v>
+        <v>152.0776402766943</v>
       </c>
       <c r="D26" s="23">
-        <v>149.99249933917798</v>
+        <v>149.98758976052559</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5837,13 +5837,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="23">
-        <v>138.81804133746257</v>
+        <v>138.81804133746542</v>
       </c>
       <c r="C27" s="23">
-        <v>151.95621824155725</v>
+        <v>152.04847193111172</v>
       </c>
       <c r="D27" s="23">
-        <v>149.33449846313019</v>
+        <v>149.33269472508505</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5851,13 +5851,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="23">
-        <v>155.85731621135642</v>
+        <v>155.8573162113469</v>
       </c>
       <c r="C28" s="23">
-        <v>151.13224640048483</v>
+        <v>151.20238857824469</v>
       </c>
       <c r="D28" s="23">
-        <v>148.5357327697711</v>
+        <v>148.534246526749</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5865,13 +5865,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="23">
-        <v>151.5245333918956</v>
+        <v>151.52453339186513</v>
       </c>
       <c r="C29" s="23">
-        <v>146.76653086171689</v>
+        <v>146.85315519317797</v>
       </c>
       <c r="D29" s="23">
-        <v>147.64353799666839</v>
+        <v>147.63940605077607</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5879,13 +5879,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="23">
-        <v>159.56668791299592</v>
+        <v>159.56668791298307</v>
       </c>
       <c r="C30" s="23">
-        <v>144.47116632154837</v>
+        <v>144.47581358456907</v>
       </c>
       <c r="D30" s="23">
-        <v>146.71224763922234</v>
+        <v>146.70327599672262</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5893,13 +5893,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="23">
-        <v>151.12577829042309</v>
+        <v>151.1257782904664</v>
       </c>
       <c r="C31" s="23">
-        <v>143.16790060128201</v>
+        <v>143.19188951074182</v>
       </c>
       <c r="D31" s="23">
-        <v>145.79671418410095</v>
+        <v>145.78178427337474</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5907,13 +5907,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="23">
-        <v>145.96357240362272</v>
+        <v>145.96357240376071</v>
       </c>
       <c r="C32" s="23">
-        <v>143.18426460201746</v>
+        <v>143.26701597792569</v>
       </c>
       <c r="D32" s="23">
-        <v>144.94574021539933</v>
+        <v>144.92455904700532</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5921,13 +5921,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="23">
-        <v>146.7659802567066</v>
+        <v>146.76598025676481</v>
       </c>
       <c r="C33" s="23">
-        <v>146.6703002941353</v>
+        <v>146.70869632361283</v>
       </c>
       <c r="D33" s="23">
-        <v>144.20277495116173</v>
+        <v>144.17751558444172</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5935,13 +5935,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="23">
-        <v>137.74650152246224</v>
+        <v>137.7465015222661</v>
       </c>
       <c r="C34" s="23">
-        <v>143.21441455276511</v>
+        <v>143.06829330681671</v>
       </c>
       <c r="D34" s="23">
-        <v>143.59765990622873</v>
+        <v>143.57222989084903</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5949,13 +5949,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="23">
-        <v>142.8430587019277</v>
+        <v>142.84305870130279</v>
       </c>
       <c r="C35" s="23">
-        <v>143.49041072556793</v>
+        <v>143.47753186062437</v>
       </c>
       <c r="D35" s="23">
-        <v>143.1462035088187</v>
+        <v>143.12442005555476</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5963,13 +5963,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="23">
-        <v>140.59231573306195</v>
+        <v>140.59231573279851</v>
       </c>
       <c r="C36" s="23">
-        <v>141.67662739598265</v>
+        <v>141.54524593768159</v>
       </c>
       <c r="D36" s="23">
-        <v>142.85070190595707</v>
+        <v>142.835557046801</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5977,13 +5977,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="23">
-        <v>136.25192484396928</v>
+        <v>136.25192484485765</v>
       </c>
       <c r="C37" s="23">
-        <v>142.01335665376354</v>
+        <v>141.8804832738669</v>
       </c>
       <c r="D37" s="23">
-        <v>142.69985501276628</v>
+        <v>142.69308118131502</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5991,13 +5991,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="23">
-        <v>134.52056074986749</v>
+        <v>134.52056075269795</v>
       </c>
       <c r="C38" s="23">
-        <v>142.95142084393885</v>
+        <v>142.96367682413009</v>
       </c>
       <c r="D38" s="23">
-        <v>142.67065930569331</v>
+        <v>142.67308077662415</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -6005,13 +6005,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="23">
-        <v>132.27529838735211</v>
+        <v>132.27529838854522</v>
       </c>
       <c r="C39" s="23">
-        <v>143.6322881851294</v>
+        <v>143.77772361577559</v>
       </c>
       <c r="D39" s="23">
-        <v>142.72862801054333</v>
+        <v>142.73794110619571</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6019,13 +6019,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="23">
-        <v>144.87373845313573</v>
+        <v>144.87373844911215</v>
       </c>
       <c r="C40" s="23">
-        <v>141.06411060855854</v>
+        <v>141.23415158052313</v>
       </c>
       <c r="D40" s="23">
-        <v>142.83384953084763</v>
+        <v>142.8466120794314</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6033,13 +6033,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="23">
-        <v>149.89913658170545</v>
+        <v>149.89913656888581</v>
       </c>
       <c r="C41" s="23">
-        <v>142.43722546826555</v>
+        <v>142.50008709181503</v>
       </c>
       <c r="D41" s="23">
-        <v>142.9443961186353</v>
+        <v>142.9574945203457</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6047,13 +6047,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="23">
-        <v>164.14987183990465</v>
+        <v>164.14987183450071</v>
       </c>
       <c r="C42" s="23">
-        <v>144.59335254098048</v>
+        <v>144.59997197751676</v>
       </c>
       <c r="D42" s="23">
-        <v>143.0214232499377</v>
+        <v>143.03323541685384</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6061,13 +6061,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="23">
-        <v>150.84993447273672</v>
+        <v>150.84993449096024</v>
       </c>
       <c r="C43" s="23">
-        <v>143.60453096039134</v>
+        <v>143.6795747673234</v>
       </c>
       <c r="D43" s="23">
-        <v>143.02765620539995</v>
+        <v>143.03876930362361</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6075,13 +6075,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="23">
-        <v>146.76823775516263</v>
+        <v>146.76823781322543</v>
       </c>
       <c r="C44" s="23">
-        <v>145.34642155952127</v>
+        <v>145.52968806471793</v>
       </c>
       <c r="D44" s="23">
-        <v>142.93253718731484</v>
+        <v>142.94703451230026</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6089,13 +6089,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="23">
-        <v>141.27943600649775</v>
+        <v>141.2794360309733</v>
       </c>
       <c r="C45" s="23">
-        <v>144.85919857411906</v>
+        <v>144.96269394054437</v>
       </c>
       <c r="D45" s="23">
-        <v>142.71317686559692</v>
+        <v>142.73729377345848</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6103,13 +6103,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="23">
-        <v>134.88987749419911</v>
+        <v>134.88987741166085</v>
       </c>
       <c r="C46" s="23">
-        <v>141.26854176407389</v>
+        <v>140.96157498654614</v>
       </c>
       <c r="D46" s="23">
-        <v>142.35717694510186</v>
+        <v>142.39820736530802</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6117,13 +6117,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="23">
-        <v>141.51078909874374</v>
+        <v>141.51078883576523</v>
       </c>
       <c r="C47" s="23">
-        <v>143.10411391687347</v>
+        <v>143.12557239727525</v>
       </c>
       <c r="D47" s="23">
-        <v>141.86476337979974</v>
+        <v>141.92907361669702</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6131,13 +6131,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="23">
-        <v>137.65812428810526</v>
+        <v>137.65812417725056</v>
       </c>
       <c r="C48" s="23">
-        <v>140.74965352561472</v>
+        <v>140.53932137060218</v>
       </c>
       <c r="D48" s="23">
-        <v>141.24653817971588</v>
+        <v>141.33925964233703</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6145,13 +6145,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="23">
-        <v>135.67189157873614</v>
+        <v>135.67189195256938</v>
       </c>
       <c r="C49" s="23">
-        <v>140.73603895881791</v>
+        <v>140.47286028963637</v>
       </c>
       <c r="D49" s="23">
-        <v>140.52913239392791</v>
+        <v>140.65221958383682</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6159,13 +6159,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="23">
-        <v>132.28222916035381</v>
+        <v>132.28223035143913</v>
       </c>
       <c r="C50" s="23">
-        <v>140.81185507990034</v>
+        <v>140.83878649488173</v>
       </c>
       <c r="D50" s="23">
-        <v>139.7463204363649</v>
+        <v>139.90293621973871</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6173,13 +6173,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="23">
-        <v>129.74514575265826</v>
+        <v>129.74514625474259</v>
       </c>
       <c r="C51" s="23">
-        <v>140.76018526334047</v>
+        <v>140.9735741346569</v>
       </c>
       <c r="D51" s="23">
-        <v>138.94108713492236</v>
+        <v>139.13272321176743</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6187,13 +6187,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="23">
-        <v>129.09772817826237</v>
+        <v>129.09772648509272</v>
       </c>
       <c r="C52" s="23">
-        <v>125.44345572143716</v>
+        <v>125.63189888549155</v>
       </c>
       <c r="D52" s="23">
-        <v>138.16077967052419</v>
+        <v>138.38589326997587</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6201,13 +6201,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="23">
-        <v>111.90396260810687</v>
+        <v>111.90395721343017</v>
       </c>
       <c r="C53" s="23">
-        <v>105.060021984369</v>
+        <v>105.11110841804673</v>
       </c>
       <c r="D53" s="23">
-        <v>137.45001399955834</v>
+        <v>137.70410820753872</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,13 +6215,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="23">
-        <v>131.29461698631593</v>
+        <v>131.29461471226998</v>
       </c>
       <c r="C54" s="23">
-        <v>116.42987037482203</v>
+        <v>116.39363841541108</v>
       </c>
       <c r="D54" s="23">
-        <v>136.8470558971776</v>
+        <v>137.12358036366476</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6229,13 +6229,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="23">
-        <v>133.30385311326845</v>
+        <v>133.30386078199106</v>
       </c>
       <c r="C55" s="23">
-        <v>124.26297064486374</v>
+        <v>124.33425952800896</v>
       </c>
       <c r="D55" s="23">
-        <v>136.380845778571</v>
+        <v>136.67255092198687</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6243,13 +6243,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="23">
-        <v>128.19076000436911</v>
+        <v>128.19078443799802</v>
       </c>
       <c r="C56" s="23">
-        <v>126.53877089646882</v>
+        <v>126.78260534625382</v>
       </c>
       <c r="D56" s="23">
-        <v>136.06982493519877</v>
+        <v>136.37012397046459</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6257,13 +6257,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="23">
-        <v>125.17404829102199</v>
+        <v>125.1740585906558</v>
       </c>
       <c r="C57" s="23">
-        <v>129.09066106950357</v>
+        <v>129.25476453920928</v>
       </c>
       <c r="D57" s="23">
-        <v>135.92414136566811</v>
+        <v>136.2259242537753</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6271,13 +6271,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="23">
-        <v>126.59620646679346</v>
+        <v>126.59617173353072</v>
       </c>
       <c r="C58" s="23">
-        <v>131.38476382450102</v>
+        <v>130.98315328612634</v>
       </c>
       <c r="D58" s="23">
-        <v>135.93985666262162</v>
+        <v>136.23979352218686</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6285,13 +6285,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="23">
-        <v>131.72758543779744</v>
+        <v>131.72747477273671</v>
       </c>
       <c r="C59" s="23">
-        <v>133.50811059480836</v>
+        <v>133.59892399962197</v>
       </c>
       <c r="D59" s="23">
-        <v>136.10800278503356</v>
+        <v>136.40369616990864</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6299,13 +6299,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="23">
-        <v>132.96981929539976</v>
+        <v>132.96977264618508</v>
       </c>
       <c r="C60" s="23">
-        <v>135.43776511823836</v>
+        <v>135.19175161980166</v>
       </c>
       <c r="D60" s="23">
-        <v>136.41659440463644</v>
+        <v>136.70289055788757</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6313,13 +6313,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="23">
-        <v>132.42170509561973</v>
+        <v>132.42186240989511</v>
       </c>
       <c r="C61" s="23">
-        <v>135.97923105517145</v>
+        <v>135.61319694446939</v>
       </c>
       <c r="D61" s="23">
-        <v>136.85254997095157</v>
+        <v>137.12038351293262</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6327,13 +6327,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="23">
-        <v>129.49189053171025</v>
+        <v>129.49239125960432</v>
       </c>
       <c r="C62" s="23">
-        <v>139.35201155899171</v>
+        <v>139.40239979552678</v>
       </c>
       <c r="D62" s="23">
-        <v>137.40121353230373</v>
+        <v>137.63561379387241</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6341,13 +6341,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="23">
-        <v>126.69345378187154</v>
+        <v>126.69366456853579</v>
       </c>
       <c r="C63" s="23">
-        <v>138.39075101551828</v>
+        <v>138.61008355763221</v>
       </c>
       <c r="D63" s="23">
-        <v>138.05015746442569</v>
+        <v>138.22313153919262</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6355,13 +6355,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="23">
-        <v>146.28896415809047</v>
+        <v>146.28825115104189</v>
       </c>
       <c r="C64" s="23">
-        <v>139.54716265632311</v>
+        <v>139.77198524330149</v>
       </c>
       <c r="D64" s="23">
-        <v>138.78993448119593</v>
+        <v>138.86107294409041</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6369,13 +6369,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="23">
-        <v>144.97246200010414</v>
+        <v>144.9074698504499</v>
       </c>
       <c r="C65" s="23">
-        <v>137.67825682421994</v>
+        <v>137.67790507256839</v>
       </c>
       <c r="D65" s="23">
-        <v>139.60825864673919</v>
+        <v>139.52551218781898</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -6383,13 +6383,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="23">
-        <v>150.19619085954542</v>
+        <v>150.14940772167688</v>
       </c>
       <c r="C66" s="23">
-        <v>136.31489355433899</v>
+        <v>136.19308287757727</v>
       </c>
       <c r="D66" s="23">
-        <v>140.48752126720049</v>
+        <v>140.19225677341413</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -6397,13 +6397,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="23">
-        <v>148.82064992180284</v>
+        <v>148.94154226537245</v>
       </c>
       <c r="C67" s="23">
-        <v>139.82633552993781</v>
+        <v>139.99169373663864</v>
       </c>
       <c r="D67" s="23">
-        <v>141.40181328922912</v>
+        <v>140.83547239155169</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -6411,13 +6411,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="23">
-        <v>143.18898687078175</v>
+        <v>143.04197497093759</v>
       </c>
       <c r="C68" s="23">
-        <v>141.79948818923302</v>
+        <v>141.828456901029</v>
       </c>
       <c r="D68" s="23">
-        <v>142.32133191397287</v>
+        <v>141.43410828512151</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -6425,27 +6425,41 @@
         <v>44409</v>
       </c>
       <c r="B69" s="23">
-        <v>141.2025348207026</v>
+        <v>141.03060228111821</v>
       </c>
       <c r="C69" s="23">
-        <v>143.84582815883468</v>
+        <v>143.82634530663671</v>
       </c>
       <c r="D69" s="23">
-        <v>143.21355123184694</v>
+        <v>141.96629857172016</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>44440</v>
       </c>
-      <c r="B70" s="24">
-        <v>141.25733334080709</v>
-      </c>
-      <c r="C70" s="24">
-        <v>145.60931096173624</v>
-      </c>
-      <c r="D70" s="24">
-        <v>144.04410694020132</v>
+      <c r="B70" s="23">
+        <v>140.98797594132151</v>
+      </c>
+      <c r="C70" s="23">
+        <v>145.08224236118642</v>
+      </c>
+      <c r="D70" s="23">
+        <v>142.41513934209877</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>44470</v>
+      </c>
+      <c r="B71" s="24">
+        <v>140.55263483141988</v>
+      </c>
+      <c r="C71" s="24">
+        <v>143.96752542309943</v>
+      </c>
+      <c r="D71" s="24">
+        <v>142.7700397487076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo con dato infal-dic21"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5480ACE0-D614-45E5-AF43-48C5D397A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F57018-D577-4BDA-A567-0CFA9635B558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
-    <sheet name="IPC-NOV-Div" sheetId="2" r:id="rId2"/>
+    <sheet name="IPC-DIC-Div" sheetId="2" r:id="rId2"/>
     <sheet name="IPC-Interanual" sheetId="3" r:id="rId3"/>
     <sheet name="Producto" sheetId="4" r:id="rId4"/>
     <sheet name="Pobreza-Aglo" sheetId="5" r:id="rId5"/>
@@ -1009,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60:E60"/>
+      <selection activeCell="C61" sqref="C61:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,6 +2043,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="36">
+        <v>44531</v>
+      </c>
+      <c r="B61" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="C61">
+        <v>3.7</v>
+      </c>
+      <c r="D61">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E61">
+        <v>1.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2053,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,25 +2110,25 @@
         <v>129</v>
       </c>
       <c r="B2" s="37">
+        <v>2.9</v>
+      </c>
+      <c r="C2" s="37">
+        <v>3.1</v>
+      </c>
+      <c r="D2" s="37">
+        <v>2.7</v>
+      </c>
+      <c r="E2" s="37">
+        <v>3.1</v>
+      </c>
+      <c r="F2" s="37">
+        <v>3.3</v>
+      </c>
+      <c r="G2" s="37">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C2" s="37">
-        <v>2</v>
-      </c>
-      <c r="D2" s="37">
-        <v>2</v>
-      </c>
-      <c r="E2" s="37">
-        <v>2.7</v>
-      </c>
-      <c r="F2" s="37">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G2" s="37">
-        <v>2.5</v>
-      </c>
       <c r="H2" s="21">
-        <v>2.2209945335743164</v>
+        <v>2.9867437146390508</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2119,25 +2136,25 @@
         <v>130</v>
       </c>
       <c r="B3" s="37">
-        <v>7.3</v>
+        <v>8.5</v>
       </c>
       <c r="C3" s="37">
-        <v>5.9</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D3" s="37">
-        <v>4.8</v>
+        <v>11.4</v>
       </c>
       <c r="E3" s="37">
-        <v>4.8</v>
+        <v>9.6</v>
       </c>
       <c r="F3" s="37">
-        <v>5.4</v>
+        <v>10.7</v>
       </c>
       <c r="G3" s="37">
-        <v>3</v>
+        <v>5.2</v>
       </c>
       <c r="H3" s="21">
-        <v>6.25328408827448</v>
+        <v>9.0991944301716856</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2145,25 +2162,25 @@
         <v>131</v>
       </c>
       <c r="B4" s="37">
-        <v>-0.6</v>
+        <v>3.3</v>
       </c>
       <c r="C4" s="37">
-        <v>0.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D4" s="37">
+        <v>1.2</v>
+      </c>
+      <c r="E4" s="37">
+        <v>1.6</v>
+      </c>
+      <c r="F4" s="37">
+        <v>2.8</v>
+      </c>
+      <c r="G4" s="37">
         <v>1.5</v>
       </c>
-      <c r="E4" s="37">
-        <v>0.7</v>
-      </c>
-      <c r="F4" s="37">
-        <v>1.2</v>
-      </c>
-      <c r="G4" s="37">
-        <v>0.3</v>
-      </c>
       <c r="H4" s="21">
-        <v>3.1641887715627703E-2</v>
+        <v>2.6199222327296878</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2171,25 +2188,25 @@
         <v>132</v>
       </c>
       <c r="B5" s="37">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="C5" s="37">
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="37">
-        <v>-0.3</v>
+        <v>1.4</v>
       </c>
       <c r="E5" s="37">
-        <v>0.9</v>
+        <v>1.6</v>
       </c>
       <c r="F5" s="37">
-        <v>0.7</v>
+        <v>2.1</v>
       </c>
       <c r="G5" s="37">
-        <v>-0.8</v>
+        <v>3</v>
       </c>
       <c r="H5" s="21">
-        <v>0.92556827125573893</v>
+        <v>1.5443996202485044</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2197,25 +2214,25 @@
         <v>133</v>
       </c>
       <c r="B6" s="37">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="C6" s="37">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
       <c r="D6" s="37">
-        <v>2.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E6" s="37">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="F6" s="37">
-        <v>4.5999999999999996</v>
+        <v>3.9</v>
       </c>
       <c r="G6" s="37">
-        <v>4.4000000000000004</v>
+        <v>1.7</v>
       </c>
       <c r="H6" s="21">
-        <v>2.4536942395441352</v>
+        <v>1.6909946166384193</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2223,25 +2240,25 @@
         <v>134</v>
       </c>
       <c r="B7" s="37">
-        <v>-11.8</v>
+        <v>-5.9</v>
       </c>
       <c r="C7" s="37">
-        <v>-5.8</v>
+        <v>-5.2</v>
       </c>
       <c r="D7" s="37">
-        <v>-1.6</v>
+        <v>-0.7</v>
       </c>
       <c r="E7" s="37">
-        <v>-4.8</v>
+        <v>-6.9</v>
       </c>
       <c r="F7" s="37">
-        <v>-2.7</v>
+        <v>-12.1</v>
       </c>
       <c r="G7" s="37">
-        <v>-1.1000000000000001</v>
+        <v>-3.7</v>
       </c>
       <c r="H7" s="21">
-        <v>-7.9754643397108698</v>
+        <v>-5.7880456737528618</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2249,25 +2266,25 @@
         <v>135</v>
       </c>
       <c r="B8" s="37">
-        <v>4.3</v>
+        <v>3.8</v>
       </c>
       <c r="C8" s="37">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
       <c r="D8" s="37">
-        <v>1.8</v>
+        <v>3.2</v>
       </c>
       <c r="E8" s="37">
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="F8" s="37">
-        <v>2.7</v>
+        <v>2</v>
       </c>
       <c r="G8" s="37">
-        <v>0.8</v>
+        <v>3.9</v>
       </c>
       <c r="H8" s="22">
-        <v>3.2248792332832288</v>
+        <v>3.6587645156742621</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2275,25 +2292,25 @@
         <v>136</v>
       </c>
       <c r="B9" s="37">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="C9" s="37">
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="D9" s="37">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E9" s="37">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="F9" s="37">
-        <v>1.7</v>
+        <v>2.9</v>
       </c>
       <c r="G9" s="37">
-        <v>1.8</v>
+        <v>3.2</v>
       </c>
       <c r="H9" s="21">
-        <v>1.9171178181551118</v>
+        <v>2.3467340040205231</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2301,25 +2318,25 @@
         <v>137</v>
       </c>
       <c r="B10" s="37">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="C10" s="37">
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="D10" s="37">
-        <v>2.2999999999999998</v>
+        <v>3.4</v>
       </c>
       <c r="E10" s="37">
-        <v>1</v>
+        <v>2.9</v>
       </c>
       <c r="F10" s="37">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="G10" s="37">
-        <v>1</v>
+        <v>3.3</v>
       </c>
       <c r="H10" s="21">
-        <v>1.5292688785707886</v>
+        <v>3.276204179732245</v>
       </c>
     </row>
   </sheetData>
@@ -2333,7 +2350,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G14"/>
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,25 +2386,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="27">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="C2" s="39">
-        <v>2.2999999999999998</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D2" s="39">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="E2" s="39">
-        <v>3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F2" s="39">
-        <v>2.7</v>
+        <v>4</v>
       </c>
       <c r="G2" s="39">
-        <v>2.7</v>
+        <v>3.9</v>
       </c>
       <c r="H2" s="29">
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2395,25 +2412,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="26">
-        <v>2.1</v>
+        <v>4.3</v>
       </c>
       <c r="C3" s="38">
-        <v>1.8</v>
+        <v>3.9</v>
       </c>
       <c r="D3" s="38">
-        <v>2.2999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="38">
-        <v>2.7</v>
+        <v>5.8</v>
       </c>
       <c r="F3" s="38">
-        <v>2.4</v>
+        <v>4.7</v>
       </c>
       <c r="G3" s="38">
-        <v>2.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H3" s="28">
-        <v>1.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2421,25 +2438,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="26">
-        <v>1.1000000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="C4" s="38">
-        <v>0.9</v>
+        <v>5.2</v>
       </c>
       <c r="D4" s="38">
-        <v>1.1000000000000001</v>
+        <v>5.7</v>
       </c>
       <c r="E4" s="38">
-        <v>2.9</v>
+        <v>6.1</v>
       </c>
       <c r="F4" s="38">
-        <v>1.5</v>
+        <v>5.3</v>
       </c>
       <c r="G4" s="38">
-        <v>1.1000000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="H4" s="28">
-        <v>0.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2447,25 +2464,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="26">
-        <v>4.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="C5" s="38">
-        <v>3.3</v>
+        <v>5.4</v>
       </c>
       <c r="D5" s="38">
-        <v>5.7</v>
+        <v>3.7</v>
       </c>
       <c r="E5" s="38">
-        <v>3.4</v>
+        <v>5.3</v>
       </c>
       <c r="F5" s="38">
-        <v>4.2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G5" s="38">
-        <v>2.4</v>
+        <v>6.4</v>
       </c>
       <c r="H5" s="28">
-        <v>2.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2473,25 +2490,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="26">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="C6" s="38">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="D6" s="38">
-        <v>2.7</v>
+        <v>1.9</v>
       </c>
       <c r="E6" s="38">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="F6" s="38">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="G6" s="38">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="H6" s="28">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2499,25 +2516,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="26">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="C7" s="38">
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="38">
+        <v>3.4</v>
+      </c>
+      <c r="E7" s="38">
+        <v>2.9</v>
+      </c>
+      <c r="F7" s="38">
         <v>2.8</v>
       </c>
-      <c r="D7" s="38">
-        <v>2.6</v>
-      </c>
-      <c r="E7" s="38">
-        <v>2.7</v>
-      </c>
-      <c r="F7" s="38">
-        <v>2.5</v>
-      </c>
       <c r="G7" s="38">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
       <c r="H7" s="28">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2525,25 +2542,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="26">
-        <v>2.4</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="38">
-        <v>2.1</v>
+        <v>0.4</v>
       </c>
       <c r="D8" s="38">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8" s="38">
-        <v>3.4</v>
+        <v>0.9</v>
       </c>
       <c r="F8" s="38">
-        <v>2.8</v>
+        <v>0.9</v>
       </c>
       <c r="G8" s="38">
-        <v>2.9</v>
+        <v>0.9</v>
       </c>
       <c r="H8" s="28">
-        <v>3.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2551,25 +2568,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="26">
-        <v>2.2000000000000002</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C9" s="38">
-        <v>1.7</v>
+        <v>6.7</v>
       </c>
       <c r="D9" s="38">
-        <v>2.2999999999999998</v>
+        <v>3.6</v>
       </c>
       <c r="E9" s="38">
+        <v>3.2</v>
+      </c>
+      <c r="F9" s="38">
+        <v>3.6</v>
+      </c>
+      <c r="G9" s="38">
+        <v>3.7</v>
+      </c>
+      <c r="H9" s="28">
         <v>3.8</v>
-      </c>
-      <c r="F9" s="38">
-        <v>2.4</v>
-      </c>
-      <c r="G9" s="38">
-        <v>3.2</v>
-      </c>
-      <c r="H9" s="28">
-        <v>3.1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2577,25 +2594,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="26">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
       <c r="C10" s="38">
-        <v>-0.1</v>
+        <v>1.5</v>
       </c>
       <c r="D10" s="38">
+        <v>2</v>
+      </c>
+      <c r="E10" s="38">
         <v>2.1</v>
       </c>
-      <c r="E10" s="38">
-        <v>0.4</v>
-      </c>
       <c r="F10" s="38">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G10" s="38">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="H10" s="28">
-        <v>0.2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2603,25 +2620,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="26">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="38">
-        <v>0.9</v>
+        <v>4.5</v>
       </c>
       <c r="D11" s="38">
-        <v>1.9</v>
+        <v>3.5</v>
       </c>
       <c r="E11" s="38">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="F11" s="38">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="G11" s="38">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="28">
-        <v>1.1000000000000001</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2629,25 +2646,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C12" s="38">
-        <v>0.4</v>
+        <v>1.6</v>
       </c>
       <c r="D12" s="38">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="38">
+        <v>0.7</v>
+      </c>
+      <c r="F12" s="38">
         <v>0</v>
       </c>
-      <c r="F12" s="38">
-        <v>0.6</v>
-      </c>
       <c r="G12" s="38">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="H12" s="28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2655,25 +2672,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="26">
-        <v>5</v>
+        <v>5.9</v>
       </c>
       <c r="C13" s="38">
-        <v>6</v>
+        <v>6.3</v>
       </c>
       <c r="D13" s="38">
-        <v>4.4000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E13" s="38">
-        <v>5.8</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F13" s="38">
-        <v>3.4</v>
+        <v>8</v>
       </c>
       <c r="G13" s="38">
-        <v>4.0999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="H13" s="28">
-        <v>2.1</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2681,25 +2698,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="26">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="C14" s="38">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="D14" s="38">
-        <v>1.9</v>
+        <v>3.6</v>
       </c>
       <c r="E14" s="38">
+        <v>3</v>
+      </c>
+      <c r="F14" s="38">
+        <v>3.6</v>
+      </c>
+      <c r="G14" s="38">
+        <v>3.9</v>
+      </c>
+      <c r="H14" s="28">
         <v>2.2000000000000002</v>
-      </c>
-      <c r="F14" s="38">
-        <v>2.9</v>
-      </c>
-      <c r="G14" s="38">
-        <v>2.6</v>
-      </c>
-      <c r="H14" s="28">
-        <v>1.9</v>
       </c>
     </row>
   </sheetData>
@@ -2749,25 +2766,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="31">
-        <v>51.2</v>
+        <v>50.9</v>
       </c>
       <c r="C2" s="40">
-        <v>50.9</v>
+        <v>51.4</v>
       </c>
       <c r="D2" s="40">
-        <v>51.4</v>
+        <v>50.5</v>
       </c>
       <c r="E2" s="40">
-        <v>51.3</v>
+        <v>49.7</v>
       </c>
       <c r="F2" s="40">
-        <v>51.2</v>
+        <v>50.8</v>
       </c>
       <c r="G2" s="40">
-        <v>51.2</v>
+        <v>50.6</v>
       </c>
       <c r="H2" s="40">
-        <v>51.5</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2775,25 +2792,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="30">
-        <v>50.5</v>
+        <v>50.3</v>
       </c>
       <c r="C3" s="23">
-        <v>48.8</v>
+        <v>50.4</v>
       </c>
       <c r="D3" s="23">
-        <v>51.8</v>
+        <v>50.8</v>
       </c>
       <c r="E3" s="23">
-        <v>53.1</v>
+        <v>48.6</v>
       </c>
       <c r="F3" s="23">
-        <v>51.9</v>
+        <v>49.5</v>
       </c>
       <c r="G3" s="23">
-        <v>52.2</v>
+        <v>50.1</v>
       </c>
       <c r="H3" s="23">
-        <v>49.9</v>
+        <v>49.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2801,25 +2818,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="30">
-        <v>52.2</v>
+        <v>55.1</v>
       </c>
       <c r="C4" s="23">
-        <v>50</v>
+        <v>53.4</v>
       </c>
       <c r="D4" s="23">
-        <v>53.7</v>
+        <v>56.7</v>
       </c>
       <c r="E4" s="23">
-        <v>60.9</v>
+        <v>61.5</v>
       </c>
       <c r="F4" s="23">
-        <v>55.2</v>
+        <v>57.5</v>
       </c>
       <c r="G4" s="23">
-        <v>52.3</v>
+        <v>54.1</v>
       </c>
       <c r="H4" s="23">
-        <v>49.6</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2827,25 +2844,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="30">
-        <v>62.8</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="C5" s="23">
-        <v>65.099999999999994</v>
+        <v>67.2</v>
       </c>
       <c r="D5" s="23">
-        <v>61.6</v>
+        <v>62.6</v>
       </c>
       <c r="E5" s="23">
-        <v>63.9</v>
+        <v>62.7</v>
       </c>
       <c r="F5" s="23">
-        <v>58.7</v>
+        <v>60.4</v>
       </c>
       <c r="G5" s="23">
-        <v>56.2</v>
+        <v>61.4</v>
       </c>
       <c r="H5" s="23">
-        <v>62.6</v>
+        <v>65.900000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2853,25 +2870,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="30">
-        <v>29.4</v>
+        <v>28.3</v>
       </c>
       <c r="C6" s="23">
-        <v>31.6</v>
+        <v>29.6</v>
       </c>
       <c r="D6" s="23">
-        <v>25.1</v>
+        <v>24.7</v>
       </c>
       <c r="E6" s="23">
         <v>31.5</v>
       </c>
       <c r="F6" s="23">
-        <v>32.799999999999997</v>
+        <v>33</v>
       </c>
       <c r="G6" s="23">
-        <v>28</v>
+        <v>27.6</v>
       </c>
       <c r="H6" s="23">
-        <v>32.6</v>
+        <v>32.200000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2879,25 +2896,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="30">
-        <v>45.2</v>
+        <v>46.6</v>
       </c>
       <c r="C7" s="23">
-        <v>45.3</v>
+        <v>47.5</v>
       </c>
       <c r="D7" s="23">
-        <v>45.3</v>
+        <v>46</v>
       </c>
       <c r="E7" s="23">
-        <v>40.6</v>
+        <v>41.8</v>
       </c>
       <c r="F7" s="23">
-        <v>43.1</v>
+        <v>44.2</v>
       </c>
       <c r="G7" s="23">
-        <v>48.2</v>
+        <v>48.9</v>
       </c>
       <c r="H7" s="23">
-        <v>49.1</v>
+        <v>48.7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2905,25 +2922,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="30">
-        <v>59</v>
+        <v>51.8</v>
       </c>
       <c r="C8" s="23">
-        <v>58.9</v>
+        <v>50.9</v>
       </c>
       <c r="D8" s="23">
-        <v>59.7</v>
+        <v>52.6</v>
       </c>
       <c r="E8" s="23">
-        <v>58.7</v>
+        <v>53.1</v>
       </c>
       <c r="F8" s="23">
-        <v>57.3</v>
+        <v>52.1</v>
       </c>
       <c r="G8" s="23">
-        <v>60.2</v>
+        <v>53.6</v>
       </c>
       <c r="H8" s="23">
-        <v>55.3</v>
+        <v>50.9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2934,22 +2951,22 @@
         <v>57.6</v>
       </c>
       <c r="C9" s="23">
-        <v>53.2</v>
+        <v>55.7</v>
       </c>
       <c r="D9" s="23">
-        <v>60.2</v>
+        <v>58.4</v>
       </c>
       <c r="E9" s="23">
-        <v>60</v>
+        <v>59.4</v>
       </c>
       <c r="F9" s="23">
-        <v>58.3</v>
+        <v>56.7</v>
       </c>
       <c r="G9" s="23">
-        <v>64.3</v>
+        <v>61.6</v>
       </c>
       <c r="H9" s="23">
-        <v>67.2</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2957,25 +2974,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="30">
-        <v>33.299999999999997</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="C10" s="23">
-        <v>33.5</v>
+        <v>35.6</v>
       </c>
       <c r="D10" s="23">
-        <v>31.7</v>
+        <v>34.5</v>
       </c>
       <c r="E10" s="23">
-        <v>36.6</v>
+        <v>38.4</v>
       </c>
       <c r="F10" s="23">
-        <v>35</v>
+        <v>38.4</v>
       </c>
       <c r="G10" s="23">
-        <v>32</v>
+        <v>35.4</v>
       </c>
       <c r="H10" s="23">
-        <v>38.799999999999997</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2983,25 +3000,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="30">
-        <v>48.8</v>
+        <v>47</v>
       </c>
       <c r="C11" s="23">
-        <v>48.9</v>
+        <v>48.4</v>
       </c>
       <c r="D11" s="23">
-        <v>51.4</v>
+        <v>46.5</v>
       </c>
       <c r="E11" s="23">
-        <v>41.7</v>
+        <v>42.3</v>
       </c>
       <c r="F11" s="23">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="G11" s="23">
-        <v>41.4</v>
+        <v>42.7</v>
       </c>
       <c r="H11" s="23">
-        <v>45.2</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3009,25 +3026,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="30">
-        <v>54.6</v>
+        <v>56.1</v>
       </c>
       <c r="C12" s="23">
-        <v>59.7</v>
+        <v>62.3</v>
       </c>
       <c r="D12" s="23">
-        <v>54.9</v>
+        <v>55.4</v>
       </c>
       <c r="E12" s="23">
-        <v>39.5</v>
+        <v>40.5</v>
       </c>
       <c r="F12" s="23">
-        <v>48.9</v>
+        <v>48.4</v>
       </c>
       <c r="G12" s="23">
-        <v>41.8</v>
+        <v>42.9</v>
       </c>
       <c r="H12" s="23">
-        <v>38.799999999999997</v>
+        <v>39.299999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3035,25 +3052,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="30">
-        <v>63.4</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="C13" s="23">
-        <v>67</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="D13" s="23">
-        <v>60.4</v>
+        <v>62</v>
       </c>
       <c r="E13" s="23">
-        <v>61.6</v>
+        <v>66.3</v>
       </c>
       <c r="F13" s="23">
-        <v>60.3</v>
+        <v>67.3</v>
       </c>
       <c r="G13" s="23">
-        <v>64.900000000000006</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="H13" s="23">
-        <v>56.9</v>
+        <v>60.2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3061,22 +3078,22 @@
         <v>24</v>
       </c>
       <c r="B14" s="30">
-        <v>36.799999999999997</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="C14" s="23">
-        <v>36.5</v>
+        <v>38.5</v>
       </c>
       <c r="D14" s="23">
-        <v>37.5</v>
+        <v>39.6</v>
       </c>
       <c r="E14" s="23">
-        <v>37.799999999999997</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="F14" s="23">
-        <v>36.6</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="G14" s="23">
-        <v>34.9</v>
+        <v>36.1</v>
       </c>
       <c r="H14" s="23">
         <v>36.700000000000003</v>
@@ -4921,8 +4938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
"Actualizo datos de diciembre a nivel fiscal y comex"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F57018-D577-4BDA-A567-0CFA9635B558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB43EA94-10D7-4F28-8D65-A7C2E877BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -2070,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
@@ -4938,8 +4938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,14 +4966,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="35">
-        <v>13274</v>
+        <v>14615</v>
       </c>
       <c r="C2" s="35">
-        <v>14537</v>
+        <v>15929</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1263</v>
+        <f>B2-C2</f>
+        <v>-1314</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4981,14 +4981,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="35">
-        <v>3728</v>
+        <v>4182</v>
       </c>
       <c r="C3">
-        <v>627</v>
+        <v>696</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>3101</v>
+        <f>B3-C3</f>
+        <v>3486</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,14 +4996,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="35">
-        <v>4069</v>
+        <v>4530</v>
       </c>
       <c r="C4" s="35">
-        <v>1745</v>
+        <v>1920</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>2324</v>
+        <f>B4-C4</f>
+        <v>2610</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5011,14 +5011,14 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>938</v>
+        <v>999</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>912</v>
+        <f>B5-C5</f>
+        <v>969</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5026,14 +5026,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="35">
-        <v>5649</v>
+        <v>6401</v>
       </c>
       <c r="C6" s="35">
-        <v>6982</v>
+        <v>7749</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-1333</v>
+        <f>B6-C6</f>
+        <v>-1348</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5041,14 +5041,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="35">
-        <v>9170</v>
+        <v>9871</v>
       </c>
       <c r="C7" s="35">
-        <v>8470</v>
+        <v>9311</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>700</v>
+        <f>B7-C7</f>
+        <v>560</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5056,14 +5056,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>715</v>
+        <v>761</v>
       </c>
       <c r="C8">
-        <v>481</v>
+        <v>541</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>234</v>
+        <f>B8-C8</f>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5071,14 +5071,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>881</v>
+        <v>956</v>
       </c>
       <c r="C9">
-        <v>488</v>
+        <v>532</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>393</v>
+        <f>B9-C9</f>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5086,14 +5086,14 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>769</v>
+        <v>836</v>
       </c>
       <c r="C10">
-        <v>661</v>
+        <v>679</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>108</v>
+        <f>B10-C10</f>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5101,14 +5101,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="35">
-        <v>6786</v>
+        <v>7441</v>
       </c>
       <c r="C11" s="35">
-        <v>3490</v>
+        <v>3928</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>3296</v>
+        <f>B11-C11</f>
+        <v>3513</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5116,14 +5116,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="35">
-        <v>5923</v>
+        <v>6299</v>
       </c>
       <c r="C12" s="35">
-        <v>12001</v>
+        <v>13538</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>-6078</v>
+        <f>B12-C12</f>
+        <v>-7239</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5131,29 +5131,29 @@
         <v>90</v>
       </c>
       <c r="B13" s="35">
-        <v>1599</v>
+        <v>1722</v>
       </c>
       <c r="C13">
-        <v>551</v>
+        <v>648</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>1048</v>
+        <f>B13-C13</f>
+        <v>1074</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B14">
-        <v>686</v>
-      </c>
-      <c r="C14">
-        <v>1030</v>
+      <c r="B14" s="35">
+        <v>723</v>
+      </c>
+      <c r="C14" s="35">
+        <v>1140</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>-344</v>
+        <f>B14-C14</f>
+        <v>-417</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5161,14 +5161,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="35">
-        <v>3808</v>
+        <v>4301</v>
       </c>
       <c r="C15" s="35">
-        <v>1281</v>
+        <v>1394</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>2527</v>
+        <f>B15-C15</f>
+        <v>2907</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5176,14 +5176,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="35">
-        <v>4286</v>
+        <v>4501</v>
       </c>
       <c r="C16" s="35">
-        <v>1352</v>
+        <v>1579</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>2934</v>
+        <f>B16-C16</f>
+        <v>2922</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5191,14 +5191,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="35">
-        <v>3795</v>
+        <v>4046</v>
       </c>
       <c r="C17">
-        <v>931</v>
+        <v>962</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>2864</v>
+        <f>B17-C17</f>
+        <v>3084</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5206,14 +5206,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>429</v>
+        <v>454</v>
       </c>
       <c r="C18">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>236</v>
+        <f>B18-C18</f>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5221,14 +5221,14 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>741</v>
+        <v>809</v>
       </c>
       <c r="C19">
-        <v>355</v>
+        <v>434</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>386</v>
+        <f>B19-C19</f>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5236,14 +5236,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="35">
-        <v>4074</v>
+        <v>4489</v>
       </c>
       <c r="C20" s="35">
-        <v>1768</v>
+        <v>1963</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>2306</v>
+        <f>B20-C20</f>
+        <v>2526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo datos comex-ene22 y EMAE-dic21"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA95741-0C61-452B-94AF-FCABB54C9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45F22AF-05A5-41FD-9397-CCE173D8D032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -683,11 +683,11 @@
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2138,7 +2138,7 @@
       <c r="D2" s="37">
         <v>2.7</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="41">
         <v>2.6</v>
       </c>
       <c r="F2" s="37">
@@ -2164,7 +2164,7 @@
       <c r="D3" s="37">
         <v>11.4</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>3</v>
       </c>
       <c r="F3" s="37">
@@ -2190,7 +2190,7 @@
       <c r="D4" s="37">
         <v>1.2</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="41">
         <v>3.4</v>
       </c>
       <c r="F4" s="37">
@@ -2216,7 +2216,7 @@
       <c r="D5" s="37">
         <v>1.4</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="41">
         <v>3.7</v>
       </c>
       <c r="F5" s="37">
@@ -2242,7 +2242,7 @@
       <c r="D6" s="37">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <v>4.2</v>
       </c>
       <c r="F6" s="37">
@@ -2268,7 +2268,7 @@
       <c r="D7" s="37">
         <v>-0.7</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>25.5</v>
       </c>
       <c r="F7" s="37">
@@ -2294,7 +2294,7 @@
       <c r="D8" s="37">
         <v>3.2</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>3.3</v>
       </c>
       <c r="F8" s="37">
@@ -2320,7 +2320,7 @@
       <c r="D9" s="37">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="41">
         <v>4.3</v>
       </c>
       <c r="F9" s="37">
@@ -2346,7 +2346,7 @@
       <c r="D10" s="37">
         <v>3.4</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="41">
         <v>3.6</v>
       </c>
       <c r="F10" s="37">
@@ -2749,7 +2749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H14"/>
     </sheetView>
   </sheetViews>
@@ -4191,14 +4191,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4802,14 +4802,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4958,7 +4958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
@@ -4986,14 +4986,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="35">
-        <v>14615</v>
+        <v>881</v>
       </c>
       <c r="C2" s="35">
-        <v>15929</v>
+        <v>1094</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1314</v>
+        <v>-213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,14 +5001,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="35">
-        <v>4182</v>
+        <v>351</v>
       </c>
       <c r="C3">
-        <v>696</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>3486</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5016,14 +5016,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="35">
-        <v>4530</v>
+        <v>354</v>
       </c>
       <c r="C4" s="35">
-        <v>1920</v>
+        <v>167</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>2610</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5031,14 +5031,14 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>999</v>
+        <v>53</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>969</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,14 +5046,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="35">
-        <v>6401</v>
+        <v>364</v>
       </c>
       <c r="C6" s="35">
-        <v>7749</v>
+        <v>495</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-1348</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,14 +5061,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="35">
-        <v>9871</v>
+        <v>836</v>
       </c>
       <c r="C7" s="35">
-        <v>9311</v>
+        <v>842</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>560</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,14 +5076,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>761</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>541</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,14 +5091,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>956</v>
+        <v>85</v>
       </c>
       <c r="C9">
-        <v>532</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>424</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,14 +5106,14 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>836</v>
+        <v>93</v>
       </c>
       <c r="C10">
-        <v>679</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>157</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,14 +5121,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="35">
-        <v>7441</v>
+        <v>423</v>
       </c>
       <c r="C11" s="35">
-        <v>3928</v>
+        <v>337</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>3513</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,14 +5136,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="35">
-        <v>6299</v>
+        <v>373</v>
       </c>
       <c r="C12" s="35">
-        <v>13538</v>
+        <v>1508</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-7239</v>
+        <v>-1135</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,14 +5151,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="35">
-        <v>1722</v>
+        <v>114</v>
       </c>
       <c r="C13">
-        <v>648</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1074</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,14 +5166,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="35">
-        <v>723</v>
+        <v>21</v>
       </c>
       <c r="C14" s="35">
-        <v>1140</v>
+        <v>78</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-417</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,14 +5181,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="35">
-        <v>4301</v>
+        <v>263</v>
       </c>
       <c r="C15" s="35">
-        <v>1394</v>
+        <v>137</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>2907</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5196,14 +5196,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="35">
-        <v>4501</v>
+        <v>213</v>
       </c>
       <c r="C16" s="35">
-        <v>1579</v>
+        <v>90</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>2922</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,14 +5211,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="35">
-        <v>4046</v>
+        <v>344</v>
       </c>
       <c r="C17">
-        <v>962</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>3084</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5226,14 +5226,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>454</v>
+        <v>92</v>
       </c>
       <c r="C18">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>241</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5241,14 +5241,14 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>809</v>
+        <v>72</v>
       </c>
       <c r="C19">
-        <v>434</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>375</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5256,14 +5256,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="35">
-        <v>4489</v>
+        <v>596</v>
       </c>
       <c r="C20" s="35">
-        <v>1963</v>
+        <v>160</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2526</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -5492,10 +5492,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5527,10 +5527,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="23">
-        <v>148.19884586644767</v>
+        <v>148.18349369128583</v>
       </c>
       <c r="D2" s="23">
-        <v>147.04978637579194</v>
+        <v>147.0621449260093</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5541,10 +5541,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="23">
-        <v>146.66443199519426</v>
+        <v>146.69673264137583</v>
       </c>
       <c r="D3" s="23">
-        <v>146.45133406442321</v>
+        <v>146.46931916127502</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5555,10 +5555,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="23">
-        <v>145.93460754708732</v>
+        <v>145.97222771976445</v>
       </c>
       <c r="D4" s="23">
-        <v>145.89156103402448</v>
+        <v>145.91393396103376</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5569,10 +5569,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="23">
-        <v>145.20706225540795</v>
+        <v>145.22398006632829</v>
       </c>
       <c r="D5" s="23">
-        <v>145.40756213630624</v>
+        <v>145.43242759617519</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5583,10 +5583,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="23">
-        <v>144.38773354699802</v>
+        <v>144.36754489711953</v>
       </c>
       <c r="D6" s="23">
-        <v>145.02727262464441</v>
+        <v>145.05270951514441</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5597,10 +5597,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="23">
-        <v>144.33981417019862</v>
+        <v>144.29996705649847</v>
       </c>
       <c r="D7" s="23">
-        <v>144.7725017112169</v>
+        <v>144.79666657392883</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5611,10 +5611,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="23">
-        <v>144.41822271027428</v>
+        <v>144.39192328281442</v>
       </c>
       <c r="D8" s="23">
-        <v>144.65206634783755</v>
+        <v>144.67341355232986</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5625,10 +5625,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="23">
-        <v>145.61066872321518</v>
+        <v>145.57360477998151</v>
       </c>
       <c r="D9" s="23">
-        <v>144.66756267583204</v>
+        <v>144.68565025066377</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5639,10 +5639,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="23">
-        <v>145.10200677610106</v>
+        <v>145.09040295998474</v>
       </c>
       <c r="D10" s="23">
-        <v>144.81449520380073</v>
+        <v>144.82907618536532</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5653,10 +5653,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="23">
-        <v>145.05051453811953</v>
+        <v>145.06323892412777</v>
       </c>
       <c r="D11" s="23">
-        <v>145.082243669294</v>
+        <v>145.09419953467454</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5667,10 +5667,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="23">
-        <v>145.72194522984853</v>
+        <v>145.74098249463347</v>
       </c>
       <c r="D12" s="23">
-        <v>145.45421373678201</v>
+        <v>145.46533963871997</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5681,10 +5681,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="23">
-        <v>146.93550040099842</v>
+        <v>146.96725526102128</v>
       </c>
       <c r="D13" s="23">
-        <v>145.91600360546803</v>
+        <v>145.92874460657271</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5692,13 +5692,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="23">
-        <v>136.63265948871924</v>
+        <v>136.63265948871936</v>
       </c>
       <c r="C14" s="23">
-        <v>147.44108712970728</v>
+        <v>147.41374726175283</v>
       </c>
       <c r="D14" s="23">
-        <v>146.4507352993646</v>
+        <v>146.4676463258906</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5706,13 +5706,13 @@
         <v>42767</v>
       </c>
       <c r="B15" s="23">
-        <v>132.15851634216514</v>
+        <v>132.15851634216529</v>
       </c>
       <c r="C15" s="23">
-        <v>146.51097269748675</v>
+        <v>146.52537665594733</v>
       </c>
       <c r="D15" s="23">
-        <v>147.04134044024414</v>
+        <v>147.06447138021485</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5720,13 +5720,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="23">
-        <v>152.62095855115712</v>
+        <v>152.62095855115732</v>
       </c>
       <c r="C16" s="23">
-        <v>147.98535109570534</v>
+        <v>148.03947623052244</v>
       </c>
       <c r="D16" s="23">
-        <v>147.66937741899972</v>
+        <v>147.69982338122074</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5734,13 +5734,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="23">
-        <v>151.94634477931669</v>
+        <v>151.94634477931689</v>
       </c>
       <c r="C17" s="23">
-        <v>147.784454919984</v>
+        <v>147.78602285073043</v>
       </c>
       <c r="D17" s="23">
-        <v>148.31353251345305</v>
+        <v>148.35126469826446</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5748,13 +5748,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="23">
-        <v>168.38920945875734</v>
+        <v>168.38920945875753</v>
       </c>
       <c r="C18" s="23">
-        <v>148.6661960152552</v>
+        <v>148.65492360321201</v>
       </c>
       <c r="D18" s="23">
-        <v>148.94763988756461</v>
+        <v>148.99144679605089</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5762,13 +5762,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="23">
-        <v>161.03568550523281</v>
+        <v>161.03568550523286</v>
       </c>
       <c r="C19" s="23">
-        <v>150.27571099056428</v>
+        <v>150.24996585517863</v>
       </c>
       <c r="D19" s="23">
-        <v>149.54071729984477</v>
+        <v>149.58823150996582</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5776,13 +5776,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="23">
-        <v>150.30605023792208</v>
+        <v>150.30605023792197</v>
       </c>
       <c r="C20" s="23">
-        <v>150.2640307788235</v>
+        <v>150.2475934817972</v>
       </c>
       <c r="D20" s="23">
-        <v>150.06061643979129</v>
+        <v>150.10859407438372</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5790,13 +5790,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="23">
-        <v>149.25534282189685</v>
+        <v>149.25534282189687</v>
       </c>
       <c r="C21" s="23">
-        <v>150.27308928517135</v>
+        <v>150.21255472865508</v>
       </c>
       <c r="D21" s="23">
-        <v>150.47367732772409</v>
+        <v>150.51864680110404</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5804,13 +5804,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="23">
-        <v>146.38655949569539</v>
+        <v>146.38655949569588</v>
       </c>
       <c r="C22" s="23">
-        <v>151.22820861629958</v>
+        <v>151.20691509597376</v>
       </c>
       <c r="D22" s="23">
-        <v>150.74645482175634</v>
+        <v>150.78576569647694</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5818,13 +5818,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="23">
-        <v>149.38594914967399</v>
+        <v>149.38594914967516</v>
       </c>
       <c r="C23" s="23">
-        <v>151.46226584928044</v>
+        <v>151.48595488640765</v>
       </c>
       <c r="D23" s="23">
-        <v>150.85290626192534</v>
+        <v>150.8845607730164</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5832,13 +5832,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="23">
-        <v>151.9260426343711</v>
+        <v>151.92604263437167</v>
       </c>
       <c r="C24" s="23">
-        <v>152.53442942784139</v>
+        <v>152.56546404872461</v>
       </c>
       <c r="D24" s="23">
-        <v>150.7705649336998</v>
+        <v>150.79311905120005</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5846,13 +5846,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="23">
-        <v>146.78338564322021</v>
+        <v>146.78338564321894</v>
       </c>
       <c r="C25" s="23">
-        <v>152.40090751194015</v>
+        <v>152.43870963463323</v>
       </c>
       <c r="D25" s="23">
-        <v>150.48779034831762</v>
+        <v>150.50093074862406</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5860,13 +5860,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="23">
-        <v>142.7409149447864</v>
+        <v>142.74091494478188</v>
       </c>
       <c r="C26" s="23">
-        <v>152.06752701123267</v>
+        <v>152.06202944140554</v>
       </c>
       <c r="D26" s="23">
-        <v>150.00904647255939</v>
+        <v>150.01368224201173</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5874,13 +5874,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="23">
-        <v>138.81804133746542</v>
+        <v>138.8180413374636</v>
       </c>
       <c r="C27" s="23">
-        <v>152.00772282968782</v>
+        <v>152.03427528771681</v>
       </c>
       <c r="D27" s="23">
-        <v>149.35367656857537</v>
+        <v>149.35171789428014</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5888,13 +5888,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="23">
-        <v>155.8573162113469</v>
+        <v>155.85731621135361</v>
       </c>
       <c r="C28" s="23">
-        <v>151.25325094513749</v>
+        <v>151.30101250711402</v>
       </c>
       <c r="D28" s="23">
-        <v>148.55634583712882</v>
+        <v>148.5501842507681</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5902,13 +5902,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="23">
-        <v>151.52453339186513</v>
+        <v>151.52453339188628</v>
       </c>
       <c r="C29" s="23">
-        <v>146.87957998802489</v>
+        <v>146.89441438237267</v>
       </c>
       <c r="D29" s="23">
-        <v>147.66383289450994</v>
+        <v>147.65587643530469</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5916,13 +5916,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="23">
-        <v>159.56668791298307</v>
+        <v>159.56668791299208</v>
       </c>
       <c r="C30" s="23">
-        <v>144.45799371072306</v>
+        <v>144.44407959951238</v>
       </c>
       <c r="D30" s="23">
-        <v>146.73061331412424</v>
+        <v>146.72356102565738</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5930,13 +5930,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="23">
-        <v>151.1257782904664</v>
+        <v>151.12577829043676</v>
       </c>
       <c r="C31" s="23">
-        <v>143.18328458974716</v>
+        <v>143.13597722709724</v>
       </c>
       <c r="D31" s="23">
-        <v>145.81188435001735</v>
+        <v>145.80745773118755</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5944,13 +5944,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="23">
-        <v>145.96357240376071</v>
+        <v>145.96357240366589</v>
       </c>
       <c r="C32" s="23">
-        <v>143.20697100566835</v>
+        <v>143.15717025828692</v>
       </c>
       <c r="D32" s="23">
-        <v>144.95683692111979</v>
+        <v>144.95551096154841</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5958,13 +5958,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="23">
-        <v>146.76598025676481</v>
+        <v>146.7659802567249</v>
       </c>
       <c r="C33" s="23">
-        <v>146.69016689265533</v>
+        <v>146.58626058192172</v>
       </c>
       <c r="D33" s="23">
-        <v>144.21077883079221</v>
+        <v>144.21199326814863</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5972,13 +5972,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="23">
-        <v>137.7465015222661</v>
+        <v>137.74650152240125</v>
       </c>
       <c r="C34" s="23">
-        <v>143.14686771003733</v>
+        <v>143.13955143189389</v>
       </c>
       <c r="D34" s="23">
-        <v>143.60488272448194</v>
+        <v>143.60711232915125</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5986,13 +5986,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="23">
-        <v>142.84305870130279</v>
+        <v>142.84305870173307</v>
       </c>
       <c r="C35" s="23">
-        <v>143.48322929966295</v>
+        <v>143.53927245031349</v>
       </c>
       <c r="D35" s="23">
-        <v>143.15513681743445</v>
+        <v>143.15732551385699</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -6000,13 +6000,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="23">
-        <v>140.59231573279851</v>
+        <v>140.59231573298001</v>
       </c>
       <c r="C36" s="23">
-        <v>141.56399670858175</v>
+        <v>141.66200928873064</v>
       </c>
       <c r="D36" s="23">
-        <v>142.86353453076143</v>
+        <v>142.86426814243052</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -6014,13 +6014,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="23">
-        <v>136.25192484485765</v>
+        <v>136.2519248442463</v>
       </c>
       <c r="C37" s="23">
-        <v>141.85603506393417</v>
+        <v>141.84057331381112</v>
       </c>
       <c r="D37" s="23">
-        <v>142.7179120481442</v>
+        <v>142.71582774306765</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -6028,13 +6028,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="23">
-        <v>134.52056075269795</v>
+        <v>134.52056075074981</v>
       </c>
       <c r="C38" s="23">
-        <v>142.94092305012808</v>
+        <v>142.93178812186963</v>
       </c>
       <c r="D38" s="23">
-        <v>142.69429995575734</v>
+        <v>142.68808503883471</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -6042,13 +6042,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="23">
-        <v>132.27529838854522</v>
+        <v>132.27529838772409</v>
       </c>
       <c r="C39" s="23">
-        <v>143.72804211770907</v>
+        <v>143.73011394626562</v>
       </c>
       <c r="D39" s="23">
-        <v>142.75596751538754</v>
+        <v>142.74407462055439</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6056,13 +6056,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="23">
-        <v>144.87373844911215</v>
+        <v>144.87373845188188</v>
       </c>
       <c r="C40" s="23">
-        <v>141.30658685259698</v>
+        <v>141.36224353890381</v>
       </c>
       <c r="D40" s="23">
-        <v>142.86251037124146</v>
+        <v>142.84420064876002</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6070,13 +6070,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="23">
-        <v>149.89913656888581</v>
+        <v>149.89913657771015</v>
       </c>
       <c r="C41" s="23">
-        <v>142.50535996942989</v>
+        <v>142.53893657365967</v>
       </c>
       <c r="D41" s="23">
-        <v>142.97260204227123</v>
+        <v>142.94828695779816</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6084,13 +6084,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="23">
-        <v>164.14987183450071</v>
+        <v>164.14987183822055</v>
       </c>
       <c r="C42" s="23">
-        <v>144.60026105357409</v>
+        <v>144.64227181273864</v>
       </c>
       <c r="D42" s="23">
-        <v>143.04874608878293</v>
+        <v>143.01947622528439</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6098,13 +6098,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="23">
-        <v>150.84993449096024</v>
+        <v>150.84993447841651</v>
       </c>
       <c r="C43" s="23">
-        <v>143.67401281365724</v>
+        <v>143.67708822197702</v>
       </c>
       <c r="D43" s="23">
-        <v>143.05531417926838</v>
+        <v>143.0229017459117</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6112,13 +6112,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="23">
-        <v>146.76823781322543</v>
+        <v>146.76823777325902</v>
       </c>
       <c r="C44" s="23">
-        <v>145.42212365910072</v>
+        <v>145.32203245985539</v>
       </c>
       <c r="D44" s="23">
-        <v>142.9647555634896</v>
+        <v>142.9316479875144</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6126,13 +6126,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="23">
-        <v>141.2794360309733</v>
+        <v>141.27943601412611</v>
       </c>
       <c r="C45" s="23">
-        <v>144.90839888281374</v>
+        <v>144.7707533533719</v>
       </c>
       <c r="D45" s="23">
-        <v>142.75523822297521</v>
+        <v>142.72363701271163</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6140,13 +6140,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="23">
-        <v>134.88987741166085</v>
+        <v>134.88987746847488</v>
       </c>
       <c r="C46" s="23">
-        <v>141.123434449901</v>
+        <v>141.10421992317856</v>
       </c>
       <c r="D46" s="23">
-        <v>142.41430982550301</v>
+        <v>142.38549936105483</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6154,13 +6154,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="23">
-        <v>141.51078883576523</v>
+        <v>141.5107890167823</v>
       </c>
       <c r="C47" s="23">
-        <v>143.15633382974227</v>
+        <v>143.25244102922133</v>
       </c>
       <c r="D47" s="23">
-        <v>141.94064965380954</v>
+        <v>141.91466926107924</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6168,13 +6168,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="23">
-        <v>137.65812417725056</v>
+        <v>137.65812425355574</v>
       </c>
       <c r="C48" s="23">
-        <v>140.54252956059784</v>
+        <v>140.68383690021861</v>
       </c>
       <c r="D48" s="23">
-        <v>141.34332416178381</v>
+        <v>141.31854021636124</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6182,13 +6182,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="23">
-        <v>135.67189195256938</v>
+        <v>135.67189169524758</v>
       </c>
       <c r="C49" s="23">
-        <v>140.43889066717938</v>
+        <v>140.33117103995428</v>
       </c>
       <c r="D49" s="23">
-        <v>140.64661962181341</v>
+        <v>140.62063183105846</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6196,13 +6196,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="23">
-        <v>132.28223035143913</v>
+        <v>132.28222953157538</v>
       </c>
       <c r="C50" s="23">
-        <v>140.82959567871032</v>
+        <v>140.76612876398124</v>
       </c>
       <c r="D50" s="23">
-        <v>139.88700593273629</v>
+        <v>139.85867453487685</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6210,13 +6210,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="23">
-        <v>129.74514625474259</v>
+        <v>129.74514590914131</v>
       </c>
       <c r="C51" s="23">
-        <v>140.9373248807764</v>
+        <v>140.84510209372061</v>
       </c>
       <c r="D51" s="23">
-        <v>139.10768559432654</v>
+        <v>139.0771256615846</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6224,13 +6224,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="23">
-        <v>129.09772648509272</v>
+        <v>129.09772765055823</v>
       </c>
       <c r="C52" s="23">
-        <v>125.67733895555091</v>
+        <v>125.68636824161807</v>
       </c>
       <c r="D52" s="23">
-        <v>138.35446133467326</v>
+        <v>138.32296688103409</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6238,13 +6238,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="23">
-        <v>111.90395721343017</v>
+        <v>111.90396092676694</v>
       </c>
       <c r="C53" s="23">
-        <v>105.16415695230512</v>
+        <v>105.26392153546615</v>
       </c>
       <c r="D53" s="23">
-        <v>137.66978446676646</v>
+        <v>137.63977832284999</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6252,13 +6252,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="23">
-        <v>131.29461471226998</v>
+        <v>131.29461627757212</v>
       </c>
       <c r="C54" s="23">
-        <v>116.4241088644595</v>
+        <v>116.49855344829493</v>
       </c>
       <c r="D54" s="23">
-        <v>137.08952937494502</v>
+        <v>137.06403734705788</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6266,13 +6266,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="23">
-        <v>133.30386078199106</v>
+        <v>133.30385550335268</v>
       </c>
       <c r="C55" s="23">
-        <v>124.25074054470862</v>
+        <v>124.28544051256891</v>
       </c>
       <c r="D55" s="23">
-        <v>136.64040778378856</v>
+        <v>136.62193576122931</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6280,13 +6280,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="23">
-        <v>128.19078443799802</v>
+        <v>128.19076761951325</v>
       </c>
       <c r="C56" s="23">
-        <v>126.6377608332724</v>
+        <v>126.47047559987693</v>
       </c>
       <c r="D56" s="23">
-        <v>136.33903937611231</v>
+        <v>136.32966287916631</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6294,13 +6294,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="23">
-        <v>125.1740585906558</v>
+        <v>125.17405150107314</v>
       </c>
       <c r="C57" s="23">
-        <v>129.20648189646315</v>
+        <v>129.02186199881285</v>
       </c>
       <c r="D57" s="23">
-        <v>136.19393432052533</v>
+        <v>136.19537725502903</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6308,13 +6308,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="23">
-        <v>126.59617173353072</v>
+        <v>126.59619564159864</v>
       </c>
       <c r="C58" s="23">
-        <v>131.17628044185966</v>
+        <v>131.16067992216838</v>
       </c>
       <c r="D58" s="23">
-        <v>136.20168813793455</v>
+        <v>136.21276952455645</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6322,13 +6322,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="23">
-        <v>131.72747477273671</v>
+        <v>131.72755094720367</v>
       </c>
       <c r="C59" s="23">
-        <v>133.70072963552099</v>
+        <v>133.88195912079445</v>
       </c>
       <c r="D59" s="23">
-        <v>136.35138645833482</v>
+        <v>136.36963535584024</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6336,13 +6336,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="23">
-        <v>132.96977264618508</v>
+        <v>132.96980475640171</v>
       </c>
       <c r="C60" s="23">
-        <v>135.14029135786697</v>
+        <v>135.3385476000374</v>
       </c>
       <c r="D60" s="23">
-        <v>136.6282317415203</v>
+        <v>136.65093643828837</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6350,13 +6350,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="23">
-        <v>132.42186240989511</v>
+        <v>132.421754125212</v>
       </c>
       <c r="C61" s="23">
-        <v>135.56285157051204</v>
+        <v>135.48862174643341</v>
       </c>
       <c r="D61" s="23">
-        <v>137.01623793389595</v>
+        <v>137.0405409406867</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6364,13 +6364,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="23">
-        <v>129.49239125960432</v>
+        <v>129.49204624937207</v>
       </c>
       <c r="C62" s="23">
-        <v>139.38952857991427</v>
+        <v>139.47059782826972</v>
       </c>
       <c r="D62" s="23">
-        <v>137.49884320419113</v>
+        <v>137.52608929702791</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6378,13 +6378,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="23">
-        <v>126.69366456853579</v>
+        <v>126.69351913459056</v>
       </c>
       <c r="C63" s="23">
-        <v>138.57310370091665</v>
+        <v>138.64854361972618</v>
       </c>
       <c r="D63" s="23">
-        <v>138.06383862563209</v>
+        <v>138.09929406731123</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6392,13 +6392,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="23">
-        <v>146.28825115104189</v>
+        <v>146.2887415952199</v>
       </c>
       <c r="C64" s="23">
-        <v>139.82183631563751</v>
+        <v>140.03411994231681</v>
       </c>
       <c r="D64" s="23">
-        <v>138.70576721621586</v>
+        <v>138.75920572497489</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6406,13 +6406,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="23">
-        <v>144.9074698504499</v>
+        <v>144.90903247458738</v>
       </c>
       <c r="C65" s="23">
-        <v>137.68852857887066</v>
+        <v>138.10772356270161</v>
       </c>
       <c r="D65" s="23">
-        <v>139.41750434754854</v>
+        <v>139.50268056921394</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -6420,13 +6420,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="23">
-        <v>150.14940772167688</v>
+        <v>150.15006642270126</v>
       </c>
       <c r="C66" s="23">
-        <v>136.20380061606969</v>
+        <v>136.59621386829264</v>
       </c>
       <c r="D66" s="23">
-        <v>140.18852672219606</v>
+        <v>140.32320851667797</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -6434,13 +6434,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="23">
-        <v>148.94154226537245</v>
+        <v>148.9393209402111</v>
       </c>
       <c r="C67" s="23">
-        <v>139.97035249185225</v>
+        <v>140.27838742367854</v>
       </c>
       <c r="D67" s="23">
-        <v>141.00096520730253</v>
+        <v>141.2066905656329</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -6448,13 +6448,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="23">
-        <v>143.06669626283102</v>
+        <v>143.16129268584584</v>
       </c>
       <c r="C68" s="23">
-        <v>141.71598812769889</v>
+        <v>141.82073247405549</v>
       </c>
       <c r="D68" s="23">
-        <v>141.8326137962049</v>
+        <v>142.13269518353229</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -6462,13 +6462,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="23">
-        <v>141.08473581933157</v>
+        <v>141.19670480423781</v>
       </c>
       <c r="C69" s="23">
-        <v>143.88754822691234</v>
+        <v>143.93941519322294</v>
       </c>
       <c r="D69" s="23">
-        <v>142.65444270442097</v>
+        <v>143.07124961991786</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -6476,13 +6476,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="23">
-        <v>140.90912111121477</v>
+        <v>140.70255570329414</v>
       </c>
       <c r="C70" s="23">
-        <v>145.13350821424933</v>
+        <v>145.1027230773804</v>
       </c>
       <c r="D70" s="23">
-        <v>143.43631674718807</v>
+        <v>143.99168738236463</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -6490,27 +6490,41 @@
         <v>44470</v>
       </c>
       <c r="B71" s="23">
-        <v>140.53477515616018</v>
+        <v>140.84838387204763</v>
       </c>
       <c r="C71" s="23">
-        <v>143.7578112399471</v>
+        <v>144.3492128906569</v>
       </c>
       <c r="D71" s="23">
-        <v>144.15187962610597</v>
+        <v>144.86090187128829</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>44501</v>
       </c>
-      <c r="B72" s="24">
-        <v>145.39422136957711</v>
-      </c>
-      <c r="C72" s="24">
-        <v>146.18132125291578</v>
-      </c>
-      <c r="D72" s="24">
-        <v>144.77954284484704</v>
+      <c r="B72" s="23">
+        <v>145.51114906453842</v>
+      </c>
+      <c r="C72" s="23">
+        <v>146.28714457565965</v>
+      </c>
+      <c r="D72" s="23">
+        <v>145.65142395437829</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>44531</v>
+      </c>
+      <c r="B73" s="24">
+        <v>145.40844696072728</v>
+      </c>
+      <c r="C73" s="24">
+        <v>147.67149712630018</v>
+      </c>
+      <c r="D73" s="24">
+        <v>146.34890457104302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo datos de comex feb22, producto 2021 y resultado fiscal"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C61D5FB-E471-409D-8C91-B231026F2E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6029D67C-2B3C-4924-AB65-178B04D458E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="138">
   <si>
     <t>Período</t>
   </si>
@@ -573,7 +573,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -589,6 +589,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,7 +629,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -683,11 +689,17 @@
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2107,7 +2119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -2155,7 +2167,7 @@
       <c r="D2" s="37">
         <v>5.2</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="41">
         <v>3.7</v>
       </c>
       <c r="F2" s="37">
@@ -2181,7 +2193,7 @@
       <c r="D3" s="37">
         <v>3.9</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>4</v>
       </c>
       <c r="F3" s="37">
@@ -2207,7 +2219,7 @@
       <c r="D4" s="37">
         <v>7.1</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="41">
         <v>8</v>
       </c>
       <c r="F4" s="37">
@@ -2233,7 +2245,7 @@
       <c r="D5" s="37">
         <v>5.3</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="41">
         <v>3.8</v>
       </c>
       <c r="F5" s="37">
@@ -2259,7 +2271,7 @@
       <c r="D6" s="37">
         <v>11.5</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <v>9</v>
       </c>
       <c r="F6" s="37">
@@ -2285,7 +2297,7 @@
       <c r="D7" s="37">
         <v>18.600000000000001</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>20.9</v>
       </c>
       <c r="F7" s="37">
@@ -2311,7 +2323,7 @@
       <c r="D8" s="37">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>5.2</v>
       </c>
       <c r="F8" s="37">
@@ -2337,7 +2349,7 @@
       <c r="D9" s="37">
         <v>4.5</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="41">
         <v>3.4</v>
       </c>
       <c r="F9" s="37">
@@ -2363,7 +2375,7 @@
       <c r="D10" s="37">
         <v>5.3</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="41">
         <v>3.6</v>
       </c>
       <c r="F10" s="37">
@@ -3144,10 +3156,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,7 +3189,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="12">
-        <v>475580.6987789463</v>
+        <v>475575.99488002178</v>
       </c>
       <c r="D2" s="12">
         <v>460369.44223294902</v>
@@ -3191,7 +3203,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="12">
-        <v>470117.04863974027</v>
+        <v>470114.51380285382</v>
       </c>
       <c r="D3" s="12">
         <v>514395.68177236198</v>
@@ -3205,7 +3217,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="12">
-        <v>493688.23277629726</v>
+        <v>493690.48358295608</v>
       </c>
       <c r="D4" s="12">
         <v>481151.97994350799</v>
@@ -3219,7 +3231,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="12">
-        <v>501074.80040353234</v>
+        <v>501079.7883181842</v>
       </c>
       <c r="D5" s="12">
         <v>484543.67687656201</v>
@@ -3233,7 +3245,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12">
-        <v>515466.69291128084</v>
+        <v>515485.07610400004</v>
       </c>
       <c r="D6" s="12">
         <v>493602.53057785501</v>
@@ -3247,7 +3259,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="12">
-        <v>526287.52177886781</v>
+        <v>526246.42406031769</v>
       </c>
       <c r="D7" s="12">
         <v>581668.24987960199</v>
@@ -3261,7 +3273,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12">
-        <v>529905.85124294367</v>
+        <v>529925.52491045627</v>
       </c>
       <c r="D8" s="12">
         <v>514697.78950542799</v>
@@ -3275,7 +3287,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="12">
-        <v>540563.70408056455</v>
+        <v>540566.74493888335</v>
       </c>
       <c r="D9" s="12">
         <v>522255.20005077199</v>
@@ -3289,7 +3301,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="12">
-        <v>554560.99902440561</v>
+        <v>554542.19231067074</v>
       </c>
       <c r="D10" s="12">
         <v>532348.21201691695</v>
@@ -3303,7 +3315,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="12">
-        <v>561169.81491956639</v>
+        <v>561184.20725406578</v>
       </c>
       <c r="D11" s="12">
         <v>614076.39260854397</v>
@@ -3317,7 +3329,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="12">
-        <v>576896.43518582615</v>
+        <v>576884.8992080309</v>
       </c>
       <c r="D12" s="12">
         <v>562978.96562687703</v>
@@ -3331,7 +3343,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="12">
-        <v>589570.36775312782</v>
+        <v>589586.3181101589</v>
       </c>
       <c r="D13" s="12">
         <v>572794.04663058801</v>
@@ -3345,7 +3357,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="12">
-        <v>603213.94885090971</v>
+        <v>603183.508143752</v>
       </c>
       <c r="D14" s="12">
         <v>576846.88569942699</v>
@@ -3359,7 +3371,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="12">
-        <v>616210.69847655308</v>
+        <v>616227.38491072564</v>
       </c>
       <c r="D15" s="12">
         <v>674620.563006485</v>
@@ -3373,7 +3385,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="12">
-        <v>624573.91952353565</v>
+        <v>624501.02919283113</v>
       </c>
       <c r="D16" s="12">
         <v>610425.69401485403</v>
@@ -3387,7 +3399,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="12">
-        <v>643771.44373336376</v>
+        <v>643858.08833705308</v>
       </c>
       <c r="D17" s="12">
         <v>625876.867863597</v>
@@ -3401,7 +3413,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="12">
-        <v>649568.57853084186</v>
+        <v>649498.56629899354</v>
       </c>
       <c r="D18" s="12">
         <v>616720.35706447798</v>
@@ -3415,7 +3427,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="12">
-        <v>653329.88824301912</v>
+        <v>653395.98861577117</v>
       </c>
       <c r="D19" s="12">
         <v>711405.50045523304</v>
@@ -3429,7 +3441,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="12">
-        <v>658526.0855344407</v>
+        <v>658445.79814075422</v>
       </c>
       <c r="D20" s="12">
         <v>647087.95974249404</v>
@@ -3443,7 +3455,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="12">
-        <v>627280.08665654622</v>
+        <v>627364.28590933036</v>
       </c>
       <c r="D21" s="12">
         <v>613490.82170264097</v>
@@ -3457,7 +3469,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>604353.82403393742</v>
+        <v>604251.23977672984</v>
       </c>
       <c r="D22" s="12">
         <v>578553.04424240498</v>
@@ -3471,7 +3483,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="12">
-        <v>591077.75225373311</v>
+        <v>591197.81675977737</v>
       </c>
       <c r="D23" s="12">
         <v>631197.75186006899</v>
@@ -3485,7 +3497,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="12">
-        <v>614278.67717957112</v>
+        <v>614251.77704788849</v>
       </c>
       <c r="D24" s="12">
         <v>610519.85461172694</v>
@@ -3499,7 +3511,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="12">
-        <v>625781.2521842561</v>
+        <v>625790.67206710181</v>
       </c>
       <c r="D25" s="12">
         <v>615220.85493729694</v>
@@ -3513,7 +3525,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="12">
-        <v>644789.01313001418</v>
+        <v>644656.33509278321</v>
       </c>
       <c r="D26" s="12">
         <v>611607.33658973</v>
@@ -3527,7 +3539,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="12">
-        <v>673595.52769258386</v>
+        <v>673796.62357125268</v>
       </c>
       <c r="D27" s="12">
         <v>733730.773968903</v>
@@ -3541,7 +3553,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="12">
-        <v>677244.35343238455</v>
+        <v>677245.75810220244</v>
       </c>
       <c r="D28" s="12">
         <v>668566.50948898599</v>
@@ -3555,7 +3567,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="12">
-        <v>686465.82351221156</v>
+        <v>686396.0010009557</v>
       </c>
       <c r="D29" s="12">
         <v>668190.097719574</v>
@@ -3569,7 +3581,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="12">
-        <v>702910.30347114604</v>
+        <v>702822.18023114896</v>
       </c>
       <c r="D30" s="12">
         <v>662325.58597269503</v>
@@ -3583,7 +3595,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="12">
-        <v>709227.10753214906</v>
+        <v>709453.73073667835</v>
       </c>
       <c r="D31" s="12">
         <v>766332.95457161299</v>
@@ -3597,7 +3609,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="12">
-        <v>715183.40697330865</v>
+        <v>715217.07363846607</v>
       </c>
       <c r="D32" s="12">
         <v>711417.39193010505</v>
@@ -3611,7 +3623,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="12">
-        <v>715805.57090580289</v>
+        <v>715633.40427611268</v>
       </c>
       <c r="D33" s="12">
         <v>703050.45640799298</v>
@@ -3625,7 +3637,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="12">
-        <v>708101.0604378581</v>
+        <v>707973.57480664295</v>
       </c>
       <c r="D34" s="12">
         <v>672685.993630504</v>
@@ -3639,7 +3651,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="12">
-        <v>683290.8369353821</v>
+        <v>683580.91010547569</v>
       </c>
       <c r="D35" s="12">
         <v>730838.27259277599</v>
@@ -3653,7 +3665,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="12">
-        <v>705279.72688988189</v>
+        <v>705262.62855204311</v>
       </c>
       <c r="D36" s="12">
         <v>703461.65253019601</v>
@@ -3667,7 +3679,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="12">
-        <v>717272.33357267547</v>
+        <v>717126.84437163593</v>
       </c>
       <c r="D37" s="12">
         <v>706958.03908231901</v>
@@ -3681,7 +3693,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="12">
-        <v>717112.53673472651</v>
+        <v>717060.7430119497</v>
       </c>
       <c r="D38" s="12">
         <v>677085.52917315101</v>
@@ -3695,7 +3707,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="12">
-        <v>720685.28631943744</v>
+        <v>720875.2460696802</v>
       </c>
       <c r="D39" s="12">
         <v>776486.60279942001</v>
@@ -3709,7 +3721,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="12">
-        <v>725535.58742117661</v>
+        <v>725496.14859723055</v>
       </c>
       <c r="D40" s="12">
         <v>721458.94421618199</v>
@@ -3723,7 +3735,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="12">
-        <v>718295.01073591749</v>
+        <v>718196.28353239805</v>
       </c>
       <c r="D41" s="12">
         <v>706597.34502250701</v>
@@ -3737,7 +3749,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="12">
-        <v>707558.45852418256</v>
+        <v>707504.85521262127</v>
       </c>
       <c r="D42" s="12">
         <v>671066.04663506302</v>
@@ -3751,7 +3763,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="12">
-        <v>703181.56088816281</v>
+        <v>703306.5882396599</v>
       </c>
       <c r="D43" s="12">
         <v>760576.86834800395</v>
@@ -3765,7 +3777,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="12">
-        <v>697574.98650736373</v>
+        <v>697497.41833730193</v>
       </c>
       <c r="D44" s="12">
         <v>690879.79825168301</v>
@@ -3779,7 +3791,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="12">
-        <v>700909.1779337523</v>
+        <v>700915.32206387667</v>
       </c>
       <c r="D45" s="12">
         <v>686701.47061871097</v>
@@ -3793,7 +3805,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="12">
-        <v>711343.55056484032</v>
+        <v>711375.93314010161</v>
       </c>
       <c r="D46" s="12">
         <v>672749.81139169901</v>
@@ -3807,7 +3819,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="12">
-        <v>728061.55982454459</v>
+        <v>728089.28302817431</v>
       </c>
       <c r="D47" s="12">
         <v>791235.96554166998</v>
@@ -3821,7 +3833,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="12">
-        <v>727465.84170856164</v>
+        <v>727364.1882352829</v>
       </c>
       <c r="D48" s="12">
         <v>718281.26544978202</v>
@@ -3835,7 +3847,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="12">
-        <v>719077.63445421401</v>
+        <v>719119.18214860151</v>
       </c>
       <c r="D49" s="12">
         <v>703681.54416900803</v>
@@ -3849,7 +3861,7 @@
         <v>29</v>
       </c>
       <c r="C50" s="12">
-        <v>712792.50733871781</v>
+        <v>712838.59891063347</v>
       </c>
       <c r="D50" s="12">
         <v>677652.08911570301</v>
@@ -3864,7 +3876,7 @@
         <v>30</v>
       </c>
       <c r="C51" s="12">
-        <v>701694.24333017843</v>
+        <v>701661.62402498827</v>
       </c>
       <c r="D51" s="12">
         <v>760703.28015165601</v>
@@ -3879,7 +3891,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="12">
-        <v>703628.70200198307</v>
+        <v>703502.85074439459</v>
       </c>
       <c r="D52" s="12">
         <v>694382.47577623103</v>
@@ -3894,7 +3906,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="12">
-        <v>707795.94171976787</v>
+        <v>707908.32071062957</v>
       </c>
       <c r="D53" s="12">
         <v>693173.54934705805</v>
@@ -3909,7 +3921,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="12">
-        <v>714635.17781266733</v>
+        <v>714595.91167597554</v>
       </c>
       <c r="D54" s="12">
         <v>681444.76611022197</v>
@@ -3924,7 +3936,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="12">
-        <v>722379.15414712264</v>
+        <v>722352.21513637132</v>
       </c>
       <c r="D55" s="12">
         <v>778401.67644931702</v>
@@ -3939,7 +3951,7 @@
         <v>31</v>
       </c>
       <c r="C56" s="12">
-        <v>730527.41861531767</v>
+        <v>730431.25721323024</v>
       </c>
       <c r="D56" s="12">
         <v>721120.42685279401</v>
@@ -3954,7 +3966,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="12">
-        <v>738018.04047618899</v>
+        <v>738180.4070257179</v>
       </c>
       <c r="D57" s="12">
         <v>724592.92163896305</v>
@@ -3969,7 +3981,7 @@
         <v>29</v>
       </c>
       <c r="C58" s="12">
-        <v>736289.24838678283</v>
+        <v>736153.86066421203</v>
       </c>
       <c r="D58" s="12">
         <v>707324.26805721398</v>
@@ -3984,7 +3996,7 @@
         <v>30</v>
       </c>
       <c r="C59" s="12">
-        <v>702642.23655074975</v>
+        <v>702572.73159596475</v>
       </c>
       <c r="D59" s="12">
         <v>747428.29995457502</v>
@@ -3999,7 +4011,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="12">
-        <v>700254.09096364852</v>
+        <v>700278.87950862665</v>
       </c>
       <c r="D60" s="12">
         <v>696101.58352180803</v>
@@ -4014,7 +4026,7 @@
         <v>32</v>
       </c>
       <c r="C61" s="12">
-        <v>690324.19601686858</v>
+        <v>690504.300149246</v>
       </c>
       <c r="D61" s="12">
         <v>678655.62038445403</v>
@@ -4029,7 +4041,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="12">
-        <v>692058.14479226689</v>
+        <v>691669.02698322793</v>
       </c>
       <c r="D62" s="12">
         <v>665690.59065187594</v>
@@ -4044,7 +4056,7 @@
         <v>30</v>
       </c>
       <c r="C63" s="12">
-        <v>696592.48711725208</v>
+        <v>696755.15893017035</v>
       </c>
       <c r="D63" s="12">
         <v>751765.13811138296</v>
@@ -4059,7 +4071,7 @@
         <v>31</v>
       </c>
       <c r="C64" s="12">
-        <v>697682.90181394049</v>
+        <v>697871.69467852404</v>
       </c>
       <c r="D64" s="12">
         <v>683911.44245860004</v>
@@ -4074,7 +4086,7 @@
         <v>32</v>
       </c>
       <c r="C65" s="12">
-        <v>685852.2310998576</v>
+        <v>685889.88423139369</v>
       </c>
       <c r="D65" s="11">
         <v>670818.59360145801</v>
@@ -4089,7 +4101,7 @@
         <v>29</v>
       </c>
       <c r="C66" s="11">
-        <v>658858.00489083584</v>
+        <v>657839.92130941316</v>
       </c>
       <c r="D66" s="11">
         <v>632469.10245408595</v>
@@ -4104,7 +4116,7 @@
         <v>30</v>
       </c>
       <c r="C67" s="11">
-        <v>559239.1902047121</v>
+        <v>559729.96657034964</v>
       </c>
       <c r="D67" s="11">
         <v>608823.50379551796</v>
@@ -4119,7 +4131,7 @@
         <v>31</v>
       </c>
       <c r="C68" s="11">
-        <v>625831.78875105421</v>
+        <v>626201.59661515127</v>
       </c>
       <c r="D68" s="11">
         <v>614416.20615719398</v>
@@ -4134,7 +4146,7 @@
         <v>32</v>
       </c>
       <c r="C69" s="11">
-        <v>653941.54519373132</v>
+        <v>654099.04286113894</v>
       </c>
       <c r="D69" s="11">
         <v>642161.71494925604</v>
@@ -4149,7 +4161,7 @@
         <v>29</v>
       </c>
       <c r="C70" s="11">
-        <v>675578.64671226148</v>
+        <v>675141.32047996053</v>
       </c>
       <c r="D70">
         <v>650821.34239924757</v>
@@ -4164,7 +4176,7 @@
         <v>30</v>
       </c>
       <c r="C71" s="11">
-        <v>669236.91863885184</v>
+        <v>671345.36190175533</v>
       </c>
       <c r="D71">
         <v>717967.93370259111</v>
@@ -4179,10 +4191,24 @@
         <v>31</v>
       </c>
       <c r="C72" s="11">
-        <v>696523.61811405595</v>
+        <v>698467.0832059501</v>
       </c>
       <c r="D72" s="11">
-        <v>687344.44412307488</v>
+        <v>687786.64721903251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="11">
+        <v>2021</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="11">
+        <v>709292.21856571629</v>
+      </c>
+      <c r="D73" s="11">
+        <v>697670.06530119025</v>
       </c>
     </row>
   </sheetData>
@@ -4208,14 +4234,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4819,14 +4845,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4975,7 +5001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
@@ -5003,14 +5029,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="35">
-        <v>881</v>
-      </c>
-      <c r="C2" s="35">
-        <v>1094</v>
+        <v>1850</v>
+      </c>
+      <c r="C2" s="43">
+        <v>2328</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-213</v>
+        <v>-478</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5018,14 +5044,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="35">
-        <v>351</v>
-      </c>
-      <c r="C3">
-        <v>53</v>
+        <v>781</v>
+      </c>
+      <c r="C3" s="43">
+        <v>125</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>298</v>
+        <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5033,14 +5059,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="35">
-        <v>354</v>
-      </c>
-      <c r="C4" s="35">
-        <v>167</v>
+        <v>746</v>
+      </c>
+      <c r="C4" s="43">
+        <v>307</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>187</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5048,14 +5074,14 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>53</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>123</v>
+      </c>
+      <c r="C5" s="43">
+        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,14 +5089,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="35">
-        <v>364</v>
-      </c>
-      <c r="C6" s="35">
-        <v>495</v>
+        <v>1031</v>
+      </c>
+      <c r="C6" s="43">
+        <v>1137</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-131</v>
+        <v>-106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5078,14 +5104,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="35">
-        <v>836</v>
-      </c>
-      <c r="C7" s="35">
-        <v>842</v>
+        <v>1737</v>
+      </c>
+      <c r="C7" s="43">
+        <v>1715</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5093,14 +5119,14 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>67</v>
+        <v>77</v>
+      </c>
+      <c r="C8" s="43">
+        <v>138</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-47</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5108,14 +5134,14 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>85</v>
-      </c>
-      <c r="C9">
-        <v>53</v>
+        <v>152</v>
+      </c>
+      <c r="C9" s="43">
+        <v>80</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5123,14 +5149,14 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>93</v>
-      </c>
-      <c r="C10">
-        <v>33</v>
+        <v>142</v>
+      </c>
+      <c r="C10" s="43">
+        <v>44</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5138,14 +5164,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="35">
-        <v>423</v>
-      </c>
-      <c r="C11" s="35">
-        <v>337</v>
+        <v>1098</v>
+      </c>
+      <c r="C11" s="43">
+        <v>647</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5153,14 +5179,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="35">
-        <v>373</v>
-      </c>
-      <c r="C12" s="35">
-        <v>1508</v>
+        <v>775</v>
+      </c>
+      <c r="C12" s="43">
+        <v>2779</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-1135</v>
+        <v>-2004</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5168,14 +5194,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="35">
-        <v>114</v>
-      </c>
-      <c r="C13">
-        <v>52</v>
+        <v>174</v>
+      </c>
+      <c r="C13" s="43">
+        <v>120</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5183,14 +5209,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="35">
-        <v>21</v>
-      </c>
-      <c r="C14" s="35">
-        <v>78</v>
+        <v>58</v>
+      </c>
+      <c r="C14" s="43">
+        <v>161</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-57</v>
+        <v>-103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5198,14 +5224,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="35">
-        <v>263</v>
-      </c>
-      <c r="C15" s="35">
-        <v>137</v>
+        <v>511</v>
+      </c>
+      <c r="C15" s="43">
+        <v>293</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5213,14 +5239,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="35">
-        <v>213</v>
-      </c>
-      <c r="C16" s="35">
-        <v>90</v>
+        <v>582</v>
+      </c>
+      <c r="C16" s="43">
+        <v>480</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5228,14 +5254,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="35">
-        <v>344</v>
-      </c>
-      <c r="C17">
-        <v>14</v>
+        <v>673</v>
+      </c>
+      <c r="C17" s="43">
+        <v>36</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>330</v>
+        <v>637</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5243,14 +5269,14 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>92</v>
-      </c>
-      <c r="C18">
-        <v>23</v>
+        <v>120</v>
+      </c>
+      <c r="C18" s="43">
+        <v>42</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5258,14 +5284,14 @@
         <v>96</v>
       </c>
       <c r="B19">
-        <v>72</v>
-      </c>
-      <c r="C19">
-        <v>45</v>
+        <v>112</v>
+      </c>
+      <c r="C19" s="43">
+        <v>84</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5273,14 +5299,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="35">
-        <v>596</v>
-      </c>
-      <c r="C20" s="35">
-        <v>160</v>
+        <v>1249</v>
+      </c>
+      <c r="C20" s="44">
+        <v>365</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>436</v>
+        <v>884</v>
       </c>
     </row>
   </sheetData>
@@ -5294,7 +5320,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5319,10 +5345,10 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>569629.40890678659</v>
+        <v>580109.3654135036</v>
       </c>
       <c r="C2">
-        <v>11.397276043853299</v>
+        <v>8.2176039378516919</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5330,10 +5356,10 @@
         <v>102</v>
       </c>
       <c r="B3">
-        <v>34778.948230747541</v>
+        <v>36648.13652029309</v>
       </c>
       <c r="C3">
-        <v>-0.84794445835578713</v>
+        <v>4.3860998002780427</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5341,10 +5367,10 @@
         <v>103</v>
       </c>
       <c r="B4">
-        <v>3738.9140914018044</v>
+        <v>1249.7113603560397</v>
       </c>
       <c r="C4">
-        <v>34.730552426653084</v>
+        <v>-19.150143374614757</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5352,10 +5378,10 @@
         <v>104</v>
       </c>
       <c r="B5">
-        <v>21713.233857963307</v>
+        <v>22724.129989370613</v>
       </c>
       <c r="C5">
-        <v>13.145985625751354</v>
+        <v>18.247420162936258</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5363,10 +5389,10 @@
         <v>105</v>
       </c>
       <c r="B6">
-        <v>119933.99121636405</v>
+        <v>122710.03414797327</v>
       </c>
       <c r="C6">
-        <v>12.728493869734736</v>
+        <v>8.543915384800993</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5374,10 +5400,10 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <v>13395.50707056335</v>
+        <v>12285.490130430609</v>
       </c>
       <c r="C7">
-        <v>5.6213435666422562</v>
+        <v>0.49655622972446523</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5385,10 +5411,10 @@
         <v>107</v>
       </c>
       <c r="B8">
-        <v>21715.967786364865</v>
+        <v>20987.63967740133</v>
       </c>
       <c r="C8">
-        <v>25.185695615024596</v>
+        <v>4.5268786278615414</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5396,10 +5422,10 @@
         <v>108</v>
       </c>
       <c r="B9">
-        <v>91487.844850292531</v>
+        <v>93443.748235928695</v>
       </c>
       <c r="C9">
-        <v>11.072848471409035</v>
+        <v>7.2357992351878675</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5407,10 +5433,10 @@
         <v>109</v>
       </c>
       <c r="B10">
-        <v>7166.7167614790624</v>
+        <v>8992.2744681564727</v>
       </c>
       <c r="C10">
-        <v>59.782555864799988</v>
+        <v>60.938820792863964</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5418,10 +5444,10 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>49992.374065828524</v>
+        <v>51632.157894787102</v>
       </c>
       <c r="C11">
-        <v>11.704739911297812</v>
+        <v>14.905791213603869</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5429,10 +5455,10 @@
         <v>111</v>
       </c>
       <c r="B12">
-        <v>25371.087569978205</v>
+        <v>26151.467050546846</v>
       </c>
       <c r="C12">
-        <v>-7.6663383227870696E-3</v>
+        <v>0.37420012180280349</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5440,10 +5466,10 @@
         <v>112</v>
       </c>
       <c r="B13">
-        <v>77129.369084939375</v>
+        <v>79143.368376477825</v>
       </c>
       <c r="C13">
-        <v>8.7616924421587861</v>
+        <v>6.5567187004549332</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5451,10 +5477,10 @@
         <v>113</v>
       </c>
       <c r="B14">
-        <v>32777.443981278891</v>
+        <v>34930.018675685875</v>
       </c>
       <c r="C14">
-        <v>8.0276619288576647</v>
+        <v>11.909663098887879</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5462,10 +5488,10 @@
         <v>114</v>
       </c>
       <c r="B15">
-        <v>27683.57840795505</v>
+        <v>28516.783116102812</v>
       </c>
       <c r="C15">
-        <v>5.1249743402094428</v>
+        <v>6.1375814244809535</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5473,10 +5499,10 @@
         <v>115</v>
       </c>
       <c r="B16">
-        <v>24083.290055386617</v>
+        <v>22663.778591606671</v>
       </c>
       <c r="C16">
-        <v>10.707868644455832</v>
+        <v>2.422746472798476</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5484,10 +5510,10 @@
         <v>116</v>
       </c>
       <c r="B17">
-        <v>14855.887112915314</v>
+        <v>14327.889062242892</v>
       </c>
       <c r="C17">
-        <v>80.989403402298592</v>
+        <v>10.245849380753791</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5495,10 +5521,10 @@
         <v>117</v>
       </c>
       <c r="B18">
-        <v>3805.2547633282738</v>
+        <v>3702.7381161434578</v>
       </c>
       <c r="C18">
-        <v>13.50127591153154</v>
+        <v>1.7208283342252662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo datos de emae y pobreza'
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6029D67C-2B3C-4924-AB65-178B04D458E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7660632B-DADB-45EE-A076-CB8072B36581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -523,12 +523,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -569,6 +563,11 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -619,14 +618,14 @@
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
@@ -653,7 +652,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -669,37 +668,37 @@
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2025,7 +2024,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="36">
+      <c r="A59" s="35">
         <v>44470</v>
       </c>
       <c r="B59" s="1">
@@ -2059,7 +2058,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="36">
+      <c r="A61" s="35">
         <v>44531</v>
       </c>
       <c r="B61" s="1">
@@ -2093,7 +2092,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="36">
+      <c r="A63" s="35">
         <v>44593</v>
       </c>
       <c r="B63" s="1">
@@ -2158,22 +2157,22 @@
       <c r="A2" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="36">
         <v>5.8</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="36">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="36">
         <v>5.2</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="40">
         <v>3.7</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="36">
         <v>4.7</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="36">
         <v>5</v>
       </c>
       <c r="H2" s="21">
@@ -2184,22 +2183,22 @@
       <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="36">
         <v>5.7</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="36">
         <v>4.3</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="36">
         <v>3.9</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="40">
         <v>4</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="36">
         <v>5</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="36">
         <v>5.4</v>
       </c>
       <c r="H3" s="21">
@@ -2210,22 +2209,22 @@
       <c r="A4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="36">
         <v>6.5</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="36">
         <v>6.5</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <v>7.1</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="40">
         <v>8</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="36">
         <v>8.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>6</v>
       </c>
       <c r="H4" s="21">
@@ -2236,22 +2235,22 @@
       <c r="A5" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="36">
         <v>4.2</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36">
         <v>2.4</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="36">
         <v>5.3</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="40">
         <v>3.8</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <v>2.4</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="36">
         <v>3.7</v>
       </c>
       <c r="H5" s="21">
@@ -2262,22 +2261,22 @@
       <c r="A6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="36">
         <v>10.4</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <v>11</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="36">
         <v>11.5</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="40">
         <v>9</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <v>15.9</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="36">
         <v>8.5</v>
       </c>
       <c r="H6" s="21">
@@ -2288,22 +2287,22 @@
       <c r="A7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="36">
         <v>32.299999999999997</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="36">
         <v>22.6</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <v>18.600000000000001</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="40">
         <v>20.9</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="36">
         <v>23.5</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="36">
         <v>13.8</v>
       </c>
       <c r="H7" s="21">
@@ -2314,22 +2313,22 @@
       <c r="A8" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="36">
         <v>3.5</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="36">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="40">
         <v>5.2</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="36">
         <v>5.6</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="36">
         <v>2.7</v>
       </c>
       <c r="H8" s="22">
@@ -2340,22 +2339,22 @@
       <c r="A9" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="36">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="36">
         <v>2.8</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="36">
         <v>4.5</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="40">
         <v>3.4</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="36">
         <v>4.5</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="36">
         <v>3.8</v>
       </c>
       <c r="H9" s="21">
@@ -2366,22 +2365,22 @@
       <c r="A10" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="36">
         <v>3.8</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="36">
         <v>3.5</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="36">
         <v>5.3</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="40">
         <v>3.6</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="36">
         <v>4.2</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="36">
         <v>4.0999999999999996</v>
       </c>
       <c r="H10" s="21">
@@ -2437,19 +2436,19 @@
       <c r="B2" s="27">
         <v>4.7</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="38">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="38">
         <v>4.7</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="38">
         <v>5</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="38">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="38">
         <v>5.4</v>
       </c>
       <c r="H2" s="29">
@@ -2463,19 +2462,19 @@
       <c r="B3" s="26">
         <v>7.5</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>8.6</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="37">
         <v>6.7</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="37">
         <v>6.3</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="37">
         <v>6.3</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="37">
         <v>7.5</v>
       </c>
       <c r="H3" s="28">
@@ -2489,19 +2488,19 @@
       <c r="B4" s="26">
         <v>2.7</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="37">
         <v>2.7</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="37">
         <v>2.4</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="37">
         <v>4</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="37">
         <v>2.8</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="37">
         <v>2.9</v>
       </c>
       <c r="H4" s="28">
@@ -2515,19 +2514,19 @@
       <c r="B5" s="26">
         <v>3.4</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="37">
         <v>2.9</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="37">
         <v>3.9</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>3.1</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="37">
         <v>3.3</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="37">
         <v>3.7</v>
       </c>
       <c r="H5" s="28">
@@ -2541,19 +2540,19 @@
       <c r="B6" s="26">
         <v>2.8</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="37">
         <v>2.5</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="37">
         <v>3.7</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <v>2.5</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="37">
         <v>0.4</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="37">
         <v>4</v>
       </c>
       <c r="H6" s="28">
@@ -2567,19 +2566,19 @@
       <c r="B7" s="26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="37">
         <v>4.3</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="37">
         <v>4.7</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="37">
         <v>4.8</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="37">
         <v>4.2</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="37">
         <v>4.3</v>
       </c>
       <c r="H7" s="28">
@@ -2593,19 +2592,19 @@
       <c r="B8" s="26">
         <v>3.6</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="37">
         <v>3.1</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="37">
         <v>3.8</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="37">
         <v>4.8</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="37">
         <v>4.3</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="37">
         <v>4.3</v>
       </c>
       <c r="H8" s="28">
@@ -2619,19 +2618,19 @@
       <c r="B9" s="26">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="37">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="37">
         <v>5.5</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="37">
         <v>5.8</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="37">
         <v>5.7</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="37">
         <v>6.1</v>
       </c>
       <c r="H9" s="28">
@@ -2645,19 +2644,19 @@
       <c r="B10" s="26">
         <v>1.5</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="37">
         <v>1.6</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="37">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="37">
         <v>1.6</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <v>1.9</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="37">
         <v>2.7</v>
       </c>
       <c r="H10" s="28">
@@ -2671,19 +2670,19 @@
       <c r="B11" s="26">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="37">
         <v>1.4</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="37">
         <v>2.4</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="37">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="37">
         <v>4.2</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="37">
         <v>3.5</v>
       </c>
       <c r="H11" s="28">
@@ -2697,19 +2696,19 @@
       <c r="B12" s="26">
         <v>2.6</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="37">
         <v>2</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="37">
         <v>2.7</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="37">
         <v>7.1</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="37">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="37">
         <v>2.2999999999999998</v>
       </c>
       <c r="H12" s="28">
@@ -2723,19 +2722,19 @@
       <c r="B13" s="26">
         <v>4.3</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="37">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="37">
         <v>3</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="37">
         <v>4.3</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="37">
         <v>6.5</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="37">
         <v>6.1</v>
       </c>
       <c r="H13" s="28">
@@ -2749,19 +2748,19 @@
       <c r="B14" s="26">
         <v>4.3</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="37">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="37">
         <v>4.2</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="37">
         <v>4</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="37">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="37">
         <v>4.9000000000000004</v>
       </c>
       <c r="H14" s="28">
@@ -2817,22 +2816,22 @@
       <c r="B2" s="31">
         <v>52.3</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="39">
         <v>53.8</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="39">
         <v>51.1</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="39">
         <v>50</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="39">
         <v>50.9</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="39">
         <v>52</v>
       </c>
-      <c r="H2" s="40">
+      <c r="H2" s="39">
         <v>52.3</v>
       </c>
     </row>
@@ -4222,7 +4221,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+      <selection activeCell="B3" sqref="B3:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4234,14 +4233,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="42"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4261,561 +4260,561 @@
       <c r="A3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="33">
-        <v>31.2</v>
-      </c>
-      <c r="C3" s="33">
-        <v>40.6</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="B3">
+        <v>27.9</v>
+      </c>
+      <c r="C3">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="D3">
+        <v>6.1</v>
+      </c>
+      <c r="E3">
         <v>8.1999999999999993</v>
-      </c>
-      <c r="E3" s="33">
-        <v>10.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="33">
-        <v>10.1</v>
-      </c>
-      <c r="C4" s="33">
-        <v>13.9</v>
-      </c>
-      <c r="D4" s="33">
-        <v>1.9</v>
-      </c>
-      <c r="E4" s="33">
-        <v>2.2000000000000002</v>
+      <c r="B4">
+        <v>10.8</v>
+      </c>
+      <c r="C4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D4">
+        <v>1.8</v>
+      </c>
+      <c r="E4">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="33">
-        <v>37.1</v>
-      </c>
-      <c r="C5" s="33">
-        <v>45.3</v>
-      </c>
-      <c r="D5" s="33">
-        <v>11.2</v>
-      </c>
-      <c r="E5" s="33">
-        <v>13.8</v>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>42.3</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>10.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="33">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="C6" s="33">
-        <v>43.7</v>
-      </c>
-      <c r="D6" s="33">
-        <v>5.3</v>
-      </c>
-      <c r="E6" s="33">
-        <v>6.9</v>
+      <c r="B6">
+        <v>33.1</v>
+      </c>
+      <c r="C6">
+        <v>44.6</v>
+      </c>
+      <c r="D6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E6">
+        <v>7.2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="33">
-        <v>28.2</v>
-      </c>
-      <c r="C7" s="33">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="D7" s="33">
-        <v>4.5</v>
-      </c>
-      <c r="E7" s="33">
-        <v>6.3</v>
+      <c r="B7">
+        <v>28.3</v>
+      </c>
+      <c r="C7">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D7">
+        <v>3.4</v>
+      </c>
+      <c r="E7">
+        <v>4.8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="33">
-        <v>36</v>
-      </c>
-      <c r="C8" s="33">
-        <v>44.3</v>
-      </c>
-      <c r="D8" s="33">
-        <v>4.2</v>
-      </c>
-      <c r="E8" s="33">
-        <v>4.7</v>
+      <c r="B8">
+        <v>36.6</v>
+      </c>
+      <c r="C8">
+        <v>47.8</v>
+      </c>
+      <c r="D8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="33">
-        <v>32.9</v>
-      </c>
-      <c r="C9" s="33">
-        <v>43</v>
-      </c>
-      <c r="D9" s="33">
-        <v>6.9</v>
-      </c>
-      <c r="E9" s="33">
-        <v>9.1</v>
+      <c r="B9">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="C9">
+        <v>27.3</v>
+      </c>
+      <c r="D9">
+        <v>5.9</v>
+      </c>
+      <c r="E9">
+        <v>7.6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="33">
-        <v>37.9</v>
-      </c>
-      <c r="C10" s="33">
-        <v>47.4</v>
-      </c>
-      <c r="D10" s="33">
-        <v>11.6</v>
-      </c>
-      <c r="E10" s="33">
-        <v>15</v>
+      <c r="B10">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E10">
+        <v>12.8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="33">
-        <v>44.6</v>
-      </c>
-      <c r="C11" s="34">
-        <v>51.9</v>
-      </c>
-      <c r="D11" s="33">
-        <v>13.3</v>
-      </c>
-      <c r="E11" s="33">
-        <v>16.899999999999999</v>
+      <c r="B11">
+        <v>42.3</v>
+      </c>
+      <c r="C11">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="33">
-        <v>30</v>
-      </c>
-      <c r="C12" s="33">
-        <v>39.4</v>
-      </c>
-      <c r="D12" s="33">
-        <v>4.7</v>
-      </c>
-      <c r="E12" s="33">
-        <v>6.5</v>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>34.1</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3.8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="33">
-        <v>37.1</v>
-      </c>
-      <c r="C13" s="33">
-        <v>46</v>
-      </c>
-      <c r="D13" s="33">
-        <v>8</v>
-      </c>
-      <c r="E13" s="33">
-        <v>10</v>
+      <c r="B13">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C13" s="43">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="D13">
+        <v>8.5</v>
+      </c>
+      <c r="E13">
+        <v>10.8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="33">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="C14" s="33">
-        <v>46.2</v>
-      </c>
-      <c r="D14" s="33">
-        <v>9.6</v>
-      </c>
-      <c r="E14" s="33">
-        <v>11.6</v>
+      <c r="B14">
+        <v>34.9</v>
+      </c>
+      <c r="C14">
+        <v>42.7</v>
+      </c>
+      <c r="D14">
+        <v>7.2</v>
+      </c>
+      <c r="E14">
+        <v>7.9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="33">
-        <v>33.4</v>
-      </c>
-      <c r="C15" s="33">
-        <v>42.5</v>
-      </c>
-      <c r="D15" s="33">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E15" s="33">
-        <v>5.7</v>
+      <c r="B15">
+        <v>29.4</v>
+      </c>
+      <c r="C15">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>6.3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="33">
-        <v>26.7</v>
-      </c>
-      <c r="C16" s="33">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="D16" s="33">
-        <v>3.1</v>
-      </c>
-      <c r="E16" s="33">
-        <v>4.5999999999999996</v>
+      <c r="B16">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>3.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="33">
-        <v>33.9</v>
-      </c>
-      <c r="C17" s="33">
-        <v>42.3</v>
-      </c>
-      <c r="D17" s="33">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="E17" s="33">
-        <v>11.2</v>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>38.9</v>
+      </c>
+      <c r="D17">
+        <v>5.9</v>
+      </c>
+      <c r="E17">
+        <v>7.8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="33">
-        <v>38.6</v>
-      </c>
-      <c r="C18" s="33">
-        <v>50.2</v>
-      </c>
-      <c r="D18" s="33">
-        <v>4.3</v>
-      </c>
-      <c r="E18" s="33">
-        <v>6.1</v>
+      <c r="B18">
+        <v>27.2</v>
+      </c>
+      <c r="C18">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D18">
+        <v>2.7</v>
+      </c>
+      <c r="E18">
+        <v>4.2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="33">
-        <v>23.1</v>
-      </c>
-      <c r="C19" s="33">
-        <v>31.7</v>
-      </c>
-      <c r="D19" s="33">
-        <v>5.2</v>
-      </c>
-      <c r="E19" s="33">
-        <v>7.7</v>
+      <c r="B19">
+        <v>22.5</v>
+      </c>
+      <c r="C19">
+        <v>30.9</v>
+      </c>
+      <c r="D19">
+        <v>5.7</v>
+      </c>
+      <c r="E19">
+        <v>6.7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="33">
-        <v>44.4</v>
-      </c>
-      <c r="C20" s="33">
-        <v>56.1</v>
-      </c>
-      <c r="D20" s="33">
-        <v>11</v>
-      </c>
-      <c r="E20" s="33">
-        <v>15.8</v>
+      <c r="B20">
+        <v>40.6</v>
+      </c>
+      <c r="C20">
+        <v>51.5</v>
+      </c>
+      <c r="D20">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E20">
+        <v>10.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="33">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="C21" s="33">
-        <v>46.6</v>
-      </c>
-      <c r="D21" s="33">
-        <v>7.8</v>
-      </c>
-      <c r="E21" s="33">
-        <v>10.8</v>
+      <c r="B21">
+        <v>29.2</v>
+      </c>
+      <c r="C21">
+        <v>40.4</v>
+      </c>
+      <c r="D21">
+        <v>5.7</v>
+      </c>
+      <c r="E21">
+        <v>7.5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="33">
-        <v>30.9</v>
-      </c>
-      <c r="C22" s="33">
-        <v>41.5</v>
-      </c>
-      <c r="D22" s="33">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="E22" s="33">
-        <v>13.5</v>
+      <c r="B22">
+        <v>23.9</v>
+      </c>
+      <c r="C22">
+        <v>29.6</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>7.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="33">
-        <v>28.3</v>
-      </c>
-      <c r="C23" s="33">
-        <v>39.4</v>
-      </c>
-      <c r="D23" s="33">
-        <v>7.9</v>
-      </c>
-      <c r="E23" s="33">
-        <v>10.6</v>
+      <c r="B23">
+        <v>24.8</v>
+      </c>
+      <c r="C23">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>5.6</v>
+      </c>
+      <c r="E23">
+        <v>7.2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="33">
-        <v>27.8</v>
-      </c>
-      <c r="C24" s="33">
-        <v>37</v>
-      </c>
-      <c r="D24" s="33">
-        <v>6.1</v>
-      </c>
-      <c r="E24" s="33">
-        <v>8.5</v>
+      <c r="B24">
+        <v>21.8</v>
+      </c>
+      <c r="C24">
+        <v>29.8</v>
+      </c>
+      <c r="D24">
+        <v>3.6</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="33">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="C25" s="33">
-        <v>50.5</v>
-      </c>
-      <c r="D25" s="33">
-        <v>7.2</v>
-      </c>
-      <c r="E25" s="33">
-        <v>10.4</v>
+      <c r="B25">
+        <v>27.9</v>
+      </c>
+      <c r="C25">
+        <v>38.6</v>
+      </c>
+      <c r="D25">
+        <v>5.5</v>
+      </c>
+      <c r="E25">
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="33">
-        <v>27.2</v>
-      </c>
-      <c r="C26" s="33">
-        <v>35</v>
-      </c>
-      <c r="D26" s="33">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="E26" s="33">
-        <v>13.2</v>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>31.5</v>
+      </c>
+      <c r="D26">
+        <v>6.4</v>
+      </c>
+      <c r="E26">
+        <v>7.5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="33">
-        <v>29.7</v>
-      </c>
-      <c r="C27" s="33">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="D27" s="33">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E27" s="33">
-        <v>6.2</v>
+      <c r="B27">
+        <v>28.8</v>
+      </c>
+      <c r="C27">
+        <v>39.9</v>
+      </c>
+      <c r="D27">
+        <v>3.4</v>
+      </c>
+      <c r="E27">
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="33">
-        <v>25.8</v>
-      </c>
-      <c r="C28" s="33">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="D28" s="33">
-        <v>7.2</v>
-      </c>
-      <c r="E28" s="33">
-        <v>9.6</v>
+      <c r="B28">
+        <v>23.7</v>
+      </c>
+      <c r="C28">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="D28">
+        <v>9.1</v>
+      </c>
+      <c r="E28">
+        <v>13.8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="33">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="C29" s="33">
-        <v>47.1</v>
-      </c>
-      <c r="D29" s="33">
-        <v>8.5</v>
-      </c>
-      <c r="E29" s="33">
-        <v>11.2</v>
+      <c r="B29">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>7.1</v>
+      </c>
+      <c r="E29">
+        <v>10.3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="33">
-        <v>18.7</v>
-      </c>
-      <c r="C30" s="33">
-        <v>23.9</v>
-      </c>
-      <c r="D30" s="33">
-        <v>2.8</v>
-      </c>
-      <c r="E30" s="33">
-        <v>2.9</v>
+      <c r="B30">
+        <v>20.8</v>
+      </c>
+      <c r="C30">
+        <v>28.1</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>2.4</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="33">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="C31" s="33">
-        <v>41</v>
-      </c>
-      <c r="D31" s="33">
-        <v>7.5</v>
-      </c>
-      <c r="E31" s="33">
-        <v>9.8000000000000007</v>
+      <c r="B31">
+        <v>25.8</v>
+      </c>
+      <c r="C31">
+        <v>33.5</v>
+      </c>
+      <c r="D31">
+        <v>4.2</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="33">
-        <v>25.9</v>
-      </c>
-      <c r="C32" s="33">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="D32" s="33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E32" s="33">
-        <v>5.4</v>
+      <c r="B32">
+        <v>26.2</v>
+      </c>
+      <c r="C32">
+        <v>35.1</v>
+      </c>
+      <c r="D32">
+        <v>3.9</v>
+      </c>
+      <c r="E32">
+        <v>3.9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="33">
-        <v>27.4</v>
-      </c>
-      <c r="C33" s="33">
-        <v>36</v>
-      </c>
-      <c r="D33" s="33">
-        <v>3.3</v>
-      </c>
-      <c r="E33" s="33">
+      <c r="B33">
+        <v>20.6</v>
+      </c>
+      <c r="C33">
+        <v>27.1</v>
+      </c>
+      <c r="D33">
         <v>4.2</v>
+      </c>
+      <c r="E33">
+        <v>4.3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="33">
-        <v>26.2</v>
-      </c>
-      <c r="C34" s="33">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="D34" s="33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E34" s="33">
-        <v>5.5</v>
+      <c r="B34">
+        <v>26.7</v>
+      </c>
+      <c r="C34">
+        <v>35.5</v>
+      </c>
+      <c r="D34">
+        <v>3.1</v>
+      </c>
+      <c r="E34">
+        <v>4.2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="33">
-        <v>25</v>
-      </c>
-      <c r="C35" s="33">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="D35" s="33">
-        <v>3.6</v>
-      </c>
-      <c r="E35" s="33">
-        <v>4.8</v>
+      <c r="B35">
+        <v>22.5</v>
+      </c>
+      <c r="C35">
+        <v>31</v>
+      </c>
+      <c r="D35">
+        <v>2.7</v>
+      </c>
+      <c r="E35">
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>
@@ -4833,7 +4832,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E9"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,14 +4844,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="42"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4873,16 +4872,16 @@
         <v>71</v>
       </c>
       <c r="B3" s="33">
-        <v>31.2</v>
+        <v>27.9</v>
       </c>
       <c r="C3" s="33">
-        <v>40.6</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="D3" s="33">
+        <v>6.1</v>
+      </c>
+      <c r="E3" s="33">
         <v>8.1999999999999993</v>
-      </c>
-      <c r="E3" s="33">
-        <v>10.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4890,16 +4889,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="33">
-        <v>32.200000000000003</v>
+        <v>27.7</v>
       </c>
       <c r="C4" s="33">
-        <v>41.5</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="D4" s="33">
-        <v>4.9000000000000004</v>
+        <v>6.6</v>
       </c>
       <c r="E4" s="33">
-        <v>6.4</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4907,16 +4906,16 @@
         <v>72</v>
       </c>
       <c r="B5" s="33">
-        <v>30.5</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="C5" s="33">
-        <v>39.200000000000003</v>
+        <v>42.7</v>
       </c>
       <c r="D5" s="33">
-        <v>8.9</v>
+        <v>4.5</v>
       </c>
       <c r="E5" s="33">
-        <v>11.5</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4924,16 +4923,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="33">
-        <v>36.299999999999997</v>
+        <v>30.4</v>
       </c>
       <c r="C6" s="33">
-        <v>45.4</v>
+        <v>39.4</v>
       </c>
       <c r="D6" s="33">
-        <v>8.9</v>
+        <v>8.1</v>
       </c>
       <c r="E6" s="33">
-        <v>11.7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4941,16 +4940,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="33">
-        <v>35</v>
+        <v>31.1</v>
       </c>
       <c r="C7" s="33">
-        <v>44.7</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="D7" s="33">
-        <v>7.3</v>
+        <v>5.7</v>
       </c>
       <c r="E7" s="33">
-        <v>9.1999999999999993</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4958,16 +4957,16 @@
         <v>73</v>
       </c>
       <c r="B8" s="33">
-        <v>31</v>
+        <v>26.2</v>
       </c>
       <c r="C8" s="33">
-        <v>42.1</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D8" s="33">
-        <v>8</v>
+        <v>5.8</v>
       </c>
       <c r="E8" s="33">
-        <v>11.1</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4975,16 +4974,16 @@
         <v>74</v>
       </c>
       <c r="B9" s="33">
-        <v>26.3</v>
+        <v>23.8</v>
       </c>
       <c r="C9" s="33">
-        <v>34.4</v>
+        <v>31.5</v>
       </c>
       <c r="D9" s="33">
-        <v>4.5999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="E9" s="33">
-        <v>5.9</v>
+        <v>4.2</v>
       </c>
     </row>
   </sheetData>
@@ -5001,7 +5000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
@@ -5028,10 +5027,10 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="34">
         <v>1850</v>
       </c>
-      <c r="C2" s="43">
+      <c r="C2" s="41">
         <v>2328</v>
       </c>
       <c r="D2">
@@ -5043,10 +5042,10 @@
       <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="34">
         <v>781</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="41">
         <v>125</v>
       </c>
       <c r="D3">
@@ -5058,10 +5057,10 @@
       <c r="A4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="34">
         <v>746</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="41">
         <v>307</v>
       </c>
       <c r="D4">
@@ -5076,7 +5075,7 @@
       <c r="B5">
         <v>123</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="41">
         <v>5</v>
       </c>
       <c r="D5">
@@ -5088,10 +5087,10 @@
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="34">
         <v>1031</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="41">
         <v>1137</v>
       </c>
       <c r="D6">
@@ -5103,10 +5102,10 @@
       <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="34">
         <v>1737</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="41">
         <v>1715</v>
       </c>
       <c r="D7">
@@ -5121,7 +5120,7 @@
       <c r="B8">
         <v>77</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="41">
         <v>138</v>
       </c>
       <c r="D8">
@@ -5136,7 +5135,7 @@
       <c r="B9">
         <v>152</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="41">
         <v>80</v>
       </c>
       <c r="D9">
@@ -5151,7 +5150,7 @@
       <c r="B10">
         <v>142</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="41">
         <v>44</v>
       </c>
       <c r="D10">
@@ -5163,10 +5162,10 @@
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="34">
         <v>1098</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="41">
         <v>647</v>
       </c>
       <c r="D11">
@@ -5178,10 +5177,10 @@
       <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="34">
         <v>775</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="41">
         <v>2779</v>
       </c>
       <c r="D12">
@@ -5193,10 +5192,10 @@
       <c r="A13" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="34">
         <v>174</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="41">
         <v>120</v>
       </c>
       <c r="D13">
@@ -5208,10 +5207,10 @@
       <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="34">
         <v>58</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="41">
         <v>161</v>
       </c>
       <c r="D14">
@@ -5223,10 +5222,10 @@
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="34">
         <v>511</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="41">
         <v>293</v>
       </c>
       <c r="D15">
@@ -5238,10 +5237,10 @@
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="34">
         <v>582</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="41">
         <v>480</v>
       </c>
       <c r="D16">
@@ -5253,10 +5252,10 @@
       <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="34">
         <v>673</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="41">
         <v>36</v>
       </c>
       <c r="D17">
@@ -5271,7 +5270,7 @@
       <c r="B18">
         <v>120</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="41">
         <v>42</v>
       </c>
       <c r="D18">
@@ -5286,7 +5285,7 @@
       <c r="B19">
         <v>112</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="41">
         <v>84</v>
       </c>
       <c r="D19">
@@ -5298,10 +5297,10 @@
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="34">
         <v>1249</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="42">
         <v>365</v>
       </c>
       <c r="D20">
@@ -5535,10 +5534,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5570,10 +5569,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="23">
-        <v>148.18349369128583</v>
+        <v>148.139109026689</v>
       </c>
       <c r="D2" s="23">
-        <v>147.0621449260093</v>
+        <v>147.07160840981032</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5584,10 +5583,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="23">
-        <v>146.69673264137583</v>
+        <v>146.69961289140326</v>
       </c>
       <c r="D3" s="23">
-        <v>146.46931916127502</v>
+        <v>146.483967919158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5598,10 +5597,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="23">
-        <v>145.97222771976445</v>
+        <v>145.98766697459678</v>
       </c>
       <c r="D4" s="23">
-        <v>145.91393396103376</v>
+        <v>145.93285377374565</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5612,10 +5611,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="23">
-        <v>145.22398006632829</v>
+        <v>145.19812212033054</v>
       </c>
       <c r="D5" s="23">
-        <v>145.43242759617519</v>
+        <v>145.45428715899183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5626,10 +5625,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="23">
-        <v>144.36754489711953</v>
+        <v>144.40215353738799</v>
       </c>
       <c r="D6" s="23">
-        <v>145.05270951514441</v>
+        <v>145.07564667926081</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5640,10 +5639,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="23">
-        <v>144.29996705649847</v>
+        <v>144.31416221953438</v>
       </c>
       <c r="D7" s="23">
-        <v>144.79666657392883</v>
+        <v>144.81868281054562</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5654,10 +5653,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="23">
-        <v>144.39192328281442</v>
+        <v>144.38741543887232</v>
       </c>
       <c r="D8" s="23">
-        <v>144.67341355232986</v>
+        <v>144.69235979593122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5668,10 +5667,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="23">
-        <v>145.57360477998151</v>
+        <v>145.60608227735642</v>
       </c>
       <c r="D9" s="23">
-        <v>144.68565025066377</v>
+        <v>144.69966672624665</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5682,10 +5681,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="23">
-        <v>145.09040295998474</v>
+        <v>145.05957284321801</v>
       </c>
       <c r="D10" s="23">
-        <v>144.82907618536532</v>
+        <v>144.83734366484433</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5696,10 +5695,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="23">
-        <v>145.06323892412777</v>
+        <v>145.09420974714644</v>
       </c>
       <c r="D11" s="23">
-        <v>145.09419953467454</v>
+        <v>145.09553807592803</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5710,10 +5709,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="23">
-        <v>145.74098249463347</v>
+        <v>145.74632296742948</v>
       </c>
       <c r="D12" s="23">
-        <v>145.46533963871997</v>
+        <v>145.45889352267432</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5724,10 +5723,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="23">
-        <v>146.96725526102128</v>
+        <v>146.93692372907955</v>
       </c>
       <c r="D13" s="23">
-        <v>145.92874460657271</v>
+        <v>145.91424840331939</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5735,13 +5734,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="23">
-        <v>136.63265948871936</v>
+        <v>136.63265948871938</v>
       </c>
       <c r="C14" s="23">
-        <v>147.41374726175283</v>
+        <v>147.41113461204898</v>
       </c>
       <c r="D14" s="23">
-        <v>146.4676463258906</v>
+        <v>146.44567113324348</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5752,10 +5751,10 @@
         <v>132.15851634216529</v>
       </c>
       <c r="C15" s="23">
-        <v>146.52537665594733</v>
+        <v>146.54015048204971</v>
       </c>
       <c r="D15" s="23">
-        <v>147.06447138021485</v>
+        <v>147.03645254032813</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5763,13 +5762,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="23">
-        <v>152.62095855115732</v>
+        <v>152.62095855115726</v>
       </c>
       <c r="C16" s="23">
-        <v>148.03947623052244</v>
+        <v>147.96184326764569</v>
       </c>
       <c r="D16" s="23">
-        <v>147.69982338122074</v>
+        <v>147.66785461517631</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5777,13 +5776,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="23">
-        <v>151.94634477931689</v>
+        <v>151.9463447793168</v>
       </c>
       <c r="C17" s="23">
-        <v>147.78602285073043</v>
+        <v>147.85652396642445</v>
       </c>
       <c r="D17" s="23">
-        <v>148.35126469826446</v>
+        <v>148.31778988846486</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5791,13 +5790,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="23">
-        <v>168.38920945875753</v>
+        <v>168.38920945875748</v>
       </c>
       <c r="C18" s="23">
-        <v>148.65492360321201</v>
+        <v>148.63747781535935</v>
       </c>
       <c r="D18" s="23">
-        <v>148.99144679605089</v>
+        <v>148.95898986593699</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5805,13 +5804,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="23">
-        <v>161.03568550523286</v>
+        <v>161.03568550523303</v>
       </c>
       <c r="C19" s="23">
-        <v>150.24996585517863</v>
+        <v>150.21570079862281</v>
       </c>
       <c r="D19" s="23">
-        <v>149.58823150996582</v>
+        <v>149.5591524303201</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5819,13 +5818,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="23">
-        <v>150.30605023792197</v>
+        <v>150.30605023792245</v>
       </c>
       <c r="C20" s="23">
-        <v>150.2475934817972</v>
+        <v>150.24764115729232</v>
       </c>
       <c r="D20" s="23">
-        <v>150.10859407438372</v>
+        <v>150.08456108965771</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5833,13 +5832,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="23">
-        <v>149.25534282189687</v>
+        <v>149.2553428218971</v>
       </c>
       <c r="C21" s="23">
-        <v>150.21255472865508</v>
+        <v>150.25055553146149</v>
       </c>
       <c r="D21" s="23">
-        <v>150.51864680110404</v>
+        <v>150.50051560049172</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5847,13 +5846,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="23">
-        <v>146.38655949569588</v>
+        <v>146.3865594956952</v>
       </c>
       <c r="C22" s="23">
-        <v>151.20691509597376</v>
+        <v>151.20766483968907</v>
       </c>
       <c r="D22" s="23">
-        <v>150.78576569647694</v>
+        <v>150.77373680025241</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5861,13 +5860,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="23">
-        <v>149.38594914967516</v>
+        <v>149.38594914967302</v>
       </c>
       <c r="C23" s="23">
-        <v>151.48595488640765</v>
+        <v>151.54451595688116</v>
       </c>
       <c r="D23" s="23">
-        <v>150.8845607730164</v>
+        <v>150.87793260807464</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5875,13 +5874,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="23">
-        <v>151.92604263437167</v>
+        <v>151.92604263437079</v>
       </c>
       <c r="C24" s="23">
-        <v>152.56546404872461</v>
+        <v>152.60793090348429</v>
       </c>
       <c r="D24" s="23">
-        <v>150.79311905120005</v>
+        <v>150.79036549399288</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5889,13 +5888,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="23">
-        <v>146.78338564321894</v>
+        <v>146.78338564322195</v>
       </c>
       <c r="C25" s="23">
-        <v>152.43870963463323</v>
+        <v>152.34556500063192</v>
       </c>
       <c r="D25" s="23">
-        <v>150.50093074862406</v>
+        <v>150.50077326010054</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5903,13 +5902,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="23">
-        <v>142.74091494478188</v>
+        <v>142.74091494479157</v>
       </c>
       <c r="C26" s="23">
-        <v>152.06202944140554</v>
+        <v>152.00144379782142</v>
       </c>
       <c r="D26" s="23">
-        <v>150.01368224201173</v>
+        <v>150.01542141707731</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5917,13 +5916,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="23">
-        <v>138.8180413374636</v>
+        <v>138.81804133746769</v>
       </c>
       <c r="C27" s="23">
-        <v>152.03427528771681</v>
+        <v>151.96394806261955</v>
       </c>
       <c r="D27" s="23">
-        <v>149.35171789428014</v>
+        <v>149.3553294810454</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5931,13 +5930,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="23">
-        <v>155.85731621135361</v>
+        <v>155.85731621133985</v>
       </c>
       <c r="C28" s="23">
-        <v>151.30101250711402</v>
+        <v>151.27938383204514</v>
       </c>
       <c r="D28" s="23">
-        <v>148.5501842507681</v>
+        <v>148.55424801714975</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5945,13 +5944,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="23">
-        <v>151.52453339188628</v>
+        <v>151.52453339184243</v>
       </c>
       <c r="C29" s="23">
-        <v>146.89441438237267</v>
+        <v>146.87340585645646</v>
       </c>
       <c r="D29" s="23">
-        <v>147.65587643530469</v>
+        <v>147.66007557512518</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5959,13 +5958,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="23">
-        <v>159.56668791299208</v>
+        <v>159.56668791297358</v>
       </c>
       <c r="C30" s="23">
-        <v>144.44407959951238</v>
+        <v>144.42988052091167</v>
       </c>
       <c r="D30" s="23">
-        <v>146.72356102565738</v>
+        <v>146.72965786082921</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5973,13 +5972,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="23">
-        <v>151.12577829043676</v>
+        <v>151.12577829049906</v>
       </c>
       <c r="C31" s="23">
-        <v>143.13597722709724</v>
+        <v>143.17458936789674</v>
       </c>
       <c r="D31" s="23">
-        <v>145.80745773118755</v>
+        <v>145.81872273332161</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5987,13 +5986,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="23">
-        <v>145.96357240366589</v>
+        <v>145.96357240386445</v>
       </c>
       <c r="C32" s="23">
-        <v>143.15717025828692</v>
+        <v>143.20050524024705</v>
       </c>
       <c r="D32" s="23">
-        <v>144.95551096154841</v>
+        <v>144.97540740406359</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -6001,13 +6000,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="23">
-        <v>146.7659802567249</v>
+        <v>146.7659802568086</v>
       </c>
       <c r="C33" s="23">
-        <v>146.58626058192172</v>
+        <v>146.66966926966157</v>
       </c>
       <c r="D33" s="23">
-        <v>144.21199326814863</v>
+        <v>144.24396586844074</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -6015,13 +6014,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="23">
-        <v>137.74650152240125</v>
+        <v>137.74650152211899</v>
       </c>
       <c r="C34" s="23">
-        <v>143.13955143189389</v>
+        <v>143.18916058132899</v>
       </c>
       <c r="D34" s="23">
-        <v>143.60711232915125</v>
+        <v>143.6535515456421</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -6029,13 +6028,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="23">
-        <v>142.84305870173307</v>
+        <v>142.84305870083375</v>
       </c>
       <c r="C35" s="23">
-        <v>143.53927245031349</v>
+        <v>143.61162662342136</v>
       </c>
       <c r="D35" s="23">
-        <v>143.15732551385699</v>
+        <v>143.21831260583366</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -6043,13 +6042,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="23">
-        <v>140.59231573298001</v>
+        <v>140.59231573260089</v>
       </c>
       <c r="C36" s="23">
-        <v>141.66200928873064</v>
+        <v>141.66959471705917</v>
       </c>
       <c r="D36" s="23">
-        <v>142.86426814243052</v>
+        <v>142.93818355135517</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -6057,13 +6056,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="23">
-        <v>136.2519248442463</v>
+        <v>136.25192484552474</v>
       </c>
       <c r="C37" s="23">
-        <v>141.84057331381112</v>
+        <v>141.73341789881025</v>
       </c>
       <c r="D37" s="23">
-        <v>142.71582774306765</v>
+        <v>142.79980513966638</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -6071,13 +6070,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="23">
-        <v>134.52056075074981</v>
+        <v>134.52056075482315</v>
       </c>
       <c r="C38" s="23">
-        <v>142.93178812186963</v>
+        <v>142.94319792611682</v>
       </c>
       <c r="D38" s="23">
-        <v>142.68808503883471</v>
+        <v>142.77706155258957</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -6085,13 +6084,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="23">
-        <v>132.27529838772409</v>
+        <v>132.27529838944116</v>
       </c>
       <c r="C39" s="23">
-        <v>143.73011394626562</v>
+        <v>143.57581774945962</v>
       </c>
       <c r="D39" s="23">
-        <v>142.74407462055439</v>
+        <v>142.83286981476959</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6099,13 +6098,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="23">
-        <v>144.87373845188188</v>
+        <v>144.87373844609147</v>
       </c>
       <c r="C40" s="23">
-        <v>141.36224353890381</v>
+        <v>141.21590207424484</v>
       </c>
       <c r="D40" s="23">
-        <v>142.84420064876002</v>
+        <v>142.92834552559086</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6113,13 +6112,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="23">
-        <v>149.89913657771015</v>
+        <v>149.89913655926117</v>
       </c>
       <c r="C41" s="23">
-        <v>142.53893657365967</v>
+        <v>142.56181720331321</v>
       </c>
       <c r="D41" s="23">
-        <v>142.94828695779816</v>
+        <v>143.02446830417739</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6127,13 +6126,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="23">
-        <v>164.14987183822055</v>
+        <v>164.14987183044366</v>
       </c>
       <c r="C42" s="23">
-        <v>144.64227181273864</v>
+        <v>144.54803805815237</v>
       </c>
       <c r="D42" s="23">
-        <v>143.01947622528439</v>
+        <v>143.0859390852616</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6141,13 +6140,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="23">
-        <v>150.84993447841651</v>
+        <v>150.84993450464239</v>
       </c>
       <c r="C43" s="23">
-        <v>143.67708822197702</v>
+        <v>143.77037642481855</v>
       </c>
       <c r="D43" s="23">
-        <v>143.0229017459117</v>
+        <v>143.07912122783236</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6155,13 +6154,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="23">
-        <v>146.76823777325902</v>
+        <v>146.76823785681836</v>
       </c>
       <c r="C44" s="23">
-        <v>145.32203245985539</v>
+        <v>145.42125270260249</v>
       </c>
       <c r="D44" s="23">
-        <v>142.9316479875144</v>
+        <v>142.97747667854608</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6169,13 +6168,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="23">
-        <v>141.27943601412611</v>
+        <v>141.2794360493493</v>
       </c>
       <c r="C45" s="23">
-        <v>144.7707533533719</v>
+        <v>145.00741083024602</v>
       </c>
       <c r="D45" s="23">
-        <v>142.72363701271163</v>
+        <v>142.75996063246714</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6183,13 +6182,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="23">
-        <v>134.88987746847488</v>
+        <v>134.88987734969228</v>
       </c>
       <c r="C46" s="23">
-        <v>141.10421992317856</v>
+        <v>141.14204482342629</v>
       </c>
       <c r="D46" s="23">
-        <v>142.38549936105483</v>
+        <v>142.41434534506752</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6197,13 +6196,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="23">
-        <v>141.5107890167823</v>
+        <v>141.51078863832441</v>
       </c>
       <c r="C47" s="23">
-        <v>143.25244102922133</v>
+        <v>143.45288494259788</v>
       </c>
       <c r="D47" s="23">
-        <v>141.91466926107924</v>
+        <v>141.93896829510354</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6211,13 +6210,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="23">
-        <v>137.65812425355574</v>
+        <v>137.65812409402241</v>
       </c>
       <c r="C48" s="23">
-        <v>140.68383690021861</v>
+        <v>140.66237255014786</v>
       </c>
       <c r="D48" s="23">
-        <v>141.31854021636124</v>
+        <v>141.34095388454946</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6225,13 +6224,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="23">
-        <v>135.67189169524758</v>
+        <v>135.67189223323882</v>
       </c>
       <c r="C49" s="23">
-        <v>140.33117103995428</v>
+        <v>140.04578163422929</v>
       </c>
       <c r="D49" s="23">
-        <v>140.62063183105846</v>
+        <v>140.64474140093998</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6239,13 +6238,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="23">
-        <v>132.28222953157538</v>
+        <v>132.28223124569112</v>
       </c>
       <c r="C50" s="23">
-        <v>140.76612876398124</v>
+        <v>140.79013043614304</v>
       </c>
       <c r="D50" s="23">
-        <v>139.85867453487685</v>
+        <v>139.88604061289249</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6253,13 +6252,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="23">
-        <v>129.74514590914131</v>
+        <v>129.74514663170137</v>
       </c>
       <c r="C51" s="23">
-        <v>140.84510209372061</v>
+        <v>140.60282169870521</v>
       </c>
       <c r="D51" s="23">
-        <v>139.0771256615846</v>
+        <v>139.10863595334621</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6267,13 +6266,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="23">
-        <v>129.09772765055823</v>
+        <v>129.0977252138824</v>
       </c>
       <c r="C52" s="23">
-        <v>125.68636824161807</v>
+        <v>125.42171449999771</v>
       </c>
       <c r="D52" s="23">
-        <v>138.32296688103409</v>
+        <v>138.35818442214642</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6281,13 +6280,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="23">
-        <v>111.90396092676694</v>
+        <v>111.90395316317499</v>
       </c>
       <c r="C53" s="23">
-        <v>105.26392153546615</v>
+        <v>105.2098461794268</v>
       </c>
       <c r="D53" s="23">
-        <v>137.63977832284999</v>
+        <v>137.68201804658736</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6295,13 +6294,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="23">
-        <v>131.29461627757212</v>
+        <v>131.29461300494506</v>
       </c>
       <c r="C54" s="23">
-        <v>116.49855344829493</v>
+        <v>116.47317016933816</v>
       </c>
       <c r="D54" s="23">
-        <v>137.06403734705788</v>
+        <v>137.11862902464813</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6309,13 +6308,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="23">
-        <v>133.30385550335268</v>
+        <v>133.30386653957163</v>
       </c>
       <c r="C55" s="23">
-        <v>124.28544051256891</v>
+        <v>124.45949093873637</v>
       </c>
       <c r="D55" s="23">
-        <v>136.62193576122931</v>
+        <v>136.69515448755575</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6323,13 +6322,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="23">
-        <v>128.19076761951325</v>
+        <v>128.19080278245926</v>
       </c>
       <c r="C56" s="23">
-        <v>126.47047559987693</v>
+        <v>126.65386668787953</v>
       </c>
       <c r="D56" s="23">
-        <v>136.32966287916631</v>
+        <v>136.42834050880154</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6337,13 +6336,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="23">
-        <v>125.17405150107314</v>
+        <v>125.17406632349137</v>
       </c>
       <c r="C57" s="23">
-        <v>129.02186199881285</v>
+        <v>129.3663149206532</v>
       </c>
       <c r="D57" s="23">
-        <v>136.19537725502903</v>
+        <v>136.32526741989781</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -6351,13 +6350,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="23">
-        <v>126.59619564159864</v>
+        <v>126.59614565623438</v>
       </c>
       <c r="C58" s="23">
-        <v>131.16067992216838</v>
+        <v>131.22903438026464</v>
       </c>
       <c r="D58" s="23">
-        <v>136.21276952455645</v>
+        <v>136.38014896092403</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6365,13 +6364,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="23">
-        <v>131.72755094720367</v>
+        <v>131.72739168680206</v>
       </c>
       <c r="C59" s="23">
-        <v>133.88195912079445</v>
+        <v>134.17056171093429</v>
       </c>
       <c r="D59" s="23">
-        <v>136.36963535584024</v>
+        <v>136.57898086523281</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6379,13 +6378,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="23">
-        <v>132.96980475640171</v>
+        <v>132.96973762254197</v>
       </c>
       <c r="C60" s="23">
-        <v>135.3385476000374</v>
+        <v>135.29368154581678</v>
       </c>
       <c r="D60" s="23">
-        <v>136.65093643828837</v>
+        <v>136.90363699823831</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6393,13 +6392,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="23">
-        <v>132.421754125212</v>
+        <v>132.42198051947332</v>
       </c>
       <c r="C61" s="23">
-        <v>135.48862174643341</v>
+        <v>135.03702741418641</v>
       </c>
       <c r="D61" s="23">
-        <v>137.0405409406867</v>
+        <v>137.33453965057083</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6407,13 +6406,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="23">
-        <v>129.49204624937207</v>
+        <v>129.49276757333357</v>
       </c>
       <c r="C62" s="23">
-        <v>139.47059782826972</v>
+        <v>139.64335426908619</v>
       </c>
       <c r="D62" s="23">
-        <v>137.52608929702791</v>
+        <v>137.85390070175555</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6421,13 +6420,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="23">
-        <v>126.69351913459056</v>
+        <v>126.69382319800599</v>
       </c>
       <c r="C63" s="23">
-        <v>138.64854361972618</v>
+        <v>138.22565030927976</v>
       </c>
       <c r="D63" s="23">
-        <v>138.09929406731123</v>
+        <v>138.44791731142826</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6435,13 +6434,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="23">
-        <v>146.2887415952199</v>
+        <v>146.28771620784292</v>
       </c>
       <c r="C64" s="23">
-        <v>140.03411994231681</v>
+        <v>139.64501718511639</v>
       </c>
       <c r="D64" s="23">
-        <v>138.75920572497489</v>
+        <v>139.10717223359487</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6449,13 +6448,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="23">
-        <v>144.90903247458738</v>
+        <v>144.90576544617173</v>
       </c>
       <c r="C65" s="23">
-        <v>138.10772356270161</v>
+        <v>138.0052948445753</v>
       </c>
       <c r="D65" s="23">
-        <v>139.50268056921394</v>
+        <v>139.81881644586807</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -6463,13 +6462,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="23">
-        <v>150.15006642270126</v>
+        <v>150.14868925533764</v>
       </c>
       <c r="C66" s="23">
-        <v>136.59621386829264</v>
+        <v>136.63853140773671</v>
       </c>
       <c r="D66" s="23">
-        <v>140.32320851667797</v>
+        <v>140.57050007116794</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -6477,13 +6476,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="23">
-        <v>148.9393209402111</v>
+        <v>148.94396513599037</v>
       </c>
       <c r="C67" s="23">
-        <v>140.27838742367854</v>
+        <v>140.52273745407999</v>
       </c>
       <c r="D67" s="23">
-        <v>141.2066905656329</v>
+        <v>141.34419744582991</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -6491,13 +6490,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="23">
-        <v>143.16129268584584</v>
+        <v>143.1827570387415</v>
       </c>
       <c r="C68" s="23">
-        <v>141.82073247405549</v>
+        <v>142.15098179747358</v>
       </c>
       <c r="D68" s="23">
-        <v>142.13269518353229</v>
+        <v>142.11756457090485</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -6505,13 +6504,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="23">
-        <v>141.19670480423781</v>
+        <v>141.20571583640663</v>
       </c>
       <c r="C69" s="23">
-        <v>143.93941519322294</v>
+        <v>144.37019481414114</v>
       </c>
       <c r="D69" s="23">
-        <v>143.07124961991786</v>
+        <v>142.86106683298576</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -6519,13 +6518,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="23">
-        <v>140.70255570329414</v>
+        <v>140.94554305470595</v>
       </c>
       <c r="C70" s="23">
-        <v>145.1027230773804</v>
+        <v>145.41772585610909</v>
       </c>
       <c r="D70" s="23">
-        <v>143.99168738236463</v>
+        <v>143.54515118614222</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -6533,13 +6532,13 @@
         <v>44470</v>
       </c>
       <c r="B71" s="23">
-        <v>140.84838387204763</v>
+        <v>140.53928207853662</v>
       </c>
       <c r="C71" s="23">
-        <v>144.3492128906569</v>
+        <v>144.52125619506972</v>
       </c>
       <c r="D71" s="23">
-        <v>144.86090187128829</v>
+        <v>144.14196855095184</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -6547,27 +6546,41 @@
         <v>44501</v>
       </c>
       <c r="B72" s="23">
-        <v>145.51114906453842</v>
+        <v>145.25244923103682</v>
       </c>
       <c r="C72" s="23">
-        <v>146.28714457565965</v>
+        <v>146.26718479231505</v>
       </c>
       <c r="D72" s="23">
-        <v>145.65142395437829</v>
+        <v>144.63260266756626</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>44531</v>
       </c>
-      <c r="B73" s="24">
-        <v>145.40844696072728</v>
-      </c>
-      <c r="C73" s="24">
-        <v>147.67149712630018</v>
-      </c>
-      <c r="D73" s="24">
-        <v>146.34890457104302</v>
+      <c r="B73" s="23">
+        <v>145.65428740631165</v>
+      </c>
+      <c r="C73" s="23">
+        <v>147.84483147827757</v>
+      </c>
+      <c r="D73" s="23">
+        <v>145.0110078556213</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B74" s="24">
+        <v>136.51119002060923</v>
+      </c>
+      <c r="C74" s="24">
+        <v>147.05486359872521</v>
+      </c>
+      <c r="D74" s="24">
+        <v>145.28387928059126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo datos ipc abr22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7660632B-DADB-45EE-A076-CB8072B36581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7D941D-2425-4FF0-9828-3CB38A1B707D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -1023,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2108,23 @@
         <v>3.1</v>
       </c>
     </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>44621</v>
+      </c>
+      <c r="B64" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="C64">
+        <v>6.2</v>
+      </c>
+      <c r="D64">
+        <v>6.4</v>
+      </c>
+      <c r="E64">
+        <v>8.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2118,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,25 +2175,25 @@
         <v>129</v>
       </c>
       <c r="B2" s="36">
-        <v>5.8</v>
+        <v>11.6</v>
       </c>
       <c r="C2" s="36">
-        <v>4.9000000000000004</v>
+        <v>11.7</v>
       </c>
       <c r="D2" s="36">
-        <v>5.2</v>
+        <v>12.9</v>
       </c>
       <c r="E2" s="40">
-        <v>3.7</v>
+        <v>15.5</v>
       </c>
       <c r="F2" s="36">
-        <v>4.7</v>
+        <v>15.7</v>
       </c>
       <c r="G2" s="36">
-        <v>5</v>
+        <v>11.7</v>
       </c>
       <c r="H2" s="21">
-        <v>4.7649305921721119</v>
+        <v>11.934528675530377</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2184,25 +2201,25 @@
         <v>130</v>
       </c>
       <c r="B3" s="36">
-        <v>5.7</v>
+        <v>7.5</v>
       </c>
       <c r="C3" s="36">
-        <v>4.3</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D3" s="36">
-        <v>3.9</v>
+        <v>6.9</v>
       </c>
       <c r="E3" s="40">
-        <v>4</v>
+        <v>9.6</v>
       </c>
       <c r="F3" s="36">
-        <v>5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G3" s="36">
-        <v>5.4</v>
+        <v>11.5</v>
       </c>
       <c r="H3" s="21">
-        <v>4.10821359915583</v>
+        <v>8.4001014574765378</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2210,25 +2227,25 @@
         <v>131</v>
       </c>
       <c r="B4" s="36">
-        <v>6.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C4" s="36">
-        <v>6.5</v>
+        <v>8.4</v>
       </c>
       <c r="D4" s="36">
-        <v>7.1</v>
+        <v>8.9</v>
       </c>
       <c r="E4" s="40">
-        <v>8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F4" s="36">
-        <v>8.1</v>
+        <v>9.5</v>
       </c>
       <c r="G4" s="36">
-        <v>6</v>
+        <v>7.6</v>
       </c>
       <c r="H4" s="21">
-        <v>6.3014522203917123</v>
+        <v>8.7716547784098218</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2236,25 +2253,25 @@
         <v>132</v>
       </c>
       <c r="B5" s="36">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="C5" s="36">
-        <v>2.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D5" s="36">
-        <v>5.3</v>
+        <v>6</v>
       </c>
       <c r="E5" s="40">
-        <v>3.8</v>
+        <v>5.2</v>
       </c>
       <c r="F5" s="36">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="G5" s="36">
-        <v>3.7</v>
+        <v>6.1</v>
       </c>
       <c r="H5" s="21">
-        <v>3.0658272884779736</v>
+        <v>3.5609891055234044</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2262,25 +2279,25 @@
         <v>133</v>
       </c>
       <c r="B6" s="36">
-        <v>10.4</v>
+        <v>2.4</v>
       </c>
       <c r="C6" s="36">
-        <v>11</v>
+        <v>3.4</v>
       </c>
       <c r="D6" s="36">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="40">
-        <v>9</v>
+        <v>2.5</v>
       </c>
       <c r="F6" s="36">
-        <v>15.9</v>
+        <v>0.3</v>
       </c>
       <c r="G6" s="36">
-        <v>8.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H6" s="21">
-        <v>9.9168014020806226</v>
+        <v>2.7657166758527696</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2288,25 +2305,25 @@
         <v>134</v>
       </c>
       <c r="B7" s="36">
-        <v>32.299999999999997</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="C7" s="36">
-        <v>22.6</v>
+        <v>5.8</v>
       </c>
       <c r="D7" s="36">
-        <v>18.600000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="E7" s="40">
-        <v>20.9</v>
+        <v>3.2</v>
       </c>
       <c r="F7" s="36">
-        <v>23.5</v>
+        <v>7</v>
       </c>
       <c r="G7" s="36">
-        <v>13.8</v>
+        <v>8.6</v>
       </c>
       <c r="H7" s="21">
-        <v>25.127176051571954</v>
+        <v>0.62889641358436776</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2314,25 +2331,25 @@
         <v>135</v>
       </c>
       <c r="B8" s="36">
-        <v>3.5</v>
+        <v>6.4</v>
       </c>
       <c r="C8" s="36">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="D8" s="36">
-        <v>4.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="E8" s="40">
-        <v>5.2</v>
+        <v>7</v>
       </c>
       <c r="F8" s="36">
-        <v>5.6</v>
+        <v>8.1</v>
       </c>
       <c r="G8" s="36">
-        <v>2.7</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H8" s="22">
-        <v>3.6765802867822606</v>
+        <v>6.7811614983588786</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2340,25 +2357,25 @@
         <v>136</v>
       </c>
       <c r="B9" s="36">
-        <v>5.0999999999999996</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C9" s="36">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
       <c r="D9" s="36">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="E9" s="40">
-        <v>3.4</v>
+        <v>4.8</v>
       </c>
       <c r="F9" s="36">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="G9" s="36">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="H9" s="21">
-        <v>4.3248683332119509</v>
+        <v>5.8957312783190829</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2369,22 +2386,22 @@
         <v>3.8</v>
       </c>
       <c r="C10" s="36">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="D10" s="36">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
       <c r="E10" s="40">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="F10" s="36">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G10" s="36">
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H10" s="21">
-        <v>3.7638794769067285</v>
+        <v>4.1429061084430119</v>
       </c>
     </row>
   </sheetData>
@@ -2398,7 +2415,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,25 +2451,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="27">
-        <v>4.7</v>
+        <v>6.7</v>
       </c>
       <c r="C2" s="38">
-        <v>4.5999999999999996</v>
+        <v>6.7</v>
       </c>
       <c r="D2" s="38">
-        <v>4.7</v>
+        <v>6.6</v>
       </c>
       <c r="E2" s="38">
-        <v>5</v>
+        <v>7.2</v>
       </c>
       <c r="F2" s="38">
-        <v>4.9000000000000004</v>
+        <v>6.8</v>
       </c>
       <c r="G2" s="38">
-        <v>5.4</v>
+        <v>6.8</v>
       </c>
       <c r="H2" s="29">
-        <v>4.8</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2460,25 +2477,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="26">
-        <v>7.5</v>
+        <v>7.2</v>
       </c>
       <c r="C3" s="37">
-        <v>8.6</v>
+        <v>6.1</v>
       </c>
       <c r="D3" s="37">
-        <v>6.7</v>
+        <v>7.9</v>
       </c>
       <c r="E3" s="37">
-        <v>6.3</v>
+        <v>7.7</v>
       </c>
       <c r="F3" s="37">
-        <v>6.3</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="G3" s="37">
-        <v>7.5</v>
+        <v>9.1</v>
       </c>
       <c r="H3" s="28">
-        <v>6</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2486,25 +2503,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="26">
-        <v>2.7</v>
+        <v>5.7</v>
       </c>
       <c r="C4" s="37">
-        <v>2.7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="37">
-        <v>2.4</v>
+        <v>5.6</v>
       </c>
       <c r="E4" s="37">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="F4" s="37">
-        <v>2.8</v>
+        <v>5.2</v>
       </c>
       <c r="G4" s="37">
-        <v>2.9</v>
+        <v>6.1</v>
       </c>
       <c r="H4" s="28">
-        <v>2.5</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2512,25 +2529,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="26">
-        <v>3.4</v>
+        <v>10.9</v>
       </c>
       <c r="C5" s="37">
-        <v>2.9</v>
+        <v>13.6</v>
       </c>
       <c r="D5" s="37">
-        <v>3.9</v>
+        <v>9.1</v>
       </c>
       <c r="E5" s="37">
-        <v>3.1</v>
+        <v>7.5</v>
       </c>
       <c r="F5" s="37">
-        <v>3.3</v>
+        <v>6.4</v>
       </c>
       <c r="G5" s="37">
-        <v>3.7</v>
+        <v>7.6</v>
       </c>
       <c r="H5" s="28">
-        <v>5.3</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2538,25 +2555,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="26">
-        <v>2.8</v>
+        <v>7.7</v>
       </c>
       <c r="C6" s="37">
-        <v>2.5</v>
+        <v>8.4</v>
       </c>
       <c r="D6" s="37">
-        <v>3.7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="37">
-        <v>2.5</v>
+        <v>15.4</v>
       </c>
       <c r="F6" s="37">
-        <v>0.4</v>
+        <v>5.6</v>
       </c>
       <c r="G6" s="37">
-        <v>4</v>
+        <v>6.3</v>
       </c>
       <c r="H6" s="28">
-        <v>2.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2570,19 +2587,19 @@
         <v>4.3</v>
       </c>
       <c r="D7" s="37">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E7" s="37">
-        <v>4.8</v>
+        <v>3.7</v>
       </c>
       <c r="F7" s="37">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G7" s="37">
-        <v>4.3</v>
+        <v>5.2</v>
       </c>
       <c r="H7" s="28">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2590,25 +2607,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="26">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="37">
-        <v>3.1</v>
+        <v>5.5</v>
       </c>
       <c r="D8" s="37">
-        <v>3.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E8" s="37">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="F8" s="37">
-        <v>4.3</v>
+        <v>5.2</v>
       </c>
       <c r="G8" s="37">
         <v>4.3</v>
       </c>
       <c r="H8" s="28">
-        <v>4.4000000000000004</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2616,25 +2633,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="26">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="C9" s="37">
-        <v>4.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="D9" s="37">
         <v>5.5</v>
       </c>
       <c r="E9" s="37">
-        <v>5.8</v>
+        <v>8</v>
       </c>
       <c r="F9" s="37">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
       <c r="G9" s="37">
-        <v>6.1</v>
+        <v>6.6</v>
       </c>
       <c r="H9" s="28">
-        <v>5.4</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2642,25 +2659,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="26">
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="C10" s="37">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="D10" s="37">
-        <v>1.1000000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="E10" s="37">
-        <v>1.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F10" s="37">
-        <v>1.9</v>
+        <v>4</v>
       </c>
       <c r="G10" s="37">
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="H10" s="28">
-        <v>0.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2668,25 +2685,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="26">
-        <v>2.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="C11" s="37">
-        <v>1.4</v>
+        <v>2.4</v>
       </c>
       <c r="D11" s="37">
-        <v>2.4</v>
+        <v>4.5</v>
       </c>
       <c r="E11" s="37">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="F11" s="37">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="G11" s="37">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="H11" s="28">
-        <v>4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2694,25 +2711,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="26">
-        <v>2.6</v>
+        <v>23.6</v>
       </c>
       <c r="C12" s="37">
-        <v>2</v>
+        <v>22.1</v>
       </c>
       <c r="D12" s="37">
-        <v>2.7</v>
+        <v>25.8</v>
       </c>
       <c r="E12" s="37">
-        <v>7.1</v>
+        <v>25.6</v>
       </c>
       <c r="F12" s="37">
-        <v>4.4000000000000004</v>
+        <v>19</v>
       </c>
       <c r="G12" s="37">
-        <v>2.2999999999999998</v>
+        <v>15.3</v>
       </c>
       <c r="H12" s="28">
-        <v>2.2999999999999998</v>
+        <v>42.9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2720,25 +2737,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="26">
-        <v>4.3</v>
+        <v>5.4</v>
       </c>
       <c r="C13" s="37">
-        <v>4.4000000000000004</v>
+        <v>5.8</v>
       </c>
       <c r="D13" s="37">
-        <v>3</v>
+        <v>5.2</v>
       </c>
       <c r="E13" s="37">
-        <v>4.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F13" s="37">
-        <v>6.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G13" s="37">
-        <v>6.1</v>
+        <v>4.7</v>
       </c>
       <c r="H13" s="28">
-        <v>7.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2746,25 +2763,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="26">
-        <v>4.3</v>
+        <v>5.5</v>
       </c>
       <c r="C14" s="37">
-        <v>4.4000000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="D14" s="37">
-        <v>4.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E14" s="37">
-        <v>4</v>
+        <v>5.3</v>
       </c>
       <c r="F14" s="37">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="G14" s="37">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="H14" s="28">
-        <v>4</v>
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>
@@ -2778,7 +2795,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+      <selection activeCell="B2" sqref="B2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,25 +2831,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="31">
-        <v>52.3</v>
+        <v>55.1</v>
       </c>
       <c r="C2" s="39">
-        <v>53.8</v>
+        <v>55.9</v>
       </c>
       <c r="D2" s="39">
-        <v>51.1</v>
+        <v>53.7</v>
       </c>
       <c r="E2" s="39">
-        <v>50</v>
+        <v>55.7</v>
       </c>
       <c r="F2" s="39">
-        <v>50.9</v>
+        <v>54.6</v>
       </c>
       <c r="G2" s="39">
-        <v>52</v>
+        <v>55.5</v>
       </c>
       <c r="H2" s="39">
-        <v>52.3</v>
+        <v>57.3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2840,25 +2857,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="30">
-        <v>55.8</v>
+        <v>59.7</v>
       </c>
       <c r="C3" s="23">
-        <v>58.8</v>
+        <v>60.6</v>
       </c>
       <c r="D3" s="23">
-        <v>54.3</v>
+        <v>58.9</v>
       </c>
       <c r="E3" s="23">
-        <v>49.8</v>
+        <v>56.5</v>
       </c>
       <c r="F3" s="23">
-        <v>52.3</v>
+        <v>59.9</v>
       </c>
       <c r="G3" s="23">
-        <v>54.5</v>
+        <v>61.6</v>
       </c>
       <c r="H3" s="23">
-        <v>52.3</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2866,25 +2883,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="30">
-        <v>49.7</v>
+        <v>48.8</v>
       </c>
       <c r="C4" s="23">
-        <v>48.4</v>
+        <v>48.1</v>
       </c>
       <c r="D4" s="23">
-        <v>50.9</v>
+        <v>49.2</v>
       </c>
       <c r="E4" s="23">
-        <v>59.1</v>
+        <v>56.4</v>
       </c>
       <c r="F4" s="23">
-        <v>50.8</v>
+        <v>49</v>
       </c>
       <c r="G4" s="23">
-        <v>48.6</v>
+        <v>48.1</v>
       </c>
       <c r="H4" s="23">
-        <v>44.9</v>
+        <v>45.9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2892,25 +2909,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="30">
-        <v>67.2</v>
+        <v>67.3</v>
       </c>
       <c r="C5" s="23">
-        <v>71.400000000000006</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="D5" s="23">
-        <v>64.400000000000006</v>
+        <v>67.5</v>
       </c>
       <c r="E5" s="23">
-        <v>64.3</v>
+        <v>70.7</v>
       </c>
       <c r="F5" s="23">
-        <v>61</v>
+        <v>61.7</v>
       </c>
       <c r="G5" s="23">
-        <v>57.9</v>
+        <v>62</v>
       </c>
       <c r="H5" s="23">
-        <v>71.599999999999994</v>
+        <v>75.8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2918,25 +2935,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="30">
-        <v>30.1</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="C6" s="23">
-        <v>32.5</v>
+        <v>42.2</v>
       </c>
       <c r="D6" s="23">
-        <v>26.7</v>
+        <v>32.6</v>
       </c>
       <c r="E6" s="23">
-        <v>35.1</v>
+        <v>52.8</v>
       </c>
       <c r="F6" s="23">
-        <v>26.4</v>
+        <v>31.5</v>
       </c>
       <c r="G6" s="23">
-        <v>26.2</v>
+        <v>30.9</v>
       </c>
       <c r="H6" s="23">
-        <v>38</v>
+        <v>47.6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2944,25 +2961,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="30">
-        <v>46.9</v>
+        <v>48.7</v>
       </c>
       <c r="C7" s="23">
-        <v>47.8</v>
+        <v>49.4</v>
       </c>
       <c r="D7" s="23">
-        <v>47</v>
+        <v>48.7</v>
       </c>
       <c r="E7" s="23">
-        <v>43</v>
+        <v>44.1</v>
       </c>
       <c r="F7" s="23">
-        <v>44.3</v>
+        <v>46.2</v>
       </c>
       <c r="G7" s="23">
-        <v>47.2</v>
+        <v>49.4</v>
       </c>
       <c r="H7" s="23">
-        <v>46</v>
+        <v>48.7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2970,25 +2987,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="30">
+        <v>54.5</v>
+      </c>
+      <c r="C8" s="23">
+        <v>55.7</v>
+      </c>
+      <c r="D8" s="23">
+        <v>53.6</v>
+      </c>
+      <c r="E8" s="23">
+        <v>52.9</v>
+      </c>
+      <c r="F8" s="23">
         <v>53.1</v>
       </c>
-      <c r="C8" s="23">
-        <v>53.5</v>
-      </c>
-      <c r="D8" s="23">
-        <v>53.4</v>
-      </c>
-      <c r="E8" s="23">
-        <v>50.4</v>
-      </c>
-      <c r="F8" s="23">
-        <v>50.7</v>
-      </c>
       <c r="G8" s="23">
-        <v>55.1</v>
+        <v>56</v>
       </c>
       <c r="H8" s="23">
-        <v>50.8</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,25 +3013,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="30">
-        <v>55</v>
+        <v>56.9</v>
       </c>
       <c r="C9" s="23">
+        <v>55.2</v>
+      </c>
+      <c r="D9" s="23">
+        <v>57.6</v>
+      </c>
+      <c r="E9" s="23">
+        <v>61.8</v>
+      </c>
+      <c r="F9" s="23">
         <v>53.3</v>
       </c>
-      <c r="D9" s="23">
-        <v>56.2</v>
-      </c>
-      <c r="E9" s="23">
-        <v>55.9</v>
-      </c>
-      <c r="F9" s="23">
-        <v>52.6</v>
-      </c>
       <c r="G9" s="23">
-        <v>59.1</v>
+        <v>62.2</v>
       </c>
       <c r="H9" s="23">
-        <v>59.9</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3022,25 +3039,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="30">
-        <v>26.3</v>
+        <v>30.6</v>
       </c>
       <c r="C10" s="23">
-        <v>27.2</v>
+        <v>29.5</v>
       </c>
       <c r="D10" s="23">
-        <v>23.9</v>
+        <v>31.5</v>
       </c>
       <c r="E10" s="23">
-        <v>29.2</v>
+        <v>33</v>
       </c>
       <c r="F10" s="23">
-        <v>27.9</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="G10" s="23">
-        <v>30</v>
+        <v>31.1</v>
       </c>
       <c r="H10" s="23">
-        <v>26.5</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3048,25 +3065,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="30">
-        <v>46.2</v>
+        <v>43.4</v>
       </c>
       <c r="C11" s="23">
-        <v>47.5</v>
+        <v>45.9</v>
       </c>
       <c r="D11" s="23">
-        <v>44.3</v>
+        <v>38.5</v>
       </c>
       <c r="E11" s="23">
-        <v>42.7</v>
+        <v>44.4</v>
       </c>
       <c r="F11" s="23">
-        <v>47.5</v>
+        <v>48.4</v>
       </c>
       <c r="G11" s="23">
-        <v>50.4</v>
+        <v>45.8</v>
       </c>
       <c r="H11" s="23">
-        <v>44.6</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3074,25 +3091,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="30">
-        <v>60.4</v>
+        <v>54.3</v>
       </c>
       <c r="C12" s="23">
-        <v>65.599999999999994</v>
+        <v>55.5</v>
       </c>
       <c r="D12" s="23">
-        <v>60.6</v>
+        <v>55.7</v>
       </c>
       <c r="E12" s="23">
-        <v>48.6</v>
+        <v>51.3</v>
       </c>
       <c r="F12" s="23">
-        <v>53.5</v>
+        <v>44</v>
       </c>
       <c r="G12" s="23">
-        <v>47.6</v>
+        <v>46.1</v>
       </c>
       <c r="H12" s="23">
-        <v>41</v>
+        <v>62.3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3100,25 +3117,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="30">
-        <v>64.099999999999994</v>
+        <v>67.8</v>
       </c>
       <c r="C13" s="23">
-        <v>66.2</v>
+        <v>71.2</v>
       </c>
       <c r="D13" s="23">
-        <v>59.1</v>
+        <v>62.4</v>
       </c>
       <c r="E13" s="23">
-        <v>65.400000000000006</v>
+        <v>66.5</v>
       </c>
       <c r="F13" s="23">
-        <v>69</v>
+        <v>70.2</v>
       </c>
       <c r="G13" s="23">
-        <v>70.400000000000006</v>
+        <v>71.5</v>
       </c>
       <c r="H13" s="23">
-        <v>67.099999999999994</v>
+        <v>69.599999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3126,25 +3143,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="30">
-        <v>43.3</v>
+        <v>48</v>
       </c>
       <c r="C14" s="23">
-        <v>43.8</v>
+        <v>49.1</v>
       </c>
       <c r="D14" s="23">
-        <v>43.2</v>
+        <v>47.3</v>
       </c>
       <c r="E14" s="23">
-        <v>42.9</v>
+        <v>47</v>
       </c>
       <c r="F14" s="23">
-        <v>45.2</v>
+        <v>47.7</v>
       </c>
       <c r="G14" s="23">
-        <v>40.299999999999997</v>
+        <v>45</v>
       </c>
       <c r="H14" s="23">
-        <v>41</v>
+        <v>47.8</v>
       </c>
     </row>
   </sheetData>
@@ -5536,7 +5553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D74"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
"Actualizo datos comex y sit fiscal marzo, emae febrero"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7D941D-2425-4FF0-9828-3CB38A1B707D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2BEDD3-93D0-47F8-848C-30D7C75466C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,11 @@
     <sheet name="Pobreza-Aglo" sheetId="5" r:id="rId5"/>
     <sheet name="Pobreza regiones" sheetId="6" r:id="rId6"/>
     <sheet name="BC por zonas" sheetId="7" r:id="rId7"/>
-    <sheet name="VAB" sheetId="8" r:id="rId8"/>
-    <sheet name="EMAE" sheetId="9" r:id="rId9"/>
-    <sheet name="Aperturas" sheetId="10" r:id="rId10"/>
+    <sheet name="Expo-ICA" sheetId="11" r:id="rId8"/>
+    <sheet name="Impo-ICA" sheetId="12" r:id="rId9"/>
+    <sheet name="VAB" sheetId="8" r:id="rId10"/>
+    <sheet name="EMAE" sheetId="9" r:id="rId11"/>
+    <sheet name="Aperturas" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="218">
   <si>
     <t>Período</t>
   </si>
@@ -453,6 +455,246 @@
   </si>
   <si>
     <t>Aguas minerales, bebidas gaseosas y jugos</t>
+  </si>
+  <si>
+    <t>Animales vivos</t>
+  </si>
+  <si>
+    <t>Pescados y mariscos sin elaborar</t>
+  </si>
+  <si>
+    <t>Miel</t>
+  </si>
+  <si>
+    <t>Hortalizas y legumbres sin elaborar</t>
+  </si>
+  <si>
+    <t>Frutas frescas</t>
+  </si>
+  <si>
+    <t>Cereales</t>
+  </si>
+  <si>
+    <t>Semillas y frutos oleaginosos</t>
+  </si>
+  <si>
+    <t>Tabaco sin elaborar</t>
+  </si>
+  <si>
+    <t>Lanas sucias</t>
+  </si>
+  <si>
+    <t>Fibras de algodón</t>
+  </si>
+  <si>
+    <t>Minerales metalíferos, escorias y cenizas</t>
+  </si>
+  <si>
+    <t>Resto de productos primarios</t>
+  </si>
+  <si>
+    <t>Carnes y sus preparados</t>
+  </si>
+  <si>
+    <t>Pescados y mariscos elaborados</t>
+  </si>
+  <si>
+    <t>Productos lácteos</t>
+  </si>
+  <si>
+    <t>Otros productos de origen animal</t>
+  </si>
+  <si>
+    <t>Frutas secas o procesadas</t>
+  </si>
+  <si>
+    <t>Café, té, yerba mate y especias</t>
+  </si>
+  <si>
+    <t>Productos de molinería y sus preparaciones</t>
+  </si>
+  <si>
+    <t>Grasas y aceites</t>
+  </si>
+  <si>
+    <t>Azúcar, cacao y artículos de confitería</t>
+  </si>
+  <si>
+    <t>Preparados de hortalizas, legumbres y frutas</t>
+  </si>
+  <si>
+    <t>Bebidas, líquidos alcohólicos y vinagre</t>
+  </si>
+  <si>
+    <t>Residuos y desperdicios de la industria alimenticia</t>
+  </si>
+  <si>
+    <t>Extractos curtientes y tintóreos</t>
+  </si>
+  <si>
+    <t>Pieles y cueros</t>
+  </si>
+  <si>
+    <t>Lanas elaboradas</t>
+  </si>
+  <si>
+    <t>Resto de MOA</t>
+  </si>
+  <si>
+    <t>Productos químicos y conexos</t>
+  </si>
+  <si>
+    <t>Materias plásticas y sus manufacturas</t>
+  </si>
+  <si>
+    <t>Caucho y sus manufacturas</t>
+  </si>
+  <si>
+    <t>Manufacturas de cuero, marroquinería, etcétera</t>
+  </si>
+  <si>
+    <t>Papel, cartón, impresos y publicaciones</t>
+  </si>
+  <si>
+    <t>Textiles y confecciones</t>
+  </si>
+  <si>
+    <t>Calzado y sus partes componentes</t>
+  </si>
+  <si>
+    <t>Manufacturas de piedra, yeso, vidrio, etcétera</t>
+  </si>
+  <si>
+    <t>Piedras, metales preciosos y sus manufacturas; monedas</t>
+  </si>
+  <si>
+    <t>Metales comunes y sus manufacturas</t>
+  </si>
+  <si>
+    <t>Máquinas y aparatos, material eléctrico</t>
+  </si>
+  <si>
+    <t>Material de transporte terrestre</t>
+  </si>
+  <si>
+    <t>Vehículos de navegación aérea, marítima y fluvial</t>
+  </si>
+  <si>
+    <t>Resto de MOI</t>
+  </si>
+  <si>
+    <t>Petróleo crudo</t>
+  </si>
+  <si>
+    <t>Carburantes</t>
+  </si>
+  <si>
+    <t>Grasas y aceites lubricantes</t>
+  </si>
+  <si>
+    <t>Gas de petróleo, otros hidrocarburos gaseosos y energía eléctrica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resto de combustibles </t>
+  </si>
+  <si>
+    <t>Productos primarios (PP)</t>
+  </si>
+  <si>
+    <t>Manufacturas de origen agropecuario (MOA)</t>
+  </si>
+  <si>
+    <t>Manufacturas de origen industrial (MOI)</t>
+  </si>
+  <si>
+    <t>Combustibles y energía (CyE)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>XVI-Máquinas, aparatos y material eléctrico; sus partes y accesorios</t>
+  </si>
+  <si>
+    <t>XVII-Material de transporte</t>
+  </si>
+  <si>
+    <t>XVIII-Instrumentos y aparatos óptica; médico-quirúrgico y relojería; instr. musicales</t>
+  </si>
+  <si>
+    <t>Resto de bienes de capital</t>
+  </si>
+  <si>
+    <t>II-Productos del reino vegetal</t>
+  </si>
+  <si>
+    <t>V-Productos minerales</t>
+  </si>
+  <si>
+    <t>VI-Productos de industrias químicas o de las industrias conexas</t>
+  </si>
+  <si>
+    <t>VII-Plástico, caucho y sus manufacturas</t>
+  </si>
+  <si>
+    <t>X-Pasta de madera; papel o cartón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XI-Materias textiles y sus manufacturas </t>
+  </si>
+  <si>
+    <t>XIII-Manufacturas de piedra, yeso, cemento, amianto, mica, cerámica y vidrio</t>
+  </si>
+  <si>
+    <t>XV-Metales comunes y sus manufacturas</t>
+  </si>
+  <si>
+    <t>Resto de bienes intermedios</t>
+  </si>
+  <si>
+    <t>Resto de combustibles y lubricantes</t>
+  </si>
+  <si>
+    <t>Resto de piezas y accesorios</t>
+  </si>
+  <si>
+    <t>I-Animales vivos y productos del reino animal</t>
+  </si>
+  <si>
+    <t>IV-Productos de las industrias alimentarias, bebidas y tabaco</t>
+  </si>
+  <si>
+    <t>XII-Calzado, sombreros, paraguas, bastones, plumas, flores artificiales y otros</t>
+  </si>
+  <si>
+    <t>XX-Mercancías y productos diversos</t>
+  </si>
+  <si>
+    <t>Resto de bienes de consumo</t>
+  </si>
+  <si>
+    <t>Bienes de capital (BK)</t>
+  </si>
+  <si>
+    <t>Bienes intermedios (BI)</t>
+  </si>
+  <si>
+    <t>Combustibles y lubricantes (CyL)</t>
+  </si>
+  <si>
+    <t>Piezas y accesorios para bienes de capital (PyA)</t>
+  </si>
+  <si>
+    <t>Bienes de consumo (BC)</t>
+  </si>
+  <si>
+    <t>Vehículos automotores de pasajeros (VA)</t>
+  </si>
+  <si>
+    <t>Resto</t>
+  </si>
+  <si>
+    <t>Concepto</t>
   </si>
 </sst>
 </file>
@@ -572,7 +814,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,12 +830,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,7 +915,6 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -690,15 +925,37 @@
     <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2024,7 +2281,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="35">
+      <c r="A59" s="34">
         <v>44470</v>
       </c>
       <c r="B59" s="1">
@@ -2058,7 +2315,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="35">
+      <c r="A61" s="34">
         <v>44531</v>
       </c>
       <c r="B61" s="1">
@@ -2092,7 +2349,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="35">
+      <c r="A63" s="34">
         <v>44593</v>
       </c>
       <c r="B63" s="1">
@@ -2132,10 +2389,1299 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2">
+        <v>580109.3654135036</v>
+      </c>
+      <c r="C2">
+        <v>8.2176039378516919</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3">
+        <v>36648.13652029309</v>
+      </c>
+      <c r="C3">
+        <v>4.3860998002780427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4">
+        <v>1249.7113603560397</v>
+      </c>
+      <c r="C4">
+        <v>-19.150143374614757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5">
+        <v>22724.129989370613</v>
+      </c>
+      <c r="C5">
+        <v>18.247420162936258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6">
+        <v>122710.03414797327</v>
+      </c>
+      <c r="C6">
+        <v>8.543915384800993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>12285.490130430609</v>
+      </c>
+      <c r="C7">
+        <v>0.49655622972446523</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8">
+        <v>20987.63967740133</v>
+      </c>
+      <c r="C8">
+        <v>4.5268786278615414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9">
+        <v>93443.748235928695</v>
+      </c>
+      <c r="C9">
+        <v>7.2357992351878675</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <v>8992.2744681564727</v>
+      </c>
+      <c r="C10">
+        <v>60.938820792863964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>51632.157894787102</v>
+      </c>
+      <c r="C11">
+        <v>14.905791213603869</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <v>26151.467050546846</v>
+      </c>
+      <c r="C12">
+        <v>0.37420012180280349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>79143.368376477825</v>
+      </c>
+      <c r="C13">
+        <v>6.5567187004549332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14">
+        <v>34930.018675685875</v>
+      </c>
+      <c r="C14">
+        <v>11.909663098887879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15">
+        <v>28516.783116102812</v>
+      </c>
+      <c r="C15">
+        <v>6.1375814244809535</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16">
+        <v>22663.778591606671</v>
+      </c>
+      <c r="C16">
+        <v>2.422746472798476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17">
+        <v>14327.889062242892</v>
+      </c>
+      <c r="C17">
+        <v>10.245849380753791</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18">
+        <v>3702.7381161434578</v>
+      </c>
+      <c r="C18">
+        <v>1.7208283342252662</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>42370</v>
+      </c>
+      <c r="B2" s="23">
+        <v>134.74645041349706</v>
+      </c>
+      <c r="C2" s="23">
+        <v>148.12674938601256</v>
+      </c>
+      <c r="D2" s="23">
+        <v>147.07826915508767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42401</v>
+      </c>
+      <c r="B3" s="23">
+        <v>134.23236103862521</v>
+      </c>
+      <c r="C3" s="23">
+        <v>146.71851040460982</v>
+      </c>
+      <c r="D3" s="23">
+        <v>146.48875794209332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>42430</v>
+      </c>
+      <c r="B4" s="23">
+        <v>150.0878942366954</v>
+      </c>
+      <c r="C4" s="23">
+        <v>145.98112910209053</v>
+      </c>
+      <c r="D4" s="23">
+        <v>145.934409413612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>42461</v>
+      </c>
+      <c r="B5" s="23">
+        <v>153.25067436662908</v>
+      </c>
+      <c r="C5" s="23">
+        <v>145.16531814296513</v>
+      </c>
+      <c r="D5" s="23">
+        <v>145.45156266489744</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>42491</v>
+      </c>
+      <c r="B6" s="23">
+        <v>163.51360808690507</v>
+      </c>
+      <c r="C6" s="23">
+        <v>144.42520822906147</v>
+      </c>
+      <c r="D6" s="23">
+        <v>145.0679762154688</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>42522</v>
+      </c>
+      <c r="B7" s="23">
+        <v>153.66209524099784</v>
+      </c>
+      <c r="C7" s="23">
+        <v>144.32391150524907</v>
+      </c>
+      <c r="D7" s="23">
+        <v>144.80592840803149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42552</v>
+      </c>
+      <c r="B8" s="23">
+        <v>143.73110098180126</v>
+      </c>
+      <c r="C8" s="23">
+        <v>144.39921210111396</v>
+      </c>
+      <c r="D8" s="23">
+        <v>144.67513342804011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>42583</v>
+      </c>
+      <c r="B9" s="23">
+        <v>143.6741026486049</v>
+      </c>
+      <c r="C9" s="23">
+        <v>145.62043889194493</v>
+      </c>
+      <c r="D9" s="23">
+        <v>144.67880875989925</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>42614</v>
+      </c>
+      <c r="B10" s="23">
+        <v>142.00773744282046</v>
+      </c>
+      <c r="C10" s="23">
+        <v>145.03341956640961</v>
+      </c>
+      <c r="D10" s="23">
+        <v>144.81345089315406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>42644</v>
+      </c>
+      <c r="B11" s="23">
+        <v>141.13686329808141</v>
+      </c>
+      <c r="C11" s="23">
+        <v>145.09054426028209</v>
+      </c>
+      <c r="D11" s="23">
+        <v>145.0698131611889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>42675</v>
+      </c>
+      <c r="B12" s="23">
+        <v>144.93832064073018</v>
+      </c>
+      <c r="C12" s="23">
+        <v>145.67736478979973</v>
+      </c>
+      <c r="D12" s="23">
+        <v>145.43353993711725</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>42705</v>
+      </c>
+      <c r="B13" s="23">
+        <v>142.59014516031914</v>
+      </c>
+      <c r="C13" s="23">
+        <v>147.00954739359531</v>
+      </c>
+      <c r="D13" s="23">
+        <v>145.89164707867505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="23">
+        <v>136.63265948871938</v>
+      </c>
+      <c r="C14" s="23">
+        <v>147.43304880344542</v>
+      </c>
+      <c r="D14" s="23">
+        <v>146.4277638128531</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>42767</v>
+      </c>
+      <c r="B15" s="23">
+        <v>132.15851634216529</v>
+      </c>
+      <c r="C15" s="23">
+        <v>146.54896179506076</v>
+      </c>
+      <c r="D15" s="23">
+        <v>147.02441785768747</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>42795</v>
+      </c>
+      <c r="B16" s="23">
+        <v>152.62095855115726</v>
+      </c>
+      <c r="C16" s="23">
+        <v>147.93111776325944</v>
+      </c>
+      <c r="D16" s="23">
+        <v>147.66191168969772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>42826</v>
+      </c>
+      <c r="B17" s="23">
+        <v>151.9463447793168</v>
+      </c>
+      <c r="C17" s="23">
+        <v>147.86943169088605</v>
+      </c>
+      <c r="D17" s="23">
+        <v>148.31731527948702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>42856</v>
+      </c>
+      <c r="B18" s="23">
+        <v>168.38920945875748</v>
+      </c>
+      <c r="C18" s="23">
+        <v>148.67510979933559</v>
+      </c>
+      <c r="D18" s="23">
+        <v>148.96269149558529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>42887</v>
+      </c>
+      <c r="B19" s="23">
+        <v>161.03568550523303</v>
+      </c>
+      <c r="C19" s="23">
+        <v>150.16516109020674</v>
+      </c>
+      <c r="D19" s="23">
+        <v>149.56568873396364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>42917</v>
+      </c>
+      <c r="B20" s="23">
+        <v>150.30605023792245</v>
+      </c>
+      <c r="C20" s="23">
+        <v>150.28622761439061</v>
+      </c>
+      <c r="D20" s="23">
+        <v>150.09250859263668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>42948</v>
+      </c>
+      <c r="B21" s="23">
+        <v>149.2553428218971</v>
+      </c>
+      <c r="C21" s="23">
+        <v>150.23081510122597</v>
+      </c>
+      <c r="D21" s="23">
+        <v>150.50849335682327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>42979</v>
+      </c>
+      <c r="B22" s="23">
+        <v>146.3865594956952</v>
+      </c>
+      <c r="C22" s="23">
+        <v>151.18881881284912</v>
+      </c>
+      <c r="D22" s="23">
+        <v>150.78029547567192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>43009</v>
+      </c>
+      <c r="B23" s="23">
+        <v>149.38594914967302</v>
+      </c>
+      <c r="C23" s="23">
+        <v>151.50665447468469</v>
+      </c>
+      <c r="D23" s="23">
+        <v>150.88197691345263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>43040</v>
+      </c>
+      <c r="B24" s="23">
+        <v>151.92604263437079</v>
+      </c>
+      <c r="C24" s="23">
+        <v>152.5738862671258</v>
+      </c>
+      <c r="D24" s="23">
+        <v>150.7914474050211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>43070</v>
+      </c>
+      <c r="B25" s="23">
+        <v>146.78338564322195</v>
+      </c>
+      <c r="C25" s="23">
+        <v>152.41747111921032</v>
+      </c>
+      <c r="D25" s="23">
+        <v>150.49895078699876</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>43101</v>
+      </c>
+      <c r="B26" s="23">
+        <v>142.74091494479157</v>
+      </c>
+      <c r="C26" s="23">
+        <v>152.049567975928</v>
+      </c>
+      <c r="D26" s="23">
+        <v>150.01087181930532</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>43132</v>
+      </c>
+      <c r="B27" s="23">
+        <v>138.81804133746769</v>
+      </c>
+      <c r="C27" s="23">
+        <v>151.91912999127334</v>
+      </c>
+      <c r="D27" s="23">
+        <v>149.34841696716697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>43160</v>
+      </c>
+      <c r="B28" s="23">
+        <v>155.85731621133985</v>
+      </c>
+      <c r="C28" s="23">
+        <v>151.27607772530757</v>
+      </c>
+      <c r="D28" s="23">
+        <v>148.54586408630811</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>43191</v>
+      </c>
+      <c r="B29" s="23">
+        <v>151.52453339184243</v>
+      </c>
+      <c r="C29" s="23">
+        <v>146.85651606456457</v>
+      </c>
+      <c r="D29" s="23">
+        <v>147.65178286935722</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43221</v>
+      </c>
+      <c r="B30" s="23">
+        <v>159.56668791297358</v>
+      </c>
+      <c r="C30" s="23">
+        <v>144.4633664791784</v>
+      </c>
+      <c r="D30" s="23">
+        <v>146.72295113348949</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>43252</v>
+      </c>
+      <c r="B31" s="23">
+        <v>151.12577829049906</v>
+      </c>
+      <c r="C31" s="23">
+        <v>143.15799320154153</v>
+      </c>
+      <c r="D31" s="23">
+        <v>145.81554418920726</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>43282</v>
+      </c>
+      <c r="B32" s="23">
+        <v>145.96357240386445</v>
+      </c>
+      <c r="C32" s="23">
+        <v>143.2354740585497</v>
+      </c>
+      <c r="D32" s="23">
+        <v>144.97796299434677</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>43313</v>
+      </c>
+      <c r="B33" s="23">
+        <v>146.7659802568086</v>
+      </c>
+      <c r="C33" s="23">
+        <v>146.61283889394917</v>
+      </c>
+      <c r="D33" s="23">
+        <v>144.2541693412889</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>43344</v>
+      </c>
+      <c r="B34" s="23">
+        <v>137.74650152211899</v>
+      </c>
+      <c r="C34" s="23">
+        <v>143.21102213875625</v>
+      </c>
+      <c r="D34" s="23">
+        <v>143.67328891291842</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>43374</v>
+      </c>
+      <c r="B35" s="23">
+        <v>142.84305870083375</v>
+      </c>
+      <c r="C35" s="23">
+        <v>143.59717491783144</v>
+      </c>
+      <c r="D35" s="23">
+        <v>143.24946950424359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>43405</v>
+      </c>
+      <c r="B36" s="23">
+        <v>140.59231573260089</v>
+      </c>
+      <c r="C36" s="23">
+        <v>141.57330496985571</v>
+      </c>
+      <c r="D36" s="23">
+        <v>142.98149848827566</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>43435</v>
+      </c>
+      <c r="B37" s="23">
+        <v>136.25192484552474</v>
+      </c>
+      <c r="C37" s="23">
+        <v>141.84415935161917</v>
+      </c>
+      <c r="D37" s="23">
+        <v>142.85441958342255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>43466</v>
+      </c>
+      <c r="B38" s="23">
+        <v>134.52056075482315</v>
+      </c>
+      <c r="C38" s="23">
+        <v>143.05186389005311</v>
+      </c>
+      <c r="D38" s="23">
+        <v>142.84054834885427</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>43497</v>
+      </c>
+      <c r="B39" s="23">
+        <v>132.27529838944116</v>
+      </c>
+      <c r="C39" s="23">
+        <v>143.47820870139054</v>
+      </c>
+      <c r="D39" s="23">
+        <v>142.90357305727738</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>43525</v>
+      </c>
+      <c r="B40" s="23">
+        <v>144.87373844609147</v>
+      </c>
+      <c r="C40" s="23">
+        <v>141.20484515839215</v>
+      </c>
+      <c r="D40" s="23">
+        <v>143.0024644035359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>43556</v>
+      </c>
+      <c r="B41" s="23">
+        <v>149.89913655926117</v>
+      </c>
+      <c r="C41" s="23">
+        <v>142.56731949207088</v>
+      </c>
+      <c r="D41" s="23">
+        <v>143.0953673108624</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>43586</v>
+      </c>
+      <c r="B42" s="23">
+        <v>164.14987183044366</v>
+      </c>
+      <c r="C42" s="23">
+        <v>144.53655329241874</v>
+      </c>
+      <c r="D42" s="23">
+        <v>143.14481092625027</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>43617</v>
+      </c>
+      <c r="B43" s="23">
+        <v>150.84993450464239</v>
+      </c>
+      <c r="C43" s="23">
+        <v>143.7763589018094</v>
+      </c>
+      <c r="D43" s="23">
+        <v>143.11657542228173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43647</v>
+      </c>
+      <c r="B44" s="23">
+        <v>146.76823785681836</v>
+      </c>
+      <c r="C44" s="23">
+        <v>145.48526409814801</v>
+      </c>
+      <c r="D44" s="23">
+        <v>142.98520983060877</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>43678</v>
+      </c>
+      <c r="B45" s="23">
+        <v>141.2794360493493</v>
+      </c>
+      <c r="C45" s="23">
+        <v>144.94695205327204</v>
+      </c>
+      <c r="D45" s="23">
+        <v>142.73237556015101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>43709</v>
+      </c>
+      <c r="B46" s="23">
+        <v>134.88987734969228</v>
+      </c>
+      <c r="C46" s="23">
+        <v>141.13849220486793</v>
+      </c>
+      <c r="D46" s="23">
+        <v>142.34960438785279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>43739</v>
+      </c>
+      <c r="B47" s="23">
+        <v>141.51078863832441</v>
+      </c>
+      <c r="C47" s="23">
+        <v>143.46543403904352</v>
+      </c>
+      <c r="D47" s="23">
+        <v>141.839344820169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>43770</v>
+      </c>
+      <c r="B48" s="23">
+        <v>137.65812409402241</v>
+      </c>
+      <c r="C48" s="23">
+        <v>140.609789502399</v>
+      </c>
+      <c r="D48" s="23">
+        <v>141.21223023562385</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>43800</v>
+      </c>
+      <c r="B49" s="23">
+        <v>135.67189223323882</v>
+      </c>
+      <c r="C49" s="23">
+        <v>140.08581558554602</v>
+      </c>
+      <c r="D49" s="23">
+        <v>140.49532939882963</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>43831</v>
+      </c>
+      <c r="B50" s="23">
+        <v>132.28223124569112</v>
+      </c>
+      <c r="C50" s="23">
+        <v>140.92680743730625</v>
+      </c>
+      <c r="D50" s="23">
+        <v>139.7260606903881</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>43862</v>
+      </c>
+      <c r="B51" s="23">
+        <v>129.74514663170137</v>
+      </c>
+      <c r="C51" s="23">
+        <v>140.47384259570757</v>
+      </c>
+      <c r="D51" s="23">
+        <v>138.94856019337411</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>43891</v>
+      </c>
+      <c r="B52" s="23">
+        <v>129.0977252138824</v>
+      </c>
+      <c r="C52" s="23">
+        <v>125.41401660184215</v>
+      </c>
+      <c r="D52" s="23">
+        <v>138.20808648877932</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>43922</v>
+      </c>
+      <c r="B53" s="23">
+        <v>111.90395316317499</v>
+      </c>
+      <c r="C53" s="23">
+        <v>105.21308015881309</v>
+      </c>
+      <c r="D53" s="23">
+        <v>137.54939442250827</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>43952</v>
+      </c>
+      <c r="B54" s="23">
+        <v>131.29461300494506</v>
+      </c>
+      <c r="C54" s="23">
+        <v>116.44348319578269</v>
+      </c>
+      <c r="D54" s="23">
+        <v>137.00727052395177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
+        <v>43983</v>
+      </c>
+      <c r="B55" s="23">
+        <v>133.30386653957163</v>
+      </c>
+      <c r="C55" s="23">
+        <v>124.48594393290077</v>
+      </c>
+      <c r="D55" s="23">
+        <v>136.60517654287645</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
+        <v>44013</v>
+      </c>
+      <c r="B56" s="23">
+        <v>128.19080278245926</v>
+      </c>
+      <c r="C56" s="23">
+        <v>126.71465647194331</v>
+      </c>
+      <c r="D56" s="23">
+        <v>136.35712034787747</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
+        <v>44044</v>
+      </c>
+      <c r="B57" s="23">
+        <v>125.17406632349137</v>
+      </c>
+      <c r="C57" s="23">
+        <v>129.30360982294195</v>
+      </c>
+      <c r="D57" s="23">
+        <v>136.26546813575504</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
+        <v>44075</v>
+      </c>
+      <c r="B58" s="23">
+        <v>126.59614565623438</v>
+      </c>
+      <c r="C58" s="23">
+        <v>131.23094969391684</v>
+      </c>
+      <c r="D58" s="23">
+        <v>136.3213351966003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>44105</v>
+      </c>
+      <c r="B59" s="23">
+        <v>131.72739168680206</v>
+      </c>
+      <c r="C59" s="23">
+        <v>134.18128510718887</v>
+      </c>
+      <c r="D59" s="23">
+        <v>136.50970722051457</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="18">
+        <v>44136</v>
+      </c>
+      <c r="B60" s="23">
+        <v>132.96973762254197</v>
+      </c>
+      <c r="C60" s="23">
+        <v>135.24331515986353</v>
+      </c>
+      <c r="D60" s="23">
+        <v>136.81530774134865</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="18">
+        <v>44166</v>
+      </c>
+      <c r="B61" s="23">
+        <v>132.42198051947332</v>
+      </c>
+      <c r="C61" s="23">
+        <v>135.07667040389356</v>
+      </c>
+      <c r="D61" s="23">
+        <v>137.21900202788663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>44197</v>
+      </c>
+      <c r="B62" s="23">
+        <v>129.49276757333357</v>
+      </c>
+      <c r="C62" s="23">
+        <v>139.88540873148725</v>
+      </c>
+      <c r="D62" s="23">
+        <v>137.70744768509203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>44228</v>
+      </c>
+      <c r="B63" s="23">
+        <v>126.69382319800599</v>
+      </c>
+      <c r="C63" s="23">
+        <v>138.00827627302886</v>
+      </c>
+      <c r="D63" s="23">
+        <v>138.27414369065789</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>44256</v>
+      </c>
+      <c r="B64" s="23">
+        <v>146.28771620784292</v>
+      </c>
+      <c r="C64" s="23">
+        <v>139.62033675897746</v>
+      </c>
+      <c r="D64" s="23">
+        <v>138.91460931275324</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>44287</v>
+      </c>
+      <c r="B65" s="23">
+        <v>144.90576544617173</v>
+      </c>
+      <c r="C65" s="23">
+        <v>137.97923540402439</v>
+      </c>
+      <c r="D65" s="23">
+        <v>139.62469470435929</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>44317</v>
+      </c>
+      <c r="B66" s="23">
+        <v>150.14868925533764</v>
+      </c>
+      <c r="C66" s="23">
+        <v>136.62395416854335</v>
+      </c>
+      <c r="D66" s="23">
+        <v>140.39946643054387</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B67" s="23">
+        <v>148.94396513599037</v>
+      </c>
+      <c r="C67" s="23">
+        <v>140.56337413383557</v>
+      </c>
+      <c r="D67" s="23">
+        <v>141.22465096830112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B68" s="23">
+        <v>143.1827570387415</v>
+      </c>
+      <c r="C68" s="23">
+        <v>142.23818738567508</v>
+      </c>
+      <c r="D68" s="23">
+        <v>142.08271224568463</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>44409</v>
+      </c>
+      <c r="B69" s="23">
+        <v>141.20571583640663</v>
+      </c>
+      <c r="C69" s="23">
+        <v>144.22434592772771</v>
+      </c>
+      <c r="D69" s="23">
+        <v>142.94703255499016</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>44440</v>
+      </c>
+      <c r="B70" s="23">
+        <v>140.94554305470595</v>
+      </c>
+      <c r="C70" s="23">
+        <v>145.47636915433617</v>
+      </c>
+      <c r="D70" s="23">
+        <v>143.7872752325373</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>44470</v>
+      </c>
+      <c r="B71" s="23">
+        <v>140.49004342379754</v>
+      </c>
+      <c r="C71" s="23">
+        <v>144.53854660195259</v>
+      </c>
+      <c r="D71" s="23">
+        <v>144.57288714025364</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>44501</v>
+      </c>
+      <c r="B72" s="23">
+        <v>145.32981978314771</v>
+      </c>
+      <c r="C72" s="23">
+        <v>146.35938683018313</v>
+      </c>
+      <c r="D72" s="23">
+        <v>145.2817323311366</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>44531</v>
+      </c>
+      <c r="B73" s="23">
+        <v>145.62615550894006</v>
+      </c>
+      <c r="C73" s="23">
+        <v>147.7353390335428</v>
+      </c>
+      <c r="D73" s="23">
+        <v>145.90323586651684</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B74" s="23">
+        <v>136.06700195253066</v>
+      </c>
+      <c r="C74" s="23">
+        <v>146.65261912716201</v>
+      </c>
+      <c r="D74" s="23">
+        <v>146.43963965561588</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>44593</v>
+      </c>
+      <c r="B75" s="24">
+        <v>138.17655785876821</v>
+      </c>
+      <c r="C75" s="24">
+        <v>149.21948044703143</v>
+      </c>
+      <c r="D75" s="24">
+        <v>146.90366897683356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
@@ -2174,22 +3720,22 @@
       <c r="A2" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="35">
         <v>11.6</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="35">
         <v>11.7</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="35">
         <v>12.9</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="39">
         <v>15.5</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="35">
         <v>15.7</v>
       </c>
-      <c r="G2" s="36">
+      <c r="G2" s="35">
         <v>11.7</v>
       </c>
       <c r="H2" s="21">
@@ -2200,22 +3746,22 @@
       <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="35">
         <v>7.5</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="35">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="35">
         <v>6.9</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="39">
         <v>9.6</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="35">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="35">
         <v>11.5</v>
       </c>
       <c r="H3" s="21">
@@ -2226,22 +3772,22 @@
       <c r="A4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="35">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="35">
         <v>8.4</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="35">
         <v>8.9</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="39">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="35">
         <v>9.5</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>7.6</v>
       </c>
       <c r="H4" s="21">
@@ -2252,22 +3798,22 @@
       <c r="A5" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="35">
         <v>1.5</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="35">
         <v>6</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="39">
         <v>5.2</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="35">
         <v>3.4</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>6.1</v>
       </c>
       <c r="H5" s="21">
@@ -2278,22 +3824,22 @@
       <c r="A6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="35">
         <v>2.4</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <v>3.4</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="35">
         <v>3</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="39">
         <v>2.5</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="35">
         <v>0.3</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>2.2999999999999998</v>
       </c>
       <c r="H6" s="21">
@@ -2304,22 +3850,22 @@
       <c r="A7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="35">
         <v>-4.9000000000000004</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>5.8</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="35">
         <v>7.1</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="39">
         <v>3.2</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="35">
         <v>7</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="35">
         <v>8.6</v>
       </c>
       <c r="H7" s="21">
@@ -2330,22 +3876,22 @@
       <c r="A8" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="35">
         <v>6.4</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <v>6.8</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="35">
         <v>6.9</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="39">
         <v>7</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>8.1</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>8.1999999999999993</v>
       </c>
       <c r="H8" s="22">
@@ -2356,22 +3902,22 @@
       <c r="A9" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="35">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <v>4.3</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="35">
         <v>3.3</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="39">
         <v>4.8</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="35">
         <v>5.8</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="35">
         <v>4</v>
       </c>
       <c r="H9" s="21">
@@ -2382,22 +3928,22 @@
       <c r="A10" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="35">
         <v>3.8</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <v>4.2</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="35">
         <v>5.4</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <v>3.8</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="35">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>5.0999999999999996</v>
       </c>
       <c r="H10" s="21">
@@ -2453,19 +3999,19 @@
       <c r="B2" s="27">
         <v>6.7</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="37">
         <v>6.7</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>6.6</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="37">
         <v>7.2</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="37">
         <v>6.8</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="37">
         <v>6.8</v>
       </c>
       <c r="H2" s="29">
@@ -2479,19 +4025,19 @@
       <c r="B3" s="26">
         <v>7.2</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="36">
         <v>6.1</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="36">
         <v>7.9</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="36">
         <v>7.7</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="36">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="36">
         <v>9.1</v>
       </c>
       <c r="H3" s="28">
@@ -2505,19 +4051,19 @@
       <c r="B4" s="26">
         <v>5.7</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="36">
         <v>6</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <v>5.6</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="36">
         <v>3.8</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="36">
         <v>5.2</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>6.1</v>
       </c>
       <c r="H4" s="28">
@@ -2531,19 +4077,19 @@
       <c r="B5" s="26">
         <v>10.9</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36">
         <v>13.6</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="36">
         <v>9.1</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="36">
         <v>7.5</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <v>6.4</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="36">
         <v>7.6</v>
       </c>
       <c r="H5" s="28">
@@ -2557,19 +4103,19 @@
       <c r="B6" s="26">
         <v>7.7</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <v>8.4</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="36">
         <v>6</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="36">
         <v>15.4</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <v>5.6</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="36">
         <v>6.3</v>
       </c>
       <c r="H6" s="28">
@@ -2583,19 +4129,19 @@
       <c r="B7" s="26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="36">
         <v>4.3</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="36">
         <v>3.7</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="36">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="36">
         <v>5.2</v>
       </c>
       <c r="H7" s="28">
@@ -2609,19 +4155,19 @@
       <c r="B8" s="26">
         <v>5</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <v>5.5</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="36">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="36">
         <v>4.5</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="36">
         <v>5.2</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="36">
         <v>4.3</v>
       </c>
       <c r="H8" s="28">
@@ -2635,19 +4181,19 @@
       <c r="B9" s="26">
         <v>5.5</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="36">
         <v>5</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="36">
         <v>5.5</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="36">
         <v>8</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="36">
         <v>6.1</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="36">
         <v>6.6</v>
       </c>
       <c r="H9" s="28">
@@ -2661,19 +4207,19 @@
       <c r="B10" s="26">
         <v>3.4</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="36">
         <v>1.9</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="36">
         <v>5.5</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="36">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="36">
         <v>4</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="36">
         <v>2.1</v>
       </c>
       <c r="H10" s="28">
@@ -2687,19 +4233,19 @@
       <c r="B11" s="26">
         <v>3.3</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="36">
         <v>2.4</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="36">
         <v>4.5</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="36">
         <v>3</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <v>3.3</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="36">
         <v>3.3</v>
       </c>
       <c r="H11" s="28">
@@ -2713,19 +4259,19 @@
       <c r="B12" s="26">
         <v>23.6</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="36">
         <v>22.1</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="36">
         <v>25.8</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="36">
         <v>25.6</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="36">
         <v>19</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="36">
         <v>15.3</v>
       </c>
       <c r="H12" s="28">
@@ -2739,19 +4285,19 @@
       <c r="B13" s="26">
         <v>5.4</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="36">
         <v>5.8</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="36">
         <v>5.2</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13" s="36">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="36">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="36">
         <v>4.7</v>
       </c>
       <c r="H13" s="28">
@@ -2765,19 +4311,19 @@
       <c r="B14" s="26">
         <v>5.5</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="36">
         <v>5.9</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="36">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="36">
         <v>5.3</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="36">
         <v>4.8</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="36">
         <v>5.5</v>
       </c>
       <c r="H14" s="28">
@@ -2833,22 +4379,22 @@
       <c r="B2" s="31">
         <v>55.1</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="38">
         <v>55.9</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="38">
         <v>53.7</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="38">
         <v>55.7</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="38">
         <v>54.6</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="38">
         <v>55.5</v>
       </c>
-      <c r="H2" s="39">
+      <c r="H2" s="38">
         <v>57.3</v>
       </c>
     </row>
@@ -4250,14 +5796,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4450,7 +5996,7 @@
       <c r="B13">
         <v>32.200000000000003</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="40">
         <v>39.700000000000003</v>
       </c>
       <c r="D13">
@@ -4861,14 +6407,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -5044,285 +6590,285 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="34">
-        <v>1850</v>
-      </c>
-      <c r="C2" s="41">
-        <v>2328</v>
+      <c r="B2" s="42">
+        <v>3091</v>
+      </c>
+      <c r="C2" s="42">
+        <v>4085</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-478</v>
+        <v>-994</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="34">
-        <v>781</v>
-      </c>
-      <c r="C3" s="41">
-        <v>125</v>
+      <c r="B3" s="42">
+        <v>1270</v>
+      </c>
+      <c r="C3" s="42">
+        <v>203</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>656</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="34">
-        <v>746</v>
-      </c>
-      <c r="C4" s="41">
-        <v>307</v>
+      <c r="B4" s="42">
+        <v>1269</v>
+      </c>
+      <c r="C4" s="42">
+        <v>502</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>439</v>
+        <v>767</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B5">
-        <v>123</v>
-      </c>
-      <c r="C5" s="41">
-        <v>5</v>
+      <c r="B5" s="42">
+        <v>241</v>
+      </c>
+      <c r="C5" s="42">
+        <v>7</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="34">
-        <v>1031</v>
-      </c>
-      <c r="C6" s="41">
-        <v>1137</v>
+      <c r="B6" s="42">
+        <v>1815</v>
+      </c>
+      <c r="C6" s="42">
+        <v>2018</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-106</v>
+        <v>-203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="34">
-        <v>1737</v>
-      </c>
-      <c r="C7" s="41">
-        <v>1715</v>
+      <c r="B7" s="42">
+        <v>2456</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2759</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>-303</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
-      <c r="B8">
-        <v>77</v>
-      </c>
-      <c r="C8" s="41">
-        <v>138</v>
+      <c r="B8" s="42">
+        <v>135</v>
+      </c>
+      <c r="C8" s="42">
+        <v>194</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-61</v>
+        <v>-59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B9">
-        <v>152</v>
-      </c>
-      <c r="C9" s="41">
-        <v>80</v>
+      <c r="B9" s="42">
+        <v>297</v>
+      </c>
+      <c r="C9" s="42">
+        <v>129</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
-      <c r="B10">
-        <v>142</v>
-      </c>
-      <c r="C10" s="41">
-        <v>44</v>
+      <c r="B10" s="42">
+        <v>149</v>
+      </c>
+      <c r="C10" s="42">
+        <v>116</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>98</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="34">
-        <v>1098</v>
-      </c>
-      <c r="C11" s="41">
-        <v>647</v>
+      <c r="B11" s="42">
+        <v>1861</v>
+      </c>
+      <c r="C11" s="42">
+        <v>1041</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>451</v>
+        <v>820</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="34">
-        <v>775</v>
-      </c>
-      <c r="C12" s="41">
-        <v>2779</v>
+      <c r="B12" s="42">
+        <v>1256</v>
+      </c>
+      <c r="C12" s="42">
+        <v>4402</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-2004</v>
+        <v>-3146</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="34">
-        <v>174</v>
-      </c>
-      <c r="C13" s="41">
-        <v>120</v>
+      <c r="B13" s="42">
+        <v>354</v>
+      </c>
+      <c r="C13" s="42">
+        <v>189</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="34">
-        <v>58</v>
-      </c>
-      <c r="C14" s="41">
-        <v>161</v>
+      <c r="B14" s="42">
+        <v>104</v>
+      </c>
+      <c r="C14" s="42">
+        <v>255</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-103</v>
+        <v>-151</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="34">
-        <v>511</v>
-      </c>
-      <c r="C15" s="41">
-        <v>293</v>
+      <c r="B15" s="42">
+        <v>909</v>
+      </c>
+      <c r="C15" s="42">
+        <v>411</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>218</v>
+        <v>498</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="34">
-        <v>582</v>
-      </c>
-      <c r="C16" s="41">
-        <v>480</v>
+      <c r="B16" s="42">
+        <v>896</v>
+      </c>
+      <c r="C16" s="42">
+        <v>791</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="34">
-        <v>673</v>
-      </c>
-      <c r="C17" s="41">
-        <v>36</v>
+      <c r="B17" s="42">
+        <v>1013</v>
+      </c>
+      <c r="C17" s="42">
+        <v>57</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>637</v>
+        <v>956</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>95</v>
       </c>
-      <c r="B18">
-        <v>120</v>
-      </c>
-      <c r="C18" s="41">
-        <v>42</v>
+      <c r="B18" s="42">
+        <v>171</v>
+      </c>
+      <c r="C18" s="42">
+        <v>52</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>96</v>
       </c>
-      <c r="B19">
-        <v>112</v>
-      </c>
-      <c r="C19" s="41">
-        <v>84</v>
+      <c r="B19" s="42">
+        <v>228</v>
+      </c>
+      <c r="C19" s="42">
+        <v>132</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="34">
-        <v>1249</v>
-      </c>
-      <c r="C20" s="42">
-        <v>365</v>
+      <c r="B20" s="43">
+        <v>1838</v>
+      </c>
+      <c r="C20" s="43">
+        <v>616</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>884</v>
+        <v>1222</v>
       </c>
     </row>
   </sheetData>
@@ -5332,1276 +6878,782 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D5C2F3-2F50-487E-8AA2-1FC33A905845}">
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2">
-        <v>580109.3654135036</v>
-      </c>
-      <c r="C2">
-        <v>8.2176039378516919</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3">
-        <v>36648.13652029309</v>
-      </c>
-      <c r="C3">
-        <v>4.3860998002780427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4">
-        <v>1249.7113603560397</v>
-      </c>
-      <c r="C4">
-        <v>-19.150143374614757</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5">
-        <v>22724.129989370613</v>
-      </c>
-      <c r="C5">
-        <v>18.247420162936258</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6">
-        <v>122710.03414797327</v>
-      </c>
-      <c r="C6">
-        <v>8.543915384800993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7">
-        <v>12285.490130430609</v>
-      </c>
-      <c r="C7">
-        <v>0.49655622972446523</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8">
-        <v>20987.63967740133</v>
-      </c>
-      <c r="C8">
-        <v>4.5268786278615414</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9">
-        <v>93443.748235928695</v>
-      </c>
-      <c r="C9">
-        <v>7.2357992351878675</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10">
-        <v>8992.2744681564727</v>
-      </c>
-      <c r="C10">
-        <v>60.938820792863964</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11">
-        <v>51632.157894787102</v>
-      </c>
-      <c r="C11">
-        <v>14.905791213603869</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12">
-        <v>26151.467050546846</v>
-      </c>
-      <c r="C12">
-        <v>0.37420012180280349</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="48">
+        <v>19352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="48">
+        <v>5819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="42">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="42">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="42">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="42">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="42">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="42">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="42">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="48">
+        <v>6702</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="42">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="42">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="42">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="42">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="42">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="42">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="42">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="42">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="42">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="42">
         <v>112</v>
       </c>
-      <c r="B13">
-        <v>79143.368376477825</v>
-      </c>
-      <c r="C13">
-        <v>6.5567187004549332</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14">
-        <v>34930.018675685875</v>
-      </c>
-      <c r="C14">
-        <v>11.909663098887879</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15">
-        <v>28516.783116102812</v>
-      </c>
-      <c r="C15">
-        <v>6.1375814244809535</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16">
-        <v>22663.778591606671</v>
-      </c>
-      <c r="C16">
-        <v>2.422746472798476</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17">
-        <v>14327.889062242892</v>
-      </c>
-      <c r="C17">
-        <v>10.245849380753791</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18">
-        <v>3702.7381161434578</v>
-      </c>
-      <c r="C18">
-        <v>1.7208283342252662</v>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="42">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="48">
+        <v>4952</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="42">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="42">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="42">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" s="42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" s="42">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="42">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="42">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="42">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="42">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="42">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="42">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="42">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" s="42">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48" s="48">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="42">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50" s="42">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" s="42">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" s="49">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="50">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D74"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>42370</v>
-      </c>
-      <c r="B2" s="23">
-        <v>134.74645041349706</v>
-      </c>
-      <c r="C2" s="23">
-        <v>148.139109026689</v>
-      </c>
-      <c r="D2" s="23">
-        <v>147.07160840981032</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>42401</v>
-      </c>
-      <c r="B3" s="23">
-        <v>134.23236103862521</v>
-      </c>
-      <c r="C3" s="23">
-        <v>146.69961289140326</v>
-      </c>
-      <c r="D3" s="23">
-        <v>146.483967919158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>42430</v>
-      </c>
-      <c r="B4" s="23">
-        <v>150.0878942366954</v>
-      </c>
-      <c r="C4" s="23">
-        <v>145.98766697459678</v>
-      </c>
-      <c r="D4" s="23">
-        <v>145.93285377374565</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>42461</v>
-      </c>
-      <c r="B5" s="23">
-        <v>153.25067436662908</v>
-      </c>
-      <c r="C5" s="23">
-        <v>145.19812212033054</v>
-      </c>
-      <c r="D5" s="23">
-        <v>145.45428715899183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>42491</v>
-      </c>
-      <c r="B6" s="23">
-        <v>163.51360808690507</v>
-      </c>
-      <c r="C6" s="23">
-        <v>144.40215353738799</v>
-      </c>
-      <c r="D6" s="23">
-        <v>145.07564667926081</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>42522</v>
-      </c>
-      <c r="B7" s="23">
-        <v>153.66209524099784</v>
-      </c>
-      <c r="C7" s="23">
-        <v>144.31416221953438</v>
-      </c>
-      <c r="D7" s="23">
-        <v>144.81868281054562</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>42552</v>
-      </c>
-      <c r="B8" s="23">
-        <v>143.73110098180126</v>
-      </c>
-      <c r="C8" s="23">
-        <v>144.38741543887232</v>
-      </c>
-      <c r="D8" s="23">
-        <v>144.69235979593122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>42583</v>
-      </c>
-      <c r="B9" s="23">
-        <v>143.6741026486049</v>
-      </c>
-      <c r="C9" s="23">
-        <v>145.60608227735642</v>
-      </c>
-      <c r="D9" s="23">
-        <v>144.69966672624665</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>42614</v>
-      </c>
-      <c r="B10" s="23">
-        <v>142.00773744282046</v>
-      </c>
-      <c r="C10" s="23">
-        <v>145.05957284321801</v>
-      </c>
-      <c r="D10" s="23">
-        <v>144.83734366484433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>42644</v>
-      </c>
-      <c r="B11" s="23">
-        <v>141.13686329808141</v>
-      </c>
-      <c r="C11" s="23">
-        <v>145.09420974714644</v>
-      </c>
-      <c r="D11" s="23">
-        <v>145.09553807592803</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>42675</v>
-      </c>
-      <c r="B12" s="23">
-        <v>144.93832064073018</v>
-      </c>
-      <c r="C12" s="23">
-        <v>145.74632296742948</v>
-      </c>
-      <c r="D12" s="23">
-        <v>145.45889352267432</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>42705</v>
-      </c>
-      <c r="B13" s="23">
-        <v>142.59014516031914</v>
-      </c>
-      <c r="C13" s="23">
-        <v>146.93692372907955</v>
-      </c>
-      <c r="D13" s="23">
-        <v>145.91424840331939</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="23">
-        <v>136.63265948871938</v>
-      </c>
-      <c r="C14" s="23">
-        <v>147.41113461204898</v>
-      </c>
-      <c r="D14" s="23">
-        <v>146.44567113324348</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>42767</v>
-      </c>
-      <c r="B15" s="23">
-        <v>132.15851634216529</v>
-      </c>
-      <c r="C15" s="23">
-        <v>146.54015048204971</v>
-      </c>
-      <c r="D15" s="23">
-        <v>147.03645254032813</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>42795</v>
-      </c>
-      <c r="B16" s="23">
-        <v>152.62095855115726</v>
-      </c>
-      <c r="C16" s="23">
-        <v>147.96184326764569</v>
-      </c>
-      <c r="D16" s="23">
-        <v>147.66785461517631</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>42826</v>
-      </c>
-      <c r="B17" s="23">
-        <v>151.9463447793168</v>
-      </c>
-      <c r="C17" s="23">
-        <v>147.85652396642445</v>
-      </c>
-      <c r="D17" s="23">
-        <v>148.31778988846486</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>42856</v>
-      </c>
-      <c r="B18" s="23">
-        <v>168.38920945875748</v>
-      </c>
-      <c r="C18" s="23">
-        <v>148.63747781535935</v>
-      </c>
-      <c r="D18" s="23">
-        <v>148.95898986593699</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>42887</v>
-      </c>
-      <c r="B19" s="23">
-        <v>161.03568550523303</v>
-      </c>
-      <c r="C19" s="23">
-        <v>150.21570079862281</v>
-      </c>
-      <c r="D19" s="23">
-        <v>149.5591524303201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>42917</v>
-      </c>
-      <c r="B20" s="23">
-        <v>150.30605023792245</v>
-      </c>
-      <c r="C20" s="23">
-        <v>150.24764115729232</v>
-      </c>
-      <c r="D20" s="23">
-        <v>150.08456108965771</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>42948</v>
-      </c>
-      <c r="B21" s="23">
-        <v>149.2553428218971</v>
-      </c>
-      <c r="C21" s="23">
-        <v>150.25055553146149</v>
-      </c>
-      <c r="D21" s="23">
-        <v>150.50051560049172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>42979</v>
-      </c>
-      <c r="B22" s="23">
-        <v>146.3865594956952</v>
-      </c>
-      <c r="C22" s="23">
-        <v>151.20766483968907</v>
-      </c>
-      <c r="D22" s="23">
-        <v>150.77373680025241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>43009</v>
-      </c>
-      <c r="B23" s="23">
-        <v>149.38594914967302</v>
-      </c>
-      <c r="C23" s="23">
-        <v>151.54451595688116</v>
-      </c>
-      <c r="D23" s="23">
-        <v>150.87793260807464</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>43040</v>
-      </c>
-      <c r="B24" s="23">
-        <v>151.92604263437079</v>
-      </c>
-      <c r="C24" s="23">
-        <v>152.60793090348429</v>
-      </c>
-      <c r="D24" s="23">
-        <v>150.79036549399288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>43070</v>
-      </c>
-      <c r="B25" s="23">
-        <v>146.78338564322195</v>
-      </c>
-      <c r="C25" s="23">
-        <v>152.34556500063192</v>
-      </c>
-      <c r="D25" s="23">
-        <v>150.50077326010054</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>43101</v>
-      </c>
-      <c r="B26" s="23">
-        <v>142.74091494479157</v>
-      </c>
-      <c r="C26" s="23">
-        <v>152.00144379782142</v>
-      </c>
-      <c r="D26" s="23">
-        <v>150.01542141707731</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>43132</v>
-      </c>
-      <c r="B27" s="23">
-        <v>138.81804133746769</v>
-      </c>
-      <c r="C27" s="23">
-        <v>151.96394806261955</v>
-      </c>
-      <c r="D27" s="23">
-        <v>149.3553294810454</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>43160</v>
-      </c>
-      <c r="B28" s="23">
-        <v>155.85731621133985</v>
-      </c>
-      <c r="C28" s="23">
-        <v>151.27938383204514</v>
-      </c>
-      <c r="D28" s="23">
-        <v>148.55424801714975</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>43191</v>
-      </c>
-      <c r="B29" s="23">
-        <v>151.52453339184243</v>
-      </c>
-      <c r="C29" s="23">
-        <v>146.87340585645646</v>
-      </c>
-      <c r="D29" s="23">
-        <v>147.66007557512518</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>43221</v>
-      </c>
-      <c r="B30" s="23">
-        <v>159.56668791297358</v>
-      </c>
-      <c r="C30" s="23">
-        <v>144.42988052091167</v>
-      </c>
-      <c r="D30" s="23">
-        <v>146.72965786082921</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>43252</v>
-      </c>
-      <c r="B31" s="23">
-        <v>151.12577829049906</v>
-      </c>
-      <c r="C31" s="23">
-        <v>143.17458936789674</v>
-      </c>
-      <c r="D31" s="23">
-        <v>145.81872273332161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>43282</v>
-      </c>
-      <c r="B32" s="23">
-        <v>145.96357240386445</v>
-      </c>
-      <c r="C32" s="23">
-        <v>143.20050524024705</v>
-      </c>
-      <c r="D32" s="23">
-        <v>144.97540740406359</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>43313</v>
-      </c>
-      <c r="B33" s="23">
-        <v>146.7659802568086</v>
-      </c>
-      <c r="C33" s="23">
-        <v>146.66966926966157</v>
-      </c>
-      <c r="D33" s="23">
-        <v>144.24396586844074</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>43344</v>
-      </c>
-      <c r="B34" s="23">
-        <v>137.74650152211899</v>
-      </c>
-      <c r="C34" s="23">
-        <v>143.18916058132899</v>
-      </c>
-      <c r="D34" s="23">
-        <v>143.6535515456421</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>43374</v>
-      </c>
-      <c r="B35" s="23">
-        <v>142.84305870083375</v>
-      </c>
-      <c r="C35" s="23">
-        <v>143.61162662342136</v>
-      </c>
-      <c r="D35" s="23">
-        <v>143.21831260583366</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>43405</v>
-      </c>
-      <c r="B36" s="23">
-        <v>140.59231573260089</v>
-      </c>
-      <c r="C36" s="23">
-        <v>141.66959471705917</v>
-      </c>
-      <c r="D36" s="23">
-        <v>142.93818355135517</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>43435</v>
-      </c>
-      <c r="B37" s="23">
-        <v>136.25192484552474</v>
-      </c>
-      <c r="C37" s="23">
-        <v>141.73341789881025</v>
-      </c>
-      <c r="D37" s="23">
-        <v>142.79980513966638</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>43466</v>
-      </c>
-      <c r="B38" s="23">
-        <v>134.52056075482315</v>
-      </c>
-      <c r="C38" s="23">
-        <v>142.94319792611682</v>
-      </c>
-      <c r="D38" s="23">
-        <v>142.77706155258957</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>43497</v>
-      </c>
-      <c r="B39" s="23">
-        <v>132.27529838944116</v>
-      </c>
-      <c r="C39" s="23">
-        <v>143.57581774945962</v>
-      </c>
-      <c r="D39" s="23">
-        <v>142.83286981476959</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>43525</v>
-      </c>
-      <c r="B40" s="23">
-        <v>144.87373844609147</v>
-      </c>
-      <c r="C40" s="23">
-        <v>141.21590207424484</v>
-      </c>
-      <c r="D40" s="23">
-        <v>142.92834552559086</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>43556</v>
-      </c>
-      <c r="B41" s="23">
-        <v>149.89913655926117</v>
-      </c>
-      <c r="C41" s="23">
-        <v>142.56181720331321</v>
-      </c>
-      <c r="D41" s="23">
-        <v>143.02446830417739</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>43586</v>
-      </c>
-      <c r="B42" s="23">
-        <v>164.14987183044366</v>
-      </c>
-      <c r="C42" s="23">
-        <v>144.54803805815237</v>
-      </c>
-      <c r="D42" s="23">
-        <v>143.0859390852616</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>43617</v>
-      </c>
-      <c r="B43" s="23">
-        <v>150.84993450464239</v>
-      </c>
-      <c r="C43" s="23">
-        <v>143.77037642481855</v>
-      </c>
-      <c r="D43" s="23">
-        <v>143.07912122783236</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>43647</v>
-      </c>
-      <c r="B44" s="23">
-        <v>146.76823785681836</v>
-      </c>
-      <c r="C44" s="23">
-        <v>145.42125270260249</v>
-      </c>
-      <c r="D44" s="23">
-        <v>142.97747667854608</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>43678</v>
-      </c>
-      <c r="B45" s="23">
-        <v>141.2794360493493</v>
-      </c>
-      <c r="C45" s="23">
-        <v>145.00741083024602</v>
-      </c>
-      <c r="D45" s="23">
-        <v>142.75996063246714</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>43709</v>
-      </c>
-      <c r="B46" s="23">
-        <v>134.88987734969228</v>
-      </c>
-      <c r="C46" s="23">
-        <v>141.14204482342629</v>
-      </c>
-      <c r="D46" s="23">
-        <v>142.41434534506752</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>43739</v>
-      </c>
-      <c r="B47" s="23">
-        <v>141.51078863832441</v>
-      </c>
-      <c r="C47" s="23">
-        <v>143.45288494259788</v>
-      </c>
-      <c r="D47" s="23">
-        <v>141.93896829510354</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>43770</v>
-      </c>
-      <c r="B48" s="23">
-        <v>137.65812409402241</v>
-      </c>
-      <c r="C48" s="23">
-        <v>140.66237255014786</v>
-      </c>
-      <c r="D48" s="23">
-        <v>141.34095388454946</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>43800</v>
-      </c>
-      <c r="B49" s="23">
-        <v>135.67189223323882</v>
-      </c>
-      <c r="C49" s="23">
-        <v>140.04578163422929</v>
-      </c>
-      <c r="D49" s="23">
-        <v>140.64474140093998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>43831</v>
-      </c>
-      <c r="B50" s="23">
-        <v>132.28223124569112</v>
-      </c>
-      <c r="C50" s="23">
-        <v>140.79013043614304</v>
-      </c>
-      <c r="D50" s="23">
-        <v>139.88604061289249</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>43862</v>
-      </c>
-      <c r="B51" s="23">
-        <v>129.74514663170137</v>
-      </c>
-      <c r="C51" s="23">
-        <v>140.60282169870521</v>
-      </c>
-      <c r="D51" s="23">
-        <v>139.10863595334621</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>43891</v>
-      </c>
-      <c r="B52" s="23">
-        <v>129.0977252138824</v>
-      </c>
-      <c r="C52" s="23">
-        <v>125.42171449999771</v>
-      </c>
-      <c r="D52" s="23">
-        <v>138.35818442214642</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>43922</v>
-      </c>
-      <c r="B53" s="23">
-        <v>111.90395316317499</v>
-      </c>
-      <c r="C53" s="23">
-        <v>105.2098461794268</v>
-      </c>
-      <c r="D53" s="23">
-        <v>137.68201804658736</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>43952</v>
-      </c>
-      <c r="B54" s="23">
-        <v>131.29461300494506</v>
-      </c>
-      <c r="C54" s="23">
-        <v>116.47317016933816</v>
-      </c>
-      <c r="D54" s="23">
-        <v>137.11862902464813</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="16">
-        <v>43983</v>
-      </c>
-      <c r="B55" s="23">
-        <v>133.30386653957163</v>
-      </c>
-      <c r="C55" s="23">
-        <v>124.45949093873637</v>
-      </c>
-      <c r="D55" s="23">
-        <v>136.69515448755575</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16">
-        <v>44013</v>
-      </c>
-      <c r="B56" s="23">
-        <v>128.19080278245926</v>
-      </c>
-      <c r="C56" s="23">
-        <v>126.65386668787953</v>
-      </c>
-      <c r="D56" s="23">
-        <v>136.42834050880154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16">
-        <v>44044</v>
-      </c>
-      <c r="B57" s="23">
-        <v>125.17406632349137</v>
-      </c>
-      <c r="C57" s="23">
-        <v>129.3663149206532</v>
-      </c>
-      <c r="D57" s="23">
-        <v>136.32526741989781</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18">
-        <v>44075</v>
-      </c>
-      <c r="B58" s="23">
-        <v>126.59614565623438</v>
-      </c>
-      <c r="C58" s="23">
-        <v>131.22903438026464</v>
-      </c>
-      <c r="D58" s="23">
-        <v>136.38014896092403</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>44105</v>
-      </c>
-      <c r="B59" s="23">
-        <v>131.72739168680206</v>
-      </c>
-      <c r="C59" s="23">
-        <v>134.17056171093429</v>
-      </c>
-      <c r="D59" s="23">
-        <v>136.57898086523281</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="18">
-        <v>44136</v>
-      </c>
-      <c r="B60" s="23">
-        <v>132.96973762254197</v>
-      </c>
-      <c r="C60" s="23">
-        <v>135.29368154581678</v>
-      </c>
-      <c r="D60" s="23">
-        <v>136.90363699823831</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="18">
-        <v>44166</v>
-      </c>
-      <c r="B61" s="23">
-        <v>132.42198051947332</v>
-      </c>
-      <c r="C61" s="23">
-        <v>135.03702741418641</v>
-      </c>
-      <c r="D61" s="23">
-        <v>137.33453965057083</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
-        <v>44197</v>
-      </c>
-      <c r="B62" s="23">
-        <v>129.49276757333357</v>
-      </c>
-      <c r="C62" s="23">
-        <v>139.64335426908619</v>
-      </c>
-      <c r="D62" s="23">
-        <v>137.85390070175555</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
-        <v>44228</v>
-      </c>
-      <c r="B63" s="23">
-        <v>126.69382319800599</v>
-      </c>
-      <c r="C63" s="23">
-        <v>138.22565030927976</v>
-      </c>
-      <c r="D63" s="23">
-        <v>138.44791731142826</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
-        <v>44256</v>
-      </c>
-      <c r="B64" s="23">
-        <v>146.28771620784292</v>
-      </c>
-      <c r="C64" s="23">
-        <v>139.64501718511639</v>
-      </c>
-      <c r="D64" s="23">
-        <v>139.10717223359487</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
-        <v>44287</v>
-      </c>
-      <c r="B65" s="23">
-        <v>144.90576544617173</v>
-      </c>
-      <c r="C65" s="23">
-        <v>138.0052948445753</v>
-      </c>
-      <c r="D65" s="23">
-        <v>139.81881644586807</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
-        <v>44317</v>
-      </c>
-      <c r="B66" s="23">
-        <v>150.14868925533764</v>
-      </c>
-      <c r="C66" s="23">
-        <v>136.63853140773671</v>
-      </c>
-      <c r="D66" s="23">
-        <v>140.57050007116794</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
-        <v>44348</v>
-      </c>
-      <c r="B67" s="23">
-        <v>148.94396513599037</v>
-      </c>
-      <c r="C67" s="23">
-        <v>140.52273745407999</v>
-      </c>
-      <c r="D67" s="23">
-        <v>141.34419744582991</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
-        <v>44378</v>
-      </c>
-      <c r="B68" s="23">
-        <v>143.1827570387415</v>
-      </c>
-      <c r="C68" s="23">
-        <v>142.15098179747358</v>
-      </c>
-      <c r="D68" s="23">
-        <v>142.11756457090485</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
-        <v>44409</v>
-      </c>
-      <c r="B69" s="23">
-        <v>141.20571583640663</v>
-      </c>
-      <c r="C69" s="23">
-        <v>144.37019481414114</v>
-      </c>
-      <c r="D69" s="23">
-        <v>142.86106683298576</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
-        <v>44440</v>
-      </c>
-      <c r="B70" s="23">
-        <v>140.94554305470595</v>
-      </c>
-      <c r="C70" s="23">
-        <v>145.41772585610909</v>
-      </c>
-      <c r="D70" s="23">
-        <v>143.54515118614222</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>44470</v>
-      </c>
-      <c r="B71" s="23">
-        <v>140.53928207853662</v>
-      </c>
-      <c r="C71" s="23">
-        <v>144.52125619506972</v>
-      </c>
-      <c r="D71" s="23">
-        <v>144.14196855095184</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
-        <v>44501</v>
-      </c>
-      <c r="B72" s="23">
-        <v>145.25244923103682</v>
-      </c>
-      <c r="C72" s="23">
-        <v>146.26718479231505</v>
-      </c>
-      <c r="D72" s="23">
-        <v>144.63260266756626</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
-        <v>44531</v>
-      </c>
-      <c r="B73" s="23">
-        <v>145.65428740631165</v>
-      </c>
-      <c r="C73" s="23">
-        <v>147.84483147827757</v>
-      </c>
-      <c r="D73" s="23">
-        <v>145.0110078556213</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
-        <v>44562</v>
-      </c>
-      <c r="B74" s="24">
-        <v>136.51119002060923</v>
-      </c>
-      <c r="C74" s="24">
-        <v>147.05486359872521</v>
-      </c>
-      <c r="D74" s="24">
-        <v>145.28387928059126</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="48">
+        <v>17958</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="48">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="42">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="42">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="42">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="42">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="48">
+        <v>6698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="42">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="42">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="42">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="42">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" s="42">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="42">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="42">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="42">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="42">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="48">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="42">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="42">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="48">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="42">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="42">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" s="42">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="48">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="42">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="42">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" s="42">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="42">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="42">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" s="42">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="42">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="42">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="42">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="42">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="42">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="42">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="48">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" s="54">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="B40" s="55">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"Actualizo con datos del EMAE marzo22 e ICA abril22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F92DB2-E17B-45AE-BDE4-5104A9BDE284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE0A110-AB20-488E-8EBD-CFC5BC285891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -2625,11 +2625,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2660,10 +2658,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="23">
-        <v>148.12674938601256</v>
+        <v>148.08853680440737</v>
       </c>
       <c r="D2" s="23">
-        <v>147.07826915508767</v>
+        <v>147.07894467655603</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,10 +2672,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="23">
-        <v>146.71851040460982</v>
+        <v>146.70619723584508</v>
       </c>
       <c r="D3" s="23">
-        <v>146.48875794209332</v>
+        <v>146.48714841044227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,10 +2686,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="23">
-        <v>145.98112910209053</v>
+        <v>145.9600809116663</v>
       </c>
       <c r="D4" s="23">
-        <v>145.934409413612</v>
+        <v>145.9314129916221</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,10 +2700,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="23">
-        <v>145.16531814296513</v>
+        <v>145.14648926456528</v>
       </c>
       <c r="D5" s="23">
-        <v>145.45156266489744</v>
+        <v>145.4484988339953</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2716,10 +2714,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="23">
-        <v>144.42520822906147</v>
+        <v>144.41002576177334</v>
       </c>
       <c r="D6" s="23">
-        <v>145.0679762154688</v>
+        <v>145.0660776782787</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2730,10 +2728,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="23">
-        <v>144.32391150524907</v>
+        <v>144.32084098901501</v>
       </c>
       <c r="D7" s="23">
-        <v>144.80592840803149</v>
+        <v>144.80563188527731</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2744,10 +2742,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="23">
-        <v>144.39921210111396</v>
+        <v>144.41702424435491</v>
       </c>
       <c r="D8" s="23">
-        <v>144.67513342804011</v>
+        <v>144.67667005064152</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2758,10 +2756,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="23">
-        <v>145.62043889194493</v>
+        <v>145.63675890860722</v>
       </c>
       <c r="D9" s="23">
-        <v>144.67880875989925</v>
+        <v>144.68234256093007</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2772,10 +2770,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="23">
-        <v>145.03341956640961</v>
+        <v>145.04660934341729</v>
       </c>
       <c r="D10" s="23">
-        <v>144.81345089315406</v>
+        <v>144.81910074296363</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,10 +2784,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="23">
-        <v>145.09054426028209</v>
+        <v>145.12013199673038</v>
       </c>
       <c r="D11" s="23">
-        <v>145.0698131611889</v>
+        <v>145.07742076669075</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,10 +2798,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="23">
-        <v>145.67736478979973</v>
+        <v>145.70331286246744</v>
       </c>
       <c r="D12" s="23">
-        <v>145.43353993711725</v>
+        <v>145.44250608592509</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,10 +2812,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="23">
-        <v>147.00954739359531</v>
+        <v>147.0153454425913</v>
       </c>
       <c r="D13" s="23">
-        <v>145.89164707867505</v>
+        <v>145.90146317744833</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2825,13 +2823,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="23">
-        <v>136.63265948871938</v>
+        <v>136.63265948871936</v>
       </c>
       <c r="C14" s="23">
-        <v>147.43304880344542</v>
+        <v>147.38041978722117</v>
       </c>
       <c r="D14" s="23">
-        <v>146.4277638128531</v>
+        <v>146.43825001671178</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,13 +2837,13 @@
         <v>42767</v>
       </c>
       <c r="B15" s="23">
-        <v>132.15851634216529</v>
+        <v>132.15851634216523</v>
       </c>
       <c r="C15" s="23">
-        <v>146.54896179506076</v>
+        <v>146.55158941664945</v>
       </c>
       <c r="D15" s="23">
-        <v>147.02441785768747</v>
+        <v>147.03575203606499</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2853,13 +2851,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="23">
-        <v>152.62095855115726</v>
+        <v>152.6209585511572</v>
       </c>
       <c r="C16" s="23">
-        <v>147.93111776325944</v>
+        <v>147.89613355347745</v>
       </c>
       <c r="D16" s="23">
-        <v>147.66191168969772</v>
+        <v>147.67452842530699</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2867,13 +2865,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="23">
-        <v>151.9463447793168</v>
+        <v>151.94634477931669</v>
       </c>
       <c r="C17" s="23">
-        <v>147.86943169088605</v>
+        <v>147.82540901566927</v>
       </c>
       <c r="D17" s="23">
-        <v>148.31731527948702</v>
+        <v>148.33170328763387</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2881,13 +2879,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="23">
-        <v>168.38920945875748</v>
+        <v>168.38920945875742</v>
       </c>
       <c r="C18" s="23">
-        <v>148.67510979933559</v>
+        <v>148.63176519921871</v>
       </c>
       <c r="D18" s="23">
-        <v>148.96269149558529</v>
+        <v>148.97919974928044</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2895,13 +2893,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="23">
-        <v>161.03568550523303</v>
+        <v>161.03568550523295</v>
       </c>
       <c r="C19" s="23">
-        <v>150.16516109020674</v>
+        <v>150.14721123530421</v>
       </c>
       <c r="D19" s="23">
-        <v>149.56568873396364</v>
+        <v>149.58452657115831</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2909,13 +2907,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="23">
-        <v>150.30605023792245</v>
+        <v>150.30605023792242</v>
       </c>
       <c r="C20" s="23">
-        <v>150.28622761439061</v>
+        <v>150.28090328064201</v>
       </c>
       <c r="D20" s="23">
-        <v>150.09250859263668</v>
+        <v>150.11347798705404</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2923,13 +2921,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="23">
-        <v>149.2553428218971</v>
+        <v>149.25534282189705</v>
       </c>
       <c r="C21" s="23">
-        <v>150.23081510122597</v>
+        <v>150.25825677377873</v>
       </c>
       <c r="D21" s="23">
-        <v>150.50849335682327</v>
+        <v>150.53083861774516</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2937,13 +2935,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="23">
-        <v>146.3865594956952</v>
+        <v>146.38655949569505</v>
       </c>
       <c r="C22" s="23">
-        <v>151.18881881284912</v>
+        <v>151.21841351040922</v>
       </c>
       <c r="D22" s="23">
-        <v>150.78029547567192</v>
+        <v>150.80252329953043</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2951,13 +2949,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="23">
-        <v>149.38594914967302</v>
+        <v>149.3859491496728</v>
       </c>
       <c r="C23" s="23">
-        <v>151.50665447468469</v>
+        <v>151.57273621545232</v>
       </c>
       <c r="D23" s="23">
-        <v>150.88197691345263</v>
+        <v>150.90221397544374</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2965,13 +2963,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="23">
-        <v>151.92604263437079</v>
+        <v>151.92604263437062</v>
       </c>
       <c r="C24" s="23">
-        <v>152.5738862671258</v>
+        <v>152.63057959583725</v>
       </c>
       <c r="D24" s="23">
-        <v>150.7914474050211</v>
+        <v>150.80809980815096</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,13 +2977,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="23">
-        <v>146.78338564322195</v>
+        <v>146.78338564322209</v>
       </c>
       <c r="C25" s="23">
-        <v>152.41747111921032</v>
+        <v>152.43328674010354</v>
       </c>
       <c r="D25" s="23">
-        <v>150.49895078699876</v>
+        <v>150.51114407137626</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2993,13 +2991,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="23">
-        <v>142.74091494479157</v>
+        <v>142.74091494479219</v>
       </c>
       <c r="C26" s="23">
-        <v>152.049567975928</v>
+        <v>151.94914317096365</v>
       </c>
       <c r="D26" s="23">
-        <v>150.01087181930532</v>
+        <v>150.01859649214254</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3007,13 +3005,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="23">
-        <v>138.81804133746769</v>
+        <v>138.81804133746789</v>
       </c>
       <c r="C27" s="23">
-        <v>151.91912999127334</v>
+        <v>151.91809766487637</v>
       </c>
       <c r="D27" s="23">
-        <v>149.34841696716697</v>
+        <v>149.35275963375383</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3021,13 +3019,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="23">
-        <v>155.85731621133985</v>
+        <v>155.85731621133883</v>
       </c>
       <c r="C28" s="23">
-        <v>151.27607772530757</v>
+        <v>151.2490990995779</v>
       </c>
       <c r="D28" s="23">
-        <v>148.54586408630811</v>
+        <v>148.54804072956912</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,13 +3033,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="23">
-        <v>151.52453339184243</v>
+        <v>151.52453339183924</v>
       </c>
       <c r="C29" s="23">
-        <v>146.85651606456457</v>
+        <v>146.80262772257743</v>
       </c>
       <c r="D29" s="23">
-        <v>147.65178286935722</v>
+        <v>147.65270900175599</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3049,13 +3047,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="23">
-        <v>159.56668791297358</v>
+        <v>159.56668791297218</v>
       </c>
       <c r="C30" s="23">
-        <v>144.4633664791784</v>
+        <v>144.40510267021185</v>
       </c>
       <c r="D30" s="23">
-        <v>146.72295113348949</v>
+        <v>146.72241926762959</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3063,13 +3061,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="23">
-        <v>151.12577829049906</v>
+        <v>151.12577829050338</v>
       </c>
       <c r="C31" s="23">
-        <v>143.15799320154153</v>
+        <v>143.11355937256997</v>
       </c>
       <c r="D31" s="23">
-        <v>145.81554418920726</v>
+        <v>145.81314411017971</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3077,13 +3075,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="23">
-        <v>145.96357240386445</v>
+        <v>145.96357240387832</v>
       </c>
       <c r="C32" s="23">
-        <v>143.2354740585497</v>
+        <v>143.20948333272955</v>
       </c>
       <c r="D32" s="23">
-        <v>144.97796299434677</v>
+        <v>144.97415847308534</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,13 +3089,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="23">
-        <v>146.7659802568086</v>
+        <v>146.7659802568144</v>
       </c>
       <c r="C33" s="23">
-        <v>146.61283889394917</v>
+        <v>146.62142368296298</v>
       </c>
       <c r="D33" s="23">
-        <v>144.2541693412889</v>
+        <v>144.24921738623993</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3105,13 +3103,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="23">
-        <v>137.74650152211899</v>
+        <v>137.74650152209912</v>
       </c>
       <c r="C34" s="23">
-        <v>143.21102213875625</v>
+        <v>143.23782748947133</v>
       </c>
       <c r="D34" s="23">
-        <v>143.67328891291842</v>
+        <v>143.66703390111249</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3119,13 +3117,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="23">
-        <v>142.84305870083375</v>
+        <v>142.84305870077048</v>
       </c>
       <c r="C35" s="23">
-        <v>143.59717491783144</v>
+        <v>143.70064390720412</v>
       </c>
       <c r="D35" s="23">
-        <v>143.24946950424359</v>
+        <v>143.24141928402844</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3133,13 +3131,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="23">
-        <v>140.59231573260089</v>
+        <v>140.59231573257421</v>
       </c>
       <c r="C36" s="23">
-        <v>141.57330496985571</v>
+        <v>141.68396100822244</v>
       </c>
       <c r="D36" s="23">
-        <v>142.98149848827566</v>
+        <v>142.97137688007027</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3147,13 +3145,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="23">
-        <v>136.25192484552474</v>
+        <v>136.25192484561447</v>
       </c>
       <c r="C37" s="23">
-        <v>141.84415935161917</v>
+        <v>141.90565663928129</v>
       </c>
       <c r="D37" s="23">
-        <v>142.85441958342255</v>
+        <v>142.84265522848568</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,13 +3159,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="23">
-        <v>134.52056075482315</v>
+        <v>134.5205607551091</v>
       </c>
       <c r="C38" s="23">
-        <v>143.05186389005311</v>
+        <v>142.93449850446279</v>
       </c>
       <c r="D38" s="23">
-        <v>142.84054834885427</v>
+        <v>142.82914751011685</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3175,13 +3173,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="23">
-        <v>132.27529838944116</v>
+        <v>132.27529838956164</v>
       </c>
       <c r="C39" s="23">
-        <v>143.47820870139054</v>
+        <v>143.48072979795421</v>
       </c>
       <c r="D39" s="23">
-        <v>142.90357305727738</v>
+        <v>142.89455816191784</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,13 +3187,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="23">
-        <v>144.87373844609147</v>
+        <v>144.87373844568478</v>
       </c>
       <c r="C40" s="23">
-        <v>141.20484515839215</v>
+        <v>141.20462489279612</v>
       </c>
       <c r="D40" s="23">
-        <v>143.0024644035359</v>
+        <v>142.99700334581658</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3203,13 +3201,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="23">
-        <v>149.89913655926117</v>
+        <v>149.89913655796551</v>
       </c>
       <c r="C41" s="23">
-        <v>142.56731949207088</v>
+        <v>142.50362614627667</v>
       </c>
       <c r="D41" s="23">
-        <v>143.0953673108624</v>
+        <v>143.09331945695143</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3217,13 +3215,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="23">
-        <v>164.14987183044366</v>
+        <v>164.14987182989748</v>
       </c>
       <c r="C42" s="23">
-        <v>144.53655329241874</v>
+        <v>144.45343487832156</v>
       </c>
       <c r="D42" s="23">
-        <v>143.14481092625027</v>
+        <v>143.14446706312381</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3231,13 +3229,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="23">
-        <v>150.84993450464239</v>
+        <v>150.849934506484</v>
       </c>
       <c r="C43" s="23">
-        <v>143.7763589018094</v>
+        <v>143.69622577268279</v>
       </c>
       <c r="D43" s="23">
-        <v>143.11657542228173</v>
+        <v>143.11474858147608</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3245,13 +3243,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="23">
-        <v>146.76823785681836</v>
+        <v>146.76823786268602</v>
       </c>
       <c r="C44" s="23">
-        <v>145.48526409814801</v>
+        <v>145.4130754195362</v>
       </c>
       <c r="D44" s="23">
-        <v>142.98520983060877</v>
+        <v>142.97784602764804</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3259,13 +3257,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="23">
-        <v>141.2794360493493</v>
+        <v>141.2794360518227</v>
       </c>
       <c r="C45" s="23">
-        <v>144.94695205327204</v>
+        <v>144.93106137022613</v>
       </c>
       <c r="D45" s="23">
-        <v>142.73237556015101</v>
+        <v>142.71436829012939</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3273,13 +3271,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="23">
-        <v>134.88987734969228</v>
+        <v>134.88987734135102</v>
       </c>
       <c r="C46" s="23">
-        <v>141.13849220486793</v>
+        <v>141.1649434678811</v>
       </c>
       <c r="D46" s="23">
-        <v>142.34960438785279</v>
+        <v>142.31517109905712</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,13 +3285,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="23">
-        <v>141.51078863832441</v>
+        <v>141.51078861174801</v>
       </c>
       <c r="C47" s="23">
-        <v>143.46543403904352</v>
+        <v>143.63032722554053</v>
       </c>
       <c r="D47" s="23">
-        <v>141.839344820169</v>
+        <v>141.78282537042838</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,13 +3299,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="23">
-        <v>137.65812409402241</v>
+        <v>137.65812408281948</v>
       </c>
       <c r="C48" s="23">
-        <v>140.609789502399</v>
+        <v>140.76417297841331</v>
       </c>
       <c r="D48" s="23">
-        <v>141.21223023562385</v>
+        <v>141.1314109980446</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,13 +3313,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="23">
-        <v>135.67189223323882</v>
+        <v>135.67189227101787</v>
       </c>
       <c r="C49" s="23">
-        <v>140.08581558554602</v>
+        <v>140.17017645777781</v>
       </c>
       <c r="D49" s="23">
-        <v>140.49532939882963</v>
+        <v>140.38932254841316</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3329,13 +3327,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="23">
-        <v>132.28223124569112</v>
+        <v>132.28223136606061</v>
       </c>
       <c r="C50" s="23">
-        <v>140.92680743730625</v>
+        <v>140.80426345718908</v>
       </c>
       <c r="D50" s="23">
-        <v>139.7260606903881</v>
+        <v>139.59485442247609</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3343,13 +3341,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="23">
-        <v>129.74514663170137</v>
+        <v>129.74514668244132</v>
       </c>
       <c r="C51" s="23">
-        <v>140.47384259570757</v>
+        <v>140.47694578224795</v>
       </c>
       <c r="D51" s="23">
-        <v>138.94856019337411</v>
+        <v>138.79157204328209</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3357,13 +3355,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="23">
-        <v>129.0977252138824</v>
+        <v>129.09772504277274</v>
       </c>
       <c r="C52" s="23">
-        <v>125.41401660184215</v>
+        <v>125.42978565211637</v>
       </c>
       <c r="D52" s="23">
-        <v>138.20808648877932</v>
+        <v>138.02390260644125</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3371,13 +3369,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="23">
-        <v>111.90395316317499</v>
+        <v>111.90395261799564</v>
       </c>
       <c r="C53" s="23">
-        <v>105.21308015881309</v>
+        <v>105.11695230194732</v>
       </c>
       <c r="D53" s="23">
-        <v>137.54939442250827</v>
+        <v>137.33748440864028</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3385,13 +3383,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="23">
-        <v>131.29461300494506</v>
+        <v>131.2946127751328</v>
       </c>
       <c r="C54" s="23">
-        <v>116.44348319578269</v>
+        <v>116.33414823619009</v>
       </c>
       <c r="D54" s="23">
-        <v>137.00727052395177</v>
+        <v>136.76914124534704</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3399,13 +3397,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="23">
-        <v>133.30386653957163</v>
+        <v>133.30386731456301</v>
       </c>
       <c r="C55" s="23">
-        <v>124.48594393290077</v>
+        <v>124.36907969892977</v>
       </c>
       <c r="D55" s="23">
-        <v>136.60517654287645</v>
+        <v>136.34561063486581</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3413,13 +3411,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="23">
-        <v>128.19080278245926</v>
+        <v>128.19080525169102</v>
       </c>
       <c r="C56" s="23">
-        <v>126.71465647194331</v>
+        <v>126.62366167030197</v>
       </c>
       <c r="D56" s="23">
-        <v>136.35712034787747</v>
+        <v>136.08232784394846</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3427,13 +3425,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="23">
-        <v>125.17406632349137</v>
+        <v>125.17406736435935</v>
       </c>
       <c r="C57" s="23">
-        <v>129.30360982294195</v>
+        <v>129.2828542177048</v>
       </c>
       <c r="D57" s="23">
-        <v>136.26546813575504</v>
+        <v>135.98498980704875</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3441,13 +3439,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="23">
-        <v>126.59614565623438</v>
+        <v>126.59614214613437</v>
       </c>
       <c r="C58" s="23">
-        <v>131.23094969391684</v>
+        <v>131.27899722398661</v>
       </c>
       <c r="D58" s="23">
-        <v>136.3213351966003</v>
+        <v>136.04766186975809</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3455,13 +3453,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="23">
-        <v>131.72739168680206</v>
+        <v>131.72738050312998</v>
       </c>
       <c r="C59" s="23">
-        <v>134.18128510718887</v>
+        <v>134.39643445493272</v>
       </c>
       <c r="D59" s="23">
-        <v>136.50970722051457</v>
+        <v>136.25720500534328</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3469,13 +3467,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="23">
-        <v>132.96973762254197</v>
+        <v>132.96973290823087</v>
       </c>
       <c r="C60" s="23">
-        <v>135.24331515986353</v>
+        <v>135.4285141899866</v>
       </c>
       <c r="D60" s="23">
-        <v>136.81530774134865</v>
+        <v>136.59836961758293</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3483,13 +3481,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="23">
-        <v>132.42198051947332</v>
+        <v>132.42199641745623</v>
       </c>
       <c r="C61" s="23">
-        <v>135.07667040389356</v>
+        <v>135.16602368979395</v>
       </c>
       <c r="D61" s="23">
-        <v>137.21900202788663</v>
+        <v>137.05342799158709</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3497,13 +3495,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="23">
-        <v>129.49276757333357</v>
+        <v>129.49281822654359</v>
       </c>
       <c r="C62" s="23">
-        <v>139.88540873148725</v>
+        <v>139.78525972338076</v>
       </c>
       <c r="D62" s="23">
-        <v>137.70744768509203</v>
+        <v>137.6052765691083</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3511,13 +3509,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="23">
-        <v>126.69382319800599</v>
+        <v>126.69384455011522</v>
       </c>
       <c r="C63" s="23">
-        <v>138.00827627302886</v>
+        <v>138.03044630307585</v>
       </c>
       <c r="D63" s="23">
-        <v>138.27414369065789</v>
+        <v>138.2359438821434</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3525,13 +3523,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="23">
-        <v>146.28771620784292</v>
+        <v>146.28764420252344</v>
       </c>
       <c r="C64" s="23">
-        <v>139.62033675897746</v>
+        <v>139.6381062498327</v>
       </c>
       <c r="D64" s="23">
-        <v>138.91460931275324</v>
+        <v>138.93453226870867</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,13 +3537,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="23">
-        <v>144.90576544617173</v>
+        <v>144.90553602709559</v>
       </c>
       <c r="C65" s="23">
-        <v>137.97923540402439</v>
+        <v>137.82903880692834</v>
       </c>
       <c r="D65" s="23">
-        <v>139.62469470435929</v>
+        <v>139.69225725618682</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3553,13 +3551,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="23">
-        <v>150.14868925533764</v>
+        <v>150.14859254712937</v>
       </c>
       <c r="C66" s="23">
-        <v>136.62395416854335</v>
+        <v>136.47324837459763</v>
       </c>
       <c r="D66" s="23">
-        <v>140.39946643054387</v>
+        <v>140.49807670127464</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3567,13 +3565,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="23">
-        <v>148.94396513599037</v>
+        <v>148.94429126327449</v>
       </c>
       <c r="C67" s="23">
-        <v>140.56337413383557</v>
+        <v>140.40316908710284</v>
       </c>
       <c r="D67" s="23">
-        <v>141.22465096830112</v>
+        <v>141.33431170593434</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3581,13 +3579,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="23">
-        <v>143.1827570387415</v>
+        <v>143.18379612614257</v>
       </c>
       <c r="C68" s="23">
-        <v>142.23818738567508</v>
+        <v>142.18349168476311</v>
       </c>
       <c r="D68" s="23">
-        <v>142.08271224568463</v>
+        <v>142.17859012439729</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3595,13 +3593,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="23">
-        <v>141.20571583640663</v>
+        <v>141.20615384828605</v>
       </c>
       <c r="C69" s="23">
-        <v>144.22434592772771</v>
+        <v>144.28645099440209</v>
       </c>
       <c r="D69" s="23">
-        <v>142.94703255499016</v>
+        <v>143.00129386917902</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3609,13 +3607,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="23">
-        <v>140.94554305470595</v>
+        <v>140.94406595542517</v>
       </c>
       <c r="C70" s="23">
-        <v>145.47636915433617</v>
+        <v>145.58250626801313</v>
       </c>
       <c r="D70" s="23">
-        <v>143.7872752325373</v>
+        <v>143.77396439520516</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,13 +3621,13 @@
         <v>44470</v>
       </c>
       <c r="B71" s="23">
-        <v>140.49004342379754</v>
+        <v>140.3671594559155</v>
       </c>
       <c r="C71" s="23">
-        <v>144.53854660195259</v>
+        <v>144.59214506676773</v>
       </c>
       <c r="D71" s="23">
-        <v>144.57288714025364</v>
+        <v>144.46901534415005</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3637,13 +3635,13 @@
         <v>44501</v>
       </c>
       <c r="B72" s="23">
-        <v>145.32981978314771</v>
+        <v>145.25498233631956</v>
       </c>
       <c r="C72" s="23">
-        <v>146.35938683018313</v>
+        <v>146.42352656552703</v>
       </c>
       <c r="D72" s="23">
-        <v>145.2817323311366</v>
+        <v>145.06642473082005</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3651,13 +3649,13 @@
         <v>44531</v>
       </c>
       <c r="B73" s="23">
-        <v>145.62615550894006</v>
+        <v>145.82387692364978</v>
       </c>
       <c r="C73" s="23">
-        <v>147.7353390335428</v>
+        <v>148.02537127377349</v>
       </c>
       <c r="D73" s="23">
-        <v>145.90323586651684</v>
+        <v>145.55523402907167</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,27 +3663,41 @@
         <v>44562</v>
       </c>
       <c r="B74" s="23">
-        <v>136.06700195253066</v>
+        <v>136.19945226919234</v>
       </c>
       <c r="C74" s="23">
-        <v>146.65261912716201</v>
+        <v>146.92534922715495</v>
       </c>
       <c r="D74" s="23">
-        <v>146.43963965561588</v>
+        <v>145.93965204793767</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>44593</v>
       </c>
-      <c r="B75" s="24">
-        <v>138.17655785876821</v>
-      </c>
-      <c r="C75" s="24">
-        <v>149.21948044703143</v>
-      </c>
-      <c r="D75" s="24">
-        <v>146.90366897683356</v>
+      <c r="B75" s="23">
+        <v>137.40830020938367</v>
+      </c>
+      <c r="C75" s="23">
+        <v>148.67367673325154</v>
+      </c>
+      <c r="D75" s="23">
+        <v>146.23625610326812</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>44621</v>
+      </c>
+      <c r="B76" s="24">
+        <v>153.35082819313141</v>
+      </c>
+      <c r="C76" s="24">
+        <v>147.57180012062108</v>
+      </c>
+      <c r="D76" s="24">
+        <v>146.47195069165483</v>
       </c>
     </row>
   </sheetData>
@@ -3698,7 +3710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6578,8 +6590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6606,14 +6618,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="41">
-        <v>3091</v>
+        <v>4461</v>
       </c>
       <c r="C2" s="41">
-        <v>4085</v>
+        <v>5716</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-994</v>
+        <v>-1255</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6621,14 +6633,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="41">
-        <v>1270</v>
+        <v>1708</v>
       </c>
       <c r="C3" s="41">
-        <v>203</v>
+        <v>271</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1067</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6636,14 +6648,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="41">
-        <v>1269</v>
+        <v>1651</v>
       </c>
       <c r="C4" s="41">
-        <v>502</v>
+        <v>756</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>767</v>
+        <v>895</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6651,14 +6663,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="41">
-        <v>241</v>
+        <v>349</v>
       </c>
       <c r="C5" s="41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>234</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6666,14 +6678,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="41">
-        <v>1815</v>
+        <v>2606</v>
       </c>
       <c r="C6" s="41">
-        <v>2018</v>
+        <v>3146</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-203</v>
+        <v>-540</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6681,14 +6693,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="41">
-        <v>2456</v>
+        <v>3614</v>
       </c>
       <c r="C7" s="41">
-        <v>2759</v>
+        <v>3729</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-303</v>
+        <v>-115</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6696,14 +6708,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="41">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="C8" s="41">
-        <v>194</v>
+        <v>250</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-59</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6711,14 +6723,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="41">
-        <v>297</v>
+        <v>425</v>
       </c>
       <c r="C9" s="41">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6726,14 +6738,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="41">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C10" s="41">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6741,14 +6753,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="41">
-        <v>1861</v>
+        <v>2731</v>
       </c>
       <c r="C11" s="41">
-        <v>1041</v>
+        <v>1438</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>820</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6756,14 +6768,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="41">
-        <v>1256</v>
+        <v>1625</v>
       </c>
       <c r="C12" s="41">
-        <v>4402</v>
+        <v>5655</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-3146</v>
+        <v>-4030</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6771,14 +6783,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="41">
-        <v>354</v>
+        <v>448</v>
       </c>
       <c r="C13" s="41">
-        <v>189</v>
+        <v>241</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6786,14 +6798,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="41">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="C14" s="41">
-        <v>255</v>
+        <v>365</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-151</v>
+        <v>-157</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6801,14 +6813,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="41">
-        <v>909</v>
+        <v>1388</v>
       </c>
       <c r="C15" s="41">
-        <v>411</v>
+        <v>591</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>498</v>
+        <v>797</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6816,14 +6828,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="41">
-        <v>896</v>
+        <v>1497</v>
       </c>
       <c r="C16" s="41">
-        <v>791</v>
+        <v>1066</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6831,14 +6843,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="41">
-        <v>1013</v>
+        <v>1627</v>
       </c>
       <c r="C17" s="41">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>956</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6846,14 +6858,14 @@
         <v>95</v>
       </c>
       <c r="B18" s="41">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="C18" s="41">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6861,14 +6873,14 @@
         <v>96</v>
       </c>
       <c r="B19" s="41">
-        <v>228</v>
+        <v>303</v>
       </c>
       <c r="C19" s="41">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -6876,14 +6888,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="42">
-        <v>1838</v>
+        <v>2445</v>
       </c>
       <c r="C20" s="42">
-        <v>616</v>
+        <v>911</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1222</v>
+        <v>1534</v>
       </c>
     </row>
   </sheetData>
@@ -6897,7 +6909,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6918,7 +6930,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="47">
-        <v>19352</v>
+        <v>27681</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6926,7 +6938,7 @@
         <v>185</v>
       </c>
       <c r="B3" s="47">
-        <v>5819</v>
+        <v>8124</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6934,7 +6946,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="41">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6942,7 +6954,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="41">
-        <v>348</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6950,7 +6962,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="41">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6958,7 +6970,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="41">
-        <v>177</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6966,7 +6978,7 @@
         <v>142</v>
       </c>
       <c r="B8" s="41">
-        <v>113</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6974,7 +6986,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="41">
-        <v>4608</v>
+        <v>6453</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -6982,7 +6994,7 @@
         <v>144</v>
       </c>
       <c r="B10" s="41">
-        <v>280</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6990,7 +7002,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="41">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6998,7 +7010,7 @@
         <v>146</v>
       </c>
       <c r="B12" s="41">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7006,7 +7018,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="41">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7014,7 +7026,7 @@
         <v>148</v>
       </c>
       <c r="B14" s="41">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7022,7 +7034,7 @@
         <v>149</v>
       </c>
       <c r="B15" s="41">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7030,7 +7042,7 @@
         <v>186</v>
       </c>
       <c r="B16" s="47">
-        <v>6702</v>
+        <v>9979</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7038,7 +7050,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="41">
-        <v>942</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7046,7 +7058,7 @@
         <v>151</v>
       </c>
       <c r="B18" s="41">
-        <v>56</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7054,7 +7066,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="41">
-        <v>336</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7062,7 +7074,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="41">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7070,7 +7082,7 @@
         <v>154</v>
       </c>
       <c r="B21" s="41">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7078,7 +7090,7 @@
         <v>155</v>
       </c>
       <c r="B22" s="41">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7086,7 +7098,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="41">
-        <v>203</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7094,7 +7106,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="41">
-        <v>1684</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7102,7 +7114,7 @@
         <v>158</v>
       </c>
       <c r="B25" s="41">
-        <v>64</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7110,7 +7122,7 @@
         <v>159</v>
       </c>
       <c r="B26" s="41">
-        <v>160</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7118,7 +7130,7 @@
         <v>160</v>
       </c>
       <c r="B27" s="41">
-        <v>205</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7126,7 +7138,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="41">
-        <v>2659</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7134,7 +7146,7 @@
         <v>162</v>
       </c>
       <c r="B29" s="41">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7142,7 +7154,7 @@
         <v>163</v>
       </c>
       <c r="B30" s="41">
-        <v>112</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7150,7 +7162,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="41">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7158,7 +7170,7 @@
         <v>165</v>
       </c>
       <c r="B32" s="41">
-        <v>130</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7166,7 +7178,7 @@
         <v>187</v>
       </c>
       <c r="B33" s="47">
-        <v>4952</v>
+        <v>6992</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7174,7 +7186,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="41">
-        <v>1551</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7182,7 +7194,7 @@
         <v>167</v>
       </c>
       <c r="B35" s="41">
-        <v>293</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7190,7 +7202,7 @@
         <v>168</v>
       </c>
       <c r="B36" s="41">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7198,7 +7210,7 @@
         <v>169</v>
       </c>
       <c r="B37" s="41">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7206,7 +7218,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="41">
-        <v>121</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7214,7 +7226,7 @@
         <v>171</v>
       </c>
       <c r="B39" s="41">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7222,7 +7234,7 @@
         <v>172</v>
       </c>
       <c r="B40" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -7230,7 +7242,7 @@
         <v>173</v>
       </c>
       <c r="B41" s="41">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -7238,7 +7250,7 @@
         <v>174</v>
       </c>
       <c r="B42" s="41">
-        <v>678</v>
+        <v>953</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -7246,7 +7258,7 @@
         <v>175</v>
       </c>
       <c r="B43" s="41">
-        <v>453</v>
+        <v>688</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -7254,7 +7266,7 @@
         <v>176</v>
       </c>
       <c r="B44" s="41">
-        <v>328</v>
+        <v>448</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -7262,7 +7274,7 @@
         <v>177</v>
       </c>
       <c r="B45" s="41">
-        <v>1304</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -7270,7 +7282,7 @@
         <v>178</v>
       </c>
       <c r="B46" s="41">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7278,7 +7290,7 @@
         <v>179</v>
       </c>
       <c r="B47" s="41">
-        <v>69</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -7286,7 +7298,7 @@
         <v>188</v>
       </c>
       <c r="B48" s="47">
-        <v>1878</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7294,7 +7306,7 @@
         <v>180</v>
       </c>
       <c r="B49" s="41">
-        <v>968</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7302,7 +7314,7 @@
         <v>181</v>
       </c>
       <c r="B50" s="41">
-        <v>453</v>
+        <v>703</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7310,7 +7322,7 @@
         <v>182</v>
       </c>
       <c r="B51" s="41">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7318,7 +7330,7 @@
         <v>183</v>
       </c>
       <c r="B52" s="48">
-        <v>383</v>
+        <v>480</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -7326,7 +7338,7 @@
         <v>184</v>
       </c>
       <c r="B53" s="49">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -7340,7 +7352,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7361,7 +7373,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="47">
-        <v>17958</v>
+        <v>24852</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7369,7 +7381,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="47">
-        <v>3089</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7377,7 +7389,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="41">
-        <v>2365</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7385,7 +7397,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="41">
-        <v>297</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7393,7 +7405,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="41">
-        <v>314</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7401,7 +7413,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="41">
-        <v>113</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7409,7 +7421,7 @@
         <v>211</v>
       </c>
       <c r="B8" s="47">
-        <v>6698</v>
+        <v>9440</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7417,7 +7429,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="41">
-        <v>445</v>
+        <v>741</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7425,7 +7437,7 @@
         <v>195</v>
       </c>
       <c r="B10" s="41">
-        <v>286</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7433,7 +7445,7 @@
         <v>196</v>
       </c>
       <c r="B11" s="41">
-        <v>2488</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7441,7 +7453,7 @@
         <v>197</v>
       </c>
       <c r="B12" s="41">
-        <v>951</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7449,7 +7461,7 @@
         <v>198</v>
       </c>
       <c r="B13" s="41">
-        <v>292</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7457,7 +7469,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="41">
-        <v>377</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7465,7 +7477,7 @@
         <v>200</v>
       </c>
       <c r="B15" s="41">
-        <v>186</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7473,7 +7485,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="41">
-        <v>1143</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7481,7 +7493,7 @@
         <v>202</v>
       </c>
       <c r="B17" s="41">
-        <v>531</v>
+        <v>698</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7489,7 +7501,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="47">
-        <v>2163</v>
+        <v>3040</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7497,7 +7509,7 @@
         <v>195</v>
       </c>
       <c r="B19" s="41">
-        <v>2106</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7505,7 +7517,7 @@
         <v>203</v>
       </c>
       <c r="B20" s="41">
-        <v>57</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7513,7 +7525,7 @@
         <v>213</v>
       </c>
       <c r="B21" s="47">
-        <v>3270</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7521,7 +7533,7 @@
         <v>190</v>
       </c>
       <c r="B22" s="41">
-        <v>2150</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7529,7 +7541,7 @@
         <v>191</v>
       </c>
       <c r="B23" s="41">
-        <v>874</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7537,7 +7549,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="41">
-        <v>246</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7545,7 +7557,7 @@
         <v>214</v>
       </c>
       <c r="B25" s="47">
-        <v>2173</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7553,7 +7565,7 @@
         <v>205</v>
       </c>
       <c r="B26" s="41">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7561,7 +7573,7 @@
         <v>194</v>
       </c>
       <c r="B27" s="41">
-        <v>161</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7569,7 +7581,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="41">
-        <v>197</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7577,7 +7589,7 @@
         <v>196</v>
       </c>
       <c r="B29" s="41">
-        <v>610</v>
+        <v>832</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7585,7 +7597,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="41">
-        <v>145</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7593,7 +7605,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="41">
-        <v>113</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7601,7 +7613,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="41">
-        <v>155</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7609,7 +7621,7 @@
         <v>190</v>
       </c>
       <c r="B33" s="41">
-        <v>163</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7617,7 +7629,7 @@
         <v>191</v>
       </c>
       <c r="B34" s="41">
-        <v>163</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7625,7 +7637,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="41">
-        <v>76</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7633,7 +7645,7 @@
         <v>208</v>
       </c>
       <c r="B36" s="41">
-        <v>148</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7641,7 +7653,7 @@
         <v>209</v>
       </c>
       <c r="B37" s="41">
-        <v>153</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7649,7 +7661,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="47">
-        <v>415</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7657,7 +7669,7 @@
         <v>191</v>
       </c>
       <c r="B39" s="53">
-        <v>415</v>
+        <v>598</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7665,7 +7677,7 @@
         <v>216</v>
       </c>
       <c r="B40" s="54">
-        <v>150</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo ica, res fiscal y producto"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76704B08-96E7-482A-898F-2CEB0229414D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33986770-7D61-4CEA-9005-0CA5FAC0754B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="218">
   <si>
     <t>Período</t>
   </si>
@@ -1282,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
@@ -2452,10 +2452,10 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>580109.3654135036</v>
+        <v>571371.42621766892</v>
       </c>
       <c r="C2">
-        <v>8.2176039378516919</v>
+        <v>6.021578205340461</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2463,10 +2463,10 @@
         <v>102</v>
       </c>
       <c r="B3">
-        <v>36648.13652029309</v>
+        <v>39792.671747015345</v>
       </c>
       <c r="C3">
-        <v>4.3860998002780427</v>
+        <v>-0.12132037450698352</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2474,10 +2474,10 @@
         <v>103</v>
       </c>
       <c r="B4">
-        <v>1249.7113603560397</v>
+        <v>1621.5132086953849</v>
       </c>
       <c r="C4">
-        <v>-19.150143374614757</v>
+        <v>-3.5279456750018534</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2485,10 +2485,10 @@
         <v>104</v>
       </c>
       <c r="B5">
-        <v>22724.129989370613</v>
+        <v>22656.313905916188</v>
       </c>
       <c r="C5">
-        <v>18.247420162936258</v>
+        <v>13.400317766955405</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2496,10 +2496,10 @@
         <v>105</v>
       </c>
       <c r="B6">
-        <v>122710.03414797327</v>
+        <v>108992.72916716749</v>
       </c>
       <c r="C6">
-        <v>8.543915384800993</v>
+        <v>4.8600348747123823</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2507,10 +2507,10 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <v>12285.490130430609</v>
+        <v>12942.275374307999</v>
       </c>
       <c r="C7">
-        <v>0.49655622972446523</v>
+        <v>5.1476925583904265</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2518,10 +2518,10 @@
         <v>107</v>
       </c>
       <c r="B8">
-        <v>20987.63967740133</v>
+        <v>22467.323062496853</v>
       </c>
       <c r="C8">
-        <v>4.5268786278615414</v>
+        <v>2.9756526723262899</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,10 +2529,10 @@
         <v>108</v>
       </c>
       <c r="B9">
-        <v>93443.748235928695</v>
+        <v>90190.059665927343</v>
       </c>
       <c r="C9">
-        <v>7.2357992351878675</v>
+        <v>5.660398988406512</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2540,10 +2540,10 @@
         <v>109</v>
       </c>
       <c r="B10">
-        <v>8992.2744681564727</v>
+        <v>9300.2054422241108</v>
       </c>
       <c r="C10">
-        <v>60.938820792863964</v>
+        <v>33.565103502550819</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2551,10 +2551,10 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>51632.157894787102</v>
+        <v>53261.090320404044</v>
       </c>
       <c r="C11">
-        <v>14.905791213603869</v>
+        <v>12.22725949424488</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2562,10 +2562,10 @@
         <v>111</v>
       </c>
       <c r="B12">
-        <v>26151.467050546846</v>
+        <v>25570.829166259125</v>
       </c>
       <c r="C12">
-        <v>0.37420012180280349</v>
+        <v>1.2523958518309453</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2573,10 +2573,10 @@
         <v>112</v>
       </c>
       <c r="B13">
-        <v>79143.368376477825</v>
+        <v>77865.228139844723</v>
       </c>
       <c r="C13">
-        <v>6.5567187004549332</v>
+        <v>5.0092778689776685</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,10 +2584,10 @@
         <v>113</v>
       </c>
       <c r="B14">
-        <v>34930.018675685875</v>
+        <v>34914.496460771283</v>
       </c>
       <c r="C14">
-        <v>11.909663098887879</v>
+        <v>9.4595469169590061</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2595,10 +2595,10 @@
         <v>114</v>
       </c>
       <c r="B15">
-        <v>28516.783116102812</v>
+        <v>27768.387873531781</v>
       </c>
       <c r="C15">
-        <v>6.1375814244809535</v>
+        <v>4.8792692299016949</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2606,10 +2606,10 @@
         <v>115</v>
       </c>
       <c r="B16">
-        <v>22663.778591606671</v>
+        <v>23390.182227267425</v>
       </c>
       <c r="C16">
-        <v>2.422746472798476</v>
+        <v>2.8213605132321629</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2617,10 +2617,10 @@
         <v>116</v>
       </c>
       <c r="B17">
-        <v>14327.889062242892</v>
+        <v>16511.100936225932</v>
       </c>
       <c r="C17">
-        <v>10.245849380753791</v>
+        <v>7.8415677899741576</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,10 +2628,10 @@
         <v>117</v>
       </c>
       <c r="B18">
-        <v>3702.7381161434578</v>
+        <v>4127.0195196139048</v>
       </c>
       <c r="C18">
-        <v>1.7208283342252662</v>
+        <v>10.54034588475834</v>
       </c>
     </row>
   </sheetData>
@@ -4764,11 +4764,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4797,7 +4795,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="12">
-        <v>475575.99488002178</v>
+        <v>475454.37399644504</v>
       </c>
       <c r="D2" s="12">
         <v>460369.44223294902</v>
@@ -4811,7 +4809,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="12">
-        <v>470114.51380285382</v>
+        <v>470205.76579705958</v>
       </c>
       <c r="D3" s="12">
         <v>514395.68177236198</v>
@@ -4825,7 +4823,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="12">
-        <v>493690.48358295608</v>
+        <v>493835.75466103636</v>
       </c>
       <c r="D4" s="12">
         <v>481151.97994350799</v>
@@ -4839,7 +4837,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="12">
-        <v>501079.7883181842</v>
+        <v>500964.88610719389</v>
       </c>
       <c r="D5" s="12">
         <v>484543.67687656201</v>
@@ -4853,7 +4851,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="12">
-        <v>515485.07610400004</v>
+        <v>515453.44834923226</v>
       </c>
       <c r="D6" s="12">
         <v>493602.53057785501</v>
@@ -4867,7 +4865,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="12">
-        <v>526246.42406031769</v>
+        <v>526221.6289373528</v>
       </c>
       <c r="D7" s="12">
         <v>581668.24987960199</v>
@@ -4881,7 +4879,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="12">
-        <v>529925.52491045627</v>
+        <v>530094.33357569715</v>
       </c>
       <c r="D8" s="12">
         <v>514697.78950542799</v>
@@ -4895,7 +4893,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="12">
-        <v>540566.74493888335</v>
+        <v>540454.35915137373</v>
       </c>
       <c r="D9" s="12">
         <v>522255.20005077199</v>
@@ -4909,7 +4907,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="12">
-        <v>554542.19231067074</v>
+        <v>554411.83501684235</v>
       </c>
       <c r="D10" s="12">
         <v>532348.21201691695</v>
@@ -4923,7 +4921,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="12">
-        <v>561184.20725406578</v>
+        <v>561221.28776810062</v>
       </c>
       <c r="D11" s="12">
         <v>614076.39260854397</v>
@@ -4937,7 +4935,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="12">
-        <v>576884.8992080309</v>
+        <v>577070.94766772434</v>
       </c>
       <c r="D12" s="12">
         <v>562978.96562687703</v>
@@ -4951,7 +4949,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="12">
-        <v>589586.3181101589</v>
+        <v>589493.54643025738</v>
       </c>
       <c r="D13" s="12">
         <v>572794.04663058801</v>
@@ -4965,7 +4963,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="12">
-        <v>603183.508143752</v>
+        <v>602984.88460172631</v>
       </c>
       <c r="D14" s="12">
         <v>576846.88569942699</v>
@@ -4979,7 +4977,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="12">
-        <v>616227.38491072564</v>
+        <v>616261.92272166093</v>
       </c>
       <c r="D15" s="12">
         <v>674620.563006485</v>
@@ -4993,7 +4991,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="12">
-        <v>624501.02919283113</v>
+        <v>624759.56800488278</v>
       </c>
       <c r="D16" s="12">
         <v>610425.69401485403</v>
@@ -5007,7 +5005,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="12">
-        <v>643858.08833705308</v>
+        <v>643763.635256093</v>
       </c>
       <c r="D17" s="12">
         <v>625876.867863597</v>
@@ -5021,7 +5019,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="12">
-        <v>649498.56629899354</v>
+        <v>649419.96757048008</v>
       </c>
       <c r="D18" s="12">
         <v>616720.35706447798</v>
@@ -5035,7 +5033,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="12">
-        <v>653395.98861577117</v>
+        <v>653269.79330575257</v>
       </c>
       <c r="D19" s="12">
         <v>711405.50045523304</v>
@@ -5049,7 +5047,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="12">
-        <v>658445.79814075422</v>
+        <v>658718.83632044296</v>
       </c>
       <c r="D20" s="12">
         <v>647087.95974249404</v>
@@ -5063,7 +5061,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="12">
-        <v>627364.28590933036</v>
+        <v>627296.04176817276</v>
       </c>
       <c r="D21" s="12">
         <v>613490.82170264097</v>
@@ -5077,7 +5075,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="12">
-        <v>604251.23977672984</v>
+        <v>604047.70825217164</v>
       </c>
       <c r="D22" s="12">
         <v>578553.04424240498</v>
@@ -5091,7 +5089,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="12">
-        <v>591197.81675977737</v>
+        <v>591229.33407328476</v>
       </c>
       <c r="D23" s="12">
         <v>631197.75186006899</v>
@@ -5105,7 +5103,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="12">
-        <v>614251.77704788849</v>
+        <v>614472.04676489066</v>
       </c>
       <c r="D24" s="12">
         <v>610519.85461172694</v>
@@ -5119,7 +5117,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="12">
-        <v>625790.67206710181</v>
+        <v>625742.41656115034</v>
       </c>
       <c r="D25" s="12">
         <v>615220.85493729694</v>
@@ -5133,7 +5131,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="12">
-        <v>644656.33509278321</v>
+        <v>644430.22641792509</v>
       </c>
       <c r="D26" s="12">
         <v>611607.33658973</v>
@@ -5147,7 +5145,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="12">
-        <v>673796.62357125268</v>
+        <v>673775.07951578847</v>
       </c>
       <c r="D27" s="12">
         <v>733730.773968903</v>
@@ -5161,7 +5159,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="12">
-        <v>677245.75810220244</v>
+        <v>677399.28333924874</v>
       </c>
       <c r="D28" s="12">
         <v>668566.50948898599</v>
@@ -5175,7 +5173,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="12">
-        <v>686396.0010009557</v>
+        <v>686490.12849423185</v>
       </c>
       <c r="D29" s="12">
         <v>668190.097719574</v>
@@ -5189,7 +5187,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="12">
-        <v>702822.18023114896</v>
+        <v>702723.80414944305</v>
       </c>
       <c r="D30" s="12">
         <v>662325.58597269503</v>
@@ -5203,7 +5201,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="12">
-        <v>709453.73073667835</v>
+        <v>709454.40590443229</v>
       </c>
       <c r="D31" s="12">
         <v>766332.95457161299</v>
@@ -5217,7 +5215,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="12">
-        <v>715217.07363846607</v>
+        <v>715220.06375098636</v>
       </c>
       <c r="D32" s="12">
         <v>711417.39193010505</v>
@@ -5231,7 +5229,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="12">
-        <v>715633.40427611268</v>
+        <v>715728.11507754482</v>
       </c>
       <c r="D33" s="12">
         <v>703050.45640799298</v>
@@ -5245,7 +5243,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="12">
-        <v>707973.57480664295</v>
+        <v>707811.87377429125</v>
       </c>
       <c r="D34" s="12">
         <v>672685.993630504</v>
@@ -5259,7 +5257,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="12">
-        <v>683580.91010547569</v>
+        <v>683648.87101095053</v>
       </c>
       <c r="D35" s="12">
         <v>730838.27259277599</v>
@@ -5273,7 +5271,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="12">
-        <v>705262.62855204311</v>
+        <v>705234.08314859425</v>
       </c>
       <c r="D36" s="12">
         <v>703461.65253019601</v>
@@ -5287,7 +5285,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="12">
-        <v>717126.84437163593</v>
+        <v>717249.12990196224</v>
       </c>
       <c r="D37" s="12">
         <v>706958.03908231901</v>
@@ -5301,7 +5299,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="12">
-        <v>717060.7430119497</v>
+        <v>717125.64588613005</v>
       </c>
       <c r="D38" s="12">
         <v>677085.52917315101</v>
@@ -5315,7 +5313,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="12">
-        <v>720875.2460696802</v>
+        <v>720802.56315849815</v>
       </c>
       <c r="D39" s="12">
         <v>776486.60279942001</v>
@@ -5329,7 +5327,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="12">
-        <v>725496.14859723055</v>
+        <v>725454.40232530748</v>
       </c>
       <c r="D40" s="12">
         <v>721458.94421618199</v>
@@ -5343,7 +5341,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="12">
-        <v>718196.28353239805</v>
+        <v>718245.80984132516</v>
       </c>
       <c r="D41" s="12">
         <v>706597.34502250701</v>
@@ -5357,7 +5355,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="12">
-        <v>707504.85521262127</v>
+        <v>707336.25313466752</v>
       </c>
       <c r="D42" s="12">
         <v>671066.04663506302</v>
@@ -5371,7 +5369,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="12">
-        <v>703306.5882396599</v>
+        <v>703266.1910445746</v>
       </c>
       <c r="D43" s="12">
         <v>760576.86834800395</v>
@@ -5385,7 +5383,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="12">
-        <v>697497.41833730193</v>
+        <v>697512.23532424343</v>
       </c>
       <c r="D44" s="12">
         <v>690879.79825168301</v>
@@ -5399,7 +5397,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="12">
-        <v>700915.32206387667</v>
+        <v>701109.50434997655</v>
       </c>
       <c r="D45" s="12">
         <v>686701.47061871097</v>
@@ -5413,7 +5411,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="12">
-        <v>711375.93314010161</v>
+        <v>711258.38599491504</v>
       </c>
       <c r="D46" s="12">
         <v>672749.81139169901</v>
@@ -5427,7 +5425,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="12">
-        <v>728089.28302817431</v>
+        <v>727839.99863887194</v>
       </c>
       <c r="D47" s="12">
         <v>791235.96554166998</v>
@@ -5441,7 +5439,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="12">
-        <v>727364.1882352829</v>
+        <v>727481.57076581276</v>
       </c>
       <c r="D48" s="12">
         <v>718281.26544978202</v>
@@ -5455,7 +5453,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="12">
-        <v>719119.18214860151</v>
+        <v>719368.63115256047</v>
       </c>
       <c r="D49" s="12">
         <v>703681.54416900803</v>
@@ -5469,7 +5467,7 @@
         <v>29</v>
       </c>
       <c r="C50" s="12">
-        <v>712838.59891063347</v>
+        <v>712640.06153844751</v>
       </c>
       <c r="D50" s="12">
         <v>677652.08911570301</v>
@@ -5484,7 +5482,7 @@
         <v>30</v>
       </c>
       <c r="C51" s="12">
-        <v>701661.62402498827</v>
+        <v>701370.99166469392</v>
       </c>
       <c r="D51" s="12">
         <v>760703.28015165601</v>
@@ -5499,7 +5497,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="12">
-        <v>703502.85074439459</v>
+        <v>703724.32076925179</v>
       </c>
       <c r="D52" s="12">
         <v>694382.47577623103</v>
@@ -5514,7 +5512,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="12">
-        <v>707908.32071062957</v>
+        <v>708176.02041825175</v>
       </c>
       <c r="D53" s="12">
         <v>693173.54934705805</v>
@@ -5529,7 +5527,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="12">
-        <v>714595.91167597554</v>
+        <v>714233.72694170265</v>
       </c>
       <c r="D54" s="12">
         <v>681444.76611022197</v>
@@ -5544,7 +5542,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="12">
-        <v>722352.21513637132</v>
+        <v>722090.59875214146</v>
       </c>
       <c r="D55" s="12">
         <v>778401.67644931702</v>
@@ -5559,7 +5557,7 @@
         <v>31</v>
       </c>
       <c r="C56" s="12">
-        <v>730431.25721323024</v>
+        <v>730682.64569057734</v>
       </c>
       <c r="D56" s="12">
         <v>721120.42685279401</v>
@@ -5574,7 +5572,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="12">
-        <v>738180.4070257179</v>
+        <v>738552.81966687483</v>
       </c>
       <c r="D57" s="12">
         <v>724592.92163896305</v>
@@ -5589,11 +5587,12 @@
         <v>29</v>
       </c>
       <c r="C58" s="12">
-        <v>736153.86066421203</v>
+        <v>735783.7993534999</v>
       </c>
       <c r="D58" s="12">
         <v>707324.26805721398</v>
       </c>
+      <c r="G58" s="32"/>
       <c r="H58" s="32"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -5604,11 +5603,12 @@
         <v>30</v>
       </c>
       <c r="C59" s="12">
-        <v>702572.73159596475</v>
+        <v>702155.70474938827</v>
       </c>
       <c r="D59" s="12">
         <v>747428.29995457502</v>
       </c>
+      <c r="G59" s="32"/>
       <c r="H59" s="32"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -5619,11 +5619,12 @@
         <v>31</v>
       </c>
       <c r="C60" s="12">
-        <v>700278.87950862665</v>
+        <v>700519.99386328529</v>
       </c>
       <c r="D60" s="12">
         <v>696101.58352180803</v>
       </c>
+      <c r="G60" s="32"/>
       <c r="H60" s="32"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -5634,11 +5635,12 @@
         <v>32</v>
       </c>
       <c r="C61" s="12">
-        <v>690504.300149246</v>
+        <v>691050.27395187633</v>
       </c>
       <c r="D61" s="12">
         <v>678655.62038445403</v>
       </c>
+      <c r="G61" s="32"/>
       <c r="H61" s="32"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -5649,11 +5651,12 @@
         <v>29</v>
       </c>
       <c r="C62" s="12">
-        <v>691669.02698322793</v>
-      </c>
-      <c r="D62" s="12">
-        <v>665690.59065187594</v>
-      </c>
+        <v>691187.80785437603</v>
+      </c>
+      <c r="D62">
+        <v>665848.71529970889</v>
+      </c>
+      <c r="G62" s="32"/>
       <c r="H62" s="32"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -5664,11 +5667,12 @@
         <v>30</v>
       </c>
       <c r="C63" s="12">
-        <v>696755.15893017035</v>
-      </c>
-      <c r="D63" s="12">
-        <v>751765.13811138296</v>
-      </c>
+        <v>696112.6913947385</v>
+      </c>
+      <c r="D63">
+        <v>751784.46077713254</v>
+      </c>
+      <c r="G63" s="32"/>
       <c r="H63" s="32"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -5679,11 +5683,12 @@
         <v>31</v>
       </c>
       <c r="C64" s="12">
-        <v>697871.69467852404</v>
-      </c>
-      <c r="D64" s="12">
-        <v>683911.44245860004</v>
-      </c>
+        <v>698265.65536115842</v>
+      </c>
+      <c r="D64">
+        <v>683900.89855257841</v>
+      </c>
+      <c r="G64" s="32"/>
       <c r="H64" s="32"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -5694,11 +5699,12 @@
         <v>32</v>
       </c>
       <c r="C65" s="12">
-        <v>685889.88423139369</v>
-      </c>
-      <c r="D65" s="11">
-        <v>670818.59360145801</v>
-      </c>
+        <v>687329.05974156479</v>
+      </c>
+      <c r="D65">
+        <v>671361.13972242002</v>
+      </c>
+      <c r="G65" s="32"/>
       <c r="H65" s="32"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -5709,10 +5715,10 @@
         <v>29</v>
       </c>
       <c r="C66" s="11">
-        <v>657839.92130941316</v>
+        <v>657711.75186022639</v>
       </c>
       <c r="D66" s="11">
-        <v>632469.10245408595</v>
+        <v>632733.36598162609</v>
       </c>
       <c r="H66" s="32"/>
     </row>
@@ -5724,10 +5730,10 @@
         <v>30</v>
       </c>
       <c r="C67" s="11">
-        <v>559729.96657034964</v>
+        <v>558526.02320056118</v>
       </c>
       <c r="D67" s="11">
-        <v>608823.50379551796</v>
+        <v>608450.80405697017</v>
       </c>
       <c r="H67" s="32"/>
     </row>
@@ -5739,10 +5745,10 @@
         <v>31</v>
       </c>
       <c r="C68" s="11">
-        <v>626201.59661515127</v>
+        <v>626583.75934842485</v>
       </c>
       <c r="D68" s="11">
-        <v>614416.20615719398</v>
+        <v>614335.69211847626</v>
       </c>
       <c r="H68" s="32"/>
     </row>
@@ -5754,10 +5760,10 @@
         <v>32</v>
       </c>
       <c r="C69" s="11">
-        <v>654099.04286113894</v>
+        <v>654358.18872116203</v>
       </c>
       <c r="D69" s="11">
-        <v>642161.71494925604</v>
+        <v>641659.86097329983</v>
       </c>
       <c r="H69" s="32"/>
     </row>
@@ -5769,10 +5775,10 @@
         <v>29</v>
       </c>
       <c r="C70" s="11">
-        <v>675141.32047996053</v>
+        <v>676335.19401415577</v>
       </c>
       <c r="D70">
-        <v>650821.34239924757</v>
+        <v>652563.11939207092</v>
       </c>
       <c r="H70" s="32"/>
     </row>
@@ -5784,10 +5790,10 @@
         <v>30</v>
       </c>
       <c r="C71" s="11">
-        <v>671345.36190175533</v>
+        <v>670924.73554681102</v>
       </c>
       <c r="D71">
-        <v>717967.93370259111</v>
+        <v>718843.1229160385</v>
       </c>
       <c r="H71" s="32"/>
     </row>
@@ -5799,10 +5805,10 @@
         <v>31</v>
       </c>
       <c r="C72" s="11">
-        <v>698467.0832059501</v>
+        <v>698323.59708729805</v>
       </c>
       <c r="D72" s="11">
-        <v>687786.64721903251</v>
+        <v>686778.32722188451</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -5813,10 +5819,24 @@
         <v>32</v>
       </c>
       <c r="C73" s="11">
-        <v>709292.21856571629</v>
+        <v>711259.17185327853</v>
       </c>
       <c r="D73" s="11">
-        <v>697670.06530119025</v>
+        <v>698658.13099747989</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="11">
+        <v>2022</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="11">
+        <v>717474.48191855289</v>
+      </c>
+      <c r="D74" s="11">
+        <v>691652.1861622748</v>
       </c>
     </row>
   </sheetData>
@@ -6610,7 +6630,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C20"/>
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6637,14 +6657,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="41">
-        <v>4461</v>
+        <v>5724</v>
       </c>
       <c r="C2" s="41">
-        <v>5716</v>
+        <v>7666</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-1255</v>
+        <v>-1942</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6652,14 +6672,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="41">
-        <v>1708</v>
+        <v>2224</v>
       </c>
       <c r="C3" s="41">
-        <v>271</v>
+        <v>350</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1437</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6667,14 +6687,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="41">
-        <v>1651</v>
+        <v>2089</v>
       </c>
       <c r="C4" s="41">
-        <v>756</v>
+        <v>1143</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>895</v>
+        <v>946</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6682,14 +6702,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="41">
-        <v>349</v>
+        <v>505</v>
       </c>
       <c r="C5" s="41">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>340</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6697,14 +6717,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="41">
-        <v>2606</v>
+        <v>3348</v>
       </c>
       <c r="C6" s="41">
-        <v>3146</v>
+        <v>4625</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-540</v>
+        <v>-1277</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6712,14 +6732,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="41">
-        <v>3614</v>
+        <v>4666</v>
       </c>
       <c r="C7" s="41">
-        <v>3729</v>
+        <v>4540</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6727,14 +6747,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="41">
-        <v>205</v>
+        <v>273</v>
       </c>
       <c r="C8" s="41">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-45</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6742,14 +6762,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="41">
-        <v>425</v>
+        <v>496</v>
       </c>
       <c r="C9" s="41">
-        <v>197</v>
+        <v>251</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6757,14 +6777,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="41">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="C10" s="41">
-        <v>155</v>
+        <v>209</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6772,14 +6792,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="41">
-        <v>2731</v>
+        <v>3465</v>
       </c>
       <c r="C11" s="41">
-        <v>1438</v>
+        <v>1829</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1293</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6787,14 +6807,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="41">
-        <v>1625</v>
+        <v>2211</v>
       </c>
       <c r="C12" s="41">
-        <v>5655</v>
+        <v>7084</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-4030</v>
+        <v>-4873</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6802,14 +6822,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="41">
-        <v>448</v>
+        <v>609</v>
       </c>
       <c r="C13" s="41">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6817,14 +6837,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="41">
-        <v>208</v>
+        <v>265</v>
       </c>
       <c r="C14" s="41">
-        <v>365</v>
+        <v>463</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-157</v>
+        <v>-198</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6832,14 +6852,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="41">
-        <v>1388</v>
+        <v>2096</v>
       </c>
       <c r="C15" s="41">
-        <v>591</v>
+        <v>710</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>797</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6847,14 +6867,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="41">
-        <v>1497</v>
+        <v>1889</v>
       </c>
       <c r="C16" s="41">
-        <v>1066</v>
+        <v>1327</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>431</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6862,14 +6882,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="41">
-        <v>1627</v>
+        <v>2174</v>
       </c>
       <c r="C17" s="41">
-        <v>134</v>
+        <v>506</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1493</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6877,14 +6897,14 @@
         <v>95</v>
       </c>
       <c r="B18" s="41">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="C18" s="41">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6892,14 +6912,14 @@
         <v>96</v>
       </c>
       <c r="B19" s="41">
-        <v>303</v>
+        <v>374</v>
       </c>
       <c r="C19" s="41">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -6907,14 +6927,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="42">
-        <v>2445</v>
+        <v>3053</v>
       </c>
       <c r="C20" s="42">
-        <v>911</v>
+        <v>1095</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1534</v>
+        <v>1958</v>
       </c>
     </row>
   </sheetData>
@@ -6949,7 +6969,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="47">
-        <v>27681</v>
+        <v>35917</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6957,7 +6977,7 @@
         <v>185</v>
       </c>
       <c r="B3" s="47">
-        <v>8124</v>
+        <v>10221</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6965,7 +6985,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="41">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6973,7 +6993,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="41">
-        <v>481</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6981,7 +7001,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="41">
-        <v>80</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6989,7 +7009,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="41">
-        <v>227</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6997,7 +7017,7 @@
         <v>142</v>
       </c>
       <c r="B8" s="41">
-        <v>165</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7005,7 +7025,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="41">
-        <v>6453</v>
+        <v>8006</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7013,7 +7033,7 @@
         <v>144</v>
       </c>
       <c r="B10" s="41">
-        <v>404</v>
+        <v>626</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7021,7 +7041,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="41">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7029,7 +7049,7 @@
         <v>146</v>
       </c>
       <c r="B12" s="41">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7037,7 +7057,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="41">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7045,7 +7065,7 @@
         <v>148</v>
       </c>
       <c r="B14" s="41">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7053,7 +7073,7 @@
         <v>149</v>
       </c>
       <c r="B15" s="41">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7061,7 +7081,7 @@
         <v>186</v>
       </c>
       <c r="B16" s="47">
-        <v>9979</v>
+        <v>13615</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7069,7 +7089,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="41">
-        <v>1294</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7077,7 +7097,7 @@
         <v>151</v>
       </c>
       <c r="B18" s="41">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7085,7 +7105,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="41">
-        <v>437</v>
+        <v>552</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7093,7 +7113,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="41">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7101,7 +7121,7 @@
         <v>154</v>
       </c>
       <c r="B21" s="41">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7109,7 +7129,7 @@
         <v>155</v>
       </c>
       <c r="B22" s="41">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7117,7 +7137,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="41">
-        <v>281</v>
+        <v>395</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7125,7 +7145,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="41">
-        <v>2647</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7133,7 +7153,7 @@
         <v>158</v>
       </c>
       <c r="B25" s="41">
-        <v>85</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7141,7 +7161,7 @@
         <v>159</v>
       </c>
       <c r="B26" s="41">
-        <v>227</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7149,7 +7169,7 @@
         <v>160</v>
       </c>
       <c r="B27" s="41">
-        <v>281</v>
+        <v>377</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7157,7 +7177,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="41">
-        <v>4099</v>
+        <v>5457</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7165,7 +7185,7 @@
         <v>162</v>
       </c>
       <c r="B29" s="41">
-        <v>86</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7173,7 +7193,7 @@
         <v>163</v>
       </c>
       <c r="B30" s="41">
-        <v>151</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7181,7 +7201,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="41">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7189,7 +7209,7 @@
         <v>165</v>
       </c>
       <c r="B32" s="41">
-        <v>176</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7197,7 +7217,7 @@
         <v>187</v>
       </c>
       <c r="B33" s="47">
-        <v>6992</v>
+        <v>8921</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7205,7 +7225,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="41">
-        <v>2085</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7213,7 +7233,7 @@
         <v>167</v>
       </c>
       <c r="B35" s="41">
-        <v>389</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7221,7 +7241,7 @@
         <v>168</v>
       </c>
       <c r="B36" s="41">
-        <v>68</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7229,7 +7249,7 @@
         <v>169</v>
       </c>
       <c r="B37" s="41">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7237,7 +7257,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="41">
-        <v>159</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7245,7 +7265,7 @@
         <v>171</v>
       </c>
       <c r="B39" s="41">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7253,7 +7273,7 @@
         <v>172</v>
       </c>
       <c r="B40" s="41">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -7261,7 +7281,7 @@
         <v>173</v>
       </c>
       <c r="B41" s="41">
-        <v>49</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -7269,7 +7289,7 @@
         <v>174</v>
       </c>
       <c r="B42" s="41">
-        <v>953</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -7277,7 +7297,7 @@
         <v>175</v>
       </c>
       <c r="B43" s="41">
-        <v>688</v>
+        <v>806</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -7285,7 +7305,7 @@
         <v>176</v>
       </c>
       <c r="B44" s="41">
-        <v>448</v>
+        <v>575</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -7293,7 +7313,7 @@
         <v>177</v>
       </c>
       <c r="B45" s="41">
-        <v>1957</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -7309,7 +7329,7 @@
         <v>179</v>
       </c>
       <c r="B47" s="41">
-        <v>94</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -7317,7 +7337,7 @@
         <v>188</v>
       </c>
       <c r="B48" s="47">
-        <v>2587</v>
+        <v>3160</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7325,7 +7345,7 @@
         <v>180</v>
       </c>
       <c r="B49" s="41">
-        <v>1280</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7333,7 +7353,7 @@
         <v>181</v>
       </c>
       <c r="B50" s="41">
-        <v>703</v>
+        <v>944</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7341,7 +7361,7 @@
         <v>182</v>
       </c>
       <c r="B51" s="41">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7349,7 +7369,7 @@
         <v>183</v>
       </c>
       <c r="B52" s="48">
-        <v>480</v>
+        <v>561</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -7357,7 +7377,7 @@
         <v>184</v>
       </c>
       <c r="B53" s="49">
-        <v>86</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -7370,7 +7390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B40"/>
     </sheetView>
   </sheetViews>
@@ -7392,7 +7412,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="47">
-        <v>24852</v>
+        <v>32722</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7400,7 +7420,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="47">
-        <v>4140</v>
+        <v>5184</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7408,7 +7428,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="41">
-        <v>3116</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7416,7 +7436,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="41">
-        <v>460</v>
+        <v>568</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7424,7 +7444,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="41">
-        <v>413</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7432,7 +7452,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="41">
-        <v>152</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7440,7 +7460,7 @@
         <v>211</v>
       </c>
       <c r="B8" s="47">
-        <v>9440</v>
+        <v>12314</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7448,7 +7468,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="41">
-        <v>741</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7456,7 +7476,7 @@
         <v>195</v>
       </c>
       <c r="B10" s="41">
-        <v>441</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7464,7 +7484,7 @@
         <v>196</v>
       </c>
       <c r="B11" s="41">
-        <v>3651</v>
+        <v>4866</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7472,7 +7492,7 @@
         <v>197</v>
       </c>
       <c r="B12" s="41">
-        <v>1269</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7480,7 +7500,7 @@
         <v>198</v>
       </c>
       <c r="B13" s="41">
-        <v>383</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7488,7 +7508,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="41">
-        <v>491</v>
+        <v>606</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7496,7 +7516,7 @@
         <v>200</v>
       </c>
       <c r="B15" s="41">
-        <v>249</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7504,7 +7524,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="41">
-        <v>1517</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7512,7 +7532,7 @@
         <v>202</v>
       </c>
       <c r="B17" s="41">
-        <v>698</v>
+        <v>905</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7520,7 +7540,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="47">
-        <v>3040</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7528,7 +7548,7 @@
         <v>195</v>
       </c>
       <c r="B19" s="41">
-        <v>2956</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7536,7 +7556,7 @@
         <v>203</v>
       </c>
       <c r="B20" s="41">
-        <v>84</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7544,7 +7564,7 @@
         <v>213</v>
       </c>
       <c r="B21" s="47">
-        <v>4551</v>
+        <v>5943</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7552,7 +7572,7 @@
         <v>190</v>
       </c>
       <c r="B22" s="41">
-        <v>3015</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7560,7 +7580,7 @@
         <v>191</v>
       </c>
       <c r="B23" s="41">
-        <v>1202</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7568,7 +7588,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="41">
-        <v>334</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7576,7 +7596,7 @@
         <v>214</v>
       </c>
       <c r="B25" s="47">
-        <v>2876</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7584,7 +7604,7 @@
         <v>205</v>
       </c>
       <c r="B26" s="41">
-        <v>121</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7592,7 +7612,7 @@
         <v>194</v>
       </c>
       <c r="B27" s="41">
-        <v>210</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7600,7 +7620,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="41">
-        <v>270</v>
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7608,7 +7628,7 @@
         <v>196</v>
       </c>
       <c r="B29" s="41">
-        <v>832</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7616,7 +7636,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="41">
-        <v>186</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7624,7 +7644,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="41">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7632,7 +7652,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="41">
-        <v>215</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7640,7 +7660,7 @@
         <v>190</v>
       </c>
       <c r="B33" s="41">
-        <v>210</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7648,7 +7668,7 @@
         <v>191</v>
       </c>
       <c r="B34" s="41">
-        <v>198</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7656,7 +7676,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="41">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7664,7 +7684,7 @@
         <v>208</v>
       </c>
       <c r="B36" s="41">
-        <v>183</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7672,7 +7692,7 @@
         <v>209</v>
       </c>
       <c r="B37" s="41">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7680,7 +7700,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="47">
-        <v>598</v>
+        <v>769</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7688,7 +7708,7 @@
         <v>191</v>
       </c>
       <c r="B39" s="53">
-        <v>598</v>
+        <v>769</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7696,7 +7716,7 @@
         <v>216</v>
       </c>
       <c r="B40" s="54">
-        <v>207</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo datos ipc junio 22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D05894-A2E8-4EEF-9564-FDAB6B45D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3596C1D1-60B0-466E-B1DD-8130AE5BC7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -1280,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,6 +2414,23 @@
       </c>
       <c r="E66">
         <v>5.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="34">
+        <v>44713</v>
+      </c>
+      <c r="B67" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="C67">
+        <v>6.6</v>
+      </c>
+      <c r="D67">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E67">
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>
@@ -2644,7 +2661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A75" sqref="A75:A77"/>
     </sheetView>
   </sheetViews>
@@ -3743,8 +3760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,25 +3800,25 @@
         <v>129</v>
       </c>
       <c r="B2" s="35">
-        <v>4.2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C2" s="35">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="D2" s="35">
-        <v>6.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E2" s="39">
-        <v>5.5</v>
+        <v>7.6</v>
       </c>
       <c r="F2" s="35">
-        <v>4.3</v>
+        <v>5.7</v>
       </c>
       <c r="G2" s="35">
-        <v>5.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H2" s="21">
-        <v>4.8011630232723812</v>
+        <v>5.0702092215244132</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3809,25 +3826,25 @@
         <v>130</v>
       </c>
       <c r="B3" s="35">
-        <v>6.5</v>
+        <v>3.1</v>
       </c>
       <c r="C3" s="35">
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
       <c r="D3" s="35">
-        <v>6.2</v>
+        <v>3.4</v>
       </c>
       <c r="E3" s="39">
-        <v>6.5</v>
+        <v>2.6</v>
       </c>
       <c r="F3" s="35">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G3" s="35">
-        <v>4.7</v>
+        <v>3.8</v>
       </c>
       <c r="H3" s="21">
-        <v>6.2071124672684608</v>
+        <v>3.1398815205748276</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3835,25 +3852,25 @@
         <v>131</v>
       </c>
       <c r="B4" s="35">
-        <v>4.3</v>
+        <v>3.8</v>
       </c>
       <c r="C4" s="35">
-        <v>4.5999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="D4" s="35">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
       <c r="E4" s="39">
         <v>4.5999999999999996</v>
       </c>
       <c r="F4" s="35">
-        <v>3.5</v>
+        <v>4.7</v>
       </c>
       <c r="G4" s="35">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
       <c r="H4" s="21">
-        <v>4.4686095393981162</v>
+        <v>4.401363834141625</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3861,25 +3878,25 @@
         <v>132</v>
       </c>
       <c r="B5" s="35">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="35">
-        <v>7</v>
+        <v>6.3</v>
       </c>
       <c r="D5" s="35">
-        <v>6.5</v>
+        <v>7.3</v>
       </c>
       <c r="E5" s="39">
-        <v>7.4</v>
+        <v>6.4</v>
       </c>
       <c r="F5" s="35">
-        <v>10.9</v>
+        <v>7.8</v>
       </c>
       <c r="G5" s="35">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="H5" s="21">
-        <v>7.2269505176777216</v>
+        <v>7.0871711248462921</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3887,25 +3904,25 @@
         <v>133</v>
       </c>
       <c r="B6" s="35">
-        <v>2.2000000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="35">
-        <v>2.8</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="35">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="E6" s="39">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="F6" s="35">
-        <v>3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G6" s="35">
-        <v>4.3</v>
+        <v>0.9</v>
       </c>
       <c r="H6" s="21">
-        <v>2.4840512806867165</v>
+        <v>0.6288169623579476</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3913,25 +3930,25 @@
         <v>134</v>
       </c>
       <c r="B7" s="35">
-        <v>-2.8</v>
+        <v>13.4</v>
       </c>
       <c r="C7" s="35">
-        <v>-4.7</v>
+        <v>7.9</v>
       </c>
       <c r="D7" s="35">
-        <v>-0.8</v>
+        <v>3.8</v>
       </c>
       <c r="E7" s="39">
-        <v>-2</v>
+        <v>6.1</v>
       </c>
       <c r="F7" s="35">
-        <v>-3.2</v>
+        <v>11.6</v>
       </c>
       <c r="G7" s="35">
-        <v>1.9</v>
+        <v>6.6</v>
       </c>
       <c r="H7" s="21">
-        <v>-2.9246417117194001</v>
+        <v>9.9488320810953823</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3939,25 +3956,25 @@
         <v>135</v>
       </c>
       <c r="B8" s="35">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="C8" s="35">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="D8" s="35">
-        <v>8.1</v>
+        <v>8.5</v>
       </c>
       <c r="E8" s="39">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
       <c r="F8" s="35">
-        <v>4.8</v>
+        <v>6.7</v>
       </c>
       <c r="G8" s="35">
-        <v>4.5</v>
+        <v>6.4</v>
       </c>
       <c r="H8" s="22">
-        <v>5.3665245275398732</v>
+        <v>6.3371534453813272</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3965,25 +3982,25 @@
         <v>136</v>
       </c>
       <c r="B9" s="35">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="C9" s="35">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="D9" s="35">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="E9" s="39">
-        <v>3.7</v>
+        <v>5</v>
       </c>
       <c r="F9" s="35">
-        <v>3.6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G9" s="35">
-        <v>5.4</v>
+        <v>3.4</v>
       </c>
       <c r="H9" s="21">
-        <v>6.0523660715741778</v>
+        <v>5.6778156100279809</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3991,25 +4008,25 @@
         <v>137</v>
       </c>
       <c r="B10" s="35">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="C10" s="35">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="D10" s="35">
-        <v>2.9</v>
+        <v>4.2</v>
       </c>
       <c r="E10" s="39">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="F10" s="35">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="G10" s="35">
-        <v>6.4</v>
+        <v>6.2</v>
       </c>
       <c r="H10" s="21">
-        <v>4.9551952738916105</v>
+        <v>5.5225809919576374</v>
       </c>
     </row>
   </sheetData>
@@ -4059,25 +4076,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="27">
+        <v>5.3</v>
+      </c>
+      <c r="C2" s="37">
+        <v>5.5</v>
+      </c>
+      <c r="D2" s="37">
+        <v>5.2</v>
+      </c>
+      <c r="E2" s="37">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F2" s="37">
+        <v>5.2</v>
+      </c>
+      <c r="G2" s="37">
+        <v>5.3</v>
+      </c>
+      <c r="H2" s="29">
         <v>5.0999999999999996</v>
-      </c>
-      <c r="C2" s="37">
-        <v>4.8</v>
-      </c>
-      <c r="D2" s="37">
-        <v>5.3</v>
-      </c>
-      <c r="E2" s="37">
-        <v>5.3</v>
-      </c>
-      <c r="F2" s="37">
-        <v>5.6</v>
-      </c>
-      <c r="G2" s="37">
-        <v>5.2</v>
-      </c>
-      <c r="H2" s="29">
-        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4085,22 +4102,22 @@
         <v>13</v>
       </c>
       <c r="B3" s="26">
-        <v>4.4000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C3" s="36">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
       <c r="D3" s="36">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="E3" s="36">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="F3" s="36">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="G3" s="36">
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H3" s="28">
         <v>4.5999999999999996</v>
@@ -4111,25 +4128,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="26">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
       <c r="C4" s="36">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="36">
-        <v>5.3</v>
+        <v>6.9</v>
       </c>
       <c r="E4" s="36">
-        <v>7.8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="36">
-        <v>6.5</v>
+        <v>5.6</v>
       </c>
       <c r="G4" s="36">
-        <v>6.5</v>
+        <v>5.8</v>
       </c>
       <c r="H4" s="28">
-        <v>5.3</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4140,22 +4157,22 @@
         <v>5.8</v>
       </c>
       <c r="C5" s="36">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="D5" s="36">
-        <v>6.7</v>
+        <v>6.1</v>
       </c>
       <c r="E5" s="36">
-        <v>4.7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="36">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="G5" s="36">
-        <v>8.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H5" s="28">
-        <v>6.3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4163,25 +4180,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="26">
-        <v>3.6</v>
+        <v>6.8</v>
       </c>
       <c r="C6" s="36">
-        <v>2.8</v>
+        <v>7.5</v>
       </c>
       <c r="D6" s="36">
-        <v>3.3</v>
+        <v>6</v>
       </c>
       <c r="E6" s="36">
-        <v>5.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F6" s="36">
-        <v>10</v>
+        <v>9.1</v>
       </c>
       <c r="G6" s="36">
-        <v>2</v>
+        <v>6.6</v>
       </c>
       <c r="H6" s="28">
-        <v>2.4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4189,25 +4206,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="26">
+        <v>6</v>
+      </c>
+      <c r="C7" s="36">
+        <v>6.3</v>
+      </c>
+      <c r="D7" s="36">
+        <v>5.8</v>
+      </c>
+      <c r="E7" s="36">
         <v>5.4</v>
       </c>
-      <c r="C7" s="36">
-        <v>5.3</v>
-      </c>
-      <c r="D7" s="36">
-        <v>5.6</v>
-      </c>
-      <c r="E7" s="36">
+      <c r="F7" s="36">
+        <v>5.8</v>
+      </c>
+      <c r="G7" s="36">
+        <v>6.4</v>
+      </c>
+      <c r="H7" s="28">
         <v>5</v>
-      </c>
-      <c r="F7" s="36">
-        <v>5.7</v>
-      </c>
-      <c r="G7" s="36">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H7" s="28">
-        <v>4.8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4215,25 +4232,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="26">
-        <v>6.2</v>
+        <v>7.4</v>
       </c>
       <c r="C8" s="36">
-        <v>6.1</v>
+        <v>7.9</v>
       </c>
       <c r="D8" s="36">
-        <v>6.3</v>
+        <v>7.1</v>
       </c>
       <c r="E8" s="36">
-        <v>6.1</v>
+        <v>6.8</v>
       </c>
       <c r="F8" s="36">
-        <v>5.9</v>
+        <v>7.6</v>
       </c>
       <c r="G8" s="36">
-        <v>6.7</v>
+        <v>7.2</v>
       </c>
       <c r="H8" s="28">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4241,25 +4258,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="26">
-        <v>6.1</v>
+        <v>4.7</v>
       </c>
       <c r="C9" s="36">
-        <v>5.4</v>
+        <v>3.4</v>
       </c>
       <c r="D9" s="36">
-        <v>7.1</v>
+        <v>5.8</v>
       </c>
       <c r="E9" s="36">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
       <c r="F9" s="36">
-        <v>6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G9" s="36">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="H9" s="28">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4267,25 +4284,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="26">
-        <v>3.1</v>
+        <v>0.4</v>
       </c>
       <c r="C10" s="36">
-        <v>3.1</v>
+        <v>0.2</v>
       </c>
       <c r="D10" s="36">
-        <v>2.8</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="36">
-        <v>2.7</v>
+        <v>1.9</v>
       </c>
       <c r="F10" s="36">
-        <v>3.8</v>
+        <v>0.9</v>
       </c>
       <c r="G10" s="36">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="28">
-        <v>4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4293,25 +4310,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="26">
-        <v>5.2</v>
+        <v>4.3</v>
       </c>
       <c r="C11" s="36">
         <v>5.2</v>
       </c>
       <c r="D11" s="36">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
       <c r="E11" s="36">
-        <v>5.0999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="F11" s="36">
-        <v>7.7</v>
+        <v>2.4</v>
       </c>
       <c r="G11" s="36">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="H11" s="28">
-        <v>5.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4319,25 +4336,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="26">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="C12" s="36">
-        <v>3.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D12" s="36">
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="E12" s="36">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="36">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="G12" s="36">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="H12" s="28">
-        <v>1.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4345,25 +4362,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="26">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="C13" s="36">
-        <v>5.2</v>
+        <v>6.6</v>
       </c>
       <c r="D13" s="36">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="E13" s="36">
+        <v>4.8</v>
+      </c>
+      <c r="F13" s="36">
+        <v>7.7</v>
+      </c>
+      <c r="G13" s="36">
+        <v>6.2</v>
+      </c>
+      <c r="H13" s="28">
         <v>7</v>
-      </c>
-      <c r="F13" s="36">
-        <v>6.4</v>
-      </c>
-      <c r="G13" s="36">
-        <v>6.6</v>
-      </c>
-      <c r="H13" s="28">
-        <v>3.6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4371,25 +4388,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="26">
+        <v>5</v>
+      </c>
+      <c r="C14" s="36">
+        <v>5.3</v>
+      </c>
+      <c r="D14" s="36">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C14" s="36">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D14" s="36">
-        <v>4.5</v>
-      </c>
       <c r="E14" s="36">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="F14" s="36">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="G14" s="36">
+        <v>4.7</v>
+      </c>
+      <c r="H14" s="28">
         <v>5.2</v>
-      </c>
-      <c r="H14" s="28">
-        <v>4.8</v>
       </c>
     </row>
   </sheetData>
@@ -4403,7 +4420,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4439,25 +4456,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="31">
-        <v>60.7</v>
+        <v>64</v>
       </c>
       <c r="C2" s="38">
-        <v>61.2</v>
+        <v>65</v>
       </c>
       <c r="D2" s="38">
-        <v>59.6</v>
+        <v>62.6</v>
       </c>
       <c r="E2" s="38">
-        <v>61.8</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="F2" s="38">
-        <v>61.7</v>
+        <v>64.8</v>
       </c>
       <c r="G2" s="38">
-        <v>60.5</v>
+        <v>63.2</v>
       </c>
       <c r="H2" s="38">
-        <v>61</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4465,25 +4482,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="30">
-        <v>64.2</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="C3" s="23">
-        <v>64.5</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="D3" s="23">
-        <v>63.1</v>
+        <v>65.3</v>
       </c>
       <c r="E3" s="23">
-        <v>64.5</v>
+        <v>67.3</v>
       </c>
       <c r="F3" s="23">
-        <v>65.8</v>
+        <v>67.3</v>
       </c>
       <c r="G3" s="23">
-        <v>64.2</v>
+        <v>65.2</v>
       </c>
       <c r="H3" s="23">
-        <v>66</v>
+        <v>68.2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4491,25 +4508,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="30">
-        <v>54.4</v>
+        <v>56.2</v>
       </c>
       <c r="C4" s="23">
-        <v>53.8</v>
+        <v>55.6</v>
       </c>
       <c r="D4" s="23">
+        <v>56.7</v>
+      </c>
+      <c r="E4" s="23">
+        <v>63.1</v>
+      </c>
+      <c r="F4" s="23">
+        <v>56.2</v>
+      </c>
+      <c r="G4" s="23">
         <v>54.1</v>
       </c>
-      <c r="E4" s="23">
-        <v>64.900000000000006</v>
-      </c>
-      <c r="F4" s="23">
-        <v>55.6</v>
-      </c>
-      <c r="G4" s="23">
-        <v>53.9</v>
-      </c>
       <c r="H4" s="23">
-        <v>49.9</v>
+        <v>52.6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4517,25 +4534,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="30">
-        <v>79.599999999999994</v>
+        <v>83.6</v>
       </c>
       <c r="C5" s="23">
-        <v>85.1</v>
+        <v>88</v>
       </c>
       <c r="D5" s="23">
-        <v>75.3</v>
+        <v>80.2</v>
       </c>
       <c r="E5" s="23">
-        <v>72.400000000000006</v>
+        <v>79.8</v>
       </c>
       <c r="F5" s="23">
-        <v>72.2</v>
+        <v>77.5</v>
       </c>
       <c r="G5" s="23">
-        <v>77.099999999999994</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="H5" s="23">
-        <v>77</v>
+        <v>83.4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4543,25 +4560,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="30">
-        <v>41.8</v>
+        <v>47.8</v>
       </c>
       <c r="C6" s="23">
-        <v>43.3</v>
+        <v>50.8</v>
       </c>
       <c r="D6" s="23">
-        <v>37.1</v>
+        <v>41.7</v>
       </c>
       <c r="E6" s="23">
-        <v>57.4</v>
+        <v>60.6</v>
       </c>
       <c r="F6" s="23">
-        <v>43.1</v>
+        <v>49.3</v>
       </c>
       <c r="G6" s="23">
-        <v>36.799999999999997</v>
+        <v>41.4</v>
       </c>
       <c r="H6" s="23">
-        <v>49.2</v>
+        <v>54.7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4569,25 +4586,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="30">
-        <v>54.8</v>
+        <v>58.9</v>
       </c>
       <c r="C7" s="23">
-        <v>55.3</v>
+        <v>59.8</v>
       </c>
       <c r="D7" s="23">
-        <v>54.8</v>
+        <v>58.9</v>
       </c>
       <c r="E7" s="23">
-        <v>51.5</v>
+        <v>54.5</v>
       </c>
       <c r="F7" s="23">
-        <v>54.7</v>
+        <v>58.4</v>
       </c>
       <c r="G7" s="23">
-        <v>56.3</v>
+        <v>60.6</v>
       </c>
       <c r="H7" s="23">
-        <v>51.6</v>
+        <v>53.9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4595,25 +4612,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="30">
-        <v>60.7</v>
+        <v>67.2</v>
       </c>
       <c r="C8" s="23">
-        <v>60.7</v>
+        <v>69.7</v>
       </c>
       <c r="D8" s="23">
-        <v>61.2</v>
+        <v>66</v>
       </c>
       <c r="E8" s="23">
-        <v>61</v>
+        <v>64.5</v>
       </c>
       <c r="F8" s="23">
-        <v>57.7</v>
+        <v>62.3</v>
       </c>
       <c r="G8" s="23">
-        <v>63.7</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="H8" s="23">
-        <v>57.6</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4621,25 +4638,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="30">
-        <v>56.7</v>
+        <v>59</v>
       </c>
       <c r="C9" s="23">
-        <v>55.2</v>
+        <v>55.4</v>
       </c>
       <c r="D9" s="23">
-        <v>57.7</v>
+        <v>61.6</v>
       </c>
       <c r="E9" s="23">
-        <v>60.6</v>
+        <v>66.8</v>
       </c>
       <c r="F9" s="23">
-        <v>54</v>
+        <v>56.6</v>
       </c>
       <c r="G9" s="23">
-        <v>58.2</v>
+        <v>64.2</v>
       </c>
       <c r="H9" s="23">
-        <v>60.6</v>
+        <v>60.2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4647,25 +4664,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="30">
-        <v>37.4</v>
+        <v>28.9</v>
       </c>
       <c r="C10" s="23">
-        <v>36.5</v>
+        <v>27.9</v>
       </c>
       <c r="D10" s="23">
-        <v>37.9</v>
+        <v>29</v>
       </c>
       <c r="E10" s="23">
-        <v>37.9</v>
+        <v>32.5</v>
       </c>
       <c r="F10" s="23">
-        <v>40.299999999999997</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="G10" s="23">
-        <v>38.1</v>
+        <v>29.5</v>
       </c>
       <c r="H10" s="23">
-        <v>37.200000000000003</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4673,25 +4690,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="30">
-        <v>51.7</v>
+        <v>54.8</v>
       </c>
       <c r="C11" s="23">
-        <v>52.3</v>
+        <v>57.4</v>
       </c>
       <c r="D11" s="23">
-        <v>49.8</v>
+        <v>51.3</v>
       </c>
       <c r="E11" s="23">
-        <v>49.1</v>
+        <v>50</v>
       </c>
       <c r="F11" s="23">
-        <v>60.8</v>
+        <v>61.9</v>
       </c>
       <c r="G11" s="23">
-        <v>50.2</v>
+        <v>52.6</v>
       </c>
       <c r="H11" s="23">
-        <v>50.8</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4699,25 +4716,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="30">
-        <v>57.7</v>
+        <v>59</v>
       </c>
       <c r="C12" s="23">
-        <v>57.2</v>
+        <v>59</v>
       </c>
       <c r="D12" s="23">
-        <v>61.9</v>
+        <v>62.7</v>
       </c>
       <c r="E12" s="23">
-        <v>51.9</v>
+        <v>51.5</v>
       </c>
       <c r="F12" s="23">
-        <v>47.8</v>
+        <v>49.1</v>
       </c>
       <c r="G12" s="23">
-        <v>50.9</v>
+        <v>54.4</v>
       </c>
       <c r="H12" s="23">
-        <v>64.2</v>
+        <v>64.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4725,25 +4742,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="30">
-        <v>76.7</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="C13" s="23">
-        <v>78.3</v>
+        <v>84.9</v>
       </c>
       <c r="D13" s="23">
-        <v>73.8</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E13" s="23">
-        <v>81.2</v>
+        <v>85.7</v>
       </c>
       <c r="F13" s="23">
-        <v>77.2</v>
+        <v>85.4</v>
       </c>
       <c r="G13" s="23">
-        <v>77.2</v>
+        <v>81.3</v>
       </c>
       <c r="H13" s="23">
-        <v>76</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4751,25 +4768,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="30">
-        <v>52.7</v>
+        <v>57.3</v>
       </c>
       <c r="C14" s="23">
-        <v>53.2</v>
+        <v>58.7</v>
       </c>
       <c r="D14" s="23">
-        <v>51.7</v>
+        <v>55</v>
       </c>
       <c r="E14" s="23">
-        <v>51.8</v>
+        <v>55.9</v>
       </c>
       <c r="F14" s="23">
-        <v>54.5</v>
+        <v>61</v>
       </c>
       <c r="G14" s="23">
-        <v>52.2</v>
+        <v>56.5</v>
       </c>
       <c r="H14" s="23">
-        <v>54.9</v>
+        <v>58.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo resultado fiscal e ica, ambos de julio"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3B648E-0320-4233-BAFF-7D5672CC2DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3366E3-2E37-4CCE-8AE5-9E1E59857962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -814,7 +814,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,12 +830,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -941,20 +935,14 @@
     <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -3790,7 +3778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
@@ -5925,14 +5913,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6536,14 +6524,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6692,7 +6680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C20"/>
     </sheetView>
   </sheetViews>
@@ -6720,14 +6708,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="30">
-        <v>7228</v>
+        <v>8770</v>
       </c>
       <c r="C2" s="30">
-        <v>9830</v>
+        <v>11727</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-2602</v>
+        <v>-2957</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6735,14 +6723,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="30">
-        <v>2607</v>
+        <v>2922</v>
       </c>
       <c r="C3" s="30">
-        <v>413</v>
+        <v>464</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>2194</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6750,14 +6738,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="30">
-        <v>2483</v>
+        <v>2933</v>
       </c>
       <c r="C4" s="30">
-        <v>1537</v>
+        <v>1984</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>949</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6765,14 +6753,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="30">
-        <v>691</v>
+        <v>838</v>
       </c>
       <c r="C5" s="30">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>676</v>
+        <v>820</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6780,14 +6768,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="30">
-        <v>4262</v>
+        <v>4841</v>
       </c>
       <c r="C6" s="30">
-        <v>6320</v>
+        <v>8113</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-2058</v>
+        <v>-3272</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6795,14 +6783,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="30">
-        <v>5585</v>
+        <v>6431</v>
       </c>
       <c r="C7" s="30">
-        <v>5551</v>
+        <v>6489</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6810,14 +6798,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="30">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="C8" s="30">
-        <v>359</v>
+        <v>411</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-26</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6825,14 +6813,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="30">
-        <v>586</v>
+        <v>669</v>
       </c>
       <c r="C9" s="30">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6840,14 +6828,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="30">
-        <v>253</v>
+        <v>317</v>
       </c>
       <c r="C10" s="30">
-        <v>263</v>
+        <v>294</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6855,14 +6843,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="30">
-        <v>4147</v>
+        <v>4893</v>
       </c>
       <c r="C11" s="30">
-        <v>2184</v>
+        <v>2509</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1963</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6870,14 +6858,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="30">
-        <v>2822</v>
+        <v>3568</v>
       </c>
       <c r="C12" s="30">
-        <v>8663</v>
+        <v>10150</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-5841</v>
+        <v>-6582</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6885,14 +6873,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="30">
-        <v>837</v>
+        <v>1084</v>
       </c>
       <c r="C13" s="30">
-        <v>355</v>
+        <v>462</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>482</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6900,14 +6888,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="30">
-        <v>348</v>
+        <v>510</v>
       </c>
       <c r="C14" s="30">
-        <v>577</v>
+        <v>663</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-229</v>
+        <v>-153</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6915,14 +6903,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="30">
-        <v>2726</v>
+        <v>3081</v>
       </c>
       <c r="C15" s="30">
-        <v>962</v>
+        <v>1158</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1764</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6930,14 +6918,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="30">
-        <v>2619</v>
+        <v>3123</v>
       </c>
       <c r="C16" s="30">
-        <v>1546</v>
+        <v>1807</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1073</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6945,14 +6933,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="30">
-        <v>2466</v>
+        <v>2827</v>
       </c>
       <c r="C17" s="30">
-        <v>696</v>
+        <v>848</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1770</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6960,14 +6948,14 @@
         <v>95</v>
       </c>
       <c r="B18" s="30">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="C18" s="30">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6975,14 +6963,14 @@
         <v>96</v>
       </c>
       <c r="B19" s="30">
-        <v>459</v>
+        <v>531</v>
       </c>
       <c r="C19" s="30">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>167</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -6990,14 +6978,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="31">
-        <v>3627</v>
+        <v>4102</v>
       </c>
       <c r="C20" s="31">
-        <v>1321</v>
+        <v>1737</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2306</v>
+        <v>2365</v>
       </c>
     </row>
   </sheetData>
@@ -7011,7 +6999,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7031,311 +7019,311 @@
       <c r="A2" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="42">
-        <v>44377</v>
+      <c r="B2" s="36">
+        <v>52151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="42">
-        <v>12256</v>
+      <c r="B3" s="36">
+        <v>14711</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="43">
-        <v>19</v>
+      <c r="B4" s="30">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="43">
-        <v>697</v>
+      <c r="B5" s="30">
+        <v>895</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="43">
-        <v>141</v>
+      <c r="B6" s="30">
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="43">
-        <v>347</v>
+      <c r="B7" s="30">
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="43">
-        <v>338</v>
+      <c r="B8" s="30">
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="43">
-        <v>9392</v>
+      <c r="B9" s="30">
+        <v>11086</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="43">
-        <v>893</v>
+      <c r="B10" s="30">
+        <v>1246</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="43">
-        <v>104</v>
+      <c r="B11" s="30">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="43">
-        <v>18</v>
+      <c r="B12" s="30">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="43">
-        <v>91</v>
+      <c r="B13" s="30">
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="43">
-        <v>144</v>
+      <c r="B14" s="30">
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="43">
-        <v>71</v>
+      <c r="B15" s="30">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="B16" s="42">
-        <v>17073</v>
+      <c r="B16" s="36">
+        <v>19986</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="43">
-        <v>2101</v>
+      <c r="B17" s="30">
+        <v>2502</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="43">
-        <v>124</v>
+      <c r="B18" s="30">
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="43">
-        <v>663</v>
+      <c r="B19" s="30">
+        <v>801</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="43">
-        <v>28</v>
+      <c r="B20" s="30">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="43">
-        <v>45</v>
+      <c r="B21" s="30">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="43">
-        <v>86</v>
+      <c r="B22" s="30">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="43">
-        <v>488</v>
+      <c r="B23" s="30">
+        <v>544</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="B24" s="43">
-        <v>5063</v>
+      <c r="B24" s="30">
+        <v>5798</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="43">
-        <v>121</v>
+      <c r="B25" s="30">
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="B26" s="43">
-        <v>392</v>
+      <c r="B26" s="30">
+        <v>460</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="43">
-        <v>452</v>
+      <c r="B27" s="30">
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B28" s="43">
-        <v>6808</v>
+      <c r="B28" s="30">
+        <v>8051</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="B29" s="43">
-        <v>137</v>
+      <c r="B29" s="30">
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B30" s="43">
-        <v>232</v>
+      <c r="B30" s="30">
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="B31" s="43">
-        <v>68</v>
+      <c r="B31" s="30">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="43">
-        <v>266</v>
+      <c r="B32" s="30">
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="B33" s="42">
-        <v>11088</v>
+      <c r="B33" s="36">
+        <v>13021</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="43">
-        <v>3244</v>
+      <c r="B34" s="30">
+        <v>3703</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="43">
-        <v>587</v>
+      <c r="B35" s="30">
+        <v>685</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="43">
-        <v>114</v>
+      <c r="B36" s="30">
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B37" s="43">
-        <v>14</v>
+      <c r="B37" s="30">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="43">
-        <v>243</v>
+      <c r="B38" s="30">
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="43">
-        <v>73</v>
+      <c r="B39" s="30">
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="43">
+      <c r="B40" s="30">
         <v>5</v>
       </c>
     </row>
@@ -7343,104 +7331,104 @@
       <c r="A41" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="43">
-        <v>82</v>
+      <c r="B41" s="30">
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="43">
-        <v>1429</v>
+      <c r="B42" s="30">
+        <v>1597</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="43">
-        <v>1040</v>
+      <c r="B43" s="30">
+        <v>1154</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="43">
-        <v>718</v>
+      <c r="B44" s="30">
+        <v>861</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="43">
-        <v>3356</v>
+      <c r="B45" s="30">
+        <v>4003</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="B46" s="43">
-        <v>38</v>
+      <c r="B46" s="30">
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="B47" s="43">
-        <v>143</v>
+      <c r="B47" s="30">
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="42">
-        <v>3961</v>
+      <c r="B48" s="36">
+        <v>4434</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="B49" s="43">
-        <v>1889</v>
+      <c r="B49" s="30">
+        <v>2036</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="B50" s="43">
-        <v>1200</v>
+      <c r="B50" s="30">
+        <v>1432</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="B51" s="43">
-        <v>51</v>
+      <c r="B51" s="30">
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="B52" s="44">
-        <v>616</v>
+      <c r="B52" s="43">
+        <v>683</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="B53" s="45">
-        <v>204</v>
+      <c r="B53" s="44">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -7453,9 +7441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7475,7 +7461,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="36">
-        <v>41284</v>
+        <v>49611</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7483,7 +7469,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="36">
-        <v>6291</v>
+        <v>7234</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7491,7 +7477,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="30">
-        <v>4700</v>
+        <v>5408</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7499,7 +7485,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="30">
-        <v>697</v>
+        <v>790</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7507,7 +7493,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="30">
-        <v>653</v>
+        <v>760</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7515,7 +7501,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="30">
-        <v>240</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7523,7 +7509,7 @@
         <v>211</v>
       </c>
       <c r="B8" s="36">
-        <v>15454</v>
+        <v>18173</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7531,7 +7517,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="30">
-        <v>1586</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7539,7 +7525,7 @@
         <v>195</v>
       </c>
       <c r="B10" s="30">
-        <v>740</v>
+        <v>850</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7547,7 +7533,7 @@
         <v>196</v>
       </c>
       <c r="B11" s="30">
-        <v>6145</v>
+        <v>7283</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7555,7 +7541,7 @@
         <v>197</v>
       </c>
       <c r="B12" s="30">
-        <v>1937</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7563,7 +7549,7 @@
         <v>198</v>
       </c>
       <c r="B13" s="30">
-        <v>606</v>
+        <v>711</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7571,7 +7557,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="30">
-        <v>732</v>
+        <v>849</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7579,7 +7565,7 @@
         <v>200</v>
       </c>
       <c r="B15" s="30">
-        <v>373</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7587,7 +7573,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="30">
-        <v>2210</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7595,7 +7581,7 @@
         <v>202</v>
       </c>
       <c r="B17" s="30">
-        <v>1125</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7603,7 +7589,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="36">
-        <v>6609</v>
+        <v>9008</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7611,7 +7597,7 @@
         <v>195</v>
       </c>
       <c r="B19" s="30">
-        <v>6460</v>
+        <v>8820</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7619,7 +7605,7 @@
         <v>203</v>
       </c>
       <c r="B20" s="30">
-        <v>149</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7627,7 +7613,7 @@
         <v>213</v>
       </c>
       <c r="B21" s="36">
-        <v>7321</v>
+        <v>8622</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7635,7 +7621,7 @@
         <v>190</v>
       </c>
       <c r="B22" s="30">
-        <v>4835</v>
+        <v>5671</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7643,7 +7629,7 @@
         <v>191</v>
       </c>
       <c r="B23" s="30">
-        <v>1946</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7651,7 +7637,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="30">
-        <v>539</v>
+        <v>626</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7659,7 +7645,7 @@
         <v>214</v>
       </c>
       <c r="B25" s="36">
-        <v>4321</v>
+        <v>5036</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7667,7 +7653,7 @@
         <v>205</v>
       </c>
       <c r="B26" s="30">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7675,7 +7661,7 @@
         <v>194</v>
       </c>
       <c r="B27" s="30">
-        <v>318</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7683,7 +7669,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="30">
-        <v>419</v>
+        <v>479</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7691,7 +7677,7 @@
         <v>196</v>
       </c>
       <c r="B29" s="30">
-        <v>1236</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7699,7 +7685,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="30">
-        <v>273</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7707,7 +7693,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="30">
-        <v>222</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7715,7 +7701,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="30">
-        <v>330</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7723,7 +7709,7 @@
         <v>190</v>
       </c>
       <c r="B33" s="30">
-        <v>323</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7731,7 +7717,7 @@
         <v>191</v>
       </c>
       <c r="B34" s="30">
-        <v>302</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7739,7 +7725,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="30">
-        <v>151</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7747,7 +7733,7 @@
         <v>208</v>
       </c>
       <c r="B36" s="30">
-        <v>272</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7755,7 +7741,7 @@
         <v>209</v>
       </c>
       <c r="B37" s="30">
-        <v>293</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7763,7 +7749,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="36">
-        <v>960</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7771,7 +7757,7 @@
         <v>191</v>
       </c>
       <c r="B39" s="40">
-        <v>960</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7779,7 +7765,7 @@
         <v>216</v>
       </c>
       <c r="B40" s="41">
-        <v>328</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo dato var ipc ago22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47386B1-D73E-444C-8E06-AF789133B8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C32334C-DEF5-4358-855E-F1D4276ADFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -1267,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68:E68"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,6 +2435,23 @@
       </c>
       <c r="E68">
         <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="23">
+        <v>44774</v>
+      </c>
+      <c r="B69" s="1">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D69">
+        <v>6.8</v>
+      </c>
+      <c r="E69">
+        <v>6.3</v>
       </c>
     </row>
   </sheetData>
@@ -2665,7 +2682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3790,9 +3807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3833,22 +3848,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="24">
-        <v>6.8</v>
+        <v>7.6</v>
       </c>
       <c r="D2" s="24">
-        <v>8.4</v>
+        <v>6.4</v>
       </c>
       <c r="E2" s="28">
-        <v>5.8</v>
+        <v>8.1</v>
       </c>
       <c r="F2" s="24">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="G2" s="24">
-        <v>7.1</v>
+        <v>6</v>
       </c>
       <c r="H2" s="16">
-        <v>6.9218070713876312</v>
+        <v>7.1518410812677402</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3856,25 +3871,25 @@
         <v>130</v>
       </c>
       <c r="B3" s="24">
-        <v>2.2000000000000002</v>
+        <v>3</v>
       </c>
       <c r="C3" s="24">
         <v>3.2</v>
       </c>
       <c r="D3" s="24">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="E3" s="28">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="F3" s="24">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="G3" s="24">
-        <v>6.5</v>
+        <v>4.8</v>
       </c>
       <c r="H3" s="16">
-        <v>3.1105941753361677</v>
+        <v>3.2770245523159325</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3882,25 +3897,25 @@
         <v>131</v>
       </c>
       <c r="B4" s="24">
-        <v>7.7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="24">
-        <v>8.1999999999999993</v>
+        <v>8</v>
       </c>
       <c r="D4" s="24">
-        <v>7.5</v>
+        <v>9.1</v>
       </c>
       <c r="E4" s="28">
-        <v>9.5</v>
+        <v>9.1</v>
       </c>
       <c r="F4" s="24">
-        <v>7.9</v>
+        <v>9</v>
       </c>
       <c r="G4" s="24">
-        <v>7.2</v>
+        <v>8.5</v>
       </c>
       <c r="H4" s="16">
-        <v>7.9041757123278877</v>
+        <v>8.5970086018116945</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3908,25 +3923,25 @@
         <v>132</v>
       </c>
       <c r="B5" s="24">
-        <v>7.8</v>
+        <v>9.4</v>
       </c>
       <c r="C5" s="24">
-        <v>10.1</v>
+        <v>10.6</v>
       </c>
       <c r="D5" s="24">
-        <v>16.3</v>
+        <v>8.9</v>
       </c>
       <c r="E5" s="28">
-        <v>9.3000000000000007</v>
+        <v>12.8</v>
       </c>
       <c r="F5" s="24">
+        <v>9.9</v>
+      </c>
+      <c r="G5" s="24">
         <v>6</v>
       </c>
-      <c r="G5" s="24">
-        <v>7.3</v>
-      </c>
       <c r="H5" s="16">
-        <v>9.1983357529325396</v>
+        <v>9.7566021424863703</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3934,25 +3949,25 @@
         <v>133</v>
       </c>
       <c r="B6" s="24">
+        <v>8.6</v>
+      </c>
+      <c r="C6" s="24">
         <v>9.4</v>
       </c>
-      <c r="C6" s="24">
-        <v>8.1999999999999993</v>
-      </c>
       <c r="D6" s="24">
-        <v>6.7</v>
+        <v>9.9</v>
       </c>
       <c r="E6" s="28">
-        <v>6.6</v>
+        <v>7.7</v>
       </c>
       <c r="F6" s="24">
-        <v>4.8</v>
+        <v>15</v>
       </c>
       <c r="G6" s="24">
-        <v>7.3</v>
+        <v>9.5</v>
       </c>
       <c r="H6" s="16">
-        <v>8.4496638740304562</v>
+        <v>8.9541242104737684</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3960,25 +3975,25 @@
         <v>134</v>
       </c>
       <c r="B7" s="24">
-        <v>8.6999999999999993</v>
+        <v>14</v>
       </c>
       <c r="C7" s="24">
-        <v>6.8</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="D7" s="24">
-        <v>6.5</v>
+        <v>18.3</v>
       </c>
       <c r="E7" s="28">
-        <v>6.3</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="F7" s="24">
-        <v>11.1</v>
+        <v>18.7</v>
       </c>
       <c r="G7" s="24">
-        <v>9.1</v>
+        <v>11.4</v>
       </c>
       <c r="H7" s="16">
-        <v>7.8585004044366746</v>
+        <v>15.238048089951196</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3986,25 +4001,25 @@
         <v>135</v>
       </c>
       <c r="B8" s="24">
-        <v>10.4</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C8" s="24">
-        <v>9.9</v>
+        <v>13.1</v>
       </c>
       <c r="D8" s="24">
-        <v>12.1</v>
+        <v>17.5</v>
       </c>
       <c r="E8" s="28">
-        <v>13</v>
+        <v>16.7</v>
       </c>
       <c r="F8" s="24">
-        <v>10.3</v>
+        <v>13.9</v>
       </c>
       <c r="G8" s="24">
-        <v>7.9</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="H8" s="16">
-        <v>10.263910333594129</v>
+        <v>11.849504137025724</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4012,25 +4027,25 @@
         <v>136</v>
       </c>
       <c r="B9" s="24">
-        <v>7.2</v>
+        <v>6.6</v>
       </c>
       <c r="C9" s="24">
-        <v>7.8</v>
+        <v>8.5</v>
       </c>
       <c r="D9" s="24">
-        <v>7.7</v>
+        <v>7</v>
       </c>
       <c r="E9" s="28">
-        <v>8.1999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="F9" s="24">
-        <v>8.8000000000000007</v>
+        <v>7.5</v>
       </c>
       <c r="G9" s="24">
-        <v>8.6999999999999993</v>
+        <v>7</v>
       </c>
       <c r="H9" s="16">
-        <v>7.6459621413905277</v>
+        <v>7.3444828516963323</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4038,25 +4053,25 @@
         <v>137</v>
       </c>
       <c r="B10" s="24">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="C10" s="24">
-        <v>8.1</v>
+        <v>7.6</v>
       </c>
       <c r="D10" s="24">
-        <v>5.6</v>
+        <v>6.3</v>
       </c>
       <c r="E10" s="28">
-        <v>3.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F10" s="24">
-        <v>8.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G10" s="24">
-        <v>9.4</v>
+        <v>6.3</v>
       </c>
       <c r="H10" s="16">
-        <v>6.8795584651099917</v>
+        <v>6.6520896902869664</v>
       </c>
     </row>
   </sheetData>
@@ -4069,9 +4084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4106,25 +4119,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="20">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="26">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="26">
-        <v>7.5</v>
+        <v>6.9</v>
       </c>
       <c r="E2" s="26">
-        <v>7.4</v>
+        <v>7.6</v>
       </c>
       <c r="F2" s="26">
-        <v>6.7</v>
+        <v>7.6</v>
       </c>
       <c r="G2" s="26">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="H2" s="20">
-        <v>8</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4132,25 +4145,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="19">
-        <v>6</v>
+        <v>7.1</v>
       </c>
       <c r="C3" s="25">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="D3" s="25">
-        <v>6.1</v>
+        <v>7.3</v>
       </c>
       <c r="E3" s="25">
-        <v>6.6</v>
+        <v>7.5</v>
       </c>
       <c r="F3" s="25">
-        <v>5.5</v>
+        <v>7.1</v>
       </c>
       <c r="G3" s="25">
-        <v>6</v>
+        <v>7.4</v>
       </c>
       <c r="H3" s="19">
-        <v>7.3</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4158,25 +4171,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="19">
-        <v>6.4</v>
+        <v>7</v>
       </c>
       <c r="C4" s="25">
+        <v>7.3</v>
+      </c>
+      <c r="D4" s="25">
+        <v>6.8</v>
+      </c>
+      <c r="E4" s="25">
         <v>6.5</v>
       </c>
-      <c r="D4" s="25">
-        <v>6.7</v>
-      </c>
-      <c r="E4" s="25">
-        <v>6.2</v>
-      </c>
       <c r="F4" s="25">
-        <v>6.1</v>
+        <v>6.9</v>
       </c>
       <c r="G4" s="25">
-        <v>5.9</v>
+        <v>6.6</v>
       </c>
       <c r="H4" s="19">
-        <v>5.3</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4184,25 +4197,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="19">
-        <v>8.5</v>
+        <v>9.9</v>
       </c>
       <c r="C5" s="25">
-        <v>7.4</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D5" s="25">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="E5" s="25">
-        <v>9.8000000000000007</v>
+        <v>10.6</v>
       </c>
       <c r="F5" s="25">
-        <v>10.1</v>
+        <v>11.7</v>
       </c>
       <c r="G5" s="25">
-        <v>9</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H5" s="19">
-        <v>11.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4210,25 +4223,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="19">
-        <v>4.5999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="C6" s="25">
-        <v>4.7</v>
+        <v>5.4</v>
       </c>
       <c r="D6" s="25">
-        <v>4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E6" s="25">
-        <v>5.5</v>
+        <v>7.9</v>
       </c>
       <c r="F6" s="25">
-        <v>4.5999999999999996</v>
+        <v>8.5</v>
       </c>
       <c r="G6" s="25">
-        <v>4.8</v>
+        <v>5.6</v>
       </c>
       <c r="H6" s="19">
-        <v>5.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4236,25 +4249,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="19">
-        <v>10.3</v>
+        <v>8.4</v>
       </c>
       <c r="C7" s="25">
-        <v>10.5</v>
+        <v>8.6</v>
       </c>
       <c r="D7" s="25">
-        <v>10.199999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="E7" s="25">
-        <v>11.2</v>
+        <v>8.6</v>
       </c>
       <c r="F7" s="25">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="G7" s="25">
-        <v>8.8000000000000007</v>
+        <v>8</v>
       </c>
       <c r="H7" s="19">
-        <v>11.2</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4262,25 +4275,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="19">
-        <v>6.8</v>
+        <v>5.7</v>
       </c>
       <c r="C8" s="25">
-        <v>7</v>
+        <v>6.3</v>
       </c>
       <c r="D8" s="25">
-        <v>7</v>
+        <v>5.3</v>
       </c>
       <c r="E8" s="25">
-        <v>6.7</v>
+        <v>5.3</v>
       </c>
       <c r="F8" s="25">
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G8" s="25">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="H8" s="19">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4288,25 +4301,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="19">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="C9" s="25">
-        <v>4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D9" s="25">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="E9" s="25">
-        <v>5.0999999999999996</v>
+        <v>7.8</v>
       </c>
       <c r="F9" s="25">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="G9" s="25">
-        <v>7.2</v>
+        <v>3.5</v>
       </c>
       <c r="H9" s="19">
-        <v>7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4314,25 +4327,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="19">
-        <v>5.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C10" s="25">
-        <v>4.7</v>
+        <v>4</v>
       </c>
       <c r="D10" s="25">
-        <v>6.1</v>
+        <v>3.8</v>
       </c>
       <c r="E10" s="25">
-        <v>6.7</v>
+        <v>3.5</v>
       </c>
       <c r="F10" s="25">
-        <v>6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G10" s="25">
-        <v>7.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H10" s="19">
-        <v>5.9</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4340,25 +4353,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="19">
-        <v>13.2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="25">
-        <v>13.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D11" s="25">
-        <v>14.3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="25">
-        <v>11.4</v>
+        <v>5.4</v>
       </c>
       <c r="F11" s="25">
-        <v>10.3</v>
+        <v>7.6</v>
       </c>
       <c r="G11" s="25">
-        <v>12.8</v>
+        <v>5.7</v>
       </c>
       <c r="H11" s="19">
-        <v>9.6999999999999993</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4366,25 +4379,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="19">
-        <v>6.1</v>
+        <v>5</v>
       </c>
       <c r="C12" s="25">
-        <v>7.9</v>
+        <v>3.8</v>
       </c>
       <c r="D12" s="25">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="E12" s="25">
-        <v>3.6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F12" s="25">
-        <v>4.4000000000000004</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G12" s="25">
-        <v>8.6</v>
+        <v>7.8</v>
       </c>
       <c r="H12" s="19">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4392,25 +4405,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="19">
-        <v>9.8000000000000007</v>
+        <v>6.7</v>
       </c>
       <c r="C13" s="25">
-        <v>11.3</v>
+        <v>6.2</v>
       </c>
       <c r="D13" s="25">
-        <v>8.8000000000000007</v>
+        <v>7.1</v>
       </c>
       <c r="E13" s="25">
-        <v>8.6</v>
+        <v>7.1</v>
       </c>
       <c r="F13" s="25">
+        <v>7.2</v>
+      </c>
+      <c r="G13" s="25">
         <v>6.8</v>
       </c>
-      <c r="G13" s="25">
-        <v>8.5</v>
-      </c>
       <c r="H13" s="19">
-        <v>10.3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4418,25 +4431,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="19">
-        <v>8.1</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C14" s="25">
         <v>8.1999999999999993</v>
       </c>
       <c r="D14" s="25">
-        <v>8.1</v>
+        <v>9.5</v>
       </c>
       <c r="E14" s="25">
-        <v>9.6999999999999993</v>
+        <v>9.5</v>
       </c>
       <c r="F14" s="25">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="G14" s="25">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="H14" s="19">
-        <v>7.3</v>
+        <v>8.4</v>
       </c>
     </row>
   </sheetData>
@@ -4449,9 +4462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4486,25 +4497,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="22">
-        <v>71</v>
+        <v>78.5</v>
       </c>
       <c r="C2" s="27">
-        <v>71.8</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="D2" s="27">
-        <v>69.900000000000006</v>
+        <v>77.7</v>
       </c>
       <c r="E2" s="27">
-        <v>72.2</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="F2" s="27">
-        <v>71.2</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="G2" s="27">
-        <v>69.7</v>
+        <v>77.5</v>
       </c>
       <c r="H2" s="27">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4512,25 +4523,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="21">
-        <v>70.599999999999994</v>
+        <v>80</v>
       </c>
       <c r="C3" s="17">
-        <v>70.7</v>
+        <v>79.8</v>
       </c>
       <c r="D3" s="17">
-        <v>69.599999999999994</v>
+        <v>79.7</v>
       </c>
       <c r="E3" s="17">
-        <v>73</v>
+        <v>82.4</v>
       </c>
       <c r="F3" s="17">
-        <v>71.7</v>
+        <v>81.3</v>
       </c>
       <c r="G3" s="17">
-        <v>69.5</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="H3" s="17">
-        <v>73.400000000000006</v>
+        <v>79.099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4538,25 +4549,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="21">
-        <v>61.2</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="C4" s="17">
-        <v>60.1</v>
+        <v>68.7</v>
       </c>
       <c r="D4" s="17">
-        <v>62.7</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E4" s="17">
-        <v>69.7</v>
+        <v>73.8</v>
       </c>
       <c r="F4" s="17">
-        <v>60.3</v>
+        <v>67.8</v>
       </c>
       <c r="G4" s="17">
-        <v>59.7</v>
+        <v>67.7</v>
       </c>
       <c r="H4" s="17">
-        <v>56.6</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4564,25 +4575,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="21">
-        <v>96.7</v>
+        <v>109</v>
       </c>
       <c r="C5" s="17">
-        <v>100.5</v>
+        <v>111.7</v>
       </c>
       <c r="D5" s="17">
-        <v>94.4</v>
+        <v>108.1</v>
       </c>
       <c r="E5" s="17">
-        <v>91.3</v>
+        <v>101.6</v>
       </c>
       <c r="F5" s="17">
-        <v>92.2</v>
+        <v>107.3</v>
       </c>
       <c r="G5" s="17">
-        <v>87.8</v>
+        <v>100.4</v>
       </c>
       <c r="H5" s="17">
-        <v>97.6</v>
+        <v>106.6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4590,25 +4601,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="21">
-        <v>50.3</v>
+        <v>56.8</v>
       </c>
       <c r="C6" s="17">
-        <v>52.4</v>
+        <v>56.2</v>
       </c>
       <c r="D6" s="17">
-        <v>43.8</v>
+        <v>52.5</v>
       </c>
       <c r="E6" s="17">
-        <v>66.5</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="F6" s="17">
-        <v>54.4</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="G6" s="17">
-        <v>44.8</v>
+        <v>56.9</v>
       </c>
       <c r="H6" s="17">
-        <v>58.5</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4616,25 +4627,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="21">
-        <v>70.7</v>
+        <v>79.2</v>
       </c>
       <c r="C7" s="17">
-        <v>71.900000000000006</v>
+        <v>81.2</v>
       </c>
       <c r="D7" s="17">
-        <v>70.400000000000006</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="E7" s="17">
-        <v>66.900000000000006</v>
+        <v>74.8</v>
       </c>
       <c r="F7" s="17">
-        <v>70.3</v>
+        <v>78.900000000000006</v>
       </c>
       <c r="G7" s="17">
-        <v>69.3</v>
+        <v>76.3</v>
       </c>
       <c r="H7" s="17">
-        <v>66.3</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4642,25 +4653,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="21">
-        <v>72.099999999999994</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="C8" s="17">
-        <v>76.400000000000006</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="D8" s="17">
+        <v>72.2</v>
+      </c>
+      <c r="E8" s="17">
+        <v>71</v>
+      </c>
+      <c r="F8" s="17">
+        <v>68</v>
+      </c>
+      <c r="G8" s="17">
+        <v>72</v>
+      </c>
+      <c r="H8" s="17">
         <v>69.900000000000006</v>
-      </c>
-      <c r="E8" s="17">
-        <v>68</v>
-      </c>
-      <c r="F8" s="17">
-        <v>65.099999999999994</v>
-      </c>
-      <c r="G8" s="17">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="H8" s="17">
-        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4668,25 +4679,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="21">
-        <v>63.9</v>
+        <v>71</v>
       </c>
       <c r="C9" s="17">
-        <v>59.1</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D9" s="17">
-        <v>67.8</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="E9" s="17">
-        <v>70.400000000000006</v>
+        <v>78.3</v>
       </c>
       <c r="F9" s="17">
-        <v>60.9</v>
+        <v>67.5</v>
       </c>
       <c r="G9" s="17">
-        <v>71.3</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="H9" s="17">
-        <v>67.3</v>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4694,25 +4705,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="21">
-        <v>35.5</v>
+        <v>41.8</v>
       </c>
       <c r="C10" s="17">
-        <v>33.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="D10" s="17">
-        <v>36.5</v>
+        <v>42.1</v>
       </c>
       <c r="E10" s="17">
-        <v>39.5</v>
+        <v>45.7</v>
       </c>
       <c r="F10" s="17">
-        <v>37.9</v>
+        <v>43.3</v>
       </c>
       <c r="G10" s="17">
-        <v>39.6</v>
+        <v>43.8</v>
       </c>
       <c r="H10" s="17">
-        <v>34</v>
+        <v>41.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4720,25 +4731,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="21">
-        <v>70</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="C11" s="17">
-        <v>71.8</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="D11" s="17">
-        <v>69.8</v>
+        <v>70.3</v>
       </c>
       <c r="E11" s="17">
-        <v>62.1</v>
+        <v>66</v>
       </c>
       <c r="F11" s="17">
-        <v>72.400000000000006</v>
+        <v>77</v>
       </c>
       <c r="G11" s="17">
-        <v>66.7</v>
+        <v>71.7</v>
       </c>
       <c r="H11" s="17">
-        <v>61.5</v>
+        <v>67.599999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4746,25 +4757,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="21">
-        <v>64.599999999999994</v>
+        <v>65.8</v>
       </c>
       <c r="C12" s="17">
-        <v>65.099999999999994</v>
+        <v>64.2</v>
       </c>
       <c r="D12" s="17">
-        <v>66.8</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="E12" s="17">
-        <v>56.7</v>
+        <v>61.6</v>
       </c>
       <c r="F12" s="17">
-        <v>54.2</v>
+        <v>51.9</v>
       </c>
       <c r="G12" s="17">
-        <v>65.5</v>
+        <v>75.3</v>
       </c>
       <c r="H12" s="17">
-        <v>68.2</v>
+        <v>73.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4772,25 +4783,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="21">
+        <v>97.5</v>
+      </c>
+      <c r="C13" s="17">
+        <v>102.8</v>
+      </c>
+      <c r="D13" s="17">
         <v>90.6</v>
       </c>
-      <c r="C13" s="17">
-        <v>94.9</v>
-      </c>
-      <c r="D13" s="17">
-        <v>85.4</v>
-      </c>
       <c r="E13" s="17">
-        <v>92.9</v>
+        <v>102.5</v>
       </c>
       <c r="F13" s="17">
-        <v>89.4</v>
+        <v>96.3</v>
       </c>
       <c r="G13" s="17">
-        <v>88.3</v>
+        <v>96.7</v>
       </c>
       <c r="H13" s="17">
-        <v>91.9</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4798,25 +4809,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="21">
-        <v>64.8</v>
+        <v>73.3</v>
       </c>
       <c r="C14" s="17">
-        <v>65.5</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="D14" s="17">
-        <v>62.7</v>
+        <v>72</v>
       </c>
       <c r="E14" s="17">
-        <v>66.400000000000006</v>
+        <v>76.2</v>
       </c>
       <c r="F14" s="17">
-        <v>68.8</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="G14" s="17">
-        <v>65</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="H14" s="17">
-        <v>65.099999999999994</v>
+        <v>72.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo dato PIB 2T 2022"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C32334C-DEF5-4358-855E-F1D4276ADFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3FE1F3-ED03-4CA1-891C-92EE82ECAD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="218">
   <si>
     <t>Período</t>
   </si>
@@ -2464,9 +2464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2490,10 +2488,10 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>571371.42621766892</v>
+        <v>644818.80193734274</v>
       </c>
       <c r="C2">
-        <v>6.021578205340461</v>
+        <v>6.6210290853380798</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2501,10 +2499,10 @@
         <v>102</v>
       </c>
       <c r="B3">
-        <v>39792.671747015345</v>
+        <v>84508.536911229836</v>
       </c>
       <c r="C3">
-        <v>-0.12132037450698352</v>
+        <v>-5.2284200767613669</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2512,10 +2510,10 @@
         <v>103</v>
       </c>
       <c r="B4">
-        <v>1621.5132086953849</v>
+        <v>2803.8809597629624</v>
       </c>
       <c r="C4">
-        <v>-3.5279456750018534</v>
+        <v>24.121911238365911</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2523,10 +2521,10 @@
         <v>104</v>
       </c>
       <c r="B5">
-        <v>22656.313905916188</v>
+        <v>23988.049228966476</v>
       </c>
       <c r="C5">
-        <v>13.400317766955405</v>
+        <v>15.455171845229259</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2534,10 +2532,10 @@
         <v>105</v>
       </c>
       <c r="B6">
-        <v>108992.72916716749</v>
+        <v>125030.84005626102</v>
       </c>
       <c r="C6">
-        <v>4.8600348747123823</v>
+        <v>7.6582005417364059</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2545,10 +2543,10 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <v>12942.275374307999</v>
+        <v>13357.03357278303</v>
       </c>
       <c r="C7">
-        <v>5.1476925583904265</v>
+        <v>4.8661425735229784</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2556,10 +2554,10 @@
         <v>107</v>
       </c>
       <c r="B8">
-        <v>22467.323062496853</v>
+        <v>20926.460098286607</v>
       </c>
       <c r="C8">
-        <v>2.9756526723262899</v>
+        <v>9.9177971809852892</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2567,10 +2565,10 @@
         <v>108</v>
       </c>
       <c r="B9">
-        <v>90190.059665927343</v>
+        <v>99050.868361418325</v>
       </c>
       <c r="C9">
-        <v>5.660398988406512</v>
+        <v>9.6644054198416143</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2578,10 +2576,10 @@
         <v>109</v>
       </c>
       <c r="B10">
-        <v>9300.2054422241108</v>
+        <v>8605.1734059229329</v>
       </c>
       <c r="C10">
-        <v>33.565103502550819</v>
+        <v>53.937982935729877</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2589,10 +2587,10 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>53261.090320404044</v>
+        <v>58863.534191324492</v>
       </c>
       <c r="C11">
-        <v>12.22725949424488</v>
+        <v>11.462822586038698</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2600,10 +2598,10 @@
         <v>111</v>
       </c>
       <c r="B12">
-        <v>25570.829166259125</v>
+        <v>25026.616863292602</v>
       </c>
       <c r="C12">
-        <v>1.2523958518309453</v>
+        <v>2.0010111212931179</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2611,10 +2609,10 @@
         <v>112</v>
       </c>
       <c r="B13">
-        <v>77865.228139844723</v>
+        <v>80068.369728395061</v>
       </c>
       <c r="C13">
-        <v>5.0092778689776685</v>
+        <v>6.3803492775227397</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2622,10 +2620,10 @@
         <v>113</v>
       </c>
       <c r="B14">
-        <v>34914.496460771283</v>
+        <v>35036.769725331389</v>
       </c>
       <c r="C14">
-        <v>9.4595469169590061</v>
+        <v>10.153457492304568</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2633,10 +2631,10 @@
         <v>114</v>
       </c>
       <c r="B15">
-        <v>27768.387873531781</v>
+        <v>28219.35604362089</v>
       </c>
       <c r="C15">
-        <v>4.8792692299016949</v>
+        <v>6.0944271712824616</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2644,10 +2642,10 @@
         <v>115</v>
       </c>
       <c r="B16">
-        <v>23390.182227267425</v>
+        <v>22412.972859499903</v>
       </c>
       <c r="C16">
-        <v>2.8213605132321629</v>
+        <v>1.0149697709420167</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2655,10 +2653,10 @@
         <v>116</v>
       </c>
       <c r="B17">
-        <v>16511.100936225932</v>
+        <v>13200.261286340125</v>
       </c>
       <c r="C17">
-        <v>7.8415677899741576</v>
+        <v>8.5935478547673796</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2666,10 +2664,10 @@
         <v>117</v>
       </c>
       <c r="B18">
-        <v>4127.0195196139048</v>
+        <v>3720.0786449073389</v>
       </c>
       <c r="C18">
-        <v>10.54034588475834</v>
+        <v>9.9078855195906499</v>
       </c>
     </row>
   </sheetData>
@@ -3807,7 +3805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4838,9 +4836,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4869,7 +4869,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="11">
-        <v>475454.37399644504</v>
+        <v>475371.05098936806</v>
       </c>
       <c r="D2" s="11">
         <v>460369.44223294902</v>
@@ -4883,7 +4883,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="11">
-        <v>470205.76579705958</v>
+        <v>470350.62814756762</v>
       </c>
       <c r="D3" s="11">
         <v>514395.68177236198</v>
@@ -4897,7 +4897,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="11">
-        <v>493835.75466103636</v>
+        <v>494069.95695165993</v>
       </c>
       <c r="D4" s="11">
         <v>481151.97994350799</v>
@@ -4911,7 +4911,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="11">
-        <v>500964.88610719389</v>
+        <v>500669.14453385782</v>
       </c>
       <c r="D5" s="11">
         <v>484543.67687656201</v>
@@ -4925,7 +4925,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="11">
-        <v>515453.44834923226</v>
+        <v>515257.73564929306</v>
       </c>
       <c r="D6" s="11">
         <v>493602.53057785501</v>
@@ -4939,7 +4939,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="11">
-        <v>526221.6289373528</v>
+        <v>526471.33379984985</v>
       </c>
       <c r="D7" s="11">
         <v>581668.24987960199</v>
@@ -4953,7 +4953,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="11">
-        <v>530094.33357569715</v>
+        <v>530356.53122616687</v>
       </c>
       <c r="D8" s="11">
         <v>514697.78950542799</v>
@@ -4967,7 +4967,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="11">
-        <v>540454.35915137373</v>
+        <v>540138.16933834716</v>
       </c>
       <c r="D9" s="11">
         <v>522255.20005077199</v>
@@ -4981,7 +4981,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="11">
-        <v>554411.83501684235</v>
+        <v>554320.72005646233</v>
       </c>
       <c r="D10" s="11">
         <v>532348.21201691695</v>
@@ -4995,7 +4995,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="11">
-        <v>561221.28776810062</v>
+        <v>561467.19958498655</v>
       </c>
       <c r="D11" s="11">
         <v>614076.39260854397</v>
@@ -5009,7 +5009,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="11">
-        <v>577070.94766772434</v>
+        <v>577137.74961009074</v>
       </c>
       <c r="D12" s="11">
         <v>562978.96562687703</v>
@@ -5023,7 +5023,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="11">
-        <v>589493.54643025738</v>
+        <v>589271.94763138681</v>
       </c>
       <c r="D13" s="11">
         <v>572794.04663058801</v>
@@ -5037,7 +5037,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="11">
-        <v>602984.88460172631</v>
+        <v>603167.9720340278</v>
       </c>
       <c r="D14" s="11">
         <v>576846.88569942699</v>
@@ -5051,7 +5051,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="11">
-        <v>616261.92272166093</v>
+        <v>616315.46326810063</v>
       </c>
       <c r="D15" s="11">
         <v>674620.563006485</v>
@@ -5065,7 +5065,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="11">
-        <v>624759.56800488278</v>
+        <v>624561.79784678563</v>
       </c>
       <c r="D16" s="11">
         <v>610425.69401485403</v>
@@ -5079,7 +5079,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="11">
-        <v>643763.635256093</v>
+        <v>643724.7774354479</v>
       </c>
       <c r="D17" s="11">
         <v>625876.867863597</v>
@@ -5093,7 +5093,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="11">
-        <v>649419.96757048008</v>
+        <v>649805.62972759677</v>
       </c>
       <c r="D18" s="11">
         <v>616720.35706447798</v>
@@ -5107,7 +5107,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="11">
-        <v>653269.79330575257</v>
+        <v>653132.8277707044</v>
       </c>
       <c r="D19" s="11">
         <v>711405.50045523304</v>
@@ -5121,7 +5121,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="11">
-        <v>658718.83632044296</v>
+        <v>658216.30872340978</v>
       </c>
       <c r="D20" s="11">
         <v>647087.95974249404</v>
@@ -5135,7 +5135,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="11">
-        <v>627296.04176817276</v>
+        <v>627549.87274313683</v>
       </c>
       <c r="D21" s="11">
         <v>613490.82170264097</v>
@@ -5149,7 +5149,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="11">
-        <v>604047.70825217164</v>
+        <v>604485.7968595376</v>
       </c>
       <c r="D22" s="11">
         <v>578553.04424240498</v>
@@ -5163,7 +5163,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="11">
-        <v>591229.33407328476</v>
+        <v>590846.68514454551</v>
       </c>
       <c r="D23" s="11">
         <v>631197.75186006899</v>
@@ -5177,7 +5177,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="11">
-        <v>614472.04676489066</v>
+        <v>614199.09600853221</v>
       </c>
       <c r="D24" s="11">
         <v>610519.85461172694</v>
@@ -5191,7 +5191,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="11">
-        <v>625742.41656115034</v>
+        <v>625959.92763888137</v>
       </c>
       <c r="D25" s="11">
         <v>615220.85493729694</v>
@@ -5205,7 +5205,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="11">
-        <v>644430.22641792509</v>
+        <v>644757.43782605673</v>
       </c>
       <c r="D26" s="11">
         <v>611607.33658973</v>
@@ -5219,7 +5219,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="11">
-        <v>673775.07951578847</v>
+        <v>673364.27754086838</v>
       </c>
       <c r="D27" s="11">
         <v>733730.773968903</v>
@@ -5233,7 +5233,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="11">
-        <v>677399.28333924874</v>
+        <v>677402.2266857496</v>
       </c>
       <c r="D28" s="11">
         <v>668566.50948898599</v>
@@ -5247,7 +5247,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="11">
-        <v>686490.12849423185</v>
+        <v>686570.77571451815</v>
       </c>
       <c r="D29" s="11">
         <v>668190.097719574</v>
@@ -5261,7 +5261,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="11">
-        <v>702723.80414944305</v>
+        <v>702649.90013330383</v>
       </c>
       <c r="D30" s="11">
         <v>662325.58597269503</v>
@@ -5275,7 +5275,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="11">
-        <v>709454.40590443229</v>
+        <v>709545.37355450576</v>
       </c>
       <c r="D31" s="11">
         <v>766332.95457161299</v>
@@ -5289,7 +5289,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="11">
-        <v>715220.06375098636</v>
+        <v>715423.01836901845</v>
       </c>
       <c r="D32" s="11">
         <v>711417.39193010505</v>
@@ -5303,7 +5303,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="11">
-        <v>715728.11507754482</v>
+        <v>715508.09682557906</v>
       </c>
       <c r="D33" s="11">
         <v>703050.45640799298</v>
@@ -5317,7 +5317,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="11">
-        <v>707811.87377429125</v>
+        <v>707750.20169942803</v>
       </c>
       <c r="D34" s="11">
         <v>672685.993630504</v>
@@ -5331,7 +5331,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="11">
-        <v>683648.87101095053</v>
+        <v>683979.57443022332</v>
       </c>
       <c r="D35" s="11">
         <v>730838.27259277599</v>
@@ -5345,7 +5345,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="11">
-        <v>705234.08314859425</v>
+        <v>705076.19439545553</v>
       </c>
       <c r="D36" s="11">
         <v>703461.65253019601</v>
@@ -5359,7 +5359,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="11">
-        <v>717249.12990196224</v>
+        <v>717137.98731069011</v>
       </c>
       <c r="D37" s="11">
         <v>706958.03908231901</v>
@@ -5373,7 +5373,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="11">
-        <v>717125.64588613005</v>
+        <v>716939.43149499106</v>
       </c>
       <c r="D38" s="11">
         <v>677085.52917315101</v>
@@ -5387,7 +5387,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="11">
-        <v>720802.56315849815</v>
+        <v>721269.52188036207</v>
       </c>
       <c r="D39" s="11">
         <v>776486.60279942001</v>
@@ -5401,7 +5401,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="11">
-        <v>725454.40232530748</v>
+        <v>725157.65159980964</v>
       </c>
       <c r="D40" s="11">
         <v>721458.94421618199</v>
@@ -5415,7 +5415,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="11">
-        <v>718245.80984132516</v>
+        <v>718261.81623609748</v>
       </c>
       <c r="D41" s="11">
         <v>706597.34502250701</v>
@@ -5429,7 +5429,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="11">
-        <v>707336.25313466752</v>
+        <v>707546.06498329213</v>
       </c>
       <c r="D42" s="11">
         <v>671066.04663506302</v>
@@ -5443,7 +5443,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="11">
-        <v>703266.1910445746</v>
+        <v>703282.00621111901</v>
       </c>
       <c r="D43" s="11">
         <v>760576.86834800395</v>
@@ -5457,7 +5457,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="11">
-        <v>697512.23532424343</v>
+        <v>697224.55344559671</v>
       </c>
       <c r="D44" s="11">
         <v>690879.79825168301</v>
@@ -5471,7 +5471,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="11">
-        <v>701109.50434997655</v>
+        <v>701171.5592134539</v>
       </c>
       <c r="D45" s="11">
         <v>686701.47061871097</v>
@@ -5485,7 +5485,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="11">
-        <v>711258.38599491504</v>
+        <v>711516.17676598986</v>
       </c>
       <c r="D46" s="11">
         <v>672749.81139169901</v>
@@ -5499,7 +5499,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="11">
-        <v>727839.99863887194</v>
+        <v>727627.86383100448</v>
       </c>
       <c r="D47" s="11">
         <v>791235.96554166998</v>
@@ -5513,7 +5513,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="11">
-        <v>727481.57076581276</v>
+        <v>727531.67644959386</v>
       </c>
       <c r="D48" s="11">
         <v>718281.26544978202</v>
@@ -5527,7 +5527,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="11">
-        <v>719368.63115256047</v>
+        <v>719272.8695055719</v>
       </c>
       <c r="D49" s="11">
         <v>703681.54416900803</v>
@@ -5541,7 +5541,7 @@
         <v>29</v>
       </c>
       <c r="C50" s="11">
-        <v>712640.06153844751</v>
+        <v>712956.4362341261</v>
       </c>
       <c r="D50" s="11">
         <v>677652.08911570301</v>
@@ -5556,7 +5556,7 @@
         <v>30</v>
       </c>
       <c r="C51" s="11">
-        <v>701370.99166469392</v>
+        <v>701050.55126605951</v>
       </c>
       <c r="D51" s="11">
         <v>760703.28015165601</v>
@@ -5571,7 +5571,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="11">
-        <v>703724.32076925179</v>
+        <v>703949.96989883191</v>
       </c>
       <c r="D52" s="11">
         <v>694382.47577623103</v>
@@ -5586,7 +5586,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="11">
-        <v>708176.02041825175</v>
+        <v>707954.43699162884</v>
       </c>
       <c r="D53" s="11">
         <v>693173.54934705805</v>
@@ -5601,7 +5601,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="11">
-        <v>714233.72694170265</v>
+        <v>714425.3181707114</v>
       </c>
       <c r="D54" s="11">
         <v>681444.76611022197</v>
@@ -5616,7 +5616,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="11">
-        <v>722090.59875214146</v>
+        <v>721952.60422123875</v>
       </c>
       <c r="D55" s="11">
         <v>778401.67644931702</v>
@@ -5631,7 +5631,7 @@
         <v>31</v>
       </c>
       <c r="C56" s="11">
-        <v>730682.64569057734</v>
+        <v>731110.36115767376</v>
       </c>
       <c r="D56" s="11">
         <v>721120.42685279401</v>
@@ -5646,7 +5646,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="11">
-        <v>738552.81966687483</v>
+        <v>738071.50750167179</v>
       </c>
       <c r="D57" s="11">
         <v>724592.92163896305</v>
@@ -5661,7 +5661,7 @@
         <v>29</v>
       </c>
       <c r="C58" s="11">
-        <v>735783.7993534999</v>
+        <v>735750.72130254249</v>
       </c>
       <c r="D58" s="11">
         <v>707324.26805721398</v>
@@ -5677,7 +5677,7 @@
         <v>30</v>
       </c>
       <c r="C59" s="11">
-        <v>702155.70474938827</v>
+        <v>702484.9729966335</v>
       </c>
       <c r="D59" s="11">
         <v>747428.29995457502</v>
@@ -5693,7 +5693,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="11">
-        <v>700519.99386328529</v>
+        <v>700839.69810909347</v>
       </c>
       <c r="D60" s="11">
         <v>696101.58352180803</v>
@@ -5709,7 +5709,7 @@
         <v>32</v>
       </c>
       <c r="C61" s="11">
-        <v>691050.27395187633</v>
+        <v>690434.37950978254</v>
       </c>
       <c r="D61" s="11">
         <v>678655.62038445403</v>
@@ -5725,7 +5725,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="11">
-        <v>691187.80785437603</v>
+        <v>691050.55900471541</v>
       </c>
       <c r="D62">
         <v>665848.71529970889</v>
@@ -5741,7 +5741,7 @@
         <v>30</v>
       </c>
       <c r="C63" s="11">
-        <v>696112.6913947385</v>
+        <v>697044.80835807486</v>
       </c>
       <c r="D63">
         <v>751784.46077713254</v>
@@ -5757,7 +5757,7 @@
         <v>31</v>
       </c>
       <c r="C64" s="11">
-        <v>698265.65536115842</v>
+        <v>698289.3802768162</v>
       </c>
       <c r="D64">
         <v>683900.89855257841</v>
@@ -5773,7 +5773,7 @@
         <v>32</v>
       </c>
       <c r="C65" s="11">
-        <v>687329.05974156479</v>
+        <v>686510.4667122321</v>
       </c>
       <c r="D65">
         <v>671361.13972242002</v>
@@ -5789,7 +5789,7 @@
         <v>29</v>
       </c>
       <c r="C66" s="10">
-        <v>657711.75186022639</v>
+        <v>657531.48587817268</v>
       </c>
       <c r="D66" s="10">
         <v>632733.36598162609</v>
@@ -5804,7 +5804,7 @@
         <v>30</v>
       </c>
       <c r="C67" s="10">
-        <v>558526.02320056118</v>
+        <v>559875.23583740985</v>
       </c>
       <c r="D67" s="10">
         <v>608450.80405697017</v>
@@ -5819,7 +5819,7 @@
         <v>31</v>
       </c>
       <c r="C68" s="10">
-        <v>626583.75934842485</v>
+        <v>626566.37454888062</v>
       </c>
       <c r="D68" s="10">
         <v>614335.69211847626</v>
@@ -5834,7 +5834,7 @@
         <v>32</v>
       </c>
       <c r="C69" s="10">
-        <v>654358.18872116203</v>
+        <v>653206.62686591013</v>
       </c>
       <c r="D69" s="10">
         <v>641659.86097329983</v>
@@ -5849,7 +5849,7 @@
         <v>29</v>
       </c>
       <c r="C70" s="10">
-        <v>676335.19401415577</v>
+        <v>676500.63372803852</v>
       </c>
       <c r="D70">
         <v>652563.11939207092</v>
@@ -5864,7 +5864,7 @@
         <v>30</v>
       </c>
       <c r="C71" s="10">
-        <v>670924.73554681102</v>
+        <v>672322.29744675709</v>
       </c>
       <c r="D71">
         <v>718843.1229160385</v>
@@ -5879,7 +5879,7 @@
         <v>31</v>
       </c>
       <c r="C72" s="10">
-        <v>698323.59708729805</v>
+        <v>698313.42888155917</v>
       </c>
       <c r="D72" s="10">
         <v>686778.32722188451</v>
@@ -5893,7 +5893,7 @@
         <v>32</v>
       </c>
       <c r="C73" s="10">
-        <v>711259.17185327853</v>
+        <v>709706.3381650534</v>
       </c>
       <c r="D73" s="10">
         <v>698658.13099747989</v>
@@ -5907,10 +5907,24 @@
         <v>29</v>
       </c>
       <c r="C74" s="10">
-        <v>717474.48191855289</v>
-      </c>
-      <c r="D74" s="10">
-        <v>691652.1861622748</v>
+        <v>718073.46755277982</v>
+      </c>
+      <c r="D74">
+        <v>691638.23860468564</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="10">
+        <v>725560.2452796225</v>
+      </c>
+      <c r="D75">
+        <v>768729.05175870494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo dato de pobreza y emae"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB6C69-CCE1-490E-8006-55DFB46D332E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ACCD68-1B83-4542-B442-9654AD125055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -2678,9 +2678,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2711,10 +2713,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="17">
-        <v>148.19399519468166</v>
+        <v>148.210530835908</v>
       </c>
       <c r="D2" s="17">
-        <v>147.04742541927328</v>
+        <v>147.05231862427431</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2725,10 +2727,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="17">
-        <v>146.81397122412966</v>
+        <v>146.78256626719059</v>
       </c>
       <c r="D3" s="17">
-        <v>146.45365635177828</v>
+        <v>146.45848210114823</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2739,10 +2741,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="17">
-        <v>145.88784822904563</v>
+        <v>145.90616353882791</v>
       </c>
       <c r="D4" s="17">
-        <v>145.89749213216714</v>
+        <v>145.90247897308097</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2753,10 +2755,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="17">
-        <v>145.18828797508394</v>
+        <v>145.16894932834771</v>
       </c>
       <c r="D5" s="17">
-        <v>145.41576636757688</v>
+        <v>145.42107596828717</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,10 +2769,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="17">
-        <v>144.20588500627795</v>
+        <v>144.20919307915884</v>
       </c>
       <c r="D6" s="17">
-        <v>145.03564691182461</v>
+        <v>145.04135842744415</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2781,10 +2783,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="17">
-        <v>144.16155834762102</v>
+        <v>144.15840206702532</v>
       </c>
       <c r="D7" s="17">
-        <v>144.77707404936973</v>
+        <v>144.78323652099661</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2795,10 +2797,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="17">
-        <v>144.43088123474598</v>
+        <v>144.42926472809444</v>
       </c>
       <c r="D8" s="17">
-        <v>144.64984601663292</v>
+        <v>144.65636014434924</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2809,10 +2811,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="17">
-        <v>145.71455737784876</v>
+        <v>145.70436143421969</v>
       </c>
       <c r="D9" s="17">
-        <v>144.65771146667788</v>
+        <v>144.66428189378348</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2823,10 +2825,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="17">
-        <v>145.1963172242188</v>
+        <v>145.19594726393498</v>
       </c>
       <c r="D10" s="17">
-        <v>144.79959947914887</v>
+        <v>144.80589673644309</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2837,10 +2839,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="17">
-        <v>145.12034229842783</v>
+        <v>145.12759174049862</v>
       </c>
       <c r="D11" s="17">
-        <v>145.06557896670319</v>
+        <v>145.07119453962363</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2851,10 +2853,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="17">
-        <v>145.65166376855396</v>
+        <v>145.65094451754513</v>
       </c>
       <c r="D12" s="17">
-        <v>145.43951144660105</v>
+        <v>145.44399345153977</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2865,10 +2867,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="17">
-        <v>147.00604586361604</v>
+        <v>147.02743893800587</v>
       </c>
       <c r="D13" s="17">
-        <v>145.90701524530635</v>
+        <v>145.90999092907316</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2879,10 +2881,10 @@
         <v>136.63265948314879</v>
       </c>
       <c r="C14" s="17">
-        <v>147.40053386138243</v>
+        <v>147.41384671523994</v>
       </c>
       <c r="D14" s="17">
-        <v>146.45064815910783</v>
+        <v>146.45186086781152</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2893,10 +2895,10 @@
         <v>132.15851633981717</v>
       </c>
       <c r="C15" s="17">
-        <v>146.54848932783884</v>
+        <v>146.52974575935971</v>
       </c>
       <c r="D15" s="17">
-        <v>147.05237750941785</v>
+        <v>147.05174628269174</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,10 +2909,10 @@
         <v>152.62095855907629</v>
       </c>
       <c r="C16" s="17">
-        <v>147.85828170805226</v>
+        <v>147.86403917977194</v>
       </c>
       <c r="D16" s="17">
-        <v>147.69255372585548</v>
+        <v>147.6901602547706</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2921,10 +2923,10 @@
         <v>151.94634480454772</v>
       </c>
       <c r="C17" s="17">
-        <v>147.79452976818141</v>
+        <v>147.79224128542739</v>
       </c>
       <c r="D17" s="17">
-        <v>148.34894916699983</v>
+        <v>148.34496512861409</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2935,10 +2937,10 @@
         <v>168.38920946939328</v>
       </c>
       <c r="C18" s="17">
-        <v>148.53126255307458</v>
+        <v>148.52576183435193</v>
       </c>
       <c r="D18" s="17">
-        <v>148.99337893258618</v>
+        <v>148.98833831031766</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2949,10 +2951,10 @@
         <v>161.03568546936668</v>
       </c>
       <c r="C19" s="17">
-        <v>150.1554962201655</v>
+        <v>150.14457613819343</v>
       </c>
       <c r="D19" s="17">
-        <v>149.59327877116431</v>
+        <v>149.58798577192454</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2963,10 +2965,10 @@
         <v>150.30605012364694</v>
       </c>
       <c r="C20" s="17">
-        <v>150.38376914393635</v>
+        <v>150.37813098487408</v>
       </c>
       <c r="D20" s="17">
-        <v>150.11519536209403</v>
+        <v>150.11050805481636</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2977,10 +2979,10 @@
         <v>149.25534277372603</v>
       </c>
       <c r="C21" s="17">
-        <v>150.41794443121492</v>
+        <v>150.40919723594126</v>
       </c>
       <c r="D21" s="17">
-        <v>150.52474397586704</v>
+        <v>150.52142384501033</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2991,10 +2993,10 @@
         <v>146.38655965814218</v>
       </c>
       <c r="C22" s="17">
-        <v>151.34596062955143</v>
+        <v>151.33849784609299</v>
       </c>
       <c r="D22" s="17">
-        <v>150.78843668263713</v>
+        <v>150.78699452839317</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,13 +3004,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="17">
-        <v>149.38594966725159</v>
+        <v>149.38594966725168</v>
       </c>
       <c r="C23" s="17">
-        <v>151.55031321950116</v>
+        <v>151.54706853750281</v>
       </c>
       <c r="D23" s="17">
-        <v>150.8807945405033</v>
+        <v>150.88147303289679</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3016,13 +3018,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="17">
-        <v>151.92604285254842</v>
+        <v>151.92604285254845</v>
       </c>
       <c r="C24" s="17">
-        <v>152.48270975457359</v>
+        <v>152.50179371975429</v>
       </c>
       <c r="D24" s="17">
-        <v>150.78195145479671</v>
+        <v>150.78478400019193</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3030,13 +3032,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="17">
-        <v>146.78338490746611</v>
+        <v>146.78338490746603</v>
       </c>
       <c r="C25" s="17">
-        <v>152.35741368451031</v>
+        <v>152.38180505983806</v>
       </c>
       <c r="D25" s="17">
-        <v>150.48395387254996</v>
+        <v>150.48876372997961</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3044,13 +3046,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="17">
-        <v>142.74091260056963</v>
+        <v>142.74091260056943</v>
       </c>
       <c r="C26" s="17">
-        <v>151.91901037393694</v>
+        <v>151.93019742381182</v>
       </c>
       <c r="D26" s="17">
-        <v>149.99416486219715</v>
+        <v>150.00056494409171</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3058,13 +3060,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="17">
-        <v>138.81804034929576</v>
+        <v>138.81804034929567</v>
       </c>
       <c r="C27" s="17">
-        <v>151.91317414824795</v>
+        <v>151.90927032801707</v>
       </c>
       <c r="D27" s="17">
-        <v>149.33480665374671</v>
+        <v>149.34220140345181</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3072,13 +3074,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="17">
-        <v>155.85731954373409</v>
+        <v>155.85731954373438</v>
       </c>
       <c r="C28" s="17">
-        <v>151.14120608995214</v>
+        <v>151.1560025920725</v>
       </c>
       <c r="D28" s="17">
-        <v>148.53958265926696</v>
+        <v>148.54734557019884</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3086,13 +3088,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="17">
-        <v>151.5245440093189</v>
+        <v>151.52454400931981</v>
       </c>
       <c r="C29" s="17">
-        <v>146.86849550364391</v>
+        <v>146.8599394529447</v>
       </c>
       <c r="D29" s="17">
-        <v>147.65395579087703</v>
+        <v>147.66160208885702</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3100,13 +3102,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="17">
-        <v>159.56669238861335</v>
+        <v>159.56669238861375</v>
       </c>
       <c r="C30" s="17">
-        <v>144.45067500291245</v>
+        <v>144.44474334257279</v>
       </c>
       <c r="D30" s="17">
-        <v>146.73010949112233</v>
+        <v>146.73747868274978</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3114,13 +3116,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="17">
-        <v>151.12576319738318</v>
+        <v>151.1257631973819</v>
       </c>
       <c r="C31" s="17">
-        <v>143.15277953253354</v>
+        <v>143.11892216170332</v>
       </c>
       <c r="D31" s="17">
-        <v>145.82212361066911</v>
+        <v>145.82924059227929</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3128,13 +3130,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="17">
-        <v>145.96352431507398</v>
+        <v>145.96352431506975</v>
       </c>
       <c r="C32" s="17">
-        <v>143.3369687850207</v>
+        <v>143.33785850231715</v>
       </c>
       <c r="D32" s="17">
-        <v>144.97937849094581</v>
+        <v>144.9863997321296</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,13 +3144,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="17">
-        <v>146.7659599856924</v>
+        <v>146.76595998569064</v>
       </c>
       <c r="C33" s="17">
-        <v>146.74635500105839</v>
+        <v>146.7186790417806</v>
       </c>
       <c r="D33" s="17">
-        <v>144.2465525511075</v>
+        <v>144.25375734689635</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3156,13 +3158,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="17">
-        <v>137.74656988202611</v>
+        <v>137.74656988203205</v>
       </c>
       <c r="C34" s="17">
-        <v>143.35276542087391</v>
+        <v>143.34961326781749</v>
       </c>
       <c r="D34" s="17">
-        <v>143.6544245829443</v>
+        <v>143.66209750607391</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3170,13 +3172,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="17">
-        <v>142.84327650511301</v>
+        <v>142.84327650513197</v>
       </c>
       <c r="C35" s="17">
-        <v>143.61355024927431</v>
+        <v>143.60184663648772</v>
       </c>
       <c r="D35" s="17">
-        <v>143.21745977128055</v>
+        <v>143.22564871078882</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3184,13 +3186,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="17">
-        <v>140.59240754476389</v>
+        <v>140.59240754477185</v>
       </c>
       <c r="C36" s="17">
-        <v>141.52612954236511</v>
+        <v>141.56397902586735</v>
       </c>
       <c r="D36" s="17">
-        <v>142.93749617417146</v>
+        <v>142.94605555883766</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3198,13 +3200,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="17">
-        <v>136.25161522908289</v>
+        <v>136.25161522905591</v>
       </c>
       <c r="C37" s="17">
-        <v>141.77551608964791</v>
+        <v>141.80557395857406</v>
       </c>
       <c r="D37" s="17">
-        <v>142.80212082585496</v>
+        <v>142.81071394292243</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,13 +3214,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="17">
-        <v>134.53623749903608</v>
+        <v>134.53623749895024</v>
       </c>
       <c r="C38" s="17">
-        <v>142.83037263883872</v>
+        <v>142.84438244513083</v>
       </c>
       <c r="D38" s="17">
-        <v>142.78556322242153</v>
+        <v>142.79369250348179</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3226,13 +3228,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="17">
-        <v>132.26788761890015</v>
+        <v>132.26788761886397</v>
       </c>
       <c r="C39" s="17">
-        <v>143.28421382141238</v>
+        <v>143.28573419617641</v>
       </c>
       <c r="D39" s="17">
-        <v>142.85048826758262</v>
+        <v>142.85781954205314</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3240,13 +3242,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="17">
-        <v>144.96325830724541</v>
+        <v>144.96325830736751</v>
       </c>
       <c r="C40" s="17">
-        <v>141.2360390172411</v>
+        <v>141.2223344295154</v>
       </c>
       <c r="D40" s="17">
-        <v>142.95654174673925</v>
+        <v>142.96277044608519</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3254,13 +3256,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="17">
-        <v>149.91623208186112</v>
+        <v>149.91623208225008</v>
       </c>
       <c r="C41" s="17">
-        <v>142.474106212664</v>
+        <v>142.47158878360182</v>
       </c>
       <c r="D41" s="17">
-        <v>143.06248855972845</v>
+        <v>143.0674049043308</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3268,13 +3270,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="17">
-        <v>164.13570357721557</v>
+        <v>164.13570357737953</v>
       </c>
       <c r="C42" s="17">
-        <v>144.75343902467932</v>
+        <v>144.70866060699998</v>
       </c>
       <c r="D42" s="17">
-        <v>143.13076952688564</v>
+        <v>143.13412583585591</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3282,13 +3284,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="17">
-        <v>150.85895656149751</v>
+        <v>150.85895656094456</v>
       </c>
       <c r="C43" s="17">
-        <v>143.88694166769642</v>
+        <v>143.87910433750196</v>
       </c>
       <c r="D43" s="17">
-        <v>143.12555065767182</v>
+        <v>143.12767745193639</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3296,13 +3298,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="17">
-        <v>146.77698127562269</v>
+        <v>146.77698127386105</v>
       </c>
       <c r="C44" s="17">
-        <v>145.57014711082331</v>
+        <v>145.59575841359464</v>
       </c>
       <c r="D44" s="17">
-        <v>143.01761658124238</v>
+        <v>143.01955888375289</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3310,13 +3312,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="17">
-        <v>141.27691429352492</v>
+        <v>141.27691429278232</v>
       </c>
       <c r="C45" s="17">
-        <v>145.06036743937511</v>
+        <v>145.03588691355861</v>
       </c>
       <c r="D45" s="17">
-        <v>142.78610658316927</v>
+        <v>142.7898692469318</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3324,13 +3326,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="17">
-        <v>134.87713523169967</v>
+        <v>134.87713523420388</v>
       </c>
       <c r="C46" s="17">
-        <v>141.21373172507688</v>
+        <v>141.19736389587337</v>
       </c>
       <c r="D46" s="17">
-        <v>142.42105823593053</v>
+        <v>142.4294878203882</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3338,13 +3340,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="17">
-        <v>141.63955566980175</v>
+        <v>141.63955567778058</v>
       </c>
       <c r="C47" s="17">
-        <v>143.67206419080745</v>
+        <v>143.65508907523966</v>
       </c>
       <c r="D47" s="17">
-        <v>141.92460299608237</v>
+        <v>141.94101653449394</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3352,13 +3354,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="17">
-        <v>137.7719220077847</v>
+        <v>137.77192201114806</v>
       </c>
       <c r="C48" s="17">
-        <v>140.63388248911917</v>
+        <v>140.67842226435656</v>
       </c>
       <c r="D48" s="17">
-        <v>141.30940696874114</v>
+        <v>141.33727014617654</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3366,13 +3368,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="17">
-        <v>135.76484313639392</v>
+        <v>135.7648431250517</v>
       </c>
       <c r="C49" s="17">
-        <v>140.1703221078896</v>
+        <v>140.21130207867455</v>
       </c>
       <c r="D49" s="17">
-        <v>140.60482351598944</v>
+        <v>140.646826395679</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3380,13 +3382,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="17">
-        <v>132.15799383097851</v>
+        <v>132.15799379484065</v>
       </c>
       <c r="C50" s="17">
-        <v>140.59984564590971</v>
+        <v>140.59828588290196</v>
       </c>
       <c r="D50" s="17">
-        <v>139.84795367448612</v>
+        <v>139.9056072871395</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3394,13 +3396,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="17">
-        <v>129.68532874950623</v>
+        <v>129.68532873427284</v>
       </c>
       <c r="C51" s="17">
-        <v>140.15528608935327</v>
+        <v>140.21019537086855</v>
       </c>
       <c r="D51" s="17">
-        <v>139.08115103220436</v>
+        <v>139.15455670807731</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3408,13 +3410,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="17">
-        <v>129.4452036709917</v>
+        <v>129.44520372236295</v>
       </c>
       <c r="C52" s="17">
-        <v>125.82222141229927</v>
+        <v>125.81544587391592</v>
       </c>
       <c r="D52" s="17">
-        <v>138.34689629645271</v>
+        <v>138.43449878444511</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,13 +3424,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="17">
-        <v>111.93059523012901</v>
+        <v>111.93059539380501</v>
       </c>
       <c r="C53" s="17">
-        <v>105.14609063407873</v>
+        <v>105.12696617995528</v>
       </c>
       <c r="D53" s="17">
-        <v>137.68725505157033</v>
+        <v>137.78632597414972</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3436,13 +3438,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="17">
-        <v>131.24787219841261</v>
+        <v>131.24787226740779</v>
       </c>
       <c r="C54" s="17">
-        <v>116.76950856720919</v>
+        <v>116.71989431958372</v>
       </c>
       <c r="D54" s="17">
-        <v>137.13635658038368</v>
+        <v>137.24342677304833</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3450,13 +3452,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="17">
-        <v>133.09348410134069</v>
+        <v>133.09348386866952</v>
       </c>
       <c r="C55" s="17">
-        <v>124.42185416124426</v>
+        <v>124.3854827223137</v>
       </c>
       <c r="D55" s="17">
-        <v>136.71900899653153</v>
+        <v>136.83025104489127</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3464,13 +3466,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="17">
-        <v>128.24284834290046</v>
+        <v>128.24284760157738</v>
       </c>
       <c r="C56" s="17">
-        <v>126.91449645461196</v>
+        <v>126.96395034325353</v>
       </c>
       <c r="D56" s="17">
-        <v>136.45174180514596</v>
+        <v>136.56298660307564</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3478,13 +3480,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="17">
-        <v>125.13820270379857</v>
+        <v>125.13820239130484</v>
       </c>
       <c r="C57" s="17">
-        <v>129.38670140063365</v>
+        <v>129.33930137224883</v>
       </c>
       <c r="D57" s="17">
-        <v>136.34095395686748</v>
+        <v>136.44798103006335</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3492,13 +3494,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="17">
-        <v>126.53017304338604</v>
+        <v>126.53017409720285</v>
       </c>
       <c r="C58" s="17">
-        <v>131.21529766007544</v>
+        <v>131.17154652165456</v>
       </c>
       <c r="D58" s="17">
-        <v>136.38019667630016</v>
+        <v>136.47969606496926</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,13 +3508,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="17">
-        <v>131.61628706837223</v>
+        <v>131.61629042598079</v>
       </c>
       <c r="C59" s="17">
-        <v>134.01704114789402</v>
+        <v>134.00842986320689</v>
       </c>
       <c r="D59" s="17">
-        <v>136.55574741906256</v>
+        <v>136.64565987002385</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3520,13 +3522,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="17">
-        <v>132.88316834734158</v>
+        <v>132.88316976269164</v>
       </c>
       <c r="C60" s="17">
-        <v>134.96409110665081</v>
+        <v>135.01811325208237</v>
       </c>
       <c r="D60" s="17">
-        <v>136.852266890923</v>
+        <v>136.9317627128161</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3534,13 +3536,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="17">
-        <v>132.30930298673249</v>
+        <v>132.30929821377384</v>
       </c>
       <c r="C61" s="17">
-        <v>134.86802616062928</v>
+        <v>134.92284873369374</v>
       </c>
       <c r="D61" s="17">
-        <v>137.24966986513732</v>
+        <v>137.31909938095455</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3548,13 +3550,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="17">
-        <v>129.61070724662031</v>
+        <v>129.61069203930271</v>
       </c>
       <c r="C62" s="17">
-        <v>139.7633128187199</v>
+        <v>139.76140677402978</v>
       </c>
       <c r="D62" s="17">
-        <v>137.73220864029813</v>
+        <v>137.79237819810285</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3562,13 +3564,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="17">
-        <v>126.88274991444005</v>
+        <v>126.88274350402092</v>
       </c>
       <c r="C63" s="17">
-        <v>137.98673799058017</v>
+        <v>138.07372842905741</v>
       </c>
       <c r="D63" s="17">
-        <v>138.29002939459448</v>
+        <v>138.34284909878332</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3576,13 +3578,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="17">
-        <v>147.05798330526144</v>
+        <v>147.05800492299821</v>
       </c>
       <c r="C64" s="17">
-        <v>140.5300495769151</v>
+        <v>140.51949921183521</v>
       </c>
       <c r="D64" s="17">
-        <v>138.91880926186428</v>
+        <v>138.96544586546307</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,13 +3592,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="17">
-        <v>144.90965443999067</v>
+        <v>144.90972331714073</v>
       </c>
       <c r="C65" s="17">
-        <v>137.83125100868563</v>
+        <v>137.81127229015937</v>
       </c>
       <c r="D65" s="17">
-        <v>139.61452958582288</v>
+        <v>139.65548122252824</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3604,13 +3606,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="17">
-        <v>150.49543813153664</v>
+        <v>150.49546716567752</v>
       </c>
       <c r="C66" s="17">
-        <v>137.31599587289136</v>
+        <v>137.21921401103157</v>
       </c>
       <c r="D66" s="17">
-        <v>140.37127349994904</v>
+        <v>140.40637343098027</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,13 +3620,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="17">
-        <v>149.13455286894037</v>
+        <v>149.13445495764941</v>
       </c>
       <c r="C67" s="17">
-        <v>140.76169863738164</v>
+        <v>140.74022393056367</v>
       </c>
       <c r="D67" s="17">
-        <v>141.17482726108986</v>
+        <v>141.20529444067228</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,13 +3634,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="17">
-        <v>142.80662967621774</v>
+        <v>142.80631771707249</v>
       </c>
       <c r="C68" s="17">
-        <v>142.06421307359645</v>
+        <v>142.14835895751847</v>
       </c>
       <c r="D68" s="17">
-        <v>142.00832104782219</v>
+        <v>142.03665120300522</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3646,13 +3648,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="17">
-        <v>141.05809896236462</v>
+        <v>141.05796746061472</v>
       </c>
       <c r="C69" s="17">
-        <v>144.34882675879112</v>
+        <v>144.27723205557436</v>
       </c>
       <c r="D69" s="17">
-        <v>142.85402098873428</v>
+        <v>142.88584272101866</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3660,13 +3662,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="17">
-        <v>140.84573230446983</v>
+        <v>140.84617576536496</v>
       </c>
       <c r="C70" s="17">
-        <v>145.47568384818251</v>
+        <v>145.4182901032425</v>
       </c>
       <c r="D70" s="17">
-        <v>143.69144946032404</v>
+        <v>143.73622742295956</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3674,13 +3676,13 @@
         <v>44470</v>
       </c>
       <c r="B71" s="17">
-        <v>140.56193664975186</v>
+        <v>140.5633495785417</v>
       </c>
       <c r="C71" s="17">
-        <v>144.47306917765241</v>
+        <v>144.47552425703893</v>
       </c>
       <c r="D71" s="17">
-        <v>144.5017919681024</v>
+        <v>144.57165292890971</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3688,13 +3690,13 @@
         <v>44501</v>
       </c>
       <c r="B72" s="17">
-        <v>145.46325291509621</v>
+        <v>145.46384851426734</v>
       </c>
       <c r="C72" s="17">
-        <v>146.16290392683246</v>
+        <v>146.21150512114775</v>
       </c>
       <c r="D72" s="17">
-        <v>145.27352508861955</v>
+        <v>145.38076506631688</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3702,13 +3704,13 @@
         <v>44531</v>
       </c>
       <c r="B73" s="17">
-        <v>146.03185867931461</v>
+        <v>146.02985015135357</v>
       </c>
       <c r="C73" s="17">
-        <v>148.14485115710946</v>
+        <v>148.20233870532689</v>
       </c>
       <c r="D73" s="17">
-        <v>146.00162068983354</v>
+        <v>146.15590465637473</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3716,13 +3718,13 @@
         <v>44562</v>
       </c>
       <c r="B74" s="17">
-        <v>136.21698889837035</v>
+        <v>136.16705638256084</v>
       </c>
       <c r="C74" s="17">
-        <v>147.0182791137764</v>
+        <v>146.98959071327914</v>
       </c>
       <c r="D74" s="17">
-        <v>146.68523745802642</v>
+        <v>146.89217078277596</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,13 +3732,13 @@
         <v>44593</v>
       </c>
       <c r="B75" s="17">
-        <v>137.65110084488177</v>
+        <v>137.61605600266572</v>
       </c>
       <c r="C75" s="17">
-        <v>148.8536268232443</v>
+        <v>148.98630677458925</v>
       </c>
       <c r="D75" s="17">
-        <v>147.32981538840437</v>
+        <v>147.58965381892176</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3744,13 +3746,13 @@
         <v>44621</v>
       </c>
       <c r="B76" s="17">
-        <v>153.85641342433848</v>
+        <v>153.93276547580172</v>
       </c>
       <c r="C76" s="17">
-        <v>148.00117455719499</v>
+        <v>148.08778556533693</v>
       </c>
       <c r="D76" s="17">
-        <v>147.94426364182635</v>
+        <v>148.25182774906801</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3758,13 +3760,13 @@
         <v>44652</v>
       </c>
       <c r="B77" s="17">
-        <v>152.85900020992258</v>
+        <v>153.54967051539364</v>
       </c>
       <c r="C77" s="17">
-        <v>148.32920805030361</v>
+        <v>148.96188540129026</v>
       </c>
       <c r="D77" s="17">
-        <v>148.54396149584483</v>
+        <v>148.88844593227813</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,27 +3774,41 @@
         <v>44682</v>
       </c>
       <c r="B78" s="17">
-        <v>161.91492093327662</v>
+        <v>162.45901581058692</v>
       </c>
       <c r="C78" s="17">
-        <v>148.54157439366949</v>
+        <v>148.97860319579968</v>
       </c>
       <c r="D78" s="17">
-        <v>149.14460919030043</v>
+        <v>149.51339604875685</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>44713</v>
       </c>
-      <c r="B79" s="18">
-        <v>158.71624347174495</v>
-      </c>
-      <c r="C79" s="18">
-        <v>150.13947378753312</v>
-      </c>
-      <c r="D79" s="18">
-        <v>149.75924495000885</v>
+      <c r="B79" s="17">
+        <v>159.38090733438185</v>
+      </c>
+      <c r="C79" s="17">
+        <v>150.75309131459943</v>
+      </c>
+      <c r="D79" s="17">
+        <v>150.1408073873078</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>44743</v>
+      </c>
+      <c r="B80" s="18">
+        <v>150.73278694947095</v>
+      </c>
+      <c r="C80" s="18">
+        <v>150.69888795783595</v>
+      </c>
+      <c r="D80" s="18">
+        <v>150.77969977562731</v>
       </c>
     </row>
   </sheetData>
@@ -5937,9 +5953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E35"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5978,16 +5992,16 @@
         <v>38</v>
       </c>
       <c r="B3">
-        <v>27.9</v>
+        <v>27.7</v>
       </c>
       <c r="C3">
-        <v>37.299999999999997</v>
+        <v>36.5</v>
       </c>
       <c r="D3">
-        <v>6.1</v>
+        <v>6.8</v>
       </c>
       <c r="E3">
-        <v>8.1999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5995,16 +6009,16 @@
         <v>39</v>
       </c>
       <c r="B4">
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>16.399999999999999</v>
+        <v>16.2</v>
       </c>
       <c r="D4">
-        <v>1.8</v>
+        <v>3.2</v>
       </c>
       <c r="E4">
-        <v>2.2999999999999998</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6012,16 +6026,16 @@
         <v>40</v>
       </c>
       <c r="B5">
-        <v>33</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="C5">
-        <v>42.3</v>
+        <v>42</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>9.4</v>
       </c>
       <c r="E5">
-        <v>10.5</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6029,16 +6043,16 @@
         <v>41</v>
       </c>
       <c r="B6">
-        <v>33.1</v>
+        <v>29.1</v>
       </c>
       <c r="C6">
-        <v>44.6</v>
+        <v>38.6</v>
       </c>
       <c r="D6">
-        <v>5.0999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="E6">
-        <v>7.2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -6046,16 +6060,16 @@
         <v>42</v>
       </c>
       <c r="B7">
-        <v>28.3</v>
+        <v>25.9</v>
       </c>
       <c r="C7">
-        <v>36.799999999999997</v>
+        <v>33.4</v>
       </c>
       <c r="D7">
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="E7">
-        <v>4.8</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -6063,16 +6077,16 @@
         <v>43</v>
       </c>
       <c r="B8">
-        <v>36.6</v>
+        <v>31.6</v>
       </c>
       <c r="C8">
-        <v>47.8</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="D8">
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6080,13 +6094,13 @@
         <v>44</v>
       </c>
       <c r="B9">
-        <v>19.899999999999999</v>
+        <v>29.8</v>
       </c>
       <c r="C9">
-        <v>27.3</v>
+        <v>38.5</v>
       </c>
       <c r="D9">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="E9">
         <v>7.6</v>
@@ -6097,16 +6111,16 @@
         <v>45</v>
       </c>
       <c r="B10">
-        <v>35.299999999999997</v>
+        <v>17.3</v>
       </c>
       <c r="C10">
-        <v>45</v>
+        <v>24.4</v>
       </c>
       <c r="D10">
-        <v>9.6999999999999993</v>
+        <v>6.1</v>
       </c>
       <c r="E10">
-        <v>12.8</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -6114,16 +6128,16 @@
         <v>46</v>
       </c>
       <c r="B11">
-        <v>42.3</v>
+        <v>41.6</v>
       </c>
       <c r="C11">
-        <v>52</v>
+        <v>49.9</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>12.9</v>
       </c>
       <c r="E11">
-        <v>19.399999999999999</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -6131,16 +6145,16 @@
         <v>47</v>
       </c>
       <c r="B12">
-        <v>25</v>
+        <v>21.5</v>
       </c>
       <c r="C12">
-        <v>34.1</v>
+        <v>28.7</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="E12">
-        <v>3.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -6148,16 +6162,16 @@
         <v>48</v>
       </c>
       <c r="B13">
-        <v>32.200000000000003</v>
+        <v>32.4</v>
       </c>
       <c r="C13" s="29">
-        <v>39.700000000000003</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="D13">
-        <v>8.5</v>
+        <v>6.4</v>
       </c>
       <c r="E13">
-        <v>10.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6165,16 +6179,16 @@
         <v>49</v>
       </c>
       <c r="B14">
-        <v>34.9</v>
+        <v>27.9</v>
       </c>
       <c r="C14">
-        <v>42.7</v>
+        <v>35.1</v>
       </c>
       <c r="D14">
-        <v>7.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E14">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6182,16 +6196,16 @@
         <v>50</v>
       </c>
       <c r="B15">
-        <v>29.4</v>
+        <v>28.2</v>
       </c>
       <c r="C15">
-        <v>36.200000000000003</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="E15">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6199,16 +6213,16 @@
         <v>51</v>
       </c>
       <c r="B16">
-        <v>28</v>
+        <v>26.4</v>
       </c>
       <c r="C16">
-        <v>34.299999999999997</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="E16">
-        <v>3.5</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6216,16 +6230,16 @@
         <v>52</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>27.4</v>
       </c>
       <c r="C17">
-        <v>38.9</v>
+        <v>34.5</v>
       </c>
       <c r="D17">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E17">
-        <v>7.8</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6233,16 +6247,16 @@
         <v>53</v>
       </c>
       <c r="B18">
-        <v>27.2</v>
+        <v>30.1</v>
       </c>
       <c r="C18">
-        <v>36.799999999999997</v>
+        <v>40</v>
       </c>
       <c r="D18">
-        <v>2.7</v>
+        <v>4.5</v>
       </c>
       <c r="E18">
-        <v>4.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6250,16 +6264,16 @@
         <v>54</v>
       </c>
       <c r="B19">
-        <v>22.5</v>
+        <v>24.6</v>
       </c>
       <c r="C19">
-        <v>30.9</v>
+        <v>33.4</v>
       </c>
       <c r="D19">
-        <v>5.7</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E19">
-        <v>6.7</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -6267,16 +6281,16 @@
         <v>55</v>
       </c>
       <c r="B20">
-        <v>40.6</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>51.5</v>
+        <v>49.2</v>
       </c>
       <c r="D20">
-        <v>8.6999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E20">
-        <v>10.5</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -6284,16 +6298,16 @@
         <v>56</v>
       </c>
       <c r="B21">
-        <v>29.2</v>
+        <v>28.4</v>
       </c>
       <c r="C21">
-        <v>40.4</v>
+        <v>40</v>
       </c>
       <c r="D21">
-        <v>5.7</v>
+        <v>7.3</v>
       </c>
       <c r="E21">
-        <v>7.5</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6301,16 +6315,16 @@
         <v>57</v>
       </c>
       <c r="B22">
-        <v>23.9</v>
+        <v>26.8</v>
       </c>
       <c r="C22">
-        <v>29.6</v>
+        <v>36.6</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E22">
-        <v>7.5</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -6318,16 +6332,16 @@
         <v>58</v>
       </c>
       <c r="B23">
-        <v>24.8</v>
+        <v>22.8</v>
       </c>
       <c r="C23">
-        <v>33</v>
+        <v>31.2</v>
       </c>
       <c r="D23">
-        <v>5.6</v>
+        <v>3.7</v>
       </c>
       <c r="E23">
-        <v>7.2</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -6335,16 +6349,16 @@
         <v>59</v>
       </c>
       <c r="B24">
-        <v>21.8</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>29.8</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D24">
-        <v>3.6</v>
+        <v>7</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -6352,16 +6366,16 @@
         <v>60</v>
       </c>
       <c r="B25">
-        <v>27.9</v>
+        <v>27.8</v>
       </c>
       <c r="C25">
-        <v>38.6</v>
+        <v>39.1</v>
       </c>
       <c r="D25">
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="E25">
-        <v>8.8000000000000007</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -6369,16 +6383,16 @@
         <v>61</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>24.5</v>
       </c>
       <c r="C26">
-        <v>31.5</v>
+        <v>32.6</v>
       </c>
       <c r="D26">
-        <v>6.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E26">
-        <v>7.5</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -6386,16 +6400,16 @@
         <v>62</v>
       </c>
       <c r="B27">
-        <v>28.8</v>
+        <v>24.8</v>
       </c>
       <c r="C27">
-        <v>39.9</v>
+        <v>33.9</v>
       </c>
       <c r="D27">
-        <v>3.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E27">
-        <v>4.4000000000000004</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -6403,16 +6417,16 @@
         <v>63</v>
       </c>
       <c r="B28">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="C28">
-        <v>33.299999999999997</v>
+        <v>35.9</v>
       </c>
       <c r="D28">
         <v>9.1</v>
       </c>
       <c r="E28">
-        <v>13.8</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -6420,16 +6434,16 @@
         <v>64</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>28.9</v>
       </c>
       <c r="C29">
-        <v>40</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="D29">
-        <v>7.1</v>
+        <v>5.6</v>
       </c>
       <c r="E29">
-        <v>10.3</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -6437,16 +6451,16 @@
         <v>65</v>
       </c>
       <c r="B30">
-        <v>20.8</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="C30">
-        <v>28.1</v>
+        <v>25.6</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="E30">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -6454,16 +6468,16 @@
         <v>66</v>
       </c>
       <c r="B31">
-        <v>25.8</v>
+        <v>29.8</v>
       </c>
       <c r="C31">
-        <v>33.5</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="D31">
-        <v>4.2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -6471,16 +6485,16 @@
         <v>67</v>
       </c>
       <c r="B32">
-        <v>26.2</v>
+        <v>23.9</v>
       </c>
       <c r="C32">
-        <v>35.1</v>
+        <v>30.2</v>
       </c>
       <c r="D32">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E32">
-        <v>3.9</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -6488,16 +6502,16 @@
         <v>68</v>
       </c>
       <c r="B33">
-        <v>20.6</v>
+        <v>17.7</v>
       </c>
       <c r="C33">
-        <v>27.1</v>
+        <v>23.9</v>
       </c>
       <c r="D33">
-        <v>4.2</v>
+        <v>2.5</v>
       </c>
       <c r="E33">
-        <v>4.3</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -6505,16 +6519,16 @@
         <v>69</v>
       </c>
       <c r="B34">
-        <v>26.7</v>
+        <v>24.5</v>
       </c>
       <c r="C34">
-        <v>35.5</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="D34">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="E34">
-        <v>4.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -6522,16 +6536,16 @@
         <v>70</v>
       </c>
       <c r="B35">
-        <v>22.5</v>
+        <v>28.1</v>
       </c>
       <c r="C35">
-        <v>31</v>
+        <v>39.4</v>
       </c>
       <c r="D35">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="E35">
-        <v>2.9</v>
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>
@@ -6549,7 +6563,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,16 +6603,16 @@
         <v>71</v>
       </c>
       <c r="B3">
-        <v>27.9</v>
+        <v>27.7</v>
       </c>
       <c r="C3">
-        <v>37.299999999999997</v>
+        <v>36.5</v>
       </c>
       <c r="D3">
-        <v>6.1</v>
+        <v>6.8</v>
       </c>
       <c r="E3">
-        <v>8.1999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6606,16 +6620,16 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>27.7</v>
+        <v>28.6</v>
       </c>
       <c r="C4">
-        <v>37.299999999999997</v>
+        <v>37</v>
       </c>
       <c r="D4">
-        <v>6.6</v>
+        <v>3.6</v>
       </c>
       <c r="E4">
-        <v>8.9</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6623,16 +6637,16 @@
         <v>72</v>
       </c>
       <c r="B5">
-        <v>32.200000000000003</v>
+        <v>28.2</v>
       </c>
       <c r="C5">
-        <v>42.7</v>
+        <v>37</v>
       </c>
       <c r="D5">
-        <v>4.5</v>
+        <v>7.9</v>
       </c>
       <c r="E5">
-        <v>6.3</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6640,16 +6654,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>30.4</v>
+        <v>28.7</v>
       </c>
       <c r="C6">
-        <v>39.4</v>
+        <v>36</v>
       </c>
       <c r="D6">
-        <v>8.1</v>
+        <v>7.4</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -6657,16 +6671,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>31.1</v>
+        <v>28.4</v>
       </c>
       <c r="C7">
         <v>39.200000000000003</v>
       </c>
       <c r="D7">
-        <v>5.7</v>
+        <v>4.8</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -6674,16 +6688,16 @@
         <v>73</v>
       </c>
       <c r="B8">
-        <v>26.2</v>
+        <v>26.3</v>
       </c>
       <c r="C8">
-        <v>35.299999999999997</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="D8">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="E8">
-        <v>7.6</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6691,16 +6705,16 @@
         <v>74</v>
       </c>
       <c r="B9">
-        <v>23.8</v>
+        <v>24.1</v>
       </c>
       <c r="C9">
-        <v>31.5</v>
+        <v>31.4</v>
       </c>
       <c r="D9">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="E9">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -6717,7 +6731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
"Actualizo dato ipc sep22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ACCD68-1B83-4542-B442-9654AD125055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4C1E9A-932B-4432-9D4B-5FAA3D454066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -1267,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,6 +2452,23 @@
       </c>
       <c r="E69">
         <v>6.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="23">
+        <v>44805</v>
+      </c>
+      <c r="B70" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C70">
+        <v>11.7</v>
+      </c>
+      <c r="D70">
+        <v>5.5</v>
+      </c>
+      <c r="E70">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>
@@ -2680,7 +2697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
@@ -4133,25 +4150,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="20">
-        <v>7</v>
+        <v>6.2</v>
       </c>
       <c r="C2" s="26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="26">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="E2" s="26">
-        <v>7.6</v>
+        <v>6.8</v>
       </c>
       <c r="F2" s="26">
-        <v>7.6</v>
+        <v>6.1</v>
       </c>
       <c r="G2" s="26">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="H2" s="20">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4159,25 +4176,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="19">
+        <v>6.7</v>
+      </c>
+      <c r="C3" s="25">
         <v>7.1</v>
       </c>
-      <c r="C3" s="25">
-        <v>6.9</v>
-      </c>
       <c r="D3" s="25">
-        <v>7.3</v>
+        <v>6.7</v>
       </c>
       <c r="E3" s="25">
-        <v>7.5</v>
+        <v>6.8</v>
       </c>
       <c r="F3" s="25">
-        <v>7.1</v>
+        <v>5.3</v>
       </c>
       <c r="G3" s="25">
-        <v>7.4</v>
+        <v>6.4</v>
       </c>
       <c r="H3" s="19">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4185,25 +4202,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="19">
-        <v>7</v>
+        <v>9.4</v>
       </c>
       <c r="C4" s="25">
-        <v>7.3</v>
+        <v>9.9</v>
       </c>
       <c r="D4" s="25">
-        <v>6.8</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E4" s="25">
-        <v>6.5</v>
+        <v>10.6</v>
       </c>
       <c r="F4" s="25">
-        <v>6.9</v>
+        <v>9.5</v>
       </c>
       <c r="G4" s="25">
-        <v>6.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H4" s="19">
-        <v>6.8</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4211,25 +4228,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="19">
-        <v>9.9</v>
+        <v>10.6</v>
       </c>
       <c r="C5" s="25">
-        <v>9.6999999999999993</v>
+        <v>11.2</v>
       </c>
       <c r="D5" s="25">
-        <v>10.1</v>
+        <v>10</v>
       </c>
       <c r="E5" s="25">
-        <v>10.6</v>
+        <v>10.5</v>
       </c>
       <c r="F5" s="25">
-        <v>11.7</v>
+        <v>11.1</v>
       </c>
       <c r="G5" s="25">
-        <v>8.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="H5" s="19">
-        <v>7.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4237,25 +4254,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="19">
-        <v>5.5</v>
+        <v>3.1</v>
       </c>
       <c r="C6" s="25">
-        <v>5.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D6" s="25">
-        <v>4.9000000000000004</v>
+        <v>3.3</v>
       </c>
       <c r="E6" s="25">
-        <v>7.9</v>
+        <v>10.4</v>
       </c>
       <c r="F6" s="25">
-        <v>8.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G6" s="25">
-        <v>5.6</v>
+        <v>3.3</v>
       </c>
       <c r="H6" s="19">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4263,25 +4280,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="19">
-        <v>8.4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="25">
-        <v>8.6</v>
+        <v>6.1</v>
       </c>
       <c r="D7" s="25">
-        <v>8.4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="25">
-        <v>8.6</v>
+        <v>5.4</v>
       </c>
       <c r="F7" s="25">
-        <v>8.5</v>
+        <v>5.6</v>
       </c>
       <c r="G7" s="25">
-        <v>8</v>
+        <v>6.9</v>
       </c>
       <c r="H7" s="19">
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4289,25 +4306,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="19">
-        <v>5.7</v>
+        <v>4.3</v>
       </c>
       <c r="C8" s="25">
-        <v>6.3</v>
+        <v>3.9</v>
       </c>
       <c r="D8" s="25">
-        <v>5.3</v>
+        <v>4.2</v>
       </c>
       <c r="E8" s="25">
         <v>5.3</v>
       </c>
       <c r="F8" s="25">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="G8" s="25">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
       <c r="H8" s="19">
-        <v>6.2</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4315,25 +4332,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="19">
-        <v>6.8</v>
+        <v>5.8</v>
       </c>
       <c r="C9" s="25">
-        <v>8.3000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="D9" s="25">
-        <v>5.9</v>
+        <v>5.4</v>
       </c>
       <c r="E9" s="25">
-        <v>7.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F9" s="25">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="G9" s="25">
         <v>3.5</v>
       </c>
       <c r="H9" s="19">
-        <v>5.7</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4341,25 +4358,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="19">
-        <v>4.0999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="C10" s="25">
-        <v>4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D10" s="25">
-        <v>3.8</v>
+        <v>2.4</v>
       </c>
       <c r="E10" s="25">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="F10" s="25">
-        <v>4.4000000000000004</v>
+        <v>3.1</v>
       </c>
       <c r="G10" s="25">
-        <v>4.4000000000000004</v>
+        <v>3.7</v>
       </c>
       <c r="H10" s="19">
-        <v>5.6</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4367,25 +4384,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="19">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="C11" s="25">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D11" s="25">
-        <v>4</v>
+        <v>5.8</v>
       </c>
       <c r="E11" s="25">
-        <v>5.4</v>
+        <v>4.3</v>
       </c>
       <c r="F11" s="25">
-        <v>7.6</v>
+        <v>4.3</v>
       </c>
       <c r="G11" s="25">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="H11" s="19">
-        <v>7.4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4393,25 +4410,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="19">
-        <v>5</v>
+        <v>3.7</v>
       </c>
       <c r="C12" s="25">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="D12" s="25">
-        <v>6.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E12" s="25">
-        <v>4.4000000000000004</v>
+        <v>1.9</v>
       </c>
       <c r="F12" s="25">
-        <v>4.9000000000000004</v>
+        <v>4</v>
       </c>
       <c r="G12" s="25">
-        <v>7.8</v>
+        <v>3.9</v>
       </c>
       <c r="H12" s="19">
-        <v>4.9000000000000004</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4419,25 +4436,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="19">
-        <v>6.7</v>
+        <v>4.8</v>
       </c>
       <c r="C13" s="25">
-        <v>6.2</v>
+        <v>3.8</v>
       </c>
       <c r="D13" s="25">
-        <v>7.1</v>
+        <v>5.8</v>
       </c>
       <c r="E13" s="25">
-        <v>7.1</v>
+        <v>5</v>
       </c>
       <c r="F13" s="25">
-        <v>7.2</v>
+        <v>6.1</v>
       </c>
       <c r="G13" s="25">
-        <v>6.8</v>
+        <v>4.3</v>
       </c>
       <c r="H13" s="19">
-        <v>6.5</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4445,25 +4462,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="19">
-        <v>8.6999999999999993</v>
+        <v>6.8</v>
       </c>
       <c r="C14" s="25">
-        <v>8.1999999999999993</v>
+        <v>7</v>
       </c>
       <c r="D14" s="25">
-        <v>9.5</v>
+        <v>6.7</v>
       </c>
       <c r="E14" s="25">
-        <v>9.5</v>
+        <v>7.3</v>
       </c>
       <c r="F14" s="25">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="G14" s="25">
-        <v>8</v>
+        <v>6.6</v>
       </c>
       <c r="H14" s="19">
-        <v>8.4</v>
+        <v>5.9</v>
       </c>
     </row>
   </sheetData>
@@ -4476,7 +4493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4511,25 +4528,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="22">
-        <v>78.5</v>
+        <v>83</v>
       </c>
       <c r="C2" s="27">
-        <v>79.099999999999994</v>
+        <v>82.9</v>
       </c>
       <c r="D2" s="27">
-        <v>77.7</v>
+        <v>82.6</v>
       </c>
       <c r="E2" s="27">
-        <v>80.400000000000006</v>
+        <v>87.5</v>
       </c>
       <c r="F2" s="27">
-        <v>79.900000000000006</v>
+        <v>84.9</v>
       </c>
       <c r="G2" s="27">
-        <v>77.5</v>
+        <v>83.1</v>
       </c>
       <c r="H2" s="27">
-        <v>76</v>
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4537,25 +4554,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="21">
-        <v>80</v>
+        <v>86.6</v>
       </c>
       <c r="C3" s="17">
-        <v>79.8</v>
+        <v>86.4</v>
       </c>
       <c r="D3" s="17">
-        <v>79.7</v>
+        <v>86.7</v>
       </c>
       <c r="E3" s="17">
-        <v>82.4</v>
+        <v>90.2</v>
       </c>
       <c r="F3" s="17">
-        <v>81.3</v>
+        <v>86</v>
       </c>
       <c r="G3" s="17">
-        <v>79.900000000000006</v>
+        <v>87</v>
       </c>
       <c r="H3" s="17">
-        <v>79.099999999999994</v>
+        <v>84.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4563,25 +4580,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="21">
-        <v>69.099999999999994</v>
+        <v>74.8</v>
       </c>
       <c r="C4" s="17">
-        <v>68.7</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="D4" s="17">
-        <v>70.099999999999994</v>
+        <v>75</v>
       </c>
       <c r="E4" s="17">
+        <v>82.9</v>
+      </c>
+      <c r="F4" s="17">
         <v>73.8</v>
       </c>
-      <c r="F4" s="17">
-        <v>67.8</v>
-      </c>
       <c r="G4" s="17">
-        <v>67.7</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="H4" s="17">
-        <v>64.5</v>
+        <v>69.599999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4589,25 +4606,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="21">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C5" s="17">
-        <v>111.7</v>
+        <v>120.5</v>
       </c>
       <c r="D5" s="17">
-        <v>108.1</v>
+        <v>117.2</v>
       </c>
       <c r="E5" s="17">
-        <v>101.6</v>
+        <v>114.1</v>
       </c>
       <c r="F5" s="17">
-        <v>107.3</v>
+        <v>117.3</v>
       </c>
       <c r="G5" s="17">
-        <v>100.4</v>
+        <v>109.6</v>
       </c>
       <c r="H5" s="17">
-        <v>106.6</v>
+        <v>112.3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4615,25 +4632,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="21">
-        <v>56.8</v>
+        <v>58.6</v>
       </c>
       <c r="C6" s="17">
-        <v>56.2</v>
+        <v>57.7</v>
       </c>
       <c r="D6" s="17">
-        <v>52.5</v>
+        <v>53.8</v>
       </c>
       <c r="E6" s="17">
-        <v>74.900000000000006</v>
+        <v>88.1</v>
       </c>
       <c r="F6" s="17">
-        <v>66.400000000000006</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="G6" s="17">
+        <v>58.5</v>
+      </c>
+      <c r="H6" s="17">
         <v>56.9</v>
-      </c>
-      <c r="H6" s="17">
-        <v>57.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4641,25 +4658,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="21">
-        <v>79.2</v>
+        <v>83.6</v>
       </c>
       <c r="C7" s="17">
-        <v>81.2</v>
+        <v>85</v>
       </c>
       <c r="D7" s="17">
-        <v>78.599999999999994</v>
+        <v>83.5</v>
       </c>
       <c r="E7" s="17">
-        <v>74.8</v>
+        <v>80.5</v>
       </c>
       <c r="F7" s="17">
-        <v>78.900000000000006</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="G7" s="17">
-        <v>76.3</v>
+        <v>83.2</v>
       </c>
       <c r="H7" s="17">
-        <v>72</v>
+        <v>77.099999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4667,25 +4684,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="21">
-        <v>74.599999999999994</v>
+        <v>74.7</v>
       </c>
       <c r="C8" s="17">
-        <v>79.099999999999994</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="D8" s="17">
         <v>72.2</v>
       </c>
       <c r="E8" s="17">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F8" s="17">
-        <v>68</v>
+        <v>71.5</v>
       </c>
       <c r="G8" s="17">
-        <v>72</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="H8" s="17">
-        <v>69.900000000000006</v>
+        <v>72.099999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4693,25 +4710,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="21">
-        <v>71</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="C9" s="17">
-        <v>68.400000000000006</v>
+        <v>73</v>
       </c>
       <c r="D9" s="17">
-        <v>73.599999999999994</v>
+        <v>78</v>
       </c>
       <c r="E9" s="17">
-        <v>78.3</v>
+        <v>83</v>
       </c>
       <c r="F9" s="17">
-        <v>67.5</v>
+        <v>74.8</v>
       </c>
       <c r="G9" s="17">
-        <v>72.599999999999994</v>
+        <v>75.7</v>
       </c>
       <c r="H9" s="17">
-        <v>69.900000000000006</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4719,25 +4736,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="21">
-        <v>41.8</v>
+        <v>41.4</v>
       </c>
       <c r="C10" s="17">
-        <v>40.799999999999997</v>
+        <v>38.5</v>
       </c>
       <c r="D10" s="17">
-        <v>42.1</v>
+        <v>43.2</v>
       </c>
       <c r="E10" s="17">
-        <v>45.7</v>
+        <v>44.8</v>
       </c>
       <c r="F10" s="17">
-        <v>43.3</v>
+        <v>46.2</v>
       </c>
       <c r="G10" s="17">
-        <v>43.8</v>
+        <v>46.2</v>
       </c>
       <c r="H10" s="17">
-        <v>41.1</v>
+        <v>40.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4745,25 +4762,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="21">
-        <v>72.099999999999994</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="C11" s="17">
-        <v>73.900000000000006</v>
+        <v>76.5</v>
       </c>
       <c r="D11" s="17">
-        <v>70.3</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="E11" s="17">
-        <v>66</v>
+        <v>67.7</v>
       </c>
       <c r="F11" s="17">
-        <v>77</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="G11" s="17">
-        <v>71.7</v>
+        <v>77.5</v>
       </c>
       <c r="H11" s="17">
-        <v>67.599999999999994</v>
+        <v>68.900000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4771,25 +4788,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="21">
-        <v>65.8</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="C12" s="17">
-        <v>64.2</v>
+        <v>63.8</v>
       </c>
       <c r="D12" s="17">
-        <v>69.900000000000006</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="E12" s="17">
-        <v>61.6</v>
+        <v>61.2</v>
       </c>
       <c r="F12" s="17">
-        <v>51.9</v>
+        <v>54.3</v>
       </c>
       <c r="G12" s="17">
-        <v>75.3</v>
+        <v>77.3</v>
       </c>
       <c r="H12" s="17">
-        <v>73.599999999999994</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4797,25 +4814,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="21">
-        <v>97.5</v>
+        <v>99</v>
       </c>
       <c r="C13" s="17">
-        <v>102.8</v>
+        <v>101.4</v>
       </c>
       <c r="D13" s="17">
-        <v>90.6</v>
+        <v>93.9</v>
       </c>
       <c r="E13" s="17">
-        <v>102.5</v>
+        <v>105.5</v>
       </c>
       <c r="F13" s="17">
-        <v>96.3</v>
+        <v>101</v>
       </c>
       <c r="G13" s="17">
-        <v>96.7</v>
+        <v>100.9</v>
       </c>
       <c r="H13" s="17">
-        <v>97</v>
+        <v>102.1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4823,25 +4840,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="21">
-        <v>73.3</v>
+        <v>81.2</v>
       </c>
       <c r="C14" s="17">
-        <v>73.599999999999994</v>
+        <v>82.4</v>
       </c>
       <c r="D14" s="17">
-        <v>72</v>
+        <v>79.8</v>
       </c>
       <c r="E14" s="17">
-        <v>76.2</v>
+        <v>83</v>
       </c>
       <c r="F14" s="17">
-        <v>76.900000000000006</v>
+        <v>82.8</v>
       </c>
       <c r="G14" s="17">
-        <v>73.099999999999994</v>
+        <v>80.7</v>
       </c>
       <c r="H14" s="17">
-        <v>72.5</v>
+        <v>76.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo datos emae ago22, ica sept22 y res. fiscal sep22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4C1E9A-932B-4432-9D4B-5FAA3D454066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC18A6-B7D5-4D55-A835-8CF179CD448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,7 +897,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
@@ -2161,7 +2160,7 @@
       <c r="E52">
         <v>4.5</v>
       </c>
-      <c r="H52" s="19"/>
+      <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -2179,7 +2178,7 @@
       <c r="E53">
         <v>3.5</v>
       </c>
-      <c r="H53" s="19"/>
+      <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -2197,7 +2196,7 @@
       <c r="E54">
         <v>3.8</v>
       </c>
-      <c r="H54" s="19"/>
+      <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -2268,7 +2267,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="23">
+      <c r="A59" s="22">
         <v>44470</v>
       </c>
       <c r="B59" s="1">
@@ -2302,7 +2301,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="23">
+      <c r="A61" s="22">
         <v>44531</v>
       </c>
       <c r="B61" s="1">
@@ -2336,7 +2335,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="23">
+      <c r="A63" s="22">
         <v>44593</v>
       </c>
       <c r="B63" s="1">
@@ -2370,7 +2369,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="23">
+      <c r="A65" s="22">
         <v>44652</v>
       </c>
       <c r="B65" s="1">
@@ -2387,7 +2386,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="23">
+      <c r="A66" s="22">
         <v>44682</v>
       </c>
       <c r="B66" s="1">
@@ -2404,7 +2403,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="23">
+      <c r="A67" s="22">
         <v>44713</v>
       </c>
       <c r="B67" s="1">
@@ -2421,7 +2420,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
+      <c r="A68" s="22">
         <v>44743</v>
       </c>
       <c r="B68" s="1">
@@ -2438,7 +2437,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="23">
+      <c r="A69" s="22">
         <v>44774</v>
       </c>
       <c r="B69" s="1">
@@ -2455,7 +2454,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
+      <c r="A70" s="22">
         <v>44805</v>
       </c>
       <c r="B70" s="1">
@@ -2695,10 +2694,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,10 +2729,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="17">
-        <v>148.210530835908</v>
+        <v>148.19319606523234</v>
       </c>
       <c r="D2" s="17">
-        <v>147.05231862427431</v>
+        <v>147.06022302320272</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2744,10 +2743,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="17">
-        <v>146.78256626719059</v>
+        <v>146.75819852395946</v>
       </c>
       <c r="D3" s="17">
-        <v>146.45848210114823</v>
+        <v>146.47227528537138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2758,10 +2757,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="17">
-        <v>145.90616353882791</v>
+        <v>145.9478660527071</v>
       </c>
       <c r="D4" s="17">
-        <v>145.90247897308097</v>
+        <v>145.92019217476229</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2772,10 +2771,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="17">
-        <v>145.16894932834771</v>
+        <v>145.06690177984089</v>
       </c>
       <c r="D5" s="17">
-        <v>145.42107596828717</v>
+        <v>145.44015965892794</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,10 +2785,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="17">
-        <v>144.20919307915884</v>
+        <v>144.2668260300112</v>
       </c>
       <c r="D6" s="17">
-        <v>145.04135842744415</v>
+        <v>145.05924917248856</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,10 +2799,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="17">
-        <v>144.15840206702532</v>
+        <v>144.20281666465243</v>
       </c>
       <c r="D7" s="17">
-        <v>144.78323652099661</v>
+        <v>144.79793295836913</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,10 +2813,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="17">
-        <v>144.42926472809444</v>
+        <v>144.41975872203935</v>
       </c>
       <c r="D8" s="17">
-        <v>144.65636014434924</v>
+        <v>144.66637702026262</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2828,10 +2827,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="17">
-        <v>145.70436143421969</v>
+        <v>145.71641471610721</v>
       </c>
       <c r="D9" s="17">
-        <v>144.66428189378348</v>
+        <v>144.66905265246055</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,10 +2841,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="17">
-        <v>145.19594726393498</v>
+        <v>145.19339998807644</v>
       </c>
       <c r="D10" s="17">
-        <v>144.80589673644309</v>
+        <v>144.80571923702598</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2856,10 +2855,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="17">
-        <v>145.12759174049862</v>
+        <v>145.1201638875927</v>
       </c>
       <c r="D11" s="17">
-        <v>145.07119453962363</v>
+        <v>145.06713860559682</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,10 +2869,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="17">
-        <v>145.65094451754513</v>
+        <v>145.65227347260395</v>
       </c>
       <c r="D12" s="17">
-        <v>145.44399345153977</v>
+        <v>145.43751462008868</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2884,10 +2883,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="17">
-        <v>147.02743893800587</v>
+        <v>147.03353783582591</v>
       </c>
       <c r="D13" s="17">
-        <v>145.90999092907316</v>
+        <v>145.9028012419096</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2898,10 +2897,10 @@
         <v>136.63265948314879</v>
       </c>
       <c r="C14" s="17">
-        <v>147.41384671523994</v>
+        <v>147.42752675530534</v>
       </c>
       <c r="D14" s="17">
-        <v>146.45186086781152</v>
+        <v>146.44541649397468</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2912,10 +2911,10 @@
         <v>132.15851633981717</v>
       </c>
       <c r="C15" s="17">
-        <v>146.52974575935971</v>
+        <v>146.48857067058901</v>
       </c>
       <c r="D15" s="17">
-        <v>147.05174628269174</v>
+        <v>147.04683834930566</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2926,10 +2925,10 @@
         <v>152.62095855907629</v>
       </c>
       <c r="C16" s="17">
-        <v>147.86403917977194</v>
+        <v>147.89153422844933</v>
       </c>
       <c r="D16" s="17">
-        <v>147.6901602547706</v>
+        <v>147.68658424960381</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2940,10 +2939,10 @@
         <v>151.94634480454772</v>
       </c>
       <c r="C17" s="17">
-        <v>147.79224128542739</v>
+        <v>147.69572219343374</v>
       </c>
       <c r="D17" s="17">
-        <v>148.34496512861409</v>
+        <v>148.34154919954861</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2954,10 +2953,10 @@
         <v>168.38920946939328</v>
       </c>
       <c r="C18" s="17">
-        <v>148.52576183435193</v>
+        <v>148.58990437305988</v>
       </c>
       <c r="D18" s="17">
-        <v>148.98833831031766</v>
+        <v>148.98385944048317</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2968,10 +2967,10 @@
         <v>161.03568546936668</v>
       </c>
       <c r="C19" s="17">
-        <v>150.14457613819343</v>
+        <v>150.17695269144946</v>
       </c>
       <c r="D19" s="17">
-        <v>149.58798577192454</v>
+        <v>149.58229946923197</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2982,10 +2981,10 @@
         <v>150.30605012364694</v>
       </c>
       <c r="C20" s="17">
-        <v>150.37813098487408</v>
+        <v>150.35627540388353</v>
       </c>
       <c r="D20" s="17">
-        <v>150.11050805481636</v>
+        <v>150.10362807419347</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2996,10 +2995,10 @@
         <v>149.25534277372603</v>
       </c>
       <c r="C21" s="17">
-        <v>150.40919723594126</v>
+        <v>150.43067339773305</v>
       </c>
       <c r="D21" s="17">
-        <v>150.52142384501033</v>
+        <v>150.51350901095469</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3010,10 +3009,10 @@
         <v>146.38655965814218</v>
       </c>
       <c r="C22" s="17">
-        <v>151.33849784609299</v>
+        <v>151.33887726526288</v>
       </c>
       <c r="D22" s="17">
-        <v>150.78699452839317</v>
+        <v>150.77833901046304</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3024,10 +3023,10 @@
         <v>149.38594966725168</v>
       </c>
       <c r="C23" s="17">
-        <v>151.54706853750281</v>
+        <v>151.56040642402039</v>
       </c>
       <c r="D23" s="17">
-        <v>150.88147303289679</v>
+        <v>150.87246729601981</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3038,10 +3037,10 @@
         <v>151.92604285254845</v>
       </c>
       <c r="C24" s="17">
-        <v>152.50179371975429</v>
+        <v>152.49953994153444</v>
       </c>
       <c r="D24" s="17">
-        <v>150.78478400019193</v>
+        <v>150.77578577823633</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3052,10 +3051,10 @@
         <v>146.78338490746603</v>
       </c>
       <c r="C25" s="17">
-        <v>152.38180505983806</v>
+        <v>152.37072095151035</v>
       </c>
       <c r="D25" s="17">
-        <v>150.48876372997961</v>
+        <v>150.4799407619503</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3066,10 +3065,10 @@
         <v>142.74091260056943</v>
       </c>
       <c r="C26" s="17">
-        <v>151.93019742381182</v>
+        <v>151.95349094118492</v>
       </c>
       <c r="D26" s="17">
-        <v>150.00056494409171</v>
+        <v>149.99191187045534</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3080,10 +3079,10 @@
         <v>138.81804034929567</v>
       </c>
       <c r="C27" s="17">
-        <v>151.90927032801707</v>
+        <v>151.85081284402526</v>
       </c>
       <c r="D27" s="17">
-        <v>149.34220140345181</v>
+        <v>149.33342346204375</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3094,10 +3093,10 @@
         <v>155.85731954373438</v>
       </c>
       <c r="C28" s="17">
-        <v>151.1560025920725</v>
+        <v>151.19116655866171</v>
       </c>
       <c r="D28" s="17">
-        <v>148.54734557019884</v>
+        <v>148.53838870981724</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3108,10 +3107,10 @@
         <v>151.52454400931981</v>
       </c>
       <c r="C29" s="17">
-        <v>146.8599394529447</v>
+        <v>146.80031512025295</v>
       </c>
       <c r="D29" s="17">
-        <v>147.66160208885702</v>
+        <v>147.65264513468284</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3122,10 +3121,10 @@
         <v>159.56669238861375</v>
       </c>
       <c r="C30" s="17">
-        <v>144.44474334257279</v>
+        <v>144.51059279483761</v>
       </c>
       <c r="D30" s="17">
-        <v>146.73747868274978</v>
+        <v>146.72893571620381</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3136,10 +3135,10 @@
         <v>151.1257631973819</v>
       </c>
       <c r="C31" s="17">
-        <v>143.11892216170332</v>
+        <v>143.11269704210511</v>
       </c>
       <c r="D31" s="17">
-        <v>145.82924059227929</v>
+        <v>145.82148132963519</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3150,10 +3149,10 @@
         <v>145.96352431506975</v>
       </c>
       <c r="C32" s="17">
-        <v>143.33785850231715</v>
+        <v>143.30356923372261</v>
       </c>
       <c r="D32" s="17">
-        <v>144.9863997321296</v>
+        <v>144.97977583206159</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3164,10 +3163,10 @@
         <v>146.76595998569064</v>
       </c>
       <c r="C33" s="17">
-        <v>146.7186790417806</v>
+        <v>146.76016341377476</v>
       </c>
       <c r="D33" s="17">
-        <v>144.25375734689635</v>
+        <v>144.24833817210268</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3178,10 +3177,10 @@
         <v>137.74656988203205</v>
       </c>
       <c r="C34" s="17">
-        <v>143.34961326781749</v>
+        <v>143.34241816439391</v>
       </c>
       <c r="D34" s="17">
-        <v>143.66209750607391</v>
+        <v>143.6572086184897</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3192,10 +3191,10 @@
         <v>142.84327650513197</v>
       </c>
       <c r="C35" s="17">
-        <v>143.60184663648772</v>
+        <v>143.63465463934358</v>
       </c>
       <c r="D35" s="17">
-        <v>143.22564871078882</v>
+        <v>143.22008822439349</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3206,10 +3205,10 @@
         <v>140.59240754477185</v>
       </c>
       <c r="C36" s="17">
-        <v>141.56397902586735</v>
+        <v>141.55875869260419</v>
       </c>
       <c r="D36" s="17">
-        <v>142.94605555883766</v>
+        <v>142.9383103511795</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3220,10 +3219,10 @@
         <v>136.25161522905591</v>
       </c>
       <c r="C37" s="17">
-        <v>141.80557395857406</v>
+        <v>141.77798628895849</v>
       </c>
       <c r="D37" s="17">
-        <v>142.81071394292243</v>
+        <v>142.79933784015981</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3234,10 +3233,10 @@
         <v>134.53623749895024</v>
       </c>
       <c r="C38" s="17">
-        <v>142.84438244513083</v>
+        <v>142.8892022226787</v>
       </c>
       <c r="D38" s="17">
-        <v>142.79369250348179</v>
+        <v>142.77753503073623</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3248,10 +3247,10 @@
         <v>132.26788761886397</v>
       </c>
       <c r="C39" s="17">
-        <v>143.28573419617641</v>
+        <v>143.24397621594952</v>
       </c>
       <c r="D39" s="17">
-        <v>142.85781954205314</v>
+        <v>142.8366555380187</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3262,10 +3261,10 @@
         <v>144.96325830736751</v>
       </c>
       <c r="C40" s="17">
-        <v>141.2223344295154</v>
+        <v>141.21927263217049</v>
       </c>
       <c r="D40" s="17">
-        <v>142.96277044608519</v>
+        <v>142.93696828520521</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3276,10 +3275,10 @@
         <v>149.91623208225008</v>
       </c>
       <c r="C41" s="17">
-        <v>142.47158878360182</v>
+        <v>142.49250440943794</v>
       </c>
       <c r="D41" s="17">
-        <v>143.0674049043308</v>
+        <v>143.03779566296782</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3290,10 +3289,10 @@
         <v>164.13570357737953</v>
       </c>
       <c r="C42" s="17">
-        <v>144.70866060699998</v>
+        <v>144.78650813021989</v>
       </c>
       <c r="D42" s="17">
-        <v>143.13412583585591</v>
+        <v>143.10188407986848</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3304,10 +3303,10 @@
         <v>150.85895656094456</v>
       </c>
       <c r="C43" s="17">
-        <v>143.87910433750196</v>
+        <v>143.78034118841927</v>
       </c>
       <c r="D43" s="17">
-        <v>143.12767745193639</v>
+        <v>143.0943431486379</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3318,10 +3317,10 @@
         <v>146.77698127386105</v>
       </c>
       <c r="C44" s="17">
-        <v>145.59575841359464</v>
+        <v>145.50646599201986</v>
       </c>
       <c r="D44" s="17">
-        <v>143.01955888375289</v>
+        <v>142.98710125619451</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3332,10 +3331,10 @@
         <v>141.27691429278232</v>
       </c>
       <c r="C45" s="17">
-        <v>145.03588691355861</v>
+        <v>145.12811801440284</v>
       </c>
       <c r="D45" s="17">
-        <v>142.7898692469318</v>
+        <v>142.76032833820668</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3346,10 +3345,10 @@
         <v>134.87713523420388</v>
       </c>
       <c r="C46" s="17">
-        <v>141.19736389587337</v>
+        <v>141.19442521657709</v>
       </c>
       <c r="D46" s="17">
-        <v>142.4294878203882</v>
+        <v>142.40469125597397</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3360,10 +3359,10 @@
         <v>141.63955567778058</v>
       </c>
       <c r="C47" s="17">
-        <v>143.65508907523966</v>
+        <v>143.70258622947267</v>
       </c>
       <c r="D47" s="17">
-        <v>141.94101653449394</v>
+        <v>141.92233746989476</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3374,10 +3373,10 @@
         <v>137.77192201114806</v>
       </c>
       <c r="C48" s="17">
-        <v>140.67842226435656</v>
+        <v>140.66496241027576</v>
       </c>
       <c r="D48" s="17">
-        <v>141.33727014617654</v>
+        <v>141.32521233085475</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3388,10 +3387,10 @@
         <v>135.7648431250517</v>
       </c>
       <c r="C49" s="17">
-        <v>140.21130207867455</v>
+        <v>140.17726477849718</v>
       </c>
       <c r="D49" s="17">
-        <v>140.646826395679</v>
+        <v>140.64130181231408</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3402,10 +3401,10 @@
         <v>132.15799379484065</v>
       </c>
       <c r="C50" s="17">
-        <v>140.59828588290196</v>
+        <v>140.66735184553832</v>
       </c>
       <c r="D50" s="17">
-        <v>139.9056072871395</v>
+        <v>139.90611786960301</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3416,10 +3415,10 @@
         <v>129.68532873427284</v>
       </c>
       <c r="C51" s="17">
-        <v>140.21019537086855</v>
+        <v>140.15095614762484</v>
       </c>
       <c r="D51" s="17">
-        <v>139.15455670807731</v>
+        <v>139.16040490527027</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3430,10 +3429,10 @@
         <v>129.44520372236295</v>
       </c>
       <c r="C52" s="17">
-        <v>125.81544587391592</v>
+        <v>125.80561913449993</v>
       </c>
       <c r="D52" s="17">
-        <v>138.43449878444511</v>
+        <v>138.44555126327614</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3444,10 +3443,10 @@
         <v>111.93059539380501</v>
       </c>
       <c r="C53" s="17">
-        <v>105.12696617995528</v>
+        <v>105.17105359476452</v>
       </c>
       <c r="D53" s="17">
-        <v>137.78632597414972</v>
+        <v>137.80207580460984</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3458,10 +3457,10 @@
         <v>131.24787226740779</v>
       </c>
       <c r="C54" s="17">
-        <v>116.71989431958372</v>
+        <v>116.76633024581852</v>
       </c>
       <c r="D54" s="17">
-        <v>137.24342677304833</v>
+        <v>137.26300651594465</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3472,10 +3471,10 @@
         <v>133.09348386866952</v>
       </c>
       <c r="C55" s="17">
-        <v>124.3854827223137</v>
+        <v>124.29495938125814</v>
       </c>
       <c r="D55" s="17">
-        <v>136.83025104489127</v>
+        <v>136.85248238324112</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3486,10 +3485,10 @@
         <v>128.24284760157738</v>
       </c>
       <c r="C56" s="17">
-        <v>126.96395034325353</v>
+        <v>126.82652113360706</v>
       </c>
       <c r="D56" s="17">
-        <v>136.56298660307564</v>
+        <v>136.58506202950926</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3500,10 +3499,10 @@
         <v>125.13820239130484</v>
       </c>
       <c r="C57" s="17">
-        <v>129.33930137224883</v>
+        <v>129.49521442464768</v>
       </c>
       <c r="D57" s="17">
-        <v>136.44798103006335</v>
+        <v>136.46816760905986</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3514,10 +3513,10 @@
         <v>126.53017409720285</v>
       </c>
       <c r="C58" s="17">
-        <v>131.17154652165456</v>
+        <v>131.15306267888315</v>
       </c>
       <c r="D58" s="17">
-        <v>136.47969606496926</v>
+        <v>136.49737500617613</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3528,10 +3527,10 @@
         <v>131.61629042598079</v>
       </c>
       <c r="C59" s="17">
-        <v>134.00842986320689</v>
+        <v>134.05114767974581</v>
       </c>
       <c r="D59" s="17">
-        <v>136.64565987002385</v>
+        <v>136.66107810102523</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3542,10 +3541,10 @@
         <v>132.88316976269164</v>
       </c>
       <c r="C60" s="17">
-        <v>135.01811325208237</v>
+        <v>135.01615310869295</v>
       </c>
       <c r="D60" s="17">
-        <v>136.9317627128161</v>
+        <v>136.94558019843319</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3556,10 +3555,10 @@
         <v>132.30929821377384</v>
       </c>
       <c r="C61" s="17">
-        <v>134.92284873369374</v>
+        <v>134.88209106052307</v>
       </c>
       <c r="D61" s="17">
-        <v>137.31909938095455</v>
+        <v>137.33253350261248</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3570,10 +3569,10 @@
         <v>129.61069203930271</v>
       </c>
       <c r="C62" s="17">
-        <v>139.76140677402978</v>
+        <v>139.85168048723571</v>
       </c>
       <c r="D62" s="17">
-        <v>137.79237819810285</v>
+        <v>137.80700223070565</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,10 +3583,10 @@
         <v>126.88274350402092</v>
       </c>
       <c r="C63" s="17">
-        <v>138.07372842905741</v>
+        <v>137.99000868591637</v>
       </c>
       <c r="D63" s="17">
-        <v>138.34284909878332</v>
+        <v>138.35968947539223</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,10 +3597,10 @@
         <v>147.05800492299821</v>
       </c>
       <c r="C64" s="17">
-        <v>140.51949921183521</v>
+        <v>140.5129452417481</v>
       </c>
       <c r="D64" s="17">
-        <v>138.96544586546307</v>
+        <v>138.98500914782772</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3612,10 +3611,10 @@
         <v>144.90972331714073</v>
       </c>
       <c r="C65" s="17">
-        <v>137.81127229015937</v>
+        <v>137.90810202646128</v>
       </c>
       <c r="D65" s="17">
-        <v>139.65548122252824</v>
+        <v>139.67804492678229</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3626,10 +3625,10 @@
         <v>150.49546716567752</v>
       </c>
       <c r="C66" s="17">
-        <v>137.21921401103157</v>
+        <v>137.32306193699105</v>
       </c>
       <c r="D66" s="17">
-        <v>140.40637343098027</v>
+        <v>140.4323847159458</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3640,10 +3639,10 @@
         <v>149.13445495764941</v>
       </c>
       <c r="C67" s="17">
-        <v>140.74022393056367</v>
+        <v>140.5395462682803</v>
       </c>
       <c r="D67" s="17">
-        <v>141.20529444067228</v>
+        <v>141.2355781828052</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3654,10 +3653,10 @@
         <v>142.80631771707249</v>
       </c>
       <c r="C68" s="17">
-        <v>142.14835895751847</v>
+        <v>141.95540441915369</v>
       </c>
       <c r="D68" s="17">
-        <v>142.03665120300522</v>
+        <v>142.07167905959997</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3668,10 +3667,10 @@
         <v>141.05796746061472</v>
       </c>
       <c r="C69" s="17">
-        <v>144.27723205557436</v>
+        <v>144.5286668918184</v>
       </c>
       <c r="D69" s="17">
-        <v>142.88584272101866</v>
+        <v>142.92414249720608</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3682,10 +3681,10 @@
         <v>140.84617576536496</v>
       </c>
       <c r="C70" s="17">
-        <v>145.4182901032425</v>
+        <v>145.35980980533893</v>
       </c>
       <c r="D70" s="17">
-        <v>143.73622742295956</v>
+        <v>143.77702201445061</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3696,10 +3695,10 @@
         <v>140.5633495785417</v>
       </c>
       <c r="C71" s="17">
-        <v>144.47552425703893</v>
+        <v>144.50759119615745</v>
       </c>
       <c r="D71" s="17">
-        <v>144.57165292890971</v>
+        <v>144.61593690699561</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3710,10 +3709,10 @@
         <v>145.46384851426734</v>
       </c>
       <c r="C72" s="17">
-        <v>146.21150512114775</v>
+        <v>146.22874448293129</v>
       </c>
       <c r="D72" s="17">
-        <v>145.38076506631688</v>
+        <v>145.42948330677413</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3724,10 +3723,10 @@
         <v>146.02985015135357</v>
       </c>
       <c r="C73" s="17">
-        <v>148.20233870532689</v>
+        <v>148.15303240439849</v>
       </c>
       <c r="D73" s="17">
-        <v>146.15590465637473</v>
+        <v>146.20825479854994</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3738,10 +3737,10 @@
         <v>136.16705638256084</v>
       </c>
       <c r="C74" s="17">
-        <v>146.98959071327914</v>
+        <v>147.12650428465804</v>
       </c>
       <c r="D74" s="17">
-        <v>146.89217078277596</v>
+        <v>146.94405632880586</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,10 +3751,10 @@
         <v>137.61605600266572</v>
       </c>
       <c r="C75" s="17">
-        <v>148.98630677458925</v>
+        <v>148.84575499812308</v>
       </c>
       <c r="D75" s="17">
-        <v>147.58965381892176</v>
+        <v>147.63256921887074</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3766,10 +3765,10 @@
         <v>153.93276547580172</v>
       </c>
       <c r="C76" s="17">
-        <v>148.08778556533693</v>
+        <v>148.0914237703972</v>
       </c>
       <c r="D76" s="17">
-        <v>148.25182774906801</v>
+        <v>148.27339211298866</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,13 +3776,13 @@
         <v>44652</v>
       </c>
       <c r="B77" s="17">
-        <v>153.54967051539364</v>
+        <v>153.38628948547043</v>
       </c>
       <c r="C77" s="17">
-        <v>148.96188540129026</v>
+        <v>148.93521555849219</v>
       </c>
       <c r="D77" s="17">
-        <v>148.88844593227813</v>
+        <v>148.87222050017624</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3791,13 +3790,13 @@
         <v>44682</v>
       </c>
       <c r="B78" s="17">
-        <v>162.45901581058692</v>
+        <v>162.38433403843436</v>
       </c>
       <c r="C78" s="17">
-        <v>148.97860319579968</v>
+        <v>149.06106096478484</v>
       </c>
       <c r="D78" s="17">
-        <v>149.51339604875685</v>
+        <v>149.44108343357962</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,27 +3804,41 @@
         <v>44713</v>
       </c>
       <c r="B79" s="17">
-        <v>159.38090733438185</v>
+        <v>159.61897013645768</v>
       </c>
       <c r="C79" s="17">
-        <v>150.75309131459943</v>
+        <v>150.69730338838366</v>
       </c>
       <c r="D79" s="17">
-        <v>150.1408073873078</v>
+        <v>149.99498950557097</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>44743</v>
       </c>
-      <c r="B80" s="18">
-        <v>150.73278694947095</v>
-      </c>
-      <c r="C80" s="18">
-        <v>150.69888795783595</v>
-      </c>
-      <c r="D80" s="18">
-        <v>150.77969977562731</v>
+      <c r="B80" s="17">
+        <v>151.18168336185485</v>
+      </c>
+      <c r="C80" s="17">
+        <v>150.85822741648312</v>
+      </c>
+      <c r="D80" s="17">
+        <v>150.54840449801696</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>44774</v>
+      </c>
+      <c r="B81" s="17">
+        <v>150.09171593050851</v>
+      </c>
+      <c r="C81" s="17">
+        <v>151.40709151954758</v>
+      </c>
+      <c r="D81" s="17">
+        <v>151.1114611234853</v>
       </c>
     </row>
   </sheetData>
@@ -3875,22 +3888,22 @@
       <c r="A2" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>7</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>7.6</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <v>6.4</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="27">
         <v>8.1</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>6.2</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="23">
         <v>6</v>
       </c>
       <c r="H2" s="16">
@@ -3901,22 +3914,22 @@
       <c r="A3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>3</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>3.2</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>3.9</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>2.9</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>2.7</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <v>4.8</v>
       </c>
       <c r="H3" s="16">
@@ -3927,22 +3940,22 @@
       <c r="A4" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>9</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>8</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>9.1</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>9.1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>9</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>8.5</v>
       </c>
       <c r="H4" s="16">
@@ -3953,22 +3966,22 @@
       <c r="A5" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>9.4</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>10.6</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>8.9</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <v>12.8</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>9.9</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>6</v>
       </c>
       <c r="H5" s="16">
@@ -3979,22 +3992,22 @@
       <c r="A6" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>8.6</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>9.4</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>9.9</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>7.7</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>15</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="23">
         <v>9.5</v>
       </c>
       <c r="H6" s="16">
@@ -4005,22 +4018,22 @@
       <c r="A7" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>14</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>17.399999999999999</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>18.3</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>16.600000000000001</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>18.7</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="23">
         <v>11.4</v>
       </c>
       <c r="H7" s="16">
@@ -4031,22 +4044,22 @@
       <c r="A8" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>13.1</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>17.5</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="27">
         <v>16.7</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>13.9</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="23">
         <v>10.199999999999999</v>
       </c>
       <c r="H8" s="16">
@@ -4057,22 +4070,22 @@
       <c r="A9" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>6.6</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>8.5</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>7</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>7.5</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>7.5</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="23">
         <v>7</v>
       </c>
       <c r="H9" s="16">
@@ -4083,22 +4096,22 @@
       <c r="A10" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>6.2</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>7.6</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <v>6.3</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="23">
         <v>8.1999999999999993</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="23">
         <v>6.3</v>
       </c>
       <c r="H10" s="16">
@@ -4149,25 +4162,25 @@
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>6.2</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="25">
         <v>6</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="25">
         <v>6.3</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="25">
         <v>6.8</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="25">
         <v>6.1</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="25">
         <v>6.1</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2" s="19">
         <v>6.1</v>
       </c>
     </row>
@@ -4175,25 +4188,25 @@
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>6.7</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>7.1</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>6.7</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <v>6.8</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="24">
         <v>5.3</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="24">
         <v>6.4</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="18">
         <v>6.7</v>
       </c>
     </row>
@@ -4201,25 +4214,25 @@
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>9.4</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>9.9</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <v>10.6</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <v>9.5</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="24">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>9.1</v>
       </c>
     </row>
@@ -4227,25 +4240,25 @@
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>10.6</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>11.2</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>10</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>10.5</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>11.1</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <v>10.8</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>8</v>
       </c>
     </row>
@@ -4253,25 +4266,25 @@
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>3.1</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>3.3</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>10.4</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <v>3.3</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>2.7</v>
       </c>
     </row>
@@ -4279,25 +4292,25 @@
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>6</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>6.1</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>6</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>5.4</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>5.6</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <v>6.9</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>6.4</v>
       </c>
     </row>
@@ -4305,25 +4318,25 @@
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>4.3</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>3.9</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>4.2</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>5.3</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>5.7</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="24">
         <v>5.3</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>4.8</v>
       </c>
     </row>
@@ -4331,25 +4344,25 @@
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>5.8</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>6.5</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>5.4</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>6.7</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="24">
         <v>3.5</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>5.4</v>
       </c>
     </row>
@@ -4357,25 +4370,25 @@
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <v>2.5</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>2.4</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>2.5</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>3.1</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="24">
         <v>3.7</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>3.4</v>
       </c>
     </row>
@@ -4383,25 +4396,25 @@
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="18">
         <v>5.2</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="24">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>5.8</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <v>4.3</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>4.3</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="24">
         <v>5.8</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>6.5</v>
       </c>
     </row>
@@ -4409,25 +4422,25 @@
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <v>3.7</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="24">
         <v>3.4</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="24">
         <v>1.9</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>4</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="24">
         <v>3.9</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -4435,25 +4448,25 @@
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>4.8</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="24">
         <v>3.8</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <v>5.8</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="24">
         <v>5</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="24">
         <v>6.1</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="24">
         <v>4.3</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>7.3</v>
       </c>
     </row>
@@ -4461,25 +4474,25 @@
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>6.8</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="24">
         <v>7</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <v>6.7</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="24">
         <v>7.3</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="24">
         <v>6.5</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="24">
         <v>6.6</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="18">
         <v>5.9</v>
       </c>
     </row>
@@ -4493,7 +4506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4527,25 +4540,25 @@
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="21">
         <v>83</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="26">
         <v>82.9</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="26">
         <v>82.6</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="26">
         <v>87.5</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="26">
         <v>84.9</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="26">
         <v>83.1</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="26">
         <v>80.099999999999994</v>
       </c>
     </row>
@@ -4553,7 +4566,7 @@
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>86.6</v>
       </c>
       <c r="C3" s="17">
@@ -4579,7 +4592,7 @@
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>74.8</v>
       </c>
       <c r="C4" s="17">
@@ -4605,7 +4618,7 @@
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>118</v>
       </c>
       <c r="C5" s="17">
@@ -4631,7 +4644,7 @@
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>58.6</v>
       </c>
       <c r="C6" s="17">
@@ -4657,7 +4670,7 @@
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>83.6</v>
       </c>
       <c r="C7" s="17">
@@ -4683,7 +4696,7 @@
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>74.7</v>
       </c>
       <c r="C8" s="17">
@@ -4709,7 +4722,7 @@
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>75.599999999999994</v>
       </c>
       <c r="C9" s="17">
@@ -4735,7 +4748,7 @@
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>41.4</v>
       </c>
       <c r="C10" s="17">
@@ -4761,7 +4774,7 @@
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>74.599999999999994</v>
       </c>
       <c r="C11" s="17">
@@ -4787,7 +4800,7 @@
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>66.599999999999994</v>
       </c>
       <c r="C12" s="17">
@@ -4813,7 +4826,7 @@
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>99</v>
       </c>
       <c r="C13" s="17">
@@ -4839,7 +4852,7 @@
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>81.2</v>
       </c>
       <c r="C14" s="17">
@@ -5981,14 +5994,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6181,7 +6194,7 @@
       <c r="B13">
         <v>32.4</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>40.299999999999997</v>
       </c>
       <c r="D13">
@@ -6592,14 +6605,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6748,7 +6761,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6773,285 +6788,285 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="30">
-        <v>10223</v>
-      </c>
-      <c r="C2" s="30">
-        <v>13534</v>
+      <c r="B2" s="29">
+        <v>11690</v>
+      </c>
+      <c r="C2" s="29">
+        <v>15276</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-3311</v>
+        <v>-3586</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="30">
-        <v>3344</v>
-      </c>
-      <c r="C3" s="30">
-        <v>542</v>
+      <c r="B3" s="29">
+        <v>3728</v>
+      </c>
+      <c r="C3" s="29">
+        <v>609</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>2802</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="30">
-        <v>3443</v>
-      </c>
-      <c r="C4" s="30">
-        <v>2380</v>
+      <c r="B4" s="29">
+        <v>3922</v>
+      </c>
+      <c r="C4" s="29">
+        <v>2703</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1063</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="30">
-        <v>980</v>
-      </c>
-      <c r="C5" s="30">
-        <v>22</v>
+      <c r="B5" s="29">
+        <v>1107</v>
+      </c>
+      <c r="C5" s="29">
+        <v>25</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>958</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="30">
-        <v>5645</v>
-      </c>
-      <c r="C6" s="30">
-        <v>9502</v>
+      <c r="B6" s="29">
+        <v>6617</v>
+      </c>
+      <c r="C6" s="29">
+        <v>10279</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-3857</v>
+        <v>-3662</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="30">
-        <v>7231</v>
-      </c>
-      <c r="C7" s="30">
-        <v>7558</v>
+      <c r="B7" s="29">
+        <v>8031</v>
+      </c>
+      <c r="C7" s="29">
+        <v>8604</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-327</v>
+        <v>-573</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="30">
-        <v>435</v>
-      </c>
-      <c r="C8" s="30">
-        <v>464</v>
+      <c r="B8" s="29">
+        <v>496</v>
+      </c>
+      <c r="C8" s="29">
+        <v>507</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-29</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="30">
-        <v>697</v>
-      </c>
-      <c r="C9" s="30">
-        <v>421</v>
+      <c r="B9" s="29">
+        <v>826</v>
+      </c>
+      <c r="C9" s="29">
+        <v>475</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="30">
-        <v>358</v>
-      </c>
-      <c r="C10" s="30">
-        <v>326</v>
+      <c r="B10" s="29">
+        <v>399</v>
+      </c>
+      <c r="C10" s="29">
+        <v>380</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="30">
-        <v>5489</v>
-      </c>
-      <c r="C11" s="30">
-        <v>2833</v>
+      <c r="B11" s="29">
+        <v>6060</v>
+      </c>
+      <c r="C11" s="29">
+        <v>3251</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2656</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="30">
-        <v>4149</v>
-      </c>
-      <c r="C12" s="30">
-        <v>11738</v>
+      <c r="B12" s="29">
+        <v>5212</v>
+      </c>
+      <c r="C12" s="29">
+        <v>13356</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-7589</v>
+        <v>-8144</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="30">
-        <v>1381</v>
-      </c>
-      <c r="C13" s="30">
-        <v>511</v>
+      <c r="B13" s="29">
+        <v>1576</v>
+      </c>
+      <c r="C13" s="29">
+        <v>566</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>870</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="30">
-        <v>574</v>
-      </c>
-      <c r="C14" s="30">
-        <v>765</v>
+      <c r="B14" s="29">
+        <v>658</v>
+      </c>
+      <c r="C14" s="29">
+        <v>887</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-191</v>
+        <v>-229</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="30">
-        <v>3457</v>
-      </c>
-      <c r="C15" s="30">
-        <v>1335</v>
+      <c r="B15" s="29">
+        <v>3637</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1444</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>2122</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="30">
-        <v>3674</v>
-      </c>
-      <c r="C16" s="30">
-        <v>2155</v>
+      <c r="B16" s="29">
+        <v>3914</v>
+      </c>
+      <c r="C16" s="29">
+        <v>2346</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1519</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="30">
-        <v>3122</v>
-      </c>
-      <c r="C17" s="30">
-        <v>931</v>
+      <c r="B17" s="29">
+        <v>3332</v>
+      </c>
+      <c r="C17" s="29">
+        <v>984</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2191</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="30">
-        <v>365</v>
-      </c>
-      <c r="C18" s="30">
-        <v>132</v>
+      <c r="B18" s="29">
+        <v>377</v>
+      </c>
+      <c r="C18" s="29">
+        <v>157</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="30">
-        <v>621</v>
-      </c>
-      <c r="C19" s="30">
-        <v>338</v>
+      <c r="B19" s="29">
+        <v>659</v>
+      </c>
+      <c r="C19" s="29">
+        <v>400</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="31">
-        <v>4534</v>
-      </c>
-      <c r="C20" s="31">
-        <v>2041</v>
+      <c r="B20" s="30">
+        <v>4891</v>
+      </c>
+      <c r="C20" s="30">
+        <v>2270</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2493</v>
+        <v>2621</v>
       </c>
     </row>
   </sheetData>
@@ -7082,419 +7097,419 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="36">
-        <v>59720</v>
+      <c r="B2" s="35">
+        <v>67131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="36">
-        <v>16680</v>
+      <c r="B3" s="35">
+        <v>18746</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="30">
-        <v>21</v>
+      <c r="B4" s="29">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="30">
-        <v>1089</v>
+      <c r="B5" s="29">
+        <v>1241</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="30">
-        <v>191</v>
+      <c r="B6" s="29">
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="30">
-        <v>441</v>
+      <c r="B7" s="29">
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="30">
-        <v>437</v>
+      <c r="B8" s="29">
+        <v>460</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="30">
-        <v>12384</v>
+      <c r="B9" s="29">
+        <v>13332</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="30">
-        <v>1534</v>
+      <c r="B10" s="29">
+        <v>2313</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="30">
-        <v>143</v>
+      <c r="B11" s="29">
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="30">
-        <v>21</v>
+      <c r="B12" s="29">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="30">
-        <v>132</v>
+      <c r="B13" s="29">
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="29">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="29">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="B16" s="35">
+        <v>25350</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="29">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="29">
         <v>186</v>
       </c>
-      <c r="B16" s="36">
-        <v>22860</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="30">
-        <v>2924</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="30">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="29">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="29">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="29">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="29">
+        <v>7401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="29">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="29">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="29">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="29">
+        <v>9814</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="29">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="30">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="30">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="30">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="B22" s="30">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="B23" s="30">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="B24" s="30">
-        <v>6718</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="30">
+      <c r="B30" s="29">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="29">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="29">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="35">
+        <v>17024</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="29">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="29">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="29">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="30">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27" s="30">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28" s="30">
-        <v>8981</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="30">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B30" s="30">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" s="30">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B32" s="30">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="B33" s="36">
-        <v>15005</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B34" s="30">
-        <v>4138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="B35" s="30">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="30">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="B37" s="30">
-        <v>21</v>
+      <c r="B37" s="29">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="30">
-        <v>314</v>
+      <c r="B38" s="29">
+        <v>348</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="30">
-        <v>98</v>
+      <c r="B39" s="29">
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B40" s="29">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="30">
-        <v>115</v>
+      <c r="B41" s="29">
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="30">
-        <v>1768</v>
+      <c r="B42" s="29">
+        <v>2040</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="30">
-        <v>1370</v>
+      <c r="B43" s="29">
+        <v>1596</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="30">
-        <v>1010</v>
+      <c r="B44" s="29">
+        <v>1160</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="30">
-        <v>4769</v>
+      <c r="B45" s="29">
+        <v>5606</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B46" s="30">
-        <v>266</v>
+      <c r="B46" s="29">
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="B47" s="30">
-        <v>193</v>
+      <c r="B47" s="29">
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="36">
-        <v>5175</v>
+      <c r="B48" s="35">
+        <v>6010</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="B49" s="30">
-        <v>2389</v>
+      <c r="B49" s="29">
+        <v>2798</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="B50" s="30">
-        <v>1653</v>
+      <c r="B50" s="29">
+        <v>1872</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="B51" s="30">
-        <v>64</v>
+      <c r="B51" s="29">
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
+      <c r="A52" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="B52" s="42">
-        <v>780</v>
+      <c r="B52" s="41">
+        <v>923</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="B53" s="43">
-        <v>288</v>
+      <c r="B53" s="42">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -7525,315 +7540,315 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="36">
-        <v>57527</v>
+      <c r="B2" s="35">
+        <v>64520</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="36">
-        <v>8393</v>
+      <c r="B3" s="35">
+        <v>9514</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="30">
-        <v>6298</v>
+      <c r="B4" s="29">
+        <v>7120</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="30">
-        <v>897</v>
+      <c r="B5" s="29">
+        <v>1036</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="30">
-        <v>884</v>
+      <c r="B6" s="29">
+        <v>1010</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="30">
-        <v>313</v>
+      <c r="B7" s="29">
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="36">
-        <v>21146</v>
+      <c r="B8" s="35">
+        <v>23744</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="30">
-        <v>2097</v>
+      <c r="B9" s="29">
+        <v>2270</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="B10" s="30">
-        <v>972</v>
+      <c r="B10" s="29">
+        <v>1116</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="30">
-        <v>8657</v>
+      <c r="B11" s="29">
+        <v>9730</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="30">
-        <v>2604</v>
+      <c r="B12" s="29">
+        <v>2943</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="30">
-        <v>820</v>
+      <c r="B13" s="29">
+        <v>935</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="30">
-        <v>960</v>
+      <c r="B14" s="29">
+        <v>1083</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="30">
-        <v>499</v>
+      <c r="B15" s="29">
+        <v>551</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="30">
-        <v>2981</v>
+      <c r="B16" s="29">
+        <v>3364</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="30">
-        <v>1556</v>
+      <c r="B17" s="29">
+        <v>1751</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="B18" s="36">
-        <v>10423</v>
+      <c r="B18" s="35">
+        <v>11213</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="B19" s="30">
-        <v>10196</v>
+      <c r="B19" s="29">
+        <v>10947</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B20" s="30">
-        <v>228</v>
+      <c r="B20" s="29">
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="B21" s="36">
-        <v>10009</v>
+      <c r="B21" s="35">
+        <v>11490</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B22" s="30">
-        <v>6525</v>
+      <c r="B22" s="29">
+        <v>7470</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="30">
-        <v>2755</v>
+      <c r="B23" s="29">
+        <v>3191</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B24" s="30">
-        <v>729</v>
+      <c r="B24" s="29">
+        <v>829</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="B25" s="36">
-        <v>5799</v>
+      <c r="B25" s="35">
+        <v>6553</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="B26" s="30">
-        <v>214</v>
+      <c r="B26" s="29">
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B27" s="30">
-        <v>415</v>
+      <c r="B27" s="29">
+        <v>473</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="B28" s="30">
-        <v>552</v>
+      <c r="B28" s="29">
+        <v>612</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="B29" s="30">
-        <v>1707</v>
+      <c r="B29" s="29">
+        <v>1932</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="30">
-        <v>362</v>
+      <c r="B30" s="29">
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="30">
-        <v>285</v>
+      <c r="B31" s="29">
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="B32" s="30">
-        <v>444</v>
+      <c r="B32" s="29">
+        <v>516</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="30">
-        <v>445</v>
+      <c r="B33" s="29">
+        <v>504</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="B34" s="30">
-        <v>396</v>
+      <c r="B34" s="29">
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B35" s="30">
-        <v>210</v>
+      <c r="B35" s="29">
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="30">
-        <v>373</v>
+      <c r="B36" s="29">
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="B37" s="30">
-        <v>396</v>
+      <c r="B37" s="29">
+        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B38" s="36">
-        <v>1311</v>
+      <c r="B38" s="35">
+        <v>1504</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="40">
-        <v>1311</v>
+      <c r="B39" s="39">
+        <v>1504</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="B40" s="41">
-        <v>445</v>
+      <c r="B40" s="40">
+        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo en base balanza comercial oct22, emae sept22 y dato fiscal oct22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117ABAF7-01BB-4EEB-BE79-960B7C2C6FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F85704E-22C7-4019-B244-DA3232953C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -943,6 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -2711,10 +2712,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,10 +2747,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="17">
-        <v>148.19319606523234</v>
+        <v>148.19237985851987</v>
       </c>
       <c r="D2" s="17">
-        <v>147.06022302320272</v>
+        <v>147.0484965554339</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,10 +2761,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="17">
-        <v>146.75819852395946</v>
+        <v>146.772631667143</v>
       </c>
       <c r="D3" s="17">
-        <v>146.47227528537138</v>
+        <v>146.45835108905862</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2774,10 +2775,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="17">
-        <v>145.9478660527071</v>
+        <v>145.91464750278519</v>
       </c>
       <c r="D4" s="17">
-        <v>145.92019217476229</v>
+        <v>145.90478393857433</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2788,10 +2789,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="17">
-        <v>145.06690177984089</v>
+        <v>145.06982544038877</v>
       </c>
       <c r="D5" s="17">
-        <v>145.44015965892794</v>
+        <v>145.4242365325272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2802,10 +2803,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="17">
-        <v>144.2668260300112</v>
+        <v>144.26546872255503</v>
       </c>
       <c r="D6" s="17">
-        <v>145.05924917248856</v>
+        <v>145.04357492377943</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,10 +2817,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="17">
-        <v>144.20281666465243</v>
+        <v>144.21001669651557</v>
       </c>
       <c r="D7" s="17">
-        <v>144.79793295836913</v>
+        <v>144.78275712690339</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2830,10 +2831,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="17">
-        <v>144.41975872203935</v>
+        <v>144.42344466410671</v>
       </c>
       <c r="D8" s="17">
-        <v>144.66637702026262</v>
+        <v>144.65140896087902</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2844,10 +2845,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="17">
-        <v>145.71641471610721</v>
+        <v>145.70503167880955</v>
       </c>
       <c r="D9" s="17">
-        <v>144.66905265246055</v>
+        <v>144.65376776304643</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2858,10 +2859,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="17">
-        <v>145.19339998807644</v>
+        <v>145.20010211132509</v>
       </c>
       <c r="D10" s="17">
-        <v>144.80571923702598</v>
+        <v>144.78957224151426</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2872,10 +2873,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="17">
-        <v>145.1201638875927</v>
+        <v>145.11420120174424</v>
       </c>
       <c r="D11" s="17">
-        <v>145.06713860559682</v>
+        <v>145.04982646793803</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2886,10 +2887,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="17">
-        <v>145.65227347260395</v>
+        <v>145.64550638376957</v>
       </c>
       <c r="D12" s="17">
-        <v>145.43751462008868</v>
+        <v>145.4191119623859</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,10 +2901,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="17">
-        <v>147.03353783582591</v>
+        <v>147.0580978054125</v>
       </c>
       <c r="D13" s="17">
-        <v>145.9028012419096</v>
+        <v>145.88366293115357</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2911,13 +2912,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="17">
-        <v>136.63265948314879</v>
+        <v>136.6326594831489</v>
       </c>
       <c r="C14" s="17">
-        <v>147.42752675530534</v>
+        <v>147.43320478790372</v>
       </c>
       <c r="D14" s="17">
-        <v>146.44541649397468</v>
+        <v>146.42619577334546</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2925,13 +2926,13 @@
         <v>42767</v>
       </c>
       <c r="B15" s="17">
-        <v>132.15851633981717</v>
+        <v>132.15851633981728</v>
       </c>
       <c r="C15" s="17">
-        <v>146.48857067058901</v>
+        <v>146.49117562075543</v>
       </c>
       <c r="D15" s="17">
-        <v>147.04683834930566</v>
+        <v>147.02838672422746</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2939,13 +2940,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="17">
-        <v>152.62095855907629</v>
+        <v>152.6209585590764</v>
       </c>
       <c r="C16" s="17">
-        <v>147.89153422844933</v>
+        <v>147.84473820642441</v>
       </c>
       <c r="D16" s="17">
-        <v>147.68658424960381</v>
+        <v>147.6698488064871</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2953,13 +2954,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="17">
-        <v>151.94634480454772</v>
+        <v>151.94634480454781</v>
       </c>
       <c r="C17" s="17">
-        <v>147.69572219343374</v>
+        <v>147.68388730388446</v>
       </c>
       <c r="D17" s="17">
-        <v>148.34154919954861</v>
+        <v>148.32745093057247</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2967,13 +2968,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="17">
-        <v>168.38920946939328</v>
+        <v>168.38920946939336</v>
       </c>
       <c r="C18" s="17">
-        <v>148.58990437305988</v>
+        <v>148.56489835625939</v>
       </c>
       <c r="D18" s="17">
-        <v>148.98385944048317</v>
+        <v>148.97285579803167</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2981,13 +2982,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="17">
-        <v>161.03568546936668</v>
+        <v>161.03568546936674</v>
       </c>
       <c r="C19" s="17">
-        <v>150.17695269144946</v>
+        <v>150.20546386180385</v>
       </c>
       <c r="D19" s="17">
-        <v>149.58229946923197</v>
+        <v>149.57431978540046</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2995,13 +2996,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="17">
-        <v>150.30605012364694</v>
+        <v>150.306050123647</v>
       </c>
       <c r="C20" s="17">
-        <v>150.35627540388353</v>
+        <v>150.35783910469979</v>
       </c>
       <c r="D20" s="17">
-        <v>150.10362807419347</v>
+        <v>150.09813070893708</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3009,13 +3010,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="17">
-        <v>149.25534277372603</v>
+        <v>149.25534277372614</v>
       </c>
       <c r="C21" s="17">
-        <v>150.43067339773305</v>
+        <v>150.43124703370367</v>
       </c>
       <c r="D21" s="17">
-        <v>150.51350901095469</v>
+        <v>150.50953103673018</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3023,13 +3024,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="17">
-        <v>146.38655965814218</v>
+        <v>146.38655965814226</v>
       </c>
       <c r="C22" s="17">
-        <v>151.33887726526288</v>
+        <v>151.33232435872102</v>
       </c>
       <c r="D22" s="17">
-        <v>150.77833901046304</v>
+        <v>150.77460329212673</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3037,13 +3038,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="17">
-        <v>149.38594966725168</v>
+        <v>149.38594966725174</v>
       </c>
       <c r="C23" s="17">
-        <v>151.56040642402039</v>
+        <v>151.5725317541775</v>
       </c>
       <c r="D23" s="17">
-        <v>150.87246729601981</v>
+        <v>150.86773884092668</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3051,13 +3052,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="17">
-        <v>151.92604285254845</v>
+        <v>151.92604285254853</v>
       </c>
       <c r="C24" s="17">
-        <v>152.49953994153444</v>
+        <v>152.50623901328706</v>
       </c>
       <c r="D24" s="17">
-        <v>150.77578577823633</v>
+        <v>150.76923027880255</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3065,13 +3066,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="17">
-        <v>146.78338490746603</v>
+        <v>146.78338490746614</v>
       </c>
       <c r="C25" s="17">
-        <v>152.37072095151035</v>
+        <v>152.4031548888702</v>
       </c>
       <c r="D25" s="17">
-        <v>150.4799407619503</v>
+        <v>150.4710379449985</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3079,13 +3080,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="17">
-        <v>142.74091260056943</v>
+        <v>142.7409126005696</v>
       </c>
       <c r="C26" s="17">
-        <v>151.95349094118492</v>
+        <v>151.94176989323091</v>
       </c>
       <c r="D26" s="17">
-        <v>149.99191187045534</v>
+        <v>149.98049897471174</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3093,13 +3094,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="17">
-        <v>138.81804034929567</v>
+        <v>138.81804034929579</v>
       </c>
       <c r="C27" s="17">
-        <v>151.85081284402526</v>
+        <v>151.84535798859653</v>
       </c>
       <c r="D27" s="17">
-        <v>149.33342346204375</v>
+        <v>149.31968556431585</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3107,13 +3108,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="17">
-        <v>155.85731954373438</v>
+        <v>155.85731954373435</v>
       </c>
       <c r="C28" s="17">
-        <v>151.19116655866171</v>
+        <v>151.15416554311437</v>
       </c>
       <c r="D28" s="17">
-        <v>148.53838870981724</v>
+        <v>148.52284338027204</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3121,13 +3122,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="17">
-        <v>151.52454400931981</v>
+        <v>151.52454400931953</v>
       </c>
       <c r="C29" s="17">
-        <v>146.80031512025295</v>
+        <v>146.77655533760023</v>
       </c>
       <c r="D29" s="17">
-        <v>147.65264513468284</v>
+        <v>147.63583734163745</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3135,13 +3136,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="17">
-        <v>159.56669238861375</v>
+        <v>159.56669238861372</v>
       </c>
       <c r="C30" s="17">
-        <v>144.51059279483761</v>
+        <v>144.4852804564421</v>
       </c>
       <c r="D30" s="17">
-        <v>146.72893571620381</v>
+        <v>146.71107890987963</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3149,13 +3150,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="17">
-        <v>151.1257631973819</v>
+        <v>151.1257631973825</v>
       </c>
       <c r="C31" s="17">
-        <v>143.11269704210511</v>
+        <v>143.10209365349945</v>
       </c>
       <c r="D31" s="17">
-        <v>145.82148132963519</v>
+        <v>145.80254451716149</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3163,13 +3164,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="17">
-        <v>145.96352431506975</v>
+        <v>145.9635243150716</v>
       </c>
       <c r="C32" s="17">
-        <v>143.30356923372261</v>
+        <v>143.28539587530634</v>
       </c>
       <c r="D32" s="17">
-        <v>144.97977583206159</v>
+        <v>144.95977751501192</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3177,13 +3178,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="17">
-        <v>146.76595998569064</v>
+        <v>146.76595998569144</v>
       </c>
       <c r="C33" s="17">
-        <v>146.76016341377476</v>
+        <v>146.73589981414585</v>
       </c>
       <c r="D33" s="17">
-        <v>144.24833817210268</v>
+        <v>144.22734431295893</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,13 +3192,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="17">
-        <v>137.74656988203205</v>
+        <v>137.74656988202969</v>
       </c>
       <c r="C34" s="17">
-        <v>143.34241816439391</v>
+        <v>143.32605789671817</v>
       </c>
       <c r="D34" s="17">
-        <v>143.6572086184897</v>
+        <v>143.63522765340281</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3205,13 +3206,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="17">
-        <v>142.84327650513197</v>
+        <v>142.84327650512429</v>
       </c>
       <c r="C35" s="17">
-        <v>143.63465463934358</v>
+        <v>143.65190193506055</v>
       </c>
       <c r="D35" s="17">
-        <v>143.22008822439349</v>
+        <v>143.19714992777318</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3219,13 +3220,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="17">
-        <v>140.59240754477185</v>
+        <v>140.59240754476866</v>
       </c>
       <c r="C36" s="17">
-        <v>141.55875869260419</v>
+        <v>141.64761143529512</v>
       </c>
       <c r="D36" s="17">
-        <v>142.9383103511795</v>
+        <v>142.91452128621515</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,13 +3234,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="17">
-        <v>136.25161522905591</v>
+        <v>136.25161522906706</v>
       </c>
       <c r="C37" s="17">
-        <v>141.77798628895849</v>
+        <v>141.84453589926852</v>
       </c>
       <c r="D37" s="17">
-        <v>142.79933784015981</v>
+        <v>142.77506876208787</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3247,13 +3248,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="17">
-        <v>134.53623749895024</v>
+        <v>134.5362374989854</v>
       </c>
       <c r="C38" s="17">
-        <v>142.8892022226787</v>
+        <v>142.88146584238217</v>
       </c>
       <c r="D38" s="17">
-        <v>142.77753503073623</v>
+        <v>142.75340444881982</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3261,13 +3262,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="17">
-        <v>132.26788761886397</v>
+        <v>132.26788761887886</v>
       </c>
       <c r="C39" s="17">
-        <v>143.24397621594952</v>
+        <v>143.21529265234551</v>
       </c>
       <c r="D39" s="17">
-        <v>142.8366555380187</v>
+        <v>142.8136001859169</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3275,13 +3276,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="17">
-        <v>144.96325830736751</v>
+        <v>144.96325830731766</v>
       </c>
       <c r="C40" s="17">
-        <v>141.21927263217049</v>
+        <v>141.16766851783873</v>
       </c>
       <c r="D40" s="17">
-        <v>142.93696828520521</v>
+        <v>142.91593338618299</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,13 +3290,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="17">
-        <v>149.91623208225008</v>
+        <v>149.91623208209108</v>
       </c>
       <c r="C41" s="17">
-        <v>142.49250440943794</v>
+        <v>142.44260564141035</v>
       </c>
       <c r="D41" s="17">
-        <v>143.03779566296782</v>
+        <v>143.0191680536519</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3303,13 +3304,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="17">
-        <v>164.13570357737953</v>
+        <v>164.13570357731254</v>
       </c>
       <c r="C42" s="17">
-        <v>144.78650813021989</v>
+        <v>144.77251483265417</v>
       </c>
       <c r="D42" s="17">
-        <v>143.10188407986848</v>
+        <v>143.08565048556366</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,13 +3318,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="17">
-        <v>150.85895656094456</v>
+        <v>150.85895656117083</v>
       </c>
       <c r="C43" s="17">
-        <v>143.78034118841927</v>
+        <v>143.76548398780506</v>
       </c>
       <c r="D43" s="17">
-        <v>143.0943431486379</v>
+        <v>143.07992918998309</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3331,13 +3332,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="17">
-        <v>146.77698127386105</v>
+        <v>146.77698127458166</v>
       </c>
       <c r="C44" s="17">
-        <v>145.50646599201986</v>
+        <v>145.39650446492485</v>
       </c>
       <c r="D44" s="17">
-        <v>142.98710125619451</v>
+        <v>142.9732813765597</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3345,13 +3346,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="17">
-        <v>141.27691429278232</v>
+        <v>141.27691429308615</v>
       </c>
       <c r="C45" s="17">
-        <v>145.12811801440284</v>
+        <v>145.0647049277747</v>
       </c>
       <c r="D45" s="17">
-        <v>142.76032833820668</v>
+        <v>142.7451462285554</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3359,13 +3360,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="17">
-        <v>134.87713523420388</v>
+        <v>134.87713523317973</v>
       </c>
       <c r="C46" s="17">
-        <v>141.19442521657709</v>
+        <v>141.16339065994785</v>
       </c>
       <c r="D46" s="17">
-        <v>142.40469125597397</v>
+        <v>142.38558654632124</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3373,13 +3374,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="17">
-        <v>141.63955567778058</v>
+        <v>141.63955567451728</v>
       </c>
       <c r="C47" s="17">
-        <v>143.70258622947267</v>
+        <v>143.76981531221247</v>
       </c>
       <c r="D47" s="17">
-        <v>141.92233746989476</v>
+        <v>141.89644436785727</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3387,13 +3388,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="17">
-        <v>137.77192201114806</v>
+        <v>137.77192200977251</v>
       </c>
       <c r="C48" s="17">
-        <v>140.66496241027576</v>
+        <v>140.82149264141492</v>
       </c>
       <c r="D48" s="17">
-        <v>141.32521233085475</v>
+        <v>141.289836568585</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3401,13 +3402,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="17">
-        <v>135.7648431250517</v>
+        <v>135.76484312969083</v>
       </c>
       <c r="C49" s="17">
-        <v>140.17726477849718</v>
+        <v>140.32468795395246</v>
       </c>
       <c r="D49" s="17">
-        <v>140.64130181231408</v>
+        <v>140.59315294047627</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3415,13 +3416,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="17">
-        <v>132.15799379484065</v>
+        <v>132.15799380962139</v>
       </c>
       <c r="C50" s="17">
-        <v>140.66735184553832</v>
+        <v>140.67904053134899</v>
       </c>
       <c r="D50" s="17">
-        <v>139.90611786960301</v>
+        <v>139.84355567430572</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3429,13 +3430,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="17">
-        <v>129.68532873427284</v>
+        <v>129.68532874050351</v>
       </c>
       <c r="C51" s="17">
-        <v>140.15095614762484</v>
+        <v>140.10099707999618</v>
       </c>
       <c r="D51" s="17">
-        <v>139.16040490527027</v>
+        <v>139.08444401802092</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3443,13 +3444,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="17">
-        <v>129.44520372236295</v>
+        <v>129.4452037013518</v>
       </c>
       <c r="C52" s="17">
-        <v>125.80561913449993</v>
+        <v>125.72159645139192</v>
       </c>
       <c r="D52" s="17">
-        <v>138.44555126327614</v>
+        <v>138.36006291970392</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3457,13 +3458,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="17">
-        <v>111.93059539380501</v>
+        <v>111.93059532686038</v>
       </c>
       <c r="C53" s="17">
-        <v>105.17105359476452</v>
+        <v>105.1046641821371</v>
       </c>
       <c r="D53" s="17">
-        <v>137.80207580460984</v>
+        <v>137.71297519484409</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3471,13 +3472,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="17">
-        <v>131.24787226740779</v>
+        <v>131.24787223918833</v>
       </c>
       <c r="C54" s="17">
-        <v>116.76633024581852</v>
+        <v>116.71787148113103</v>
       </c>
       <c r="D54" s="17">
-        <v>137.26300651594465</v>
+        <v>137.17721937566057</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3485,13 +3486,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="17">
-        <v>133.09348386866952</v>
+        <v>133.0934839638339</v>
       </c>
       <c r="C55" s="17">
-        <v>124.29495938125814</v>
+        <v>124.25328646248698</v>
       </c>
       <c r="D55" s="17">
-        <v>136.85248238324112</v>
+        <v>136.77665864752683</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3499,13 +3500,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="17">
-        <v>128.24284760157738</v>
+        <v>128.24284790478424</v>
       </c>
       <c r="C56" s="17">
-        <v>126.82652113360706</v>
+        <v>126.64552515403477</v>
       </c>
       <c r="D56" s="17">
-        <v>136.58506202950926</v>
+        <v>136.52432275443365</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3513,13 +3514,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="17">
-        <v>125.13820239130484</v>
+        <v>125.13820251911724</v>
       </c>
       <c r="C57" s="17">
-        <v>129.49521442464768</v>
+        <v>129.3819762898612</v>
       </c>
       <c r="D57" s="17">
-        <v>136.46816760905986</v>
+        <v>136.42574330401877</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3527,13 +3528,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="17">
-        <v>126.53017409720285</v>
+        <v>126.5301736661838</v>
       </c>
       <c r="C58" s="17">
-        <v>131.15306267888315</v>
+        <v>131.13179669817799</v>
       </c>
       <c r="D58" s="17">
-        <v>136.49737500617613</v>
+        <v>136.47316517131264</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3541,13 +3542,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="17">
-        <v>131.61629042598079</v>
+        <v>131.61628905269333</v>
       </c>
       <c r="C59" s="17">
-        <v>134.05114767974581</v>
+        <v>134.19286226569571</v>
       </c>
       <c r="D59" s="17">
-        <v>136.66107810102523</v>
+        <v>136.65130870208512</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3555,13 +3556,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="17">
-        <v>132.88316976269164</v>
+        <v>132.88316918380275</v>
       </c>
       <c r="C60" s="17">
-        <v>135.01615310869295</v>
+        <v>135.27143785058203</v>
       </c>
       <c r="D60" s="17">
-        <v>136.94558019843319</v>
+        <v>136.94278399632844</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3569,13 +3570,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="17">
-        <v>132.30929821377384</v>
+        <v>132.30930016595045</v>
       </c>
       <c r="C61" s="17">
-        <v>134.88209106052307</v>
+        <v>135.07940598390283</v>
       </c>
       <c r="D61" s="17">
-        <v>137.33253350261248</v>
+        <v>137.32929146286472</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3583,13 +3584,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="17">
-        <v>129.61069203930271</v>
+        <v>129.61069825921177</v>
       </c>
       <c r="C62" s="17">
-        <v>139.85168048723571</v>
+        <v>139.87920625013007</v>
       </c>
       <c r="D62" s="17">
-        <v>137.80700223070565</v>
+        <v>137.79543913216662</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,13 +3598,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="17">
-        <v>126.88274350402092</v>
+        <v>126.88274612593136</v>
       </c>
       <c r="C63" s="17">
-        <v>137.99000868591637</v>
+        <v>137.94819065381114</v>
       </c>
       <c r="D63" s="17">
-        <v>138.35968947539223</v>
+        <v>138.33200143916417</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3611,13 +3612,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="17">
-        <v>147.05800492299821</v>
+        <v>147.05799608117897</v>
       </c>
       <c r="C64" s="17">
-        <v>140.5129452417481</v>
+        <v>140.33760340215474</v>
       </c>
       <c r="D64" s="17">
-        <v>138.98500914782772</v>
+        <v>138.93486202061874</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,13 +3626,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="17">
-        <v>144.90972331714073</v>
+        <v>144.90969514586067</v>
       </c>
       <c r="C65" s="17">
-        <v>137.90810202646128</v>
+        <v>137.80083870345672</v>
       </c>
       <c r="D65" s="17">
-        <v>139.67804492678229</v>
+        <v>139.60103326191395</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3639,13 +3640,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="17">
-        <v>150.49546716567752</v>
+        <v>150.49545529049234</v>
       </c>
       <c r="C66" s="17">
-        <v>137.32306193699105</v>
+        <v>137.25454377297802</v>
       </c>
       <c r="D66" s="17">
-        <v>140.4323847159458</v>
+        <v>140.32774087690987</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3653,13 +3654,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="17">
-        <v>149.13445495764941</v>
+        <v>149.13449500411494</v>
       </c>
       <c r="C67" s="17">
-        <v>140.5395462682803</v>
+        <v>140.48134628111507</v>
       </c>
       <c r="D67" s="17">
-        <v>141.2355781828052</v>
+        <v>141.10829997154894</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3667,13 +3668,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="17">
-        <v>142.80631771707249</v>
+        <v>142.80644531074435</v>
       </c>
       <c r="C68" s="17">
-        <v>141.95540441915369</v>
+        <v>141.70211913249832</v>
       </c>
       <c r="D68" s="17">
-        <v>142.07167905959997</v>
+        <v>141.93341494198324</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3681,13 +3682,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="17">
-        <v>141.05796746061472</v>
+        <v>141.05802124583437</v>
       </c>
       <c r="C69" s="17">
-        <v>144.5286668918184</v>
+        <v>144.38046699038483</v>
       </c>
       <c r="D69" s="17">
-        <v>142.92414249720608</v>
+        <v>142.78967852681285</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,13 +3696,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="17">
-        <v>140.84617576536496</v>
+        <v>140.84599438647376</v>
       </c>
       <c r="C70" s="17">
-        <v>145.35980980533893</v>
+        <v>145.40122095174848</v>
       </c>
       <c r="D70" s="17">
-        <v>143.77702201445061</v>
+        <v>143.66264957240395</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3709,13 +3710,13 @@
         <v>44470</v>
       </c>
       <c r="B71" s="17">
-        <v>140.5633495785417</v>
+        <v>140.56277167988108</v>
       </c>
       <c r="C71" s="17">
-        <v>144.50759119615745</v>
+        <v>144.69616451868598</v>
       </c>
       <c r="D71" s="17">
-        <v>144.61593690699561</v>
+        <v>144.5376991346985</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3723,13 +3724,13 @@
         <v>44501</v>
       </c>
       <c r="B72" s="17">
-        <v>145.46384851426734</v>
+        <v>145.46360490965989</v>
       </c>
       <c r="C72" s="17">
-        <v>146.22874448293129</v>
+        <v>146.54739710419332</v>
       </c>
       <c r="D72" s="17">
-        <v>145.42948330677413</v>
+        <v>145.40016491802103</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,13 +3738,13 @@
         <v>44531</v>
       </c>
       <c r="B73" s="17">
-        <v>146.02985015135357</v>
+        <v>146.03067165462195</v>
       </c>
       <c r="C73" s="17">
-        <v>148.15303240439849</v>
+        <v>148.42949606976043</v>
       </c>
       <c r="D73" s="17">
-        <v>146.20825479854994</v>
+        <v>146.23548339305833</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3751,13 +3752,13 @@
         <v>44562</v>
       </c>
       <c r="B74" s="17">
-        <v>136.16705638256084</v>
+        <v>136.16967380752766</v>
       </c>
       <c r="C74" s="17">
-        <v>147.12650428465804</v>
+        <v>147.23422214808681</v>
       </c>
       <c r="D74" s="17">
-        <v>146.94405632880586</v>
+        <v>147.03166789730989</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3765,13 +3766,13 @@
         <v>44593</v>
       </c>
       <c r="B75" s="17">
-        <v>137.61605600266572</v>
+        <v>137.61715933933209</v>
       </c>
       <c r="C75" s="17">
-        <v>148.84575499812308</v>
+        <v>148.85552038412391</v>
       </c>
       <c r="D75" s="17">
-        <v>147.63256921887074</v>
+        <v>147.78066383873758</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3779,13 +3780,13 @@
         <v>44621</v>
       </c>
       <c r="B76" s="17">
-        <v>153.93276547580172</v>
+        <v>153.92904471416887</v>
       </c>
       <c r="C76" s="17">
-        <v>148.0914237703972</v>
+        <v>147.82211063790649</v>
       </c>
       <c r="D76" s="17">
-        <v>148.27339211298866</v>
+        <v>148.47954122952919</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3793,13 +3794,13 @@
         <v>44652</v>
       </c>
       <c r="B77" s="17">
-        <v>153.38628948547043</v>
+        <v>153.42927067661543</v>
       </c>
       <c r="C77" s="17">
-        <v>148.93521555849219</v>
+        <v>148.6272707738834</v>
       </c>
       <c r="D77" s="17">
-        <v>148.87222050017624</v>
+        <v>149.13247230389123</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,13 +3808,13 @@
         <v>44682</v>
       </c>
       <c r="B78" s="17">
-        <v>162.38433403843436</v>
+        <v>162.36956646957179</v>
       </c>
       <c r="C78" s="17">
-        <v>149.06106096478484</v>
+        <v>148.85765239579808</v>
       </c>
       <c r="D78" s="17">
-        <v>149.44108343357962</v>
+        <v>149.74859581019382</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3821,13 +3822,13 @@
         <v>44713</v>
       </c>
       <c r="B79" s="17">
-        <v>159.61897013645768</v>
+        <v>159.59075651417527</v>
       </c>
       <c r="C79" s="17">
-        <v>150.69730338838366</v>
+        <v>150.81494224018516</v>
       </c>
       <c r="D79" s="17">
-        <v>149.99498950557097</v>
+        <v>150.3400992818124</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,13 +3836,13 @@
         <v>44743</v>
       </c>
       <c r="B80" s="17">
-        <v>151.18168336185485</v>
+        <v>151.26536125023031</v>
       </c>
       <c r="C80" s="17">
-        <v>150.85822741648312</v>
+        <v>151.37012851826515</v>
       </c>
       <c r="D80" s="17">
-        <v>150.54840449801696</v>
+        <v>150.92028290133237</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3849,13 +3850,27 @@
         <v>44774</v>
       </c>
       <c r="B81" s="17">
-        <v>150.09171593050851</v>
+        <v>150.32807739350432</v>
       </c>
       <c r="C81" s="17">
-        <v>151.40709151954758</v>
+        <v>152.44244407206827</v>
       </c>
       <c r="D81" s="17">
-        <v>151.1114611234853</v>
+        <v>151.49886737458965</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>44805</v>
+      </c>
+      <c r="B82" s="44">
+        <v>147.54987496056535</v>
+      </c>
+      <c r="C82" s="44">
+        <v>152.02935683288021</v>
+      </c>
+      <c r="D82" s="44">
+        <v>152.08181081617525</v>
       </c>
     </row>
   </sheetData>
@@ -3868,7 +3883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6808,14 +6823,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="29">
-        <v>11690</v>
+        <v>13092</v>
       </c>
       <c r="C2" s="29">
-        <v>15276</v>
+        <v>16758</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-3586</v>
+        <v>-3666</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6823,14 +6838,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="29">
-        <v>3728</v>
+        <v>4156</v>
       </c>
       <c r="C3" s="29">
-        <v>609</v>
+        <v>666</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>3119</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6838,14 +6853,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="29">
-        <v>3922</v>
+        <v>4344</v>
       </c>
       <c r="C4" s="29">
-        <v>2703</v>
+        <v>3007</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1219</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6853,14 +6868,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="29">
-        <v>1107</v>
+        <v>1281</v>
       </c>
       <c r="C5" s="29">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1082</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6868,14 +6883,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="29">
-        <v>6617</v>
+        <v>7454</v>
       </c>
       <c r="C6" s="29">
-        <v>10279</v>
+        <v>11098</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-3662</v>
+        <v>-3644</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6883,14 +6898,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="29">
-        <v>8031</v>
+        <v>9208</v>
       </c>
       <c r="C7" s="29">
-        <v>8604</v>
+        <v>9539</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-573</v>
+        <v>-331</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6898,14 +6913,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="29">
-        <v>496</v>
+        <v>589</v>
       </c>
       <c r="C8" s="29">
-        <v>507</v>
+        <v>553</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6913,14 +6928,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="29">
-        <v>826</v>
+        <v>910</v>
       </c>
       <c r="C9" s="29">
-        <v>475</v>
+        <v>513</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>351</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6928,14 +6943,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="29">
-        <v>399</v>
+        <v>486</v>
       </c>
       <c r="C10" s="29">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6943,14 +6958,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="29">
-        <v>6060</v>
+        <v>6555</v>
       </c>
       <c r="C11" s="29">
-        <v>3251</v>
+        <v>3582</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2809</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6958,14 +6973,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="29">
-        <v>5212</v>
+        <v>6838</v>
       </c>
       <c r="C12" s="29">
-        <v>13356</v>
+        <v>14858</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-8144</v>
+        <v>-8020</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6973,14 +6988,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="29">
-        <v>1576</v>
+        <v>1730</v>
       </c>
       <c r="C13" s="29">
-        <v>566</v>
+        <v>609</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1010</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6988,14 +7003,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="29">
-        <v>658</v>
+        <v>710</v>
       </c>
       <c r="C14" s="29">
-        <v>887</v>
+        <v>974</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-229</v>
+        <v>-264</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7003,14 +7018,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="29">
-        <v>3637</v>
+        <v>3800</v>
       </c>
       <c r="C15" s="29">
-        <v>1444</v>
+        <v>1655</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>2193</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7018,14 +7033,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="29">
-        <v>3914</v>
+        <v>4141</v>
       </c>
       <c r="C16" s="29">
-        <v>2346</v>
+        <v>2385</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1568</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7033,14 +7048,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="29">
-        <v>3332</v>
+        <v>3539</v>
       </c>
       <c r="C17" s="29">
-        <v>984</v>
+        <v>1108</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2348</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7048,14 +7063,14 @@
         <v>95</v>
       </c>
       <c r="B18" s="29">
-        <v>377</v>
+        <v>409</v>
       </c>
       <c r="C18" s="29">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7063,14 +7078,14 @@
         <v>96</v>
       </c>
       <c r="B19" s="29">
-        <v>659</v>
+        <v>746</v>
       </c>
       <c r="C19" s="29">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>259</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7078,14 +7093,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="30">
-        <v>4891</v>
+        <v>5157</v>
       </c>
       <c r="C20" s="30">
-        <v>2270</v>
+        <v>2433</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2621</v>
+        <v>2724</v>
       </c>
     </row>
   </sheetData>
@@ -7098,9 +7113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D5C2F3-2F50-487E-8AA2-1FC33A905845}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B53"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7120,7 +7133,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="35">
-        <v>67131</v>
+        <v>75144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7128,7 +7141,7 @@
         <v>185</v>
       </c>
       <c r="B3" s="35">
-        <v>18746</v>
+        <v>21116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7136,7 +7149,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="29">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7144,7 +7157,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="29">
-        <v>1241</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7152,7 +7165,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="29">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7160,7 +7173,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="29">
-        <v>491</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7168,7 +7181,7 @@
         <v>142</v>
       </c>
       <c r="B8" s="29">
-        <v>460</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7176,7 +7189,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="29">
-        <v>13332</v>
+        <v>14047</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7184,7 +7197,7 @@
         <v>144</v>
       </c>
       <c r="B10" s="29">
-        <v>2313</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7192,7 +7205,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="29">
-        <v>176</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7208,7 +7221,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="29">
-        <v>151</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7216,7 +7229,7 @@
         <v>148</v>
       </c>
       <c r="B14" s="29">
-        <v>221</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7224,7 +7237,7 @@
         <v>149</v>
       </c>
       <c r="B15" s="29">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7232,7 +7245,7 @@
         <v>186</v>
       </c>
       <c r="B16" s="35">
-        <v>25350</v>
+        <v>27899</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7240,7 +7253,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="29">
-        <v>3283</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7248,7 +7261,7 @@
         <v>151</v>
       </c>
       <c r="B18" s="29">
-        <v>186</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7256,7 +7269,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="29">
-        <v>1035</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7264,7 +7277,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="29">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7272,7 +7285,7 @@
         <v>154</v>
       </c>
       <c r="B21" s="29">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7280,7 +7293,7 @@
         <v>155</v>
       </c>
       <c r="B22" s="29">
-        <v>130</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7288,7 +7301,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="29">
-        <v>758</v>
+        <v>825</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7296,7 +7309,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="29">
-        <v>7401</v>
+        <v>7832</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7304,7 +7317,7 @@
         <v>158</v>
       </c>
       <c r="B25" s="29">
-        <v>207</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7312,7 +7325,7 @@
         <v>159</v>
       </c>
       <c r="B26" s="29">
-        <v>618</v>
+        <v>694</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7320,7 +7333,7 @@
         <v>160</v>
       </c>
       <c r="B27" s="29">
-        <v>722</v>
+        <v>814</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7328,7 +7341,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="29">
-        <v>9814</v>
+        <v>10976</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7336,7 +7349,7 @@
         <v>162</v>
       </c>
       <c r="B29" s="29">
-        <v>223</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7344,7 +7357,7 @@
         <v>163</v>
       </c>
       <c r="B30" s="29">
-        <v>354</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7352,7 +7365,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="29">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7360,7 +7373,7 @@
         <v>165</v>
       </c>
       <c r="B32" s="29">
-        <v>395</v>
+        <v>436</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7368,7 +7381,7 @@
         <v>187</v>
       </c>
       <c r="B33" s="35">
-        <v>17024</v>
+        <v>19263</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7376,7 +7389,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="29">
-        <v>4512</v>
+        <v>5132</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7384,7 +7397,7 @@
         <v>167</v>
       </c>
       <c r="B35" s="29">
-        <v>859</v>
+        <v>926</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7392,7 +7405,7 @@
         <v>168</v>
       </c>
       <c r="B36" s="29">
-        <v>180</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7400,7 +7413,7 @@
         <v>169</v>
       </c>
       <c r="B37" s="29">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7408,7 +7421,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="29">
-        <v>348</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7416,7 +7429,7 @@
         <v>171</v>
       </c>
       <c r="B39" s="29">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7424,7 +7437,7 @@
         <v>172</v>
       </c>
       <c r="B40" s="29">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -7432,7 +7445,7 @@
         <v>173</v>
       </c>
       <c r="B41" s="29">
-        <v>131</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -7440,7 +7453,7 @@
         <v>174</v>
       </c>
       <c r="B42" s="29">
-        <v>2040</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -7448,7 +7461,7 @@
         <v>175</v>
       </c>
       <c r="B43" s="29">
-        <v>1596</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -7456,7 +7469,7 @@
         <v>176</v>
       </c>
       <c r="B44" s="29">
-        <v>1160</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -7464,7 +7477,7 @@
         <v>177</v>
       </c>
       <c r="B45" s="29">
-        <v>5606</v>
+        <v>6493</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -7472,7 +7485,7 @@
         <v>178</v>
       </c>
       <c r="B46" s="29">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7480,7 +7493,7 @@
         <v>179</v>
       </c>
       <c r="B47" s="29">
-        <v>218</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -7488,7 +7501,7 @@
         <v>188</v>
       </c>
       <c r="B48" s="35">
-        <v>6010</v>
+        <v>6866</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7496,7 +7509,7 @@
         <v>180</v>
       </c>
       <c r="B49" s="29">
-        <v>2798</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7504,7 +7517,7 @@
         <v>181</v>
       </c>
       <c r="B50" s="29">
-        <v>1872</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7512,7 +7525,7 @@
         <v>182</v>
       </c>
       <c r="B51" s="29">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7520,7 +7533,7 @@
         <v>183</v>
       </c>
       <c r="B52" s="41">
-        <v>923</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -7528,7 +7541,7 @@
         <v>184</v>
       </c>
       <c r="B53" s="42">
-        <v>347</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -7541,7 +7554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B40"/>
     </sheetView>
   </sheetViews>
@@ -7563,7 +7576,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="35">
-        <v>64520</v>
+        <v>70738</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7571,7 +7584,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="35">
-        <v>9514</v>
+        <v>10510</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7579,7 +7592,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="29">
-        <v>7120</v>
+        <v>7898</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7587,7 +7600,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="29">
-        <v>1036</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7595,7 +7608,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="29">
-        <v>1010</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7603,7 +7616,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="29">
-        <v>348</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7611,7 +7624,7 @@
         <v>211</v>
       </c>
       <c r="B8" s="35">
-        <v>23744</v>
+        <v>26077</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7619,7 +7632,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="29">
-        <v>2270</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7627,7 +7640,7 @@
         <v>195</v>
       </c>
       <c r="B10" s="29">
-        <v>1116</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7635,7 +7648,7 @@
         <v>196</v>
       </c>
       <c r="B11" s="29">
-        <v>9730</v>
+        <v>10801</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7643,7 +7656,7 @@
         <v>197</v>
       </c>
       <c r="B12" s="29">
-        <v>2943</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7651,7 +7664,7 @@
         <v>198</v>
       </c>
       <c r="B13" s="29">
-        <v>935</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7659,7 +7672,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="29">
-        <v>1083</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7667,7 +7680,7 @@
         <v>200</v>
       </c>
       <c r="B15" s="29">
-        <v>551</v>
+        <v>594</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7675,7 +7688,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="29">
-        <v>3364</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7683,7 +7696,7 @@
         <v>202</v>
       </c>
       <c r="B17" s="29">
-        <v>1751</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7691,7 +7704,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="35">
-        <v>11213</v>
+        <v>11959</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7699,7 +7712,7 @@
         <v>195</v>
       </c>
       <c r="B19" s="29">
-        <v>10947</v>
+        <v>11657</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7707,7 +7720,7 @@
         <v>203</v>
       </c>
       <c r="B20" s="29">
-        <v>266</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7715,7 +7728,7 @@
         <v>213</v>
       </c>
       <c r="B21" s="35">
-        <v>11490</v>
+        <v>12721</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7723,7 +7736,7 @@
         <v>190</v>
       </c>
       <c r="B22" s="29">
-        <v>7470</v>
+        <v>8252</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7731,7 +7744,7 @@
         <v>191</v>
       </c>
       <c r="B23" s="29">
-        <v>3191</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7739,7 +7752,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="29">
-        <v>829</v>
+        <v>915</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7747,7 +7760,7 @@
         <v>214</v>
       </c>
       <c r="B25" s="35">
-        <v>6553</v>
+        <v>7229</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7755,7 +7768,7 @@
         <v>205</v>
       </c>
       <c r="B26" s="29">
-        <v>232</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7763,7 +7776,7 @@
         <v>194</v>
       </c>
       <c r="B27" s="29">
-        <v>473</v>
+        <v>520</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7771,7 +7784,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="29">
-        <v>612</v>
+        <v>672</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7779,7 +7792,7 @@
         <v>196</v>
       </c>
       <c r="B29" s="29">
-        <v>1932</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7787,7 +7800,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="29">
-        <v>404</v>
+        <v>443</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7795,7 +7808,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="29">
-        <v>321</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7803,7 +7816,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="29">
-        <v>516</v>
+        <v>579</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7811,7 +7824,7 @@
         <v>190</v>
       </c>
       <c r="B33" s="29">
-        <v>504</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7819,7 +7832,7 @@
         <v>191</v>
       </c>
       <c r="B34" s="29">
-        <v>435</v>
+        <v>490</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7827,7 +7840,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="29">
-        <v>239</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7835,7 +7848,7 @@
         <v>208</v>
       </c>
       <c r="B36" s="29">
-        <v>430</v>
+        <v>478</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7843,7 +7856,7 @@
         <v>209</v>
       </c>
       <c r="B37" s="29">
-        <v>456</v>
+        <v>502</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7851,7 +7864,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="35">
-        <v>1504</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7859,7 +7872,7 @@
         <v>191</v>
       </c>
       <c r="B39" s="39">
-        <v>1504</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7867,7 +7880,7 @@
         <v>216</v>
       </c>
       <c r="B40" s="40">
-        <v>503</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo comex, pib, vab, resultado fiscal, todos datos publicados en diciembre"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F99382-8C00-4EC3-A5D5-2AEB6CFC4473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302D5D3E-73CA-454C-87C2-1F4CAE071FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="218">
   <si>
     <t>Período</t>
   </si>
@@ -2515,7 +2515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2539,10 +2539,10 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>644818.80193734274</v>
+        <v>604239.82005176414</v>
       </c>
       <c r="C2">
-        <v>6.6210290853380798</v>
+        <v>6.1627049964170677</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2550,10 +2550,10 @@
         <v>102</v>
       </c>
       <c r="B3">
-        <v>84508.536911229836</v>
+        <v>34609.850082682562</v>
       </c>
       <c r="C3">
-        <v>-5.2284200767613669</v>
+        <v>-0.7600608736383907</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,10 +2561,10 @@
         <v>103</v>
       </c>
       <c r="B4">
-        <v>2803.8809597629624</v>
+        <v>3683.9182903702886</v>
       </c>
       <c r="C4">
-        <v>24.121911238365911</v>
+        <v>-1.4690049688209195</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2572,10 +2572,10 @@
         <v>104</v>
       </c>
       <c r="B5">
-        <v>23988.049228966476</v>
+        <v>24815.413011887398</v>
       </c>
       <c r="C5">
-        <v>15.455171845229259</v>
+        <v>14.359903604077505</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,10 +2583,10 @@
         <v>105</v>
       </c>
       <c r="B6">
-        <v>125030.84005626102</v>
+        <v>128077.84352465972</v>
       </c>
       <c r="C6">
-        <v>7.6582005417364059</v>
+        <v>6.3895704518543317</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2594,10 +2594,10 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <v>13357.03357278303</v>
+        <v>12900.731841850526</v>
       </c>
       <c r="C7">
-        <v>4.8661425735229784</v>
+        <v>-3.6461925708421439</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,10 +2605,10 @@
         <v>107</v>
       </c>
       <c r="B8">
-        <v>20926.460098286607</v>
+        <v>22693.628212376221</v>
       </c>
       <c r="C8">
-        <v>9.9177971809852892</v>
+        <v>7.5419163076783313</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>108</v>
       </c>
       <c r="B9">
-        <v>99050.868361418325</v>
+        <v>98360.582675962229</v>
       </c>
       <c r="C9">
-        <v>9.6644054198416143</v>
+        <v>7.3452431993092926</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2627,10 +2627,10 @@
         <v>109</v>
       </c>
       <c r="B10">
-        <v>8605.1734059229329</v>
+        <v>10062.077919942609</v>
       </c>
       <c r="C10">
-        <v>53.937982935729877</v>
+        <v>37.257757147650253</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,10 +2638,10 @@
         <v>110</v>
       </c>
       <c r="B11">
-        <v>58863.534191324492</v>
+        <v>54466.722677375285</v>
       </c>
       <c r="C11">
-        <v>11.462822586038698</v>
+        <v>8.3012935180134093</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,10 +2649,10 @@
         <v>111</v>
       </c>
       <c r="B12">
-        <v>25026.616863292602</v>
+        <v>25325.660388867425</v>
       </c>
       <c r="C12">
-        <v>2.0010111212931179</v>
+        <v>0.11972507097841589</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,10 +2660,10 @@
         <v>112</v>
       </c>
       <c r="B13">
-        <v>80068.369728395061</v>
+        <v>81395.539159269145</v>
       </c>
       <c r="C13">
-        <v>6.3803492775227397</v>
+        <v>5.7724516292565031</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,10 +2671,10 @@
         <v>113</v>
       </c>
       <c r="B14">
-        <v>35036.769725331389</v>
+        <v>35045.475513507183</v>
       </c>
       <c r="C14">
-        <v>10.153457492304568</v>
+        <v>7.1450044565892989</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,10 +2682,10 @@
         <v>114</v>
       </c>
       <c r="B15">
-        <v>28219.35604362089</v>
+        <v>28731.347627695432</v>
       </c>
       <c r="C15">
-        <v>6.0944271712824616</v>
+        <v>4.5054769107826909</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2693,10 +2693,10 @@
         <v>115</v>
       </c>
       <c r="B16">
-        <v>22412.972859499903</v>
+        <v>24147.558005581537</v>
       </c>
       <c r="C16">
-        <v>1.0149697709420167</v>
+        <v>0.91081857301009705</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2704,10 +2704,10 @@
         <v>116</v>
       </c>
       <c r="B17">
-        <v>13200.261286340125</v>
+        <v>15951.253364358658</v>
       </c>
       <c r="C17">
-        <v>8.5935478547673796</v>
+        <v>9.7667034880939863</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2715,10 +2715,10 @@
         <v>117</v>
       </c>
       <c r="B18">
-        <v>3720.0786449073389</v>
+        <v>3972.2177553779075</v>
       </c>
       <c r="C18">
-        <v>9.9078855195906499</v>
+        <v>4.26482342152259</v>
       </c>
     </row>
   </sheetData>
@@ -2729,11 +2729,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2764,10 +2762,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="17">
-        <v>148.19237985851987</v>
+        <v>148.0650628528569</v>
       </c>
       <c r="D2" s="17">
-        <v>147.0484965554339</v>
+        <v>147.16062971742542</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2778,10 +2776,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="17">
-        <v>146.772631667143</v>
+        <v>146.9075304079289</v>
       </c>
       <c r="D3" s="17">
-        <v>146.45835108905862</v>
+        <v>146.57463454067693</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2792,10 +2790,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="17">
-        <v>145.91464750278519</v>
+        <v>145.92830487193189</v>
       </c>
       <c r="D4" s="17">
-        <v>145.90478393857433</v>
+        <v>146.01982728733202</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2806,10 +2804,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="17">
-        <v>145.06982544038877</v>
+        <v>144.94388170802097</v>
       </c>
       <c r="D5" s="17">
-        <v>145.4242365325272</v>
+        <v>145.53315242166636</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2820,10 +2818,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="17">
-        <v>144.26546872255503</v>
+        <v>144.29815974818419</v>
       </c>
       <c r="D6" s="17">
-        <v>145.04357492377943</v>
+        <v>145.142178097612</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2834,10 +2832,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="17">
-        <v>144.21001669651557</v>
+        <v>144.29446749597443</v>
       </c>
       <c r="D7" s="17">
-        <v>144.78275712690339</v>
+        <v>144.8677964880095</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2848,10 +2846,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="17">
-        <v>144.42344466410671</v>
+        <v>144.53502610100892</v>
       </c>
       <c r="D8" s="17">
-        <v>144.65140896087902</v>
+        <v>144.72101713607358</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2862,10 +2860,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="17">
-        <v>145.70503167880955</v>
+        <v>145.64580941505207</v>
       </c>
       <c r="D9" s="17">
-        <v>144.65376776304643</v>
+        <v>144.70790273343761</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2876,10 +2874,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="17">
-        <v>145.20010211132509</v>
+        <v>145.12993257741965</v>
       </c>
       <c r="D10" s="17">
-        <v>144.78957224151426</v>
+        <v>144.82990846152947</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2890,10 +2888,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="17">
-        <v>145.11420120174424</v>
+        <v>145.02458430845522</v>
       </c>
       <c r="D11" s="17">
-        <v>145.04982646793803</v>
+        <v>145.07945532736332</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2904,10 +2902,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="17">
-        <v>145.64550638376957</v>
+        <v>145.66752245028053</v>
       </c>
       <c r="D12" s="17">
-        <v>145.4191119623859</v>
+        <v>145.44244899141765</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2918,10 +2916,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="17">
-        <v>147.0580978054125</v>
+        <v>147.13107179805505</v>
       </c>
       <c r="D13" s="17">
-        <v>145.88366293115357</v>
+        <v>145.9048249703755</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2932,10 +2930,10 @@
         <v>136.6326594831489</v>
       </c>
       <c r="C14" s="17">
-        <v>147.43320478790372</v>
+        <v>147.40210317604033</v>
       </c>
       <c r="D14" s="17">
-        <v>146.42619577334546</v>
+        <v>146.44853008350006</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2946,10 +2944,10 @@
         <v>132.15851633981728</v>
       </c>
       <c r="C15" s="17">
-        <v>146.49117562075543</v>
+        <v>146.6865832282453</v>
       </c>
       <c r="D15" s="17">
-        <v>147.02838672422746</v>
+        <v>147.05389879204489</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2960,10 +2958,10 @@
         <v>152.6209585590764</v>
       </c>
       <c r="C16" s="17">
-        <v>147.84473820642441</v>
+        <v>147.73440044060894</v>
       </c>
       <c r="D16" s="17">
-        <v>147.6698488064871</v>
+        <v>147.69916752155194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2974,10 +2972,10 @@
         <v>151.94634480454781</v>
       </c>
       <c r="C17" s="17">
-        <v>147.68388730388446</v>
+        <v>147.77019822655461</v>
       </c>
       <c r="D17" s="17">
-        <v>148.32745093057247</v>
+        <v>148.36044522152838</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2988,10 +2986,10 @@
         <v>168.38920946939336</v>
       </c>
       <c r="C18" s="17">
-        <v>148.56489835625939</v>
+        <v>148.44457269750393</v>
       </c>
       <c r="D18" s="17">
-        <v>148.97285579803167</v>
+        <v>149.00862379953398</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,10 +3000,10 @@
         <v>161.03568546936674</v>
       </c>
       <c r="C19" s="17">
-        <v>150.20546386180385</v>
+        <v>150.20856841045313</v>
       </c>
       <c r="D19" s="17">
-        <v>149.57431978540046</v>
+        <v>149.61248161164602</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3016,10 +3014,10 @@
         <v>150.306050123647</v>
       </c>
       <c r="C20" s="17">
-        <v>150.35783910469979</v>
+        <v>150.32413268885281</v>
       </c>
       <c r="D20" s="17">
-        <v>150.09813070893708</v>
+        <v>150.13859742503777</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3030,10 +3028,10 @@
         <v>149.25534277372614</v>
       </c>
       <c r="C21" s="17">
-        <v>150.43124703370367</v>
+        <v>150.43598525592051</v>
       </c>
       <c r="D21" s="17">
-        <v>150.50953103673018</v>
+        <v>150.55255742055374</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3044,10 +3042,10 @@
         <v>146.38655965814226</v>
       </c>
       <c r="C22" s="17">
-        <v>151.33232435872102</v>
+        <v>151.32734251369416</v>
       </c>
       <c r="D22" s="17">
-        <v>150.77460329212673</v>
+        <v>150.82035212514253</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3058,10 +3056,10 @@
         <v>149.38594966725174</v>
       </c>
       <c r="C23" s="17">
-        <v>151.5725317541775</v>
+        <v>151.52851832000425</v>
       </c>
       <c r="D23" s="17">
-        <v>150.86773884092668</v>
+        <v>150.916554352096</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3072,10 +3070,10 @@
         <v>151.92604285254853</v>
       </c>
       <c r="C24" s="17">
-        <v>152.50623901328706</v>
+        <v>152.52949564070778</v>
       </c>
       <c r="D24" s="17">
-        <v>150.76923027880255</v>
+        <v>150.82088726994988</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3083,13 +3081,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="17">
-        <v>146.78338490746614</v>
+        <v>146.78338490746617</v>
       </c>
       <c r="C25" s="17">
-        <v>152.4031548888702</v>
+        <v>152.43480369407132</v>
       </c>
       <c r="D25" s="17">
-        <v>150.4710379449985</v>
+        <v>150.5246437249447</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3100,10 +3098,10 @@
         <v>142.7409126005696</v>
       </c>
       <c r="C26" s="17">
-        <v>151.94176989323091</v>
+        <v>151.82991809905184</v>
       </c>
       <c r="D26" s="17">
-        <v>149.98049897471174</v>
+        <v>150.03522760546565</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3114,10 +3112,10 @@
         <v>138.81804034929579</v>
       </c>
       <c r="C27" s="17">
-        <v>151.84535798859653</v>
+        <v>151.96207126250218</v>
       </c>
       <c r="D27" s="17">
-        <v>149.31968556431585</v>
+        <v>149.3747653829968</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3128,10 +3126,10 @@
         <v>155.85731954373435</v>
       </c>
       <c r="C28" s="17">
-        <v>151.15416554311437</v>
+        <v>151.2655514784459</v>
       </c>
       <c r="D28" s="17">
-        <v>148.52284338027204</v>
+        <v>148.57773886815133</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,10 +3140,10 @@
         <v>151.52454400931953</v>
       </c>
       <c r="C29" s="17">
-        <v>146.77655533760023</v>
+        <v>146.84942820963926</v>
       </c>
       <c r="D29" s="17">
-        <v>147.63583734163745</v>
+        <v>147.68990700101085</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,13 +3151,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="17">
-        <v>159.56669238861372</v>
+        <v>159.56669238861366</v>
       </c>
       <c r="C30" s="17">
-        <v>144.4852804564421</v>
+        <v>144.3509902622736</v>
       </c>
       <c r="D30" s="17">
-        <v>146.71107890987963</v>
+        <v>146.76423733470699</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,13 +3165,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="17">
-        <v>151.1257631973825</v>
+        <v>151.12576319738255</v>
       </c>
       <c r="C31" s="17">
-        <v>143.10209365349945</v>
+        <v>143.09737349619945</v>
       </c>
       <c r="D31" s="17">
-        <v>145.80254451716149</v>
+        <v>145.85476572538985</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3181,13 +3179,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="17">
-        <v>145.9635243150716</v>
+        <v>145.96352431507171</v>
       </c>
       <c r="C32" s="17">
-        <v>143.28539587530634</v>
+        <v>143.26162965761117</v>
       </c>
       <c r="D32" s="17">
-        <v>144.95977751501192</v>
+        <v>145.01122776495876</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3195,13 +3193,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="17">
-        <v>146.76595998569144</v>
+        <v>146.7659599856915</v>
       </c>
       <c r="C33" s="17">
-        <v>146.73589981414585</v>
+        <v>146.7393591773432</v>
       </c>
       <c r="D33" s="17">
-        <v>144.22734431295893</v>
+        <v>144.27758437864924</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3209,13 +3207,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="17">
-        <v>137.74656988202969</v>
+        <v>137.74656988202952</v>
       </c>
       <c r="C34" s="17">
-        <v>143.32605789671817</v>
+        <v>143.29100993151249</v>
       </c>
       <c r="D34" s="17">
-        <v>143.63522765340281</v>
+        <v>143.68290235280026</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3223,13 +3221,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="17">
-        <v>142.84327650512429</v>
+        <v>142.84327650512373</v>
       </c>
       <c r="C35" s="17">
-        <v>143.65190193506055</v>
+        <v>143.54603232318621</v>
       </c>
       <c r="D35" s="17">
-        <v>143.19714992777318</v>
+        <v>143.24031204669467</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3237,13 +3235,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="17">
-        <v>140.59240754476866</v>
+        <v>140.59240754476843</v>
       </c>
       <c r="C36" s="17">
-        <v>141.64761143529512</v>
+        <v>141.61375455448996</v>
       </c>
       <c r="D36" s="17">
-        <v>142.91452128621515</v>
+        <v>142.95100533555495</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,13 +3249,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="17">
-        <v>136.25161522906706</v>
+        <v>136.25161522906785</v>
       </c>
       <c r="C37" s="17">
-        <v>141.84453589926852</v>
+        <v>141.98950727812081</v>
       </c>
       <c r="D37" s="17">
-        <v>142.77506876208787</v>
+        <v>142.80273508665451</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3265,13 +3263,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="17">
-        <v>134.5362374989854</v>
+        <v>134.53623749898799</v>
       </c>
       <c r="C38" s="17">
-        <v>142.88146584238217</v>
+        <v>142.8973872145053</v>
       </c>
       <c r="D38" s="17">
-        <v>142.75340444881982</v>
+        <v>142.77095602943402</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3279,13 +3277,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="17">
-        <v>132.26788761887886</v>
+        <v>132.26788761887991</v>
       </c>
       <c r="C39" s="17">
-        <v>143.21529265234551</v>
+        <v>143.20357057444366</v>
       </c>
       <c r="D39" s="17">
-        <v>142.8136001859169</v>
+        <v>142.82022724008482</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3293,13 +3291,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="17">
-        <v>144.96325830731766</v>
+        <v>144.96325830731405</v>
       </c>
       <c r="C40" s="17">
-        <v>141.16766851783873</v>
+        <v>141.38388914585209</v>
       </c>
       <c r="D40" s="17">
-        <v>142.91593338618299</v>
+        <v>142.91215659973219</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3307,13 +3305,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="17">
-        <v>149.91623208209108</v>
+        <v>149.9162320820796</v>
       </c>
       <c r="C41" s="17">
-        <v>142.44260564141035</v>
+        <v>142.65095554294282</v>
       </c>
       <c r="D41" s="17">
-        <v>143.0191680536519</v>
+        <v>143.00748813763317</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,13 +3319,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="17">
-        <v>164.13570357731254</v>
+        <v>164.13570357730771</v>
       </c>
       <c r="C42" s="17">
-        <v>144.77251483265417</v>
+        <v>144.57034012513461</v>
       </c>
       <c r="D42" s="17">
-        <v>143.08565048556366</v>
+        <v>143.07025963437189</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3335,13 +3333,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="17">
-        <v>150.85895656117083</v>
+        <v>150.85895656118743</v>
       </c>
       <c r="C43" s="17">
-        <v>143.76548398780506</v>
+        <v>143.61368189454609</v>
       </c>
       <c r="D43" s="17">
-        <v>143.07992918998309</v>
+        <v>143.06610950201841</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3349,13 +3347,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="17">
-        <v>146.77698127458166</v>
+        <v>146.77698127463378</v>
       </c>
       <c r="C44" s="17">
-        <v>145.39650446492485</v>
+        <v>145.37675682299056</v>
       </c>
       <c r="D44" s="17">
-        <v>142.9732813765597</v>
+        <v>142.96697525486996</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3363,13 +3361,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="17">
-        <v>141.27691429308615</v>
+        <v>141.27691429310812</v>
       </c>
       <c r="C45" s="17">
-        <v>145.0647049277747</v>
+        <v>145.08993748228016</v>
       </c>
       <c r="D45" s="17">
-        <v>142.7451462285554</v>
+        <v>142.75199125542613</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3377,13 +3375,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="17">
-        <v>134.87713523317973</v>
+        <v>134.87713523310566</v>
       </c>
       <c r="C46" s="17">
-        <v>141.16339065994785</v>
+        <v>141.07066978807862</v>
       </c>
       <c r="D46" s="17">
-        <v>142.38558654632124</v>
+        <v>142.41014971948846</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3391,13 +3389,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="17">
-        <v>141.63955567451728</v>
+        <v>141.63955567428133</v>
       </c>
       <c r="C47" s="17">
-        <v>143.76981531221247</v>
+        <v>143.80652842066678</v>
       </c>
       <c r="D47" s="17">
-        <v>141.89644436785727</v>
+        <v>141.94164969889943</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3405,13 +3403,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="17">
-        <v>137.77192200977251</v>
+        <v>137.77192200967303</v>
       </c>
       <c r="C48" s="17">
-        <v>140.82149264141492</v>
+        <v>140.79735348527882</v>
       </c>
       <c r="D48" s="17">
-        <v>141.289836568585</v>
+        <v>141.35654502607264</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3419,13 +3417,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="17">
-        <v>135.76484312969083</v>
+        <v>135.76484313002629</v>
       </c>
       <c r="C49" s="17">
-        <v>140.32468795395246</v>
+        <v>140.32455693999214</v>
       </c>
       <c r="D49" s="17">
-        <v>140.59315294047627</v>
+        <v>140.68083902734506</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3433,13 +3431,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="17">
-        <v>132.15799380962139</v>
+        <v>132.15799381069021</v>
       </c>
       <c r="C50" s="17">
-        <v>140.67904053134899</v>
+        <v>140.62190418688232</v>
       </c>
       <c r="D50" s="17">
-        <v>139.84355567430572</v>
+        <v>139.95015540596611</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3447,13 +3445,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="17">
-        <v>129.68532874050351</v>
+        <v>129.68532874095405</v>
       </c>
       <c r="C51" s="17">
-        <v>140.10099707999618</v>
+        <v>140.29965570258665</v>
       </c>
       <c r="D51" s="17">
-        <v>139.08444401802092</v>
+        <v>139.20683488112493</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3461,13 +3459,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="17">
-        <v>129.4452037013518</v>
+        <v>129.44520369983249</v>
       </c>
       <c r="C52" s="17">
-        <v>125.72159645139192</v>
+        <v>125.87931335805784</v>
       </c>
       <c r="D52" s="17">
-        <v>138.36006291970392</v>
+        <v>138.49385219104721</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3475,13 +3473,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="17">
-        <v>111.93059532686038</v>
+        <v>111.93059532201961</v>
       </c>
       <c r="C53" s="17">
-        <v>105.1046641821371</v>
+        <v>105.13234331594289</v>
       </c>
       <c r="D53" s="17">
-        <v>137.71297519484409</v>
+        <v>137.8546179840605</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3489,13 +3487,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="17">
-        <v>131.24787223918833</v>
+        <v>131.24787223714782</v>
       </c>
       <c r="C54" s="17">
-        <v>116.71787148113103</v>
+        <v>116.58753854631702</v>
       </c>
       <c r="D54" s="17">
-        <v>137.17721937566057</v>
+        <v>137.32475724496192</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3503,13 +3501,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="17">
-        <v>133.0934839638339</v>
+        <v>133.09348397071517</v>
       </c>
       <c r="C55" s="17">
-        <v>124.25328646248698</v>
+        <v>124.15989241411549</v>
       </c>
       <c r="D55" s="17">
-        <v>136.77665864752683</v>
+        <v>136.92887619452682</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3517,13 +3515,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="17">
-        <v>128.24284790478424</v>
+        <v>128.24284792670909</v>
       </c>
       <c r="C56" s="17">
-        <v>126.64552515403477</v>
+        <v>126.6655807195807</v>
       </c>
       <c r="D56" s="17">
-        <v>136.52432275443365</v>
+        <v>136.68115583974284</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3531,13 +3529,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="17">
-        <v>125.13820251911724</v>
+        <v>125.1382025283593</v>
       </c>
       <c r="C57" s="17">
-        <v>129.3819762898612</v>
+        <v>129.29180320032862</v>
       </c>
       <c r="D57" s="17">
-        <v>136.42574330401877</v>
+        <v>136.58709506912953</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3545,13 +3543,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="17">
-        <v>126.5301736661838</v>
+        <v>126.53017363501691</v>
       </c>
       <c r="C58" s="17">
-        <v>131.13179669817799</v>
+        <v>131.0584299852282</v>
       </c>
       <c r="D58" s="17">
-        <v>136.47316517131264</v>
+        <v>136.63875395835049</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3559,13 +3557,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="17">
-        <v>131.61628905269333</v>
+        <v>131.61628895339123</v>
       </c>
       <c r="C59" s="17">
-        <v>134.19286226569571</v>
+        <v>134.10490654825793</v>
       </c>
       <c r="D59" s="17">
-        <v>136.65130870208512</v>
+        <v>136.82005066788221</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3573,13 +3571,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="17">
-        <v>132.88316918380275</v>
+        <v>132.88316914194343</v>
       </c>
       <c r="C60" s="17">
-        <v>135.27143785058203</v>
+        <v>135.24991311557051</v>
       </c>
       <c r="D60" s="17">
-        <v>136.94278399632844</v>
+        <v>137.11242836257298</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3587,13 +3585,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="17">
-        <v>132.30930016595045</v>
+        <v>132.3093003071119</v>
       </c>
       <c r="C61" s="17">
-        <v>135.07940598390283</v>
+        <v>135.22917933967807</v>
       </c>
       <c r="D61" s="17">
-        <v>137.32929146286472</v>
+        <v>137.49626731512231</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3601,13 +3599,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="17">
-        <v>129.61069825921177</v>
+        <v>129.610698708972</v>
       </c>
       <c r="C62" s="17">
-        <v>139.87920625013007</v>
+        <v>139.91549938191574</v>
       </c>
       <c r="D62" s="17">
-        <v>137.79543913216662</v>
+        <v>137.95511712706508</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,13 +3613,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="17">
-        <v>126.88274612593136</v>
+        <v>126.88274631552113</v>
       </c>
       <c r="C63" s="17">
-        <v>137.94819065381114</v>
+        <v>138.26577566988215</v>
       </c>
       <c r="D63" s="17">
-        <v>138.33200143916417</v>
+        <v>138.47973026303899</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3629,13 +3627,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="17">
-        <v>147.05799608117897</v>
+        <v>147.05799544182895</v>
       </c>
       <c r="C64" s="17">
-        <v>140.33760340215474</v>
+        <v>140.37123413945545</v>
       </c>
       <c r="D64" s="17">
-        <v>138.93486202061874</v>
+        <v>139.06681338292128</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3643,13 +3641,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="17">
-        <v>144.90969514586067</v>
+        <v>144.90969310880172</v>
       </c>
       <c r="C65" s="17">
-        <v>137.80083870345672</v>
+        <v>137.76675909316174</v>
       </c>
       <c r="D65" s="17">
-        <v>139.60103326191395</v>
+        <v>139.71466175052245</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3657,13 +3655,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="17">
-        <v>150.49545529049234</v>
+        <v>150.49545443180037</v>
       </c>
       <c r="C66" s="17">
-        <v>137.25454377297802</v>
+        <v>137.13017466215635</v>
       </c>
       <c r="D66" s="17">
-        <v>140.32774087690987</v>
+        <v>140.4223201066178</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3671,13 +3669,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="17">
-        <v>149.13449500411494</v>
+        <v>149.13449789986612</v>
       </c>
       <c r="C67" s="17">
-        <v>140.48134628111507</v>
+        <v>140.35974832438589</v>
       </c>
       <c r="D67" s="17">
-        <v>141.10829997154894</v>
+        <v>141.18572147383466</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3685,13 +3683,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="17">
-        <v>142.80644531074435</v>
+        <v>142.8064545370143</v>
       </c>
       <c r="C68" s="17">
-        <v>141.70211913249832</v>
+        <v>141.60077216106737</v>
       </c>
       <c r="D68" s="17">
-        <v>141.93341494198324</v>
+        <v>141.99815597900087</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3699,13 +3697,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="17">
-        <v>141.05802124583437</v>
+        <v>141.05802513503161</v>
       </c>
       <c r="C69" s="17">
-        <v>144.38046699038483</v>
+        <v>144.31369646238247</v>
       </c>
       <c r="D69" s="17">
-        <v>142.78967852681285</v>
+        <v>142.84874325914762</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3713,13 +3711,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="17">
-        <v>140.84599438647376</v>
+        <v>140.84598127100656</v>
       </c>
       <c r="C70" s="17">
-        <v>145.40122095174848</v>
+        <v>145.37961468037298</v>
       </c>
       <c r="D70" s="17">
-        <v>143.66264957240395</v>
+        <v>143.7252231535364</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3727,13 +3725,13 @@
         <v>44470</v>
       </c>
       <c r="B71" s="17">
-        <v>140.56277167988108</v>
+        <v>140.56272989215773</v>
       </c>
       <c r="C71" s="17">
-        <v>144.69616451868598</v>
+        <v>144.69684882807081</v>
       </c>
       <c r="D71" s="17">
-        <v>144.5376991346985</v>
+        <v>144.61245366063383</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3741,13 +3739,13 @@
         <v>44501</v>
       </c>
       <c r="B72" s="17">
-        <v>145.46360490965989</v>
+        <v>145.46358729466505</v>
       </c>
       <c r="C72" s="17">
-        <v>146.54739710419332</v>
+        <v>146.6009691575189</v>
       </c>
       <c r="D72" s="17">
-        <v>145.40016491802103</v>
+        <v>145.49409467328042</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,13 +3753,13 @@
         <v>44531</v>
       </c>
       <c r="B73" s="17">
-        <v>146.03067165462195</v>
+        <v>146.0307310573402</v>
       </c>
       <c r="C73" s="17">
-        <v>148.42949606976043</v>
+        <v>148.45750127996357</v>
       </c>
       <c r="D73" s="17">
-        <v>146.23548339305833</v>
+        <v>146.35654431802971</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3769,13 +3767,13 @@
         <v>44562</v>
       </c>
       <c r="B74" s="17">
-        <v>136.16967380752766</v>
+        <v>136.16986307276909</v>
       </c>
       <c r="C74" s="17">
-        <v>147.23422214808681</v>
+        <v>147.24634476690883</v>
       </c>
       <c r="D74" s="17">
-        <v>147.03166789730989</v>
+        <v>147.18587969725795</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3783,13 +3781,13 @@
         <v>44593</v>
       </c>
       <c r="B75" s="17">
-        <v>137.61715933933209</v>
+        <v>137.617239121186</v>
       </c>
       <c r="C75" s="17">
-        <v>148.85552038412391</v>
+        <v>148.99222128680049</v>
       </c>
       <c r="D75" s="17">
-        <v>147.78066383873758</v>
+        <v>147.96903279660489</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,13 +3795,13 @@
         <v>44621</v>
       </c>
       <c r="B76" s="17">
-        <v>153.92904471416887</v>
+        <v>153.92877566654988</v>
       </c>
       <c r="C76" s="17">
-        <v>147.82211063790649</v>
+        <v>148.08809522272688</v>
       </c>
       <c r="D76" s="17">
-        <v>148.47954122952919</v>
+        <v>148.69633696387527</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3811,13 +3809,13 @@
         <v>44652</v>
       </c>
       <c r="B77" s="17">
-        <v>153.42927067661543</v>
+        <v>153.7335940552577</v>
       </c>
       <c r="C77" s="17">
-        <v>148.6272707738834</v>
+        <v>148.82447919501493</v>
       </c>
       <c r="D77" s="17">
-        <v>149.13247230389123</v>
+        <v>149.36659803837014</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3825,13 +3823,13 @@
         <v>44682</v>
       </c>
       <c r="B78" s="17">
-        <v>162.36956646957179</v>
+        <v>162.67850048218298</v>
       </c>
       <c r="C78" s="17">
-        <v>148.85765239579808</v>
+        <v>148.94865733916654</v>
       </c>
       <c r="D78" s="17">
-        <v>149.74859581019382</v>
+        <v>149.98357023495882</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3839,13 +3837,13 @@
         <v>44713</v>
       </c>
       <c r="B79" s="17">
-        <v>159.59075651417527</v>
+        <v>159.89943888973366</v>
       </c>
       <c r="C79" s="17">
-        <v>150.81494224018516</v>
+        <v>151.02506962983165</v>
       </c>
       <c r="D79" s="17">
-        <v>150.3400992818124</v>
+        <v>150.5558020731728</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3853,13 +3851,13 @@
         <v>44743</v>
       </c>
       <c r="B80" s="17">
-        <v>151.26536125023031</v>
+        <v>151.23553183575578</v>
       </c>
       <c r="C80" s="17">
-        <v>151.37012851826515</v>
+        <v>151.46419030101069</v>
       </c>
       <c r="D80" s="17">
-        <v>150.92028290133237</v>
+        <v>151.09524699292953</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3867,27 +3865,41 @@
         <v>44774</v>
       </c>
       <c r="B81" s="17">
-        <v>150.32807739350432</v>
+        <v>150.23651545882615</v>
       </c>
       <c r="C81" s="17">
-        <v>152.44244407206827</v>
+        <v>152.64615012831652</v>
       </c>
       <c r="D81" s="17">
-        <v>151.49886737458965</v>
+        <v>151.61296382170369</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>44805</v>
       </c>
-      <c r="B82" s="43">
-        <v>147.54987496056535</v>
-      </c>
-      <c r="C82" s="43">
-        <v>152.02935683288021</v>
-      </c>
-      <c r="D82" s="43">
-        <v>152.08181081617525</v>
+      <c r="B82" s="17">
+        <v>147.36123681909788</v>
+      </c>
+      <c r="C82" s="17">
+        <v>152.31771154641231</v>
+      </c>
+      <c r="D82" s="17">
+        <v>152.11812609635166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>44835</v>
+      </c>
+      <c r="B83" s="43">
+        <v>146.85409350369895</v>
+      </c>
+      <c r="C83" s="43">
+        <v>151.88771401612976</v>
+      </c>
+      <c r="D83" s="43">
+        <v>152.62137208876123</v>
       </c>
     </row>
   </sheetData>
@@ -3900,7 +3912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4935,10 +4947,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4968,7 +4980,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="11">
-        <v>475371.05098936806</v>
+        <v>475346.60482497915</v>
       </c>
       <c r="D2" s="11">
         <v>460369.44223294902</v>
@@ -4982,7 +4994,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="11">
-        <v>470350.62814756762</v>
+        <v>470369.47564368765</v>
       </c>
       <c r="D3" s="11">
         <v>514395.68177236198</v>
@@ -4996,7 +5008,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="11">
-        <v>494069.95695165993</v>
+        <v>494104.21576874424</v>
       </c>
       <c r="D4" s="11">
         <v>481151.97994350799</v>
@@ -5010,7 +5022,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="11">
-        <v>500669.14453385782</v>
+        <v>500640.48438888183</v>
       </c>
       <c r="D5" s="11">
         <v>484543.67687656201</v>
@@ -5024,7 +5036,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="11">
-        <v>515257.73564929306</v>
+        <v>515222.78948754398</v>
       </c>
       <c r="D6" s="11">
         <v>493602.53057785501</v>
@@ -5038,7 +5050,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="11">
-        <v>526471.33379984985</v>
+        <v>526520.44061326212</v>
       </c>
       <c r="D7" s="11">
         <v>581668.24987960199</v>
@@ -5052,7 +5064,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="11">
-        <v>530356.53122616687</v>
+        <v>530368.74749629863</v>
       </c>
       <c r="D8" s="11">
         <v>514697.78950542799</v>
@@ -5066,7 +5078,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="11">
-        <v>540138.16933834716</v>
+        <v>540111.79241655173</v>
       </c>
       <c r="D9" s="11">
         <v>522255.20005077199</v>
@@ -5080,7 +5092,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="11">
-        <v>554320.72005646233</v>
+        <v>554337.88460732426</v>
       </c>
       <c r="D10" s="11">
         <v>532348.21201691695</v>
@@ -5094,7 +5106,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="11">
-        <v>561467.19958498655</v>
+        <v>561472.4314419172</v>
       </c>
       <c r="D11" s="11">
         <v>614076.39260854397</v>
@@ -5108,7 +5120,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="11">
-        <v>577137.74961009074</v>
+        <v>577098.03119365929</v>
       </c>
       <c r="D12" s="11">
         <v>562978.96562687703</v>
@@ -5122,7 +5134,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="11">
-        <v>589271.94763138681</v>
+        <v>589289.26964002522</v>
       </c>
       <c r="D13" s="11">
         <v>572794.04663058801</v>
@@ -5136,7 +5148,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="11">
-        <v>603167.9720340278</v>
+        <v>603175.76508721686</v>
       </c>
       <c r="D14" s="11">
         <v>576846.88569942699</v>
@@ -5150,7 +5162,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="11">
-        <v>616315.46326810063</v>
+        <v>616309.48457227251</v>
       </c>
       <c r="D15" s="11">
         <v>674620.563006485</v>
@@ -5164,7 +5176,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="11">
-        <v>624561.79784678563</v>
+        <v>624535.10259633034</v>
       </c>
       <c r="D16" s="11">
         <v>610425.69401485403</v>
@@ -5178,7 +5190,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="11">
-        <v>643724.7774354479</v>
+        <v>643749.65832854214</v>
       </c>
       <c r="D17" s="11">
         <v>625876.867863597</v>
@@ -5192,7 +5204,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="11">
-        <v>649805.62972759677</v>
+        <v>649778.31207872008</v>
       </c>
       <c r="D18" s="11">
         <v>616720.35706447798</v>
@@ -5206,7 +5218,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="11">
-        <v>653132.8277707044</v>
+        <v>653135.87805250078</v>
       </c>
       <c r="D19" s="11">
         <v>711405.50045523304</v>
@@ -5220,7 +5232,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="11">
-        <v>658216.30872340978</v>
+        <v>658206.46208567265</v>
       </c>
       <c r="D20" s="11">
         <v>647087.95974249404</v>
@@ -5234,7 +5246,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="11">
-        <v>627549.87274313683</v>
+        <v>627583.98674795462</v>
       </c>
       <c r="D21" s="11">
         <v>613490.82170264097</v>
@@ -5248,7 +5260,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="11">
-        <v>604485.7968595376</v>
+        <v>604467.32324628218</v>
       </c>
       <c r="D22" s="11">
         <v>578553.04424240498</v>
@@ -5262,7 +5274,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="11">
-        <v>590846.68514454551</v>
+        <v>590816.51552377664</v>
       </c>
       <c r="D23" s="11">
         <v>631197.75186006899</v>
@@ -5276,7 +5288,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="11">
-        <v>614199.09600853221</v>
+        <v>614236.46101588104</v>
       </c>
       <c r="D24" s="11">
         <v>610519.85461172694</v>
@@ -5290,7 +5302,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="11">
-        <v>625959.92763888137</v>
+        <v>625971.20586555882</v>
       </c>
       <c r="D25" s="11">
         <v>615220.85493729694</v>
@@ -5304,7 +5316,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="11">
-        <v>644757.43782605673</v>
+        <v>644751.28759089438</v>
       </c>
       <c r="D26" s="11">
         <v>611607.33658973</v>
@@ -5318,7 +5330,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="11">
-        <v>673364.27754086838</v>
+        <v>673332.50228821358</v>
       </c>
       <c r="D27" s="11">
         <v>733730.773968903</v>
@@ -5332,7 +5344,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="11">
-        <v>677402.2266857496</v>
+        <v>677455.06279834348</v>
       </c>
       <c r="D28" s="11">
         <v>668566.50948898599</v>
@@ -5346,7 +5358,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="11">
-        <v>686570.77571451815</v>
+        <v>686555.86508974305</v>
       </c>
       <c r="D29" s="11">
         <v>668190.097719574</v>
@@ -5360,7 +5372,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="11">
-        <v>702649.90013330383</v>
+        <v>702611.95411781606</v>
       </c>
       <c r="D30" s="11">
         <v>662325.58597269503</v>
@@ -5374,7 +5386,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="11">
-        <v>709545.37355450576</v>
+        <v>709524.81803765707</v>
       </c>
       <c r="D31" s="11">
         <v>766332.95457161299</v>
@@ -5388,7 +5400,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="11">
-        <v>715423.01836901845</v>
+        <v>715499.52217016229</v>
       </c>
       <c r="D32" s="11">
         <v>711417.39193010505</v>
@@ -5402,7 +5414,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="11">
-        <v>715508.09682557906</v>
+        <v>715490.09455677262</v>
       </c>
       <c r="D33" s="11">
         <v>703050.45640799298</v>
@@ -5416,7 +5428,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="11">
-        <v>707750.20169942803</v>
+        <v>707728.83681350737</v>
       </c>
       <c r="D34" s="11">
         <v>672685.993630504</v>
@@ -5430,7 +5442,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="11">
-        <v>683979.57443022332</v>
+        <v>683958.45333459717</v>
       </c>
       <c r="D35" s="11">
         <v>730838.27259277599</v>
@@ -5444,7 +5456,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="11">
-        <v>705076.19439545553</v>
+        <v>705130.18780354073</v>
       </c>
       <c r="D36" s="11">
         <v>703461.65253019601</v>
@@ -5458,7 +5470,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="11">
-        <v>717137.98731069011</v>
+        <v>717126.47988415032</v>
       </c>
       <c r="D37" s="11">
         <v>706958.03908231901</v>
@@ -5472,7 +5484,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="11">
-        <v>716939.43149499106</v>
+        <v>716866.23164218897</v>
       </c>
       <c r="D38" s="11">
         <v>677085.52917315101</v>
@@ -5486,7 +5498,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="11">
-        <v>721269.52188036207</v>
+        <v>721282.46480787836</v>
       </c>
       <c r="D39" s="11">
         <v>776486.60279942001</v>
@@ -5500,7 +5512,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="11">
-        <v>725157.65159980964</v>
+        <v>725204.00567040662</v>
       </c>
       <c r="D40" s="11">
         <v>721458.94421618199</v>
@@ -5514,7 +5526,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="11">
-        <v>718261.81623609748</v>
+        <v>718275.71909078571</v>
       </c>
       <c r="D41" s="11">
         <v>706597.34502250701</v>
@@ -5528,7 +5540,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="11">
-        <v>707546.06498329213</v>
+        <v>707531.31986237713</v>
       </c>
       <c r="D42" s="11">
         <v>671066.04663506302</v>
@@ -5542,7 +5554,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="11">
-        <v>703282.00621111901</v>
+        <v>703282.45282505837</v>
       </c>
       <c r="D43" s="11">
         <v>760576.86834800395</v>
@@ -5556,7 +5568,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="11">
-        <v>697224.55344559671</v>
+        <v>697239.2336517009</v>
       </c>
       <c r="D44" s="11">
         <v>690879.79825168301</v>
@@ -5570,7 +5582,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="11">
-        <v>701171.5592134539</v>
+        <v>701171.17751432455</v>
       </c>
       <c r="D45" s="11">
         <v>686701.47061871097</v>
@@ -5584,7 +5596,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="11">
-        <v>711516.17676598986</v>
+        <v>711506.94750436209</v>
       </c>
       <c r="D46" s="11">
         <v>672749.81139169901</v>
@@ -5598,7 +5610,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="11">
-        <v>727627.86383100448</v>
+        <v>727644.95621369022</v>
       </c>
       <c r="D47" s="11">
         <v>791235.96554166998</v>
@@ -5612,7 +5624,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="11">
-        <v>727531.67644959386</v>
+        <v>727525.85686184897</v>
       </c>
       <c r="D48" s="11">
         <v>718281.26544978202</v>
@@ -5626,7 +5638,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="11">
-        <v>719272.8695055719</v>
+        <v>719270.82597225765</v>
       </c>
       <c r="D49" s="11">
         <v>703681.54416900803</v>
@@ -5640,7 +5652,7 @@
         <v>29</v>
       </c>
       <c r="C50" s="11">
-        <v>712956.4362341261</v>
+        <v>712959.08414114174</v>
       </c>
       <c r="D50" s="11">
         <v>677652.08911570301</v>
@@ -5655,7 +5667,7 @@
         <v>30</v>
       </c>
       <c r="C51" s="11">
-        <v>701050.55126605951</v>
+        <v>701050.49382605171</v>
       </c>
       <c r="D51" s="11">
         <v>760703.28015165601</v>
@@ -5670,7 +5682,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="11">
-        <v>703949.96989883191</v>
+        <v>703919.56072469149</v>
       </c>
       <c r="D52" s="11">
         <v>694382.47577623103</v>
@@ -5685,7 +5697,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="11">
-        <v>707954.43699162884</v>
+        <v>707982.25569876132</v>
       </c>
       <c r="D53" s="11">
         <v>693173.54934705805</v>
@@ -5700,7 +5712,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="11">
-        <v>714425.3181707114</v>
+        <v>714450.30999806512</v>
       </c>
       <c r="D54" s="11">
         <v>681444.76611022197</v>
@@ -5715,7 +5727,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="11">
-        <v>721952.60422123875</v>
+        <v>721889.15127896471</v>
       </c>
       <c r="D55" s="11">
         <v>778401.67644931702</v>
@@ -5730,7 +5742,7 @@
         <v>31</v>
       </c>
       <c r="C56" s="11">
-        <v>731110.36115767376</v>
+        <v>731048.32202709105</v>
       </c>
       <c r="D56" s="11">
         <v>721120.42685279401</v>
@@ -5745,7 +5757,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="11">
-        <v>738071.50750167179</v>
+        <v>738172.0077471754</v>
       </c>
       <c r="D57" s="11">
         <v>724592.92163896305</v>
@@ -5760,7 +5772,7 @@
         <v>29</v>
       </c>
       <c r="C58" s="11">
-        <v>735750.72130254249</v>
+        <v>735851.09244015114</v>
       </c>
       <c r="D58" s="11">
         <v>707324.26805721398</v>
@@ -5776,7 +5788,7 @@
         <v>30</v>
       </c>
       <c r="C59" s="11">
-        <v>702484.9729966335</v>
+        <v>702281.527022189</v>
       </c>
       <c r="D59" s="11">
         <v>747428.29995457502</v>
@@ -5792,7 +5804,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="11">
-        <v>700839.69810909347</v>
+        <v>700655.1084711774</v>
       </c>
       <c r="D60" s="11">
         <v>696101.58352180803</v>
@@ -5808,7 +5820,7 @@
         <v>32</v>
       </c>
       <c r="C61" s="11">
-        <v>690434.37950978254</v>
+        <v>690722.04398453119</v>
       </c>
       <c r="D61" s="11">
         <v>678655.62038445403</v>
@@ -5824,7 +5836,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="11">
-        <v>691050.55900471541</v>
+        <v>691264.64982409915</v>
       </c>
       <c r="D62">
         <v>665848.71529970889</v>
@@ -5840,7 +5852,7 @@
         <v>30</v>
       </c>
       <c r="C63" s="11">
-        <v>697044.80835807486</v>
+        <v>696681.98073515797</v>
       </c>
       <c r="D63">
         <v>751784.46077713254</v>
@@ -5856,7 +5868,7 @@
         <v>31</v>
       </c>
       <c r="C64" s="11">
-        <v>698289.3802768162</v>
+        <v>697817.77533158055</v>
       </c>
       <c r="D64">
         <v>683900.89855257841</v>
@@ -5872,7 +5884,7 @@
         <v>32</v>
       </c>
       <c r="C65" s="11">
-        <v>686510.4667122321</v>
+        <v>687130.80846100091</v>
       </c>
       <c r="D65">
         <v>671361.13972242002</v>
@@ -5888,7 +5900,7 @@
         <v>29</v>
       </c>
       <c r="C66" s="10">
-        <v>657531.48587817268</v>
+        <v>657817.61671771028</v>
       </c>
       <c r="D66" s="10">
         <v>632733.36598162609</v>
@@ -5903,7 +5915,7 @@
         <v>30</v>
       </c>
       <c r="C67" s="10">
-        <v>559875.23583740985</v>
+        <v>559305.11399589793</v>
       </c>
       <c r="D67" s="10">
         <v>608450.80405697017</v>
@@ -5918,7 +5930,7 @@
         <v>31</v>
       </c>
       <c r="C68" s="10">
-        <v>626566.37454888062</v>
+        <v>625824.17363747943</v>
       </c>
       <c r="D68" s="10">
         <v>614335.69211847626</v>
@@ -5933,7 +5945,7 @@
         <v>32</v>
       </c>
       <c r="C69" s="10">
-        <v>653206.62686591013</v>
+        <v>654232.81877928693</v>
       </c>
       <c r="D69" s="10">
         <v>641659.86097329983</v>
@@ -5948,7 +5960,7 @@
         <v>29</v>
       </c>
       <c r="C70" s="10">
-        <v>676500.63372803852</v>
+        <v>676820.60726520116</v>
       </c>
       <c r="D70">
         <v>652563.11939207092</v>
@@ -5963,7 +5975,7 @@
         <v>30</v>
       </c>
       <c r="C71" s="10">
-        <v>672322.29744675709</v>
+        <v>671491.08789045829</v>
       </c>
       <c r="D71">
         <v>718843.1229160385</v>
@@ -5978,7 +5990,7 @@
         <v>31</v>
       </c>
       <c r="C72" s="10">
-        <v>698313.42888155917</v>
+        <v>697424.37797260308</v>
       </c>
       <c r="D72" s="10">
         <v>686778.32722188451</v>
@@ -5992,7 +6004,7 @@
         <v>32</v>
       </c>
       <c r="C73" s="10">
-        <v>709706.3381650534</v>
+        <v>711106.62508873863</v>
       </c>
       <c r="D73" s="10">
         <v>698658.13099747989</v>
@@ -6006,7 +6018,7 @@
         <v>29</v>
       </c>
       <c r="C74" s="10">
-        <v>718073.46755277982</v>
+        <v>718498.71666119352</v>
       </c>
       <c r="D74">
         <v>691638.23860468564</v>
@@ -6020,10 +6032,24 @@
         <v>30</v>
       </c>
       <c r="C75" s="10">
-        <v>725560.2452796225</v>
+        <v>725729.43123048346</v>
       </c>
       <c r="D75">
-        <v>768729.05175870494</v>
+        <v>770219.87505852256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C76" s="10">
+        <v>738067.27836371807</v>
+      </c>
+      <c r="D76" s="10">
+        <v>727597.95469722245</v>
       </c>
     </row>
   </sheetData>
@@ -6842,14 +6868,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="29">
-        <v>13092</v>
+        <v>14487</v>
       </c>
       <c r="C2" s="29">
-        <v>16758</v>
+        <v>18030</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-3666</v>
+        <v>-3543</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6857,14 +6883,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="29">
-        <v>4156</v>
+        <v>4578</v>
       </c>
       <c r="C3" s="29">
-        <v>666</v>
+        <v>711</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>3490</v>
+        <v>3867</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6872,14 +6898,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="29">
-        <v>4344</v>
+        <v>4834</v>
       </c>
       <c r="C4" s="29">
-        <v>3007</v>
+        <v>3186</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1337</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6887,14 +6913,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="29">
-        <v>1281</v>
+        <v>1404</v>
       </c>
       <c r="C5" s="29">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6902,14 +6928,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="29">
-        <v>7454</v>
+        <v>7998</v>
       </c>
       <c r="C6" s="29">
-        <v>11098</v>
+        <v>11811</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-3644</v>
+        <v>-3813</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6917,14 +6943,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="29">
-        <v>9208</v>
+        <v>10263</v>
       </c>
       <c r="C7" s="29">
-        <v>9539</v>
+        <v>10427</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-331</v>
+        <v>-164</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6932,14 +6958,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="29">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="C8" s="29">
-        <v>553</v>
+        <v>602</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6947,14 +6973,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="29">
-        <v>910</v>
+        <v>986</v>
       </c>
       <c r="C9" s="29">
-        <v>513</v>
+        <v>557</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>397</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,14 +6988,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="29">
-        <v>486</v>
+        <v>512</v>
       </c>
       <c r="C10" s="29">
-        <v>389</v>
+        <v>408</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -6977,14 +7003,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="29">
-        <v>6555</v>
+        <v>7235</v>
       </c>
       <c r="C11" s="29">
-        <v>3582</v>
+        <v>3931</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2973</v>
+        <v>3304</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6992,14 +7018,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="29">
-        <v>6838</v>
+        <v>7672</v>
       </c>
       <c r="C12" s="29">
-        <v>14858</v>
+        <v>16320</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-8020</v>
+        <v>-8648</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7007,14 +7033,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="29">
-        <v>1730</v>
+        <v>1969</v>
       </c>
       <c r="C13" s="29">
-        <v>609</v>
+        <v>689</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1121</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7022,14 +7048,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="29">
-        <v>710</v>
+        <v>766</v>
       </c>
       <c r="C14" s="29">
-        <v>974</v>
+        <v>1088</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-264</v>
+        <v>-322</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7037,14 +7063,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="29">
-        <v>3800</v>
+        <v>4153</v>
       </c>
       <c r="C15" s="29">
-        <v>1655</v>
+        <v>1767</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>2145</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7052,14 +7078,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="29">
-        <v>4141</v>
+        <v>4333</v>
       </c>
       <c r="C16" s="29">
-        <v>2385</v>
+        <v>2507</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1756</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7067,14 +7093,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="29">
-        <v>3539</v>
+        <v>3786</v>
       </c>
       <c r="C17" s="29">
-        <v>1108</v>
+        <v>1158</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2431</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7082,14 +7108,14 @@
         <v>95</v>
       </c>
       <c r="B18" s="29">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="C18" s="29">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7097,14 +7123,14 @@
         <v>96</v>
       </c>
       <c r="B19" s="29">
-        <v>746</v>
+        <v>839</v>
       </c>
       <c r="C19" s="29">
-        <v>406</v>
+        <v>447</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>340</v>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7112,14 +7138,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="30">
-        <v>5157</v>
+        <v>5444</v>
       </c>
       <c r="C20" s="30">
-        <v>2433</v>
+        <v>2630</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2724</v>
+        <v>2814</v>
       </c>
     </row>
   </sheetData>
@@ -7152,7 +7178,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="35">
-        <v>75144</v>
+        <v>82293</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7160,7 +7186,7 @@
         <v>185</v>
       </c>
       <c r="B3" s="35">
-        <v>21116</v>
+        <v>22586</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7168,7 +7194,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="29">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7176,7 +7202,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="29">
-        <v>1357</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7184,7 +7210,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="29">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7192,7 +7218,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="29">
-        <v>531</v>
+        <v>568</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7200,7 +7226,7 @@
         <v>142</v>
       </c>
       <c r="B8" s="29">
-        <v>480</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7208,7 +7234,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="29">
-        <v>14047</v>
+        <v>14684</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7216,7 +7242,7 @@
         <v>144</v>
       </c>
       <c r="B10" s="29">
-        <v>3659</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7224,7 +7250,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="29">
-        <v>224</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7232,7 +7258,7 @@
         <v>146</v>
       </c>
       <c r="B12" s="29">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7240,7 +7266,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="29">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7248,7 +7274,7 @@
         <v>148</v>
       </c>
       <c r="B14" s="29">
-        <v>260</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7256,7 +7282,7 @@
         <v>149</v>
       </c>
       <c r="B15" s="29">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7264,7 +7290,7 @@
         <v>186</v>
       </c>
       <c r="B16" s="35">
-        <v>27899</v>
+        <v>30767</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7272,7 +7298,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="29">
-        <v>3618</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7280,7 +7306,7 @@
         <v>151</v>
       </c>
       <c r="B18" s="29">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7288,7 +7314,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="29">
-        <v>1191</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7296,7 +7322,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="29">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7304,7 +7330,7 @@
         <v>154</v>
       </c>
       <c r="B21" s="29">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7312,7 +7338,7 @@
         <v>155</v>
       </c>
       <c r="B22" s="29">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7320,7 +7346,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="29">
-        <v>825</v>
+        <v>923</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7328,7 +7354,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="29">
-        <v>7832</v>
+        <v>8591</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7336,7 +7362,7 @@
         <v>158</v>
       </c>
       <c r="B25" s="29">
-        <v>235</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7344,7 +7370,7 @@
         <v>159</v>
       </c>
       <c r="B26" s="29">
-        <v>694</v>
+        <v>756</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7352,7 +7378,7 @@
         <v>160</v>
       </c>
       <c r="B27" s="29">
-        <v>814</v>
+        <v>882</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7360,7 +7386,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="29">
-        <v>10976</v>
+        <v>12230</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7368,7 +7394,7 @@
         <v>162</v>
       </c>
       <c r="B29" s="29">
-        <v>265</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7376,7 +7402,7 @@
         <v>163</v>
       </c>
       <c r="B30" s="29">
-        <v>394</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7384,7 +7410,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="29">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7392,7 +7418,7 @@
         <v>165</v>
       </c>
       <c r="B32" s="29">
-        <v>436</v>
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7400,7 +7426,7 @@
         <v>187</v>
       </c>
       <c r="B33" s="35">
-        <v>19263</v>
+        <v>21389</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7408,7 +7434,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="29">
-        <v>5132</v>
+        <v>5727</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7416,7 +7442,7 @@
         <v>167</v>
       </c>
       <c r="B35" s="29">
-        <v>926</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7424,7 +7450,7 @@
         <v>168</v>
       </c>
       <c r="B36" s="29">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7432,7 +7458,7 @@
         <v>169</v>
       </c>
       <c r="B37" s="29">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7440,7 +7466,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="29">
-        <v>388</v>
+        <v>430</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7448,7 +7474,7 @@
         <v>171</v>
       </c>
       <c r="B39" s="29">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7456,7 +7482,7 @@
         <v>172</v>
       </c>
       <c r="B40" s="29">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -7464,7 +7490,7 @@
         <v>173</v>
       </c>
       <c r="B41" s="29">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -7472,7 +7498,7 @@
         <v>174</v>
       </c>
       <c r="B42" s="29">
-        <v>2249</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -7480,7 +7506,7 @@
         <v>175</v>
       </c>
       <c r="B43" s="29">
-        <v>1775</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -7488,7 +7514,7 @@
         <v>176</v>
       </c>
       <c r="B44" s="29">
-        <v>1316</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -7496,7 +7522,7 @@
         <v>177</v>
       </c>
       <c r="B45" s="29">
-        <v>6493</v>
+        <v>7341</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -7504,7 +7530,7 @@
         <v>178</v>
       </c>
       <c r="B46" s="29">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7512,7 +7538,7 @@
         <v>179</v>
       </c>
       <c r="B47" s="29">
-        <v>245</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -7520,7 +7546,7 @@
         <v>188</v>
       </c>
       <c r="B48" s="35">
-        <v>6866</v>
+        <v>7551</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7528,7 +7554,7 @@
         <v>180</v>
       </c>
       <c r="B49" s="29">
-        <v>3226</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7536,7 +7562,7 @@
         <v>181</v>
       </c>
       <c r="B50" s="29">
-        <v>2105</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7544,7 +7570,7 @@
         <v>182</v>
       </c>
       <c r="B51" s="29">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7552,7 +7578,7 @@
         <v>183</v>
       </c>
       <c r="B52" s="41">
-        <v>1060</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -7560,7 +7586,7 @@
         <v>184</v>
       </c>
       <c r="B53" s="42">
-        <v>397</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -7573,9 +7599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7595,7 +7619,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="35">
-        <v>70738</v>
+        <v>76493</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7603,7 +7627,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="35">
-        <v>10510</v>
+        <v>11582</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7611,7 +7635,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="29">
-        <v>7898</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7619,7 +7643,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="29">
-        <v>1129</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7627,7 +7651,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="29">
-        <v>1106</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7635,7 +7659,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="29">
-        <v>378</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7643,7 +7667,7 @@
         <v>211</v>
       </c>
       <c r="B8" s="35">
-        <v>26077</v>
+        <v>28161</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7651,7 +7675,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="29">
-        <v>2378</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7659,7 +7683,7 @@
         <v>195</v>
       </c>
       <c r="B10" s="29">
-        <v>1254</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7667,7 +7691,7 @@
         <v>196</v>
       </c>
       <c r="B11" s="29">
-        <v>10801</v>
+        <v>11662</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7675,7 +7699,7 @@
         <v>197</v>
       </c>
       <c r="B12" s="29">
-        <v>3245</v>
+        <v>3574</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7683,7 +7707,7 @@
         <v>198</v>
       </c>
       <c r="B13" s="29">
-        <v>1014</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7691,7 +7715,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="29">
-        <v>1188</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7699,7 +7723,7 @@
         <v>200</v>
       </c>
       <c r="B15" s="29">
-        <v>594</v>
+        <v>634</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7707,7 +7731,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="29">
-        <v>3679</v>
+        <v>3993</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7715,7 +7739,7 @@
         <v>202</v>
       </c>
       <c r="B17" s="29">
-        <v>1924</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7723,7 +7747,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="35">
-        <v>11959</v>
+        <v>12419</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7731,7 +7755,7 @@
         <v>195</v>
       </c>
       <c r="B19" s="29">
-        <v>11657</v>
+        <v>12084</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7739,7 +7763,7 @@
         <v>203</v>
       </c>
       <c r="B20" s="29">
-        <v>302</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7747,7 +7771,7 @@
         <v>213</v>
       </c>
       <c r="B21" s="35">
-        <v>12721</v>
+        <v>14011</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7755,7 +7779,7 @@
         <v>190</v>
       </c>
       <c r="B22" s="29">
-        <v>8252</v>
+        <v>9053</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7763,7 +7787,7 @@
         <v>191</v>
       </c>
       <c r="B23" s="29">
-        <v>3553</v>
+        <v>3943</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7771,7 +7795,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="29">
-        <v>915</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7779,7 +7803,7 @@
         <v>214</v>
       </c>
       <c r="B25" s="35">
-        <v>7229</v>
+        <v>7890</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7787,7 +7811,7 @@
         <v>205</v>
       </c>
       <c r="B26" s="29">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7795,7 +7819,7 @@
         <v>194</v>
       </c>
       <c r="B27" s="29">
-        <v>520</v>
+        <v>565</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7803,7 +7827,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="29">
-        <v>672</v>
+        <v>725</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7811,7 +7835,7 @@
         <v>196</v>
       </c>
       <c r="B29" s="29">
-        <v>2124</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7819,7 +7843,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="29">
-        <v>443</v>
+        <v>480</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7827,7 +7851,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="29">
-        <v>358</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7835,7 +7859,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="29">
-        <v>579</v>
+        <v>640</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7843,7 +7867,7 @@
         <v>190</v>
       </c>
       <c r="B33" s="29">
-        <v>545</v>
+        <v>589</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7851,7 +7875,7 @@
         <v>191</v>
       </c>
       <c r="B34" s="29">
-        <v>490</v>
+        <v>527</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7859,7 +7883,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="29">
-        <v>268</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7867,7 +7891,7 @@
         <v>208</v>
       </c>
       <c r="B36" s="29">
-        <v>478</v>
+        <v>524</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7875,7 +7899,7 @@
         <v>209</v>
       </c>
       <c r="B37" s="29">
-        <v>502</v>
+        <v>554</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7883,7 +7907,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="35">
-        <v>1706</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7891,7 +7915,7 @@
         <v>191</v>
       </c>
       <c r="B39" s="39">
-        <v>1706</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7899,7 +7923,7 @@
         <v>216</v>
       </c>
       <c r="B40" s="40">
-        <v>535</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo con datos fiscales y de comex para diciembre22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5E44BA-CC4C-4C52-87C4-7E34E05E22E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F6B155-8E48-458E-8F2E-2B2EF0B6A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -915,9 +915,6 @@
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -943,6 +940,10 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -3909,13 +3910,13 @@
       <c r="A83" s="4">
         <v>44835</v>
       </c>
-      <c r="B83" s="43">
+      <c r="B83" s="42">
         <v>146.85409350369895</v>
       </c>
-      <c r="C83" s="43">
+      <c r="C83" s="42">
         <v>151.88771401612976</v>
       </c>
-      <c r="D83" s="43">
+      <c r="D83" s="42">
         <v>152.62137208876123</v>
       </c>
     </row>
@@ -3929,7 +3930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
@@ -6092,14 +6093,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6703,14 +6704,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6860,7 +6861,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6887,14 +6888,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="29">
-        <v>14487</v>
+        <v>15793</v>
       </c>
       <c r="C2" s="29">
-        <v>18030</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D20" si="0">B2-C2</f>
-        <v>-3543</v>
+        <v>19264</v>
+      </c>
+      <c r="D2" s="44">
+        <f>B2-C2</f>
+        <v>-3471</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6902,14 +6903,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="29">
-        <v>4578</v>
+        <v>4938</v>
       </c>
       <c r="C3" s="29">
-        <v>711</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>3867</v>
+        <v>778</v>
+      </c>
+      <c r="D3" s="44">
+        <f t="shared" ref="D3:D20" si="0">B3-C3</f>
+        <v>4160</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6917,14 +6918,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="29">
-        <v>4834</v>
+        <v>5313</v>
       </c>
       <c r="C4" s="29">
-        <v>3186</v>
-      </c>
-      <c r="D4">
+        <v>3377</v>
+      </c>
+      <c r="D4" s="44">
         <f t="shared" si="0"/>
-        <v>1648</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6932,14 +6933,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="29">
-        <v>1404</v>
+        <v>1480</v>
       </c>
       <c r="C5" s="29">
-        <v>33</v>
-      </c>
-      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="D5" s="44">
         <f t="shared" si="0"/>
-        <v>1371</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6947,14 +6948,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="29">
-        <v>7998</v>
+        <v>8653</v>
       </c>
       <c r="C6" s="29">
-        <v>11811</v>
-      </c>
-      <c r="D6">
+        <v>12557</v>
+      </c>
+      <c r="D6" s="44">
         <f t="shared" si="0"/>
-        <v>-3813</v>
+        <v>-3904</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,14 +6963,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="29">
-        <v>10263</v>
+        <v>10846</v>
       </c>
       <c r="C7" s="29">
-        <v>10427</v>
-      </c>
-      <c r="D7">
+        <v>11118</v>
+      </c>
+      <c r="D7" s="44">
         <f t="shared" si="0"/>
-        <v>-164</v>
+        <v>-272</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6977,14 +6978,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="29">
-        <v>613</v>
+        <v>685</v>
       </c>
       <c r="C8" s="29">
-        <v>602</v>
-      </c>
-      <c r="D8">
+        <v>652</v>
+      </c>
+      <c r="D8" s="44">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6992,14 +6993,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="29">
-        <v>986</v>
+        <v>1092</v>
       </c>
       <c r="C9" s="29">
-        <v>557</v>
-      </c>
-      <c r="D9">
+        <v>586</v>
+      </c>
+      <c r="D9" s="44">
         <f t="shared" si="0"/>
-        <v>429</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7007,14 +7008,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="29">
-        <v>512</v>
+        <v>581</v>
       </c>
       <c r="C10" s="29">
-        <v>408</v>
-      </c>
-      <c r="D10">
+        <v>432</v>
+      </c>
+      <c r="D10" s="44">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7022,14 +7023,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="29">
-        <v>7235</v>
+        <v>7894</v>
       </c>
       <c r="C11" s="29">
-        <v>3931</v>
-      </c>
-      <c r="D11">
+        <v>4225</v>
+      </c>
+      <c r="D11" s="44">
         <f t="shared" si="0"/>
-        <v>3304</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7037,14 +7038,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="29">
-        <v>7672</v>
+        <v>8022</v>
       </c>
       <c r="C12" s="29">
-        <v>16320</v>
-      </c>
-      <c r="D12">
+        <v>17516</v>
+      </c>
+      <c r="D12" s="44">
         <f t="shared" si="0"/>
-        <v>-8648</v>
+        <v>-9494</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7052,14 +7053,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="29">
-        <v>1969</v>
+        <v>2020</v>
       </c>
       <c r="C13" s="29">
-        <v>689</v>
-      </c>
-      <c r="D13">
+        <v>729</v>
+      </c>
+      <c r="D13" s="44">
         <f t="shared" si="0"/>
-        <v>1280</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7067,14 +7068,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="29">
-        <v>766</v>
+        <v>795</v>
       </c>
       <c r="C14" s="29">
-        <v>1088</v>
-      </c>
-      <c r="D14">
+        <v>1201</v>
+      </c>
+      <c r="D14" s="44">
         <f t="shared" si="0"/>
-        <v>-322</v>
+        <v>-406</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7082,14 +7083,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="29">
-        <v>4153</v>
+        <v>4555</v>
       </c>
       <c r="C15" s="29">
-        <v>1767</v>
-      </c>
-      <c r="D15">
+        <v>1849</v>
+      </c>
+      <c r="D15" s="44">
         <f t="shared" si="0"/>
-        <v>2386</v>
+        <v>2706</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7097,14 +7098,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="29">
-        <v>4333</v>
+        <v>4655</v>
       </c>
       <c r="C16" s="29">
-        <v>2507</v>
-      </c>
-      <c r="D16">
+        <v>2534</v>
+      </c>
+      <c r="D16" s="44">
         <f t="shared" si="0"/>
-        <v>1826</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7112,14 +7113,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="29">
-        <v>3786</v>
+        <v>3964</v>
       </c>
       <c r="C17" s="29">
-        <v>1158</v>
-      </c>
-      <c r="D17">
+        <v>1179</v>
+      </c>
+      <c r="D17" s="44">
         <f t="shared" si="0"/>
-        <v>2628</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7127,44 +7128,44 @@
         <v>95</v>
       </c>
       <c r="B18" s="29">
-        <v>420</v>
+        <v>463</v>
       </c>
       <c r="C18" s="29">
-        <v>189</v>
-      </c>
-      <c r="D18">
+        <v>195</v>
+      </c>
+      <c r="D18" s="44">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="29">
-        <v>839</v>
-      </c>
-      <c r="C19" s="29">
-        <v>447</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="45">
+        <v>864</v>
+      </c>
+      <c r="C19" s="45">
+        <v>515</v>
+      </c>
+      <c r="D19" s="44">
         <f t="shared" si="0"/>
-        <v>392</v>
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="30">
-        <v>5444</v>
-      </c>
-      <c r="C20" s="30">
-        <v>2630</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="45">
+        <v>5832</v>
+      </c>
+      <c r="C20" s="45">
+        <v>2779</v>
+      </c>
+      <c r="D20" s="44">
         <f t="shared" si="0"/>
-        <v>2814</v>
+        <v>3053</v>
       </c>
     </row>
   </sheetData>
@@ -7193,419 +7194,419 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="35">
-        <v>82293</v>
+      <c r="B2" s="34">
+        <v>88446</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="35">
-        <v>22586</v>
+      <c r="B3" s="34">
+        <v>23868</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>138</v>
       </c>
       <c r="B4" s="29">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>139</v>
       </c>
       <c r="B5" s="29">
-        <v>1448</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>140</v>
       </c>
       <c r="B6" s="29">
-        <v>236</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>141</v>
       </c>
       <c r="B7" s="29">
-        <v>568</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="29">
-        <v>500</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>143</v>
       </c>
       <c r="B9" s="29">
-        <v>14684</v>
+        <v>15575</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B10" s="29">
-        <v>4230</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>145</v>
       </c>
       <c r="B11" s="29">
-        <v>283</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>146</v>
       </c>
       <c r="B12" s="29">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>147</v>
       </c>
       <c r="B13" s="29">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="29">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="34">
+        <v>33119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="29">
+        <v>4158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="29">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="29">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="29">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="29">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="29">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="29">
+        <v>9170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="29">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="29">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="29">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="29">
+        <v>13249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="29">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="29">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="29">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="29">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="34">
+        <v>23061</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="29">
+        <v>6119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="29">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="29">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" s="29">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="29">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="29">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="29">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="B16" s="35">
-        <v>30767</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="29">
-        <v>3909</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="29">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="29">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="29">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="29">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="B22" s="29">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="B23" s="29">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="B24" s="29">
-        <v>8591</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="29">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="29">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27" s="29">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28" s="29">
-        <v>12230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="29">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="B30" s="29">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" s="29">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="B32" s="29">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="B33" s="35">
-        <v>21389</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="B34" s="29">
-        <v>5727</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="B35" s="29">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="29">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="B37" s="29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B38" s="29">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="B39" s="29">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
-        <v>172</v>
-      </c>
       <c r="B40" s="29">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>173</v>
       </c>
       <c r="B41" s="29">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>174</v>
       </c>
       <c r="B42" s="29">
-        <v>2407</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>175</v>
       </c>
       <c r="B43" s="29">
-        <v>1942</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>176</v>
       </c>
       <c r="B44" s="29">
-        <v>1467</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="30" t="s">
         <v>177</v>
       </c>
       <c r="B45" s="29">
-        <v>7341</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>178</v>
       </c>
       <c r="B46" s="29">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>179</v>
       </c>
       <c r="B47" s="29">
-        <v>273</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="35">
-        <v>7551</v>
+      <c r="B48" s="34">
+        <v>8398</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="30" t="s">
         <v>180</v>
       </c>
       <c r="B49" s="29">
-        <v>3541</v>
+        <v>3867</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="30" t="s">
         <v>181</v>
       </c>
       <c r="B50" s="29">
-        <v>2285</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="30" t="s">
         <v>182</v>
       </c>
       <c r="B51" s="29">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="B52" s="41">
-        <v>1187</v>
+      <c r="B52" s="40">
+        <v>1369</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="B53" s="42">
-        <v>453</v>
+      <c r="B53" s="41">
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -7618,7 +7619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7634,315 +7637,315 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="35">
-        <v>76493</v>
+      <c r="B2" s="34">
+        <v>81523</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="35">
-        <v>11582</v>
+      <c r="B3" s="34">
+        <v>12454</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>190</v>
       </c>
       <c r="B4" s="29">
-        <v>8731</v>
+        <v>9352</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>191</v>
       </c>
       <c r="B5" s="29">
-        <v>1218</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>192</v>
       </c>
       <c r="B6" s="29">
-        <v>1220</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>193</v>
       </c>
       <c r="B7" s="29">
-        <v>413</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="35">
-        <v>28161</v>
+      <c r="B8" s="34">
+        <v>30009</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="35" t="s">
         <v>194</v>
       </c>
       <c r="B9" s="29">
-        <v>2465</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="35" t="s">
         <v>195</v>
       </c>
       <c r="B10" s="29">
-        <v>1358</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="35" t="s">
         <v>196</v>
       </c>
       <c r="B11" s="29">
-        <v>11662</v>
+        <v>12381</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>197</v>
       </c>
       <c r="B12" s="29">
-        <v>3574</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>198</v>
       </c>
       <c r="B13" s="29">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="29">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="29">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="29">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="34">
+        <v>12868</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="29">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="29">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="34">
+        <v>15037</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="29">
+        <v>9705</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="29">
+        <v>4231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" s="29">
         <v>1100</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="34">
+        <v>8567</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="29">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="29">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" s="29">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="29">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="29">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="29">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" s="29">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="B16" s="29">
-        <v>3993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" s="29">
-        <v>2082</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="B18" s="35">
-        <v>12419</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="B19" s="29">
-        <v>12084</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="B20" s="29">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="B21" s="35">
-        <v>14011</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="B31" s="29">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="29">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="B22" s="29">
-        <v>9053</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="B33" s="29">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="29">
-        <v>3943</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="B24" s="29">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="B25" s="35">
-        <v>7890</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="B26" s="29">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27" s="29">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="B28" s="29">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="B29" s="29">
-        <v>2338</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" s="29">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="B31" s="29">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>207</v>
-      </c>
-      <c r="B32" s="29">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="B33" s="29">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
+      <c r="B34" s="29">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="29">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="29">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="29">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="34">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="B34" s="29">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="B35" s="29">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>208</v>
-      </c>
-      <c r="B36" s="29">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="B37" s="29">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="B38" s="35">
-        <v>1868</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="B39" s="39">
-        <v>1868</v>
+      <c r="B39" s="38">
+        <v>1996</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="B40" s="40">
-        <v>561</v>
+      <c r="B40" s="39">
+        <v>592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo dato IPC ene23"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBBA5B8-A981-40F9-8B85-D95E653052F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0640FD1E-1420-4FEB-BECB-54A71CA3F85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -942,6 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -1257,7 +1258,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1265,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73:E73"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,6 +2519,23 @@
       </c>
       <c r="E73">
         <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="22">
+        <v>44927</v>
+      </c>
+      <c r="B74" s="1">
+        <v>6</v>
+      </c>
+      <c r="C74">
+        <v>7.9</v>
+      </c>
+      <c r="D74">
+        <v>5.4</v>
+      </c>
+      <c r="E74">
+        <v>7.1</v>
       </c>
     </row>
   </sheetData>
@@ -2746,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3981,25 +3999,25 @@
         <v>129</v>
       </c>
       <c r="B2" s="23">
-        <v>6.7</v>
+        <v>3.9</v>
       </c>
       <c r="C2" s="23">
-        <v>5.5</v>
-      </c>
-      <c r="D2" s="23">
         <v>4.7</v>
       </c>
+      <c r="D2" s="45">
+        <v>4.5</v>
+      </c>
       <c r="E2" s="27">
-        <v>3.9</v>
+        <v>5</v>
       </c>
       <c r="F2" s="23">
-        <v>5.6</v>
+        <v>5.2</v>
       </c>
       <c r="G2" s="23">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="H2" s="16">
-        <v>5.7811072314744472</v>
+        <v>4.3505747899345248</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4007,25 +4025,25 @@
         <v>130</v>
       </c>
       <c r="B3" s="23">
+        <v>3.9</v>
+      </c>
+      <c r="C3" s="23">
+        <v>4</v>
+      </c>
+      <c r="D3" s="45">
         <v>3</v>
       </c>
-      <c r="C3" s="23">
-        <v>2.8</v>
-      </c>
-      <c r="D3" s="23">
-        <v>3</v>
-      </c>
       <c r="E3" s="27">
-        <v>1.9</v>
+        <v>3.7</v>
       </c>
       <c r="F3" s="23">
-        <v>1.3</v>
+        <v>4.2</v>
       </c>
       <c r="G3" s="23">
-        <v>1.5</v>
+        <v>4.7</v>
       </c>
       <c r="H3" s="16">
-        <v>2.7104372959828815</v>
+        <v>3.9729491721527843</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4033,25 +4051,25 @@
         <v>131</v>
       </c>
       <c r="B4" s="23">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="C4" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="D4" s="23">
-        <v>3.3</v>
+        <v>5</v>
+      </c>
+      <c r="D4" s="45">
+        <v>4.7</v>
       </c>
       <c r="E4" s="27">
-        <v>3.7</v>
+        <v>4.3</v>
       </c>
       <c r="F4" s="23">
-        <v>5.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G4" s="23">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H4" s="16">
-        <v>4.5748634597068571</v>
+        <v>4.7980030262997131</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4059,25 +4077,25 @@
         <v>132</v>
       </c>
       <c r="B5" s="23">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="C5" s="23">
-        <v>3.4</v>
-      </c>
-      <c r="D5" s="23">
-        <v>2.2999999999999998</v>
+        <v>5.9</v>
+      </c>
+      <c r="D5" s="45">
+        <v>4.2</v>
       </c>
       <c r="E5" s="27">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="F5" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5" s="23">
-        <v>3.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H5" s="16">
-        <v>3.2585617546448287</v>
+        <v>4.5381878659563668</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4085,25 +4103,25 @@
         <v>133</v>
       </c>
       <c r="B6" s="23">
-        <v>10</v>
+        <v>11.6</v>
       </c>
       <c r="C6" s="23">
-        <v>11.8</v>
-      </c>
-      <c r="D6" s="23">
-        <v>9.5</v>
+        <v>11</v>
+      </c>
+      <c r="D6" s="45">
+        <v>11.1</v>
       </c>
       <c r="E6" s="27">
-        <v>10.1</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="F6" s="23">
-        <v>11.9</v>
+        <v>13</v>
       </c>
       <c r="G6" s="23">
-        <v>10.8</v>
+        <v>6.6</v>
       </c>
       <c r="H6" s="16">
-        <v>10.693876032523253</v>
+        <v>11.328161553523852</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4111,25 +4129,25 @@
         <v>134</v>
       </c>
       <c r="B7" s="23">
-        <v>8.9</v>
+        <v>16.7</v>
       </c>
       <c r="C7" s="23">
-        <v>3.7</v>
-      </c>
-      <c r="D7" s="23">
-        <v>1.9</v>
+        <v>21.4</v>
+      </c>
+      <c r="D7" s="45">
+        <v>22.3</v>
       </c>
       <c r="E7" s="27">
-        <v>1.8</v>
+        <v>27.5</v>
       </c>
       <c r="F7" s="23">
-        <v>-7.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G7" s="23">
-        <v>-0.8</v>
+        <v>11</v>
       </c>
       <c r="H7" s="16">
-        <v>5.3981385841979979</v>
+        <v>18.783144086032433</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4137,25 +4155,25 @@
         <v>135</v>
       </c>
       <c r="B8" s="23">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="C8" s="23">
-        <v>4.3</v>
-      </c>
-      <c r="D8" s="23">
-        <v>2.9</v>
+        <v>5.9</v>
+      </c>
+      <c r="D8" s="45">
+        <v>7.6</v>
       </c>
       <c r="E8" s="27">
-        <v>4.2</v>
+        <v>5.9</v>
       </c>
       <c r="F8" s="23">
-        <v>4.3</v>
+        <v>5</v>
       </c>
       <c r="G8" s="23">
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H8" s="16">
-        <v>4.0457604635309563</v>
+        <v>5.3605104694679939</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4163,25 +4181,25 @@
         <v>136</v>
       </c>
       <c r="B9" s="23">
-        <v>3.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C9" s="23">
-        <v>3.3</v>
-      </c>
-      <c r="D9" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="45">
+        <v>3.9</v>
+      </c>
+      <c r="E9" s="27">
+        <v>5.7</v>
+      </c>
+      <c r="F9" s="23">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G9" s="23">
         <v>2.5</v>
       </c>
-      <c r="E9" s="27">
-        <v>3.9</v>
-      </c>
-      <c r="F9" s="23">
-        <v>5.8</v>
-      </c>
-      <c r="G9" s="23">
-        <v>3.1</v>
-      </c>
       <c r="H9" s="16">
-        <v>3.3537378532720874</v>
+        <v>3.8502752079279334</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4189,25 +4207,25 @@
         <v>137</v>
       </c>
       <c r="B10" s="23">
-        <v>9.3000000000000007</v>
+        <v>10</v>
       </c>
       <c r="C10" s="23">
-        <v>6.8</v>
-      </c>
-      <c r="D10" s="23">
-        <v>4.9000000000000004</v>
+        <v>5.2</v>
+      </c>
+      <c r="D10" s="45">
+        <v>7.8</v>
       </c>
       <c r="E10" s="27">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
       <c r="F10" s="23">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="G10" s="23">
-        <v>6.2</v>
+        <v>5.8</v>
       </c>
       <c r="H10" s="16">
-        <v>7.5694508692788487</v>
+        <v>7.3876880211027673</v>
       </c>
     </row>
   </sheetData>
@@ -4257,25 +4275,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="19">
-        <v>5.0999999999999996</v>
+        <v>6</v>
       </c>
       <c r="C2" s="25">
-        <v>5.3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="25">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="E2" s="25">
-        <v>4.8</v>
+        <v>5.6</v>
       </c>
       <c r="F2" s="25">
-        <v>4.7</v>
+        <v>6.3</v>
       </c>
       <c r="G2" s="25">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="H2" s="19">
-        <v>4.5</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4283,25 +4301,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="18">
-        <v>4.7</v>
+        <v>6.8</v>
       </c>
       <c r="C3" s="24">
+        <v>6.6</v>
+      </c>
+      <c r="D3" s="24">
+        <v>6.9</v>
+      </c>
+      <c r="E3" s="24">
+        <v>6.6</v>
+      </c>
+      <c r="F3" s="24">
+        <v>7.9</v>
+      </c>
+      <c r="G3" s="24">
+        <v>7</v>
+      </c>
+      <c r="H3" s="18">
         <v>5.5</v>
-      </c>
-      <c r="D3" s="24">
-        <v>4.5</v>
-      </c>
-      <c r="E3" s="24">
-        <v>3.6</v>
-      </c>
-      <c r="F3" s="24">
-        <v>3.3</v>
-      </c>
-      <c r="G3" s="24">
-        <v>2.7</v>
-      </c>
-      <c r="H3" s="18">
-        <v>3.4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4309,25 +4327,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="18">
-        <v>7.1</v>
+        <v>7.3</v>
       </c>
       <c r="C4" s="24">
-        <v>6.7</v>
+        <v>7.6</v>
       </c>
       <c r="D4" s="24">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="24">
         <v>7</v>
       </c>
       <c r="F4" s="24">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="G4" s="24">
-        <v>8.1999999999999993</v>
+        <v>6.6</v>
       </c>
       <c r="H4" s="18">
-        <v>7.1</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4335,25 +4353,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="18">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C5" s="24">
-        <v>4.0999999999999996</v>
+        <v>1.4</v>
       </c>
       <c r="D5" s="24">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="E5" s="24">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="F5" s="24">
-        <v>4.2</v>
+        <v>2.5</v>
       </c>
       <c r="G5" s="24">
-        <v>4.3</v>
+        <v>2.9</v>
       </c>
       <c r="H5" s="18">
-        <v>4.2</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4361,25 +4379,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="18">
-        <v>4.2</v>
+        <v>8</v>
       </c>
       <c r="C6" s="24">
-        <v>4.2</v>
+        <v>7.8</v>
       </c>
       <c r="D6" s="24">
-        <v>4.4000000000000004</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E6" s="24">
-        <v>4.4000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="F6" s="24">
-        <v>3.5</v>
+        <v>7.3</v>
       </c>
       <c r="G6" s="24">
-        <v>3.6</v>
+        <v>11.7</v>
       </c>
       <c r="H6" s="18">
-        <v>4.3</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4387,25 +4405,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="18">
+        <v>5.4</v>
+      </c>
+      <c r="C7" s="24">
+        <v>5</v>
+      </c>
+      <c r="D7" s="24">
+        <v>5.6</v>
+      </c>
+      <c r="E7" s="24">
+        <v>6.5</v>
+      </c>
+      <c r="F7" s="24">
+        <v>5.7</v>
+      </c>
+      <c r="G7" s="24">
         <v>5.9</v>
       </c>
-      <c r="C7" s="24">
-        <v>6.3</v>
-      </c>
-      <c r="D7" s="24">
-        <v>5.5</v>
-      </c>
-      <c r="E7" s="24">
-        <v>6.6</v>
-      </c>
-      <c r="F7" s="24">
-        <v>6.4</v>
-      </c>
-      <c r="G7" s="24">
-        <v>6</v>
-      </c>
       <c r="H7" s="18">
-        <v>4</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4413,25 +4431,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="18">
-        <v>5.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C8" s="24">
         <v>5.5</v>
       </c>
       <c r="D8" s="24">
-        <v>6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E8" s="24">
-        <v>5.2</v>
+        <v>4.2</v>
       </c>
       <c r="F8" s="24">
-        <v>5.5</v>
+        <v>4.3</v>
       </c>
       <c r="G8" s="24">
-        <v>5.6</v>
+        <v>4</v>
       </c>
       <c r="H8" s="18">
-        <v>5.7</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4439,25 +4457,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="18">
+        <v>5.9</v>
+      </c>
+      <c r="C9" s="24">
+        <v>6.3</v>
+      </c>
+      <c r="D9" s="24">
+        <v>5.9</v>
+      </c>
+      <c r="E9" s="24">
+        <v>5.3</v>
+      </c>
+      <c r="F9" s="24">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G9" s="24">
         <v>5.8</v>
       </c>
-      <c r="C9" s="24">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D9" s="24">
-        <v>6.1</v>
-      </c>
-      <c r="E9" s="24">
-        <v>6.3</v>
-      </c>
-      <c r="F9" s="24">
-        <v>6.2</v>
-      </c>
-      <c r="G9" s="24">
-        <v>8.1</v>
-      </c>
       <c r="H9" s="18">
-        <v>5.0999999999999996</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4465,25 +4483,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="18">
-        <v>3.4</v>
+        <v>8</v>
       </c>
       <c r="C10" s="24">
-        <v>2.6</v>
+        <v>8.1</v>
       </c>
       <c r="D10" s="24">
-        <v>3.5</v>
+        <v>7.4</v>
       </c>
       <c r="E10" s="24">
-        <v>3.7</v>
+        <v>7</v>
       </c>
       <c r="F10" s="24">
-        <v>5.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G10" s="24">
-        <v>6.2</v>
+        <v>8</v>
       </c>
       <c r="H10" s="18">
-        <v>3.6</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4491,25 +4509,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="18">
-        <v>4.5999999999999996</v>
+        <v>9</v>
       </c>
       <c r="C11" s="24">
-        <v>3.9</v>
+        <v>10.5</v>
       </c>
       <c r="D11" s="24">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
       <c r="E11" s="24">
-        <v>6.5</v>
+        <v>7.6</v>
       </c>
       <c r="F11" s="24">
-        <v>6.4</v>
+        <v>7.3</v>
       </c>
       <c r="G11" s="24">
-        <v>4.9000000000000004</v>
+        <v>7.8</v>
       </c>
       <c r="H11" s="18">
-        <v>6</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4517,25 +4535,25 @@
         <v>22</v>
       </c>
       <c r="B12" s="18">
-        <v>3.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="24">
-        <v>5.5</v>
+        <v>0.7</v>
       </c>
       <c r="D12" s="24">
-        <v>2.9</v>
+        <v>2</v>
       </c>
       <c r="E12" s="24">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F12" s="24">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G12" s="24">
-        <v>2.1</v>
+        <v>1.2</v>
       </c>
       <c r="H12" s="18">
-        <v>1.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4543,25 +4561,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="18">
-        <v>7.2</v>
+        <v>6.2</v>
       </c>
       <c r="C13" s="24">
-        <v>7.4</v>
+        <v>5.5</v>
       </c>
       <c r="D13" s="24">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="E13" s="24">
-        <v>7.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F13" s="24">
-        <v>6.5</v>
+        <v>8.9</v>
       </c>
       <c r="G13" s="24">
-        <v>8.5</v>
+        <v>7.7</v>
       </c>
       <c r="H13" s="18">
-        <v>7.4</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4569,25 +4587,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="18">
-        <v>5.7</v>
+        <v>6.8</v>
       </c>
       <c r="C14" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="24">
-        <v>5.5</v>
+        <v>6.6</v>
       </c>
       <c r="E14" s="24">
-        <v>4.5</v>
+        <v>7.8</v>
       </c>
       <c r="F14" s="24">
-        <v>6.6</v>
+        <v>5.8</v>
       </c>
       <c r="G14" s="24">
-        <v>5.7</v>
+        <v>7.4</v>
       </c>
       <c r="H14" s="18">
-        <v>5.0999999999999996</v>
+        <v>6.3</v>
       </c>
     </row>
   </sheetData>
@@ -4600,9 +4618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4637,25 +4653,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="21">
-        <v>94.8</v>
+        <v>98.8</v>
       </c>
       <c r="C2" s="26">
-        <v>95.2</v>
+        <v>99</v>
       </c>
       <c r="D2" s="26">
-        <v>94.2</v>
+        <v>98.3</v>
       </c>
       <c r="E2" s="26">
-        <v>96</v>
+        <v>100.2</v>
       </c>
       <c r="F2" s="26">
-        <v>95.1</v>
+        <v>99.4</v>
       </c>
       <c r="G2" s="26">
-        <v>94.4</v>
+        <v>98.7</v>
       </c>
       <c r="H2" s="26">
-        <v>94.3</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4663,25 +4679,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="20">
+        <v>98.4</v>
+      </c>
+      <c r="C3" s="17">
+        <v>100.3</v>
+      </c>
+      <c r="D3" s="17">
+        <v>96.7</v>
+      </c>
+      <c r="E3" s="17">
+        <v>97.9</v>
+      </c>
+      <c r="F3" s="17">
         <v>95</v>
       </c>
-      <c r="C3" s="17">
-        <v>97.5</v>
-      </c>
-      <c r="D3" s="17">
-        <v>93.3</v>
-      </c>
-      <c r="E3" s="17">
-        <v>92.6</v>
-      </c>
-      <c r="F3" s="17">
-        <v>89.9</v>
-      </c>
       <c r="G3" s="17">
-        <v>91.7</v>
+        <v>96.8</v>
       </c>
       <c r="H3" s="17">
-        <v>97.5</v>
+        <v>100.7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4689,25 +4705,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="20">
-        <v>92.9</v>
+        <v>103.3</v>
       </c>
       <c r="C4" s="17">
-        <v>92.7</v>
+        <v>104</v>
       </c>
       <c r="D4" s="17">
-        <v>94</v>
+        <v>103.3</v>
       </c>
       <c r="E4" s="17">
-        <v>95.8</v>
+        <v>105.4</v>
       </c>
       <c r="F4" s="17">
-        <v>90</v>
+        <v>100.7</v>
       </c>
       <c r="G4" s="17">
-        <v>91.9</v>
+        <v>101.3</v>
       </c>
       <c r="H4" s="17">
-        <v>88.4</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4715,25 +4731,25 @@
         <v>15</v>
       </c>
       <c r="B5" s="20">
-        <v>120.8</v>
+        <v>120.6</v>
       </c>
       <c r="C5" s="17">
-        <v>121.3</v>
+        <v>120.1</v>
       </c>
       <c r="D5" s="17">
-        <v>120.5</v>
+        <v>121.4</v>
       </c>
       <c r="E5" s="17">
-        <v>115.5</v>
+        <v>117.6</v>
       </c>
       <c r="F5" s="17">
-        <v>123.8</v>
+        <v>122</v>
       </c>
       <c r="G5" s="17">
-        <v>117.6</v>
+        <v>117.8</v>
       </c>
       <c r="H5" s="17">
-        <v>121.6</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4741,25 +4757,25 @@
         <v>16</v>
       </c>
       <c r="B6" s="20">
-        <v>80.400000000000006</v>
+        <v>91.5</v>
       </c>
       <c r="C6" s="17">
-        <v>83.2</v>
+        <v>95.6</v>
       </c>
       <c r="D6" s="17">
-        <v>73</v>
+        <v>84.3</v>
       </c>
       <c r="E6" s="17">
-        <v>111.8</v>
+        <v>113.1</v>
       </c>
       <c r="F6" s="17">
-        <v>87</v>
+        <v>96.4</v>
       </c>
       <c r="G6" s="17">
-        <v>68.7</v>
+        <v>82.9</v>
       </c>
       <c r="H6" s="17">
-        <v>75.5</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4767,25 +4783,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="20">
-        <v>97.2</v>
+        <v>101.2</v>
       </c>
       <c r="C7" s="17">
-        <v>98</v>
+        <v>100.6</v>
       </c>
       <c r="D7" s="17">
-        <v>97.8</v>
+        <v>102.8</v>
       </c>
       <c r="E7" s="17">
-        <v>95.3</v>
+        <v>101.7</v>
       </c>
       <c r="F7" s="17">
-        <v>97.4</v>
+        <v>101.1</v>
       </c>
       <c r="G7" s="17">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H7" s="17">
-        <v>87.1</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4793,25 +4809,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="20">
-        <v>90.9</v>
+        <v>92.3</v>
       </c>
       <c r="C8" s="17">
-        <v>91.7</v>
+        <v>92.8</v>
       </c>
       <c r="D8" s="17">
-        <v>90.8</v>
+        <v>92.5</v>
       </c>
       <c r="E8" s="17">
-        <v>88.2</v>
+        <v>89.5</v>
       </c>
       <c r="F8" s="17">
-        <v>89.4</v>
+        <v>91.6</v>
       </c>
       <c r="G8" s="17">
-        <v>92.6</v>
+        <v>93.3</v>
       </c>
       <c r="H8" s="17">
-        <v>87.4</v>
+        <v>89.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4819,25 +4835,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="20">
-        <v>86.2</v>
+        <v>92</v>
       </c>
       <c r="C9" s="17">
-        <v>80.2</v>
+        <v>87.8</v>
       </c>
       <c r="D9" s="17">
-        <v>91</v>
+        <v>95.3</v>
       </c>
       <c r="E9" s="17">
-        <v>94.2</v>
+        <v>98.4</v>
       </c>
       <c r="F9" s="17">
-        <v>89.7</v>
+        <v>93.7</v>
       </c>
       <c r="G9" s="17">
-        <v>93.3</v>
+        <v>98.2</v>
       </c>
       <c r="H9" s="17">
-        <v>84.5</v>
+        <v>88.6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4845,25 +4861,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="20">
-        <v>67.8</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="C10" s="17">
-        <v>66.599999999999994</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="D10" s="17">
-        <v>67.3</v>
+        <v>69.2</v>
       </c>
       <c r="E10" s="17">
-        <v>70.400000000000006</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="F10" s="17">
-        <v>70.400000000000006</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="G10" s="17">
-        <v>77.5</v>
+        <v>78.7</v>
       </c>
       <c r="H10" s="17">
-        <v>67.3</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4871,25 +4887,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="20">
-        <v>83.2</v>
+        <v>91.6</v>
       </c>
       <c r="C11" s="17">
-        <v>82.2</v>
+        <v>91.5</v>
       </c>
       <c r="D11" s="17">
-        <v>81.8</v>
+        <v>89.9</v>
       </c>
       <c r="E11" s="17">
-        <v>82.4</v>
+        <v>90.4</v>
       </c>
       <c r="F11" s="17">
-        <v>90.4</v>
+        <v>97.5</v>
       </c>
       <c r="G11" s="17">
-        <v>89.3</v>
+        <v>93.2</v>
       </c>
       <c r="H11" s="17">
-        <v>86.9</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4897,22 +4913,22 @@
         <v>22</v>
       </c>
       <c r="B12" s="20">
-        <v>86.3</v>
+        <v>86.9</v>
       </c>
       <c r="C12" s="17">
         <v>91.1</v>
       </c>
       <c r="D12" s="17">
-        <v>88.7</v>
+        <v>91</v>
       </c>
       <c r="E12" s="17">
-        <v>63.8</v>
+        <v>63.1</v>
       </c>
       <c r="F12" s="17">
-        <v>61.1</v>
+        <v>59</v>
       </c>
       <c r="G12" s="17">
-        <v>84.3</v>
+        <v>84.9</v>
       </c>
       <c r="H12" s="17">
         <v>82.8</v>
@@ -4923,25 +4939,25 @@
         <v>23</v>
       </c>
       <c r="B13" s="20">
-        <v>108.8</v>
+        <v>109.9</v>
       </c>
       <c r="C13" s="17">
-        <v>110.4</v>
+        <v>109.5</v>
       </c>
       <c r="D13" s="17">
-        <v>105.6</v>
+        <v>108.5</v>
       </c>
       <c r="E13" s="17">
-        <v>104.9</v>
+        <v>103.7</v>
       </c>
       <c r="F13" s="17">
-        <v>107.7</v>
+        <v>114.6</v>
       </c>
       <c r="G13" s="17">
-        <v>109.5</v>
+        <v>107.4</v>
       </c>
       <c r="H13" s="17">
-        <v>124.1</v>
+        <v>128.6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4949,25 +4965,25 @@
         <v>24</v>
       </c>
       <c r="B14" s="20">
-        <v>97.8</v>
+        <v>102.6</v>
       </c>
       <c r="C14" s="17">
-        <v>99.2</v>
+        <v>103.2</v>
       </c>
       <c r="D14" s="17">
-        <v>95</v>
+        <v>100.2</v>
       </c>
       <c r="E14" s="17">
-        <v>97.5</v>
+        <v>106.6</v>
       </c>
       <c r="F14" s="17">
-        <v>101.2</v>
+        <v>102.9</v>
       </c>
       <c r="G14" s="17">
-        <v>98.3</v>
+        <v>105.5</v>
       </c>
       <c r="H14" s="17">
-        <v>100.5</v>
+        <v>106.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo dato fiscal(ene23), comex(ene23) y EMAE(dic22)"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0640FD1E-1420-4FEB-BECB-54A71CA3F85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEEEC0E-5568-40F4-BC1B-6BD07E43BF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -939,10 +939,10 @@
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Millares 2" xfId="6" xr:uid="{FE049F7D-2F48-430C-A6DF-C6EF2EAFCD09}"/>
@@ -2762,7 +2762,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2795,10 +2795,10 @@
         <v>134.74645041349706</v>
       </c>
       <c r="C2" s="17">
-        <v>148.06837655019177</v>
+        <v>148.09781687508269</v>
       </c>
       <c r="D2" s="17">
-        <v>147.16551169690666</v>
+        <v>147.14774244532654</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2809,10 +2809,10 @@
         <v>134.23236103862521</v>
       </c>
       <c r="C3" s="17">
-        <v>146.89390746145679</v>
+        <v>146.85724058197701</v>
       </c>
       <c r="D3" s="17">
-        <v>146.58096921123607</v>
+        <v>146.56012078879479</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2823,10 +2823,10 @@
         <v>150.0878942366954</v>
       </c>
       <c r="C4" s="17">
-        <v>145.93861412106708</v>
+        <v>145.91183905423966</v>
       </c>
       <c r="D4" s="17">
-        <v>146.02780883939749</v>
+        <v>146.00464141468905</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2837,10 +2837,10 @@
         <v>153.25067436662908</v>
       </c>
       <c r="C5" s="17">
-        <v>144.92583830611622</v>
+        <v>144.94045883030842</v>
       </c>
       <c r="D5" s="17">
-        <v>145.54258020771528</v>
+        <v>145.51844932058611</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2851,10 +2851,10 @@
         <v>163.51360808690507</v>
       </c>
       <c r="C6" s="17">
-        <v>144.29880566854044</v>
+        <v>144.28815945954597</v>
       </c>
       <c r="D6" s="17">
-        <v>145.15237920515557</v>
+        <v>145.12909256360066</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2865,10 +2865,10 @@
         <v>153.66209524099784</v>
       </c>
       <c r="C7" s="17">
-        <v>144.31186497751932</v>
+        <v>144.29695670672598</v>
       </c>
       <c r="D7" s="17">
-        <v>144.87764988273338</v>
+        <v>144.85734759313118</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2879,10 +2879,10 @@
         <v>143.73110098180126</v>
       </c>
       <c r="C8" s="17">
-        <v>144.53084253362229</v>
+        <v>144.5293133812859</v>
       </c>
       <c r="D8" s="17">
-        <v>144.72909537766017</v>
+        <v>144.71396590970363</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2893,10 +2893,10 @@
         <v>143.6741026486049</v>
       </c>
       <c r="C9" s="17">
-        <v>145.64921557765905</v>
+        <v>145.62859095858317</v>
       </c>
       <c r="D9" s="17">
-        <v>144.71277692563149</v>
+        <v>144.70459239852221</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,10 +2907,10 @@
         <v>142.00773744282046</v>
       </c>
       <c r="C10" s="17">
-        <v>145.13070998219706</v>
+        <v>145.14335425694165</v>
       </c>
       <c r="D10" s="17">
-        <v>144.83056500409469</v>
+        <v>144.82969525678999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2921,10 +2921,10 @@
         <v>141.13686329808141</v>
       </c>
       <c r="C11" s="17">
-        <v>145.0274228044903</v>
+        <v>145.04100595588346</v>
       </c>
       <c r="D11" s="17">
-        <v>145.07535526748032</v>
+        <v>145.08137119882068</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2935,10 +2935,10 @@
         <v>144.93832064073018</v>
       </c>
       <c r="C12" s="17">
-        <v>145.66981735968793</v>
+        <v>145.67021135835745</v>
       </c>
       <c r="D12" s="17">
-        <v>145.43350036999664</v>
+        <v>145.44555093391483</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2949,10 +2949,10 @@
         <v>142.59014516031914</v>
       </c>
       <c r="C13" s="17">
-        <v>147.12593839261095</v>
+        <v>147.16640630451579</v>
       </c>
       <c r="D13" s="17">
-        <v>145.89149062929727</v>
+        <v>145.90850125081869</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2960,13 +2960,13 @@
         <v>42736</v>
       </c>
       <c r="B14" s="17">
-        <v>136.6326594831489</v>
+        <v>136.6326594831485</v>
       </c>
       <c r="C14" s="17">
-        <v>147.39725835631219</v>
+        <v>147.42694362959375</v>
       </c>
       <c r="D14" s="17">
-        <v>146.43179333426133</v>
+        <v>146.45256013743753</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2974,13 +2974,13 @@
         <v>42767</v>
       </c>
       <c r="B15" s="17">
-        <v>132.15851633981728</v>
+        <v>132.15851633981686</v>
       </c>
       <c r="C15" s="17">
-        <v>146.6968247749389</v>
+        <v>146.64593944951392</v>
       </c>
       <c r="D15" s="17">
-        <v>147.03519059275723</v>
+        <v>147.05850079219746</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2988,13 +2988,13 @@
         <v>42795</v>
       </c>
       <c r="B16" s="17">
-        <v>152.6209585590764</v>
+        <v>152.62095855907597</v>
       </c>
       <c r="C16" s="17">
-        <v>147.72900371364153</v>
+        <v>147.72834469571572</v>
       </c>
       <c r="D16" s="17">
-        <v>147.68013838016415</v>
+        <v>147.70482600905757</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,13 +3002,13 @@
         <v>42826</v>
       </c>
       <c r="B17" s="17">
-        <v>151.94634480454781</v>
+        <v>151.94634480454735</v>
       </c>
       <c r="C17" s="17">
-        <v>147.75487367868138</v>
+        <v>147.77279586107181</v>
       </c>
       <c r="D17" s="17">
-        <v>148.34261372363508</v>
+        <v>148.36748499434708</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3016,13 +3016,13 @@
         <v>42856</v>
       </c>
       <c r="B18" s="17">
-        <v>168.38920946939336</v>
+        <v>168.38920946939297</v>
       </c>
       <c r="C18" s="17">
-        <v>148.45732696422368</v>
+        <v>148.43003835797487</v>
       </c>
       <c r="D18" s="17">
-        <v>148.9932798162819</v>
+        <v>149.01724779008339</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3030,13 +3030,13 @@
         <v>42887</v>
       </c>
       <c r="B19" s="17">
-        <v>161.03568546936674</v>
+        <v>161.03568546936634</v>
       </c>
       <c r="C19" s="17">
-        <v>150.21113869160331</v>
+        <v>150.19858684933394</v>
       </c>
       <c r="D19" s="17">
-        <v>149.60053164965973</v>
+        <v>149.62274626727162</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3044,13 +3044,13 @@
         <v>42917</v>
       </c>
       <c r="B20" s="17">
-        <v>150.306050123647</v>
+        <v>150.3060501236466</v>
       </c>
       <c r="C20" s="17">
-        <v>150.32261694242445</v>
+        <v>150.31733326732902</v>
       </c>
       <c r="D20" s="17">
-        <v>150.13045811802581</v>
+        <v>150.15033572994142</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3058,13 +3058,13 @@
         <v>42948</v>
       </c>
       <c r="B21" s="17">
-        <v>149.25534277372614</v>
+        <v>149.25534277372569</v>
       </c>
       <c r="C21" s="17">
-        <v>150.43915440027206</v>
+        <v>150.39979835382428</v>
       </c>
       <c r="D21" s="17">
-        <v>150.54812066513648</v>
+        <v>150.56533138942777</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3072,13 +3072,13 @@
         <v>42979</v>
       </c>
       <c r="B22" s="17">
-        <v>146.38655965814226</v>
+        <v>146.38655965814183</v>
       </c>
       <c r="C22" s="17">
-        <v>151.32568911576828</v>
+        <v>151.33295464927085</v>
       </c>
       <c r="D22" s="17">
-        <v>150.81902753322555</v>
+        <v>150.83344617993779</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3086,13 +3086,13 @@
         <v>43009</v>
       </c>
       <c r="B23" s="17">
-        <v>149.38594966725174</v>
+        <v>149.38594966725128</v>
       </c>
       <c r="C23" s="17">
-        <v>151.54012169303923</v>
+        <v>151.53625500268183</v>
       </c>
       <c r="D23" s="17">
-        <v>150.91745688009632</v>
+        <v>150.92905479310608</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3100,13 +3100,13 @@
         <v>43040</v>
       </c>
       <c r="B24" s="17">
-        <v>151.92604285254853</v>
+        <v>151.92604285254808</v>
       </c>
       <c r="C24" s="17">
-        <v>152.5257498832292</v>
+        <v>152.55051588792227</v>
       </c>
       <c r="D24" s="17">
-        <v>150.82296108907613</v>
+        <v>150.83182630722638</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3114,13 +3114,13 @@
         <v>43070</v>
       </c>
       <c r="B25" s="17">
-        <v>146.78338490746617</v>
+        <v>146.78338490746575</v>
       </c>
       <c r="C25" s="17">
-        <v>152.42694607851507</v>
+        <v>152.48719827636265</v>
       </c>
       <c r="D25" s="17">
-        <v>150.5270449588468</v>
+        <v>150.5331688523361</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3128,13 +3128,13 @@
         <v>43101</v>
       </c>
       <c r="B26" s="17">
-        <v>142.7409126005696</v>
+        <v>142.7409126005692</v>
       </c>
       <c r="C26" s="17">
-        <v>151.82610769740921</v>
+        <v>151.84036377032953</v>
       </c>
       <c r="D26" s="17">
-        <v>150.03756827544137</v>
+        <v>150.04059878510134</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,13 +3142,13 @@
         <v>43132</v>
       </c>
       <c r="B27" s="17">
-        <v>138.81804034929579</v>
+        <v>138.81804034929542</v>
       </c>
       <c r="C27" s="17">
-        <v>151.98396963640329</v>
+        <v>151.92325866345433</v>
       </c>
       <c r="D27" s="17">
-        <v>149.3771569468511</v>
+        <v>149.37605848894052</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3156,13 +3156,13 @@
         <v>43160</v>
       </c>
       <c r="B28" s="17">
-        <v>155.85731954373435</v>
+        <v>155.85731954373392</v>
       </c>
       <c r="C28" s="17">
-        <v>151.24746350618796</v>
+        <v>151.27137411238155</v>
       </c>
       <c r="D28" s="17">
-        <v>148.580423967728</v>
+        <v>148.57415388200747</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3170,13 +3170,13 @@
         <v>43191</v>
       </c>
       <c r="B29" s="17">
-        <v>151.52454400931953</v>
+        <v>151.52454400931902</v>
       </c>
       <c r="C29" s="17">
-        <v>146.82771213268268</v>
+        <v>146.87579763196308</v>
       </c>
       <c r="D29" s="17">
-        <v>147.69287884531127</v>
+        <v>147.68151513282908</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3184,13 +3184,13 @@
         <v>43221</v>
       </c>
       <c r="B30" s="17">
-        <v>159.56669238861366</v>
+        <v>159.56669238861323</v>
       </c>
       <c r="C30" s="17">
-        <v>144.37241328125432</v>
+        <v>144.34823349934697</v>
       </c>
       <c r="D30" s="17">
-        <v>146.76736044494908</v>
+        <v>146.75215694767078</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3198,13 +3198,13 @@
         <v>43252</v>
       </c>
       <c r="B31" s="17">
-        <v>151.12576319738255</v>
+        <v>151.12576319738221</v>
       </c>
       <c r="C31" s="17">
-        <v>143.0976665541726</v>
+        <v>143.10557866363186</v>
       </c>
       <c r="D31" s="17">
-        <v>145.85810740138365</v>
+        <v>145.84010598244873</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,13 +3212,13 @@
         <v>43282</v>
       </c>
       <c r="B32" s="17">
-        <v>145.96352431507171</v>
+        <v>145.96352431507151</v>
       </c>
       <c r="C32" s="17">
-        <v>143.26131070415764</v>
+        <v>143.23184346794673</v>
       </c>
       <c r="D32" s="17">
-        <v>145.01513235593322</v>
+        <v>144.99421232515724</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3226,13 +3226,13 @@
         <v>43313</v>
       </c>
       <c r="B33" s="17">
-        <v>146.7659599856915</v>
+        <v>146.76595998569118</v>
       </c>
       <c r="C33" s="17">
-        <v>146.74026409879454</v>
+        <v>146.65355195921521</v>
       </c>
       <c r="D33" s="17">
-        <v>144.28264787360311</v>
+        <v>144.25758501399085</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3240,13 +3240,13 @@
         <v>43344</v>
       </c>
       <c r="B34" s="17">
-        <v>137.74656988202952</v>
+        <v>137.74656988202872</v>
       </c>
       <c r="C34" s="17">
-        <v>143.29042396351292</v>
+        <v>143.26783703687346</v>
       </c>
       <c r="D34" s="17">
-        <v>143.68971469656995</v>
+        <v>143.65881925415161</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3254,13 +3254,13 @@
         <v>43374</v>
       </c>
       <c r="B35" s="17">
-        <v>142.84327650512373</v>
+        <v>142.84327650512213</v>
       </c>
       <c r="C35" s="17">
-        <v>143.56872690125093</v>
+        <v>143.52476137383422</v>
       </c>
       <c r="D35" s="17">
-        <v>143.24912601430844</v>
+        <v>143.21141367009361</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3268,13 +3268,13 @@
         <v>43405</v>
       </c>
       <c r="B36" s="17">
-        <v>140.59240754476843</v>
+        <v>140.5924075447675</v>
       </c>
       <c r="C36" s="17">
-        <v>141.60204697826842</v>
+        <v>141.62798228025744</v>
       </c>
       <c r="D36" s="17">
-        <v>142.9617651496836</v>
+        <v>142.91665261396898</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3282,13 +3282,13 @@
         <v>43435</v>
       </c>
       <c r="B37" s="17">
-        <v>136.25161522906785</v>
+        <v>136.2516152290691</v>
       </c>
       <c r="C37" s="17">
-        <v>141.97852027627547</v>
+        <v>142.12604325936684</v>
       </c>
       <c r="D37" s="17">
-        <v>142.8151166095854</v>
+        <v>142.76254981779087</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3296,13 +3296,13 @@
         <v>43466</v>
       </c>
       <c r="B38" s="17">
-        <v>134.53623749898799</v>
+        <v>134.53623749899296</v>
       </c>
       <c r="C38" s="17">
-        <v>142.8915726944098</v>
+        <v>142.915814990097</v>
       </c>
       <c r="D38" s="17">
-        <v>142.78417220454361</v>
+        <v>142.72631811243264</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3310,13 +3310,13 @@
         <v>43497</v>
       </c>
       <c r="B39" s="17">
-        <v>132.26788761887991</v>
+        <v>132.26788761888179</v>
       </c>
       <c r="C39" s="17">
-        <v>143.23220057987191</v>
+        <v>143.20019087771206</v>
       </c>
       <c r="D39" s="17">
-        <v>142.83346381420793</v>
+        <v>142.77229080015582</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3324,13 +3324,13 @@
         <v>43525</v>
       </c>
       <c r="B40" s="17">
-        <v>144.96325830731405</v>
+        <v>144.96325830730592</v>
       </c>
       <c r="C40" s="17">
-        <v>141.36107366051658</v>
+        <v>141.40369891096537</v>
       </c>
       <c r="D40" s="17">
-        <v>142.92469947473447</v>
+        <v>142.86133864058453</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3338,13 +3338,13 @@
         <v>43556</v>
       </c>
       <c r="B41" s="17">
-        <v>149.9162320820796</v>
+        <v>149.91623208205462</v>
       </c>
       <c r="C41" s="17">
-        <v>142.62327659011936</v>
+        <v>142.70199676589843</v>
       </c>
       <c r="D41" s="17">
-        <v>143.01881694179355</v>
+        <v>142.95357625404674</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3352,13 +3352,13 @@
         <v>43586</v>
       </c>
       <c r="B42" s="17">
-        <v>164.13570357730771</v>
+        <v>164.13570357729694</v>
       </c>
       <c r="C42" s="17">
-        <v>144.60122888300947</v>
+        <v>144.58149929767112</v>
       </c>
       <c r="D42" s="17">
-        <v>143.0799096105855</v>
+        <v>143.01223617616571</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3366,13 +3366,13 @@
         <v>43617</v>
       </c>
       <c r="B43" s="17">
-        <v>150.85895656118743</v>
+        <v>150.85895656122187</v>
       </c>
       <c r="C43" s="17">
-        <v>143.61047208949321</v>
+        <v>143.61434682079923</v>
       </c>
       <c r="D43" s="17">
-        <v>143.07461921173061</v>
+        <v>143.00403710196426</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3380,13 +3380,13 @@
         <v>43647</v>
       </c>
       <c r="B44" s="17">
-        <v>146.77698127463378</v>
+        <v>146.7769812747444</v>
       </c>
       <c r="C44" s="17">
-        <v>145.39219255892044</v>
+        <v>145.28977300206037</v>
       </c>
       <c r="D44" s="17">
-        <v>142.97483419586715</v>
+        <v>142.9018562689761</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3394,13 +3394,13 @@
         <v>43678</v>
       </c>
       <c r="B45" s="17">
-        <v>141.27691429310812</v>
+        <v>141.2769142931545</v>
       </c>
       <c r="C45" s="17">
-        <v>145.08550199009713</v>
+        <v>144.89910955782955</v>
       </c>
       <c r="D45" s="17">
-        <v>142.75956000725711</v>
+        <v>142.68571854186578</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3408,13 +3408,13 @@
         <v>43709</v>
       </c>
       <c r="B46" s="17">
-        <v>134.87713523310566</v>
+        <v>134.87713523294735</v>
       </c>
       <c r="C46" s="17">
-        <v>141.05966954432927</v>
+        <v>140.99359106200325</v>
       </c>
       <c r="D46" s="17">
-        <v>142.41767359280928</v>
+        <v>142.34531275735853</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,13 +3422,13 @@
         <v>43739</v>
       </c>
       <c r="B47" s="17">
-        <v>141.63955567428133</v>
+        <v>141.63955567377783</v>
       </c>
       <c r="C47" s="17">
-        <v>143.82161022379026</v>
+        <v>143.7371699735244</v>
       </c>
       <c r="D47" s="17">
-        <v>141.94931598206523</v>
+        <v>141.88120481699931</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3436,13 +3436,13 @@
         <v>43770</v>
       </c>
       <c r="B48" s="17">
-        <v>137.77192200967303</v>
+        <v>137.77192200946055</v>
       </c>
       <c r="C48" s="17">
-        <v>140.80166602491136</v>
+        <v>140.81708738145784</v>
       </c>
       <c r="D48" s="17">
-        <v>141.36471046422182</v>
+        <v>141.30362010796878</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3450,13 +3450,13 @@
         <v>43800</v>
       </c>
       <c r="B49" s="17">
-        <v>135.76484313002629</v>
+        <v>135.76484313074099</v>
       </c>
       <c r="C49" s="17">
-        <v>140.30516259723419</v>
+        <v>140.63134878513057</v>
       </c>
       <c r="D49" s="17">
-        <v>140.68979647034365</v>
+        <v>140.63768085501479</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3464,13 +3464,13 @@
         <v>43831</v>
       </c>
       <c r="B50" s="17">
-        <v>132.15799381069021</v>
+        <v>132.15799381296819</v>
       </c>
       <c r="C50" s="17">
-        <v>140.61473242796882</v>
+        <v>140.65729925832272</v>
       </c>
       <c r="D50" s="17">
-        <v>139.96014359248343</v>
+        <v>139.9191333128702</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3478,13 +3478,13 @@
         <v>43862</v>
       </c>
       <c r="B51" s="17">
-        <v>129.68532874095405</v>
+        <v>129.68532874191402</v>
       </c>
       <c r="C51" s="17">
-        <v>140.31908623537217</v>
+        <v>140.32575675023256</v>
       </c>
       <c r="D51" s="17">
-        <v>139.21805108426324</v>
+        <v>139.18900783095796</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3492,13 +3492,13 @@
         <v>43891</v>
       </c>
       <c r="B52" s="17">
-        <v>129.44520369983249</v>
+        <v>129.44520369659313</v>
       </c>
       <c r="C52" s="17">
-        <v>125.86705458418078</v>
+        <v>125.91927216854077</v>
       </c>
       <c r="D52" s="17">
-        <v>138.50641777755985</v>
+        <v>138.4902358628824</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,13 +3506,13 @@
         <v>43922</v>
       </c>
       <c r="B53" s="17">
-        <v>111.93059532201961</v>
+        <v>111.93059531169958</v>
       </c>
       <c r="C53" s="17">
-        <v>105.10984650307633</v>
+        <v>105.19549569078674</v>
       </c>
       <c r="D53" s="17">
-        <v>137.86880740764732</v>
+        <v>137.86402249960867</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3520,13 +3520,13 @@
         <v>43952</v>
       </c>
       <c r="B54" s="17">
-        <v>131.24787223714782</v>
+        <v>131.24787223279728</v>
       </c>
       <c r="C54" s="17">
-        <v>116.63095080481291</v>
+        <v>116.6356757165868</v>
       </c>
       <c r="D54" s="17">
-        <v>137.34095259667907</v>
+        <v>137.34290559876689</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3534,13 +3534,13 @@
         <v>43983</v>
       </c>
       <c r="B55" s="17">
-        <v>133.09348397071517</v>
+        <v>133.09348398538438</v>
       </c>
       <c r="C55" s="17">
-        <v>124.13897696847657</v>
+        <v>124.06219066432595</v>
       </c>
       <c r="D55" s="17">
-        <v>136.94781435747083</v>
+        <v>136.94847100359183</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3548,13 +3548,13 @@
         <v>44013</v>
       </c>
       <c r="B56" s="17">
-        <v>128.24284792670909</v>
+        <v>128.24284797344825</v>
       </c>
       <c r="C56" s="17">
-        <v>126.68722284602633</v>
+        <v>126.48169377401011</v>
       </c>
       <c r="D56" s="17">
-        <v>136.70340799295516</v>
+        <v>136.69398106494586</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3562,13 +3562,13 @@
         <v>44044</v>
       </c>
       <c r="B57" s="17">
-        <v>125.1382025283593</v>
+        <v>125.13820254806124</v>
       </c>
       <c r="C57" s="17">
-        <v>129.28685424969046</v>
+        <v>128.96562651603864</v>
       </c>
       <c r="D57" s="17">
-        <v>136.61299835823039</v>
+        <v>136.58405649488188</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3576,13 +3576,13 @@
         <v>44075</v>
       </c>
       <c r="B58" s="17">
-        <v>126.53017363501691</v>
+        <v>126.53017356857445</v>
       </c>
       <c r="C58" s="17">
-        <v>131.04173680941341</v>
+        <v>130.88590985923526</v>
       </c>
       <c r="D58" s="17">
-        <v>136.66794110594628</v>
+        <v>136.61360440365993</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,13 +3590,13 @@
         <v>44105</v>
       </c>
       <c r="B59" s="17">
-        <v>131.61628895339123</v>
+        <v>131.61628874169719</v>
       </c>
       <c r="C59" s="17">
-        <v>134.07793925226929</v>
+        <v>134.02986284037127</v>
       </c>
       <c r="D59" s="17">
-        <v>136.85124092749905</v>
+        <v>136.77169201880636</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3604,13 +3604,13 @@
         <v>44136</v>
       </c>
       <c r="B60" s="17">
-        <v>132.88316914194343</v>
+        <v>132.88316905270671</v>
       </c>
       <c r="C60" s="17">
-        <v>135.29890080898795</v>
+        <v>135.30660655054666</v>
       </c>
       <c r="D60" s="17">
-        <v>137.14402609014866</v>
+        <v>137.04515097576154</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,13 +3618,13 @@
         <v>44166</v>
       </c>
       <c r="B61" s="17">
-        <v>132.3093003071119</v>
+        <v>132.30930060804135</v>
       </c>
       <c r="C61" s="17">
-        <v>135.20715894224278</v>
+        <v>135.81507063305821</v>
       </c>
       <c r="D61" s="17">
-        <v>137.52588921752243</v>
+        <v>137.41811208742175</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,13 +3632,13 @@
         <v>44197</v>
       </c>
       <c r="B62" s="17">
-        <v>129.610698708972</v>
+        <v>129.61069966777643</v>
       </c>
       <c r="C62" s="17">
-        <v>139.90089424564295</v>
+        <v>140.13191348587628</v>
       </c>
       <c r="D62" s="17">
-        <v>137.97990028266349</v>
+        <v>137.87732105479864</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3646,13 +3646,13 @@
         <v>44228</v>
       </c>
       <c r="B63" s="17">
-        <v>126.88274631552113</v>
+        <v>126.88274671969066</v>
       </c>
       <c r="C63" s="17">
-        <v>138.28647871907674</v>
+        <v>138.4275992873936</v>
       </c>
       <c r="D63" s="17">
-        <v>138.4980601803025</v>
+        <v>138.4141919828086</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3660,13 +3660,13 @@
         <v>44256</v>
       </c>
       <c r="B64" s="17">
-        <v>147.05799544182895</v>
+        <v>147.05799407885365</v>
       </c>
       <c r="C64" s="17">
-        <v>140.36513622652942</v>
+        <v>140.51268092875048</v>
       </c>
       <c r="D64" s="17">
-        <v>139.07615973506969</v>
+        <v>139.02480039186969</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3674,13 +3674,13 @@
         <v>44287</v>
       </c>
       <c r="B65" s="17">
-        <v>144.90969310880172</v>
+        <v>144.9096887661716</v>
       </c>
       <c r="C65" s="17">
-        <v>137.74375392028099</v>
+        <v>137.88513632109948</v>
       </c>
       <c r="D65" s="17">
-        <v>139.71433944499429</v>
+        <v>139.70710396471853</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3688,13 +3688,13 @@
         <v>44317</v>
       </c>
       <c r="B66" s="17">
-        <v>150.49545443180037</v>
+        <v>150.49545260122883</v>
       </c>
       <c r="C66" s="17">
-        <v>137.19119607252691</v>
+        <v>137.22027153098713</v>
       </c>
       <c r="D66" s="17">
-        <v>140.41497042744754</v>
+        <v>140.45967490703219</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3702,13 +3702,13 @@
         <v>44348</v>
       </c>
       <c r="B67" s="17">
-        <v>149.13449789986612</v>
+        <v>149.13450407306641</v>
       </c>
       <c r="C67" s="17">
-        <v>140.32173208689076</v>
+        <v>140.12579309253849</v>
       </c>
       <c r="D67" s="17">
-        <v>141.17764447334883</v>
+        <v>141.27775183804007</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3716,13 +3716,13 @@
         <v>44378</v>
       </c>
       <c r="B68" s="17">
-        <v>142.8064545370143</v>
+        <v>142.80647420569977</v>
       </c>
       <c r="C68" s="17">
-        <v>141.62972725466724</v>
+        <v>141.27264880871439</v>
       </c>
       <c r="D68" s="17">
-        <v>141.99764210728739</v>
+        <v>142.15193061731117</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,13 +3730,13 @@
         <v>44409</v>
       </c>
       <c r="B69" s="17">
-        <v>141.05802513503161</v>
+        <v>141.05803342607391</v>
       </c>
       <c r="C69" s="17">
-        <v>144.30176368327537</v>
+        <v>143.74897698232903</v>
       </c>
       <c r="D69" s="17">
-        <v>142.86665819967635</v>
+        <v>143.06881995107352</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3744,13 +3744,13 @@
         <v>44440</v>
       </c>
       <c r="B70" s="17">
-        <v>140.84598127100656</v>
+        <v>140.84595331127741</v>
       </c>
       <c r="C70" s="17">
-        <v>145.36259236587628</v>
+        <v>145.0604612240455</v>
       </c>
       <c r="D70" s="17">
-        <v>143.77200107855131</v>
+        <v>144.01102590569977</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3758,13 +3758,13 @@
         <v>44470</v>
       </c>
       <c r="B71" s="17">
-        <v>140.56272989215773</v>
+        <v>140.56264080852878</v>
       </c>
       <c r="C71" s="17">
-        <v>144.62888957056836</v>
+        <v>144.55183869603636</v>
       </c>
       <c r="D71" s="17">
-        <v>144.69554632370048</v>
+        <v>144.95649677137283</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,13 +3772,13 @@
         <v>44501</v>
       </c>
       <c r="B72" s="17">
-        <v>145.46358729466505</v>
+        <v>145.4635497427825</v>
       </c>
       <c r="C72" s="17">
-        <v>146.70741979876979</v>
+        <v>146.65903176718891</v>
       </c>
       <c r="D72" s="17">
-        <v>145.61569868523989</v>
+        <v>145.87816087475483</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3786,13 +3786,13 @@
         <v>44531</v>
       </c>
       <c r="B73" s="17">
-        <v>146.0307310573402</v>
+        <v>146.0308576928503</v>
       </c>
       <c r="C73" s="17">
-        <v>148.41900989621203</v>
+        <v>149.26224313263376</v>
       </c>
       <c r="D73" s="17">
-        <v>146.50980831310974</v>
+        <v>146.7531169522745</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3800,13 +3800,13 @@
         <v>44562</v>
       </c>
       <c r="B74" s="17">
-        <v>136.16986307276909</v>
+        <v>136.17026655131809</v>
       </c>
       <c r="C74" s="17">
-        <v>147.21341377443508</v>
+        <v>147.49494935702728</v>
       </c>
       <c r="D74" s="17">
-        <v>147.35486304706717</v>
+        <v>147.55694889224671</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3814,13 +3814,13 @@
         <v>44593</v>
       </c>
       <c r="B75" s="17">
-        <v>137.617239121186</v>
+        <v>137.61740920158263</v>
       </c>
       <c r="C75" s="17">
-        <v>149.00643074227634</v>
+        <v>149.10294568240926</v>
       </c>
       <c r="D75" s="17">
-        <v>148.12818372691501</v>
+        <v>148.2651262486435</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3828,13 +3828,13 @@
         <v>44621</v>
       </c>
       <c r="B76" s="17">
-        <v>153.92877566654988</v>
+        <v>153.92820210760286</v>
       </c>
       <c r="C76" s="17">
-        <v>148.10681675972117</v>
+        <v>148.11457731302491</v>
       </c>
       <c r="D76" s="17">
-        <v>148.81440500007113</v>
+        <v>148.85663132445455</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3842,13 +3842,13 @@
         <v>44652</v>
       </c>
       <c r="B77" s="17">
-        <v>153.7335940552577</v>
+        <v>153.73176661577565</v>
       </c>
       <c r="C77" s="17">
-        <v>148.88416764773058</v>
+        <v>148.79348765392908</v>
       </c>
       <c r="D77" s="17">
-        <v>149.40720186961954</v>
+        <v>149.31387547172068</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3856,13 +3856,13 @@
         <v>44682</v>
       </c>
       <c r="B78" s="17">
-        <v>162.67850048218298</v>
+        <v>162.67773015217838</v>
       </c>
       <c r="C78" s="17">
-        <v>149.03364735393936</v>
+        <v>148.85244899491508</v>
       </c>
       <c r="D78" s="17">
-        <v>149.90512937459496</v>
+        <v>149.6245422284571</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,13 +3870,13 @@
         <v>44713</v>
       </c>
       <c r="B79" s="17">
-        <v>159.89943888973366</v>
+        <v>159.90203665921888</v>
       </c>
       <c r="C79" s="17">
-        <v>150.88039116233975</v>
+        <v>150.35623869760067</v>
       </c>
       <c r="D79" s="17">
-        <v>150.31388490153151</v>
+        <v>149.78570102318994</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3884,13 +3884,13 @@
         <v>44743</v>
       </c>
       <c r="B80" s="17">
-        <v>151.61466889369831</v>
+        <v>151.62523505266708</v>
       </c>
       <c r="C80" s="17">
-        <v>151.57814690308513</v>
+        <v>151.04488741377708</v>
       </c>
       <c r="D80" s="17">
-        <v>150.64656984103775</v>
+        <v>149.80668479922696</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3898,13 +3898,13 @@
         <v>44774</v>
       </c>
       <c r="B81" s="17">
-        <v>150.58993119562615</v>
+        <v>150.5545553591578</v>
       </c>
       <c r="C81" s="17">
-        <v>152.58608104180763</v>
+        <v>151.73337784840572</v>
       </c>
       <c r="D81" s="17">
-        <v>150.91865213081715</v>
+        <v>149.70614942465329</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3912,13 +3912,13 @@
         <v>44805</v>
       </c>
       <c r="B82" s="17">
-        <v>147.74911928720712</v>
+        <v>147.77392896470533</v>
       </c>
       <c r="C82" s="17">
-        <v>152.26382403084355</v>
+        <v>151.54695098021597</v>
       </c>
       <c r="D82" s="17">
-        <v>151.14867612093704</v>
+        <v>149.51476668199351</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3926,27 +3926,41 @@
         <v>44835</v>
       </c>
       <c r="B83" s="17">
-        <v>146.87275857789527</v>
+        <v>146.35148234037158</v>
       </c>
       <c r="C83" s="17">
-        <v>151.45079830459446</v>
+        <v>150.01978092665649</v>
       </c>
       <c r="D83" s="17">
-        <v>151.36018804297072</v>
+        <v>149.27163358050691</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>44866</v>
       </c>
-      <c r="B84" s="42">
-        <v>149.21673266811041</v>
-      </c>
-      <c r="C84" s="42">
-        <v>150.36968857203433</v>
-      </c>
-      <c r="D84" s="42">
-        <v>151.57527643654004</v>
+      <c r="B84" s="17">
+        <v>148.78816323630795</v>
+      </c>
+      <c r="C84" s="17">
+        <v>148.92648035457407</v>
+      </c>
+      <c r="D84" s="17">
+        <v>149.01839605802999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>44896</v>
+      </c>
+      <c r="B85" s="42">
+        <v>144.27192644032635</v>
+      </c>
+      <c r="C85" s="42">
+        <v>147.4034481235731</v>
+      </c>
+      <c r="D85" s="42">
+        <v>148.79477432103994</v>
       </c>
     </row>
   </sheetData>
@@ -4004,7 +4018,7 @@
       <c r="C2" s="23">
         <v>4.7</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="44">
         <v>4.5</v>
       </c>
       <c r="E2" s="27">
@@ -4030,7 +4044,7 @@
       <c r="C3" s="23">
         <v>4</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="44">
         <v>3</v>
       </c>
       <c r="E3" s="27">
@@ -4056,7 +4070,7 @@
       <c r="C4" s="23">
         <v>5</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="44">
         <v>4.7</v>
       </c>
       <c r="E4" s="27">
@@ -4082,7 +4096,7 @@
       <c r="C5" s="23">
         <v>5.9</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <v>4.2</v>
       </c>
       <c r="E5" s="27">
@@ -4108,7 +4122,7 @@
       <c r="C6" s="23">
         <v>11</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <v>11.1</v>
       </c>
       <c r="E6" s="27">
@@ -4134,7 +4148,7 @@
       <c r="C7" s="23">
         <v>21.4</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
         <v>22.3</v>
       </c>
       <c r="E7" s="27">
@@ -4160,7 +4174,7 @@
       <c r="C8" s="23">
         <v>5.9</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="44">
         <v>7.6</v>
       </c>
       <c r="E8" s="27">
@@ -4186,7 +4200,7 @@
       <c r="C9" s="23">
         <v>3.5</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="44">
         <v>3.9</v>
       </c>
       <c r="E9" s="27">
@@ -4212,7 +4226,7 @@
       <c r="C10" s="23">
         <v>5.2</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <v>7.8</v>
       </c>
       <c r="E10" s="27">
@@ -4618,7 +4632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6120,14 +6134,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6731,14 +6745,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6887,9 +6901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6915,14 +6927,14 @@
         <v>79</v>
       </c>
       <c r="B2" s="29">
-        <v>15793</v>
+        <v>924</v>
       </c>
       <c r="C2" s="29">
-        <v>19264</v>
+        <v>1305</v>
       </c>
       <c r="D2" s="43">
         <f>B2-C2</f>
-        <v>-3471</v>
+        <v>-381</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6930,14 +6942,14 @@
         <v>80</v>
       </c>
       <c r="B3" s="29">
-        <v>4938</v>
+        <v>251</v>
       </c>
       <c r="C3" s="29">
-        <v>778</v>
+        <v>56</v>
       </c>
       <c r="D3" s="43">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
-        <v>4160</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6945,14 +6957,14 @@
         <v>81</v>
       </c>
       <c r="B4" s="29">
-        <v>5313</v>
+        <v>463</v>
       </c>
       <c r="C4" s="29">
-        <v>3377</v>
+        <v>162</v>
       </c>
       <c r="D4" s="43">
         <f t="shared" si="0"/>
-        <v>1936</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6960,14 +6972,14 @@
         <v>82</v>
       </c>
       <c r="B5" s="29">
-        <v>1480</v>
+        <v>92</v>
       </c>
       <c r="C5" s="29">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D5" s="43">
         <f t="shared" si="0"/>
-        <v>1445</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -6975,14 +6987,14 @@
         <v>83</v>
       </c>
       <c r="B6" s="29">
-        <v>8653</v>
+        <v>613</v>
       </c>
       <c r="C6" s="29">
-        <v>12557</v>
+        <v>784</v>
       </c>
       <c r="D6" s="43">
         <f t="shared" si="0"/>
-        <v>-3904</v>
+        <v>-171</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6990,14 +7002,14 @@
         <v>84</v>
       </c>
       <c r="B7" s="29">
-        <v>10846</v>
+        <v>609</v>
       </c>
       <c r="C7" s="29">
-        <v>11118</v>
+        <v>858</v>
       </c>
       <c r="D7" s="43">
         <f t="shared" si="0"/>
-        <v>-272</v>
+        <v>-249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7005,14 +7017,14 @@
         <v>85</v>
       </c>
       <c r="B8" s="29">
-        <v>685</v>
+        <v>38</v>
       </c>
       <c r="C8" s="29">
-        <v>652</v>
+        <v>40</v>
       </c>
       <c r="D8" s="43">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7020,14 +7032,14 @@
         <v>86</v>
       </c>
       <c r="B9" s="29">
-        <v>1092</v>
+        <v>157</v>
       </c>
       <c r="C9" s="29">
-        <v>586</v>
+        <v>49</v>
       </c>
       <c r="D9" s="43">
         <f t="shared" si="0"/>
-        <v>506</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7035,14 +7047,14 @@
         <v>87</v>
       </c>
       <c r="B10" s="29">
-        <v>581</v>
+        <v>27</v>
       </c>
       <c r="C10" s="29">
-        <v>432</v>
+        <v>2</v>
       </c>
       <c r="D10" s="43">
         <f t="shared" si="0"/>
-        <v>149</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7050,14 +7062,14 @@
         <v>88</v>
       </c>
       <c r="B11" s="29">
-        <v>7894</v>
+        <v>364</v>
       </c>
       <c r="C11" s="29">
-        <v>4225</v>
+        <v>382</v>
       </c>
       <c r="D11" s="43">
         <f t="shared" si="0"/>
-        <v>3669</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7065,14 +7077,14 @@
         <v>89</v>
       </c>
       <c r="B12" s="29">
-        <v>8022</v>
+        <v>422</v>
       </c>
       <c r="C12" s="29">
-        <v>17516</v>
+        <v>1145</v>
       </c>
       <c r="D12" s="43">
         <f t="shared" si="0"/>
-        <v>-9494</v>
+        <v>-723</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7080,14 +7092,14 @@
         <v>90</v>
       </c>
       <c r="B13" s="29">
-        <v>2020</v>
+        <v>76</v>
       </c>
       <c r="C13" s="29">
-        <v>729</v>
+        <v>40</v>
       </c>
       <c r="D13" s="43">
         <f t="shared" si="0"/>
-        <v>1291</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7095,14 +7107,14 @@
         <v>91</v>
       </c>
       <c r="B14" s="29">
-        <v>795</v>
+        <v>48</v>
       </c>
       <c r="C14" s="29">
-        <v>1201</v>
+        <v>101</v>
       </c>
       <c r="D14" s="43">
         <f t="shared" si="0"/>
-        <v>-406</v>
+        <v>-53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7110,14 +7122,14 @@
         <v>92</v>
       </c>
       <c r="B15" s="29">
-        <v>4555</v>
+        <v>188</v>
       </c>
       <c r="C15" s="29">
-        <v>1849</v>
+        <v>108</v>
       </c>
       <c r="D15" s="43">
         <f t="shared" si="0"/>
-        <v>2706</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7125,14 +7137,14 @@
         <v>93</v>
       </c>
       <c r="B16" s="29">
-        <v>4655</v>
+        <v>132</v>
       </c>
       <c r="C16" s="29">
-        <v>2534</v>
+        <v>112</v>
       </c>
       <c r="D16" s="43">
         <f t="shared" si="0"/>
-        <v>2121</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7140,14 +7152,14 @@
         <v>94</v>
       </c>
       <c r="B17" s="29">
-        <v>3964</v>
+        <v>154</v>
       </c>
       <c r="C17" s="29">
-        <v>1179</v>
+        <v>12</v>
       </c>
       <c r="D17" s="43">
         <f t="shared" si="0"/>
-        <v>2785</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7155,14 +7167,14 @@
         <v>95</v>
       </c>
       <c r="B18" s="29">
-        <v>463</v>
+        <v>17</v>
       </c>
       <c r="C18" s="29">
-        <v>195</v>
+        <v>22</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" si="0"/>
-        <v>268</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7170,14 +7182,14 @@
         <v>96</v>
       </c>
       <c r="B19" s="29">
-        <v>864</v>
+        <v>37</v>
       </c>
       <c r="C19" s="29">
-        <v>515</v>
+        <v>23</v>
       </c>
       <c r="D19" s="43">
         <f t="shared" si="0"/>
-        <v>349</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7185,14 +7197,14 @@
         <v>97</v>
       </c>
       <c r="B20" s="29">
-        <v>5832</v>
+        <v>288</v>
       </c>
       <c r="C20" s="29">
-        <v>2779</v>
+        <v>177</v>
       </c>
       <c r="D20" s="43">
         <f t="shared" si="0"/>
-        <v>3053</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -7225,7 +7237,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="34">
-        <v>88446</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7233,7 +7245,7 @@
         <v>185</v>
       </c>
       <c r="B3" s="34">
-        <v>23868</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7241,7 +7253,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="29">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7249,7 +7261,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="29">
-        <v>1539</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7257,7 +7269,7 @@
         <v>140</v>
       </c>
       <c r="B6" s="29">
-        <v>248</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7265,7 +7277,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="29">
-        <v>635</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7273,7 +7285,7 @@
         <v>142</v>
       </c>
       <c r="B8" s="29">
-        <v>525</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7281,7 +7293,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="29">
-        <v>15575</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7289,7 +7301,7 @@
         <v>144</v>
       </c>
       <c r="B10" s="29">
-        <v>4347</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7297,7 +7309,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="29">
-        <v>317</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7305,7 +7317,7 @@
         <v>146</v>
       </c>
       <c r="B12" s="29">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7313,7 +7325,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="29">
-        <v>177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7321,7 +7333,7 @@
         <v>148</v>
       </c>
       <c r="B14" s="29">
-        <v>300</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7329,7 +7341,7 @@
         <v>149</v>
       </c>
       <c r="B15" s="29">
-        <v>148</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7337,7 +7349,7 @@
         <v>186</v>
       </c>
       <c r="B16" s="34">
-        <v>33119</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7345,7 +7357,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="29">
-        <v>4158</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7353,7 +7365,7 @@
         <v>151</v>
       </c>
       <c r="B18" s="29">
-        <v>265</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7361,7 +7373,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="29">
-        <v>1422</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7369,7 +7381,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="29">
-        <v>58</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7377,7 +7389,7 @@
         <v>154</v>
       </c>
       <c r="B21" s="29">
-        <v>122</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7385,7 +7397,7 @@
         <v>155</v>
       </c>
       <c r="B22" s="29">
-        <v>177</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7393,7 +7405,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="29">
-        <v>1020</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7401,7 +7413,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="29">
-        <v>9170</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7409,7 +7421,7 @@
         <v>158</v>
       </c>
       <c r="B25" s="29">
-        <v>297</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7417,7 +7429,7 @@
         <v>159</v>
       </c>
       <c r="B26" s="29">
-        <v>814</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7425,7 +7437,7 @@
         <v>160</v>
       </c>
       <c r="B27" s="29">
-        <v>948</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7433,7 +7445,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="29">
-        <v>13249</v>
+        <v>664</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7441,7 +7453,7 @@
         <v>162</v>
       </c>
       <c r="B29" s="29">
-        <v>319</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7449,7 +7461,7 @@
         <v>163</v>
       </c>
       <c r="B30" s="29">
-        <v>463</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7457,7 +7469,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="29">
-        <v>127</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7465,7 +7477,7 @@
         <v>165</v>
       </c>
       <c r="B32" s="29">
-        <v>510</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7473,7 +7485,7 @@
         <v>187</v>
       </c>
       <c r="B33" s="34">
-        <v>23061</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7481,7 +7493,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="29">
-        <v>6119</v>
+        <v>311</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7489,7 +7501,7 @@
         <v>167</v>
       </c>
       <c r="B35" s="29">
-        <v>1083</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7497,7 +7509,7 @@
         <v>168</v>
       </c>
       <c r="B36" s="29">
-        <v>225</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7505,7 +7517,7 @@
         <v>169</v>
       </c>
       <c r="B37" s="29">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7513,7 +7525,7 @@
         <v>170</v>
       </c>
       <c r="B38" s="29">
-        <v>464</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7521,7 +7533,7 @@
         <v>171</v>
       </c>
       <c r="B39" s="29">
-        <v>143</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7529,7 +7541,7 @@
         <v>172</v>
       </c>
       <c r="B40" s="29">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -7537,7 +7549,7 @@
         <v>173</v>
       </c>
       <c r="B41" s="29">
-        <v>177</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -7545,7 +7557,7 @@
         <v>174</v>
       </c>
       <c r="B42" s="29">
-        <v>2680</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -7553,7 +7565,7 @@
         <v>175</v>
       </c>
       <c r="B43" s="29">
-        <v>2043</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -7561,7 +7573,7 @@
         <v>176</v>
       </c>
       <c r="B44" s="29">
-        <v>1594</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -7569,7 +7581,7 @@
         <v>177</v>
       </c>
       <c r="B45" s="29">
-        <v>7950</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -7577,7 +7589,7 @@
         <v>178</v>
       </c>
       <c r="B46" s="29">
-        <v>247</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7585,7 +7597,7 @@
         <v>179</v>
       </c>
       <c r="B47" s="29">
-        <v>296</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -7593,7 +7605,7 @@
         <v>188</v>
       </c>
       <c r="B48" s="34">
-        <v>8398</v>
+        <v>507</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7601,7 +7613,7 @@
         <v>180</v>
       </c>
       <c r="B49" s="29">
-        <v>3867</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7609,7 +7621,7 @@
         <v>181</v>
       </c>
       <c r="B50" s="29">
-        <v>2573</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7617,7 +7629,7 @@
         <v>182</v>
       </c>
       <c r="B51" s="29">
-        <v>90</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7625,7 +7637,7 @@
         <v>183</v>
       </c>
       <c r="B52" s="40">
-        <v>1369</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -7633,7 +7645,7 @@
         <v>184</v>
       </c>
       <c r="B53" s="41">
-        <v>498</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -7646,8 +7658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7668,7 +7680,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="34">
-        <v>81523</v>
+        <v>5384</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7676,7 +7688,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="34">
-        <v>12454</v>
+        <v>875</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -7684,7 +7696,7 @@
         <v>190</v>
       </c>
       <c r="B4" s="29">
-        <v>9352</v>
+        <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7692,7 +7704,7 @@
         <v>191</v>
       </c>
       <c r="B5" s="29">
-        <v>1340</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7700,7 +7712,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="29">
-        <v>1318</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7708,7 +7720,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="29">
-        <v>444</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -7716,7 +7728,7 @@
         <v>211</v>
       </c>
       <c r="B8" s="34">
-        <v>30009</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -7724,7 +7736,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="29">
-        <v>2533</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7732,7 +7744,7 @@
         <v>195</v>
       </c>
       <c r="B10" s="29">
-        <v>1461</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7740,7 +7752,7 @@
         <v>196</v>
       </c>
       <c r="B11" s="29">
-        <v>12381</v>
+        <v>701</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7748,7 +7760,7 @@
         <v>197</v>
       </c>
       <c r="B12" s="29">
-        <v>3842</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -7756,7 +7768,7 @@
         <v>198</v>
       </c>
       <c r="B13" s="29">
-        <v>1199</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -7764,7 +7776,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="29">
-        <v>1388</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7772,7 +7784,7 @@
         <v>200</v>
       </c>
       <c r="B15" s="29">
-        <v>671</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7780,7 +7792,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="29">
-        <v>4329</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7788,7 +7800,7 @@
         <v>202</v>
       </c>
       <c r="B17" s="29">
-        <v>2204</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7796,7 +7808,7 @@
         <v>212</v>
       </c>
       <c r="B18" s="34">
-        <v>12868</v>
+        <v>712</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7804,7 +7816,7 @@
         <v>195</v>
       </c>
       <c r="B19" s="29">
-        <v>12500</v>
+        <v>677</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7812,7 +7824,7 @@
         <v>203</v>
       </c>
       <c r="B20" s="29">
-        <v>368</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7820,7 +7832,7 @@
         <v>213</v>
       </c>
       <c r="B21" s="34">
-        <v>15037</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7828,7 +7840,7 @@
         <v>190</v>
       </c>
       <c r="B22" s="29">
-        <v>9705</v>
+        <v>776</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7836,7 +7848,7 @@
         <v>191</v>
       </c>
       <c r="B23" s="29">
-        <v>4231</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7844,7 +7856,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="29">
-        <v>1100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7852,7 +7864,7 @@
         <v>214</v>
       </c>
       <c r="B25" s="34">
-        <v>8567</v>
+        <v>627</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7860,7 +7872,7 @@
         <v>205</v>
       </c>
       <c r="B26" s="29">
-        <v>280</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7868,7 +7880,7 @@
         <v>194</v>
       </c>
       <c r="B27" s="29">
-        <v>629</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7876,7 +7888,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="29">
-        <v>790</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7884,7 +7896,7 @@
         <v>196</v>
       </c>
       <c r="B29" s="29">
-        <v>2538</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7892,7 +7904,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="29">
-        <v>512</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7900,7 +7912,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="29">
-        <v>423</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7908,7 +7920,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="29">
-        <v>697</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7916,7 +7928,7 @@
         <v>190</v>
       </c>
       <c r="B33" s="29">
-        <v>628</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7924,7 +7936,7 @@
         <v>191</v>
       </c>
       <c r="B34" s="29">
-        <v>578</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7932,7 +7944,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="29">
-        <v>316</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7940,7 +7952,7 @@
         <v>208</v>
       </c>
       <c r="B36" s="29">
-        <v>569</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7948,7 +7960,7 @@
         <v>209</v>
       </c>
       <c r="B37" s="29">
-        <v>605</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7956,7 +7968,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="34">
-        <v>1996</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7964,7 +7976,7 @@
         <v>191</v>
       </c>
       <c r="B39" s="38">
-        <v>1996</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7972,7 +7984,7 @@
         <v>216</v>
       </c>
       <c r="B40" s="39">
-        <v>592</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Actualizo dato var ipc feb 23"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEEEC0E-5568-40F4-BC1B-6BD07E43BF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A922E24-A1ED-46C4-A2AE-0272ECF745CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -898,9 +898,6 @@
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -908,9 +905,6 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -939,7 +933,6 @@
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1266,11 +1259,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74:E74"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2267,7 +2258,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="22">
+      <c r="A59" s="19">
         <v>44470</v>
       </c>
       <c r="B59" s="1">
@@ -2301,7 +2292,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="22">
+      <c r="A61" s="19">
         <v>44531</v>
       </c>
       <c r="B61" s="1">
@@ -2335,7 +2326,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="22">
+      <c r="A63" s="19">
         <v>44593</v>
       </c>
       <c r="B63" s="1">
@@ -2369,7 +2360,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="22">
+      <c r="A65" s="19">
         <v>44652</v>
       </c>
       <c r="B65" s="1">
@@ -2386,7 +2377,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="22">
+      <c r="A66" s="19">
         <v>44682</v>
       </c>
       <c r="B66" s="1">
@@ -2403,7 +2394,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="22">
+      <c r="A67" s="19">
         <v>44713</v>
       </c>
       <c r="B67" s="1">
@@ -2420,7 +2411,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="22">
+      <c r="A68" s="19">
         <v>44743</v>
       </c>
       <c r="B68" s="1">
@@ -2437,7 +2428,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="22">
+      <c r="A69" s="19">
         <v>44774</v>
       </c>
       <c r="B69" s="1">
@@ -2454,7 +2445,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="22">
+      <c r="A70" s="19">
         <v>44805</v>
       </c>
       <c r="B70" s="1">
@@ -2471,7 +2462,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="22">
+      <c r="A71" s="19">
         <v>44835</v>
       </c>
       <c r="B71" s="1">
@@ -2488,7 +2479,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="22">
+      <c r="A72" s="19">
         <v>44866</v>
       </c>
       <c r="B72" s="1">
@@ -2505,7 +2496,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="22">
+      <c r="A73" s="19">
         <v>44896</v>
       </c>
       <c r="B73" s="1">
@@ -2522,7 +2513,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="22">
+      <c r="A74" s="19">
         <v>44927</v>
       </c>
       <c r="B74" s="1">
@@ -2536,6 +2527,23 @@
       </c>
       <c r="E74">
         <v>7.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="19">
+        <v>44958</v>
+      </c>
+      <c r="B75" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="C75">
+        <v>3.3</v>
+      </c>
+      <c r="D75">
+        <v>7.7</v>
+      </c>
+      <c r="E75">
+        <v>5.0999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -3953,13 +3961,13 @@
       <c r="A85" s="4">
         <v>44896</v>
       </c>
-      <c r="B85" s="42">
+      <c r="B85" s="38">
         <v>144.27192644032635</v>
       </c>
-      <c r="C85" s="42">
+      <c r="C85" s="38">
         <v>147.4034481235731</v>
       </c>
-      <c r="D85" s="42">
+      <c r="D85" s="38">
         <v>148.79477432103994</v>
       </c>
     </row>
@@ -3973,8 +3981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,234 +4020,234 @@
       <c r="A2" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="23">
-        <v>3.9</v>
-      </c>
-      <c r="C2" s="23">
-        <v>4.7</v>
-      </c>
-      <c r="D2" s="44">
-        <v>4.5</v>
-      </c>
-      <c r="E2" s="27">
-        <v>5</v>
-      </c>
-      <c r="F2" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="G2" s="23">
-        <v>4.8</v>
+      <c r="B2" s="20">
+        <v>6.1</v>
+      </c>
+      <c r="C2" s="20">
+        <v>5.5</v>
+      </c>
+      <c r="D2" s="20">
+        <v>6</v>
+      </c>
+      <c r="E2" s="20">
+        <v>7.9</v>
+      </c>
+      <c r="F2" s="20">
+        <v>5.5</v>
+      </c>
+      <c r="G2" s="20">
+        <v>5.8</v>
       </c>
       <c r="H2" s="16">
-        <v>4.3505747899345248</v>
+        <v>5.9607099111174788</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="23">
-        <v>3.9</v>
-      </c>
-      <c r="C3" s="23">
-        <v>4</v>
-      </c>
-      <c r="D3" s="44">
-        <v>3</v>
-      </c>
-      <c r="E3" s="27">
-        <v>3.7</v>
-      </c>
-      <c r="F3" s="23">
-        <v>4.2</v>
-      </c>
-      <c r="G3" s="23">
-        <v>4.7</v>
+      <c r="B3" s="20">
+        <v>21.1</v>
+      </c>
+      <c r="C3" s="20">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D3" s="20">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E3" s="20">
+        <v>20</v>
+      </c>
+      <c r="F3" s="20">
+        <v>22.8</v>
+      </c>
+      <c r="G3" s="20">
+        <v>13.8</v>
       </c>
       <c r="H3" s="16">
-        <v>3.9729491721527843</v>
+        <v>19.09464634090352</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="23">
-        <v>4.7</v>
-      </c>
-      <c r="C4" s="23">
-        <v>5</v>
-      </c>
-      <c r="D4" s="44">
-        <v>4.7</v>
-      </c>
-      <c r="E4" s="27">
-        <v>4.3</v>
-      </c>
-      <c r="F4" s="23">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="G4" s="23">
-        <v>4.9000000000000004</v>
+      <c r="B4" s="20">
+        <v>8</v>
+      </c>
+      <c r="C4" s="20">
+        <v>6.9</v>
+      </c>
+      <c r="D4" s="20">
+        <v>9.5</v>
+      </c>
+      <c r="E4" s="20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F4" s="20">
+        <v>7.8</v>
+      </c>
+      <c r="G4" s="20">
+        <v>6.1</v>
       </c>
       <c r="H4" s="16">
-        <v>4.7980030262997131</v>
+        <v>7.5055318101936441</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="23">
-        <v>3.4</v>
-      </c>
-      <c r="C5" s="23">
-        <v>5.9</v>
-      </c>
-      <c r="D5" s="44">
-        <v>4.2</v>
-      </c>
-      <c r="E5" s="27">
-        <v>4.5</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="B5" s="20">
         <v>5</v>
       </c>
-      <c r="G5" s="23">
-        <v>4.9000000000000004</v>
+      <c r="C5" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D5" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E5" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F5" s="20">
+        <v>5.4</v>
+      </c>
+      <c r="G5" s="20">
+        <v>5.7</v>
       </c>
       <c r="H5" s="16">
-        <v>4.5381878659563668</v>
+        <v>5.0485065098853088</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="23">
-        <v>11.6</v>
-      </c>
-      <c r="C6" s="23">
-        <v>11</v>
-      </c>
-      <c r="D6" s="44">
-        <v>11.1</v>
-      </c>
-      <c r="E6" s="27">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="F6" s="23">
-        <v>13</v>
-      </c>
-      <c r="G6" s="23">
-        <v>6.6</v>
+      <c r="B6" s="20">
+        <v>17.5</v>
+      </c>
+      <c r="C6" s="20">
+        <v>11.3</v>
+      </c>
+      <c r="D6" s="20">
+        <v>14.1</v>
+      </c>
+      <c r="E6" s="20">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F6" s="20">
+        <v>9.9</v>
+      </c>
+      <c r="G6" s="20">
+        <v>8.3000000000000007</v>
       </c>
       <c r="H6" s="16">
-        <v>11.328161553523852</v>
+        <v>13.780525715182135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="23">
-        <v>16.7</v>
-      </c>
-      <c r="C7" s="23">
-        <v>21.4</v>
-      </c>
-      <c r="D7" s="44">
-        <v>22.3</v>
-      </c>
-      <c r="E7" s="27">
-        <v>27.5</v>
-      </c>
-      <c r="F7" s="23">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="G7" s="23">
-        <v>11</v>
+      <c r="B7" s="20">
+        <v>-1.7</v>
+      </c>
+      <c r="C7" s="20">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="D7" s="20">
+        <v>-1.3</v>
+      </c>
+      <c r="E7" s="20">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="F7" s="20">
+        <v>-0.9</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1.5</v>
       </c>
       <c r="H7" s="16">
-        <v>18.783144086032433</v>
+        <v>-1.6671651067101112</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="23">
-        <v>4.8</v>
-      </c>
-      <c r="C8" s="23">
-        <v>5.9</v>
-      </c>
-      <c r="D8" s="44">
-        <v>7.6</v>
-      </c>
-      <c r="E8" s="27">
-        <v>5.9</v>
-      </c>
-      <c r="F8" s="23">
-        <v>5</v>
-      </c>
-      <c r="G8" s="23">
-        <v>4.4000000000000004</v>
+      <c r="B8" s="20">
+        <v>7.1</v>
+      </c>
+      <c r="C8" s="20">
+        <v>6</v>
+      </c>
+      <c r="D8" s="20">
+        <v>7.5</v>
+      </c>
+      <c r="E8" s="20">
+        <v>8.9</v>
+      </c>
+      <c r="F8" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G8" s="20">
+        <v>5.7</v>
       </c>
       <c r="H8" s="16">
-        <v>5.3605104694679939</v>
+        <v>6.7276290174242748</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="23">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C9" s="23">
-        <v>3.5</v>
-      </c>
-      <c r="D9" s="44">
-        <v>3.9</v>
-      </c>
-      <c r="E9" s="27">
-        <v>5.7</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="B9" s="20">
+        <v>5.4</v>
+      </c>
+      <c r="C9" s="20">
+        <v>5.2</v>
+      </c>
+      <c r="D9" s="20">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G9" s="23">
-        <v>2.5</v>
+      <c r="E9" s="20">
+        <v>5</v>
+      </c>
+      <c r="F9" s="20">
+        <v>6.6</v>
+      </c>
+      <c r="G9" s="20">
+        <v>5.0999999999999996</v>
       </c>
       <c r="H9" s="16">
-        <v>3.8502752079279334</v>
+        <v>5.2223310525710387</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="23">
-        <v>10</v>
-      </c>
-      <c r="C10" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="D10" s="44">
-        <v>7.8</v>
-      </c>
-      <c r="E10" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="F10" s="23">
-        <v>6.1</v>
-      </c>
-      <c r="G10" s="23">
-        <v>5.8</v>
+      <c r="B10" s="20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C10" s="20">
+        <v>6</v>
+      </c>
+      <c r="D10" s="20">
+        <v>8.9</v>
+      </c>
+      <c r="E10" s="20">
+        <v>9.1</v>
+      </c>
+      <c r="F10" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="G10" s="20">
+        <v>5.7</v>
       </c>
       <c r="H10" s="16">
-        <v>7.3876880211027673</v>
+        <v>5.9278894843187935</v>
       </c>
     </row>
   </sheetData>
@@ -4252,9 +4260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4288,338 +4294,338 @@
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="19">
-        <v>6</v>
-      </c>
-      <c r="C2" s="25">
-        <v>6</v>
-      </c>
-      <c r="D2" s="25">
-        <v>6.1</v>
-      </c>
-      <c r="E2" s="25">
-        <v>5.6</v>
-      </c>
-      <c r="F2" s="25">
-        <v>6.3</v>
-      </c>
-      <c r="G2" s="25">
+      <c r="B2" s="22">
+        <v>6.6</v>
+      </c>
+      <c r="C2" s="22">
+        <v>6.7</v>
+      </c>
+      <c r="D2" s="22">
         <v>6.4</v>
       </c>
-      <c r="H2" s="19">
-        <v>5.9</v>
+      <c r="E2" s="22">
+        <v>7.8</v>
+      </c>
+      <c r="F2" s="22">
+        <v>7.3</v>
+      </c>
+      <c r="G2" s="22">
+        <v>6.7</v>
+      </c>
+      <c r="H2" s="22">
+        <v>5.8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="18">
-        <v>6.8</v>
-      </c>
-      <c r="C3" s="24">
-        <v>6.6</v>
-      </c>
-      <c r="D3" s="24">
-        <v>6.9</v>
-      </c>
-      <c r="E3" s="24">
-        <v>6.6</v>
-      </c>
-      <c r="F3" s="24">
-        <v>7.9</v>
-      </c>
-      <c r="G3" s="24">
-        <v>7</v>
-      </c>
-      <c r="H3" s="18">
-        <v>5.5</v>
+      <c r="B3" s="21">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C3" s="21">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D3" s="21">
+        <v>9.1</v>
+      </c>
+      <c r="E3" s="21">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F3" s="21">
+        <v>10.6</v>
+      </c>
+      <c r="G3" s="21">
+        <v>10.6</v>
+      </c>
+      <c r="H3" s="21">
+        <v>8.1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="18">
-        <v>7.3</v>
-      </c>
-      <c r="C4" s="24">
-        <v>7.6</v>
-      </c>
-      <c r="D4" s="24">
-        <v>7</v>
-      </c>
-      <c r="E4" s="24">
-        <v>7</v>
-      </c>
-      <c r="F4" s="24">
-        <v>7.3</v>
-      </c>
-      <c r="G4" s="24">
-        <v>6.6</v>
-      </c>
-      <c r="H4" s="18">
-        <v>7.9</v>
+      <c r="B4" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="C4" s="21">
+        <v>5.3</v>
+      </c>
+      <c r="D4" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E4" s="21">
+        <v>6.4</v>
+      </c>
+      <c r="F4" s="21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="H4" s="21">
+        <v>4.7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="18">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C5" s="24">
-        <v>1.4</v>
-      </c>
-      <c r="D5" s="24">
+      <c r="B5" s="21">
+        <v>3.9</v>
+      </c>
+      <c r="C5" s="21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D5" s="21">
         <v>3</v>
       </c>
-      <c r="E5" s="24">
-        <v>3.4</v>
-      </c>
-      <c r="F5" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="G5" s="24">
-        <v>2.9</v>
-      </c>
-      <c r="H5" s="18">
-        <v>3.9</v>
+      <c r="E5" s="21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F5" s="21">
+        <v>3.6</v>
+      </c>
+      <c r="G5" s="21">
+        <v>2.7</v>
+      </c>
+      <c r="H5" s="21">
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="18">
-        <v>8</v>
-      </c>
-      <c r="C6" s="24">
-        <v>7.8</v>
-      </c>
-      <c r="D6" s="24">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="E6" s="24">
-        <v>3.2</v>
-      </c>
-      <c r="F6" s="24">
-        <v>7.3</v>
-      </c>
-      <c r="G6" s="24">
-        <v>11.7</v>
-      </c>
-      <c r="H6" s="18">
-        <v>8.1</v>
+      <c r="B6" s="21">
+        <v>4.8</v>
+      </c>
+      <c r="C6" s="21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D6" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="E6" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F6" s="21">
+        <v>2.9</v>
+      </c>
+      <c r="G6" s="21">
+        <v>4.7</v>
+      </c>
+      <c r="H6" s="21">
+        <v>3.8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C7" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D7" s="21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E7" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="F7" s="21">
         <v>5.4</v>
       </c>
-      <c r="C7" s="24">
+      <c r="G7" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="H7" s="21">
         <v>5</v>
-      </c>
-      <c r="D7" s="24">
-        <v>5.6</v>
-      </c>
-      <c r="E7" s="24">
-        <v>6.5</v>
-      </c>
-      <c r="F7" s="24">
-        <v>5.7</v>
-      </c>
-      <c r="G7" s="24">
-        <v>5.9</v>
-      </c>
-      <c r="H7" s="18">
-        <v>6.2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="18">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C8" s="24">
-        <v>5.5</v>
-      </c>
-      <c r="D8" s="24">
+      <c r="B8" s="21">
+        <v>5.3</v>
+      </c>
+      <c r="C8" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="D8" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="E8" s="21">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E8" s="24">
-        <v>4.2</v>
-      </c>
-      <c r="F8" s="24">
-        <v>4.3</v>
-      </c>
-      <c r="G8" s="24">
-        <v>4</v>
-      </c>
-      <c r="H8" s="18">
-        <v>4.5</v>
+      <c r="F8" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G8" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="H8" s="21">
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="18">
-        <v>5.9</v>
-      </c>
-      <c r="C9" s="24">
-        <v>6.3</v>
-      </c>
-      <c r="D9" s="24">
-        <v>5.9</v>
-      </c>
-      <c r="E9" s="24">
-        <v>5.3</v>
-      </c>
-      <c r="F9" s="24">
+      <c r="B9" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G9" s="24">
-        <v>5.8</v>
-      </c>
-      <c r="H9" s="18">
-        <v>5.8</v>
+      <c r="C9" s="21">
+        <v>4.5</v>
+      </c>
+      <c r="D9" s="21">
+        <v>4.8</v>
+      </c>
+      <c r="E9" s="21">
+        <v>7.1</v>
+      </c>
+      <c r="F9" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="G9" s="21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H9" s="21">
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="18">
-        <v>8</v>
-      </c>
-      <c r="C10" s="24">
-        <v>8.1</v>
-      </c>
-      <c r="D10" s="24">
-        <v>7.4</v>
-      </c>
-      <c r="E10" s="24">
-        <v>7</v>
-      </c>
-      <c r="F10" s="24">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="G10" s="24">
-        <v>8</v>
-      </c>
-      <c r="H10" s="18">
-        <v>9.3000000000000007</v>
+      <c r="B10" s="21">
+        <v>7.8</v>
+      </c>
+      <c r="C10" s="21">
+        <v>7.8</v>
+      </c>
+      <c r="D10" s="21">
+        <v>9</v>
+      </c>
+      <c r="E10" s="21">
+        <v>9</v>
+      </c>
+      <c r="F10" s="21">
+        <v>6.2</v>
+      </c>
+      <c r="G10" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="H10" s="21">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="18">
-        <v>9</v>
-      </c>
-      <c r="C11" s="24">
-        <v>10.5</v>
-      </c>
-      <c r="D11" s="24">
-        <v>7.9</v>
-      </c>
-      <c r="E11" s="24">
-        <v>7.6</v>
-      </c>
-      <c r="F11" s="24">
-        <v>7.3</v>
-      </c>
-      <c r="G11" s="24">
-        <v>7.8</v>
-      </c>
-      <c r="H11" s="18">
-        <v>7.1</v>
+      <c r="B11" s="21">
+        <v>6.1</v>
+      </c>
+      <c r="C11" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="D11" s="21">
+        <v>6.3</v>
+      </c>
+      <c r="E11" s="21">
+        <v>7.2</v>
+      </c>
+      <c r="F11" s="21">
+        <v>10.9</v>
+      </c>
+      <c r="G11" s="21">
+        <v>5.3</v>
+      </c>
+      <c r="H11" s="21">
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C12" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="D12" s="24">
-        <v>2</v>
-      </c>
-      <c r="E12" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="F12" s="24">
-        <v>0</v>
-      </c>
-      <c r="G12" s="24">
-        <v>1.2</v>
-      </c>
-      <c r="H12" s="18">
-        <v>0.3</v>
+      <c r="B12" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="C12" s="21">
+        <v>4.2</v>
+      </c>
+      <c r="D12" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="21">
+        <v>14.9</v>
+      </c>
+      <c r="F12" s="21">
+        <v>2.1</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="21">
+        <v>2.7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="18">
-        <v>6.2</v>
-      </c>
-      <c r="C13" s="24">
-        <v>5.5</v>
-      </c>
-      <c r="D13" s="24">
-        <v>6.3</v>
-      </c>
-      <c r="E13" s="24">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F13" s="24">
-        <v>8.9</v>
-      </c>
-      <c r="G13" s="24">
-        <v>7.7</v>
-      </c>
-      <c r="H13" s="18">
-        <v>8.3000000000000007</v>
+      <c r="B13" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="C13" s="21">
+        <v>7.8</v>
+      </c>
+      <c r="D13" s="21">
+        <v>6.7</v>
+      </c>
+      <c r="E13" s="21">
+        <v>9.9</v>
+      </c>
+      <c r="F13" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="G13" s="21">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H13" s="21">
+        <v>6.7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="18">
-        <v>6.8</v>
-      </c>
-      <c r="C14" s="24">
+      <c r="B14" s="21">
+        <v>6.5</v>
+      </c>
+      <c r="C14" s="21">
         <v>7</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="21">
+        <v>6.2</v>
+      </c>
+      <c r="E14" s="21">
         <v>6.6</v>
       </c>
-      <c r="E14" s="24">
-        <v>7.8</v>
-      </c>
-      <c r="F14" s="24">
-        <v>5.8</v>
-      </c>
-      <c r="G14" s="24">
-        <v>7.4</v>
-      </c>
-      <c r="H14" s="18">
-        <v>6.3</v>
+      <c r="F14" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="G14" s="21">
+        <v>5.9</v>
+      </c>
+      <c r="H14" s="21">
+        <v>4.7</v>
       </c>
     </row>
   </sheetData>
@@ -4632,7 +4638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4666,338 +4674,338 @@
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="21">
-        <v>98.8</v>
-      </c>
-      <c r="C2" s="26">
-        <v>99</v>
-      </c>
-      <c r="D2" s="26">
-        <v>98.3</v>
-      </c>
-      <c r="E2" s="26">
-        <v>100.2</v>
-      </c>
-      <c r="F2" s="26">
-        <v>99.4</v>
-      </c>
-      <c r="G2" s="26">
-        <v>98.7</v>
-      </c>
-      <c r="H2" s="26">
-        <v>98.6</v>
+      <c r="B2" s="23">
+        <v>102.5</v>
+      </c>
+      <c r="C2" s="23">
+        <v>103.1</v>
+      </c>
+      <c r="D2" s="23">
+        <v>101.5</v>
+      </c>
+      <c r="E2" s="23">
+        <v>105.5</v>
+      </c>
+      <c r="F2" s="23">
+        <v>104.1</v>
+      </c>
+      <c r="G2" s="23">
+        <v>101.2</v>
+      </c>
+      <c r="H2" s="23">
+        <v>100.3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20">
-        <v>98.4</v>
+      <c r="B3" s="17">
+        <v>102.6</v>
       </c>
       <c r="C3" s="17">
-        <v>100.3</v>
+        <v>103.3</v>
       </c>
       <c r="D3" s="17">
-        <v>96.7</v>
+        <v>101.2</v>
       </c>
       <c r="E3" s="17">
-        <v>97.9</v>
+        <v>104.4</v>
       </c>
       <c r="F3" s="17">
-        <v>95</v>
+        <v>102.9</v>
       </c>
       <c r="G3" s="17">
-        <v>96.8</v>
+        <v>102.4</v>
       </c>
       <c r="H3" s="17">
-        <v>100.7</v>
+        <v>104.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20">
-        <v>103.3</v>
+      <c r="B4" s="17">
+        <v>108.4</v>
       </c>
       <c r="C4" s="17">
-        <v>104</v>
+        <v>109.2</v>
       </c>
       <c r="D4" s="17">
-        <v>103.3</v>
+        <v>108.7</v>
       </c>
       <c r="E4" s="17">
-        <v>105.4</v>
+        <v>110.2</v>
       </c>
       <c r="F4" s="17">
-        <v>100.7</v>
+        <v>104.7</v>
       </c>
       <c r="G4" s="17">
-        <v>101.3</v>
+        <v>105.9</v>
       </c>
       <c r="H4" s="17">
-        <v>99.7</v>
+        <v>104.1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="20">
-        <v>120.6</v>
+      <c r="B5" s="17">
+        <v>121.7</v>
       </c>
       <c r="C5" s="17">
-        <v>120.1</v>
+        <v>123.8</v>
       </c>
       <c r="D5" s="17">
-        <v>121.4</v>
+        <v>119.6</v>
       </c>
       <c r="E5" s="17">
-        <v>117.6</v>
+        <v>120.7</v>
       </c>
       <c r="F5" s="17">
-        <v>122</v>
+        <v>122.6</v>
       </c>
       <c r="G5" s="17">
-        <v>117.8</v>
+        <v>115.5</v>
       </c>
       <c r="H5" s="17">
-        <v>123</v>
+        <v>122.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="20">
-        <v>91.5</v>
+      <c r="B6" s="17">
+        <v>95.2</v>
       </c>
       <c r="C6" s="17">
-        <v>95.6</v>
+        <v>99.7</v>
       </c>
       <c r="D6" s="17">
-        <v>84.3</v>
+        <v>87.7</v>
       </c>
       <c r="E6" s="17">
-        <v>113.1</v>
+        <v>118.4</v>
       </c>
       <c r="F6" s="17">
-        <v>96.4</v>
+        <v>101.4</v>
       </c>
       <c r="G6" s="17">
-        <v>82.9</v>
+        <v>84.2</v>
       </c>
       <c r="H6" s="17">
-        <v>81.7</v>
+        <v>83.4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20">
-        <v>101.2</v>
+      <c r="B7" s="17">
+        <v>102.4</v>
       </c>
       <c r="C7" s="17">
-        <v>100.6</v>
+        <v>102.1</v>
       </c>
       <c r="D7" s="17">
-        <v>102.8</v>
+        <v>102.6</v>
       </c>
       <c r="E7" s="17">
-        <v>101.7</v>
+        <v>106.9</v>
       </c>
       <c r="F7" s="17">
-        <v>101.1</v>
+        <v>103.4</v>
       </c>
       <c r="G7" s="17">
-        <v>103</v>
+        <v>104.7</v>
       </c>
       <c r="H7" s="17">
-        <v>94</v>
+        <v>96.4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20">
-        <v>92.3</v>
+      <c r="B8" s="17">
+        <v>95.4</v>
       </c>
       <c r="C8" s="17">
-        <v>92.8</v>
+        <v>97.1</v>
       </c>
       <c r="D8" s="17">
-        <v>92.5</v>
+        <v>95.4</v>
       </c>
       <c r="E8" s="17">
-        <v>89.5</v>
+        <v>89.2</v>
       </c>
       <c r="F8" s="17">
-        <v>91.6</v>
+        <v>93.1</v>
       </c>
       <c r="G8" s="17">
-        <v>93.3</v>
+        <v>95</v>
       </c>
       <c r="H8" s="17">
-        <v>89.5</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="20">
-        <v>92</v>
+      <c r="B9" s="17">
+        <v>91.8</v>
       </c>
       <c r="C9" s="17">
-        <v>87.8</v>
+        <v>88.6</v>
       </c>
       <c r="D9" s="17">
-        <v>95.3</v>
+        <v>94.1</v>
       </c>
       <c r="E9" s="17">
-        <v>98.4</v>
+        <v>100.8</v>
       </c>
       <c r="F9" s="17">
-        <v>93.7</v>
+        <v>93.1</v>
       </c>
       <c r="G9" s="17">
-        <v>98.2</v>
+        <v>96.1</v>
       </c>
       <c r="H9" s="17">
-        <v>88.6</v>
+        <v>87.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="20">
-        <v>68.599999999999994</v>
+      <c r="B10" s="17">
+        <v>79.2</v>
       </c>
       <c r="C10" s="17">
-        <v>65.599999999999994</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="D10" s="17">
-        <v>69.2</v>
+        <v>82.5</v>
       </c>
       <c r="E10" s="17">
-        <v>69.900000000000006</v>
+        <v>82.1</v>
       </c>
       <c r="F10" s="17">
-        <v>74.900000000000006</v>
+        <v>82.3</v>
       </c>
       <c r="G10" s="17">
-        <v>78.7</v>
+        <v>83.7</v>
       </c>
       <c r="H10" s="17">
-        <v>72</v>
+        <v>77.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20">
-        <v>91.6</v>
+      <c r="B11" s="17">
+        <v>98.8</v>
       </c>
       <c r="C11" s="17">
-        <v>91.5</v>
+        <v>99.1</v>
       </c>
       <c r="D11" s="17">
-        <v>89.9</v>
+        <v>97.1</v>
       </c>
       <c r="E11" s="17">
-        <v>90.4</v>
+        <v>96.1</v>
       </c>
       <c r="F11" s="17">
-        <v>97.5</v>
+        <v>110.1</v>
       </c>
       <c r="G11" s="17">
-        <v>93.2</v>
+        <v>96.5</v>
       </c>
       <c r="H11" s="17">
-        <v>94.3</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="20">
-        <v>86.9</v>
+      <c r="B12" s="17">
+        <v>87.8</v>
       </c>
       <c r="C12" s="17">
-        <v>91.1</v>
+        <v>95.2</v>
       </c>
       <c r="D12" s="17">
-        <v>91</v>
+        <v>87.4</v>
       </c>
       <c r="E12" s="17">
-        <v>63.1</v>
+        <v>75</v>
       </c>
       <c r="F12" s="17">
-        <v>59</v>
+        <v>55.4</v>
       </c>
       <c r="G12" s="17">
-        <v>84.9</v>
+        <v>81.5</v>
       </c>
       <c r="H12" s="17">
-        <v>82.8</v>
+        <v>83.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="20">
-        <v>109.9</v>
+      <c r="B13" s="17">
+        <v>116.4</v>
       </c>
       <c r="C13" s="17">
-        <v>109.5</v>
+        <v>116.2</v>
       </c>
       <c r="D13" s="17">
-        <v>108.5</v>
+        <v>115.9</v>
       </c>
       <c r="E13" s="17">
-        <v>103.7</v>
+        <v>114.5</v>
       </c>
       <c r="F13" s="17">
+        <v>116.7</v>
+      </c>
+      <c r="G13" s="17">
         <v>114.6</v>
       </c>
-      <c r="G13" s="17">
-        <v>107.4</v>
-      </c>
       <c r="H13" s="17">
-        <v>128.6</v>
+        <v>126.9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20">
-        <v>102.6</v>
+      <c r="B14" s="17">
+        <v>106.8</v>
       </c>
       <c r="C14" s="17">
-        <v>103.2</v>
+        <v>108.4</v>
       </c>
       <c r="D14" s="17">
-        <v>100.2</v>
+        <v>104</v>
       </c>
       <c r="E14" s="17">
-        <v>106.6</v>
+        <v>111.7</v>
       </c>
       <c r="F14" s="17">
-        <v>102.9</v>
+        <v>105.2</v>
       </c>
       <c r="G14" s="17">
-        <v>105.5</v>
+        <v>107.4</v>
       </c>
       <c r="H14" s="17">
-        <v>106.6</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -6134,14 +6142,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="45"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6334,7 +6342,7 @@
       <c r="B13">
         <v>32.4</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="24">
         <v>40.299999999999997</v>
       </c>
       <c r="D13">
@@ -6745,14 +6753,14 @@
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="45"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -6926,13 +6934,13 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="25">
         <v>924</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="25">
         <v>1305</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="39">
         <f>B2-C2</f>
         <v>-381</v>
       </c>
@@ -6941,13 +6949,13 @@
       <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="25">
         <v>251</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="25">
         <v>56</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="39">
         <f t="shared" ref="D3:D20" si="0">B3-C3</f>
         <v>195</v>
       </c>
@@ -6956,13 +6964,13 @@
       <c r="A4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="25">
         <v>463</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="25">
         <v>162</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="39">
         <f t="shared" si="0"/>
         <v>301</v>
       </c>
@@ -6971,13 +6979,13 @@
       <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="25">
         <v>92</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="25">
         <v>4</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="39">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
@@ -6986,13 +6994,13 @@
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="25">
         <v>613</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="25">
         <v>784</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="39">
         <f t="shared" si="0"/>
         <v>-171</v>
       </c>
@@ -7001,13 +7009,13 @@
       <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="25">
         <v>609</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="25">
         <v>858</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="39">
         <f t="shared" si="0"/>
         <v>-249</v>
       </c>
@@ -7016,13 +7024,13 @@
       <c r="A8" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="25">
         <v>38</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="25">
         <v>40</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="39">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
@@ -7031,13 +7039,13 @@
       <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="25">
         <v>157</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="25">
         <v>49</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="39">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
@@ -7046,13 +7054,13 @@
       <c r="A10" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="25">
         <v>27</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="25">
         <v>2</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="39">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -7061,13 +7069,13 @@
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="25">
         <v>364</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="25">
         <v>382</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="39">
         <f t="shared" si="0"/>
         <v>-18</v>
       </c>
@@ -7076,13 +7084,13 @@
       <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="25">
         <v>422</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="25">
         <v>1145</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="39">
         <f t="shared" si="0"/>
         <v>-723</v>
       </c>
@@ -7091,13 +7099,13 @@
       <c r="A13" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="25">
         <v>76</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="25">
         <v>40</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="39">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -7106,13 +7114,13 @@
       <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="25">
         <v>48</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="25">
         <v>101</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="39">
         <f t="shared" si="0"/>
         <v>-53</v>
       </c>
@@ -7121,13 +7129,13 @@
       <c r="A15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="25">
         <v>188</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="25">
         <v>108</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="39">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
@@ -7136,13 +7144,13 @@
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="25">
         <v>132</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="25">
         <v>112</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="39">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -7151,13 +7159,13 @@
       <c r="A17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="25">
         <v>154</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="25">
         <v>12</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="39">
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
@@ -7166,13 +7174,13 @@
       <c r="A18" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="25">
         <v>17</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="25">
         <v>22</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="39">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
@@ -7181,13 +7189,13 @@
       <c r="A19" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="25">
         <v>37</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="25">
         <v>23</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="39">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -7196,13 +7204,13 @@
       <c r="A20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="25">
         <v>288</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="25">
         <v>177</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="39">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
@@ -7233,418 +7241,418 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="30">
         <v>4900</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="30">
         <v>1082</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="25">
         <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="25">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="25">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="25">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="25">
         <v>740</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="25">
         <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="25">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="25">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="25">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="30">
         <v>1847</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="25">
         <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="25">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="25">
         <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="25">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="25">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="25">
         <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="25">
         <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="25">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="25">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="25">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="25">
         <v>664</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="25">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B30" s="29">
+      <c r="B30" s="25">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="25">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="25">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="B33" s="34">
+      <c r="B33" s="30">
         <v>1464</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="29">
+      <c r="B34" s="25">
         <v>311</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="29">
+      <c r="B35" s="25">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="29">
+      <c r="B36" s="25">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="29">
+      <c r="B38" s="25">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="29">
+      <c r="B39" s="25">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="29">
+      <c r="B40" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="29">
+      <c r="B41" s="25">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="29">
+      <c r="B42" s="25">
         <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="29">
+      <c r="B43" s="25">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="29">
+      <c r="B44" s="25">
         <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="29">
+      <c r="B45" s="25">
         <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="B46" s="29">
+      <c r="B46" s="25">
         <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="B47" s="29">
+      <c r="B47" s="25">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="34">
+      <c r="B48" s="30">
         <v>507</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B49" s="29">
+      <c r="B49" s="25">
         <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="B50" s="29">
+      <c r="B50" s="25">
         <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="B51" s="29">
+      <c r="B51" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="B52" s="40">
+      <c r="B52" s="36">
         <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="37">
         <v>69</v>
       </c>
     </row>
@@ -7658,7 +7666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E8907-CC26-40BE-9773-A1E4E22BE731}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7676,314 +7684,314 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="30">
         <v>5384</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="30">
         <v>875</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="25">
         <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="25">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="25">
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="25">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="30">
         <v>1859</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="25">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="25">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="25">
         <v>701</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="25">
         <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="25">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="25">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="25">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="25">
         <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="25">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="30">
         <v>712</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="25">
         <v>677</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="25">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="30">
         <v>1173</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="25">
         <v>776</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="25">
         <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="25">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B25" s="30">
         <v>627</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="25">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="25">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="25">
         <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="25">
         <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="29">
+      <c r="B30" s="25">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="25">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="25">
         <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="25">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="B34" s="29">
+      <c r="B34" s="25">
         <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="B35" s="29">
+      <c r="B35" s="25">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="29">
+      <c r="B36" s="25">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="25">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="B38" s="34">
+      <c r="B38" s="30">
         <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="38">
+      <c r="B39" s="34">
         <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="B40" s="39">
+      <c r="B40" s="35">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Actualizo res fiscal feb23, pib 4to trim 22 y comex-feb22"
</commit_message>
<xml_diff>
--- a/bases/indicadores.xlsx
+++ b/bases/indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\indeco\indeco\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A922E24-A1ED-46C4-A2AE-0272ECF745CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AE32C6-A880-46DA-A061-4ED42B8F22AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC-Seriemensual" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="218">
   <si>
     <t>Período</t>
   </si>
@@ -814,7 +814,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +830,12 @@
     <fill>
       <pa